<commit_message>
Optimize conv and pool
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A18816-A9D9-4134-BE74-05D909DA118D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCF5176-BD7E-4735-8C78-C601B4DCF69F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7860" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
@@ -772,14 +772,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DDF8812-1429-4032-9C9C-F25909298566}">
   <dimension ref="A1:Q69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="124" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L67" sqref="L67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="2" customWidth="1"/>
     <col min="4" max="4" width="9" style="2" bestFit="1" customWidth="1"/>
@@ -788,18 +788,18 @@
     <col min="7" max="7" width="8" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="44.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="13.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="44.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -850,7 +850,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -882,7 +882,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -936,7 +936,7 @@
         <v>99.84</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -958,7 +958,7 @@
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>60016</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>71.680000000000007</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -1081,7 +1081,7 @@
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>532.48</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1211,7 +1211,7 @@
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1233,7 +1233,7 @@
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -1257,7 +1257,7 @@
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>143.36000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
@@ -1333,7 +1333,7 @@
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>532.48</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>17</v>
       </c>
@@ -1463,7 +1463,7 @@
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1485,7 +1485,7 @@
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
@@ -1509,7 +1509,7 @@
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>21</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>28926.720000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>22</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>286.72000000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>23</v>
       </c>
@@ -1632,7 +1632,7 @@
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>24</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>2129.92</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>26</v>
       </c>
@@ -1762,7 +1762,7 @@
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>27</v>
       </c>
@@ -1784,7 +1784,7 @@
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>28</v>
       </c>
@@ -1808,7 +1808,7 @@
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>573.44000000000005</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>30</v>
       </c>
@@ -1884,7 +1884,7 @@
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>31</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>32</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>2129.92</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>33</v>
       </c>
@@ -2014,7 +2014,7 @@
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>34</v>
       </c>
@@ -2036,7 +2036,7 @@
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>35</v>
       </c>
@@ -2060,7 +2060,7 @@
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>36</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>13411.84</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>37</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>860.16000000000008</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>38</v>
       </c>
@@ -2183,7 +2183,7 @@
       <c r="O37" s="5"/>
       <c r="P37" s="5"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>39</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>40</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>4792.32</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>41</v>
       </c>
@@ -2313,7 +2313,7 @@
       <c r="O40" s="5"/>
       <c r="P40" s="5"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>42</v>
       </c>
@@ -2335,7 +2335,7 @@
       <c r="O41" s="5"/>
       <c r="P41" s="5"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>43</v>
       </c>
@@ -2359,7 +2359,7 @@
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>44</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>1290.2400000000002</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>45</v>
       </c>
@@ -2435,7 +2435,7 @@
       <c r="O44" s="5"/>
       <c r="P44" s="5"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>46</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>47</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>4792.32</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>48</v>
       </c>
@@ -2565,7 +2565,7 @@
       <c r="O47" s="5"/>
       <c r="P47" s="5"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>49</v>
       </c>
@@ -2587,7 +2587,7 @@
       <c r="O48" s="5"/>
       <c r="P48" s="5"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>50</v>
       </c>
@@ -2611,7 +2611,7 @@
       <c r="O49" s="3"/>
       <c r="P49" s="3"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>51</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>1720.3200000000002</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>52</v>
       </c>
@@ -2687,7 +2687,7 @@
       <c r="O51" s="5"/>
       <c r="P51" s="5"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>53</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>54</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>8519.68</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>55</v>
       </c>
@@ -2817,7 +2817,7 @@
       <c r="O54" s="5"/>
       <c r="P54" s="5"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>56</v>
       </c>
@@ -2839,7 +2839,7 @@
       <c r="O55" s="5"/>
       <c r="P55" s="5"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>57</v>
       </c>
@@ -2863,7 +2863,7 @@
       <c r="O56" s="3"/>
       <c r="P56" s="3"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>58</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>2293.7600000000002</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>59</v>
       </c>
@@ -2939,7 +2939,7 @@
       <c r="O58" s="5"/>
       <c r="P58" s="5"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>60</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>61</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>8519.68</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>62</v>
       </c>
@@ -3069,7 +3069,7 @@
       <c r="O61" s="5"/>
       <c r="P61" s="5"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>63</v>
       </c>
@@ -3091,7 +3091,7 @@
       <c r="O62" s="5"/>
       <c r="P62" s="5"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>64</v>
       </c>
@@ -3115,7 +3115,7 @@
       <c r="O63" s="3"/>
       <c r="P63" s="3"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>65</v>
       </c>
@@ -3137,7 +3137,7 @@
       <c r="O64" s="5"/>
       <c r="P64" s="5"/>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>66</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>35840</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>67</v>
       </c>
@@ -3213,7 +3213,7 @@
       <c r="O66" s="5"/>
       <c r="P66" s="5"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>68</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>1000</v>
       </c>
       <c r="L67" s="6">
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
       <c r="M67" s="6">
         <v>1</v>
@@ -3253,14 +3253,14 @@
       </c>
       <c r="O67" s="6">
         <f>K67*L67</f>
-        <v>800</v>
+        <v>1200</v>
       </c>
       <c r="P67" s="6">
         <f>K67*L67*M67</f>
-        <v>800</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>69</v>
       </c>
@@ -3282,7 +3282,7 @@
       <c r="O68" s="3"/>
       <c r="P68" s="3"/>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I69" s="2">
         <f>SUM(I2:I68)</f>
         <v>3071416</v>
@@ -3301,11 +3301,11 @@
       </c>
       <c r="O69" s="2">
         <f t="shared" ref="O69:P69" si="32">SUM(O3:O68)</f>
-        <v>182583.68000000002</v>
+        <v>182983.68000000002</v>
       </c>
       <c r="P69" s="2">
         <f t="shared" si="32"/>
-        <v>178282.88</v>
+        <v>178682.88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use Additional Wrapper for MCB, Sanity PASS
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8532D2-4055-41BB-B712-9A7CDF2E7D89}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4700FD16-FED2-46B1-A5C2-91D24FD96C7D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7860" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
@@ -770,11 +770,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DDF8812-1429-4032-9C9C-F25909298566}">
-  <dimension ref="A1:Q69"/>
+  <dimension ref="A1:Q70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L71" sqref="L71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3308,6 +3308,12 @@
         <v>178682.88</v>
       </c>
     </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J70" s="2">
+        <f>J69*16/1024/8</f>
+        <v>2405.375</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="B1:B69" xr:uid="{5611B078-3ED8-409A-972B-20710E035DA1}"/>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Add p1 path in memory control block, sanity pass
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4700FD16-FED2-46B1-A5C2-91D24FD96C7D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114768CC-2717-495D-A552-10D04B853CF3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7860" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
@@ -429,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -445,6 +445,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -772,9 +775,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DDF8812-1429-4032-9C9C-F25909298566}">
   <dimension ref="A1:Q70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="124" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L71" sqref="L71"/>
+      <selection pane="bottomLeft" activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -787,7 +790,7 @@
     <col min="6" max="6" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
@@ -821,10 +824,10 @@
       <c r="G1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="7"/>
+      <c r="I1" s="8"/>
       <c r="J1" s="2" t="s">
         <v>86</v>
       </c>
@@ -3309,6 +3312,10 @@
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="I70" s="7">
+        <f>I69*16/1024/8</f>
+        <v>5998.859375</v>
+      </c>
       <c r="J70" s="2">
         <f>J69*16/1024/8</f>
         <v>2405.375</v>

</xml_diff>

<commit_message>
Update dma and fifo interface of csb, update csb and estimation table
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114768CC-2717-495D-A552-10D04B853CF3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89684071-EAAD-49D0-8873-0FE862000615}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7860" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="SqueezeNet @ 100MHz + 312.5MHz" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SqueezeNet @ 100MHz + 312.5MHz'!$B$1:$B$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SqueezeNet @ 100MHz + 312.5MHz'!$B$1:$B$70</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="116">
   <si>
     <t>INPUT</t>
   </si>
@@ -363,6 +363,24 @@
   </si>
   <si>
     <t>Operation Time Considering Parallelity(us)</t>
+  </si>
+  <si>
+    <t>Weight Mem</t>
+  </si>
+  <si>
+    <t>Data Mem</t>
+  </si>
+  <si>
+    <t>Bias Mem</t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>Output Mem</t>
+  </si>
+  <si>
+    <t>Op Paral</t>
   </si>
 </sst>
 </file>
@@ -417,10 +435,59 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -429,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -450,7 +517,67 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -773,16 +900,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DDF8812-1429-4032-9C9C-F25909298566}">
-  <dimension ref="A1:Q70"/>
+  <dimension ref="A1:AA73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J68" sqref="J68"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="2" customWidth="1"/>
     <col min="4" max="4" width="9" style="2" bestFit="1" customWidth="1"/>
@@ -790,19 +917,24 @@
     <col min="6" max="6" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="44.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.08984375" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="6.81640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="13.1796875" style="14" customWidth="1"/>
+    <col min="19" max="19" width="13.1796875" style="15" customWidth="1"/>
+    <col min="20" max="20" width="13.1796875" style="14" customWidth="1"/>
+    <col min="21" max="21" width="17.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="44.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -824,36 +956,58 @@
       <c r="G1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="8"/>
+      <c r="I1" s="26"/>
       <c r="J1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="L1" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="S1" s="28"/>
+      <c r="T1" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -872,20 +1026,35 @@
         <v>150528</v>
       </c>
       <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3">
+      <c r="K2" s="9"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16">
+        <v>655360</v>
+      </c>
+      <c r="S2" s="17">
+        <f>R2+I2/2-1</f>
+        <v>730623</v>
+      </c>
+      <c r="T2" s="16"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3">
         <f>0.0000032*I2</f>
         <v>0.4816896</v>
       </c>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="2" t="s">
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -916,30 +1085,60 @@
       <c r="J3" s="4">
         <v>1728</v>
       </c>
-      <c r="K3" s="4">
-        <f>D3*E3</f>
-        <v>192</v>
-      </c>
-      <c r="L3" s="4">
+      <c r="K3" s="10"/>
+      <c r="L3" s="18">
+        <v>4096</v>
+      </c>
+      <c r="M3" s="18">
+        <f>L3+J3/2-1</f>
+        <v>4959</v>
+      </c>
+      <c r="N3" s="18">
+        <f>M3+1</f>
+        <v>4960</v>
+      </c>
+      <c r="O3" s="18">
+        <f>N3+E3/2-1</f>
+        <v>4991</v>
+      </c>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18">
+        <f>S2+1</f>
+        <v>730624</v>
+      </c>
+      <c r="S3" s="19">
+        <f>R3+I3/2-1</f>
+        <v>1124895</v>
+      </c>
+      <c r="T3" s="18">
+        <f>U3/E3</f>
+        <v>36963</v>
+      </c>
+      <c r="U3" s="4">
+        <f>D3*I3</f>
+        <v>2365632</v>
+      </c>
+      <c r="V3" s="4">
         <v>0.52</v>
       </c>
-      <c r="M3" s="4">
-        <v>1</v>
-      </c>
-      <c r="N3" s="4">
+      <c r="W3" s="4">
+        <v>1</v>
+      </c>
+      <c r="X3" s="4">
         <f>0.0000032*J3+0.0000064*I3</f>
         <v>5.0522111999999995</v>
       </c>
-      <c r="O3" s="4">
-        <f>K3*L3</f>
-        <v>99.84</v>
-      </c>
-      <c r="P3" s="4">
-        <f>K3*L3*M3</f>
-        <v>99.84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Y3" s="4">
+        <f>U3*V3</f>
+        <v>1230128.6400000001</v>
+      </c>
+      <c r="Z3" s="4">
+        <f>T3*V3*W3</f>
+        <v>19220.760000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -954,14 +1153,24 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="K4" s="11"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="20"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -972,7 +1181,9 @@
         <v>83</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="E5" s="6">
+        <v>64</v>
+      </c>
       <c r="F5" s="6">
         <v>2</v>
       </c>
@@ -986,29 +1197,48 @@
         <v>193600</v>
       </c>
       <c r="J5" s="6"/>
-      <c r="K5" s="6">
+      <c r="K5" s="12"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22">
+        <f>S3+1</f>
+        <v>1124896</v>
+      </c>
+      <c r="S5" s="23">
+        <f>R5+I5/2-1</f>
+        <v>1221695</v>
+      </c>
+      <c r="T5" s="22">
+        <f>U5/E5</f>
+        <v>3025</v>
+      </c>
+      <c r="U5" s="6">
         <v>193600</v>
       </c>
-      <c r="L5" s="6">
+      <c r="V5" s="6">
         <v>0.31</v>
       </c>
-      <c r="M5" s="6">
-        <v>1</v>
-      </c>
-      <c r="N5" s="6">
+      <c r="W5" s="6">
+        <v>1</v>
+      </c>
+      <c r="X5" s="6">
         <f>0.0000064*I5</f>
         <v>1.2390399999999999</v>
       </c>
-      <c r="O5" s="6">
-        <f>K5*L5</f>
+      <c r="Y5" s="6">
+        <f>U5*V5</f>
         <v>60016</v>
       </c>
-      <c r="P5" s="6">
-        <f>K5*L5*M5</f>
-        <v>60016</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Z5" s="6">
+        <f>T5*V5*W5</f>
+        <v>937.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -1039,30 +1269,61 @@
       <c r="J6" s="4">
         <v>1024</v>
       </c>
-      <c r="K6" s="4">
-        <f>D6*E6</f>
-        <v>1024</v>
-      </c>
-      <c r="L6" s="4">
+      <c r="K6" s="10"/>
+      <c r="L6" s="18">
+        <f>L3+J3/2+E3/2</f>
+        <v>4992</v>
+      </c>
+      <c r="M6" s="18">
+        <f>L6+J6/2-1</f>
+        <v>5503</v>
+      </c>
+      <c r="N6" s="18">
+        <f>M6+1</f>
+        <v>5504</v>
+      </c>
+      <c r="O6" s="18">
+        <f>N6+E6/2-1</f>
+        <v>5511</v>
+      </c>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18">
+        <f>S5+1</f>
+        <v>1221696</v>
+      </c>
+      <c r="S6" s="19">
+        <f>R6+I6/2-1</f>
+        <v>1245895</v>
+      </c>
+      <c r="T6" s="18">
+        <f>U6/E6</f>
+        <v>193600</v>
+      </c>
+      <c r="U6" s="4">
+        <f>D6*I6</f>
+        <v>3097600</v>
+      </c>
+      <c r="V6" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M6" s="4">
-        <v>1</v>
-      </c>
-      <c r="N6" s="4">
+      <c r="W6" s="4">
+        <v>1</v>
+      </c>
+      <c r="X6" s="4">
         <f>0.0000032*J6+0.0000064*I6</f>
         <v>0.3130368</v>
       </c>
-      <c r="O6" s="4">
-        <f>K6*L6</f>
-        <v>71.680000000000007</v>
-      </c>
-      <c r="P6" s="4">
-        <f>K6*L6*M6</f>
-        <v>71.680000000000007</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Y6" s="4">
+        <f>U6*V6</f>
+        <v>216832.00000000003</v>
+      </c>
+      <c r="Z6" s="4">
+        <f>T6*V6*W6</f>
+        <v>13552.000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -1077,14 +1338,24 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="K7" s="11"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -1115,30 +1386,61 @@
       <c r="J8" s="4">
         <v>1024</v>
       </c>
-      <c r="K8" s="4">
-        <f t="shared" ref="K8:K9" si="0">D8*E8</f>
-        <v>1024</v>
-      </c>
-      <c r="L8" s="4">
+      <c r="K8" s="10"/>
+      <c r="L8" s="18">
+        <f>L6+J6/2+E6/2</f>
+        <v>5512</v>
+      </c>
+      <c r="M8" s="18">
+        <f t="shared" ref="M8:M9" si="0">L8+J8/2-1</f>
+        <v>6023</v>
+      </c>
+      <c r="N8" s="18">
+        <f t="shared" ref="N8:N9" si="1">M8+1</f>
+        <v>6024</v>
+      </c>
+      <c r="O8" s="18">
+        <f>N8+E8/2-1</f>
+        <v>6055</v>
+      </c>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18">
+        <f>S6+1</f>
+        <v>1245896</v>
+      </c>
+      <c r="S8" s="19">
+        <f>R8+I8/2-1</f>
+        <v>1342695</v>
+      </c>
+      <c r="T8" s="18">
+        <f>U8/E8</f>
+        <v>48400</v>
+      </c>
+      <c r="U8" s="4">
+        <f>D8*I8</f>
+        <v>3097600</v>
+      </c>
+      <c r="V8" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M8" s="4">
+      <c r="W8" s="4">
         <v>0</v>
       </c>
-      <c r="N8" s="4">
-        <f t="shared" ref="N8:N9" si="1">0.0000032*J8+0.0000064*I8</f>
+      <c r="X8" s="4">
+        <f>0.0000032*J8+0.0000064*I8</f>
         <v>1.2423168</v>
       </c>
-      <c r="O8" s="4">
-        <f t="shared" ref="O8:O9" si="2">K8*L8</f>
-        <v>71.680000000000007</v>
-      </c>
-      <c r="P8" s="4">
-        <f t="shared" ref="P8:P9" si="3">K8*L8*M8</f>
+      <c r="Y8" s="4">
+        <f t="shared" ref="Y8:Y9" si="2">U8*V8</f>
+        <v>216832.00000000003</v>
+      </c>
+      <c r="Z8" s="4">
+        <f t="shared" ref="Z8:Z9" si="3">T8*V8*W8</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -1169,30 +1471,61 @@
       <c r="J9" s="4">
         <v>9216</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="10"/>
+      <c r="L9" s="18">
+        <f>L8+J8/2+E8/2</f>
+        <v>6056</v>
+      </c>
+      <c r="M9" s="18">
         <f t="shared" si="0"/>
-        <v>1024</v>
-      </c>
-      <c r="L9" s="4">
+        <v>10663</v>
+      </c>
+      <c r="N9" s="18">
+        <f t="shared" si="1"/>
+        <v>10664</v>
+      </c>
+      <c r="O9" s="18">
+        <f>N9+E9/2-1</f>
+        <v>10695</v>
+      </c>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18">
+        <f>S8+1</f>
+        <v>1342696</v>
+      </c>
+      <c r="S9" s="19">
+        <f>R9+I9/2-1</f>
+        <v>1439495</v>
+      </c>
+      <c r="T9" s="18">
+        <f>U9/E9</f>
+        <v>48400</v>
+      </c>
+      <c r="U9" s="4">
+        <f>D9*I9</f>
+        <v>3097600</v>
+      </c>
+      <c r="V9" s="4">
         <v>0.52</v>
       </c>
-      <c r="M9" s="4">
-        <v>1</v>
-      </c>
-      <c r="N9" s="4">
-        <f t="shared" si="1"/>
+      <c r="W9" s="4">
+        <v>1</v>
+      </c>
+      <c r="X9" s="4">
+        <f>0.0000032*J9+0.0000064*I9</f>
         <v>1.2685312</v>
       </c>
-      <c r="O9" s="4">
+      <c r="Y9" s="4">
         <f t="shared" si="2"/>
-        <v>532.48</v>
-      </c>
-      <c r="P9" s="4">
+        <v>1610752</v>
+      </c>
+      <c r="Z9" s="4">
         <f t="shared" si="3"/>
-        <v>532.48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+        <v>25168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1207,14 +1540,24 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="K10" s="11"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1229,14 +1572,24 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="K11" s="11"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="20"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -1253,14 +1606,24 @@
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="K12" s="9"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
@@ -1291,30 +1654,61 @@
       <c r="J13" s="4">
         <v>2048</v>
       </c>
-      <c r="K13" s="4">
-        <f>D13*E13</f>
-        <v>2048</v>
-      </c>
-      <c r="L13" s="4">
+      <c r="K13" s="10"/>
+      <c r="L13" s="18">
+        <f>L9+J9/2+E9/2</f>
+        <v>10696</v>
+      </c>
+      <c r="M13" s="18">
+        <f>L13+J13/2-1</f>
+        <v>11719</v>
+      </c>
+      <c r="N13" s="18">
+        <f>M13+1</f>
+        <v>11720</v>
+      </c>
+      <c r="O13" s="18">
+        <f>N13+E13/2-1</f>
+        <v>11727</v>
+      </c>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18">
+        <f>S9+1</f>
+        <v>1439496</v>
+      </c>
+      <c r="S13" s="19">
+        <f>R13+I13/2-1</f>
+        <v>1463695</v>
+      </c>
+      <c r="T13" s="18">
+        <f>U13/E13</f>
+        <v>387200</v>
+      </c>
+      <c r="U13" s="4">
+        <f>D13*I13</f>
+        <v>6195200</v>
+      </c>
+      <c r="V13" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M13" s="4">
-        <v>1</v>
-      </c>
-      <c r="N13" s="4">
+      <c r="W13" s="4">
+        <v>1</v>
+      </c>
+      <c r="X13" s="4">
         <f>0.0000032*J13+0.0000064*I13</f>
         <v>0.31631359999999997</v>
       </c>
-      <c r="O13" s="4">
-        <f>K13*L13</f>
-        <v>143.36000000000001</v>
-      </c>
-      <c r="P13" s="4">
-        <f>K13*L13*M13</f>
-        <v>143.36000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Y13" s="4">
+        <f>U13*V13</f>
+        <v>433664.00000000006</v>
+      </c>
+      <c r="Z13" s="4">
+        <f>T13*V13*W13</f>
+        <v>27104.000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
@@ -1329,14 +1723,24 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="K14" s="11"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="20"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
@@ -1367,30 +1771,61 @@
       <c r="J15" s="4">
         <v>1024</v>
       </c>
-      <c r="K15" s="4">
-        <f t="shared" ref="K15:K16" si="4">D15*E15</f>
-        <v>1024</v>
-      </c>
-      <c r="L15" s="4">
+      <c r="K15" s="10"/>
+      <c r="L15" s="18">
+        <f>L13+J13/2+E13/2</f>
+        <v>11728</v>
+      </c>
+      <c r="M15" s="18">
+        <f t="shared" ref="M15:M16" si="4">L15+J15/2-1</f>
+        <v>12239</v>
+      </c>
+      <c r="N15" s="18">
+        <f t="shared" ref="N15:N16" si="5">M15+1</f>
+        <v>12240</v>
+      </c>
+      <c r="O15" s="18">
+        <f>N15+E15/2-1</f>
+        <v>12271</v>
+      </c>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18">
+        <f>S13+1</f>
+        <v>1463696</v>
+      </c>
+      <c r="S15" s="19">
+        <f>R15+I15/2-1</f>
+        <v>1560495</v>
+      </c>
+      <c r="T15" s="18">
+        <f>U15/E15</f>
+        <v>48400</v>
+      </c>
+      <c r="U15" s="4">
+        <f>D15*I15</f>
+        <v>3097600</v>
+      </c>
+      <c r="V15" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M15" s="4">
+      <c r="W15" s="4">
         <v>0</v>
       </c>
-      <c r="N15" s="4">
-        <f t="shared" ref="N15:N16" si="5">0.0000032*J15+0.0000064*I15</f>
+      <c r="X15" s="4">
+        <f>0.0000032*J15+0.0000064*I15</f>
         <v>1.2423168</v>
       </c>
-      <c r="O15" s="4">
-        <f t="shared" ref="O15:O16" si="6">K15*L15</f>
-        <v>71.680000000000007</v>
-      </c>
-      <c r="P15" s="4">
-        <f t="shared" ref="P15:P16" si="7">K15*L15*M15</f>
+      <c r="Y15" s="4">
+        <f t="shared" ref="Y15:Y16" si="6">U15*V15</f>
+        <v>216832.00000000003</v>
+      </c>
+      <c r="Z15" s="4">
+        <f t="shared" ref="Z15:Z16" si="7">T15*V15*W15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -1421,30 +1856,61 @@
       <c r="J16" s="4">
         <v>9216</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="10"/>
+      <c r="L16" s="18">
+        <f>L15+J15/2+E15/2</f>
+        <v>12272</v>
+      </c>
+      <c r="M16" s="18">
         <f t="shared" si="4"/>
-        <v>1024</v>
-      </c>
-      <c r="L16" s="4">
+        <v>16879</v>
+      </c>
+      <c r="N16" s="18">
+        <f t="shared" si="5"/>
+        <v>16880</v>
+      </c>
+      <c r="O16" s="18">
+        <f>N16+E16/2-1</f>
+        <v>16911</v>
+      </c>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="18">
+        <f>S15+1</f>
+        <v>1560496</v>
+      </c>
+      <c r="S16" s="19">
+        <f>R16+I16/2-1</f>
+        <v>1657295</v>
+      </c>
+      <c r="T16" s="18">
+        <f>U16/E16</f>
+        <v>48400</v>
+      </c>
+      <c r="U16" s="4">
+        <f>D16*I16</f>
+        <v>3097600</v>
+      </c>
+      <c r="V16" s="4">
         <v>0.52</v>
       </c>
-      <c r="M16" s="4">
-        <v>1</v>
-      </c>
-      <c r="N16" s="4">
-        <f t="shared" si="5"/>
+      <c r="W16" s="4">
+        <v>1</v>
+      </c>
+      <c r="X16" s="4">
+        <f>0.0000032*J16+0.0000064*I16</f>
         <v>1.2685312</v>
       </c>
-      <c r="O16" s="4">
+      <c r="Y16" s="4">
         <f t="shared" si="6"/>
-        <v>532.48</v>
-      </c>
-      <c r="P16" s="4">
+        <v>1610752</v>
+      </c>
+      <c r="Z16" s="4">
         <f t="shared" si="7"/>
-        <v>532.48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+        <v>25168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>17</v>
       </c>
@@ -1459,14 +1925,24 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K17" s="11"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="20"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="5"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1481,14 +1957,24 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K18" s="11"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="20"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="5"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
@@ -1505,14 +1991,24 @@
       </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K19" s="9"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="16"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="3"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>21</v>
       </c>
@@ -1523,7 +2019,9 @@
         <v>83</v>
       </c>
       <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="E20" s="6">
+        <v>128</v>
+      </c>
       <c r="F20" s="6">
         <v>2</v>
       </c>
@@ -1537,29 +2035,48 @@
         <v>93312</v>
       </c>
       <c r="J20" s="6"/>
-      <c r="K20" s="6">
+      <c r="K20" s="12"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="22"/>
+      <c r="R20" s="22">
+        <f>S16+1</f>
+        <v>1657296</v>
+      </c>
+      <c r="S20" s="23">
+        <f>R20+I20/2-1</f>
+        <v>1703951</v>
+      </c>
+      <c r="T20" s="22">
+        <f>U20/E20</f>
+        <v>729</v>
+      </c>
+      <c r="U20" s="6">
         <v>93312</v>
       </c>
-      <c r="L20" s="6">
+      <c r="V20" s="6">
         <v>0.31</v>
       </c>
-      <c r="M20" s="6">
-        <v>1</v>
-      </c>
-      <c r="N20" s="6">
+      <c r="W20" s="6">
+        <v>1</v>
+      </c>
+      <c r="X20" s="6">
         <f>0.0000064*I20</f>
         <v>0.59719679999999997</v>
       </c>
-      <c r="O20" s="6">
-        <f>K20*L20</f>
+      <c r="Y20" s="6">
+        <f>U20*V20</f>
         <v>28926.720000000001</v>
       </c>
-      <c r="P20" s="6">
-        <f>K20*L20*M20</f>
-        <v>28926.720000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Z20" s="6">
+        <f>T20*V20*W20</f>
+        <v>225.99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>22</v>
       </c>
@@ -1590,30 +2107,61 @@
       <c r="J21" s="4">
         <v>4096</v>
       </c>
-      <c r="K21" s="4">
-        <f>D21*E21</f>
-        <v>4096</v>
-      </c>
-      <c r="L21" s="4">
+      <c r="K21" s="10"/>
+      <c r="L21" s="18">
+        <f>L16+J16/2+E16/2</f>
+        <v>16912</v>
+      </c>
+      <c r="M21" s="18">
+        <f>L21+J21/2-1</f>
+        <v>18959</v>
+      </c>
+      <c r="N21" s="18">
+        <f>M21+1</f>
+        <v>18960</v>
+      </c>
+      <c r="O21" s="18">
+        <f>N21+E21/2-1</f>
+        <v>18975</v>
+      </c>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18">
+        <f>S20+1</f>
+        <v>1703952</v>
+      </c>
+      <c r="S21" s="19">
+        <f>R21+I21/2-1</f>
+        <v>1715615</v>
+      </c>
+      <c r="T21" s="18">
+        <f>U21/E21</f>
+        <v>93312</v>
+      </c>
+      <c r="U21" s="4">
+        <f>D21*I21</f>
+        <v>2985984</v>
+      </c>
+      <c r="V21" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M21" s="4">
-        <v>1</v>
-      </c>
-      <c r="N21" s="4">
+      <c r="W21" s="4">
+        <v>1</v>
+      </c>
+      <c r="X21" s="4">
         <f>0.0000032*J21+0.0000064*I21</f>
         <v>0.16240640000000001</v>
       </c>
-      <c r="O21" s="4">
-        <f>K21*L21</f>
-        <v>286.72000000000003</v>
-      </c>
-      <c r="P21" s="4">
-        <f>K21*L21*M21</f>
-        <v>286.72000000000003</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Y21" s="4">
+        <f>U21*V21</f>
+        <v>209018.88000000003</v>
+      </c>
+      <c r="Z21" s="4">
+        <f>T21*V21*W21</f>
+        <v>6531.8400000000011</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>23</v>
       </c>
@@ -1628,14 +2176,24 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K22" s="11"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="20"/>
+      <c r="S22" s="21"/>
+      <c r="T22" s="20"/>
+      <c r="U22" s="5"/>
+      <c r="V22" s="5"/>
+      <c r="W22" s="5"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="5"/>
+      <c r="Z22" s="5"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>24</v>
       </c>
@@ -1666,30 +2224,61 @@
       <c r="J23" s="4">
         <v>4096</v>
       </c>
-      <c r="K23" s="4">
-        <f t="shared" ref="K23:K24" si="8">D23*E23</f>
-        <v>4096</v>
-      </c>
-      <c r="L23" s="4">
+      <c r="K23" s="10"/>
+      <c r="L23" s="18">
+        <f>L21+J21/2+E21/2</f>
+        <v>18976</v>
+      </c>
+      <c r="M23" s="18">
+        <f t="shared" ref="M23:M24" si="8">L23+J23/2-1</f>
+        <v>21023</v>
+      </c>
+      <c r="N23" s="18">
+        <f t="shared" ref="N23:N24" si="9">M23+1</f>
+        <v>21024</v>
+      </c>
+      <c r="O23" s="18">
+        <f>N23+E23/2-1</f>
+        <v>21087</v>
+      </c>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18">
+        <f>S21+1</f>
+        <v>1715616</v>
+      </c>
+      <c r="S23" s="19">
+        <f>R23+I23/2-1</f>
+        <v>1762271</v>
+      </c>
+      <c r="T23" s="18">
+        <f>U23/E23</f>
+        <v>23328</v>
+      </c>
+      <c r="U23" s="4">
+        <f>D23*I23</f>
+        <v>2985984</v>
+      </c>
+      <c r="V23" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M23" s="4">
+      <c r="W23" s="4">
         <v>0</v>
       </c>
-      <c r="N23" s="4">
-        <f t="shared" ref="N23:N24" si="9">0.0000032*J23+0.0000064*I23</f>
+      <c r="X23" s="4">
+        <f>0.0000032*J23+0.0000064*I23</f>
         <v>0.61030399999999996</v>
       </c>
-      <c r="O23" s="4">
-        <f t="shared" ref="O23:O24" si="10">K23*L23</f>
-        <v>286.72000000000003</v>
-      </c>
-      <c r="P23" s="4">
-        <f t="shared" ref="P23:P24" si="11">K23*L23*M23</f>
+      <c r="Y23" s="4">
+        <f t="shared" ref="Y23:Y24" si="10">U23*V23</f>
+        <v>209018.88000000003</v>
+      </c>
+      <c r="Z23" s="4">
+        <f t="shared" ref="Z23:Z24" si="11">T23*V23*W23</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
@@ -1720,30 +2309,61 @@
       <c r="J24" s="4">
         <v>36864</v>
       </c>
-      <c r="K24" s="4">
+      <c r="K24" s="10"/>
+      <c r="L24" s="18">
+        <f>L23+J23/2+E23/2</f>
+        <v>21088</v>
+      </c>
+      <c r="M24" s="18">
         <f t="shared" si="8"/>
-        <v>4096</v>
-      </c>
-      <c r="L24" s="4">
+        <v>39519</v>
+      </c>
+      <c r="N24" s="18">
+        <f t="shared" si="9"/>
+        <v>39520</v>
+      </c>
+      <c r="O24" s="18">
+        <f>N24+E24/2-1</f>
+        <v>39583</v>
+      </c>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18">
+        <f>S23+1</f>
+        <v>1762272</v>
+      </c>
+      <c r="S24" s="19">
+        <f>R24+I24/2-1</f>
+        <v>1808927</v>
+      </c>
+      <c r="T24" s="18">
+        <f>U24/E24</f>
+        <v>23328</v>
+      </c>
+      <c r="U24" s="4">
+        <f>D24*I24</f>
+        <v>2985984</v>
+      </c>
+      <c r="V24" s="4">
         <v>0.52</v>
       </c>
-      <c r="M24" s="4">
-        <v>1</v>
-      </c>
-      <c r="N24" s="4">
-        <f t="shared" si="9"/>
+      <c r="W24" s="4">
+        <v>1</v>
+      </c>
+      <c r="X24" s="4">
+        <f>0.0000032*J24+0.0000064*I24</f>
         <v>0.71516159999999995</v>
       </c>
-      <c r="O24" s="4">
+      <c r="Y24" s="4">
         <f t="shared" si="10"/>
-        <v>2129.92</v>
-      </c>
-      <c r="P24" s="4">
+        <v>1552711.6800000002</v>
+      </c>
+      <c r="Z24" s="4">
         <f t="shared" si="11"/>
-        <v>2129.92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+        <v>12130.560000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>26</v>
       </c>
@@ -1758,14 +2378,24 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
-      <c r="P25" s="5"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K25" s="11"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="20"/>
+      <c r="O25" s="20"/>
+      <c r="P25" s="20"/>
+      <c r="Q25" s="20"/>
+      <c r="R25" s="20"/>
+      <c r="S25" s="21"/>
+      <c r="T25" s="20"/>
+      <c r="U25" s="5"/>
+      <c r="V25" s="5"/>
+      <c r="W25" s="5"/>
+      <c r="X25" s="5"/>
+      <c r="Y25" s="5"/>
+      <c r="Z25" s="5"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>27</v>
       </c>
@@ -1780,14 +2410,24 @@
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="5"/>
-      <c r="P26" s="5"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K26" s="11"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="20"/>
+      <c r="O26" s="20"/>
+      <c r="P26" s="20"/>
+      <c r="Q26" s="20"/>
+      <c r="R26" s="20"/>
+      <c r="S26" s="21"/>
+      <c r="T26" s="20"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="5"/>
+      <c r="W26" s="5"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="5"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>28</v>
       </c>
@@ -1804,14 +2444,24 @@
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K27" s="9"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="16"/>
+      <c r="S27" s="17"/>
+      <c r="T27" s="16"/>
+      <c r="U27" s="3"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+      <c r="X27" s="3"/>
+      <c r="Y27" s="3"/>
+      <c r="Z27" s="3"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
@@ -1842,30 +2492,61 @@
       <c r="J28" s="4">
         <v>8192</v>
       </c>
-      <c r="K28" s="4">
-        <f>D28*E28</f>
-        <v>8192</v>
-      </c>
-      <c r="L28" s="4">
+      <c r="K28" s="10"/>
+      <c r="L28" s="18">
+        <f>L24+J24/2+E24/2</f>
+        <v>39584</v>
+      </c>
+      <c r="M28" s="18">
+        <f>L28+J28/2-1</f>
+        <v>43679</v>
+      </c>
+      <c r="N28" s="18">
+        <f>M28+1</f>
+        <v>43680</v>
+      </c>
+      <c r="O28" s="18">
+        <f>N28+E28/2-1</f>
+        <v>43695</v>
+      </c>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18">
+        <f>S24+1</f>
+        <v>1808928</v>
+      </c>
+      <c r="S28" s="19">
+        <f>R28+I28/2-1</f>
+        <v>1820591</v>
+      </c>
+      <c r="T28" s="18">
+        <f>U28/E28</f>
+        <v>186624</v>
+      </c>
+      <c r="U28" s="4">
+        <f>D28*I28</f>
+        <v>5971968</v>
+      </c>
+      <c r="V28" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M28" s="4">
-        <v>1</v>
-      </c>
-      <c r="N28" s="4">
+      <c r="W28" s="4">
+        <v>1</v>
+      </c>
+      <c r="X28" s="4">
         <f>0.0000032*J28+0.0000064*I28</f>
         <v>0.17551359999999999</v>
       </c>
-      <c r="O28" s="4">
-        <f>K28*L28</f>
-        <v>573.44000000000005</v>
-      </c>
-      <c r="P28" s="4">
-        <f>K28*L28*M28</f>
-        <v>573.44000000000005</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Y28" s="4">
+        <f>U28*V28</f>
+        <v>418037.76000000007</v>
+      </c>
+      <c r="Z28" s="4">
+        <f>T28*V28*W28</f>
+        <v>13063.680000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>30</v>
       </c>
@@ -1880,14 +2561,24 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K29" s="11"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
+      <c r="P29" s="20"/>
+      <c r="Q29" s="20"/>
+      <c r="R29" s="20"/>
+      <c r="S29" s="21"/>
+      <c r="T29" s="20"/>
+      <c r="U29" s="5"/>
+      <c r="V29" s="5"/>
+      <c r="W29" s="5"/>
+      <c r="X29" s="5"/>
+      <c r="Y29" s="5"/>
+      <c r="Z29" s="5"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>31</v>
       </c>
@@ -1918,30 +2609,61 @@
       <c r="J30" s="4">
         <v>4096</v>
       </c>
-      <c r="K30" s="4">
-        <f t="shared" ref="K30:K31" si="12">D30*E30</f>
-        <v>4096</v>
-      </c>
-      <c r="L30" s="4">
+      <c r="K30" s="10"/>
+      <c r="L30" s="18">
+        <f>L28+J28/2+E28/2</f>
+        <v>43696</v>
+      </c>
+      <c r="M30" s="18">
+        <f t="shared" ref="M30:M31" si="12">L30+J30/2-1</f>
+        <v>45743</v>
+      </c>
+      <c r="N30" s="18">
+        <f t="shared" ref="N30:N31" si="13">M30+1</f>
+        <v>45744</v>
+      </c>
+      <c r="O30" s="18">
+        <f>N30+E30/2-1</f>
+        <v>45807</v>
+      </c>
+      <c r="P30" s="18"/>
+      <c r="Q30" s="18"/>
+      <c r="R30" s="18">
+        <f>S28+1</f>
+        <v>1820592</v>
+      </c>
+      <c r="S30" s="19">
+        <f>R30+I30/2-1</f>
+        <v>1867247</v>
+      </c>
+      <c r="T30" s="18">
+        <f>U30/E30</f>
+        <v>23328</v>
+      </c>
+      <c r="U30" s="4">
+        <f>D30*I30</f>
+        <v>2985984</v>
+      </c>
+      <c r="V30" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M30" s="4">
+      <c r="W30" s="4">
         <v>0</v>
       </c>
-      <c r="N30" s="4">
-        <f t="shared" ref="N30:N31" si="13">0.0000032*J30+0.0000064*I30</f>
+      <c r="X30" s="4">
+        <f>0.0000032*J30+0.0000064*I30</f>
         <v>0.61030399999999996</v>
       </c>
-      <c r="O30" s="4">
-        <f t="shared" ref="O30:O31" si="14">K30*L30</f>
-        <v>286.72000000000003</v>
-      </c>
-      <c r="P30" s="4">
-        <f t="shared" ref="P30:P31" si="15">K30*L30*M30</f>
+      <c r="Y30" s="4">
+        <f t="shared" ref="Y30:Y31" si="14">U30*V30</f>
+        <v>209018.88000000003</v>
+      </c>
+      <c r="Z30" s="4">
+        <f t="shared" ref="Z30:Z31" si="15">T30*V30*W30</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>32</v>
       </c>
@@ -1972,30 +2694,61 @@
       <c r="J31" s="4">
         <v>36864</v>
       </c>
-      <c r="K31" s="4">
+      <c r="K31" s="10"/>
+      <c r="L31" s="18">
+        <f>L30+J30/2+E30/2</f>
+        <v>45808</v>
+      </c>
+      <c r="M31" s="18">
         <f t="shared" si="12"/>
-        <v>4096</v>
-      </c>
-      <c r="L31" s="4">
+        <v>64239</v>
+      </c>
+      <c r="N31" s="18">
+        <f t="shared" si="13"/>
+        <v>64240</v>
+      </c>
+      <c r="O31" s="18">
+        <f>N31+E31/2-1</f>
+        <v>64303</v>
+      </c>
+      <c r="P31" s="18"/>
+      <c r="Q31" s="18"/>
+      <c r="R31" s="18">
+        <f>S30+1</f>
+        <v>1867248</v>
+      </c>
+      <c r="S31" s="19">
+        <f>R31+I31/2-1</f>
+        <v>1913903</v>
+      </c>
+      <c r="T31" s="18">
+        <f>U31/E31</f>
+        <v>23328</v>
+      </c>
+      <c r="U31" s="4">
+        <f>D31*I31</f>
+        <v>2985984</v>
+      </c>
+      <c r="V31" s="4">
         <v>0.52</v>
       </c>
-      <c r="M31" s="4">
-        <v>1</v>
-      </c>
-      <c r="N31" s="4">
-        <f t="shared" si="13"/>
+      <c r="W31" s="4">
+        <v>1</v>
+      </c>
+      <c r="X31" s="4">
+        <f>0.0000032*J31+0.0000064*I31</f>
         <v>0.71516159999999995</v>
       </c>
-      <c r="O31" s="4">
+      <c r="Y31" s="4">
         <f t="shared" si="14"/>
-        <v>2129.92</v>
-      </c>
-      <c r="P31" s="4">
+        <v>1552711.6800000002</v>
+      </c>
+      <c r="Z31" s="4">
         <f t="shared" si="15"/>
-        <v>2129.92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+        <v>12130.560000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>33</v>
       </c>
@@ -2010,14 +2763,24 @@
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
-      <c r="P32" s="5"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K32" s="11"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="20"/>
+      <c r="N32" s="20"/>
+      <c r="O32" s="20"/>
+      <c r="P32" s="20"/>
+      <c r="Q32" s="20"/>
+      <c r="R32" s="20"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="20"/>
+      <c r="U32" s="5"/>
+      <c r="V32" s="5"/>
+      <c r="W32" s="5"/>
+      <c r="X32" s="5"/>
+      <c r="Y32" s="5"/>
+      <c r="Z32" s="5"/>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>34</v>
       </c>
@@ -2032,14 +2795,24 @@
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="5"/>
-      <c r="O33" s="5"/>
-      <c r="P33" s="5"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K33" s="11"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20"/>
+      <c r="N33" s="20"/>
+      <c r="O33" s="20"/>
+      <c r="P33" s="20"/>
+      <c r="Q33" s="20"/>
+      <c r="R33" s="20"/>
+      <c r="S33" s="21"/>
+      <c r="T33" s="20"/>
+      <c r="U33" s="5"/>
+      <c r="V33" s="5"/>
+      <c r="W33" s="5"/>
+      <c r="X33" s="5"/>
+      <c r="Y33" s="5"/>
+      <c r="Z33" s="5"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>35</v>
       </c>
@@ -2056,14 +2829,24 @@
       </c>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
-      <c r="O34" s="3"/>
-      <c r="P34" s="3"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K34" s="9"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="16"/>
+      <c r="S34" s="17"/>
+      <c r="T34" s="16"/>
+      <c r="U34" s="3"/>
+      <c r="V34" s="3"/>
+      <c r="W34" s="3"/>
+      <c r="X34" s="3"/>
+      <c r="Y34" s="3"/>
+      <c r="Z34" s="3"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>36</v>
       </c>
@@ -2074,7 +2857,9 @@
         <v>83</v>
       </c>
       <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
+      <c r="E35" s="6">
+        <v>256</v>
+      </c>
       <c r="F35" s="6">
         <v>2</v>
       </c>
@@ -2088,29 +2873,48 @@
         <v>43624</v>
       </c>
       <c r="J35" s="6"/>
-      <c r="K35" s="6">
+      <c r="K35" s="12"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="22"/>
+      <c r="N35" s="22"/>
+      <c r="O35" s="22"/>
+      <c r="P35" s="22"/>
+      <c r="Q35" s="22"/>
+      <c r="R35" s="22">
+        <f>S31+1</f>
+        <v>1913904</v>
+      </c>
+      <c r="S35" s="23">
+        <f>R35+I35/2-1</f>
+        <v>1935715</v>
+      </c>
+      <c r="T35" s="22">
+        <f>U35/E35</f>
+        <v>169</v>
+      </c>
+      <c r="U35" s="6">
         <v>43264</v>
       </c>
-      <c r="L35" s="6">
+      <c r="V35" s="6">
         <v>0.31</v>
       </c>
-      <c r="M35" s="6">
-        <v>1</v>
-      </c>
-      <c r="N35" s="6">
+      <c r="W35" s="6">
+        <v>1</v>
+      </c>
+      <c r="X35" s="6">
         <f>0.0000064*I35</f>
         <v>0.27919359999999999</v>
       </c>
-      <c r="O35" s="6">
-        <f>K35*L35</f>
+      <c r="Y35" s="6">
+        <f>U35*V35</f>
         <v>13411.84</v>
       </c>
-      <c r="P35" s="6">
-        <f>K35*L35*M35</f>
-        <v>13411.84</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Z35" s="6">
+        <f>T35*V35*W35</f>
+        <v>52.39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>37</v>
       </c>
@@ -2141,30 +2945,61 @@
       <c r="J36" s="4">
         <v>12288</v>
       </c>
-      <c r="K36" s="4">
-        <f>D36*E36</f>
-        <v>12288</v>
-      </c>
-      <c r="L36" s="4">
+      <c r="K36" s="10"/>
+      <c r="L36" s="18">
+        <f>L31+J31/2+E31/2</f>
+        <v>64304</v>
+      </c>
+      <c r="M36" s="18">
+        <f>L36+J36/2-1</f>
+        <v>70447</v>
+      </c>
+      <c r="N36" s="18">
+        <f>M36+1</f>
+        <v>70448</v>
+      </c>
+      <c r="O36" s="18">
+        <f>N36+E36/2-1</f>
+        <v>70471</v>
+      </c>
+      <c r="P36" s="18"/>
+      <c r="Q36" s="18"/>
+      <c r="R36" s="18">
+        <f>S35+1</f>
+        <v>1935716</v>
+      </c>
+      <c r="S36" s="19">
+        <f>R36+I36/2-1</f>
+        <v>1939771</v>
+      </c>
+      <c r="T36" s="18">
+        <f>U36/E36</f>
+        <v>43264</v>
+      </c>
+      <c r="U36" s="4">
+        <f>D36*I36</f>
+        <v>2076672</v>
+      </c>
+      <c r="V36" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M36" s="4">
-        <v>1</v>
-      </c>
-      <c r="N36" s="4">
+      <c r="W36" s="4">
+        <v>1</v>
+      </c>
+      <c r="X36" s="4">
         <f>0.0000032*J36+0.0000064*I36</f>
         <v>9.1238399999999997E-2</v>
       </c>
-      <c r="O36" s="4">
-        <f>K36*L36</f>
-        <v>860.16000000000008</v>
-      </c>
-      <c r="P36" s="4">
-        <f>K36*L36*M36</f>
-        <v>860.16000000000008</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Y36" s="4">
+        <f>U36*V36</f>
+        <v>145367.04000000001</v>
+      </c>
+      <c r="Z36" s="4">
+        <f>T36*V36*W36</f>
+        <v>3028.4800000000005</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>38</v>
       </c>
@@ -2179,14 +3014,24 @@
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
-      <c r="N37" s="5"/>
-      <c r="O37" s="5"/>
-      <c r="P37" s="5"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K37" s="11"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="20"/>
+      <c r="N37" s="20"/>
+      <c r="O37" s="20"/>
+      <c r="P37" s="20"/>
+      <c r="Q37" s="20"/>
+      <c r="R37" s="20"/>
+      <c r="S37" s="21"/>
+      <c r="T37" s="20"/>
+      <c r="U37" s="5"/>
+      <c r="V37" s="5"/>
+      <c r="W37" s="5"/>
+      <c r="X37" s="5"/>
+      <c r="Y37" s="5"/>
+      <c r="Z37" s="5"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>39</v>
       </c>
@@ -2217,30 +3062,61 @@
       <c r="J38" s="4">
         <v>9216</v>
       </c>
-      <c r="K38" s="4">
-        <f t="shared" ref="K38:K39" si="16">D38*E38</f>
-        <v>9216</v>
-      </c>
-      <c r="L38" s="4">
+      <c r="K38" s="10"/>
+      <c r="L38" s="18">
+        <f>L36+J36/2+E36/2</f>
+        <v>70472</v>
+      </c>
+      <c r="M38" s="18">
+        <f t="shared" ref="M38:M39" si="16">L38+J38/2-1</f>
+        <v>75079</v>
+      </c>
+      <c r="N38" s="18">
+        <f>M38+1</f>
+        <v>75080</v>
+      </c>
+      <c r="O38" s="18">
+        <f>N38+E38/2-1</f>
+        <v>75175</v>
+      </c>
+      <c r="P38" s="18"/>
+      <c r="Q38" s="18"/>
+      <c r="R38" s="18">
+        <f>S36+1</f>
+        <v>1939772</v>
+      </c>
+      <c r="S38" s="19">
+        <f>R38+I38/2-1</f>
+        <v>1955995</v>
+      </c>
+      <c r="T38" s="18">
+        <f>U38/E38</f>
+        <v>8112</v>
+      </c>
+      <c r="U38" s="4">
+        <f>D38*I38</f>
+        <v>1557504</v>
+      </c>
+      <c r="V38" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M38" s="4">
+      <c r="W38" s="4">
         <v>0</v>
       </c>
-      <c r="N38" s="4">
-        <f t="shared" ref="N38:N39" si="17">0.0000032*J38+0.0000064*I38</f>
+      <c r="X38" s="4">
+        <f>0.0000032*J38+0.0000064*I38</f>
         <v>0.23715839999999999</v>
       </c>
-      <c r="O38" s="4">
-        <f t="shared" ref="O38:O39" si="18">K38*L38</f>
-        <v>645.12000000000012</v>
-      </c>
-      <c r="P38" s="4">
-        <f t="shared" ref="P38:P39" si="19">K38*L38*M38</f>
+      <c r="Y38" s="4">
+        <f t="shared" ref="Y38:Y39" si="17">U38*V38</f>
+        <v>109025.28000000001</v>
+      </c>
+      <c r="Z38" s="4">
+        <f t="shared" ref="Z38:Z39" si="18">T38*V38*W38</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>40</v>
       </c>
@@ -2271,30 +3147,61 @@
       <c r="J39" s="4">
         <v>82944</v>
       </c>
-      <c r="K39" s="4">
+      <c r="K39" s="10"/>
+      <c r="L39" s="18">
+        <f>L38+J38/2+E38/2</f>
+        <v>75176</v>
+      </c>
+      <c r="M39" s="18">
         <f t="shared" si="16"/>
-        <v>9216</v>
-      </c>
-      <c r="L39" s="4">
+        <v>116647</v>
+      </c>
+      <c r="N39" s="18">
+        <f>M39+1</f>
+        <v>116648</v>
+      </c>
+      <c r="O39" s="18">
+        <f>N39+E39/2-1</f>
+        <v>116743</v>
+      </c>
+      <c r="P39" s="18"/>
+      <c r="Q39" s="18"/>
+      <c r="R39" s="18">
+        <f>S38+1</f>
+        <v>1955996</v>
+      </c>
+      <c r="S39" s="19">
+        <f>R39+I39/2-1</f>
+        <v>1972219</v>
+      </c>
+      <c r="T39" s="18">
+        <f>U39/E39</f>
+        <v>8112</v>
+      </c>
+      <c r="U39" s="4">
+        <f>D39*I39</f>
+        <v>1557504</v>
+      </c>
+      <c r="V39" s="4">
         <v>0.52</v>
       </c>
-      <c r="M39" s="4">
-        <v>1</v>
-      </c>
-      <c r="N39" s="4">
+      <c r="W39" s="4">
+        <v>1</v>
+      </c>
+      <c r="X39" s="4">
+        <f>0.0000032*J39+0.0000064*I39</f>
+        <v>0.47308800000000001</v>
+      </c>
+      <c r="Y39" s="4">
         <f t="shared" si="17"/>
-        <v>0.47308800000000001</v>
-      </c>
-      <c r="O39" s="4">
+        <v>809902.08000000007</v>
+      </c>
+      <c r="Z39" s="4">
         <f t="shared" si="18"/>
-        <v>4792.32</v>
-      </c>
-      <c r="P39" s="4">
-        <f t="shared" si="19"/>
-        <v>4792.32</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+        <v>4218.24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>41</v>
       </c>
@@ -2309,14 +3216,24 @@
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
-      <c r="K40" s="5"/>
-      <c r="L40" s="5"/>
-      <c r="M40" s="5"/>
-      <c r="N40" s="5"/>
-      <c r="O40" s="5"/>
-      <c r="P40" s="5"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K40" s="11"/>
+      <c r="L40" s="20"/>
+      <c r="M40" s="20"/>
+      <c r="N40" s="20"/>
+      <c r="O40" s="20"/>
+      <c r="P40" s="20"/>
+      <c r="Q40" s="20"/>
+      <c r="R40" s="20"/>
+      <c r="S40" s="21"/>
+      <c r="T40" s="20"/>
+      <c r="U40" s="5"/>
+      <c r="V40" s="5"/>
+      <c r="W40" s="5"/>
+      <c r="X40" s="5"/>
+      <c r="Y40" s="5"/>
+      <c r="Z40" s="5"/>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>42</v>
       </c>
@@ -2331,14 +3248,24 @@
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
-      <c r="L41" s="5"/>
-      <c r="M41" s="5"/>
-      <c r="N41" s="5"/>
-      <c r="O41" s="5"/>
-      <c r="P41" s="5"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K41" s="11"/>
+      <c r="L41" s="20"/>
+      <c r="M41" s="20"/>
+      <c r="N41" s="20"/>
+      <c r="O41" s="20"/>
+      <c r="P41" s="20"/>
+      <c r="Q41" s="20"/>
+      <c r="R41" s="20"/>
+      <c r="S41" s="21"/>
+      <c r="T41" s="20"/>
+      <c r="U41" s="5"/>
+      <c r="V41" s="5"/>
+      <c r="W41" s="5"/>
+      <c r="X41" s="5"/>
+      <c r="Y41" s="5"/>
+      <c r="Z41" s="5"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>43</v>
       </c>
@@ -2355,14 +3282,24 @@
       </c>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
-      <c r="O42" s="3"/>
-      <c r="P42" s="3"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K42" s="9"/>
+      <c r="L42" s="16"/>
+      <c r="M42" s="16"/>
+      <c r="N42" s="16"/>
+      <c r="O42" s="16"/>
+      <c r="P42" s="16"/>
+      <c r="Q42" s="16"/>
+      <c r="R42" s="16"/>
+      <c r="S42" s="17"/>
+      <c r="T42" s="16"/>
+      <c r="U42" s="3"/>
+      <c r="V42" s="3"/>
+      <c r="W42" s="3"/>
+      <c r="X42" s="3"/>
+      <c r="Y42" s="3"/>
+      <c r="Z42" s="3"/>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>44</v>
       </c>
@@ -2393,30 +3330,61 @@
       <c r="J43" s="4">
         <v>18432</v>
       </c>
-      <c r="K43" s="4">
-        <f>D43*E43</f>
-        <v>18432</v>
-      </c>
-      <c r="L43" s="4">
+      <c r="K43" s="10"/>
+      <c r="L43" s="18">
+        <f>L39+J39/2+E39/2</f>
+        <v>116744</v>
+      </c>
+      <c r="M43" s="18">
+        <f>L43+J43/2-1</f>
+        <v>125959</v>
+      </c>
+      <c r="N43" s="18">
+        <f>M43+1</f>
+        <v>125960</v>
+      </c>
+      <c r="O43" s="18">
+        <f>N43+E43/2-1</f>
+        <v>125983</v>
+      </c>
+      <c r="P43" s="18"/>
+      <c r="Q43" s="18"/>
+      <c r="R43" s="18">
+        <f>S39+1</f>
+        <v>1972220</v>
+      </c>
+      <c r="S43" s="19">
+        <f>R43+I43/2-1</f>
+        <v>1976275</v>
+      </c>
+      <c r="T43" s="18">
+        <f>U43/E43</f>
+        <v>64896</v>
+      </c>
+      <c r="U43" s="4">
+        <f>D43*I43</f>
+        <v>3115008</v>
+      </c>
+      <c r="V43" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M43" s="4">
-        <v>1</v>
-      </c>
-      <c r="N43" s="4">
+      <c r="W43" s="4">
+        <v>1</v>
+      </c>
+      <c r="X43" s="4">
         <f>0.0000032*J43+0.0000064*I43</f>
         <v>0.1108992</v>
       </c>
-      <c r="O43" s="4">
-        <f>K43*L43</f>
-        <v>1290.2400000000002</v>
-      </c>
-      <c r="P43" s="4">
-        <f>K43*L43*M43</f>
-        <v>1290.2400000000002</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Y43" s="4">
+        <f>U43*V43</f>
+        <v>218050.56000000003</v>
+      </c>
+      <c r="Z43" s="4">
+        <f>T43*V43*W43</f>
+        <v>4542.72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>45</v>
       </c>
@@ -2431,14 +3399,24 @@
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
-      <c r="K44" s="5"/>
-      <c r="L44" s="5"/>
-      <c r="M44" s="5"/>
-      <c r="N44" s="5"/>
-      <c r="O44" s="5"/>
-      <c r="P44" s="5"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K44" s="11"/>
+      <c r="L44" s="20"/>
+      <c r="M44" s="20"/>
+      <c r="N44" s="20"/>
+      <c r="O44" s="20"/>
+      <c r="P44" s="20"/>
+      <c r="Q44" s="20"/>
+      <c r="R44" s="20"/>
+      <c r="S44" s="21"/>
+      <c r="T44" s="20"/>
+      <c r="U44" s="5"/>
+      <c r="V44" s="5"/>
+      <c r="W44" s="5"/>
+      <c r="X44" s="5"/>
+      <c r="Y44" s="5"/>
+      <c r="Z44" s="5"/>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>46</v>
       </c>
@@ -2469,30 +3447,61 @@
       <c r="J45" s="4">
         <v>9216</v>
       </c>
-      <c r="K45" s="4">
-        <f t="shared" ref="K45:K46" si="20">D45*E45</f>
-        <v>9216</v>
-      </c>
-      <c r="L45" s="4">
+      <c r="K45" s="10"/>
+      <c r="L45" s="18">
+        <f>L43+J43/2+E43/2</f>
+        <v>125984</v>
+      </c>
+      <c r="M45" s="18">
+        <f t="shared" ref="M45:M46" si="19">L45+J45/2-1</f>
+        <v>130591</v>
+      </c>
+      <c r="N45" s="18">
+        <f t="shared" ref="N45:N46" si="20">M45+1</f>
+        <v>130592</v>
+      </c>
+      <c r="O45" s="18">
+        <f>N45+E45/2-1</f>
+        <v>130687</v>
+      </c>
+      <c r="P45" s="18"/>
+      <c r="Q45" s="18"/>
+      <c r="R45" s="18">
+        <f>S43+1</f>
+        <v>1976276</v>
+      </c>
+      <c r="S45" s="19">
+        <f>R45+I45/2-1</f>
+        <v>1992499</v>
+      </c>
+      <c r="T45" s="18">
+        <f>U45/E45</f>
+        <v>8112</v>
+      </c>
+      <c r="U45" s="4">
+        <f>D45*I45</f>
+        <v>1557504</v>
+      </c>
+      <c r="V45" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M45" s="4">
+      <c r="W45" s="4">
         <v>0</v>
       </c>
-      <c r="N45" s="4">
-        <f t="shared" ref="N45:N46" si="21">0.0000032*J45+0.0000064*I45</f>
+      <c r="X45" s="4">
+        <f>0.0000032*J45+0.0000064*I45</f>
         <v>0.23715839999999999</v>
       </c>
-      <c r="O45" s="4">
-        <f t="shared" ref="O45:O46" si="22">K45*L45</f>
-        <v>645.12000000000012</v>
-      </c>
-      <c r="P45" s="4">
-        <f t="shared" ref="P45:P46" si="23">K45*L45*M45</f>
+      <c r="Y45" s="4">
+        <f t="shared" ref="Y45:Y46" si="21">U45*V45</f>
+        <v>109025.28000000001</v>
+      </c>
+      <c r="Z45" s="4">
+        <f t="shared" ref="Z45:Z46" si="22">T45*V45*W45</f>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>47</v>
       </c>
@@ -2523,30 +3532,61 @@
       <c r="J46" s="4">
         <v>82944</v>
       </c>
-      <c r="K46" s="4">
+      <c r="K46" s="10"/>
+      <c r="L46" s="18">
+        <f>L45+J45/2+E45/2</f>
+        <v>130688</v>
+      </c>
+      <c r="M46" s="18">
+        <f t="shared" si="19"/>
+        <v>172159</v>
+      </c>
+      <c r="N46" s="18">
         <f t="shared" si="20"/>
-        <v>9216</v>
-      </c>
-      <c r="L46" s="4">
+        <v>172160</v>
+      </c>
+      <c r="O46" s="18">
+        <f>N46+E46/2-1</f>
+        <v>172255</v>
+      </c>
+      <c r="P46" s="18"/>
+      <c r="Q46" s="18"/>
+      <c r="R46" s="18">
+        <f>S45+1</f>
+        <v>1992500</v>
+      </c>
+      <c r="S46" s="19">
+        <f>R46+I46/2-1</f>
+        <v>2008723</v>
+      </c>
+      <c r="T46" s="18">
+        <f>U46/E46</f>
+        <v>8112</v>
+      </c>
+      <c r="U46" s="4">
+        <f>D46*I46</f>
+        <v>1557504</v>
+      </c>
+      <c r="V46" s="4">
         <v>0.52</v>
       </c>
-      <c r="M46" s="4">
-        <v>1</v>
-      </c>
-      <c r="N46" s="4">
+      <c r="W46" s="4">
+        <v>1</v>
+      </c>
+      <c r="X46" s="4">
+        <f>0.0000032*J46+0.0000064*I46</f>
+        <v>0.47308800000000001</v>
+      </c>
+      <c r="Y46" s="4">
         <f t="shared" si="21"/>
-        <v>0.47308800000000001</v>
-      </c>
-      <c r="O46" s="4">
+        <v>809902.08000000007</v>
+      </c>
+      <c r="Z46" s="4">
         <f t="shared" si="22"/>
-        <v>4792.32</v>
-      </c>
-      <c r="P46" s="4">
-        <f t="shared" si="23"/>
-        <v>4792.32</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+        <v>4218.24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>48</v>
       </c>
@@ -2561,14 +3601,24 @@
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5"/>
-      <c r="M47" s="5"/>
-      <c r="N47" s="5"/>
-      <c r="O47" s="5"/>
-      <c r="P47" s="5"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K47" s="11"/>
+      <c r="L47" s="20"/>
+      <c r="M47" s="20"/>
+      <c r="N47" s="20"/>
+      <c r="O47" s="20"/>
+      <c r="P47" s="20"/>
+      <c r="Q47" s="20"/>
+      <c r="R47" s="20"/>
+      <c r="S47" s="21"/>
+      <c r="T47" s="20"/>
+      <c r="U47" s="5"/>
+      <c r="V47" s="5"/>
+      <c r="W47" s="5"/>
+      <c r="X47" s="5"/>
+      <c r="Y47" s="5"/>
+      <c r="Z47" s="5"/>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>49</v>
       </c>
@@ -2583,14 +3633,24 @@
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
-      <c r="K48" s="5"/>
-      <c r="L48" s="5"/>
-      <c r="M48" s="5"/>
-      <c r="N48" s="5"/>
-      <c r="O48" s="5"/>
-      <c r="P48" s="5"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K48" s="11"/>
+      <c r="L48" s="20"/>
+      <c r="M48" s="20"/>
+      <c r="N48" s="20"/>
+      <c r="O48" s="20"/>
+      <c r="P48" s="20"/>
+      <c r="Q48" s="20"/>
+      <c r="R48" s="20"/>
+      <c r="S48" s="21"/>
+      <c r="T48" s="20"/>
+      <c r="U48" s="5"/>
+      <c r="V48" s="5"/>
+      <c r="W48" s="5"/>
+      <c r="X48" s="5"/>
+      <c r="Y48" s="5"/>
+      <c r="Z48" s="5"/>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>50</v>
       </c>
@@ -2607,14 +3667,24 @@
       </c>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
-      <c r="N49" s="3"/>
-      <c r="O49" s="3"/>
-      <c r="P49" s="3"/>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K49" s="9"/>
+      <c r="L49" s="16"/>
+      <c r="M49" s="16"/>
+      <c r="N49" s="16"/>
+      <c r="O49" s="16"/>
+      <c r="P49" s="16"/>
+      <c r="Q49" s="16"/>
+      <c r="R49" s="16"/>
+      <c r="S49" s="17"/>
+      <c r="T49" s="16"/>
+      <c r="U49" s="3"/>
+      <c r="V49" s="3"/>
+      <c r="W49" s="3"/>
+      <c r="X49" s="3"/>
+      <c r="Y49" s="3"/>
+      <c r="Z49" s="3"/>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>51</v>
       </c>
@@ -2645,30 +3715,61 @@
       <c r="J50" s="4">
         <v>24576</v>
       </c>
-      <c r="K50" s="4">
-        <f>D50*E50</f>
-        <v>24576</v>
-      </c>
-      <c r="L50" s="4">
+      <c r="K50" s="10"/>
+      <c r="L50" s="18">
+        <f>L46+J46/2+E46/2</f>
+        <v>172256</v>
+      </c>
+      <c r="M50" s="18">
+        <f>L50+J50/2-1</f>
+        <v>184543</v>
+      </c>
+      <c r="N50" s="18">
+        <f>M50+1</f>
+        <v>184544</v>
+      </c>
+      <c r="O50" s="18">
+        <f>N50+E50/2-1</f>
+        <v>184575</v>
+      </c>
+      <c r="P50" s="18"/>
+      <c r="Q50" s="18"/>
+      <c r="R50" s="18">
+        <f>S46+1</f>
+        <v>2008724</v>
+      </c>
+      <c r="S50" s="19">
+        <f>R50+I50/2-1</f>
+        <v>2014131</v>
+      </c>
+      <c r="T50" s="18">
+        <f>U50/E50</f>
+        <v>64896</v>
+      </c>
+      <c r="U50" s="4">
+        <f>D50*I50</f>
+        <v>4153344</v>
+      </c>
+      <c r="V50" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M50" s="4">
-        <v>1</v>
-      </c>
-      <c r="N50" s="4">
+      <c r="W50" s="4">
+        <v>1</v>
+      </c>
+      <c r="X50" s="4">
         <f>0.0000032*J50+0.0000064*I50</f>
         <v>0.14786559999999999</v>
       </c>
-      <c r="O50" s="4">
-        <f>K50*L50</f>
-        <v>1720.3200000000002</v>
-      </c>
-      <c r="P50" s="4">
-        <f>K50*L50*M50</f>
-        <v>1720.3200000000002</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Y50" s="4">
+        <f>U50*V50</f>
+        <v>290734.08000000002</v>
+      </c>
+      <c r="Z50" s="4">
+        <f>T50*V50*W50</f>
+        <v>4542.72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>52</v>
       </c>
@@ -2683,14 +3784,24 @@
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
-      <c r="K51" s="5"/>
-      <c r="L51" s="5"/>
-      <c r="M51" s="5"/>
-      <c r="N51" s="5"/>
-      <c r="O51" s="5"/>
-      <c r="P51" s="5"/>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K51" s="11"/>
+      <c r="L51" s="20"/>
+      <c r="M51" s="20"/>
+      <c r="N51" s="20"/>
+      <c r="O51" s="20"/>
+      <c r="P51" s="20"/>
+      <c r="Q51" s="20"/>
+      <c r="R51" s="20"/>
+      <c r="S51" s="21"/>
+      <c r="T51" s="20"/>
+      <c r="U51" s="5"/>
+      <c r="V51" s="5"/>
+      <c r="W51" s="5"/>
+      <c r="X51" s="5"/>
+      <c r="Y51" s="5"/>
+      <c r="Z51" s="5"/>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>53</v>
       </c>
@@ -2721,30 +3832,61 @@
       <c r="J52" s="4">
         <v>16384</v>
       </c>
-      <c r="K52" s="4">
-        <f t="shared" ref="K52:K53" si="24">D52*E52</f>
-        <v>16384</v>
-      </c>
-      <c r="L52" s="4">
+      <c r="K52" s="10"/>
+      <c r="L52" s="18">
+        <f>L50+J50/2+E50/2</f>
+        <v>184576</v>
+      </c>
+      <c r="M52" s="18">
+        <f t="shared" ref="M52:M53" si="23">L52+J52/2-1</f>
+        <v>192767</v>
+      </c>
+      <c r="N52" s="18">
+        <f t="shared" ref="N52:N53" si="24">M52+1</f>
+        <v>192768</v>
+      </c>
+      <c r="O52" s="18">
+        <f>N52+E52/2-1</f>
+        <v>192895</v>
+      </c>
+      <c r="P52" s="18"/>
+      <c r="Q52" s="18"/>
+      <c r="R52" s="18">
+        <f>S50+1</f>
+        <v>2014132</v>
+      </c>
+      <c r="S52" s="19">
+        <f>R52+I52/2-1</f>
+        <v>2035763</v>
+      </c>
+      <c r="T52" s="18">
+        <f>U52/E52</f>
+        <v>10816</v>
+      </c>
+      <c r="U52" s="4">
+        <f>D52*I52</f>
+        <v>2768896</v>
+      </c>
+      <c r="V52" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M52" s="4">
+      <c r="W52" s="4">
         <v>0</v>
       </c>
-      <c r="N52" s="4">
-        <f t="shared" ref="N52:N53" si="25">0.0000032*J52+0.0000064*I52</f>
+      <c r="X52" s="4">
+        <f>0.0000032*J52+0.0000064*I52</f>
         <v>0.32931840000000001</v>
       </c>
-      <c r="O52" s="4">
-        <f t="shared" ref="O52:O53" si="26">K52*L52</f>
-        <v>1146.8800000000001</v>
-      </c>
-      <c r="P52" s="4">
-        <f t="shared" ref="P52:P53" si="27">K52*L52*M52</f>
+      <c r="Y52" s="4">
+        <f t="shared" ref="Y52:Y53" si="25">U52*V52</f>
+        <v>193822.72000000003</v>
+      </c>
+      <c r="Z52" s="4">
+        <f t="shared" ref="Z52:Z53" si="26">T52*V52*W52</f>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>54</v>
       </c>
@@ -2775,30 +3917,61 @@
       <c r="J53" s="4">
         <v>147456</v>
       </c>
-      <c r="K53" s="4">
+      <c r="K53" s="10"/>
+      <c r="L53" s="18">
+        <f>L52+J52/2+E52/2</f>
+        <v>192896</v>
+      </c>
+      <c r="M53" s="18">
+        <f t="shared" si="23"/>
+        <v>266623</v>
+      </c>
+      <c r="N53" s="18">
         <f t="shared" si="24"/>
-        <v>16384</v>
-      </c>
-      <c r="L53" s="4">
+        <v>266624</v>
+      </c>
+      <c r="O53" s="18">
+        <f>N53+E53/2-1</f>
+        <v>266751</v>
+      </c>
+      <c r="P53" s="18"/>
+      <c r="Q53" s="18"/>
+      <c r="R53" s="18">
+        <f>S52+1</f>
+        <v>2035764</v>
+      </c>
+      <c r="S53" s="19">
+        <f>R53+I53/2-1</f>
+        <v>2057395</v>
+      </c>
+      <c r="T53" s="18">
+        <f>U53/E52</f>
+        <v>10816</v>
+      </c>
+      <c r="U53" s="4">
+        <f>D53*I53</f>
+        <v>2768896</v>
+      </c>
+      <c r="V53" s="4">
         <v>0.52</v>
       </c>
-      <c r="M53" s="4">
-        <v>1</v>
-      </c>
-      <c r="N53" s="4">
+      <c r="W53" s="4">
+        <v>1</v>
+      </c>
+      <c r="X53" s="4">
+        <f>0.0000032*J53+0.0000064*I53</f>
+        <v>0.74874879999999999</v>
+      </c>
+      <c r="Y53" s="4">
         <f t="shared" si="25"/>
-        <v>0.74874879999999999</v>
-      </c>
-      <c r="O53" s="4">
+        <v>1439825.9200000002</v>
+      </c>
+      <c r="Z53" s="4">
         <f t="shared" si="26"/>
-        <v>8519.68</v>
-      </c>
-      <c r="P53" s="4">
-        <f t="shared" si="27"/>
-        <v>8519.68</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+        <v>5624.3200000000006</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>55</v>
       </c>
@@ -2813,14 +3986,24 @@
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
-      <c r="K54" s="5"/>
-      <c r="L54" s="5"/>
-      <c r="M54" s="5"/>
-      <c r="N54" s="5"/>
-      <c r="O54" s="5"/>
-      <c r="P54" s="5"/>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K54" s="11"/>
+      <c r="L54" s="20"/>
+      <c r="M54" s="20"/>
+      <c r="N54" s="20"/>
+      <c r="O54" s="20"/>
+      <c r="P54" s="20"/>
+      <c r="Q54" s="20"/>
+      <c r="R54" s="20"/>
+      <c r="S54" s="21"/>
+      <c r="T54" s="20"/>
+      <c r="U54" s="5"/>
+      <c r="V54" s="5"/>
+      <c r="W54" s="5"/>
+      <c r="X54" s="5"/>
+      <c r="Y54" s="5"/>
+      <c r="Z54" s="5"/>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>56</v>
       </c>
@@ -2835,14 +4018,24 @@
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
-      <c r="K55" s="5"/>
-      <c r="L55" s="5"/>
-      <c r="M55" s="5"/>
-      <c r="N55" s="5"/>
-      <c r="O55" s="5"/>
-      <c r="P55" s="5"/>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K55" s="11"/>
+      <c r="L55" s="20"/>
+      <c r="M55" s="20"/>
+      <c r="N55" s="20"/>
+      <c r="O55" s="20"/>
+      <c r="P55" s="20"/>
+      <c r="Q55" s="20"/>
+      <c r="R55" s="20"/>
+      <c r="S55" s="21"/>
+      <c r="T55" s="20"/>
+      <c r="U55" s="5"/>
+      <c r="V55" s="5"/>
+      <c r="W55" s="5"/>
+      <c r="X55" s="5"/>
+      <c r="Y55" s="5"/>
+      <c r="Z55" s="5"/>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>57</v>
       </c>
@@ -2859,14 +4052,24 @@
       </c>
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
-      <c r="K56" s="3"/>
-      <c r="L56" s="3"/>
-      <c r="M56" s="3"/>
-      <c r="N56" s="3"/>
-      <c r="O56" s="3"/>
-      <c r="P56" s="3"/>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K56" s="9"/>
+      <c r="L56" s="16"/>
+      <c r="M56" s="16"/>
+      <c r="N56" s="16"/>
+      <c r="O56" s="16"/>
+      <c r="P56" s="16"/>
+      <c r="Q56" s="16"/>
+      <c r="R56" s="16"/>
+      <c r="S56" s="17"/>
+      <c r="T56" s="16"/>
+      <c r="U56" s="3"/>
+      <c r="V56" s="3"/>
+      <c r="W56" s="3"/>
+      <c r="X56" s="3"/>
+      <c r="Y56" s="3"/>
+      <c r="Z56" s="3"/>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>58</v>
       </c>
@@ -2897,30 +4100,61 @@
       <c r="J57" s="4">
         <v>32768</v>
       </c>
-      <c r="K57" s="4">
-        <f>D57*E57</f>
-        <v>32768</v>
-      </c>
-      <c r="L57" s="4">
+      <c r="K57" s="10"/>
+      <c r="L57" s="18">
+        <f>L53+J53/2+E53/2</f>
+        <v>266752</v>
+      </c>
+      <c r="M57" s="18">
+        <f>L57+J57/2-1</f>
+        <v>283135</v>
+      </c>
+      <c r="N57" s="18">
+        <f>M57+1</f>
+        <v>283136</v>
+      </c>
+      <c r="O57" s="18">
+        <f>N57+E57/2-1</f>
+        <v>283167</v>
+      </c>
+      <c r="P57" s="18"/>
+      <c r="Q57" s="18"/>
+      <c r="R57" s="18">
+        <f>S53+1</f>
+        <v>2057396</v>
+      </c>
+      <c r="S57" s="19">
+        <f>R57+I57/2-1</f>
+        <v>2062803</v>
+      </c>
+      <c r="T57" s="18">
+        <f>U57/E57</f>
+        <v>86528</v>
+      </c>
+      <c r="U57" s="4">
+        <f>D57*I57</f>
+        <v>5537792</v>
+      </c>
+      <c r="V57" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M57" s="4">
-        <v>1</v>
-      </c>
-      <c r="N57" s="4">
+      <c r="W57" s="4">
+        <v>1</v>
+      </c>
+      <c r="X57" s="4">
         <f>0.0000032*J57+0.0000064*I57</f>
         <v>0.17408000000000001</v>
       </c>
-      <c r="O57" s="4">
-        <f>K57*L57</f>
-        <v>2293.7600000000002</v>
-      </c>
-      <c r="P57" s="4">
-        <f>K57*L57*M57</f>
-        <v>2293.7600000000002</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Y57" s="4">
+        <f>U57*V57</f>
+        <v>387645.44000000006</v>
+      </c>
+      <c r="Z57" s="4">
+        <f>T57*V57*W57</f>
+        <v>6056.9600000000009</v>
+      </c>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>59</v>
       </c>
@@ -2935,14 +4169,24 @@
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
       <c r="J58" s="5"/>
-      <c r="K58" s="5"/>
-      <c r="L58" s="5"/>
-      <c r="M58" s="5"/>
-      <c r="N58" s="5"/>
-      <c r="O58" s="5"/>
-      <c r="P58" s="5"/>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K58" s="11"/>
+      <c r="L58" s="20"/>
+      <c r="M58" s="20"/>
+      <c r="N58" s="20"/>
+      <c r="O58" s="20"/>
+      <c r="P58" s="20"/>
+      <c r="Q58" s="20"/>
+      <c r="R58" s="20"/>
+      <c r="S58" s="21"/>
+      <c r="T58" s="20"/>
+      <c r="U58" s="5"/>
+      <c r="V58" s="5"/>
+      <c r="W58" s="5"/>
+      <c r="X58" s="5"/>
+      <c r="Y58" s="5"/>
+      <c r="Z58" s="5"/>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>60</v>
       </c>
@@ -2973,30 +4217,61 @@
       <c r="J59" s="4">
         <v>16384</v>
       </c>
-      <c r="K59" s="4">
-        <f t="shared" ref="K59:K60" si="28">D59*E59</f>
-        <v>16384</v>
-      </c>
-      <c r="L59" s="4">
+      <c r="K59" s="10"/>
+      <c r="L59" s="18">
+        <f>L57+J57/2+E57/2</f>
+        <v>283168</v>
+      </c>
+      <c r="M59" s="18">
+        <f t="shared" ref="M59:M60" si="27">L59+J59/2-1</f>
+        <v>291359</v>
+      </c>
+      <c r="N59" s="18">
+        <f t="shared" ref="N59:N60" si="28">M59+1</f>
+        <v>291360</v>
+      </c>
+      <c r="O59" s="18">
+        <f>N59+E59/2-1</f>
+        <v>291487</v>
+      </c>
+      <c r="P59" s="18"/>
+      <c r="Q59" s="18"/>
+      <c r="R59" s="18">
+        <f>S57+1</f>
+        <v>2062804</v>
+      </c>
+      <c r="S59" s="19">
+        <f>R59+I59/2-1</f>
+        <v>2084435</v>
+      </c>
+      <c r="T59" s="18">
+        <f>U59/E59</f>
+        <v>10816</v>
+      </c>
+      <c r="U59" s="4">
+        <f>D59*I59</f>
+        <v>2768896</v>
+      </c>
+      <c r="V59" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M59" s="4">
+      <c r="W59" s="4">
         <v>0</v>
       </c>
-      <c r="N59" s="4">
-        <f t="shared" ref="N59:N60" si="29">0.0000032*J59+0.0000064*I59</f>
+      <c r="X59" s="4">
+        <f>0.0000032*J59+0.0000064*I59</f>
         <v>0.32931840000000001</v>
       </c>
-      <c r="O59" s="4">
-        <f t="shared" ref="O59:O60" si="30">K59*L59</f>
-        <v>1146.8800000000001</v>
-      </c>
-      <c r="P59" s="4">
-        <f t="shared" ref="P59:P60" si="31">K59*L59*M59</f>
+      <c r="Y59" s="4">
+        <f t="shared" ref="Y59:Y60" si="29">U59*V59</f>
+        <v>193822.72000000003</v>
+      </c>
+      <c r="Z59" s="4">
+        <f t="shared" ref="Z59:Z60" si="30">T59*V59*W59</f>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>61</v>
       </c>
@@ -3027,30 +4302,61 @@
       <c r="J60" s="4">
         <v>147456</v>
       </c>
-      <c r="K60" s="4">
+      <c r="K60" s="10"/>
+      <c r="L60" s="18">
+        <f>L59+J59/2+E59/2</f>
+        <v>291488</v>
+      </c>
+      <c r="M60" s="18">
+        <f t="shared" si="27"/>
+        <v>365215</v>
+      </c>
+      <c r="N60" s="18">
         <f t="shared" si="28"/>
-        <v>16384</v>
-      </c>
-      <c r="L60" s="4">
+        <v>365216</v>
+      </c>
+      <c r="O60" s="18">
+        <f>N60+E60/2-1</f>
+        <v>365343</v>
+      </c>
+      <c r="P60" s="18"/>
+      <c r="Q60" s="18"/>
+      <c r="R60" s="18">
+        <f>S59+1</f>
+        <v>2084436</v>
+      </c>
+      <c r="S60" s="19">
+        <f>R60+I60/2-1</f>
+        <v>2106067</v>
+      </c>
+      <c r="T60" s="18">
+        <f>U60/E60</f>
+        <v>10816</v>
+      </c>
+      <c r="U60" s="4">
+        <f>D60*I60</f>
+        <v>2768896</v>
+      </c>
+      <c r="V60" s="4">
         <v>0.52</v>
       </c>
-      <c r="M60" s="4">
-        <v>1</v>
-      </c>
-      <c r="N60" s="4">
+      <c r="W60" s="4">
+        <v>1</v>
+      </c>
+      <c r="X60" s="4">
+        <f>0.0000032*J60+0.0000064*I60</f>
+        <v>0.74874879999999999</v>
+      </c>
+      <c r="Y60" s="4">
         <f t="shared" si="29"/>
-        <v>0.74874879999999999</v>
-      </c>
-      <c r="O60" s="4">
+        <v>1439825.9200000002</v>
+      </c>
+      <c r="Z60" s="4">
         <f t="shared" si="30"/>
-        <v>8519.68</v>
-      </c>
-      <c r="P60" s="4">
-        <f t="shared" si="31"/>
-        <v>8519.68</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+        <v>5624.3200000000006</v>
+      </c>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>62</v>
       </c>
@@ -3065,14 +4371,24 @@
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
-      <c r="K61" s="5"/>
-      <c r="L61" s="5"/>
-      <c r="M61" s="5"/>
-      <c r="N61" s="5"/>
-      <c r="O61" s="5"/>
-      <c r="P61" s="5"/>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K61" s="11"/>
+      <c r="L61" s="20"/>
+      <c r="M61" s="20"/>
+      <c r="N61" s="20"/>
+      <c r="O61" s="20"/>
+      <c r="P61" s="20"/>
+      <c r="Q61" s="20"/>
+      <c r="R61" s="20"/>
+      <c r="S61" s="21"/>
+      <c r="T61" s="20"/>
+      <c r="U61" s="5"/>
+      <c r="V61" s="5"/>
+      <c r="W61" s="5"/>
+      <c r="X61" s="5"/>
+      <c r="Y61" s="5"/>
+      <c r="Z61" s="5"/>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>63</v>
       </c>
@@ -3087,14 +4403,24 @@
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
       <c r="J62" s="5"/>
-      <c r="K62" s="5"/>
-      <c r="L62" s="5"/>
-      <c r="M62" s="5"/>
-      <c r="N62" s="5"/>
-      <c r="O62" s="5"/>
-      <c r="P62" s="5"/>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K62" s="11"/>
+      <c r="L62" s="20"/>
+      <c r="M62" s="20"/>
+      <c r="N62" s="20"/>
+      <c r="O62" s="20"/>
+      <c r="P62" s="20"/>
+      <c r="Q62" s="20"/>
+      <c r="R62" s="20"/>
+      <c r="S62" s="21"/>
+      <c r="T62" s="20"/>
+      <c r="U62" s="5"/>
+      <c r="V62" s="5"/>
+      <c r="W62" s="5"/>
+      <c r="X62" s="5"/>
+      <c r="Y62" s="5"/>
+      <c r="Z62" s="5"/>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>64</v>
       </c>
@@ -3111,14 +4437,24 @@
       </c>
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
-      <c r="K63" s="3"/>
-      <c r="L63" s="3"/>
-      <c r="M63" s="3"/>
-      <c r="N63" s="3"/>
-      <c r="O63" s="3"/>
-      <c r="P63" s="3"/>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K63" s="9"/>
+      <c r="L63" s="16"/>
+      <c r="M63" s="16"/>
+      <c r="N63" s="16"/>
+      <c r="O63" s="16"/>
+      <c r="P63" s="16"/>
+      <c r="Q63" s="16"/>
+      <c r="R63" s="16"/>
+      <c r="S63" s="17"/>
+      <c r="T63" s="16"/>
+      <c r="U63" s="3"/>
+      <c r="V63" s="3"/>
+      <c r="W63" s="3"/>
+      <c r="X63" s="3"/>
+      <c r="Y63" s="3"/>
+      <c r="Z63" s="3"/>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>65</v>
       </c>
@@ -3133,14 +4469,24 @@
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
       <c r="J64" s="5"/>
-      <c r="K64" s="5"/>
-      <c r="L64" s="5"/>
-      <c r="M64" s="5"/>
-      <c r="N64" s="5"/>
-      <c r="O64" s="5"/>
-      <c r="P64" s="5"/>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K64" s="11"/>
+      <c r="L64" s="20"/>
+      <c r="M64" s="20"/>
+      <c r="N64" s="20"/>
+      <c r="O64" s="20"/>
+      <c r="P64" s="20"/>
+      <c r="Q64" s="20"/>
+      <c r="R64" s="20"/>
+      <c r="S64" s="21"/>
+      <c r="T64" s="20"/>
+      <c r="U64" s="5"/>
+      <c r="V64" s="5"/>
+      <c r="W64" s="5"/>
+      <c r="X64" s="5"/>
+      <c r="Y64" s="5"/>
+      <c r="Z64" s="5"/>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>66</v>
       </c>
@@ -3171,30 +4517,61 @@
       <c r="J65" s="4">
         <v>512000</v>
       </c>
-      <c r="K65" s="4">
-        <f>D65*E65</f>
-        <v>512000</v>
-      </c>
-      <c r="L65" s="4">
+      <c r="K65" s="10"/>
+      <c r="L65" s="18">
+        <f>L60+J60/2+E60/2</f>
+        <v>365344</v>
+      </c>
+      <c r="M65" s="18">
+        <f>L65+J65/2-1</f>
+        <v>621343</v>
+      </c>
+      <c r="N65" s="18">
+        <f>M65+1</f>
+        <v>621344</v>
+      </c>
+      <c r="O65" s="18">
+        <f>N65+E65/2-1</f>
+        <v>621843</v>
+      </c>
+      <c r="P65" s="18"/>
+      <c r="Q65" s="18"/>
+      <c r="R65" s="18">
+        <f>S60+1</f>
+        <v>2106068</v>
+      </c>
+      <c r="S65" s="19">
+        <f>R65+I65/2-1</f>
+        <v>2190567</v>
+      </c>
+      <c r="T65" s="18">
+        <f>U65/E65</f>
+        <v>86528</v>
+      </c>
+      <c r="U65" s="4">
+        <f>D65*I65</f>
+        <v>86528000</v>
+      </c>
+      <c r="V65" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M65" s="4">
-        <v>1</v>
-      </c>
-      <c r="N65" s="4">
+      <c r="W65" s="4">
+        <v>1</v>
+      </c>
+      <c r="X65" s="4">
         <f>0.0000032*J65+0.0000064*I65</f>
         <v>2.7199999999999998</v>
       </c>
-      <c r="O65" s="4">
-        <f>K65*L65</f>
-        <v>35840</v>
-      </c>
-      <c r="P65" s="4">
-        <f>K65*L65*M65</f>
-        <v>35840</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Y65" s="4">
+        <f>U65*V65</f>
+        <v>6056960.0000000009</v>
+      </c>
+      <c r="Z65" s="4">
+        <f>T65*V65*W65</f>
+        <v>6056.9600000000009</v>
+      </c>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>67</v>
       </c>
@@ -3209,14 +4586,24 @@
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
-      <c r="K66" s="5"/>
-      <c r="L66" s="5"/>
-      <c r="M66" s="5"/>
-      <c r="N66" s="5"/>
-      <c r="O66" s="5"/>
-      <c r="P66" s="5"/>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K66" s="11"/>
+      <c r="L66" s="20"/>
+      <c r="M66" s="20"/>
+      <c r="N66" s="20"/>
+      <c r="O66" s="20"/>
+      <c r="P66" s="20"/>
+      <c r="Q66" s="20"/>
+      <c r="R66" s="20"/>
+      <c r="S66" s="21"/>
+      <c r="T66" s="20"/>
+      <c r="U66" s="5"/>
+      <c r="V66" s="5"/>
+      <c r="W66" s="5"/>
+      <c r="X66" s="5"/>
+      <c r="Y66" s="5"/>
+      <c r="Z66" s="5"/>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>68</v>
       </c>
@@ -3227,7 +4614,9 @@
         <v>103</v>
       </c>
       <c r="D67" s="6"/>
-      <c r="E67" s="6"/>
+      <c r="E67" s="6">
+        <v>1000</v>
+      </c>
       <c r="F67" s="6">
         <v>1</v>
       </c>
@@ -3241,29 +4630,47 @@
         <v>1000</v>
       </c>
       <c r="J67" s="6"/>
-      <c r="K67" s="6">
+      <c r="K67" s="12"/>
+      <c r="L67" s="22"/>
+      <c r="M67" s="22"/>
+      <c r="N67" s="22"/>
+      <c r="O67" s="22"/>
+      <c r="P67" s="22"/>
+      <c r="Q67" s="22"/>
+      <c r="R67" s="22">
+        <f>S65+1</f>
+        <v>2190568</v>
+      </c>
+      <c r="S67" s="23">
+        <f>R67+I67/2-1</f>
+        <v>2191067</v>
+      </c>
+      <c r="T67" s="22">
         <v>1000</v>
       </c>
-      <c r="L67" s="6">
+      <c r="U67" s="6">
+        <v>1000</v>
+      </c>
+      <c r="V67" s="6">
         <v>1.2</v>
       </c>
-      <c r="M67" s="6">
-        <v>1</v>
-      </c>
-      <c r="N67" s="6">
+      <c r="W67" s="6">
+        <v>1</v>
+      </c>
+      <c r="X67" s="6">
         <f>0.0000064*I67</f>
         <v>6.3999999999999994E-3</v>
       </c>
-      <c r="O67" s="6">
-        <f>K67*L67</f>
+      <c r="Y67" s="6">
+        <f>U67*V67</f>
         <v>1200</v>
       </c>
-      <c r="P67" s="6">
-        <f>K67*L67*M67</f>
+      <c r="Z67" s="6">
+        <f>T67*V67*W67</f>
         <v>1200</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>69</v>
       </c>
@@ -3278,14 +4685,24 @@
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
-      <c r="K68" s="3"/>
-      <c r="L68" s="3"/>
-      <c r="M68" s="3"/>
-      <c r="N68" s="3"/>
-      <c r="O68" s="3"/>
-      <c r="P68" s="3"/>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K68" s="9"/>
+      <c r="L68" s="16"/>
+      <c r="M68" s="16"/>
+      <c r="N68" s="16"/>
+      <c r="O68" s="16"/>
+      <c r="P68" s="16"/>
+      <c r="Q68" s="16"/>
+      <c r="R68" s="16"/>
+      <c r="S68" s="17"/>
+      <c r="T68" s="16"/>
+      <c r="U68" s="3"/>
+      <c r="V68" s="3"/>
+      <c r="W68" s="3"/>
+      <c r="X68" s="3"/>
+      <c r="Y68" s="3"/>
+      <c r="Z68" s="3"/>
+    </row>
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="I69" s="2">
         <f>SUM(I2:I68)</f>
         <v>3071416</v>
@@ -3294,24 +4711,33 @@
         <f>SUM(J3:J68)</f>
         <v>1231552</v>
       </c>
-      <c r="K69" s="2">
-        <f>SUM(K3:K68)</f>
-        <v>1069672</v>
-      </c>
-      <c r="N69" s="2">
-        <f>SUM(N2:N68)</f>
+      <c r="L69" s="24"/>
+      <c r="M69" s="24"/>
+      <c r="N69" s="24"/>
+      <c r="O69" s="24"/>
+      <c r="P69" s="24"/>
+      <c r="Q69" s="24"/>
+      <c r="R69" s="24"/>
+      <c r="S69" s="25"/>
+      <c r="T69" s="24"/>
+      <c r="U69" s="2">
+        <f>SUM(U3:U68)</f>
+        <v>163998312</v>
+      </c>
+      <c r="X69" s="2">
+        <f>SUM(X2:X68)</f>
         <v>23.116339199999999</v>
       </c>
-      <c r="O69" s="2">
-        <f t="shared" ref="O69:P69" si="32">SUM(O3:O68)</f>
-        <v>182983.68000000002</v>
-      </c>
-      <c r="P69" s="2">
-        <f t="shared" si="32"/>
-        <v>178682.88</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Y69" s="2">
+        <f t="shared" ref="Y69:Z69" si="31">SUM(Y3:Y68)</f>
+        <v>21993774.080000002</v>
+      </c>
+      <c r="Z69" s="2">
+        <f t="shared" si="31"/>
+        <v>200398.49000000002</v>
+      </c>
+    </row>
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="I70" s="7">
         <f>I69*16/1024/8</f>
         <v>5998.859375</v>
@@ -3320,11 +4746,57 @@
         <f>J69*16/1024/8</f>
         <v>2405.375</v>
       </c>
+      <c r="L70" s="24"/>
+      <c r="M70" s="24"/>
+      <c r="N70" s="24"/>
+      <c r="O70" s="24"/>
+      <c r="P70" s="24"/>
+      <c r="Q70" s="24"/>
+      <c r="R70" s="24"/>
+      <c r="S70" s="25"/>
+      <c r="T70" s="24"/>
+    </row>
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="L71" s="24"/>
+      <c r="M71" s="24"/>
+      <c r="N71" s="24"/>
+      <c r="O71" s="24"/>
+      <c r="P71" s="24"/>
+      <c r="Q71" s="24"/>
+      <c r="R71" s="24"/>
+      <c r="S71" s="25"/>
+      <c r="T71" s="24"/>
+    </row>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="L72" s="24"/>
+      <c r="M72" s="24"/>
+      <c r="N72" s="24"/>
+      <c r="O72" s="24"/>
+      <c r="P72" s="24"/>
+      <c r="Q72" s="24"/>
+      <c r="R72" s="24"/>
+      <c r="S72" s="25"/>
+      <c r="T72" s="24"/>
+    </row>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="L73" s="24"/>
+      <c r="M73" s="24"/>
+      <c r="N73" s="24"/>
+      <c r="O73" s="24"/>
+      <c r="P73" s="24"/>
+      <c r="Q73" s="24"/>
+      <c r="R73" s="24"/>
+      <c r="S73" s="25"/>
+      <c r="T73" s="24"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B69" xr:uid="{5611B078-3ED8-409A-972B-20710E035DA1}"/>
-  <mergeCells count="1">
+  <autoFilter ref="B1:B70" xr:uid="{5611B078-3ED8-409A-972B-20710E035DA1}"/>
+  <mergeCells count="5">
     <mergeCell ref="H1:I1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update csb and estimation
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA509EF-2FEE-4C55-88D9-41108E438C7C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89684071-EAAD-49D0-8873-0FE862000615}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7860" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="116">
   <si>
     <t>INPUT</t>
   </si>
@@ -378,6 +378,9 @@
   </si>
   <si>
     <t>Output Mem</t>
+  </si>
+  <si>
+    <t>Op Paral</t>
   </si>
 </sst>
 </file>
@@ -514,9 +517,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -533,9 +533,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -572,6 +569,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -897,11 +900,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DDF8812-1429-4032-9C9C-F25909298566}">
-  <dimension ref="A1:Z73"/>
+  <dimension ref="A1:AA73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -916,21 +919,22 @@
     <col min="8" max="8" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.08984375" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="6.81640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="13.1796875" style="16" customWidth="1"/>
-    <col min="19" max="19" width="13.1796875" style="17" customWidth="1"/>
-    <col min="20" max="20" width="17.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="44.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="9.1796875" style="1"/>
+    <col min="11" max="11" width="22.08984375" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="6.81640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="13.1796875" style="14" customWidth="1"/>
+    <col min="19" max="19" width="13.1796875" style="15" customWidth="1"/>
+    <col min="20" max="20" width="13.1796875" style="14" customWidth="1"/>
+    <col min="21" max="21" width="17.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="44.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -952,55 +956,58 @@
       <c r="G1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="8"/>
+      <c r="I1" s="26"/>
       <c r="J1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15" t="s">
+      <c r="M1" s="27"/>
+      <c r="N1" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15" t="s">
+      <c r="O1" s="27"/>
+      <c r="P1" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15" t="s">
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27" t="s">
         <v>114</v>
       </c>
       <c r="S1" s="28"/>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1019,34 +1026,35 @@
         <v>150528</v>
       </c>
       <c r="J2" s="3"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18">
+      <c r="K2" s="9"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16">
         <v>655360</v>
       </c>
-      <c r="S2" s="19">
+      <c r="S2" s="17">
         <f>R2+I2/2-1</f>
         <v>730623</v>
       </c>
-      <c r="T2" s="3"/>
+      <c r="T2" s="16"/>
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
-      <c r="W2" s="3">
+      <c r="W2" s="3"/>
+      <c r="X2" s="3">
         <f>0.0000032*I2</f>
         <v>0.4816896</v>
       </c>
-      <c r="X2" s="3"/>
       <c r="Y2" s="3"/>
-      <c r="Z2" s="2" t="s">
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -1077,56 +1085,60 @@
       <c r="J3" s="4">
         <v>1728</v>
       </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="20">
+      <c r="K3" s="10"/>
+      <c r="L3" s="18">
         <v>4096</v>
       </c>
-      <c r="M3" s="20">
+      <c r="M3" s="18">
         <f>L3+J3/2-1</f>
         <v>4959</v>
       </c>
-      <c r="N3" s="20">
+      <c r="N3" s="18">
         <f>M3+1</f>
         <v>4960</v>
       </c>
-      <c r="O3" s="20">
+      <c r="O3" s="18">
         <f>N3+E3/2-1</f>
         <v>4991</v>
       </c>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20">
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18">
         <f>S2+1</f>
         <v>730624</v>
       </c>
-      <c r="S3" s="21">
+      <c r="S3" s="19">
         <f>R3+I3/2-1</f>
         <v>1124895</v>
       </c>
-      <c r="T3" s="4">
-        <f>D3*E3</f>
-        <v>192</v>
+      <c r="T3" s="18">
+        <f>U3/E3</f>
+        <v>36963</v>
       </c>
       <c r="U3" s="4">
+        <f>D3*I3</f>
+        <v>2365632</v>
+      </c>
+      <c r="V3" s="4">
         <v>0.52</v>
       </c>
-      <c r="V3" s="4">
-        <v>1</v>
-      </c>
       <c r="W3" s="4">
+        <v>1</v>
+      </c>
+      <c r="X3" s="4">
         <f>0.0000032*J3+0.0000064*I3</f>
         <v>5.0522111999999995</v>
       </c>
-      <c r="X3" s="4">
-        <f>T3*U3</f>
-        <v>99.84</v>
-      </c>
       <c r="Y3" s="4">
-        <f>T3*U3*V3</f>
-        <v>99.84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+        <f>U3*V3</f>
+        <v>1230128.6400000001</v>
+      </c>
+      <c r="Z3" s="4">
+        <f>T3*V3*W3</f>
+        <v>19220.760000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -1141,23 +1153,24 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="5"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="20"/>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z4" s="5"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -1168,7 +1181,9 @@
         <v>83</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="E5" s="6">
+        <v>64</v>
+      </c>
       <c r="F5" s="6">
         <v>2</v>
       </c>
@@ -1182,44 +1197,48 @@
         <v>193600</v>
       </c>
       <c r="J5" s="6"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="24"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="24">
+      <c r="K5" s="12"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22">
         <f>S3+1</f>
         <v>1124896</v>
       </c>
-      <c r="S5" s="25">
+      <c r="S5" s="23">
         <f>R5+I5/2-1</f>
         <v>1221695</v>
       </c>
-      <c r="T5" s="6">
+      <c r="T5" s="22">
+        <f>U5/E5</f>
+        <v>3025</v>
+      </c>
+      <c r="U5" s="6">
         <v>193600</v>
       </c>
-      <c r="U5" s="6">
+      <c r="V5" s="6">
         <v>0.31</v>
       </c>
-      <c r="V5" s="6">
-        <v>1</v>
-      </c>
       <c r="W5" s="6">
+        <v>1</v>
+      </c>
+      <c r="X5" s="6">
         <f>0.0000064*I5</f>
         <v>1.2390399999999999</v>
       </c>
-      <c r="X5" s="6">
-        <f>T5*U5</f>
+      <c r="Y5" s="6">
+        <f>U5*V5</f>
         <v>60016</v>
       </c>
-      <c r="Y5" s="6">
-        <f>T5*U5*V5</f>
-        <v>60016</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z5" s="6">
+        <f>T5*V5*W5</f>
+        <v>937.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -1250,57 +1269,61 @@
       <c r="J6" s="4">
         <v>1024</v>
       </c>
-      <c r="K6" s="11"/>
-      <c r="L6" s="20">
+      <c r="K6" s="10"/>
+      <c r="L6" s="18">
         <f>L3+J3/2+E3/2</f>
         <v>4992</v>
       </c>
-      <c r="M6" s="20">
+      <c r="M6" s="18">
         <f>L6+J6/2-1</f>
         <v>5503</v>
       </c>
-      <c r="N6" s="20">
+      <c r="N6" s="18">
         <f>M6+1</f>
         <v>5504</v>
       </c>
-      <c r="O6" s="20">
+      <c r="O6" s="18">
         <f>N6+E6/2-1</f>
         <v>5511</v>
       </c>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="20">
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18">
         <f>S5+1</f>
         <v>1221696</v>
       </c>
-      <c r="S6" s="21">
+      <c r="S6" s="19">
         <f>R6+I6/2-1</f>
         <v>1245895</v>
       </c>
-      <c r="T6" s="4">
-        <f>D6*E6</f>
-        <v>1024</v>
+      <c r="T6" s="18">
+        <f>U6/E6</f>
+        <v>193600</v>
       </c>
       <c r="U6" s="4">
+        <f>D6*I6</f>
+        <v>3097600</v>
+      </c>
+      <c r="V6" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="V6" s="4">
-        <v>1</v>
-      </c>
       <c r="W6" s="4">
+        <v>1</v>
+      </c>
+      <c r="X6" s="4">
         <f>0.0000032*J6+0.0000064*I6</f>
         <v>0.3130368</v>
       </c>
-      <c r="X6" s="4">
-        <f>T6*U6</f>
-        <v>71.680000000000007</v>
-      </c>
       <c r="Y6" s="4">
-        <f>T6*U6*V6</f>
-        <v>71.680000000000007</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+        <f>U6*V6</f>
+        <v>216832.00000000003</v>
+      </c>
+      <c r="Z6" s="4">
+        <f>T6*V6*W6</f>
+        <v>13552.000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -1315,23 +1338,24 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="5"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="20"/>
       <c r="U7" s="5"/>
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z7" s="5"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -1362,57 +1386,61 @@
       <c r="J8" s="4">
         <v>1024</v>
       </c>
-      <c r="K8" s="11"/>
-      <c r="L8" s="20">
+      <c r="K8" s="10"/>
+      <c r="L8" s="18">
         <f>L6+J6/2+E6/2</f>
         <v>5512</v>
       </c>
-      <c r="M8" s="20">
+      <c r="M8" s="18">
         <f t="shared" ref="M8:M9" si="0">L8+J8/2-1</f>
         <v>6023</v>
       </c>
-      <c r="N8" s="20">
+      <c r="N8" s="18">
         <f t="shared" ref="N8:N9" si="1">M8+1</f>
         <v>6024</v>
       </c>
-      <c r="O8" s="20">
+      <c r="O8" s="18">
         <f>N8+E8/2-1</f>
         <v>6055</v>
       </c>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="20"/>
-      <c r="R8" s="20">
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18">
         <f>S6+1</f>
         <v>1245896</v>
       </c>
-      <c r="S8" s="21">
+      <c r="S8" s="19">
         <f>R8+I8/2-1</f>
         <v>1342695</v>
       </c>
-      <c r="T8" s="4">
-        <f>D8*E8</f>
-        <v>1024</v>
+      <c r="T8" s="18">
+        <f>U8/E8</f>
+        <v>48400</v>
       </c>
       <c r="U8" s="4">
+        <f>D8*I8</f>
+        <v>3097600</v>
+      </c>
+      <c r="V8" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="V8" s="4">
+      <c r="W8" s="4">
         <v>0</v>
       </c>
-      <c r="W8" s="4">
+      <c r="X8" s="4">
         <f>0.0000032*J8+0.0000064*I8</f>
         <v>1.2423168</v>
       </c>
-      <c r="X8" s="4">
-        <f t="shared" ref="X8:X9" si="2">T8*U8</f>
-        <v>71.680000000000007</v>
-      </c>
       <c r="Y8" s="4">
-        <f t="shared" ref="Y8:Y9" si="3">T8*U8*V8</f>
+        <f t="shared" ref="Y8:Y9" si="2">U8*V8</f>
+        <v>216832.00000000003</v>
+      </c>
+      <c r="Z8" s="4">
+        <f t="shared" ref="Z8:Z9" si="3">T8*V8*W8</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -1443,57 +1471,61 @@
       <c r="J9" s="4">
         <v>9216</v>
       </c>
-      <c r="K9" s="11"/>
-      <c r="L9" s="20">
+      <c r="K9" s="10"/>
+      <c r="L9" s="18">
         <f>L8+J8/2+E8/2</f>
         <v>6056</v>
       </c>
-      <c r="M9" s="20">
+      <c r="M9" s="18">
         <f t="shared" si="0"/>
         <v>10663</v>
       </c>
-      <c r="N9" s="20">
+      <c r="N9" s="18">
         <f t="shared" si="1"/>
         <v>10664</v>
       </c>
-      <c r="O9" s="20">
+      <c r="O9" s="18">
         <f>N9+E9/2-1</f>
         <v>10695</v>
       </c>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="20"/>
-      <c r="R9" s="20">
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18">
         <f>S8+1</f>
         <v>1342696</v>
       </c>
-      <c r="S9" s="21">
+      <c r="S9" s="19">
         <f>R9+I9/2-1</f>
         <v>1439495</v>
       </c>
-      <c r="T9" s="4">
-        <f>D9*E9</f>
-        <v>1024</v>
+      <c r="T9" s="18">
+        <f>U9/E9</f>
+        <v>48400</v>
       </c>
       <c r="U9" s="4">
+        <f>D9*I9</f>
+        <v>3097600</v>
+      </c>
+      <c r="V9" s="4">
         <v>0.52</v>
       </c>
-      <c r="V9" s="4">
-        <v>1</v>
-      </c>
       <c r="W9" s="4">
+        <v>1</v>
+      </c>
+      <c r="X9" s="4">
         <f>0.0000032*J9+0.0000064*I9</f>
         <v>1.2685312</v>
       </c>
-      <c r="X9" s="4">
+      <c r="Y9" s="4">
         <f t="shared" si="2"/>
-        <v>532.48</v>
-      </c>
-      <c r="Y9" s="4">
+        <v>1610752</v>
+      </c>
+      <c r="Z9" s="4">
         <f t="shared" si="3"/>
-        <v>532.48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+        <v>25168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1508,23 +1540,24 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="22"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="5"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="20"/>
       <c r="U10" s="5"/>
       <c r="V10" s="5"/>
       <c r="W10" s="5"/>
       <c r="X10" s="5"/>
       <c r="Y10" s="5"/>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z10" s="5"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1539,23 +1572,24 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="22"/>
-      <c r="R11" s="22"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="5"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="20"/>
       <c r="U11" s="5"/>
       <c r="V11" s="5"/>
       <c r="W11" s="5"/>
       <c r="X11" s="5"/>
       <c r="Y11" s="5"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z11" s="5"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -1572,23 +1606,24 @@
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="19"/>
-      <c r="T12" s="3"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="16"/>
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z12" s="3"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
@@ -1619,57 +1654,61 @@
       <c r="J13" s="4">
         <v>2048</v>
       </c>
-      <c r="K13" s="11"/>
-      <c r="L13" s="20">
+      <c r="K13" s="10"/>
+      <c r="L13" s="18">
         <f>L9+J9/2+E9/2</f>
         <v>10696</v>
       </c>
-      <c r="M13" s="20">
+      <c r="M13" s="18">
         <f>L13+J13/2-1</f>
         <v>11719</v>
       </c>
-      <c r="N13" s="20">
+      <c r="N13" s="18">
         <f>M13+1</f>
         <v>11720</v>
       </c>
-      <c r="O13" s="20">
+      <c r="O13" s="18">
         <f>N13+E13/2-1</f>
         <v>11727</v>
       </c>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="20"/>
-      <c r="R13" s="20">
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18">
         <f>S9+1</f>
         <v>1439496</v>
       </c>
-      <c r="S13" s="21">
+      <c r="S13" s="19">
         <f>R13+I13/2-1</f>
         <v>1463695</v>
       </c>
-      <c r="T13" s="4">
-        <f>D13*E13</f>
-        <v>2048</v>
+      <c r="T13" s="18">
+        <f>U13/E13</f>
+        <v>387200</v>
       </c>
       <c r="U13" s="4">
+        <f>D13*I13</f>
+        <v>6195200</v>
+      </c>
+      <c r="V13" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="V13" s="4">
-        <v>1</v>
-      </c>
       <c r="W13" s="4">
+        <v>1</v>
+      </c>
+      <c r="X13" s="4">
         <f>0.0000032*J13+0.0000064*I13</f>
         <v>0.31631359999999997</v>
       </c>
-      <c r="X13" s="4">
-        <f>T13*U13</f>
-        <v>143.36000000000001</v>
-      </c>
       <c r="Y13" s="4">
-        <f>T13*U13*V13</f>
-        <v>143.36000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+        <f>U13*V13</f>
+        <v>433664.00000000006</v>
+      </c>
+      <c r="Z13" s="4">
+        <f>T13*V13*W13</f>
+        <v>27104.000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
@@ -1684,23 +1723,24 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="22"/>
-      <c r="S14" s="23"/>
-      <c r="T14" s="5"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="20"/>
       <c r="U14" s="5"/>
       <c r="V14" s="5"/>
       <c r="W14" s="5"/>
       <c r="X14" s="5"/>
       <c r="Y14" s="5"/>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z14" s="5"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
@@ -1731,57 +1771,61 @@
       <c r="J15" s="4">
         <v>1024</v>
       </c>
-      <c r="K15" s="11"/>
-      <c r="L15" s="20">
+      <c r="K15" s="10"/>
+      <c r="L15" s="18">
         <f>L13+J13/2+E13/2</f>
         <v>11728</v>
       </c>
-      <c r="M15" s="20">
+      <c r="M15" s="18">
         <f t="shared" ref="M15:M16" si="4">L15+J15/2-1</f>
         <v>12239</v>
       </c>
-      <c r="N15" s="20">
+      <c r="N15" s="18">
         <f t="shared" ref="N15:N16" si="5">M15+1</f>
         <v>12240</v>
       </c>
-      <c r="O15" s="20">
+      <c r="O15" s="18">
         <f>N15+E15/2-1</f>
         <v>12271</v>
       </c>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="20"/>
-      <c r="R15" s="20">
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18">
         <f>S13+1</f>
         <v>1463696</v>
       </c>
-      <c r="S15" s="21">
+      <c r="S15" s="19">
         <f>R15+I15/2-1</f>
         <v>1560495</v>
       </c>
-      <c r="T15" s="4">
-        <f>D15*E15</f>
-        <v>1024</v>
+      <c r="T15" s="18">
+        <f>U15/E15</f>
+        <v>48400</v>
       </c>
       <c r="U15" s="4">
+        <f>D15*I15</f>
+        <v>3097600</v>
+      </c>
+      <c r="V15" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="V15" s="4">
+      <c r="W15" s="4">
         <v>0</v>
       </c>
-      <c r="W15" s="4">
+      <c r="X15" s="4">
         <f>0.0000032*J15+0.0000064*I15</f>
         <v>1.2423168</v>
       </c>
-      <c r="X15" s="4">
-        <f t="shared" ref="X15:X16" si="6">T15*U15</f>
-        <v>71.680000000000007</v>
-      </c>
       <c r="Y15" s="4">
-        <f t="shared" ref="Y15:Y16" si="7">T15*U15*V15</f>
+        <f t="shared" ref="Y15:Y16" si="6">U15*V15</f>
+        <v>216832.00000000003</v>
+      </c>
+      <c r="Z15" s="4">
+        <f t="shared" ref="Z15:Z16" si="7">T15*V15*W15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -1812,57 +1856,61 @@
       <c r="J16" s="4">
         <v>9216</v>
       </c>
-      <c r="K16" s="11"/>
-      <c r="L16" s="20">
+      <c r="K16" s="10"/>
+      <c r="L16" s="18">
         <f>L15+J15/2+E15/2</f>
         <v>12272</v>
       </c>
-      <c r="M16" s="20">
+      <c r="M16" s="18">
         <f t="shared" si="4"/>
         <v>16879</v>
       </c>
-      <c r="N16" s="20">
+      <c r="N16" s="18">
         <f t="shared" si="5"/>
         <v>16880</v>
       </c>
-      <c r="O16" s="20">
+      <c r="O16" s="18">
         <f>N16+E16/2-1</f>
         <v>16911</v>
       </c>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="20"/>
-      <c r="R16" s="20">
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="18">
         <f>S15+1</f>
         <v>1560496</v>
       </c>
-      <c r="S16" s="21">
+      <c r="S16" s="19">
         <f>R16+I16/2-1</f>
         <v>1657295</v>
       </c>
-      <c r="T16" s="4">
-        <f>D16*E16</f>
-        <v>1024</v>
+      <c r="T16" s="18">
+        <f>U16/E16</f>
+        <v>48400</v>
       </c>
       <c r="U16" s="4">
+        <f>D16*I16</f>
+        <v>3097600</v>
+      </c>
+      <c r="V16" s="4">
         <v>0.52</v>
       </c>
-      <c r="V16" s="4">
-        <v>1</v>
-      </c>
       <c r="W16" s="4">
+        <v>1</v>
+      </c>
+      <c r="X16" s="4">
         <f>0.0000032*J16+0.0000064*I16</f>
         <v>1.2685312</v>
       </c>
-      <c r="X16" s="4">
+      <c r="Y16" s="4">
         <f t="shared" si="6"/>
-        <v>532.48</v>
-      </c>
-      <c r="Y16" s="4">
+        <v>1610752</v>
+      </c>
+      <c r="Z16" s="4">
         <f t="shared" si="7"/>
-        <v>532.48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+        <v>25168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>17</v>
       </c>
@@ -1877,23 +1925,24 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="22"/>
-      <c r="S17" s="23"/>
-      <c r="T17" s="5"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="20"/>
       <c r="U17" s="5"/>
       <c r="V17" s="5"/>
       <c r="W17" s="5"/>
       <c r="X17" s="5"/>
       <c r="Y17" s="5"/>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z17" s="5"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1908,23 +1957,24 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
-      <c r="S18" s="23"/>
-      <c r="T18" s="5"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="20"/>
       <c r="U18" s="5"/>
       <c r="V18" s="5"/>
       <c r="W18" s="5"/>
       <c r="X18" s="5"/>
       <c r="Y18" s="5"/>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z18" s="5"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
@@ -1941,23 +1991,24 @@
       </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="19"/>
-      <c r="T19" s="3"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="16"/>
       <c r="U19" s="3"/>
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
       <c r="Y19" s="3"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z19" s="3"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>21</v>
       </c>
@@ -1968,7 +2019,9 @@
         <v>83</v>
       </c>
       <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="E20" s="6">
+        <v>128</v>
+      </c>
       <c r="F20" s="6">
         <v>2</v>
       </c>
@@ -1982,44 +2035,48 @@
         <v>93312</v>
       </c>
       <c r="J20" s="6"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="24">
+      <c r="K20" s="12"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="22"/>
+      <c r="R20" s="22">
         <f>S16+1</f>
         <v>1657296</v>
       </c>
-      <c r="S20" s="25">
+      <c r="S20" s="23">
         <f>R20+I20/2-1</f>
         <v>1703951</v>
       </c>
-      <c r="T20" s="6">
+      <c r="T20" s="22">
+        <f>U20/E20</f>
+        <v>729</v>
+      </c>
+      <c r="U20" s="6">
         <v>93312</v>
       </c>
-      <c r="U20" s="6">
+      <c r="V20" s="6">
         <v>0.31</v>
       </c>
-      <c r="V20" s="6">
-        <v>1</v>
-      </c>
       <c r="W20" s="6">
+        <v>1</v>
+      </c>
+      <c r="X20" s="6">
         <f>0.0000064*I20</f>
         <v>0.59719679999999997</v>
       </c>
-      <c r="X20" s="6">
-        <f>T20*U20</f>
+      <c r="Y20" s="6">
+        <f>U20*V20</f>
         <v>28926.720000000001</v>
       </c>
-      <c r="Y20" s="6">
-        <f>T20*U20*V20</f>
-        <v>28926.720000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z20" s="6">
+        <f>T20*V20*W20</f>
+        <v>225.99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>22</v>
       </c>
@@ -2050,57 +2107,61 @@
       <c r="J21" s="4">
         <v>4096</v>
       </c>
-      <c r="K21" s="11"/>
-      <c r="L21" s="20">
+      <c r="K21" s="10"/>
+      <c r="L21" s="18">
         <f>L16+J16/2+E16/2</f>
         <v>16912</v>
       </c>
-      <c r="M21" s="20">
+      <c r="M21" s="18">
         <f>L21+J21/2-1</f>
         <v>18959</v>
       </c>
-      <c r="N21" s="20">
+      <c r="N21" s="18">
         <f>M21+1</f>
         <v>18960</v>
       </c>
-      <c r="O21" s="20">
+      <c r="O21" s="18">
         <f>N21+E21/2-1</f>
         <v>18975</v>
       </c>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="20"/>
-      <c r="R21" s="20">
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18">
         <f>S20+1</f>
         <v>1703952</v>
       </c>
-      <c r="S21" s="21">
+      <c r="S21" s="19">
         <f>R21+I21/2-1</f>
         <v>1715615</v>
       </c>
-      <c r="T21" s="4">
-        <f>D21*E21</f>
-        <v>4096</v>
+      <c r="T21" s="18">
+        <f>U21/E21</f>
+        <v>93312</v>
       </c>
       <c r="U21" s="4">
+        <f>D21*I21</f>
+        <v>2985984</v>
+      </c>
+      <c r="V21" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="V21" s="4">
-        <v>1</v>
-      </c>
       <c r="W21" s="4">
+        <v>1</v>
+      </c>
+      <c r="X21" s="4">
         <f>0.0000032*J21+0.0000064*I21</f>
         <v>0.16240640000000001</v>
       </c>
-      <c r="X21" s="4">
-        <f>T21*U21</f>
-        <v>286.72000000000003</v>
-      </c>
       <c r="Y21" s="4">
-        <f>T21*U21*V21</f>
-        <v>286.72000000000003</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+        <f>U21*V21</f>
+        <v>209018.88000000003</v>
+      </c>
+      <c r="Z21" s="4">
+        <f>T21*V21*W21</f>
+        <v>6531.8400000000011</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>23</v>
       </c>
@@ -2115,23 +2176,24 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="22"/>
-      <c r="S22" s="23"/>
-      <c r="T22" s="5"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="20"/>
+      <c r="S22" s="21"/>
+      <c r="T22" s="20"/>
       <c r="U22" s="5"/>
       <c r="V22" s="5"/>
       <c r="W22" s="5"/>
       <c r="X22" s="5"/>
       <c r="Y22" s="5"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z22" s="5"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>24</v>
       </c>
@@ -2162,57 +2224,61 @@
       <c r="J23" s="4">
         <v>4096</v>
       </c>
-      <c r="K23" s="11"/>
-      <c r="L23" s="20">
+      <c r="K23" s="10"/>
+      <c r="L23" s="18">
         <f>L21+J21/2+E21/2</f>
         <v>18976</v>
       </c>
-      <c r="M23" s="20">
+      <c r="M23" s="18">
         <f t="shared" ref="M23:M24" si="8">L23+J23/2-1</f>
         <v>21023</v>
       </c>
-      <c r="N23" s="20">
+      <c r="N23" s="18">
         <f t="shared" ref="N23:N24" si="9">M23+1</f>
         <v>21024</v>
       </c>
-      <c r="O23" s="20">
+      <c r="O23" s="18">
         <f>N23+E23/2-1</f>
         <v>21087</v>
       </c>
-      <c r="P23" s="20"/>
-      <c r="Q23" s="20"/>
-      <c r="R23" s="20">
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18">
         <f>S21+1</f>
         <v>1715616</v>
       </c>
-      <c r="S23" s="21">
+      <c r="S23" s="19">
         <f>R23+I23/2-1</f>
         <v>1762271</v>
       </c>
-      <c r="T23" s="4">
-        <f>D23*E23</f>
-        <v>4096</v>
+      <c r="T23" s="18">
+        <f>U23/E23</f>
+        <v>23328</v>
       </c>
       <c r="U23" s="4">
+        <f>D23*I23</f>
+        <v>2985984</v>
+      </c>
+      <c r="V23" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="V23" s="4">
+      <c r="W23" s="4">
         <v>0</v>
       </c>
-      <c r="W23" s="4">
+      <c r="X23" s="4">
         <f>0.0000032*J23+0.0000064*I23</f>
         <v>0.61030399999999996</v>
       </c>
-      <c r="X23" s="4">
-        <f t="shared" ref="X23:X24" si="10">T23*U23</f>
-        <v>286.72000000000003</v>
-      </c>
       <c r="Y23" s="4">
-        <f t="shared" ref="Y23:Y24" si="11">T23*U23*V23</f>
+        <f t="shared" ref="Y23:Y24" si="10">U23*V23</f>
+        <v>209018.88000000003</v>
+      </c>
+      <c r="Z23" s="4">
+        <f t="shared" ref="Z23:Z24" si="11">T23*V23*W23</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
@@ -2243,57 +2309,61 @@
       <c r="J24" s="4">
         <v>36864</v>
       </c>
-      <c r="K24" s="11"/>
-      <c r="L24" s="20">
+      <c r="K24" s="10"/>
+      <c r="L24" s="18">
         <f>L23+J23/2+E23/2</f>
         <v>21088</v>
       </c>
-      <c r="M24" s="20">
+      <c r="M24" s="18">
         <f t="shared" si="8"/>
         <v>39519</v>
       </c>
-      <c r="N24" s="20">
+      <c r="N24" s="18">
         <f t="shared" si="9"/>
         <v>39520</v>
       </c>
-      <c r="O24" s="20">
+      <c r="O24" s="18">
         <f>N24+E24/2-1</f>
         <v>39583</v>
       </c>
-      <c r="P24" s="20"/>
-      <c r="Q24" s="20"/>
-      <c r="R24" s="20">
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18">
         <f>S23+1</f>
         <v>1762272</v>
       </c>
-      <c r="S24" s="21">
+      <c r="S24" s="19">
         <f>R24+I24/2-1</f>
         <v>1808927</v>
       </c>
-      <c r="T24" s="4">
-        <f>D24*E24</f>
-        <v>4096</v>
+      <c r="T24" s="18">
+        <f>U24/E24</f>
+        <v>23328</v>
       </c>
       <c r="U24" s="4">
+        <f>D24*I24</f>
+        <v>2985984</v>
+      </c>
+      <c r="V24" s="4">
         <v>0.52</v>
       </c>
-      <c r="V24" s="4">
-        <v>1</v>
-      </c>
       <c r="W24" s="4">
+        <v>1</v>
+      </c>
+      <c r="X24" s="4">
         <f>0.0000032*J24+0.0000064*I24</f>
         <v>0.71516159999999995</v>
       </c>
-      <c r="X24" s="4">
+      <c r="Y24" s="4">
         <f t="shared" si="10"/>
-        <v>2129.92</v>
-      </c>
-      <c r="Y24" s="4">
+        <v>1552711.6800000002</v>
+      </c>
+      <c r="Z24" s="4">
         <f t="shared" si="11"/>
-        <v>2129.92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+        <v>12130.560000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>26</v>
       </c>
@@ -2308,23 +2378,24 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="22"/>
-      <c r="Q25" s="22"/>
-      <c r="R25" s="22"/>
-      <c r="S25" s="23"/>
-      <c r="T25" s="5"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="20"/>
+      <c r="O25" s="20"/>
+      <c r="P25" s="20"/>
+      <c r="Q25" s="20"/>
+      <c r="R25" s="20"/>
+      <c r="S25" s="21"/>
+      <c r="T25" s="20"/>
       <c r="U25" s="5"/>
       <c r="V25" s="5"/>
       <c r="W25" s="5"/>
       <c r="X25" s="5"/>
       <c r="Y25" s="5"/>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z25" s="5"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>27</v>
       </c>
@@ -2339,23 +2410,24 @@
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="22"/>
-      <c r="P26" s="22"/>
-      <c r="Q26" s="22"/>
-      <c r="R26" s="22"/>
-      <c r="S26" s="23"/>
-      <c r="T26" s="5"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="20"/>
+      <c r="O26" s="20"/>
+      <c r="P26" s="20"/>
+      <c r="Q26" s="20"/>
+      <c r="R26" s="20"/>
+      <c r="S26" s="21"/>
+      <c r="T26" s="20"/>
       <c r="U26" s="5"/>
       <c r="V26" s="5"/>
       <c r="W26" s="5"/>
       <c r="X26" s="5"/>
       <c r="Y26" s="5"/>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z26" s="5"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>28</v>
       </c>
@@ -2372,23 +2444,24 @@
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18"/>
-      <c r="O27" s="18"/>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="18"/>
-      <c r="R27" s="18"/>
-      <c r="S27" s="19"/>
-      <c r="T27" s="3"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="16"/>
+      <c r="S27" s="17"/>
+      <c r="T27" s="16"/>
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
       <c r="X27" s="3"/>
       <c r="Y27" s="3"/>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z27" s="3"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
@@ -2419,57 +2492,61 @@
       <c r="J28" s="4">
         <v>8192</v>
       </c>
-      <c r="K28" s="11"/>
-      <c r="L28" s="20">
+      <c r="K28" s="10"/>
+      <c r="L28" s="18">
         <f>L24+J24/2+E24/2</f>
         <v>39584</v>
       </c>
-      <c r="M28" s="20">
+      <c r="M28" s="18">
         <f>L28+J28/2-1</f>
         <v>43679</v>
       </c>
-      <c r="N28" s="20">
+      <c r="N28" s="18">
         <f>M28+1</f>
         <v>43680</v>
       </c>
-      <c r="O28" s="20">
+      <c r="O28" s="18">
         <f>N28+E28/2-1</f>
         <v>43695</v>
       </c>
-      <c r="P28" s="20"/>
-      <c r="Q28" s="20"/>
-      <c r="R28" s="20">
+      <c r="P28" s="18"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18">
         <f>S24+1</f>
         <v>1808928</v>
       </c>
-      <c r="S28" s="21">
+      <c r="S28" s="19">
         <f>R28+I28/2-1</f>
         <v>1820591</v>
       </c>
-      <c r="T28" s="4">
-        <f>D28*E28</f>
-        <v>8192</v>
+      <c r="T28" s="18">
+        <f>U28/E28</f>
+        <v>186624</v>
       </c>
       <c r="U28" s="4">
+        <f>D28*I28</f>
+        <v>5971968</v>
+      </c>
+      <c r="V28" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="V28" s="4">
-        <v>1</v>
-      </c>
       <c r="W28" s="4">
+        <v>1</v>
+      </c>
+      <c r="X28" s="4">
         <f>0.0000032*J28+0.0000064*I28</f>
         <v>0.17551359999999999</v>
       </c>
-      <c r="X28" s="4">
-        <f>T28*U28</f>
-        <v>573.44000000000005</v>
-      </c>
       <c r="Y28" s="4">
-        <f>T28*U28*V28</f>
-        <v>573.44000000000005</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+        <f>U28*V28</f>
+        <v>418037.76000000007</v>
+      </c>
+      <c r="Z28" s="4">
+        <f>T28*V28*W28</f>
+        <v>13063.680000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>30</v>
       </c>
@@ -2484,23 +2561,24 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="22"/>
-      <c r="O29" s="22"/>
-      <c r="P29" s="22"/>
-      <c r="Q29" s="22"/>
-      <c r="R29" s="22"/>
-      <c r="S29" s="23"/>
-      <c r="T29" s="5"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
+      <c r="P29" s="20"/>
+      <c r="Q29" s="20"/>
+      <c r="R29" s="20"/>
+      <c r="S29" s="21"/>
+      <c r="T29" s="20"/>
       <c r="U29" s="5"/>
       <c r="V29" s="5"/>
       <c r="W29" s="5"/>
       <c r="X29" s="5"/>
       <c r="Y29" s="5"/>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z29" s="5"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>31</v>
       </c>
@@ -2531,57 +2609,61 @@
       <c r="J30" s="4">
         <v>4096</v>
       </c>
-      <c r="K30" s="11"/>
-      <c r="L30" s="20">
+      <c r="K30" s="10"/>
+      <c r="L30" s="18">
         <f>L28+J28/2+E28/2</f>
         <v>43696</v>
       </c>
-      <c r="M30" s="20">
+      <c r="M30" s="18">
         <f t="shared" ref="M30:M31" si="12">L30+J30/2-1</f>
         <v>45743</v>
       </c>
-      <c r="N30" s="20">
+      <c r="N30" s="18">
         <f t="shared" ref="N30:N31" si="13">M30+1</f>
         <v>45744</v>
       </c>
-      <c r="O30" s="20">
+      <c r="O30" s="18">
         <f>N30+E30/2-1</f>
         <v>45807</v>
       </c>
-      <c r="P30" s="20"/>
-      <c r="Q30" s="20"/>
-      <c r="R30" s="20">
+      <c r="P30" s="18"/>
+      <c r="Q30" s="18"/>
+      <c r="R30" s="18">
         <f>S28+1</f>
         <v>1820592</v>
       </c>
-      <c r="S30" s="21">
+      <c r="S30" s="19">
         <f>R30+I30/2-1</f>
         <v>1867247</v>
       </c>
-      <c r="T30" s="4">
-        <f>D30*E30</f>
-        <v>4096</v>
+      <c r="T30" s="18">
+        <f>U30/E30</f>
+        <v>23328</v>
       </c>
       <c r="U30" s="4">
+        <f>D30*I30</f>
+        <v>2985984</v>
+      </c>
+      <c r="V30" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="V30" s="4">
+      <c r="W30" s="4">
         <v>0</v>
       </c>
-      <c r="W30" s="4">
+      <c r="X30" s="4">
         <f>0.0000032*J30+0.0000064*I30</f>
         <v>0.61030399999999996</v>
       </c>
-      <c r="X30" s="4">
-        <f t="shared" ref="X30:X31" si="14">T30*U30</f>
-        <v>286.72000000000003</v>
-      </c>
       <c r="Y30" s="4">
-        <f t="shared" ref="Y30:Y31" si="15">T30*U30*V30</f>
+        <f t="shared" ref="Y30:Y31" si="14">U30*V30</f>
+        <v>209018.88000000003</v>
+      </c>
+      <c r="Z30" s="4">
+        <f t="shared" ref="Z30:Z31" si="15">T30*V30*W30</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>32</v>
       </c>
@@ -2612,57 +2694,61 @@
       <c r="J31" s="4">
         <v>36864</v>
       </c>
-      <c r="K31" s="11"/>
-      <c r="L31" s="20">
+      <c r="K31" s="10"/>
+      <c r="L31" s="18">
         <f>L30+J30/2+E30/2</f>
         <v>45808</v>
       </c>
-      <c r="M31" s="20">
+      <c r="M31" s="18">
         <f t="shared" si="12"/>
         <v>64239</v>
       </c>
-      <c r="N31" s="20">
+      <c r="N31" s="18">
         <f t="shared" si="13"/>
         <v>64240</v>
       </c>
-      <c r="O31" s="20">
+      <c r="O31" s="18">
         <f>N31+E31/2-1</f>
         <v>64303</v>
       </c>
-      <c r="P31" s="20"/>
-      <c r="Q31" s="20"/>
-      <c r="R31" s="20">
+      <c r="P31" s="18"/>
+      <c r="Q31" s="18"/>
+      <c r="R31" s="18">
         <f>S30+1</f>
         <v>1867248</v>
       </c>
-      <c r="S31" s="21">
+      <c r="S31" s="19">
         <f>R31+I31/2-1</f>
         <v>1913903</v>
       </c>
-      <c r="T31" s="4">
-        <f>D31*E31</f>
-        <v>4096</v>
+      <c r="T31" s="18">
+        <f>U31/E31</f>
+        <v>23328</v>
       </c>
       <c r="U31" s="4">
+        <f>D31*I31</f>
+        <v>2985984</v>
+      </c>
+      <c r="V31" s="4">
         <v>0.52</v>
       </c>
-      <c r="V31" s="4">
-        <v>1</v>
-      </c>
       <c r="W31" s="4">
+        <v>1</v>
+      </c>
+      <c r="X31" s="4">
         <f>0.0000032*J31+0.0000064*I31</f>
         <v>0.71516159999999995</v>
       </c>
-      <c r="X31" s="4">
+      <c r="Y31" s="4">
         <f t="shared" si="14"/>
-        <v>2129.92</v>
-      </c>
-      <c r="Y31" s="4">
+        <v>1552711.6800000002</v>
+      </c>
+      <c r="Z31" s="4">
         <f t="shared" si="15"/>
-        <v>2129.92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+        <v>12130.560000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>33</v>
       </c>
@@ -2677,23 +2763,24 @@
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="22"/>
-      <c r="M32" s="22"/>
-      <c r="N32" s="22"/>
-      <c r="O32" s="22"/>
-      <c r="P32" s="22"/>
-      <c r="Q32" s="22"/>
-      <c r="R32" s="22"/>
-      <c r="S32" s="23"/>
-      <c r="T32" s="5"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="20"/>
+      <c r="N32" s="20"/>
+      <c r="O32" s="20"/>
+      <c r="P32" s="20"/>
+      <c r="Q32" s="20"/>
+      <c r="R32" s="20"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="20"/>
       <c r="U32" s="5"/>
       <c r="V32" s="5"/>
       <c r="W32" s="5"/>
       <c r="X32" s="5"/>
       <c r="Y32" s="5"/>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z32" s="5"/>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>34</v>
       </c>
@@ -2708,23 +2795,24 @@
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
-      <c r="K33" s="12"/>
-      <c r="L33" s="22"/>
-      <c r="M33" s="22"/>
-      <c r="N33" s="22"/>
-      <c r="O33" s="22"/>
-      <c r="P33" s="22"/>
-      <c r="Q33" s="22"/>
-      <c r="R33" s="22"/>
-      <c r="S33" s="23"/>
-      <c r="T33" s="5"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20"/>
+      <c r="N33" s="20"/>
+      <c r="O33" s="20"/>
+      <c r="P33" s="20"/>
+      <c r="Q33" s="20"/>
+      <c r="R33" s="20"/>
+      <c r="S33" s="21"/>
+      <c r="T33" s="20"/>
       <c r="U33" s="5"/>
       <c r="V33" s="5"/>
       <c r="W33" s="5"/>
       <c r="X33" s="5"/>
       <c r="Y33" s="5"/>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z33" s="5"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>35</v>
       </c>
@@ -2741,23 +2829,24 @@
       </c>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="18"/>
-      <c r="N34" s="18"/>
-      <c r="O34" s="18"/>
-      <c r="P34" s="18"/>
-      <c r="Q34" s="18"/>
-      <c r="R34" s="18"/>
-      <c r="S34" s="19"/>
-      <c r="T34" s="3"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="16"/>
+      <c r="S34" s="17"/>
+      <c r="T34" s="16"/>
       <c r="U34" s="3"/>
       <c r="V34" s="3"/>
       <c r="W34" s="3"/>
       <c r="X34" s="3"/>
       <c r="Y34" s="3"/>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z34" s="3"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>36</v>
       </c>
@@ -2768,7 +2857,9 @@
         <v>83</v>
       </c>
       <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
+      <c r="E35" s="6">
+        <v>256</v>
+      </c>
       <c r="F35" s="6">
         <v>2</v>
       </c>
@@ -2782,44 +2873,48 @@
         <v>43624</v>
       </c>
       <c r="J35" s="6"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="24"/>
-      <c r="M35" s="24"/>
-      <c r="N35" s="24"/>
-      <c r="O35" s="24"/>
-      <c r="P35" s="24"/>
-      <c r="Q35" s="24"/>
-      <c r="R35" s="24">
+      <c r="K35" s="12"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="22"/>
+      <c r="N35" s="22"/>
+      <c r="O35" s="22"/>
+      <c r="P35" s="22"/>
+      <c r="Q35" s="22"/>
+      <c r="R35" s="22">
         <f>S31+1</f>
         <v>1913904</v>
       </c>
-      <c r="S35" s="25">
+      <c r="S35" s="23">
         <f>R35+I35/2-1</f>
         <v>1935715</v>
       </c>
-      <c r="T35" s="6">
+      <c r="T35" s="22">
+        <f>U35/E35</f>
+        <v>169</v>
+      </c>
+      <c r="U35" s="6">
         <v>43264</v>
       </c>
-      <c r="U35" s="6">
+      <c r="V35" s="6">
         <v>0.31</v>
       </c>
-      <c r="V35" s="6">
-        <v>1</v>
-      </c>
       <c r="W35" s="6">
+        <v>1</v>
+      </c>
+      <c r="X35" s="6">
         <f>0.0000064*I35</f>
         <v>0.27919359999999999</v>
       </c>
-      <c r="X35" s="6">
-        <f>T35*U35</f>
+      <c r="Y35" s="6">
+        <f>U35*V35</f>
         <v>13411.84</v>
       </c>
-      <c r="Y35" s="6">
-        <f>T35*U35*V35</f>
-        <v>13411.84</v>
-      </c>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z35" s="6">
+        <f>T35*V35*W35</f>
+        <v>52.39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>37</v>
       </c>
@@ -2850,57 +2945,61 @@
       <c r="J36" s="4">
         <v>12288</v>
       </c>
-      <c r="K36" s="11"/>
-      <c r="L36" s="20">
+      <c r="K36" s="10"/>
+      <c r="L36" s="18">
         <f>L31+J31/2+E31/2</f>
         <v>64304</v>
       </c>
-      <c r="M36" s="20">
+      <c r="M36" s="18">
         <f>L36+J36/2-1</f>
         <v>70447</v>
       </c>
-      <c r="N36" s="20">
+      <c r="N36" s="18">
         <f>M36+1</f>
         <v>70448</v>
       </c>
-      <c r="O36" s="20">
+      <c r="O36" s="18">
         <f>N36+E36/2-1</f>
         <v>70471</v>
       </c>
-      <c r="P36" s="20"/>
-      <c r="Q36" s="20"/>
-      <c r="R36" s="20">
+      <c r="P36" s="18"/>
+      <c r="Q36" s="18"/>
+      <c r="R36" s="18">
         <f>S35+1</f>
         <v>1935716</v>
       </c>
-      <c r="S36" s="21">
+      <c r="S36" s="19">
         <f>R36+I36/2-1</f>
         <v>1939771</v>
       </c>
-      <c r="T36" s="4">
-        <f>D36*E36</f>
-        <v>12288</v>
+      <c r="T36" s="18">
+        <f>U36/E36</f>
+        <v>43264</v>
       </c>
       <c r="U36" s="4">
+        <f>D36*I36</f>
+        <v>2076672</v>
+      </c>
+      <c r="V36" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="V36" s="4">
-        <v>1</v>
-      </c>
       <c r="W36" s="4">
+        <v>1</v>
+      </c>
+      <c r="X36" s="4">
         <f>0.0000032*J36+0.0000064*I36</f>
         <v>9.1238399999999997E-2</v>
       </c>
-      <c r="X36" s="4">
-        <f>T36*U36</f>
-        <v>860.16000000000008</v>
-      </c>
       <c r="Y36" s="4">
-        <f>T36*U36*V36</f>
-        <v>860.16000000000008</v>
-      </c>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+        <f>U36*V36</f>
+        <v>145367.04000000001</v>
+      </c>
+      <c r="Z36" s="4">
+        <f>T36*V36*W36</f>
+        <v>3028.4800000000005</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>38</v>
       </c>
@@ -2915,23 +3014,24 @@
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
-      <c r="K37" s="12"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="22"/>
-      <c r="N37" s="22"/>
-      <c r="O37" s="22"/>
-      <c r="P37" s="22"/>
-      <c r="Q37" s="22"/>
-      <c r="R37" s="22"/>
-      <c r="S37" s="23"/>
-      <c r="T37" s="5"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="20"/>
+      <c r="N37" s="20"/>
+      <c r="O37" s="20"/>
+      <c r="P37" s="20"/>
+      <c r="Q37" s="20"/>
+      <c r="R37" s="20"/>
+      <c r="S37" s="21"/>
+      <c r="T37" s="20"/>
       <c r="U37" s="5"/>
       <c r="V37" s="5"/>
       <c r="W37" s="5"/>
       <c r="X37" s="5"/>
       <c r="Y37" s="5"/>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z37" s="5"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>39</v>
       </c>
@@ -2962,57 +3062,61 @@
       <c r="J38" s="4">
         <v>9216</v>
       </c>
-      <c r="K38" s="11"/>
-      <c r="L38" s="20">
+      <c r="K38" s="10"/>
+      <c r="L38" s="18">
         <f>L36+J36/2+E36/2</f>
         <v>70472</v>
       </c>
-      <c r="M38" s="20">
+      <c r="M38" s="18">
         <f t="shared" ref="M38:M39" si="16">L38+J38/2-1</f>
         <v>75079</v>
       </c>
-      <c r="N38" s="20">
+      <c r="N38" s="18">
         <f>M38+1</f>
         <v>75080</v>
       </c>
-      <c r="O38" s="20">
+      <c r="O38" s="18">
         <f>N38+E38/2-1</f>
         <v>75175</v>
       </c>
-      <c r="P38" s="20"/>
-      <c r="Q38" s="20"/>
-      <c r="R38" s="20">
+      <c r="P38" s="18"/>
+      <c r="Q38" s="18"/>
+      <c r="R38" s="18">
         <f>S36+1</f>
         <v>1939772</v>
       </c>
-      <c r="S38" s="21">
+      <c r="S38" s="19">
         <f>R38+I38/2-1</f>
         <v>1955995</v>
       </c>
-      <c r="T38" s="4">
-        <f>D38*E38</f>
-        <v>9216</v>
+      <c r="T38" s="18">
+        <f>U38/E38</f>
+        <v>8112</v>
       </c>
       <c r="U38" s="4">
+        <f>D38*I38</f>
+        <v>1557504</v>
+      </c>
+      <c r="V38" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="V38" s="4">
+      <c r="W38" s="4">
         <v>0</v>
       </c>
-      <c r="W38" s="4">
+      <c r="X38" s="4">
         <f>0.0000032*J38+0.0000064*I38</f>
         <v>0.23715839999999999</v>
       </c>
-      <c r="X38" s="4">
-        <f t="shared" ref="X38:X39" si="17">T38*U38</f>
-        <v>645.12000000000012</v>
-      </c>
       <c r="Y38" s="4">
-        <f t="shared" ref="Y38:Y39" si="18">T38*U38*V38</f>
+        <f t="shared" ref="Y38:Y39" si="17">U38*V38</f>
+        <v>109025.28000000001</v>
+      </c>
+      <c r="Z38" s="4">
+        <f t="shared" ref="Z38:Z39" si="18">T38*V38*W38</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>40</v>
       </c>
@@ -3043,57 +3147,61 @@
       <c r="J39" s="4">
         <v>82944</v>
       </c>
-      <c r="K39" s="11"/>
-      <c r="L39" s="20">
+      <c r="K39" s="10"/>
+      <c r="L39" s="18">
         <f>L38+J38/2+E38/2</f>
         <v>75176</v>
       </c>
-      <c r="M39" s="20">
+      <c r="M39" s="18">
         <f t="shared" si="16"/>
         <v>116647</v>
       </c>
-      <c r="N39" s="20">
+      <c r="N39" s="18">
         <f>M39+1</f>
         <v>116648</v>
       </c>
-      <c r="O39" s="20">
+      <c r="O39" s="18">
         <f>N39+E39/2-1</f>
         <v>116743</v>
       </c>
-      <c r="P39" s="20"/>
-      <c r="Q39" s="20"/>
-      <c r="R39" s="20">
+      <c r="P39" s="18"/>
+      <c r="Q39" s="18"/>
+      <c r="R39" s="18">
         <f>S38+1</f>
         <v>1955996</v>
       </c>
-      <c r="S39" s="21">
+      <c r="S39" s="19">
         <f>R39+I39/2-1</f>
         <v>1972219</v>
       </c>
-      <c r="T39" s="4">
-        <f>D39*E39</f>
-        <v>9216</v>
+      <c r="T39" s="18">
+        <f>U39/E39</f>
+        <v>8112</v>
       </c>
       <c r="U39" s="4">
+        <f>D39*I39</f>
+        <v>1557504</v>
+      </c>
+      <c r="V39" s="4">
         <v>0.52</v>
       </c>
-      <c r="V39" s="4">
-        <v>1</v>
-      </c>
       <c r="W39" s="4">
+        <v>1</v>
+      </c>
+      <c r="X39" s="4">
         <f>0.0000032*J39+0.0000064*I39</f>
         <v>0.47308800000000001</v>
       </c>
-      <c r="X39" s="4">
+      <c r="Y39" s="4">
         <f t="shared" si="17"/>
-        <v>4792.32</v>
-      </c>
-      <c r="Y39" s="4">
+        <v>809902.08000000007</v>
+      </c>
+      <c r="Z39" s="4">
         <f t="shared" si="18"/>
-        <v>4792.32</v>
-      </c>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+        <v>4218.24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>41</v>
       </c>
@@ -3108,23 +3216,24 @@
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
-      <c r="K40" s="12"/>
-      <c r="L40" s="22"/>
-      <c r="M40" s="22"/>
-      <c r="N40" s="22"/>
-      <c r="O40" s="22"/>
-      <c r="P40" s="22"/>
-      <c r="Q40" s="22"/>
-      <c r="R40" s="22"/>
-      <c r="S40" s="23"/>
-      <c r="T40" s="5"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="20"/>
+      <c r="M40" s="20"/>
+      <c r="N40" s="20"/>
+      <c r="O40" s="20"/>
+      <c r="P40" s="20"/>
+      <c r="Q40" s="20"/>
+      <c r="R40" s="20"/>
+      <c r="S40" s="21"/>
+      <c r="T40" s="20"/>
       <c r="U40" s="5"/>
       <c r="V40" s="5"/>
       <c r="W40" s="5"/>
       <c r="X40" s="5"/>
       <c r="Y40" s="5"/>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z40" s="5"/>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>42</v>
       </c>
@@ -3139,23 +3248,24 @@
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
-      <c r="K41" s="12"/>
-      <c r="L41" s="22"/>
-      <c r="M41" s="22"/>
-      <c r="N41" s="22"/>
-      <c r="O41" s="22"/>
-      <c r="P41" s="22"/>
-      <c r="Q41" s="22"/>
-      <c r="R41" s="22"/>
-      <c r="S41" s="23"/>
-      <c r="T41" s="5"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="20"/>
+      <c r="M41" s="20"/>
+      <c r="N41" s="20"/>
+      <c r="O41" s="20"/>
+      <c r="P41" s="20"/>
+      <c r="Q41" s="20"/>
+      <c r="R41" s="20"/>
+      <c r="S41" s="21"/>
+      <c r="T41" s="20"/>
       <c r="U41" s="5"/>
       <c r="V41" s="5"/>
       <c r="W41" s="5"/>
       <c r="X41" s="5"/>
       <c r="Y41" s="5"/>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z41" s="5"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>43</v>
       </c>
@@ -3172,23 +3282,24 @@
       </c>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
-      <c r="K42" s="10"/>
-      <c r="L42" s="18"/>
-      <c r="M42" s="18"/>
-      <c r="N42" s="18"/>
-      <c r="O42" s="18"/>
-      <c r="P42" s="18"/>
-      <c r="Q42" s="18"/>
-      <c r="R42" s="18"/>
-      <c r="S42" s="19"/>
-      <c r="T42" s="3"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="16"/>
+      <c r="M42" s="16"/>
+      <c r="N42" s="16"/>
+      <c r="O42" s="16"/>
+      <c r="P42" s="16"/>
+      <c r="Q42" s="16"/>
+      <c r="R42" s="16"/>
+      <c r="S42" s="17"/>
+      <c r="T42" s="16"/>
       <c r="U42" s="3"/>
       <c r="V42" s="3"/>
       <c r="W42" s="3"/>
       <c r="X42" s="3"/>
       <c r="Y42" s="3"/>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z42" s="3"/>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>44</v>
       </c>
@@ -3219,57 +3330,61 @@
       <c r="J43" s="4">
         <v>18432</v>
       </c>
-      <c r="K43" s="11"/>
-      <c r="L43" s="20">
+      <c r="K43" s="10"/>
+      <c r="L43" s="18">
         <f>L39+J39/2+E39/2</f>
         <v>116744</v>
       </c>
-      <c r="M43" s="20">
+      <c r="M43" s="18">
         <f>L43+J43/2-1</f>
         <v>125959</v>
       </c>
-      <c r="N43" s="20">
+      <c r="N43" s="18">
         <f>M43+1</f>
         <v>125960</v>
       </c>
-      <c r="O43" s="20">
+      <c r="O43" s="18">
         <f>N43+E43/2-1</f>
         <v>125983</v>
       </c>
-      <c r="P43" s="20"/>
-      <c r="Q43" s="20"/>
-      <c r="R43" s="20">
+      <c r="P43" s="18"/>
+      <c r="Q43" s="18"/>
+      <c r="R43" s="18">
         <f>S39+1</f>
         <v>1972220</v>
       </c>
-      <c r="S43" s="21">
+      <c r="S43" s="19">
         <f>R43+I43/2-1</f>
         <v>1976275</v>
       </c>
-      <c r="T43" s="4">
-        <f>D43*E43</f>
-        <v>18432</v>
+      <c r="T43" s="18">
+        <f>U43/E43</f>
+        <v>64896</v>
       </c>
       <c r="U43" s="4">
+        <f>D43*I43</f>
+        <v>3115008</v>
+      </c>
+      <c r="V43" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="V43" s="4">
-        <v>1</v>
-      </c>
       <c r="W43" s="4">
+        <v>1</v>
+      </c>
+      <c r="X43" s="4">
         <f>0.0000032*J43+0.0000064*I43</f>
         <v>0.1108992</v>
       </c>
-      <c r="X43" s="4">
-        <f>T43*U43</f>
-        <v>1290.2400000000002</v>
-      </c>
       <c r="Y43" s="4">
-        <f>T43*U43*V43</f>
-        <v>1290.2400000000002</v>
-      </c>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+        <f>U43*V43</f>
+        <v>218050.56000000003</v>
+      </c>
+      <c r="Z43" s="4">
+        <f>T43*V43*W43</f>
+        <v>4542.72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>45</v>
       </c>
@@ -3284,23 +3399,24 @@
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
-      <c r="K44" s="12"/>
-      <c r="L44" s="22"/>
-      <c r="M44" s="22"/>
-      <c r="N44" s="22"/>
-      <c r="O44" s="22"/>
-      <c r="P44" s="22"/>
-      <c r="Q44" s="22"/>
-      <c r="R44" s="22"/>
-      <c r="S44" s="23"/>
-      <c r="T44" s="5"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="20"/>
+      <c r="M44" s="20"/>
+      <c r="N44" s="20"/>
+      <c r="O44" s="20"/>
+      <c r="P44" s="20"/>
+      <c r="Q44" s="20"/>
+      <c r="R44" s="20"/>
+      <c r="S44" s="21"/>
+      <c r="T44" s="20"/>
       <c r="U44" s="5"/>
       <c r="V44" s="5"/>
       <c r="W44" s="5"/>
       <c r="X44" s="5"/>
       <c r="Y44" s="5"/>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z44" s="5"/>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>46</v>
       </c>
@@ -3331,57 +3447,61 @@
       <c r="J45" s="4">
         <v>9216</v>
       </c>
-      <c r="K45" s="11"/>
-      <c r="L45" s="20">
+      <c r="K45" s="10"/>
+      <c r="L45" s="18">
         <f>L43+J43/2+E43/2</f>
         <v>125984</v>
       </c>
-      <c r="M45" s="20">
+      <c r="M45" s="18">
         <f t="shared" ref="M45:M46" si="19">L45+J45/2-1</f>
         <v>130591</v>
       </c>
-      <c r="N45" s="20">
+      <c r="N45" s="18">
         <f t="shared" ref="N45:N46" si="20">M45+1</f>
         <v>130592</v>
       </c>
-      <c r="O45" s="20">
+      <c r="O45" s="18">
         <f>N45+E45/2-1</f>
         <v>130687</v>
       </c>
-      <c r="P45" s="20"/>
-      <c r="Q45" s="20"/>
-      <c r="R45" s="20">
+      <c r="P45" s="18"/>
+      <c r="Q45" s="18"/>
+      <c r="R45" s="18">
         <f>S43+1</f>
         <v>1976276</v>
       </c>
-      <c r="S45" s="21">
+      <c r="S45" s="19">
         <f>R45+I45/2-1</f>
         <v>1992499</v>
       </c>
-      <c r="T45" s="4">
-        <f>D45*E45</f>
-        <v>9216</v>
+      <c r="T45" s="18">
+        <f>U45/E45</f>
+        <v>8112</v>
       </c>
       <c r="U45" s="4">
+        <f>D45*I45</f>
+        <v>1557504</v>
+      </c>
+      <c r="V45" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="V45" s="4">
+      <c r="W45" s="4">
         <v>0</v>
       </c>
-      <c r="W45" s="4">
+      <c r="X45" s="4">
         <f>0.0000032*J45+0.0000064*I45</f>
         <v>0.23715839999999999</v>
       </c>
-      <c r="X45" s="4">
-        <f t="shared" ref="X45:X46" si="21">T45*U45</f>
-        <v>645.12000000000012</v>
-      </c>
       <c r="Y45" s="4">
-        <f t="shared" ref="Y45:Y46" si="22">T45*U45*V45</f>
+        <f t="shared" ref="Y45:Y46" si="21">U45*V45</f>
+        <v>109025.28000000001</v>
+      </c>
+      <c r="Z45" s="4">
+        <f t="shared" ref="Z45:Z46" si="22">T45*V45*W45</f>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>47</v>
       </c>
@@ -3412,57 +3532,61 @@
       <c r="J46" s="4">
         <v>82944</v>
       </c>
-      <c r="K46" s="11"/>
-      <c r="L46" s="20">
+      <c r="K46" s="10"/>
+      <c r="L46" s="18">
         <f>L45+J45/2+E45/2</f>
         <v>130688</v>
       </c>
-      <c r="M46" s="20">
+      <c r="M46" s="18">
         <f t="shared" si="19"/>
         <v>172159</v>
       </c>
-      <c r="N46" s="20">
+      <c r="N46" s="18">
         <f t="shared" si="20"/>
         <v>172160</v>
       </c>
-      <c r="O46" s="20">
+      <c r="O46" s="18">
         <f>N46+E46/2-1</f>
         <v>172255</v>
       </c>
-      <c r="P46" s="20"/>
-      <c r="Q46" s="20"/>
-      <c r="R46" s="20">
+      <c r="P46" s="18"/>
+      <c r="Q46" s="18"/>
+      <c r="R46" s="18">
         <f>S45+1</f>
         <v>1992500</v>
       </c>
-      <c r="S46" s="21">
+      <c r="S46" s="19">
         <f>R46+I46/2-1</f>
         <v>2008723</v>
       </c>
-      <c r="T46" s="4">
-        <f>D46*E46</f>
-        <v>9216</v>
+      <c r="T46" s="18">
+        <f>U46/E46</f>
+        <v>8112</v>
       </c>
       <c r="U46" s="4">
+        <f>D46*I46</f>
+        <v>1557504</v>
+      </c>
+      <c r="V46" s="4">
         <v>0.52</v>
       </c>
-      <c r="V46" s="4">
-        <v>1</v>
-      </c>
       <c r="W46" s="4">
+        <v>1</v>
+      </c>
+      <c r="X46" s="4">
         <f>0.0000032*J46+0.0000064*I46</f>
         <v>0.47308800000000001</v>
       </c>
-      <c r="X46" s="4">
+      <c r="Y46" s="4">
         <f t="shared" si="21"/>
-        <v>4792.32</v>
-      </c>
-      <c r="Y46" s="4">
+        <v>809902.08000000007</v>
+      </c>
+      <c r="Z46" s="4">
         <f t="shared" si="22"/>
-        <v>4792.32</v>
-      </c>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+        <v>4218.24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>48</v>
       </c>
@@ -3477,23 +3601,24 @@
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
-      <c r="K47" s="12"/>
-      <c r="L47" s="22"/>
-      <c r="M47" s="22"/>
-      <c r="N47" s="22"/>
-      <c r="O47" s="22"/>
-      <c r="P47" s="22"/>
-      <c r="Q47" s="22"/>
-      <c r="R47" s="22"/>
-      <c r="S47" s="23"/>
-      <c r="T47" s="5"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="20"/>
+      <c r="M47" s="20"/>
+      <c r="N47" s="20"/>
+      <c r="O47" s="20"/>
+      <c r="P47" s="20"/>
+      <c r="Q47" s="20"/>
+      <c r="R47" s="20"/>
+      <c r="S47" s="21"/>
+      <c r="T47" s="20"/>
       <c r="U47" s="5"/>
       <c r="V47" s="5"/>
       <c r="W47" s="5"/>
       <c r="X47" s="5"/>
       <c r="Y47" s="5"/>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z47" s="5"/>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>49</v>
       </c>
@@ -3508,23 +3633,24 @@
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
-      <c r="K48" s="12"/>
-      <c r="L48" s="22"/>
-      <c r="M48" s="22"/>
-      <c r="N48" s="22"/>
-      <c r="O48" s="22"/>
-      <c r="P48" s="22"/>
-      <c r="Q48" s="22"/>
-      <c r="R48" s="22"/>
-      <c r="S48" s="23"/>
-      <c r="T48" s="5"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="20"/>
+      <c r="M48" s="20"/>
+      <c r="N48" s="20"/>
+      <c r="O48" s="20"/>
+      <c r="P48" s="20"/>
+      <c r="Q48" s="20"/>
+      <c r="R48" s="20"/>
+      <c r="S48" s="21"/>
+      <c r="T48" s="20"/>
       <c r="U48" s="5"/>
       <c r="V48" s="5"/>
       <c r="W48" s="5"/>
       <c r="X48" s="5"/>
       <c r="Y48" s="5"/>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z48" s="5"/>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>50</v>
       </c>
@@ -3541,23 +3667,24 @@
       </c>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
-      <c r="K49" s="10"/>
-      <c r="L49" s="18"/>
-      <c r="M49" s="18"/>
-      <c r="N49" s="18"/>
-      <c r="O49" s="18"/>
-      <c r="P49" s="18"/>
-      <c r="Q49" s="18"/>
-      <c r="R49" s="18"/>
-      <c r="S49" s="19"/>
-      <c r="T49" s="3"/>
+      <c r="K49" s="9"/>
+      <c r="L49" s="16"/>
+      <c r="M49" s="16"/>
+      <c r="N49" s="16"/>
+      <c r="O49" s="16"/>
+      <c r="P49" s="16"/>
+      <c r="Q49" s="16"/>
+      <c r="R49" s="16"/>
+      <c r="S49" s="17"/>
+      <c r="T49" s="16"/>
       <c r="U49" s="3"/>
       <c r="V49" s="3"/>
       <c r="W49" s="3"/>
       <c r="X49" s="3"/>
       <c r="Y49" s="3"/>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z49" s="3"/>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>51</v>
       </c>
@@ -3588,57 +3715,61 @@
       <c r="J50" s="4">
         <v>24576</v>
       </c>
-      <c r="K50" s="11"/>
-      <c r="L50" s="20">
+      <c r="K50" s="10"/>
+      <c r="L50" s="18">
         <f>L46+J46/2+E46/2</f>
         <v>172256</v>
       </c>
-      <c r="M50" s="20">
+      <c r="M50" s="18">
         <f>L50+J50/2-1</f>
         <v>184543</v>
       </c>
-      <c r="N50" s="20">
+      <c r="N50" s="18">
         <f>M50+1</f>
         <v>184544</v>
       </c>
-      <c r="O50" s="20">
+      <c r="O50" s="18">
         <f>N50+E50/2-1</f>
         <v>184575</v>
       </c>
-      <c r="P50" s="20"/>
-      <c r="Q50" s="20"/>
-      <c r="R50" s="20">
+      <c r="P50" s="18"/>
+      <c r="Q50" s="18"/>
+      <c r="R50" s="18">
         <f>S46+1</f>
         <v>2008724</v>
       </c>
-      <c r="S50" s="21">
+      <c r="S50" s="19">
         <f>R50+I50/2-1</f>
         <v>2014131</v>
       </c>
-      <c r="T50" s="4">
-        <f>D50*E50</f>
-        <v>24576</v>
+      <c r="T50" s="18">
+        <f>U50/E50</f>
+        <v>64896</v>
       </c>
       <c r="U50" s="4">
+        <f>D50*I50</f>
+        <v>4153344</v>
+      </c>
+      <c r="V50" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="V50" s="4">
-        <v>1</v>
-      </c>
       <c r="W50" s="4">
+        <v>1</v>
+      </c>
+      <c r="X50" s="4">
         <f>0.0000032*J50+0.0000064*I50</f>
         <v>0.14786559999999999</v>
       </c>
-      <c r="X50" s="4">
-        <f>T50*U50</f>
-        <v>1720.3200000000002</v>
-      </c>
       <c r="Y50" s="4">
-        <f>T50*U50*V50</f>
-        <v>1720.3200000000002</v>
-      </c>
-    </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+        <f>U50*V50</f>
+        <v>290734.08000000002</v>
+      </c>
+      <c r="Z50" s="4">
+        <f>T50*V50*W50</f>
+        <v>4542.72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>52</v>
       </c>
@@ -3653,23 +3784,24 @@
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
-      <c r="K51" s="12"/>
-      <c r="L51" s="22"/>
-      <c r="M51" s="22"/>
-      <c r="N51" s="22"/>
-      <c r="O51" s="22"/>
-      <c r="P51" s="22"/>
-      <c r="Q51" s="22"/>
-      <c r="R51" s="22"/>
-      <c r="S51" s="23"/>
-      <c r="T51" s="5"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="20"/>
+      <c r="M51" s="20"/>
+      <c r="N51" s="20"/>
+      <c r="O51" s="20"/>
+      <c r="P51" s="20"/>
+      <c r="Q51" s="20"/>
+      <c r="R51" s="20"/>
+      <c r="S51" s="21"/>
+      <c r="T51" s="20"/>
       <c r="U51" s="5"/>
       <c r="V51" s="5"/>
       <c r="W51" s="5"/>
       <c r="X51" s="5"/>
       <c r="Y51" s="5"/>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z51" s="5"/>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>53</v>
       </c>
@@ -3700,57 +3832,61 @@
       <c r="J52" s="4">
         <v>16384</v>
       </c>
-      <c r="K52" s="11"/>
-      <c r="L52" s="20">
+      <c r="K52" s="10"/>
+      <c r="L52" s="18">
         <f>L50+J50/2+E50/2</f>
         <v>184576</v>
       </c>
-      <c r="M52" s="20">
+      <c r="M52" s="18">
         <f t="shared" ref="M52:M53" si="23">L52+J52/2-1</f>
         <v>192767</v>
       </c>
-      <c r="N52" s="20">
+      <c r="N52" s="18">
         <f t="shared" ref="N52:N53" si="24">M52+1</f>
         <v>192768</v>
       </c>
-      <c r="O52" s="20">
+      <c r="O52" s="18">
         <f>N52+E52/2-1</f>
         <v>192895</v>
       </c>
-      <c r="P52" s="20"/>
-      <c r="Q52" s="20"/>
-      <c r="R52" s="20">
+      <c r="P52" s="18"/>
+      <c r="Q52" s="18"/>
+      <c r="R52" s="18">
         <f>S50+1</f>
         <v>2014132</v>
       </c>
-      <c r="S52" s="21">
+      <c r="S52" s="19">
         <f>R52+I52/2-1</f>
         <v>2035763</v>
       </c>
-      <c r="T52" s="4">
-        <f>D52*E52</f>
-        <v>16384</v>
+      <c r="T52" s="18">
+        <f>U52/E52</f>
+        <v>10816</v>
       </c>
       <c r="U52" s="4">
+        <f>D52*I52</f>
+        <v>2768896</v>
+      </c>
+      <c r="V52" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="V52" s="4">
+      <c r="W52" s="4">
         <v>0</v>
       </c>
-      <c r="W52" s="4">
+      <c r="X52" s="4">
         <f>0.0000032*J52+0.0000064*I52</f>
         <v>0.32931840000000001</v>
       </c>
-      <c r="X52" s="4">
-        <f t="shared" ref="X52:X53" si="25">T52*U52</f>
-        <v>1146.8800000000001</v>
-      </c>
       <c r="Y52" s="4">
-        <f t="shared" ref="Y52:Y53" si="26">T52*U52*V52</f>
+        <f t="shared" ref="Y52:Y53" si="25">U52*V52</f>
+        <v>193822.72000000003</v>
+      </c>
+      <c r="Z52" s="4">
+        <f t="shared" ref="Z52:Z53" si="26">T52*V52*W52</f>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>54</v>
       </c>
@@ -3781,57 +3917,61 @@
       <c r="J53" s="4">
         <v>147456</v>
       </c>
-      <c r="K53" s="11"/>
-      <c r="L53" s="20">
+      <c r="K53" s="10"/>
+      <c r="L53" s="18">
         <f>L52+J52/2+E52/2</f>
         <v>192896</v>
       </c>
-      <c r="M53" s="20">
+      <c r="M53" s="18">
         <f t="shared" si="23"/>
         <v>266623</v>
       </c>
-      <c r="N53" s="20">
+      <c r="N53" s="18">
         <f t="shared" si="24"/>
         <v>266624</v>
       </c>
-      <c r="O53" s="20">
+      <c r="O53" s="18">
         <f>N53+E53/2-1</f>
         <v>266751</v>
       </c>
-      <c r="P53" s="20"/>
-      <c r="Q53" s="20"/>
-      <c r="R53" s="20">
+      <c r="P53" s="18"/>
+      <c r="Q53" s="18"/>
+      <c r="R53" s="18">
         <f>S52+1</f>
         <v>2035764</v>
       </c>
-      <c r="S53" s="21">
+      <c r="S53" s="19">
         <f>R53+I53/2-1</f>
         <v>2057395</v>
       </c>
-      <c r="T53" s="4">
-        <f>D53*E53</f>
-        <v>16384</v>
+      <c r="T53" s="18">
+        <f>U53/E52</f>
+        <v>10816</v>
       </c>
       <c r="U53" s="4">
+        <f>D53*I53</f>
+        <v>2768896</v>
+      </c>
+      <c r="V53" s="4">
         <v>0.52</v>
       </c>
-      <c r="V53" s="4">
-        <v>1</v>
-      </c>
       <c r="W53" s="4">
+        <v>1</v>
+      </c>
+      <c r="X53" s="4">
         <f>0.0000032*J53+0.0000064*I53</f>
         <v>0.74874879999999999</v>
       </c>
-      <c r="X53" s="4">
+      <c r="Y53" s="4">
         <f t="shared" si="25"/>
-        <v>8519.68</v>
-      </c>
-      <c r="Y53" s="4">
+        <v>1439825.9200000002</v>
+      </c>
+      <c r="Z53" s="4">
         <f t="shared" si="26"/>
-        <v>8519.68</v>
-      </c>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+        <v>5624.3200000000006</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>55</v>
       </c>
@@ -3846,23 +3986,24 @@
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
-      <c r="K54" s="12"/>
-      <c r="L54" s="22"/>
-      <c r="M54" s="22"/>
-      <c r="N54" s="22"/>
-      <c r="O54" s="22"/>
-      <c r="P54" s="22"/>
-      <c r="Q54" s="22"/>
-      <c r="R54" s="22"/>
-      <c r="S54" s="23"/>
-      <c r="T54" s="5"/>
+      <c r="K54" s="11"/>
+      <c r="L54" s="20"/>
+      <c r="M54" s="20"/>
+      <c r="N54" s="20"/>
+      <c r="O54" s="20"/>
+      <c r="P54" s="20"/>
+      <c r="Q54" s="20"/>
+      <c r="R54" s="20"/>
+      <c r="S54" s="21"/>
+      <c r="T54" s="20"/>
       <c r="U54" s="5"/>
       <c r="V54" s="5"/>
       <c r="W54" s="5"/>
       <c r="X54" s="5"/>
       <c r="Y54" s="5"/>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z54" s="5"/>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>56</v>
       </c>
@@ -3877,23 +4018,24 @@
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
-      <c r="K55" s="12"/>
-      <c r="L55" s="22"/>
-      <c r="M55" s="22"/>
-      <c r="N55" s="22"/>
-      <c r="O55" s="22"/>
-      <c r="P55" s="22"/>
-      <c r="Q55" s="22"/>
-      <c r="R55" s="22"/>
-      <c r="S55" s="23"/>
-      <c r="T55" s="5"/>
+      <c r="K55" s="11"/>
+      <c r="L55" s="20"/>
+      <c r="M55" s="20"/>
+      <c r="N55" s="20"/>
+      <c r="O55" s="20"/>
+      <c r="P55" s="20"/>
+      <c r="Q55" s="20"/>
+      <c r="R55" s="20"/>
+      <c r="S55" s="21"/>
+      <c r="T55" s="20"/>
       <c r="U55" s="5"/>
       <c r="V55" s="5"/>
       <c r="W55" s="5"/>
       <c r="X55" s="5"/>
       <c r="Y55" s="5"/>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z55" s="5"/>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>57</v>
       </c>
@@ -3910,23 +4052,24 @@
       </c>
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
-      <c r="K56" s="10"/>
-      <c r="L56" s="18"/>
-      <c r="M56" s="18"/>
-      <c r="N56" s="18"/>
-      <c r="O56" s="18"/>
-      <c r="P56" s="18"/>
-      <c r="Q56" s="18"/>
-      <c r="R56" s="18"/>
-      <c r="S56" s="19"/>
-      <c r="T56" s="3"/>
+      <c r="K56" s="9"/>
+      <c r="L56" s="16"/>
+      <c r="M56" s="16"/>
+      <c r="N56" s="16"/>
+      <c r="O56" s="16"/>
+      <c r="P56" s="16"/>
+      <c r="Q56" s="16"/>
+      <c r="R56" s="16"/>
+      <c r="S56" s="17"/>
+      <c r="T56" s="16"/>
       <c r="U56" s="3"/>
       <c r="V56" s="3"/>
       <c r="W56" s="3"/>
       <c r="X56" s="3"/>
       <c r="Y56" s="3"/>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z56" s="3"/>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>58</v>
       </c>
@@ -3957,57 +4100,61 @@
       <c r="J57" s="4">
         <v>32768</v>
       </c>
-      <c r="K57" s="11"/>
-      <c r="L57" s="20">
+      <c r="K57" s="10"/>
+      <c r="L57" s="18">
         <f>L53+J53/2+E53/2</f>
         <v>266752</v>
       </c>
-      <c r="M57" s="20">
+      <c r="M57" s="18">
         <f>L57+J57/2-1</f>
         <v>283135</v>
       </c>
-      <c r="N57" s="20">
+      <c r="N57" s="18">
         <f>M57+1</f>
         <v>283136</v>
       </c>
-      <c r="O57" s="20">
+      <c r="O57" s="18">
         <f>N57+E57/2-1</f>
         <v>283167</v>
       </c>
-      <c r="P57" s="20"/>
-      <c r="Q57" s="20"/>
-      <c r="R57" s="20">
+      <c r="P57" s="18"/>
+      <c r="Q57" s="18"/>
+      <c r="R57" s="18">
         <f>S53+1</f>
         <v>2057396</v>
       </c>
-      <c r="S57" s="21">
+      <c r="S57" s="19">
         <f>R57+I57/2-1</f>
         <v>2062803</v>
       </c>
-      <c r="T57" s="4">
-        <f>D57*E57</f>
-        <v>32768</v>
+      <c r="T57" s="18">
+        <f>U57/E57</f>
+        <v>86528</v>
       </c>
       <c r="U57" s="4">
+        <f>D57*I57</f>
+        <v>5537792</v>
+      </c>
+      <c r="V57" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="V57" s="4">
-        <v>1</v>
-      </c>
       <c r="W57" s="4">
+        <v>1</v>
+      </c>
+      <c r="X57" s="4">
         <f>0.0000032*J57+0.0000064*I57</f>
         <v>0.17408000000000001</v>
       </c>
-      <c r="X57" s="4">
-        <f>T57*U57</f>
-        <v>2293.7600000000002</v>
-      </c>
       <c r="Y57" s="4">
-        <f>T57*U57*V57</f>
-        <v>2293.7600000000002</v>
-      </c>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+        <f>U57*V57</f>
+        <v>387645.44000000006</v>
+      </c>
+      <c r="Z57" s="4">
+        <f>T57*V57*W57</f>
+        <v>6056.9600000000009</v>
+      </c>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>59</v>
       </c>
@@ -4022,23 +4169,24 @@
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
       <c r="J58" s="5"/>
-      <c r="K58" s="12"/>
-      <c r="L58" s="22"/>
-      <c r="M58" s="22"/>
-      <c r="N58" s="22"/>
-      <c r="O58" s="22"/>
-      <c r="P58" s="22"/>
-      <c r="Q58" s="22"/>
-      <c r="R58" s="22"/>
-      <c r="S58" s="23"/>
-      <c r="T58" s="5"/>
+      <c r="K58" s="11"/>
+      <c r="L58" s="20"/>
+      <c r="M58" s="20"/>
+      <c r="N58" s="20"/>
+      <c r="O58" s="20"/>
+      <c r="P58" s="20"/>
+      <c r="Q58" s="20"/>
+      <c r="R58" s="20"/>
+      <c r="S58" s="21"/>
+      <c r="T58" s="20"/>
       <c r="U58" s="5"/>
       <c r="V58" s="5"/>
       <c r="W58" s="5"/>
       <c r="X58" s="5"/>
       <c r="Y58" s="5"/>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z58" s="5"/>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>60</v>
       </c>
@@ -4069,57 +4217,61 @@
       <c r="J59" s="4">
         <v>16384</v>
       </c>
-      <c r="K59" s="11"/>
-      <c r="L59" s="20">
+      <c r="K59" s="10"/>
+      <c r="L59" s="18">
         <f>L57+J57/2+E57/2</f>
         <v>283168</v>
       </c>
-      <c r="M59" s="20">
+      <c r="M59" s="18">
         <f t="shared" ref="M59:M60" si="27">L59+J59/2-1</f>
         <v>291359</v>
       </c>
-      <c r="N59" s="20">
+      <c r="N59" s="18">
         <f t="shared" ref="N59:N60" si="28">M59+1</f>
         <v>291360</v>
       </c>
-      <c r="O59" s="20">
+      <c r="O59" s="18">
         <f>N59+E59/2-1</f>
         <v>291487</v>
       </c>
-      <c r="P59" s="20"/>
-      <c r="Q59" s="20"/>
-      <c r="R59" s="20">
+      <c r="P59" s="18"/>
+      <c r="Q59" s="18"/>
+      <c r="R59" s="18">
         <f>S57+1</f>
         <v>2062804</v>
       </c>
-      <c r="S59" s="21">
+      <c r="S59" s="19">
         <f>R59+I59/2-1</f>
         <v>2084435</v>
       </c>
-      <c r="T59" s="4">
-        <f>D59*E59</f>
-        <v>16384</v>
+      <c r="T59" s="18">
+        <f>U59/E59</f>
+        <v>10816</v>
       </c>
       <c r="U59" s="4">
+        <f>D59*I59</f>
+        <v>2768896</v>
+      </c>
+      <c r="V59" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="V59" s="4">
+      <c r="W59" s="4">
         <v>0</v>
       </c>
-      <c r="W59" s="4">
+      <c r="X59" s="4">
         <f>0.0000032*J59+0.0000064*I59</f>
         <v>0.32931840000000001</v>
       </c>
-      <c r="X59" s="4">
-        <f t="shared" ref="X59:X60" si="29">T59*U59</f>
-        <v>1146.8800000000001</v>
-      </c>
       <c r="Y59" s="4">
-        <f t="shared" ref="Y59:Y60" si="30">T59*U59*V59</f>
+        <f t="shared" ref="Y59:Y60" si="29">U59*V59</f>
+        <v>193822.72000000003</v>
+      </c>
+      <c r="Z59" s="4">
+        <f t="shared" ref="Z59:Z60" si="30">T59*V59*W59</f>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>61</v>
       </c>
@@ -4150,57 +4302,61 @@
       <c r="J60" s="4">
         <v>147456</v>
       </c>
-      <c r="K60" s="11"/>
-      <c r="L60" s="20">
+      <c r="K60" s="10"/>
+      <c r="L60" s="18">
         <f>L59+J59/2+E59/2</f>
         <v>291488</v>
       </c>
-      <c r="M60" s="20">
+      <c r="M60" s="18">
         <f t="shared" si="27"/>
         <v>365215</v>
       </c>
-      <c r="N60" s="20">
+      <c r="N60" s="18">
         <f t="shared" si="28"/>
         <v>365216</v>
       </c>
-      <c r="O60" s="20">
+      <c r="O60" s="18">
         <f>N60+E60/2-1</f>
         <v>365343</v>
       </c>
-      <c r="P60" s="20"/>
-      <c r="Q60" s="20"/>
-      <c r="R60" s="20">
+      <c r="P60" s="18"/>
+      <c r="Q60" s="18"/>
+      <c r="R60" s="18">
         <f>S59+1</f>
         <v>2084436</v>
       </c>
-      <c r="S60" s="21">
+      <c r="S60" s="19">
         <f>R60+I60/2-1</f>
         <v>2106067</v>
       </c>
-      <c r="T60" s="4">
-        <f>D60*E60</f>
-        <v>16384</v>
+      <c r="T60" s="18">
+        <f>U60/E60</f>
+        <v>10816</v>
       </c>
       <c r="U60" s="4">
+        <f>D60*I60</f>
+        <v>2768896</v>
+      </c>
+      <c r="V60" s="4">
         <v>0.52</v>
       </c>
-      <c r="V60" s="4">
-        <v>1</v>
-      </c>
       <c r="W60" s="4">
+        <v>1</v>
+      </c>
+      <c r="X60" s="4">
         <f>0.0000032*J60+0.0000064*I60</f>
         <v>0.74874879999999999</v>
       </c>
-      <c r="X60" s="4">
+      <c r="Y60" s="4">
         <f t="shared" si="29"/>
-        <v>8519.68</v>
-      </c>
-      <c r="Y60" s="4">
+        <v>1439825.9200000002</v>
+      </c>
+      <c r="Z60" s="4">
         <f t="shared" si="30"/>
-        <v>8519.68</v>
-      </c>
-    </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+        <v>5624.3200000000006</v>
+      </c>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>62</v>
       </c>
@@ -4215,23 +4371,24 @@
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
-      <c r="K61" s="12"/>
-      <c r="L61" s="22"/>
-      <c r="M61" s="22"/>
-      <c r="N61" s="22"/>
-      <c r="O61" s="22"/>
-      <c r="P61" s="22"/>
-      <c r="Q61" s="22"/>
-      <c r="R61" s="22"/>
-      <c r="S61" s="23"/>
-      <c r="T61" s="5"/>
+      <c r="K61" s="11"/>
+      <c r="L61" s="20"/>
+      <c r="M61" s="20"/>
+      <c r="N61" s="20"/>
+      <c r="O61" s="20"/>
+      <c r="P61" s="20"/>
+      <c r="Q61" s="20"/>
+      <c r="R61" s="20"/>
+      <c r="S61" s="21"/>
+      <c r="T61" s="20"/>
       <c r="U61" s="5"/>
       <c r="V61" s="5"/>
       <c r="W61" s="5"/>
       <c r="X61" s="5"/>
       <c r="Y61" s="5"/>
-    </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z61" s="5"/>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>63</v>
       </c>
@@ -4246,23 +4403,24 @@
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
       <c r="J62" s="5"/>
-      <c r="K62" s="12"/>
-      <c r="L62" s="22"/>
-      <c r="M62" s="22"/>
-      <c r="N62" s="22"/>
-      <c r="O62" s="22"/>
-      <c r="P62" s="22"/>
-      <c r="Q62" s="22"/>
-      <c r="R62" s="22"/>
-      <c r="S62" s="23"/>
-      <c r="T62" s="5"/>
+      <c r="K62" s="11"/>
+      <c r="L62" s="20"/>
+      <c r="M62" s="20"/>
+      <c r="N62" s="20"/>
+      <c r="O62" s="20"/>
+      <c r="P62" s="20"/>
+      <c r="Q62" s="20"/>
+      <c r="R62" s="20"/>
+      <c r="S62" s="21"/>
+      <c r="T62" s="20"/>
       <c r="U62" s="5"/>
       <c r="V62" s="5"/>
       <c r="W62" s="5"/>
       <c r="X62" s="5"/>
       <c r="Y62" s="5"/>
-    </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z62" s="5"/>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>64</v>
       </c>
@@ -4279,23 +4437,24 @@
       </c>
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
-      <c r="K63" s="10"/>
-      <c r="L63" s="18"/>
-      <c r="M63" s="18"/>
-      <c r="N63" s="18"/>
-      <c r="O63" s="18"/>
-      <c r="P63" s="18"/>
-      <c r="Q63" s="18"/>
-      <c r="R63" s="18"/>
-      <c r="S63" s="19"/>
-      <c r="T63" s="3"/>
+      <c r="K63" s="9"/>
+      <c r="L63" s="16"/>
+      <c r="M63" s="16"/>
+      <c r="N63" s="16"/>
+      <c r="O63" s="16"/>
+      <c r="P63" s="16"/>
+      <c r="Q63" s="16"/>
+      <c r="R63" s="16"/>
+      <c r="S63" s="17"/>
+      <c r="T63" s="16"/>
       <c r="U63" s="3"/>
       <c r="V63" s="3"/>
       <c r="W63" s="3"/>
       <c r="X63" s="3"/>
       <c r="Y63" s="3"/>
-    </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z63" s="3"/>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>65</v>
       </c>
@@ -4310,23 +4469,24 @@
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
       <c r="J64" s="5"/>
-      <c r="K64" s="12"/>
-      <c r="L64" s="22"/>
-      <c r="M64" s="22"/>
-      <c r="N64" s="22"/>
-      <c r="O64" s="22"/>
-      <c r="P64" s="22"/>
-      <c r="Q64" s="22"/>
-      <c r="R64" s="22"/>
-      <c r="S64" s="23"/>
-      <c r="T64" s="5"/>
+      <c r="K64" s="11"/>
+      <c r="L64" s="20"/>
+      <c r="M64" s="20"/>
+      <c r="N64" s="20"/>
+      <c r="O64" s="20"/>
+      <c r="P64" s="20"/>
+      <c r="Q64" s="20"/>
+      <c r="R64" s="20"/>
+      <c r="S64" s="21"/>
+      <c r="T64" s="20"/>
       <c r="U64" s="5"/>
       <c r="V64" s="5"/>
       <c r="W64" s="5"/>
       <c r="X64" s="5"/>
       <c r="Y64" s="5"/>
-    </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z64" s="5"/>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>66</v>
       </c>
@@ -4357,57 +4517,61 @@
       <c r="J65" s="4">
         <v>512000</v>
       </c>
-      <c r="K65" s="11"/>
-      <c r="L65" s="20">
+      <c r="K65" s="10"/>
+      <c r="L65" s="18">
         <f>L60+J60/2+E60/2</f>
         <v>365344</v>
       </c>
-      <c r="M65" s="20">
+      <c r="M65" s="18">
         <f>L65+J65/2-1</f>
         <v>621343</v>
       </c>
-      <c r="N65" s="20">
+      <c r="N65" s="18">
         <f>M65+1</f>
         <v>621344</v>
       </c>
-      <c r="O65" s="20">
+      <c r="O65" s="18">
         <f>N65+E65/2-1</f>
         <v>621843</v>
       </c>
-      <c r="P65" s="20"/>
-      <c r="Q65" s="20"/>
-      <c r="R65" s="20">
+      <c r="P65" s="18"/>
+      <c r="Q65" s="18"/>
+      <c r="R65" s="18">
         <f>S60+1</f>
         <v>2106068</v>
       </c>
-      <c r="S65" s="21">
+      <c r="S65" s="19">
         <f>R65+I65/2-1</f>
         <v>2190567</v>
       </c>
-      <c r="T65" s="4">
-        <f>D65*E65</f>
-        <v>512000</v>
+      <c r="T65" s="18">
+        <f>U65/E65</f>
+        <v>86528</v>
       </c>
       <c r="U65" s="4">
+        <f>D65*I65</f>
+        <v>86528000</v>
+      </c>
+      <c r="V65" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="V65" s="4">
-        <v>1</v>
-      </c>
       <c r="W65" s="4">
+        <v>1</v>
+      </c>
+      <c r="X65" s="4">
         <f>0.0000032*J65+0.0000064*I65</f>
         <v>2.7199999999999998</v>
       </c>
-      <c r="X65" s="4">
-        <f>T65*U65</f>
-        <v>35840</v>
-      </c>
       <c r="Y65" s="4">
-        <f>T65*U65*V65</f>
-        <v>35840</v>
-      </c>
-    </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
+        <f>U65*V65</f>
+        <v>6056960.0000000009</v>
+      </c>
+      <c r="Z65" s="4">
+        <f>T65*V65*W65</f>
+        <v>6056.9600000000009</v>
+      </c>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>67</v>
       </c>
@@ -4422,23 +4586,24 @@
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
-      <c r="K66" s="12"/>
-      <c r="L66" s="22"/>
-      <c r="M66" s="22"/>
-      <c r="N66" s="22"/>
-      <c r="O66" s="22"/>
-      <c r="P66" s="22"/>
-      <c r="Q66" s="22"/>
-      <c r="R66" s="22"/>
-      <c r="S66" s="23"/>
-      <c r="T66" s="5"/>
+      <c r="K66" s="11"/>
+      <c r="L66" s="20"/>
+      <c r="M66" s="20"/>
+      <c r="N66" s="20"/>
+      <c r="O66" s="20"/>
+      <c r="P66" s="20"/>
+      <c r="Q66" s="20"/>
+      <c r="R66" s="20"/>
+      <c r="S66" s="21"/>
+      <c r="T66" s="20"/>
       <c r="U66" s="5"/>
       <c r="V66" s="5"/>
       <c r="W66" s="5"/>
       <c r="X66" s="5"/>
       <c r="Y66" s="5"/>
-    </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z66" s="5"/>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>68</v>
       </c>
@@ -4449,7 +4614,9 @@
         <v>103</v>
       </c>
       <c r="D67" s="6"/>
-      <c r="E67" s="6"/>
+      <c r="E67" s="6">
+        <v>1000</v>
+      </c>
       <c r="F67" s="6">
         <v>1</v>
       </c>
@@ -4463,44 +4630,47 @@
         <v>1000</v>
       </c>
       <c r="J67" s="6"/>
-      <c r="K67" s="13"/>
-      <c r="L67" s="24"/>
-      <c r="M67" s="24"/>
-      <c r="N67" s="24"/>
-      <c r="O67" s="24"/>
-      <c r="P67" s="24"/>
-      <c r="Q67" s="24"/>
-      <c r="R67" s="24">
+      <c r="K67" s="12"/>
+      <c r="L67" s="22"/>
+      <c r="M67" s="22"/>
+      <c r="N67" s="22"/>
+      <c r="O67" s="22"/>
+      <c r="P67" s="22"/>
+      <c r="Q67" s="22"/>
+      <c r="R67" s="22">
         <f>S65+1</f>
         <v>2190568</v>
       </c>
-      <c r="S67" s="25">
+      <c r="S67" s="23">
         <f>R67+I67/2-1</f>
         <v>2191067</v>
       </c>
-      <c r="T67" s="6">
+      <c r="T67" s="22">
         <v>1000</v>
       </c>
       <c r="U67" s="6">
+        <v>1000</v>
+      </c>
+      <c r="V67" s="6">
         <v>1.2</v>
       </c>
-      <c r="V67" s="6">
-        <v>1</v>
-      </c>
       <c r="W67" s="6">
+        <v>1</v>
+      </c>
+      <c r="X67" s="6">
         <f>0.0000064*I67</f>
         <v>6.3999999999999994E-3</v>
       </c>
-      <c r="X67" s="6">
-        <f>T67*U67</f>
+      <c r="Y67" s="6">
+        <f>U67*V67</f>
         <v>1200</v>
       </c>
-      <c r="Y67" s="6">
-        <f>T67*U67*V67</f>
+      <c r="Z67" s="6">
+        <f>T67*V67*W67</f>
         <v>1200</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>69</v>
       </c>
@@ -4515,23 +4685,24 @@
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
-      <c r="K68" s="10"/>
-      <c r="L68" s="18"/>
-      <c r="M68" s="18"/>
-      <c r="N68" s="18"/>
-      <c r="O68" s="18"/>
-      <c r="P68" s="18"/>
-      <c r="Q68" s="18"/>
-      <c r="R68" s="18"/>
-      <c r="S68" s="19"/>
-      <c r="T68" s="3"/>
+      <c r="K68" s="9"/>
+      <c r="L68" s="16"/>
+      <c r="M68" s="16"/>
+      <c r="N68" s="16"/>
+      <c r="O68" s="16"/>
+      <c r="P68" s="16"/>
+      <c r="Q68" s="16"/>
+      <c r="R68" s="16"/>
+      <c r="S68" s="17"/>
+      <c r="T68" s="16"/>
       <c r="U68" s="3"/>
       <c r="V68" s="3"/>
       <c r="W68" s="3"/>
       <c r="X68" s="3"/>
       <c r="Y68" s="3"/>
-    </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z68" s="3"/>
+    </row>
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="I69" s="2">
         <f>SUM(I2:I68)</f>
         <v>3071416</v>
@@ -4540,32 +4711,33 @@
         <f>SUM(J3:J68)</f>
         <v>1231552</v>
       </c>
-      <c r="L69" s="26"/>
-      <c r="M69" s="26"/>
-      <c r="N69" s="26"/>
-      <c r="O69" s="26"/>
-      <c r="P69" s="26"/>
-      <c r="Q69" s="26"/>
-      <c r="R69" s="26"/>
-      <c r="S69" s="27"/>
-      <c r="T69" s="2">
-        <f>SUM(T3:T68)</f>
-        <v>1069672</v>
-      </c>
-      <c r="W69" s="2">
-        <f>SUM(W2:W68)</f>
+      <c r="L69" s="24"/>
+      <c r="M69" s="24"/>
+      <c r="N69" s="24"/>
+      <c r="O69" s="24"/>
+      <c r="P69" s="24"/>
+      <c r="Q69" s="24"/>
+      <c r="R69" s="24"/>
+      <c r="S69" s="25"/>
+      <c r="T69" s="24"/>
+      <c r="U69" s="2">
+        <f>SUM(U3:U68)</f>
+        <v>163998312</v>
+      </c>
+      <c r="X69" s="2">
+        <f>SUM(X2:X68)</f>
         <v>23.116339199999999</v>
       </c>
-      <c r="X69" s="2">
-        <f t="shared" ref="X69:Y69" si="31">SUM(X3:X68)</f>
-        <v>182983.68000000002</v>
-      </c>
       <c r="Y69" s="2">
+        <f t="shared" ref="Y69:Z69" si="31">SUM(Y3:Y68)</f>
+        <v>21993774.080000002</v>
+      </c>
+      <c r="Z69" s="2">
         <f t="shared" si="31"/>
-        <v>178682.88</v>
-      </c>
-    </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+        <v>200398.49000000002</v>
+      </c>
+    </row>
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="I70" s="7">
         <f>I69*16/1024/8</f>
         <v>5998.859375</v>
@@ -4574,44 +4746,48 @@
         <f>J69*16/1024/8</f>
         <v>2405.375</v>
       </c>
-      <c r="L70" s="26"/>
-      <c r="M70" s="26"/>
-      <c r="N70" s="26"/>
-      <c r="O70" s="26"/>
-      <c r="P70" s="26"/>
-      <c r="Q70" s="26"/>
-      <c r="R70" s="26"/>
-      <c r="S70" s="27"/>
-    </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="L71" s="26"/>
-      <c r="M71" s="26"/>
-      <c r="N71" s="26"/>
-      <c r="O71" s="26"/>
-      <c r="P71" s="26"/>
-      <c r="Q71" s="26"/>
-      <c r="R71" s="26"/>
-      <c r="S71" s="27"/>
-    </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="L72" s="26"/>
-      <c r="M72" s="26"/>
-      <c r="N72" s="26"/>
-      <c r="O72" s="26"/>
-      <c r="P72" s="26"/>
-      <c r="Q72" s="26"/>
-      <c r="R72" s="26"/>
-      <c r="S72" s="27"/>
-    </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="L73" s="26"/>
-      <c r="M73" s="26"/>
-      <c r="N73" s="26"/>
-      <c r="O73" s="26"/>
-      <c r="P73" s="26"/>
-      <c r="Q73" s="26"/>
-      <c r="R73" s="26"/>
-      <c r="S73" s="27"/>
+      <c r="L70" s="24"/>
+      <c r="M70" s="24"/>
+      <c r="N70" s="24"/>
+      <c r="O70" s="24"/>
+      <c r="P70" s="24"/>
+      <c r="Q70" s="24"/>
+      <c r="R70" s="24"/>
+      <c r="S70" s="25"/>
+      <c r="T70" s="24"/>
+    </row>
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="L71" s="24"/>
+      <c r="M71" s="24"/>
+      <c r="N71" s="24"/>
+      <c r="O71" s="24"/>
+      <c r="P71" s="24"/>
+      <c r="Q71" s="24"/>
+      <c r="R71" s="24"/>
+      <c r="S71" s="25"/>
+      <c r="T71" s="24"/>
+    </row>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="L72" s="24"/>
+      <c r="M72" s="24"/>
+      <c r="N72" s="24"/>
+      <c r="O72" s="24"/>
+      <c r="P72" s="24"/>
+      <c r="Q72" s="24"/>
+      <c r="R72" s="24"/>
+      <c r="S72" s="25"/>
+      <c r="T72" s="24"/>
+    </row>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="L73" s="24"/>
+      <c r="M73" s="24"/>
+      <c r="N73" s="24"/>
+      <c r="O73" s="24"/>
+      <c r="P73" s="24"/>
+      <c r="Q73" s="24"/>
+      <c r="R73" s="24"/>
+      <c r="S73" s="25"/>
+      <c r="T73" s="24"/>
     </row>
   </sheetData>
   <autoFilter ref="B1:B70" xr:uid="{5611B078-3ED8-409A-972B-20710E035DA1}"/>

</xml_diff>

<commit_message>
Use MEC cmac, change design
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89684071-EAAD-49D0-8873-0FE862000615}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED3EE31-7757-4292-B76C-EABD2284D0AA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7860" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7860" activeTab="1" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
   <sheets>
     <sheet name="SqueezeNet @ 100MHz + 312.5MHz" sheetId="1" r:id="rId1"/>
+    <sheet name="SqueezeNet v2 MEC Parallel Ch" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SqueezeNet @ 100MHz + 312.5MHz'!$B$1:$B$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'SqueezeNet v2 MEC Parallel Ch'!$B$1:$B$70</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="117">
   <si>
     <t>INPUT</t>
   </si>
@@ -381,6 +383,9 @@
   </si>
   <si>
     <t>Op Paral</t>
+  </si>
+  <si>
+    <t>Operations</t>
   </si>
 </sst>
 </file>
@@ -496,7 +501,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -569,6 +574,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -902,9 +910,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DDF8812-1429-4032-9C9C-F25909298566}">
   <dimension ref="A1:AA73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X2" sqref="X2"/>
+    <sheetView topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -956,32 +964,32 @@
       <c r="G1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="26"/>
+      <c r="I1" s="27"/>
       <c r="J1" s="2" t="s">
         <v>86</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27" t="s">
+      <c r="M1" s="28"/>
+      <c r="N1" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27" t="s">
+      <c r="O1" s="28"/>
+      <c r="P1" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27" t="s">
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="S1" s="28"/>
+      <c r="S1" s="29"/>
       <c r="T1" s="14" t="s">
         <v>115</v>
       </c>
@@ -4801,4 +4809,3811 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80B23C6-EAEB-43B1-B045-456C36085CFA}">
+  <dimension ref="A1:Z70"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U1:U1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="13" max="21" width="0" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="19" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.08984375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A1" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="U1" s="29"/>
+      <c r="V1" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="W1" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="X1" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y1" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z1" s="26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" s="3">
+        <v>224</v>
+      </c>
+      <c r="J2" s="3">
+        <f>I2^2*E2</f>
+        <v>150528</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16">
+        <v>655360</v>
+      </c>
+      <c r="U2" s="17">
+        <f>T2+J2/2-1</f>
+        <v>730623</v>
+      </c>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3">
+        <f>0.0000032*J2</f>
+        <v>0.4816896</v>
+      </c>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="4">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4">
+        <v>64</v>
+      </c>
+      <c r="F3" s="4">
+        <v>2</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I3" s="4">
+        <v>111</v>
+      </c>
+      <c r="J3" s="4">
+        <f>I3^2*E3</f>
+        <v>788544</v>
+      </c>
+      <c r="K3" s="4">
+        <f>I3^2*D3</f>
+        <v>36963</v>
+      </c>
+      <c r="L3" s="4">
+        <v>1728</v>
+      </c>
+      <c r="M3" s="10"/>
+      <c r="N3" s="18">
+        <v>4096</v>
+      </c>
+      <c r="O3" s="18">
+        <f>N3+L3/2-1</f>
+        <v>4959</v>
+      </c>
+      <c r="P3" s="18">
+        <f>O3+1</f>
+        <v>4960</v>
+      </c>
+      <c r="Q3" s="18">
+        <f>P3+E3/2-1</f>
+        <v>4991</v>
+      </c>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="18">
+        <f>U2+1</f>
+        <v>730624</v>
+      </c>
+      <c r="U3" s="19">
+        <f>T3+J3/2-1</f>
+        <v>1124895</v>
+      </c>
+      <c r="V3" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W3" s="4">
+        <v>1</v>
+      </c>
+      <c r="X3" s="4">
+        <f>0.0000032*L3+0.0000064*J3</f>
+        <v>5.0522111999999995</v>
+      </c>
+      <c r="Y3" s="4">
+        <f>K3*V3*W3</f>
+        <v>7392.6</v>
+      </c>
+      <c r="Z3" s="26"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
+      <c r="U4" s="21"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="26"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6">
+        <v>64</v>
+      </c>
+      <c r="F5" s="6">
+        <v>2</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="I5" s="6">
+        <v>55</v>
+      </c>
+      <c r="J5" s="6">
+        <f>I5^2*E5</f>
+        <v>193600</v>
+      </c>
+      <c r="K5" s="6">
+        <f>J5</f>
+        <v>193600</v>
+      </c>
+      <c r="L5" s="6"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="22">
+        <f>U3+1</f>
+        <v>1124896</v>
+      </c>
+      <c r="U5" s="23">
+        <f>T5+J5/2-1</f>
+        <v>1221695</v>
+      </c>
+      <c r="V5" s="6">
+        <v>0.31</v>
+      </c>
+      <c r="W5" s="6">
+        <v>1</v>
+      </c>
+      <c r="X5" s="6">
+        <f>0.0000064*J5</f>
+        <v>1.2390399999999999</v>
+      </c>
+      <c r="Y5" s="6">
+        <f>K5*V5*W5</f>
+        <v>60016</v>
+      </c>
+      <c r="Z5" s="26"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="4">
+        <v>64</v>
+      </c>
+      <c r="E6" s="4">
+        <v>16</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" s="4">
+        <v>55</v>
+      </c>
+      <c r="J6" s="4">
+        <f>I6^2*E6</f>
+        <v>48400</v>
+      </c>
+      <c r="K6" s="4">
+        <f>I6^2*D6</f>
+        <v>193600</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1024</v>
+      </c>
+      <c r="M6" s="10"/>
+      <c r="N6" s="18">
+        <f>N3+L3/2+E3/2</f>
+        <v>4992</v>
+      </c>
+      <c r="O6" s="18">
+        <f>N6+L6/2-1</f>
+        <v>5503</v>
+      </c>
+      <c r="P6" s="18">
+        <f>O6+1</f>
+        <v>5504</v>
+      </c>
+      <c r="Q6" s="18">
+        <f>P6+E6/2-1</f>
+        <v>5511</v>
+      </c>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18">
+        <f>U5+1</f>
+        <v>1221696</v>
+      </c>
+      <c r="U6" s="19">
+        <f>T6+J6/2-1</f>
+        <v>1245895</v>
+      </c>
+      <c r="V6" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W6" s="4">
+        <v>1</v>
+      </c>
+      <c r="X6" s="4">
+        <f>0.0000032*L6+0.0000064*J6</f>
+        <v>0.3130368</v>
+      </c>
+      <c r="Y6" s="4">
+        <f>K6*V6*W6</f>
+        <v>38720</v>
+      </c>
+      <c r="Z6" s="26"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="21"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="26"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="4">
+        <v>16</v>
+      </c>
+      <c r="E8" s="4">
+        <v>64</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I8" s="4">
+        <v>55</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" ref="J8:J9" si="0">I8^2*E8</f>
+        <v>193600</v>
+      </c>
+      <c r="K8" s="4">
+        <f t="shared" ref="K8:K9" si="1">I8^2*D8</f>
+        <v>48400</v>
+      </c>
+      <c r="L8" s="4">
+        <v>1024</v>
+      </c>
+      <c r="M8" s="10"/>
+      <c r="N8" s="18">
+        <f>N6+L6/2+E6/2</f>
+        <v>5512</v>
+      </c>
+      <c r="O8" s="18">
+        <f t="shared" ref="O8:O9" si="2">N8+L8/2-1</f>
+        <v>6023</v>
+      </c>
+      <c r="P8" s="18">
+        <f t="shared" ref="P8:P9" si="3">O8+1</f>
+        <v>6024</v>
+      </c>
+      <c r="Q8" s="18">
+        <f>P8+E8/2-1</f>
+        <v>6055</v>
+      </c>
+      <c r="R8" s="18"/>
+      <c r="S8" s="18"/>
+      <c r="T8" s="18">
+        <f>U6+1</f>
+        <v>1245896</v>
+      </c>
+      <c r="U8" s="19">
+        <f>T8+J8/2-1</f>
+        <v>1342695</v>
+      </c>
+      <c r="V8" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W8" s="4">
+        <v>0</v>
+      </c>
+      <c r="X8" s="4">
+        <f>0.0000032*L8+0.0000064*J8</f>
+        <v>1.2423168</v>
+      </c>
+      <c r="Y8" s="4">
+        <f t="shared" ref="Y8:Y9" si="4">K8*V8*W8</f>
+        <v>0</v>
+      </c>
+      <c r="Z8" s="26"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="4">
+        <v>16</v>
+      </c>
+      <c r="E9" s="4">
+        <v>64</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I9" s="4">
+        <v>55</v>
+      </c>
+      <c r="J9" s="4">
+        <f t="shared" si="0"/>
+        <v>193600</v>
+      </c>
+      <c r="K9" s="4">
+        <f t="shared" si="1"/>
+        <v>48400</v>
+      </c>
+      <c r="L9" s="4">
+        <v>9216</v>
+      </c>
+      <c r="M9" s="10"/>
+      <c r="N9" s="18">
+        <f>N8+L8/2+E8/2</f>
+        <v>6056</v>
+      </c>
+      <c r="O9" s="18">
+        <f t="shared" si="2"/>
+        <v>10663</v>
+      </c>
+      <c r="P9" s="18">
+        <f t="shared" si="3"/>
+        <v>10664</v>
+      </c>
+      <c r="Q9" s="18">
+        <f>P9+E9/2-1</f>
+        <v>10695</v>
+      </c>
+      <c r="R9" s="18"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="18">
+        <f>U8+1</f>
+        <v>1342696</v>
+      </c>
+      <c r="U9" s="19">
+        <f>T9+J9/2-1</f>
+        <v>1439495</v>
+      </c>
+      <c r="V9" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W9" s="4">
+        <v>1</v>
+      </c>
+      <c r="X9" s="4">
+        <f>0.0000032*L9+0.0000064*J9</f>
+        <v>1.2685312</v>
+      </c>
+      <c r="Y9" s="4">
+        <f t="shared" si="4"/>
+        <v>9680</v>
+      </c>
+      <c r="Z9" s="26"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="21"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="26"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="20"/>
+      <c r="U11" s="21"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="26"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I12" s="3">
+        <v>55</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="17"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="26"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="4">
+        <v>128</v>
+      </c>
+      <c r="E13" s="4">
+        <v>16</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I13" s="4">
+        <v>55</v>
+      </c>
+      <c r="J13" s="4">
+        <f>I13^2*E13</f>
+        <v>48400</v>
+      </c>
+      <c r="K13" s="4">
+        <f>I13^2*D13</f>
+        <v>387200</v>
+      </c>
+      <c r="L13" s="4">
+        <v>2048</v>
+      </c>
+      <c r="M13" s="10"/>
+      <c r="N13" s="18">
+        <f>N9+L9/2+E9/2</f>
+        <v>10696</v>
+      </c>
+      <c r="O13" s="18">
+        <f>N13+L13/2-1</f>
+        <v>11719</v>
+      </c>
+      <c r="P13" s="18">
+        <f>O13+1</f>
+        <v>11720</v>
+      </c>
+      <c r="Q13" s="18">
+        <f>P13+E13/2-1</f>
+        <v>11727</v>
+      </c>
+      <c r="R13" s="18"/>
+      <c r="S13" s="18"/>
+      <c r="T13" s="18">
+        <f>U9+1</f>
+        <v>1439496</v>
+      </c>
+      <c r="U13" s="19">
+        <f>T13+J13/2-1</f>
+        <v>1463695</v>
+      </c>
+      <c r="V13" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W13" s="4">
+        <v>1</v>
+      </c>
+      <c r="X13" s="4">
+        <f>0.0000032*L13+0.0000064*J13</f>
+        <v>0.31631359999999997</v>
+      </c>
+      <c r="Y13" s="4">
+        <f>K13*V13*W13</f>
+        <v>77440</v>
+      </c>
+      <c r="Z13" s="26"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="20"/>
+      <c r="U14" s="21"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="26"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="4">
+        <v>16</v>
+      </c>
+      <c r="E15" s="4">
+        <v>64</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I15" s="4">
+        <v>55</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" ref="J15:J16" si="5">I15^2*E15</f>
+        <v>193600</v>
+      </c>
+      <c r="K15" s="4">
+        <f t="shared" ref="K15:K16" si="6">I15^2*D15</f>
+        <v>48400</v>
+      </c>
+      <c r="L15" s="4">
+        <v>1024</v>
+      </c>
+      <c r="M15" s="10"/>
+      <c r="N15" s="18">
+        <f>N13+L13/2+E13/2</f>
+        <v>11728</v>
+      </c>
+      <c r="O15" s="18">
+        <f t="shared" ref="O15:O16" si="7">N15+L15/2-1</f>
+        <v>12239</v>
+      </c>
+      <c r="P15" s="18">
+        <f t="shared" ref="P15:P16" si="8">O15+1</f>
+        <v>12240</v>
+      </c>
+      <c r="Q15" s="18">
+        <f>P15+E15/2-1</f>
+        <v>12271</v>
+      </c>
+      <c r="R15" s="18"/>
+      <c r="S15" s="18"/>
+      <c r="T15" s="18">
+        <f>U13+1</f>
+        <v>1463696</v>
+      </c>
+      <c r="U15" s="19">
+        <f>T15+J15/2-1</f>
+        <v>1560495</v>
+      </c>
+      <c r="V15" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W15" s="4">
+        <v>0</v>
+      </c>
+      <c r="X15" s="4">
+        <f>0.0000032*L15+0.0000064*J15</f>
+        <v>1.2423168</v>
+      </c>
+      <c r="Y15" s="4">
+        <f t="shared" ref="Y15:Y16" si="9">K15*V15*W15</f>
+        <v>0</v>
+      </c>
+      <c r="Z15" s="26"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="4">
+        <v>16</v>
+      </c>
+      <c r="E16" s="4">
+        <v>64</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I16" s="4">
+        <v>55</v>
+      </c>
+      <c r="J16" s="4">
+        <f t="shared" si="5"/>
+        <v>193600</v>
+      </c>
+      <c r="K16" s="4">
+        <f t="shared" si="6"/>
+        <v>48400</v>
+      </c>
+      <c r="L16" s="4">
+        <v>9216</v>
+      </c>
+      <c r="M16" s="10"/>
+      <c r="N16" s="18">
+        <f>N15+L15/2+E15/2</f>
+        <v>12272</v>
+      </c>
+      <c r="O16" s="18">
+        <f t="shared" si="7"/>
+        <v>16879</v>
+      </c>
+      <c r="P16" s="18">
+        <f t="shared" si="8"/>
+        <v>16880</v>
+      </c>
+      <c r="Q16" s="18">
+        <f>P16+E16/2-1</f>
+        <v>16911</v>
+      </c>
+      <c r="R16" s="18"/>
+      <c r="S16" s="18"/>
+      <c r="T16" s="18">
+        <f>U15+1</f>
+        <v>1560496</v>
+      </c>
+      <c r="U16" s="19">
+        <f>T16+J16/2-1</f>
+        <v>1657295</v>
+      </c>
+      <c r="V16" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W16" s="4">
+        <v>1</v>
+      </c>
+      <c r="X16" s="4">
+        <f>0.0000032*L16+0.0000064*J16</f>
+        <v>1.2685312</v>
+      </c>
+      <c r="Y16" s="4">
+        <f t="shared" si="9"/>
+        <v>9680</v>
+      </c>
+      <c r="Z16" s="26"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="20"/>
+      <c r="T17" s="20"/>
+      <c r="U17" s="21"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="26"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="20"/>
+      <c r="T18" s="20"/>
+      <c r="U18" s="21"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="26"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I19" s="3">
+        <v>55</v>
+      </c>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="16"/>
+      <c r="T19" s="16"/>
+      <c r="U19" s="17"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="26"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6">
+        <v>128</v>
+      </c>
+      <c r="F20" s="6">
+        <v>2</v>
+      </c>
+      <c r="G20" s="6">
+        <v>0</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I20" s="6">
+        <v>27</v>
+      </c>
+      <c r="J20" s="6">
+        <f>I20^2*E20</f>
+        <v>93312</v>
+      </c>
+      <c r="K20" s="6">
+        <f>J20</f>
+        <v>93312</v>
+      </c>
+      <c r="L20" s="6"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="22"/>
+      <c r="R20" s="22"/>
+      <c r="S20" s="22"/>
+      <c r="T20" s="22">
+        <f>U16+1</f>
+        <v>1657296</v>
+      </c>
+      <c r="U20" s="23">
+        <f>T20+J20/2-1</f>
+        <v>1703951</v>
+      </c>
+      <c r="V20" s="6">
+        <v>0.31</v>
+      </c>
+      <c r="W20" s="6">
+        <v>1</v>
+      </c>
+      <c r="X20" s="6">
+        <f>0.0000064*J20</f>
+        <v>0.59719679999999997</v>
+      </c>
+      <c r="Y20" s="6">
+        <f>K20*V20*W20</f>
+        <v>28926.720000000001</v>
+      </c>
+      <c r="Z20" s="26"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="4">
+        <v>128</v>
+      </c>
+      <c r="E21" s="4">
+        <v>32</v>
+      </c>
+      <c r="F21" s="4">
+        <v>1</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I21" s="4">
+        <v>27</v>
+      </c>
+      <c r="J21" s="4">
+        <f>I21^2*E21</f>
+        <v>23328</v>
+      </c>
+      <c r="K21" s="4">
+        <f>I21^2*D21</f>
+        <v>93312</v>
+      </c>
+      <c r="L21" s="4">
+        <v>4096</v>
+      </c>
+      <c r="M21" s="10"/>
+      <c r="N21" s="18">
+        <f>N16+L16/2+E16/2</f>
+        <v>16912</v>
+      </c>
+      <c r="O21" s="18">
+        <f>N21+L21/2-1</f>
+        <v>18959</v>
+      </c>
+      <c r="P21" s="18">
+        <f>O21+1</f>
+        <v>18960</v>
+      </c>
+      <c r="Q21" s="18">
+        <f>P21+E21/2-1</f>
+        <v>18975</v>
+      </c>
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
+      <c r="T21" s="18">
+        <f>U20+1</f>
+        <v>1703952</v>
+      </c>
+      <c r="U21" s="19">
+        <f>T21+J21/2-1</f>
+        <v>1715615</v>
+      </c>
+      <c r="V21" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W21" s="4">
+        <v>1</v>
+      </c>
+      <c r="X21" s="4">
+        <f>0.0000032*L21+0.0000064*J21</f>
+        <v>0.16240640000000001</v>
+      </c>
+      <c r="Y21" s="4">
+        <f>K21*V21*W21</f>
+        <v>18662.400000000001</v>
+      </c>
+      <c r="Z21" s="26"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="20"/>
+      <c r="S22" s="20"/>
+      <c r="T22" s="20"/>
+      <c r="U22" s="21"/>
+      <c r="V22" s="5"/>
+      <c r="W22" s="5"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="5"/>
+      <c r="Z22" s="26"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="4">
+        <v>32</v>
+      </c>
+      <c r="E23" s="4">
+        <v>128</v>
+      </c>
+      <c r="F23" s="4">
+        <v>1</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I23" s="4">
+        <v>27</v>
+      </c>
+      <c r="J23" s="4">
+        <f t="shared" ref="J23:J24" si="10">I23^2*E23</f>
+        <v>93312</v>
+      </c>
+      <c r="K23" s="4">
+        <f t="shared" ref="K23:K24" si="11">I23^2*D23</f>
+        <v>23328</v>
+      </c>
+      <c r="L23" s="4">
+        <v>4096</v>
+      </c>
+      <c r="M23" s="10"/>
+      <c r="N23" s="18">
+        <f>N21+L21/2+E21/2</f>
+        <v>18976</v>
+      </c>
+      <c r="O23" s="18">
+        <f t="shared" ref="O23:O24" si="12">N23+L23/2-1</f>
+        <v>21023</v>
+      </c>
+      <c r="P23" s="18">
+        <f t="shared" ref="P23:P24" si="13">O23+1</f>
+        <v>21024</v>
+      </c>
+      <c r="Q23" s="18">
+        <f>P23+E23/2-1</f>
+        <v>21087</v>
+      </c>
+      <c r="R23" s="18"/>
+      <c r="S23" s="18"/>
+      <c r="T23" s="18">
+        <f>U21+1</f>
+        <v>1715616</v>
+      </c>
+      <c r="U23" s="19">
+        <f>T23+J23/2-1</f>
+        <v>1762271</v>
+      </c>
+      <c r="V23" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W23" s="4">
+        <v>0</v>
+      </c>
+      <c r="X23" s="4">
+        <f>0.0000032*L23+0.0000064*J23</f>
+        <v>0.61030399999999996</v>
+      </c>
+      <c r="Y23" s="4">
+        <f t="shared" ref="Y23:Y24" si="14">K23*V23*W23</f>
+        <v>0</v>
+      </c>
+      <c r="Z23" s="26"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="4">
+        <v>32</v>
+      </c>
+      <c r="E24" s="4">
+        <v>128</v>
+      </c>
+      <c r="F24" s="4">
+        <v>1</v>
+      </c>
+      <c r="G24" s="4">
+        <v>1</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I24" s="4">
+        <v>27</v>
+      </c>
+      <c r="J24" s="4">
+        <f t="shared" si="10"/>
+        <v>93312</v>
+      </c>
+      <c r="K24" s="4">
+        <f t="shared" si="11"/>
+        <v>23328</v>
+      </c>
+      <c r="L24" s="4">
+        <v>36864</v>
+      </c>
+      <c r="M24" s="10"/>
+      <c r="N24" s="18">
+        <f>N23+L23/2+E23/2</f>
+        <v>21088</v>
+      </c>
+      <c r="O24" s="18">
+        <f t="shared" si="12"/>
+        <v>39519</v>
+      </c>
+      <c r="P24" s="18">
+        <f t="shared" si="13"/>
+        <v>39520</v>
+      </c>
+      <c r="Q24" s="18">
+        <f>P24+E24/2-1</f>
+        <v>39583</v>
+      </c>
+      <c r="R24" s="18"/>
+      <c r="S24" s="18"/>
+      <c r="T24" s="18">
+        <f>U23+1</f>
+        <v>1762272</v>
+      </c>
+      <c r="U24" s="19">
+        <f>T24+J24/2-1</f>
+        <v>1808927</v>
+      </c>
+      <c r="V24" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W24" s="4">
+        <v>1</v>
+      </c>
+      <c r="X24" s="4">
+        <f>0.0000032*L24+0.0000064*J24</f>
+        <v>0.71516159999999995</v>
+      </c>
+      <c r="Y24" s="4">
+        <f t="shared" si="14"/>
+        <v>4665.6000000000004</v>
+      </c>
+      <c r="Z24" s="26"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A25" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="20"/>
+      <c r="O25" s="20"/>
+      <c r="P25" s="20"/>
+      <c r="Q25" s="20"/>
+      <c r="R25" s="20"/>
+      <c r="S25" s="20"/>
+      <c r="T25" s="20"/>
+      <c r="U25" s="21"/>
+      <c r="V25" s="5"/>
+      <c r="W25" s="5"/>
+      <c r="X25" s="5"/>
+      <c r="Y25" s="5"/>
+      <c r="Z25" s="26"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="20"/>
+      <c r="O26" s="20"/>
+      <c r="P26" s="20"/>
+      <c r="Q26" s="20"/>
+      <c r="R26" s="20"/>
+      <c r="S26" s="20"/>
+      <c r="T26" s="20"/>
+      <c r="U26" s="21"/>
+      <c r="V26" s="5"/>
+      <c r="W26" s="5"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="26"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I27" s="3">
+        <v>27</v>
+      </c>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="16"/>
+      <c r="S27" s="16"/>
+      <c r="T27" s="16"/>
+      <c r="U27" s="17"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+      <c r="X27" s="3"/>
+      <c r="Y27" s="3"/>
+      <c r="Z27" s="26"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="4">
+        <v>256</v>
+      </c>
+      <c r="E28" s="4">
+        <v>32</v>
+      </c>
+      <c r="F28" s="4">
+        <v>1</v>
+      </c>
+      <c r="G28" s="4">
+        <v>0</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I28" s="4">
+        <v>27</v>
+      </c>
+      <c r="J28" s="4">
+        <f>I28^2*E28</f>
+        <v>23328</v>
+      </c>
+      <c r="K28" s="4">
+        <f>I28^2*D28</f>
+        <v>186624</v>
+      </c>
+      <c r="L28" s="4">
+        <v>8192</v>
+      </c>
+      <c r="M28" s="10"/>
+      <c r="N28" s="18">
+        <f>N24+L24/2+E24/2</f>
+        <v>39584</v>
+      </c>
+      <c r="O28" s="18">
+        <f>N28+L28/2-1</f>
+        <v>43679</v>
+      </c>
+      <c r="P28" s="18">
+        <f>O28+1</f>
+        <v>43680</v>
+      </c>
+      <c r="Q28" s="18">
+        <f>P28+E28/2-1</f>
+        <v>43695</v>
+      </c>
+      <c r="R28" s="18"/>
+      <c r="S28" s="18"/>
+      <c r="T28" s="18">
+        <f>U24+1</f>
+        <v>1808928</v>
+      </c>
+      <c r="U28" s="19">
+        <f>T28+J28/2-1</f>
+        <v>1820591</v>
+      </c>
+      <c r="V28" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W28" s="4">
+        <v>1</v>
+      </c>
+      <c r="X28" s="4">
+        <f>0.0000032*L28+0.0000064*J28</f>
+        <v>0.17551359999999999</v>
+      </c>
+      <c r="Y28" s="4">
+        <f>K28*V28*W28</f>
+        <v>37324.800000000003</v>
+      </c>
+      <c r="Z28" s="26"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
+      <c r="P29" s="20"/>
+      <c r="Q29" s="20"/>
+      <c r="R29" s="20"/>
+      <c r="S29" s="20"/>
+      <c r="T29" s="20"/>
+      <c r="U29" s="21"/>
+      <c r="V29" s="5"/>
+      <c r="W29" s="5"/>
+      <c r="X29" s="5"/>
+      <c r="Y29" s="5"/>
+      <c r="Z29" s="26"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30" s="4">
+        <v>32</v>
+      </c>
+      <c r="E30" s="4">
+        <v>128</v>
+      </c>
+      <c r="F30" s="4">
+        <v>1</v>
+      </c>
+      <c r="G30" s="4">
+        <v>0</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I30" s="4">
+        <v>27</v>
+      </c>
+      <c r="J30" s="4">
+        <f t="shared" ref="J30:J31" si="15">I30^2*E30</f>
+        <v>93312</v>
+      </c>
+      <c r="K30" s="4">
+        <f t="shared" ref="K30:K31" si="16">I30^2*D30</f>
+        <v>23328</v>
+      </c>
+      <c r="L30" s="4">
+        <v>4096</v>
+      </c>
+      <c r="M30" s="10"/>
+      <c r="N30" s="18">
+        <f>N28+L28/2+E28/2</f>
+        <v>43696</v>
+      </c>
+      <c r="O30" s="18">
+        <f t="shared" ref="O30:O31" si="17">N30+L30/2-1</f>
+        <v>45743</v>
+      </c>
+      <c r="P30" s="18">
+        <f t="shared" ref="P30:P31" si="18">O30+1</f>
+        <v>45744</v>
+      </c>
+      <c r="Q30" s="18">
+        <f>P30+E30/2-1</f>
+        <v>45807</v>
+      </c>
+      <c r="R30" s="18"/>
+      <c r="S30" s="18"/>
+      <c r="T30" s="18">
+        <f>U28+1</f>
+        <v>1820592</v>
+      </c>
+      <c r="U30" s="19">
+        <f>T30+J30/2-1</f>
+        <v>1867247</v>
+      </c>
+      <c r="V30" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W30" s="4">
+        <v>0</v>
+      </c>
+      <c r="X30" s="4">
+        <f>0.0000032*L30+0.0000064*J30</f>
+        <v>0.61030399999999996</v>
+      </c>
+      <c r="Y30" s="4">
+        <f t="shared" ref="Y30:Y31" si="19">K30*V30*W30</f>
+        <v>0</v>
+      </c>
+      <c r="Z30" s="26"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A31" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="4">
+        <v>32</v>
+      </c>
+      <c r="E31" s="4">
+        <v>128</v>
+      </c>
+      <c r="F31" s="4">
+        <v>1</v>
+      </c>
+      <c r="G31" s="4">
+        <v>1</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I31" s="4">
+        <v>27</v>
+      </c>
+      <c r="J31" s="4">
+        <f t="shared" si="15"/>
+        <v>93312</v>
+      </c>
+      <c r="K31" s="4">
+        <f t="shared" si="16"/>
+        <v>23328</v>
+      </c>
+      <c r="L31" s="4">
+        <v>36864</v>
+      </c>
+      <c r="M31" s="10"/>
+      <c r="N31" s="18">
+        <f>N30+L30/2+E30/2</f>
+        <v>45808</v>
+      </c>
+      <c r="O31" s="18">
+        <f t="shared" si="17"/>
+        <v>64239</v>
+      </c>
+      <c r="P31" s="18">
+        <f t="shared" si="18"/>
+        <v>64240</v>
+      </c>
+      <c r="Q31" s="18">
+        <f>P31+E31/2-1</f>
+        <v>64303</v>
+      </c>
+      <c r="R31" s="18"/>
+      <c r="S31" s="18"/>
+      <c r="T31" s="18">
+        <f>U30+1</f>
+        <v>1867248</v>
+      </c>
+      <c r="U31" s="19">
+        <f>T31+J31/2-1</f>
+        <v>1913903</v>
+      </c>
+      <c r="V31" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W31" s="4">
+        <v>1</v>
+      </c>
+      <c r="X31" s="4">
+        <f>0.0000032*L31+0.0000064*J31</f>
+        <v>0.71516159999999995</v>
+      </c>
+      <c r="Y31" s="4">
+        <f t="shared" si="19"/>
+        <v>4665.6000000000004</v>
+      </c>
+      <c r="Z31" s="26"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A32" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="20"/>
+      <c r="O32" s="20"/>
+      <c r="P32" s="20"/>
+      <c r="Q32" s="20"/>
+      <c r="R32" s="20"/>
+      <c r="S32" s="20"/>
+      <c r="T32" s="20"/>
+      <c r="U32" s="21"/>
+      <c r="V32" s="5"/>
+      <c r="W32" s="5"/>
+      <c r="X32" s="5"/>
+      <c r="Y32" s="5"/>
+      <c r="Z32" s="26"/>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A33" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="20"/>
+      <c r="O33" s="20"/>
+      <c r="P33" s="20"/>
+      <c r="Q33" s="20"/>
+      <c r="R33" s="20"/>
+      <c r="S33" s="20"/>
+      <c r="T33" s="20"/>
+      <c r="U33" s="21"/>
+      <c r="V33" s="5"/>
+      <c r="W33" s="5"/>
+      <c r="X33" s="5"/>
+      <c r="Y33" s="5"/>
+      <c r="Z33" s="26"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="16"/>
+      <c r="S34" s="16"/>
+      <c r="T34" s="16"/>
+      <c r="U34" s="17"/>
+      <c r="V34" s="3"/>
+      <c r="W34" s="3"/>
+      <c r="X34" s="3"/>
+      <c r="Y34" s="3"/>
+      <c r="Z34" s="26"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A35" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6">
+        <v>256</v>
+      </c>
+      <c r="F35" s="6">
+        <v>2</v>
+      </c>
+      <c r="G35" s="6">
+        <v>0</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I35" s="6">
+        <v>13</v>
+      </c>
+      <c r="J35" s="6">
+        <f>I35^2*E35</f>
+        <v>43264</v>
+      </c>
+      <c r="K35" s="6">
+        <f>J35</f>
+        <v>43264</v>
+      </c>
+      <c r="L35" s="6"/>
+      <c r="M35" s="12"/>
+      <c r="N35" s="22"/>
+      <c r="O35" s="22"/>
+      <c r="P35" s="22"/>
+      <c r="Q35" s="22"/>
+      <c r="R35" s="22"/>
+      <c r="S35" s="22"/>
+      <c r="T35" s="22">
+        <f>U31+1</f>
+        <v>1913904</v>
+      </c>
+      <c r="U35" s="23">
+        <f>T35+J35/2-1</f>
+        <v>1935535</v>
+      </c>
+      <c r="V35" s="6">
+        <v>0.31</v>
+      </c>
+      <c r="W35" s="6">
+        <v>1</v>
+      </c>
+      <c r="X35" s="6">
+        <f>0.0000064*J35</f>
+        <v>0.27688960000000001</v>
+      </c>
+      <c r="Y35" s="6">
+        <f>K35*V35*W35</f>
+        <v>13411.84</v>
+      </c>
+      <c r="Z35" s="26"/>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A36" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="4">
+        <v>256</v>
+      </c>
+      <c r="E36" s="4">
+        <v>48</v>
+      </c>
+      <c r="F36" s="4">
+        <v>1</v>
+      </c>
+      <c r="G36" s="4">
+        <v>0</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I36" s="4">
+        <v>13</v>
+      </c>
+      <c r="J36" s="4">
+        <f>I36^2*E36</f>
+        <v>8112</v>
+      </c>
+      <c r="K36" s="4">
+        <f>I36^2*D36</f>
+        <v>43264</v>
+      </c>
+      <c r="L36" s="4">
+        <v>12288</v>
+      </c>
+      <c r="M36" s="10"/>
+      <c r="N36" s="18">
+        <f>N31+L31/2+E31/2</f>
+        <v>64304</v>
+      </c>
+      <c r="O36" s="18">
+        <f>N36+L36/2-1</f>
+        <v>70447</v>
+      </c>
+      <c r="P36" s="18">
+        <f>O36+1</f>
+        <v>70448</v>
+      </c>
+      <c r="Q36" s="18">
+        <f>P36+E36/2-1</f>
+        <v>70471</v>
+      </c>
+      <c r="R36" s="18"/>
+      <c r="S36" s="18"/>
+      <c r="T36" s="18">
+        <f>U35+1</f>
+        <v>1935536</v>
+      </c>
+      <c r="U36" s="19">
+        <f>T36+J36/2-1</f>
+        <v>1939591</v>
+      </c>
+      <c r="V36" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W36" s="4">
+        <v>1</v>
+      </c>
+      <c r="X36" s="4">
+        <f>0.0000032*L36+0.0000064*J36</f>
+        <v>9.1238399999999997E-2</v>
+      </c>
+      <c r="Y36" s="4">
+        <f>K36*V36*W36</f>
+        <v>8652.8000000000011</v>
+      </c>
+      <c r="Z36" s="26"/>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A37" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="20"/>
+      <c r="O37" s="20"/>
+      <c r="P37" s="20"/>
+      <c r="Q37" s="20"/>
+      <c r="R37" s="20"/>
+      <c r="S37" s="20"/>
+      <c r="T37" s="20"/>
+      <c r="U37" s="21"/>
+      <c r="V37" s="5"/>
+      <c r="W37" s="5"/>
+      <c r="X37" s="5"/>
+      <c r="Y37" s="5"/>
+      <c r="Z37" s="26"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A38" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="4">
+        <v>48</v>
+      </c>
+      <c r="E38" s="4">
+        <v>192</v>
+      </c>
+      <c r="F38" s="4">
+        <v>1</v>
+      </c>
+      <c r="G38" s="4">
+        <v>0</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I38" s="4">
+        <v>13</v>
+      </c>
+      <c r="J38" s="4">
+        <f t="shared" ref="J38:J39" si="20">I38^2*E38</f>
+        <v>32448</v>
+      </c>
+      <c r="K38" s="4">
+        <f t="shared" ref="K38:K39" si="21">I38^2*D38</f>
+        <v>8112</v>
+      </c>
+      <c r="L38" s="4">
+        <v>9216</v>
+      </c>
+      <c r="M38" s="10"/>
+      <c r="N38" s="18">
+        <f>N36+L36/2+E36/2</f>
+        <v>70472</v>
+      </c>
+      <c r="O38" s="18">
+        <f t="shared" ref="O38:O39" si="22">N38+L38/2-1</f>
+        <v>75079</v>
+      </c>
+      <c r="P38" s="18">
+        <f>O38+1</f>
+        <v>75080</v>
+      </c>
+      <c r="Q38" s="18">
+        <f>P38+E38/2-1</f>
+        <v>75175</v>
+      </c>
+      <c r="R38" s="18"/>
+      <c r="S38" s="18"/>
+      <c r="T38" s="18">
+        <f>U36+1</f>
+        <v>1939592</v>
+      </c>
+      <c r="U38" s="19">
+        <f>T38+J38/2-1</f>
+        <v>1955815</v>
+      </c>
+      <c r="V38" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W38" s="4">
+        <v>0</v>
+      </c>
+      <c r="X38" s="4">
+        <f>0.0000032*L38+0.0000064*J38</f>
+        <v>0.23715839999999999</v>
+      </c>
+      <c r="Y38" s="4">
+        <f t="shared" ref="Y38:Y39" si="23">K38*V38*W38</f>
+        <v>0</v>
+      </c>
+      <c r="Z38" s="26"/>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A39" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" s="4">
+        <v>48</v>
+      </c>
+      <c r="E39" s="4">
+        <v>192</v>
+      </c>
+      <c r="F39" s="4">
+        <v>1</v>
+      </c>
+      <c r="G39" s="4">
+        <v>1</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I39" s="4">
+        <v>13</v>
+      </c>
+      <c r="J39" s="4">
+        <f t="shared" si="20"/>
+        <v>32448</v>
+      </c>
+      <c r="K39" s="4">
+        <f t="shared" si="21"/>
+        <v>8112</v>
+      </c>
+      <c r="L39" s="4">
+        <v>82944</v>
+      </c>
+      <c r="M39" s="10"/>
+      <c r="N39" s="18">
+        <f>N38+L38/2+E38/2</f>
+        <v>75176</v>
+      </c>
+      <c r="O39" s="18">
+        <f t="shared" si="22"/>
+        <v>116647</v>
+      </c>
+      <c r="P39" s="18">
+        <f>O39+1</f>
+        <v>116648</v>
+      </c>
+      <c r="Q39" s="18">
+        <f>P39+E39/2-1</f>
+        <v>116743</v>
+      </c>
+      <c r="R39" s="18"/>
+      <c r="S39" s="18"/>
+      <c r="T39" s="18">
+        <f>U38+1</f>
+        <v>1955816</v>
+      </c>
+      <c r="U39" s="19">
+        <f>T39+J39/2-1</f>
+        <v>1972039</v>
+      </c>
+      <c r="V39" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W39" s="4">
+        <v>1</v>
+      </c>
+      <c r="X39" s="4">
+        <f>0.0000032*L39+0.0000064*J39</f>
+        <v>0.47308800000000001</v>
+      </c>
+      <c r="Y39" s="4">
+        <f t="shared" si="23"/>
+        <v>1622.4</v>
+      </c>
+      <c r="Z39" s="26"/>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A40" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="11"/>
+      <c r="N40" s="20"/>
+      <c r="O40" s="20"/>
+      <c r="P40" s="20"/>
+      <c r="Q40" s="20"/>
+      <c r="R40" s="20"/>
+      <c r="S40" s="20"/>
+      <c r="T40" s="20"/>
+      <c r="U40" s="21"/>
+      <c r="V40" s="5"/>
+      <c r="W40" s="5"/>
+      <c r="X40" s="5"/>
+      <c r="Y40" s="5"/>
+      <c r="Z40" s="26"/>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A41" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="11"/>
+      <c r="N41" s="20"/>
+      <c r="O41" s="20"/>
+      <c r="P41" s="20"/>
+      <c r="Q41" s="20"/>
+      <c r="R41" s="20"/>
+      <c r="S41" s="20"/>
+      <c r="T41" s="20"/>
+      <c r="U41" s="21"/>
+      <c r="V41" s="5"/>
+      <c r="W41" s="5"/>
+      <c r="X41" s="5"/>
+      <c r="Y41" s="5"/>
+      <c r="Z41" s="26"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A42" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I42" s="3">
+        <v>13</v>
+      </c>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="9"/>
+      <c r="N42" s="16"/>
+      <c r="O42" s="16"/>
+      <c r="P42" s="16"/>
+      <c r="Q42" s="16"/>
+      <c r="R42" s="16"/>
+      <c r="S42" s="16"/>
+      <c r="T42" s="16"/>
+      <c r="U42" s="17"/>
+      <c r="V42" s="3"/>
+      <c r="W42" s="3"/>
+      <c r="X42" s="3"/>
+      <c r="Y42" s="3"/>
+      <c r="Z42" s="26"/>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A43" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" s="4">
+        <v>384</v>
+      </c>
+      <c r="E43" s="4">
+        <v>48</v>
+      </c>
+      <c r="F43" s="4">
+        <v>1</v>
+      </c>
+      <c r="G43" s="4">
+        <v>0</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I43" s="4">
+        <v>13</v>
+      </c>
+      <c r="J43" s="4">
+        <f>I43^2*E43</f>
+        <v>8112</v>
+      </c>
+      <c r="K43" s="4">
+        <f>I43^2*D43</f>
+        <v>64896</v>
+      </c>
+      <c r="L43" s="4">
+        <v>18432</v>
+      </c>
+      <c r="M43" s="10"/>
+      <c r="N43" s="18">
+        <f>N39+L39/2+E39/2</f>
+        <v>116744</v>
+      </c>
+      <c r="O43" s="18">
+        <f>N43+L43/2-1</f>
+        <v>125959</v>
+      </c>
+      <c r="P43" s="18">
+        <f>O43+1</f>
+        <v>125960</v>
+      </c>
+      <c r="Q43" s="18">
+        <f>P43+E43/2-1</f>
+        <v>125983</v>
+      </c>
+      <c r="R43" s="18"/>
+      <c r="S43" s="18"/>
+      <c r="T43" s="18">
+        <f>U39+1</f>
+        <v>1972040</v>
+      </c>
+      <c r="U43" s="19">
+        <f>T43+J43/2-1</f>
+        <v>1976095</v>
+      </c>
+      <c r="V43" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W43" s="4">
+        <v>1</v>
+      </c>
+      <c r="X43" s="4">
+        <f>0.0000032*L43+0.0000064*J43</f>
+        <v>0.1108992</v>
+      </c>
+      <c r="Y43" s="4">
+        <f>K43*V43*W43</f>
+        <v>12979.2</v>
+      </c>
+      <c r="Z43" s="26"/>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A44" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="20"/>
+      <c r="O44" s="20"/>
+      <c r="P44" s="20"/>
+      <c r="Q44" s="20"/>
+      <c r="R44" s="20"/>
+      <c r="S44" s="20"/>
+      <c r="T44" s="20"/>
+      <c r="U44" s="21"/>
+      <c r="V44" s="5"/>
+      <c r="W44" s="5"/>
+      <c r="X44" s="5"/>
+      <c r="Y44" s="5"/>
+      <c r="Z44" s="26"/>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A45" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D45" s="4">
+        <v>48</v>
+      </c>
+      <c r="E45" s="4">
+        <v>192</v>
+      </c>
+      <c r="F45" s="4">
+        <v>1</v>
+      </c>
+      <c r="G45" s="4">
+        <v>0</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I45" s="4">
+        <v>13</v>
+      </c>
+      <c r="J45" s="4">
+        <f t="shared" ref="J45:J46" si="24">I45^2*E45</f>
+        <v>32448</v>
+      </c>
+      <c r="K45" s="4">
+        <f t="shared" ref="K45:K46" si="25">I45^2*D45</f>
+        <v>8112</v>
+      </c>
+      <c r="L45" s="4">
+        <v>9216</v>
+      </c>
+      <c r="M45" s="10"/>
+      <c r="N45" s="18">
+        <f>N43+L43/2+E43/2</f>
+        <v>125984</v>
+      </c>
+      <c r="O45" s="18">
+        <f t="shared" ref="O45:O46" si="26">N45+L45/2-1</f>
+        <v>130591</v>
+      </c>
+      <c r="P45" s="18">
+        <f t="shared" ref="P45:P46" si="27">O45+1</f>
+        <v>130592</v>
+      </c>
+      <c r="Q45" s="18">
+        <f>P45+E45/2-1</f>
+        <v>130687</v>
+      </c>
+      <c r="R45" s="18"/>
+      <c r="S45" s="18"/>
+      <c r="T45" s="18">
+        <f>U43+1</f>
+        <v>1976096</v>
+      </c>
+      <c r="U45" s="19">
+        <f>T45+J45/2-1</f>
+        <v>1992319</v>
+      </c>
+      <c r="V45" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W45" s="4">
+        <v>0</v>
+      </c>
+      <c r="X45" s="4">
+        <f>0.0000032*L45+0.0000064*J45</f>
+        <v>0.23715839999999999</v>
+      </c>
+      <c r="Y45" s="4">
+        <f t="shared" ref="Y45:Y46" si="28">K45*V45*W45</f>
+        <v>0</v>
+      </c>
+      <c r="Z45" s="26"/>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A46" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D46" s="4">
+        <v>48</v>
+      </c>
+      <c r="E46" s="4">
+        <v>192</v>
+      </c>
+      <c r="F46" s="4">
+        <v>1</v>
+      </c>
+      <c r="G46" s="4">
+        <v>1</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I46" s="4">
+        <v>13</v>
+      </c>
+      <c r="J46" s="4">
+        <f t="shared" si="24"/>
+        <v>32448</v>
+      </c>
+      <c r="K46" s="4">
+        <f t="shared" si="25"/>
+        <v>8112</v>
+      </c>
+      <c r="L46" s="4">
+        <v>82944</v>
+      </c>
+      <c r="M46" s="10"/>
+      <c r="N46" s="18">
+        <f>N45+L45/2+E45/2</f>
+        <v>130688</v>
+      </c>
+      <c r="O46" s="18">
+        <f t="shared" si="26"/>
+        <v>172159</v>
+      </c>
+      <c r="P46" s="18">
+        <f t="shared" si="27"/>
+        <v>172160</v>
+      </c>
+      <c r="Q46" s="18">
+        <f>P46+E46/2-1</f>
+        <v>172255</v>
+      </c>
+      <c r="R46" s="18"/>
+      <c r="S46" s="18"/>
+      <c r="T46" s="18">
+        <f>U45+1</f>
+        <v>1992320</v>
+      </c>
+      <c r="U46" s="19">
+        <f>T46+J46/2-1</f>
+        <v>2008543</v>
+      </c>
+      <c r="V46" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W46" s="4">
+        <v>1</v>
+      </c>
+      <c r="X46" s="4">
+        <f>0.0000032*L46+0.0000064*J46</f>
+        <v>0.47308800000000001</v>
+      </c>
+      <c r="Y46" s="4">
+        <f t="shared" si="28"/>
+        <v>1622.4</v>
+      </c>
+      <c r="Z46" s="26"/>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A47" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="20"/>
+      <c r="O47" s="20"/>
+      <c r="P47" s="20"/>
+      <c r="Q47" s="20"/>
+      <c r="R47" s="20"/>
+      <c r="S47" s="20"/>
+      <c r="T47" s="20"/>
+      <c r="U47" s="21"/>
+      <c r="V47" s="5"/>
+      <c r="W47" s="5"/>
+      <c r="X47" s="5"/>
+      <c r="Y47" s="5"/>
+      <c r="Z47" s="26"/>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A48" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="11"/>
+      <c r="N48" s="20"/>
+      <c r="O48" s="20"/>
+      <c r="P48" s="20"/>
+      <c r="Q48" s="20"/>
+      <c r="R48" s="20"/>
+      <c r="S48" s="20"/>
+      <c r="T48" s="20"/>
+      <c r="U48" s="21"/>
+      <c r="V48" s="5"/>
+      <c r="W48" s="5"/>
+      <c r="X48" s="5"/>
+      <c r="Y48" s="5"/>
+      <c r="Z48" s="26"/>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I49" s="3">
+        <v>13</v>
+      </c>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="9"/>
+      <c r="N49" s="16"/>
+      <c r="O49" s="16"/>
+      <c r="P49" s="16"/>
+      <c r="Q49" s="16"/>
+      <c r="R49" s="16"/>
+      <c r="S49" s="16"/>
+      <c r="T49" s="16"/>
+      <c r="U49" s="17"/>
+      <c r="V49" s="3"/>
+      <c r="W49" s="3"/>
+      <c r="X49" s="3"/>
+      <c r="Y49" s="3"/>
+      <c r="Z49" s="26"/>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A50" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50" s="4">
+        <v>384</v>
+      </c>
+      <c r="E50" s="4">
+        <v>64</v>
+      </c>
+      <c r="F50" s="4">
+        <v>1</v>
+      </c>
+      <c r="G50" s="4">
+        <v>0</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="I50" s="4">
+        <v>13</v>
+      </c>
+      <c r="J50" s="4">
+        <f>I50^2*E50</f>
+        <v>10816</v>
+      </c>
+      <c r="K50" s="4">
+        <f>I50^2*D50</f>
+        <v>64896</v>
+      </c>
+      <c r="L50" s="4">
+        <v>24576</v>
+      </c>
+      <c r="M50" s="10"/>
+      <c r="N50" s="18">
+        <f>N46+L46/2+E46/2</f>
+        <v>172256</v>
+      </c>
+      <c r="O50" s="18">
+        <f>N50+L50/2-1</f>
+        <v>184543</v>
+      </c>
+      <c r="P50" s="18">
+        <f>O50+1</f>
+        <v>184544</v>
+      </c>
+      <c r="Q50" s="18">
+        <f>P50+E50/2-1</f>
+        <v>184575</v>
+      </c>
+      <c r="R50" s="18"/>
+      <c r="S50" s="18"/>
+      <c r="T50" s="18">
+        <f>U46+1</f>
+        <v>2008544</v>
+      </c>
+      <c r="U50" s="19">
+        <f>T50+J50/2-1</f>
+        <v>2013951</v>
+      </c>
+      <c r="V50" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W50" s="4">
+        <v>1</v>
+      </c>
+      <c r="X50" s="4">
+        <f>0.0000032*L50+0.0000064*J50</f>
+        <v>0.14786559999999999</v>
+      </c>
+      <c r="Y50" s="4">
+        <f>K50*V50*W50</f>
+        <v>12979.2</v>
+      </c>
+      <c r="Z50" s="26"/>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A51" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="11"/>
+      <c r="N51" s="20"/>
+      <c r="O51" s="20"/>
+      <c r="P51" s="20"/>
+      <c r="Q51" s="20"/>
+      <c r="R51" s="20"/>
+      <c r="S51" s="20"/>
+      <c r="T51" s="20"/>
+      <c r="U51" s="21"/>
+      <c r="V51" s="5"/>
+      <c r="W51" s="5"/>
+      <c r="X51" s="5"/>
+      <c r="Y51" s="5"/>
+      <c r="Z51" s="26"/>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A52" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D52" s="4">
+        <v>64</v>
+      </c>
+      <c r="E52" s="4">
+        <v>256</v>
+      </c>
+      <c r="F52" s="4">
+        <v>1</v>
+      </c>
+      <c r="G52" s="4">
+        <v>0</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I52" s="4">
+        <v>13</v>
+      </c>
+      <c r="J52" s="4">
+        <f t="shared" ref="J52:J53" si="29">I52^2*E52</f>
+        <v>43264</v>
+      </c>
+      <c r="K52" s="4">
+        <f t="shared" ref="K52:K53" si="30">I52^2*D52</f>
+        <v>10816</v>
+      </c>
+      <c r="L52" s="4">
+        <v>16384</v>
+      </c>
+      <c r="M52" s="10"/>
+      <c r="N52" s="18">
+        <f>N50+L50/2+E50/2</f>
+        <v>184576</v>
+      </c>
+      <c r="O52" s="18">
+        <f t="shared" ref="O52:O53" si="31">N52+L52/2-1</f>
+        <v>192767</v>
+      </c>
+      <c r="P52" s="18">
+        <f t="shared" ref="P52:P53" si="32">O52+1</f>
+        <v>192768</v>
+      </c>
+      <c r="Q52" s="18">
+        <f>P52+E52/2-1</f>
+        <v>192895</v>
+      </c>
+      <c r="R52" s="18"/>
+      <c r="S52" s="18"/>
+      <c r="T52" s="18">
+        <f>U50+1</f>
+        <v>2013952</v>
+      </c>
+      <c r="U52" s="19">
+        <f>T52+J52/2-1</f>
+        <v>2035583</v>
+      </c>
+      <c r="V52" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W52" s="4">
+        <v>0</v>
+      </c>
+      <c r="X52" s="4">
+        <f>0.0000032*L52+0.0000064*J52</f>
+        <v>0.32931840000000001</v>
+      </c>
+      <c r="Y52" s="4">
+        <f t="shared" ref="Y52:Y53" si="33">K52*V52*W52</f>
+        <v>0</v>
+      </c>
+      <c r="Z52" s="26"/>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A53" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D53" s="4">
+        <v>64</v>
+      </c>
+      <c r="E53" s="4">
+        <v>256</v>
+      </c>
+      <c r="F53" s="4">
+        <v>1</v>
+      </c>
+      <c r="G53" s="4">
+        <v>1</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I53" s="4">
+        <v>13</v>
+      </c>
+      <c r="J53" s="4">
+        <f t="shared" si="29"/>
+        <v>43264</v>
+      </c>
+      <c r="K53" s="4">
+        <f t="shared" si="30"/>
+        <v>10816</v>
+      </c>
+      <c r="L53" s="4">
+        <v>147456</v>
+      </c>
+      <c r="M53" s="10"/>
+      <c r="N53" s="18">
+        <f>N52+L52/2+E52/2</f>
+        <v>192896</v>
+      </c>
+      <c r="O53" s="18">
+        <f t="shared" si="31"/>
+        <v>266623</v>
+      </c>
+      <c r="P53" s="18">
+        <f t="shared" si="32"/>
+        <v>266624</v>
+      </c>
+      <c r="Q53" s="18">
+        <f>P53+E53/2-1</f>
+        <v>266751</v>
+      </c>
+      <c r="R53" s="18"/>
+      <c r="S53" s="18"/>
+      <c r="T53" s="18">
+        <f>U52+1</f>
+        <v>2035584</v>
+      </c>
+      <c r="U53" s="19">
+        <f>T53+J53/2-1</f>
+        <v>2057215</v>
+      </c>
+      <c r="V53" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W53" s="4">
+        <v>1</v>
+      </c>
+      <c r="X53" s="4">
+        <f>0.0000032*L53+0.0000064*J53</f>
+        <v>0.74874879999999999</v>
+      </c>
+      <c r="Y53" s="4">
+        <f t="shared" si="33"/>
+        <v>2163.2000000000003</v>
+      </c>
+      <c r="Z53" s="26"/>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A54" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="11"/>
+      <c r="N54" s="20"/>
+      <c r="O54" s="20"/>
+      <c r="P54" s="20"/>
+      <c r="Q54" s="20"/>
+      <c r="R54" s="20"/>
+      <c r="S54" s="20"/>
+      <c r="T54" s="20"/>
+      <c r="U54" s="21"/>
+      <c r="V54" s="5"/>
+      <c r="W54" s="5"/>
+      <c r="X54" s="5"/>
+      <c r="Y54" s="5"/>
+      <c r="Z54" s="26"/>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A55" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
+      <c r="M55" s="11"/>
+      <c r="N55" s="20"/>
+      <c r="O55" s="20"/>
+      <c r="P55" s="20"/>
+      <c r="Q55" s="20"/>
+      <c r="R55" s="20"/>
+      <c r="S55" s="20"/>
+      <c r="T55" s="20"/>
+      <c r="U55" s="21"/>
+      <c r="V55" s="5"/>
+      <c r="W55" s="5"/>
+      <c r="X55" s="5"/>
+      <c r="Y55" s="5"/>
+      <c r="Z55" s="26"/>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A56" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="I56" s="3">
+        <v>13</v>
+      </c>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+      <c r="L56" s="3"/>
+      <c r="M56" s="9"/>
+      <c r="N56" s="16"/>
+      <c r="O56" s="16"/>
+      <c r="P56" s="16"/>
+      <c r="Q56" s="16"/>
+      <c r="R56" s="16"/>
+      <c r="S56" s="16"/>
+      <c r="T56" s="16"/>
+      <c r="U56" s="17"/>
+      <c r="V56" s="3"/>
+      <c r="W56" s="3"/>
+      <c r="X56" s="3"/>
+      <c r="Y56" s="3"/>
+      <c r="Z56" s="26"/>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A57" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D57" s="4">
+        <v>512</v>
+      </c>
+      <c r="E57" s="4">
+        <v>64</v>
+      </c>
+      <c r="F57" s="4">
+        <v>1</v>
+      </c>
+      <c r="G57" s="4">
+        <v>0</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="I57" s="4">
+        <v>13</v>
+      </c>
+      <c r="J57" s="4">
+        <f>I57^2*E57</f>
+        <v>10816</v>
+      </c>
+      <c r="K57" s="4">
+        <f>I57^2*D57</f>
+        <v>86528</v>
+      </c>
+      <c r="L57" s="4">
+        <v>32768</v>
+      </c>
+      <c r="M57" s="10"/>
+      <c r="N57" s="18">
+        <f>N53+L53/2+E53/2</f>
+        <v>266752</v>
+      </c>
+      <c r="O57" s="18">
+        <f>N57+L57/2-1</f>
+        <v>283135</v>
+      </c>
+      <c r="P57" s="18">
+        <f>O57+1</f>
+        <v>283136</v>
+      </c>
+      <c r="Q57" s="18">
+        <f>P57+E57/2-1</f>
+        <v>283167</v>
+      </c>
+      <c r="R57" s="18"/>
+      <c r="S57" s="18"/>
+      <c r="T57" s="18">
+        <f>U53+1</f>
+        <v>2057216</v>
+      </c>
+      <c r="U57" s="19">
+        <f>T57+J57/2-1</f>
+        <v>2062623</v>
+      </c>
+      <c r="V57" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W57" s="4">
+        <v>1</v>
+      </c>
+      <c r="X57" s="4">
+        <f>0.0000032*L57+0.0000064*J57</f>
+        <v>0.17408000000000001</v>
+      </c>
+      <c r="Y57" s="4">
+        <f>K57*V57*W57</f>
+        <v>17305.600000000002</v>
+      </c>
+      <c r="Z57" s="26"/>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A58" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
+      <c r="K58" s="5"/>
+      <c r="L58" s="5"/>
+      <c r="M58" s="11"/>
+      <c r="N58" s="20"/>
+      <c r="O58" s="20"/>
+      <c r="P58" s="20"/>
+      <c r="Q58" s="20"/>
+      <c r="R58" s="20"/>
+      <c r="S58" s="20"/>
+      <c r="T58" s="20"/>
+      <c r="U58" s="21"/>
+      <c r="V58" s="5"/>
+      <c r="W58" s="5"/>
+      <c r="X58" s="5"/>
+      <c r="Y58" s="5"/>
+      <c r="Z58" s="26"/>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A59" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D59" s="4">
+        <v>64</v>
+      </c>
+      <c r="E59" s="4">
+        <v>256</v>
+      </c>
+      <c r="F59" s="4">
+        <v>1</v>
+      </c>
+      <c r="G59" s="4">
+        <v>0</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I59" s="4">
+        <v>13</v>
+      </c>
+      <c r="J59" s="4">
+        <f t="shared" ref="J59:J60" si="34">I59^2*E59</f>
+        <v>43264</v>
+      </c>
+      <c r="K59" s="4">
+        <f t="shared" ref="K59:K60" si="35">I59^2*D59</f>
+        <v>10816</v>
+      </c>
+      <c r="L59" s="4">
+        <v>16384</v>
+      </c>
+      <c r="M59" s="10"/>
+      <c r="N59" s="18">
+        <f>N57+L57/2+E57/2</f>
+        <v>283168</v>
+      </c>
+      <c r="O59" s="18">
+        <f t="shared" ref="O59:O60" si="36">N59+L59/2-1</f>
+        <v>291359</v>
+      </c>
+      <c r="P59" s="18">
+        <f t="shared" ref="P59:P60" si="37">O59+1</f>
+        <v>291360</v>
+      </c>
+      <c r="Q59" s="18">
+        <f>P59+E59/2-1</f>
+        <v>291487</v>
+      </c>
+      <c r="R59" s="18"/>
+      <c r="S59" s="18"/>
+      <c r="T59" s="18">
+        <f>U57+1</f>
+        <v>2062624</v>
+      </c>
+      <c r="U59" s="19">
+        <f>T59+J59/2-1</f>
+        <v>2084255</v>
+      </c>
+      <c r="V59" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W59" s="4">
+        <v>0</v>
+      </c>
+      <c r="X59" s="4">
+        <f>0.0000032*L59+0.0000064*J59</f>
+        <v>0.32931840000000001</v>
+      </c>
+      <c r="Y59" s="4">
+        <f t="shared" ref="Y59:Y60" si="38">K59*V59*W59</f>
+        <v>0</v>
+      </c>
+      <c r="Z59" s="26"/>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A60" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D60" s="4">
+        <v>64</v>
+      </c>
+      <c r="E60" s="4">
+        <v>256</v>
+      </c>
+      <c r="F60" s="4">
+        <v>1</v>
+      </c>
+      <c r="G60" s="4">
+        <v>1</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I60" s="4">
+        <v>13</v>
+      </c>
+      <c r="J60" s="4">
+        <f t="shared" si="34"/>
+        <v>43264</v>
+      </c>
+      <c r="K60" s="4">
+        <f t="shared" si="35"/>
+        <v>10816</v>
+      </c>
+      <c r="L60" s="4">
+        <v>147456</v>
+      </c>
+      <c r="M60" s="10"/>
+      <c r="N60" s="18">
+        <f>N59+L59/2+E59/2</f>
+        <v>291488</v>
+      </c>
+      <c r="O60" s="18">
+        <f t="shared" si="36"/>
+        <v>365215</v>
+      </c>
+      <c r="P60" s="18">
+        <f t="shared" si="37"/>
+        <v>365216</v>
+      </c>
+      <c r="Q60" s="18">
+        <f>P60+E60/2-1</f>
+        <v>365343</v>
+      </c>
+      <c r="R60" s="18"/>
+      <c r="S60" s="18"/>
+      <c r="T60" s="18">
+        <f>U59+1</f>
+        <v>2084256</v>
+      </c>
+      <c r="U60" s="19">
+        <f>T60+J60/2-1</f>
+        <v>2105887</v>
+      </c>
+      <c r="V60" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W60" s="4">
+        <v>1</v>
+      </c>
+      <c r="X60" s="4">
+        <f>0.0000032*L60+0.0000064*J60</f>
+        <v>0.74874879999999999</v>
+      </c>
+      <c r="Y60" s="4">
+        <f t="shared" si="38"/>
+        <v>2163.2000000000003</v>
+      </c>
+      <c r="Z60" s="26"/>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A61" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="5"/>
+      <c r="L61" s="5"/>
+      <c r="M61" s="11"/>
+      <c r="N61" s="20"/>
+      <c r="O61" s="20"/>
+      <c r="P61" s="20"/>
+      <c r="Q61" s="20"/>
+      <c r="R61" s="20"/>
+      <c r="S61" s="20"/>
+      <c r="T61" s="20"/>
+      <c r="U61" s="21"/>
+      <c r="V61" s="5"/>
+      <c r="W61" s="5"/>
+      <c r="X61" s="5"/>
+      <c r="Y61" s="5"/>
+      <c r="Z61" s="26"/>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A62" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="5"/>
+      <c r="K62" s="5"/>
+      <c r="L62" s="5"/>
+      <c r="M62" s="11"/>
+      <c r="N62" s="20"/>
+      <c r="O62" s="20"/>
+      <c r="P62" s="20"/>
+      <c r="Q62" s="20"/>
+      <c r="R62" s="20"/>
+      <c r="S62" s="20"/>
+      <c r="T62" s="20"/>
+      <c r="U62" s="21"/>
+      <c r="V62" s="5"/>
+      <c r="W62" s="5"/>
+      <c r="X62" s="5"/>
+      <c r="Y62" s="5"/>
+      <c r="Z62" s="26"/>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A63" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="I63" s="3">
+        <v>13</v>
+      </c>
+      <c r="J63" s="3"/>
+      <c r="K63" s="3"/>
+      <c r="L63" s="3"/>
+      <c r="M63" s="9"/>
+      <c r="N63" s="16"/>
+      <c r="O63" s="16"/>
+      <c r="P63" s="16"/>
+      <c r="Q63" s="16"/>
+      <c r="R63" s="16"/>
+      <c r="S63" s="16"/>
+      <c r="T63" s="16"/>
+      <c r="U63" s="17"/>
+      <c r="V63" s="3"/>
+      <c r="W63" s="3"/>
+      <c r="X63" s="3"/>
+      <c r="Y63" s="3"/>
+      <c r="Z63" s="26"/>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A64" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5"/>
+      <c r="K64" s="5"/>
+      <c r="L64" s="5"/>
+      <c r="M64" s="11"/>
+      <c r="N64" s="20"/>
+      <c r="O64" s="20"/>
+      <c r="P64" s="20"/>
+      <c r="Q64" s="20"/>
+      <c r="R64" s="20"/>
+      <c r="S64" s="20"/>
+      <c r="T64" s="20"/>
+      <c r="U64" s="21"/>
+      <c r="V64" s="5"/>
+      <c r="W64" s="5"/>
+      <c r="X64" s="5"/>
+      <c r="Y64" s="5"/>
+      <c r="Z64" s="26"/>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A65" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D65" s="4">
+        <v>512</v>
+      </c>
+      <c r="E65" s="4">
+        <v>1000</v>
+      </c>
+      <c r="F65" s="4">
+        <v>1</v>
+      </c>
+      <c r="G65" s="4">
+        <v>0</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I65" s="4">
+        <v>13</v>
+      </c>
+      <c r="J65" s="4">
+        <f>I65^2*E65</f>
+        <v>169000</v>
+      </c>
+      <c r="K65" s="4">
+        <f>I65^2*D65</f>
+        <v>86528</v>
+      </c>
+      <c r="L65" s="4">
+        <v>512000</v>
+      </c>
+      <c r="M65" s="10"/>
+      <c r="N65" s="18">
+        <f>N60+L60/2+E60/2</f>
+        <v>365344</v>
+      </c>
+      <c r="O65" s="18">
+        <f>N65+L65/2-1</f>
+        <v>621343</v>
+      </c>
+      <c r="P65" s="18">
+        <f>O65+1</f>
+        <v>621344</v>
+      </c>
+      <c r="Q65" s="18">
+        <f>P65+E65/2-1</f>
+        <v>621843</v>
+      </c>
+      <c r="R65" s="18"/>
+      <c r="S65" s="18"/>
+      <c r="T65" s="18">
+        <f>U60+1</f>
+        <v>2105888</v>
+      </c>
+      <c r="U65" s="19">
+        <f>T65+J65/2-1</f>
+        <v>2190387</v>
+      </c>
+      <c r="V65" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W65" s="4">
+        <v>1</v>
+      </c>
+      <c r="X65" s="4">
+        <f>0.0000032*L65+0.0000064*J65</f>
+        <v>2.7199999999999998</v>
+      </c>
+      <c r="Y65" s="4">
+        <f>K65*V65*W65</f>
+        <v>17305.600000000002</v>
+      </c>
+      <c r="Z65" s="26"/>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A66" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
+      <c r="K66" s="5"/>
+      <c r="L66" s="5"/>
+      <c r="M66" s="11"/>
+      <c r="N66" s="20"/>
+      <c r="O66" s="20"/>
+      <c r="P66" s="20"/>
+      <c r="Q66" s="20"/>
+      <c r="R66" s="20"/>
+      <c r="S66" s="20"/>
+      <c r="T66" s="20"/>
+      <c r="U66" s="21"/>
+      <c r="V66" s="5"/>
+      <c r="W66" s="5"/>
+      <c r="X66" s="5"/>
+      <c r="Y66" s="5"/>
+      <c r="Z66" s="26"/>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A67" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6">
+        <v>1000</v>
+      </c>
+      <c r="F67" s="6">
+        <v>1</v>
+      </c>
+      <c r="G67" s="6">
+        <v>0</v>
+      </c>
+      <c r="H67" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I67" s="6">
+        <v>1</v>
+      </c>
+      <c r="J67" s="6">
+        <f>I67^2*E67</f>
+        <v>1000</v>
+      </c>
+      <c r="K67" s="6">
+        <f>J67</f>
+        <v>1000</v>
+      </c>
+      <c r="L67" s="6"/>
+      <c r="M67" s="12"/>
+      <c r="N67" s="22"/>
+      <c r="O67" s="22"/>
+      <c r="P67" s="22"/>
+      <c r="Q67" s="22"/>
+      <c r="R67" s="22"/>
+      <c r="S67" s="22"/>
+      <c r="T67" s="22">
+        <f>U65+1</f>
+        <v>2190388</v>
+      </c>
+      <c r="U67" s="23">
+        <f>T67+J67/2-1</f>
+        <v>2190887</v>
+      </c>
+      <c r="V67" s="6">
+        <v>1.2</v>
+      </c>
+      <c r="W67" s="6">
+        <v>1</v>
+      </c>
+      <c r="X67" s="6">
+        <f>0.0000064*J67</f>
+        <v>6.3999999999999994E-3</v>
+      </c>
+      <c r="Y67" s="6">
+        <f>K67*V67*W67</f>
+        <v>1200</v>
+      </c>
+      <c r="Z67" s="26"/>
+    </row>
+    <row r="68" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A68" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
+      <c r="M68" s="9"/>
+      <c r="N68" s="16"/>
+      <c r="O68" s="16"/>
+      <c r="P68" s="16"/>
+      <c r="Q68" s="16"/>
+      <c r="R68" s="16"/>
+      <c r="S68" s="16"/>
+      <c r="T68" s="16"/>
+      <c r="U68" s="17"/>
+      <c r="V68" s="3"/>
+      <c r="W68" s="3"/>
+      <c r="X68" s="3"/>
+      <c r="Y68" s="3"/>
+      <c r="Z68" s="26"/>
+    </row>
+    <row r="69" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A69" s="26"/>
+      <c r="B69" s="26"/>
+      <c r="C69" s="26"/>
+      <c r="D69" s="26"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="26"/>
+      <c r="G69" s="26"/>
+      <c r="H69" s="26"/>
+      <c r="I69" s="26"/>
+      <c r="J69" s="26">
+        <f>SUM(J2:J68)</f>
+        <v>3071056</v>
+      </c>
+      <c r="K69" s="26"/>
+      <c r="L69" s="26">
+        <f>SUM(L3:L68)</f>
+        <v>1231552</v>
+      </c>
+      <c r="M69" s="13"/>
+      <c r="N69" s="24"/>
+      <c r="O69" s="24"/>
+      <c r="P69" s="24"/>
+      <c r="Q69" s="24"/>
+      <c r="R69" s="24"/>
+      <c r="S69" s="24"/>
+      <c r="T69" s="24"/>
+      <c r="U69" s="25"/>
+      <c r="V69" s="26"/>
+      <c r="W69" s="26"/>
+      <c r="X69" s="26">
+        <f>SUM(X2:X68)</f>
+        <v>23.114035199999996</v>
+      </c>
+      <c r="Y69" s="26">
+        <f t="shared" ref="Y69" si="39">SUM(Y3:Y68)</f>
+        <v>388579.16000000003</v>
+      </c>
+      <c r="Z69" s="26"/>
+    </row>
+    <row r="70" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A70" s="26"/>
+      <c r="B70" s="26"/>
+      <c r="C70" s="26"/>
+      <c r="D70" s="26"/>
+      <c r="E70" s="26"/>
+      <c r="F70" s="26"/>
+      <c r="G70" s="26"/>
+      <c r="H70" s="26"/>
+      <c r="I70" s="26"/>
+      <c r="J70" s="26">
+        <f>J69*16/1024/8</f>
+        <v>5998.15625</v>
+      </c>
+      <c r="K70" s="26"/>
+      <c r="L70" s="26">
+        <f>L69*16/1024/8</f>
+        <v>2405.375</v>
+      </c>
+      <c r="M70" s="13"/>
+      <c r="N70" s="24"/>
+      <c r="O70" s="24"/>
+      <c r="P70" s="24"/>
+      <c r="Q70" s="24"/>
+      <c r="R70" s="24"/>
+      <c r="S70" s="24"/>
+      <c r="T70" s="24"/>
+      <c r="U70" s="25"/>
+      <c r="V70" s="26"/>
+      <c r="W70" s="26"/>
+      <c r="X70" s="26"/>
+      <c r="Y70" s="26"/>
+      <c r="Z70" s="26"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:B70" xr:uid="{009522EF-F8DC-42BE-8F4B-D751FC8B03E1}"/>
+  <mergeCells count="5">
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix submodule reset, fix parallelism
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF30648-3F2D-4D3A-9C43-46D32F2485BC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A01F76A-E7AE-4EAF-863A-EE77608D3C57}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7860" activeTab="1" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
@@ -873,30 +873,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -929,16 +905,40 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1317,32 +1317,32 @@
       <c r="G1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="54" t="s">
+      <c r="H1" s="68" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="54"/>
+      <c r="I1" s="68"/>
       <c r="J1" s="2" t="s">
         <v>86</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="L1" s="55" t="s">
+      <c r="L1" s="69" t="s">
         <v>110</v>
       </c>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55" t="s">
+      <c r="M1" s="69"/>
+      <c r="N1" s="69" t="s">
         <v>112</v>
       </c>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55" t="s">
+      <c r="O1" s="69"/>
+      <c r="P1" s="69" t="s">
         <v>111</v>
       </c>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55" t="s">
+      <c r="Q1" s="69"/>
+      <c r="R1" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="S1" s="56"/>
+      <c r="S1" s="70"/>
       <c r="T1" s="14" t="s">
         <v>115</v>
       </c>
@@ -5168,8 +5168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80B23C6-EAEB-43B1-B045-456C36085CFA}">
   <dimension ref="A1:AC71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="X68" sqref="X68"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5186,11 +5186,11 @@
     <col min="13" max="13" width="12.90625" style="41" customWidth="1"/>
     <col min="14" max="14" width="7.81640625" style="41" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.81640625" style="42" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.81640625" style="67" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.81640625" style="59" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6.81640625" style="53" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.81640625" style="73" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.81640625" style="65" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6.81640625" style="53" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.81640625" style="73" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.81640625" style="65" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="5.81640625" style="53" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="17.26953125" style="51" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="9.81640625" style="51" bestFit="1" customWidth="1"/>
@@ -5204,42 +5204,42 @@
     <row r="1" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A1" s="27"/>
       <c r="B1" s="28"/>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="74" t="s">
         <v>117</v>
       </c>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
       <c r="F1" s="29" t="s">
         <v>118</v>
       </c>
       <c r="G1" s="28"/>
       <c r="H1" s="28"/>
-      <c r="I1" s="58" t="s">
+      <c r="I1" s="72" t="s">
         <v>142</v>
       </c>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="61" t="s">
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="75" t="s">
         <v>113</v>
       </c>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="55"/>
-      <c r="W1" s="55"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="57" t="s">
+      <c r="Q1" s="69"/>
+      <c r="R1" s="69"/>
+      <c r="S1" s="69"/>
+      <c r="T1" s="69"/>
+      <c r="U1" s="69"/>
+      <c r="V1" s="69"/>
+      <c r="W1" s="69"/>
+      <c r="X1" s="70"/>
+      <c r="Y1" s="71" t="s">
         <v>139</v>
       </c>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
+      <c r="Z1" s="68"/>
+      <c r="AA1" s="68"/>
+      <c r="AB1" s="68"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
@@ -5248,10 +5248,10 @@
       <c r="B2" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="72" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="58"/>
+      <c r="D2" s="72"/>
       <c r="E2" s="30" t="s">
         <v>84</v>
       </c>
@@ -5264,11 +5264,11 @@
       <c r="H2" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="I2" s="58" t="s">
+      <c r="I2" s="72" t="s">
         <v>77</v>
       </c>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
       <c r="L2" s="30" t="s">
         <v>116</v>
       </c>
@@ -5281,25 +5281,25 @@
       <c r="O2" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="P2" s="74" t="s">
+      <c r="P2" s="76" t="s">
         <v>119</v>
       </c>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="75" t="s">
+      <c r="Q2" s="77"/>
+      <c r="R2" s="77" t="s">
         <v>120</v>
       </c>
-      <c r="S2" s="75"/>
-      <c r="T2" s="75" t="s">
+      <c r="S2" s="77"/>
+      <c r="T2" s="77" t="s">
         <v>121</v>
       </c>
-      <c r="U2" s="75"/>
+      <c r="U2" s="77"/>
       <c r="V2" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="W2" s="76" t="s">
+      <c r="W2" s="66" t="s">
         <v>122</v>
       </c>
-      <c r="X2" s="77" t="s">
+      <c r="X2" s="67" t="s">
         <v>123</v>
       </c>
       <c r="Y2" s="26" t="s">
@@ -5347,7 +5347,7 @@
       <c r="M3" s="32"/>
       <c r="N3" s="32"/>
       <c r="O3" s="33"/>
-      <c r="P3" s="62">
+      <c r="P3" s="54">
         <f>R4</f>
         <v>805888</v>
       </c>
@@ -5355,14 +5355,14 @@
         <f>DEC2HEX(P3)</f>
         <v>C4C00</v>
       </c>
-      <c r="R3" s="68">
+      <c r="R3" s="60">
         <v>655360</v>
       </c>
       <c r="S3" s="16" t="str">
         <f>DEC2HEX(R3)</f>
         <v>A0000</v>
       </c>
-      <c r="T3" s="68"/>
+      <c r="T3" s="60"/>
       <c r="U3" s="16"/>
       <c r="V3" s="43"/>
       <c r="W3" s="43"/>
@@ -5429,7 +5429,7 @@
         <f>_xlfn.CEILING.MATH(D4^2*E4/2)*F4</f>
         <v>896</v>
       </c>
-      <c r="P4" s="63">
+      <c r="P4" s="55">
         <f>R6</f>
         <v>1594432</v>
       </c>
@@ -5437,7 +5437,7 @@
         <f>DEC2HEX(P4)</f>
         <v>185440</v>
       </c>
-      <c r="R4" s="69">
+      <c r="R4" s="61">
         <f>R3+K3</f>
         <v>805888</v>
       </c>
@@ -5445,7 +5445,7 @@
         <f>DEC2HEX(R4)</f>
         <v>C4C00</v>
       </c>
-      <c r="T4" s="69">
+      <c r="T4" s="61">
         <v>4096</v>
       </c>
       <c r="U4" s="18" t="str">
@@ -5497,11 +5497,11 @@
       <c r="M5" s="36"/>
       <c r="N5" s="36"/>
       <c r="O5" s="37"/>
-      <c r="P5" s="64"/>
+      <c r="P5" s="56"/>
       <c r="Q5" s="20"/>
-      <c r="R5" s="70"/>
+      <c r="R5" s="62"/>
       <c r="S5" s="20"/>
-      <c r="T5" s="70"/>
+      <c r="T5" s="62"/>
       <c r="U5" s="20"/>
       <c r="V5" s="47"/>
       <c r="W5" s="47"/>
@@ -5550,7 +5550,7 @@
       <c r="M6" s="38"/>
       <c r="N6" s="38"/>
       <c r="O6" s="39"/>
-      <c r="P6" s="65">
+      <c r="P6" s="57">
         <f>R7</f>
         <v>1788032</v>
       </c>
@@ -5558,7 +5558,7 @@
         <f>DEC2HEX(P6)</f>
         <v>1B4880</v>
       </c>
-      <c r="R6" s="71">
+      <c r="R6" s="63">
         <f>R4+K4</f>
         <v>1594432</v>
       </c>
@@ -5566,7 +5566,7 @@
         <f>DEC2HEX(R6)</f>
         <v>185440</v>
       </c>
-      <c r="T6" s="71"/>
+      <c r="T6" s="63"/>
       <c r="U6" s="22" t="s">
         <v>150</v>
       </c>
@@ -5646,7 +5646,7 @@
         <f>_xlfn.CEILING.MATH(D7^2*E7/2)*F7</f>
         <v>512</v>
       </c>
-      <c r="P7" s="63">
+      <c r="P7" s="55">
         <f>R9</f>
         <v>1836432</v>
       </c>
@@ -5654,7 +5654,7 @@
         <f>DEC2HEX(P7)</f>
         <v>1C0590</v>
       </c>
-      <c r="R7" s="69">
+      <c r="R7" s="61">
         <f>R6+K6</f>
         <v>1788032</v>
       </c>
@@ -5662,7 +5662,7 @@
         <f>DEC2HEX(R7)</f>
         <v>1B4880</v>
       </c>
-      <c r="T7" s="69">
+      <c r="T7" s="61">
         <f>T4+O4</f>
         <v>4992</v>
       </c>
@@ -5715,11 +5715,11 @@
       <c r="M8" s="36"/>
       <c r="N8" s="36"/>
       <c r="O8" s="37"/>
-      <c r="P8" s="64"/>
+      <c r="P8" s="56"/>
       <c r="Q8" s="20"/>
-      <c r="R8" s="70"/>
+      <c r="R8" s="62"/>
       <c r="S8" s="20"/>
-      <c r="T8" s="70"/>
+      <c r="T8" s="62"/>
       <c r="U8" s="20"/>
       <c r="V8" s="47"/>
       <c r="W8" s="47"/>
@@ -5781,7 +5781,7 @@
         <f t="shared" ref="O9:O10" si="4">_xlfn.CEILING.MATH(D9^2*E9/2)*F9</f>
         <v>512</v>
       </c>
-      <c r="P9" s="63">
+      <c r="P9" s="55">
         <f>R10</f>
         <v>2030032</v>
       </c>
@@ -5789,7 +5789,7 @@
         <f t="shared" ref="Q9:Q10" si="5">DEC2HEX(P9)</f>
         <v>1EF9D0</v>
       </c>
-      <c r="R9" s="69">
+      <c r="R9" s="61">
         <f>R7+K7</f>
         <v>1836432</v>
       </c>
@@ -5797,7 +5797,7 @@
         <f t="shared" ref="S9:S10" si="6">DEC2HEX(R9)</f>
         <v>1C0590</v>
       </c>
-      <c r="T9" s="69">
+      <c r="T9" s="61">
         <f>T7+O7</f>
         <v>5504</v>
       </c>
@@ -5881,7 +5881,7 @@
         <f t="shared" si="4"/>
         <v>4608</v>
       </c>
-      <c r="P10" s="63">
+      <c r="P10" s="55">
         <f>R14</f>
         <v>2223632</v>
       </c>
@@ -5889,7 +5889,7 @@
         <f t="shared" si="5"/>
         <v>21EE10</v>
       </c>
-      <c r="R10" s="69">
+      <c r="R10" s="61">
         <f>R9+K9</f>
         <v>2030032</v>
       </c>
@@ -5897,7 +5897,7 @@
         <f t="shared" si="6"/>
         <v>1EF9D0</v>
       </c>
-      <c r="T10" s="69">
+      <c r="T10" s="61">
         <f>T9+O9</f>
         <v>6016</v>
       </c>
@@ -5950,11 +5950,11 @@
       <c r="M11" s="36"/>
       <c r="N11" s="36"/>
       <c r="O11" s="37"/>
-      <c r="P11" s="64"/>
+      <c r="P11" s="56"/>
       <c r="Q11" s="20"/>
-      <c r="R11" s="70"/>
+      <c r="R11" s="62"/>
       <c r="S11" s="20"/>
-      <c r="T11" s="70"/>
+      <c r="T11" s="62"/>
       <c r="U11" s="20"/>
       <c r="V11" s="47"/>
       <c r="W11" s="47"/>
@@ -5985,11 +5985,11 @@
       <c r="M12" s="36"/>
       <c r="N12" s="36"/>
       <c r="O12" s="37"/>
-      <c r="P12" s="64"/>
+      <c r="P12" s="56"/>
       <c r="Q12" s="20"/>
-      <c r="R12" s="70"/>
+      <c r="R12" s="62"/>
       <c r="S12" s="20"/>
-      <c r="T12" s="70"/>
+      <c r="T12" s="62"/>
       <c r="U12" s="20"/>
       <c r="V12" s="47"/>
       <c r="W12" s="47"/>
@@ -6024,11 +6024,11 @@
       <c r="M13" s="32"/>
       <c r="N13" s="32"/>
       <c r="O13" s="33"/>
-      <c r="P13" s="62"/>
+      <c r="P13" s="54"/>
       <c r="Q13" s="16"/>
-      <c r="R13" s="68"/>
+      <c r="R13" s="60"/>
       <c r="S13" s="16"/>
-      <c r="T13" s="68"/>
+      <c r="T13" s="60"/>
       <c r="U13" s="16"/>
       <c r="V13" s="43"/>
       <c r="W13" s="43"/>
@@ -6090,7 +6090,7 @@
         <f>_xlfn.CEILING.MATH(D14^2*E14/2)*F14</f>
         <v>1024</v>
       </c>
-      <c r="P14" s="63">
+      <c r="P14" s="55">
         <f>R16</f>
         <v>2272032</v>
       </c>
@@ -6098,7 +6098,7 @@
         <f>DEC2HEX(P14)</f>
         <v>22AB20</v>
       </c>
-      <c r="R14" s="69">
+      <c r="R14" s="61">
         <f>R10+K10</f>
         <v>2223632</v>
       </c>
@@ -6106,7 +6106,7 @@
         <f>DEC2HEX(R14)</f>
         <v>21EE10</v>
       </c>
-      <c r="T14" s="69">
+      <c r="T14" s="61">
         <f>T10+O10</f>
         <v>10624</v>
       </c>
@@ -6159,11 +6159,11 @@
       <c r="M15" s="36"/>
       <c r="N15" s="36"/>
       <c r="O15" s="37"/>
-      <c r="P15" s="64"/>
+      <c r="P15" s="56"/>
       <c r="Q15" s="20"/>
-      <c r="R15" s="70"/>
+      <c r="R15" s="62"/>
       <c r="S15" s="20"/>
-      <c r="T15" s="70"/>
+      <c r="T15" s="62"/>
       <c r="U15" s="20"/>
       <c r="V15" s="47"/>
       <c r="W15" s="47"/>
@@ -6225,7 +6225,7 @@
         <f t="shared" ref="O16:O17" si="12">_xlfn.CEILING.MATH(D16^2*E16/2)*F16</f>
         <v>512</v>
       </c>
-      <c r="P16" s="63">
+      <c r="P16" s="55">
         <f>R17</f>
         <v>2465632</v>
       </c>
@@ -6233,7 +6233,7 @@
         <f t="shared" ref="Q16:Q17" si="13">DEC2HEX(P16)</f>
         <v>259F60</v>
       </c>
-      <c r="R16" s="69">
+      <c r="R16" s="61">
         <f>R14+K14</f>
         <v>2272032</v>
       </c>
@@ -6241,7 +6241,7 @@
         <f t="shared" ref="S16:S17" si="14">DEC2HEX(R16)</f>
         <v>22AB20</v>
       </c>
-      <c r="T16" s="69">
+      <c r="T16" s="61">
         <f>T14+O14</f>
         <v>11648</v>
       </c>
@@ -6325,7 +6325,7 @@
         <f t="shared" si="12"/>
         <v>4608</v>
       </c>
-      <c r="P17" s="63">
+      <c r="P17" s="55">
         <f>R21</f>
         <v>2659232</v>
       </c>
@@ -6333,7 +6333,7 @@
         <f t="shared" si="13"/>
         <v>2893A0</v>
       </c>
-      <c r="R17" s="69">
+      <c r="R17" s="61">
         <f>R16+K16</f>
         <v>2465632</v>
       </c>
@@ -6341,7 +6341,7 @@
         <f t="shared" si="14"/>
         <v>259F60</v>
       </c>
-      <c r="T17" s="69">
+      <c r="T17" s="61">
         <f>T16+O16</f>
         <v>12160</v>
       </c>
@@ -6394,11 +6394,11 @@
       <c r="M18" s="36"/>
       <c r="N18" s="36"/>
       <c r="O18" s="37"/>
-      <c r="P18" s="64"/>
+      <c r="P18" s="56"/>
       <c r="Q18" s="20"/>
-      <c r="R18" s="70"/>
+      <c r="R18" s="62"/>
       <c r="S18" s="20"/>
-      <c r="T18" s="70"/>
+      <c r="T18" s="62"/>
       <c r="U18" s="20"/>
       <c r="V18" s="47"/>
       <c r="W18" s="47"/>
@@ -6429,11 +6429,11 @@
       <c r="M19" s="36"/>
       <c r="N19" s="36"/>
       <c r="O19" s="37"/>
-      <c r="P19" s="64"/>
+      <c r="P19" s="56"/>
       <c r="Q19" s="20"/>
-      <c r="R19" s="70"/>
+      <c r="R19" s="62"/>
       <c r="S19" s="20"/>
-      <c r="T19" s="70"/>
+      <c r="T19" s="62"/>
       <c r="U19" s="20"/>
       <c r="V19" s="47"/>
       <c r="W19" s="47"/>
@@ -6468,11 +6468,11 @@
       <c r="M20" s="32"/>
       <c r="N20" s="32"/>
       <c r="O20" s="33"/>
-      <c r="P20" s="62"/>
+      <c r="P20" s="54"/>
       <c r="Q20" s="16"/>
-      <c r="R20" s="68"/>
+      <c r="R20" s="60"/>
       <c r="S20" s="16"/>
-      <c r="T20" s="68"/>
+      <c r="T20" s="60"/>
       <c r="U20" s="16"/>
       <c r="V20" s="43"/>
       <c r="W20" s="43"/>
@@ -6521,7 +6521,7 @@
       <c r="M21" s="38"/>
       <c r="N21" s="38"/>
       <c r="O21" s="39"/>
-      <c r="P21" s="65">
+      <c r="P21" s="57">
         <f>R22</f>
         <v>2752544</v>
       </c>
@@ -6529,7 +6529,7 @@
         <f>DEC2HEX(P21)</f>
         <v>2A0020</v>
       </c>
-      <c r="R21" s="71">
+      <c r="R21" s="63">
         <f>R17+K17</f>
         <v>2659232</v>
       </c>
@@ -6537,7 +6537,7 @@
         <f>DEC2HEX(R21)</f>
         <v>2893A0</v>
       </c>
-      <c r="T21" s="71"/>
+      <c r="T21" s="63"/>
       <c r="U21" s="22" t="s">
         <v>150</v>
       </c>
@@ -6617,7 +6617,7 @@
         <f>_xlfn.CEILING.MATH(D22^2*E22/2)*F22</f>
         <v>2048</v>
       </c>
-      <c r="P22" s="63">
+      <c r="P22" s="55">
         <f>R24</f>
         <v>2775872</v>
       </c>
@@ -6625,7 +6625,7 @@
         <f>DEC2HEX(P22)</f>
         <v>2A5B40</v>
       </c>
-      <c r="R22" s="69">
+      <c r="R22" s="61">
         <f>R21+K21</f>
         <v>2752544</v>
       </c>
@@ -6633,7 +6633,7 @@
         <f>DEC2HEX(R22)</f>
         <v>2A0020</v>
       </c>
-      <c r="T22" s="69">
+      <c r="T22" s="61">
         <f>T17+O17</f>
         <v>16768</v>
       </c>
@@ -6686,11 +6686,11 @@
       <c r="M23" s="36"/>
       <c r="N23" s="36"/>
       <c r="O23" s="37"/>
-      <c r="P23" s="64"/>
+      <c r="P23" s="56"/>
       <c r="Q23" s="20"/>
-      <c r="R23" s="70"/>
+      <c r="R23" s="62"/>
       <c r="S23" s="20"/>
-      <c r="T23" s="70"/>
+      <c r="T23" s="62"/>
       <c r="U23" s="20"/>
       <c r="V23" s="47"/>
       <c r="W23" s="47"/>
@@ -6752,7 +6752,7 @@
         <f t="shared" ref="O24:O25" si="20">_xlfn.CEILING.MATH(D24^2*E24/2)*F24</f>
         <v>2048</v>
       </c>
-      <c r="P24" s="63">
+      <c r="P24" s="55">
         <f>R25</f>
         <v>2869184</v>
       </c>
@@ -6760,7 +6760,7 @@
         <f t="shared" ref="Q24:Q25" si="21">DEC2HEX(P24)</f>
         <v>2BC7C0</v>
       </c>
-      <c r="R24" s="69">
+      <c r="R24" s="61">
         <f>R22+K22</f>
         <v>2775872</v>
       </c>
@@ -6768,7 +6768,7 @@
         <f t="shared" ref="S24:S25" si="22">DEC2HEX(R24)</f>
         <v>2A5B40</v>
       </c>
-      <c r="T24" s="69">
+      <c r="T24" s="61">
         <f>T22+O22</f>
         <v>18816</v>
       </c>
@@ -6852,7 +6852,7 @@
         <f t="shared" si="20"/>
         <v>18432</v>
       </c>
-      <c r="P25" s="63">
+      <c r="P25" s="55">
         <f>R29</f>
         <v>2962496</v>
       </c>
@@ -6860,7 +6860,7 @@
         <f t="shared" si="21"/>
         <v>2D3440</v>
       </c>
-      <c r="R25" s="69">
+      <c r="R25" s="61">
         <f>R24+K24</f>
         <v>2869184</v>
       </c>
@@ -6868,7 +6868,7 @@
         <f t="shared" si="22"/>
         <v>2BC7C0</v>
       </c>
-      <c r="T25" s="69">
+      <c r="T25" s="61">
         <f>T24+O24</f>
         <v>20864</v>
       </c>
@@ -6921,11 +6921,11 @@
       <c r="M26" s="36"/>
       <c r="N26" s="36"/>
       <c r="O26" s="37"/>
-      <c r="P26" s="64"/>
+      <c r="P26" s="56"/>
       <c r="Q26" s="20"/>
-      <c r="R26" s="70"/>
+      <c r="R26" s="62"/>
       <c r="S26" s="20"/>
-      <c r="T26" s="70"/>
+      <c r="T26" s="62"/>
       <c r="U26" s="20"/>
       <c r="V26" s="47"/>
       <c r="W26" s="47"/>
@@ -6956,11 +6956,11 @@
       <c r="M27" s="36"/>
       <c r="N27" s="36"/>
       <c r="O27" s="37"/>
-      <c r="P27" s="64"/>
+      <c r="P27" s="56"/>
       <c r="Q27" s="20"/>
-      <c r="R27" s="70"/>
+      <c r="R27" s="62"/>
       <c r="S27" s="20"/>
-      <c r="T27" s="70"/>
+      <c r="T27" s="62"/>
       <c r="U27" s="20"/>
       <c r="V27" s="47"/>
       <c r="W27" s="47"/>
@@ -6995,11 +6995,11 @@
       <c r="M28" s="32"/>
       <c r="N28" s="32"/>
       <c r="O28" s="33"/>
-      <c r="P28" s="62"/>
+      <c r="P28" s="54"/>
       <c r="Q28" s="16"/>
-      <c r="R28" s="68"/>
+      <c r="R28" s="60"/>
       <c r="S28" s="16"/>
-      <c r="T28" s="68"/>
+      <c r="T28" s="60"/>
       <c r="U28" s="16"/>
       <c r="V28" s="43"/>
       <c r="W28" s="43"/>
@@ -7061,7 +7061,7 @@
         <f>_xlfn.CEILING.MATH(D29^2*E29/2)*F29</f>
         <v>4096</v>
       </c>
-      <c r="P29" s="63">
+      <c r="P29" s="55">
         <f>R31</f>
         <v>2985824</v>
       </c>
@@ -7069,7 +7069,7 @@
         <f>DEC2HEX(P29)</f>
         <v>2D8F60</v>
       </c>
-      <c r="R29" s="69">
+      <c r="R29" s="61">
         <f>R25+K25</f>
         <v>2962496</v>
       </c>
@@ -7077,7 +7077,7 @@
         <f>DEC2HEX(R29)</f>
         <v>2D3440</v>
       </c>
-      <c r="T29" s="69">
+      <c r="T29" s="61">
         <f>T25+O25</f>
         <v>39296</v>
       </c>
@@ -7130,11 +7130,11 @@
       <c r="M30" s="36"/>
       <c r="N30" s="36"/>
       <c r="O30" s="37"/>
-      <c r="P30" s="64"/>
+      <c r="P30" s="56"/>
       <c r="Q30" s="20"/>
-      <c r="R30" s="70"/>
+      <c r="R30" s="62"/>
       <c r="S30" s="20"/>
-      <c r="T30" s="70"/>
+      <c r="T30" s="62"/>
       <c r="U30" s="20"/>
       <c r="V30" s="47"/>
       <c r="W30" s="47"/>
@@ -7196,7 +7196,7 @@
         <f t="shared" ref="O31:O32" si="28">_xlfn.CEILING.MATH(D31^2*E31/2)*F31</f>
         <v>2048</v>
       </c>
-      <c r="P31" s="63">
+      <c r="P31" s="55">
         <f>R32</f>
         <v>3079136</v>
       </c>
@@ -7204,7 +7204,7 @@
         <f t="shared" ref="Q31:Q32" si="29">DEC2HEX(P31)</f>
         <v>2EFBE0</v>
       </c>
-      <c r="R31" s="69">
+      <c r="R31" s="61">
         <f>R29+K29</f>
         <v>2985824</v>
       </c>
@@ -7212,7 +7212,7 @@
         <f t="shared" ref="S31:S32" si="30">DEC2HEX(R31)</f>
         <v>2D8F60</v>
       </c>
-      <c r="T31" s="69">
+      <c r="T31" s="61">
         <f>T29+O29</f>
         <v>43392</v>
       </c>
@@ -7296,7 +7296,7 @@
         <f t="shared" si="28"/>
         <v>18432</v>
       </c>
-      <c r="P32" s="63">
+      <c r="P32" s="55">
         <f>R36</f>
         <v>3172448</v>
       </c>
@@ -7304,7 +7304,7 @@
         <f t="shared" si="29"/>
         <v>306860</v>
       </c>
-      <c r="R32" s="69">
+      <c r="R32" s="61">
         <f>R31+K31</f>
         <v>3079136</v>
       </c>
@@ -7312,7 +7312,7 @@
         <f t="shared" si="30"/>
         <v>2EFBE0</v>
       </c>
-      <c r="T32" s="69">
+      <c r="T32" s="61">
         <f>T31+O31</f>
         <v>45440</v>
       </c>
@@ -7365,11 +7365,11 @@
       <c r="M33" s="36"/>
       <c r="N33" s="36"/>
       <c r="O33" s="37"/>
-      <c r="P33" s="64"/>
+      <c r="P33" s="56"/>
       <c r="Q33" s="20"/>
-      <c r="R33" s="70"/>
+      <c r="R33" s="62"/>
       <c r="S33" s="20"/>
-      <c r="T33" s="70"/>
+      <c r="T33" s="62"/>
       <c r="U33" s="20"/>
       <c r="V33" s="47"/>
       <c r="W33" s="47"/>
@@ -7400,11 +7400,11 @@
       <c r="M34" s="36"/>
       <c r="N34" s="36"/>
       <c r="O34" s="37"/>
-      <c r="P34" s="64"/>
+      <c r="P34" s="56"/>
       <c r="Q34" s="20"/>
-      <c r="R34" s="70"/>
+      <c r="R34" s="62"/>
       <c r="S34" s="20"/>
-      <c r="T34" s="70"/>
+      <c r="T34" s="62"/>
       <c r="U34" s="20"/>
       <c r="V34" s="47"/>
       <c r="W34" s="47"/>
@@ -7437,11 +7437,11 @@
       <c r="M35" s="32"/>
       <c r="N35" s="32"/>
       <c r="O35" s="33"/>
-      <c r="P35" s="62"/>
+      <c r="P35" s="54"/>
       <c r="Q35" s="16"/>
-      <c r="R35" s="68"/>
+      <c r="R35" s="60"/>
       <c r="S35" s="16"/>
-      <c r="T35" s="68"/>
+      <c r="T35" s="60"/>
       <c r="U35" s="16"/>
       <c r="V35" s="43"/>
       <c r="W35" s="43"/>
@@ -7490,7 +7490,7 @@
       <c r="M36" s="38"/>
       <c r="N36" s="38"/>
       <c r="O36" s="39"/>
-      <c r="P36" s="65">
+      <c r="P36" s="57">
         <f>R37</f>
         <v>3215712</v>
       </c>
@@ -7498,7 +7498,7 @@
         <f>DEC2HEX(P36)</f>
         <v>311160</v>
       </c>
-      <c r="R36" s="71">
+      <c r="R36" s="63">
         <f>R32+K32</f>
         <v>3172448</v>
       </c>
@@ -7506,7 +7506,7 @@
         <f>DEC2HEX(R36)</f>
         <v>306860</v>
       </c>
-      <c r="T36" s="71"/>
+      <c r="T36" s="63"/>
       <c r="U36" s="22" t="s">
         <v>150</v>
       </c>
@@ -7586,7 +7586,7 @@
         <f>_xlfn.CEILING.MATH(D37^2*E37/2)*F37</f>
         <v>6144</v>
       </c>
-      <c r="P37" s="63">
+      <c r="P37" s="55">
         <f>R39</f>
         <v>3223824</v>
       </c>
@@ -7594,7 +7594,7 @@
         <f>DEC2HEX(P37)</f>
         <v>313110</v>
       </c>
-      <c r="R37" s="69">
+      <c r="R37" s="61">
         <f>R36+K36</f>
         <v>3215712</v>
       </c>
@@ -7602,7 +7602,7 @@
         <f>DEC2HEX(R37)</f>
         <v>311160</v>
       </c>
-      <c r="T37" s="69">
+      <c r="T37" s="61">
         <f>T32+O32</f>
         <v>63872</v>
       </c>
@@ -7655,11 +7655,11 @@
       <c r="M38" s="36"/>
       <c r="N38" s="36"/>
       <c r="O38" s="37"/>
-      <c r="P38" s="64"/>
+      <c r="P38" s="56"/>
       <c r="Q38" s="20"/>
-      <c r="R38" s="70"/>
+      <c r="R38" s="62"/>
       <c r="S38" s="20"/>
-      <c r="T38" s="70"/>
+      <c r="T38" s="62"/>
       <c r="U38" s="20"/>
       <c r="V38" s="47"/>
       <c r="W38" s="47"/>
@@ -7721,7 +7721,7 @@
         <f t="shared" ref="O39:O40" si="36">_xlfn.CEILING.MATH(D39^2*E39/2)*F39</f>
         <v>4608</v>
       </c>
-      <c r="P39" s="63">
+      <c r="P39" s="55">
         <f>R40</f>
         <v>3256272</v>
       </c>
@@ -7729,7 +7729,7 @@
         <f t="shared" ref="Q39:Q40" si="37">DEC2HEX(P39)</f>
         <v>31AFD0</v>
       </c>
-      <c r="R39" s="69">
+      <c r="R39" s="61">
         <f>R37+K37</f>
         <v>3223824</v>
       </c>
@@ -7737,7 +7737,7 @@
         <f t="shared" ref="S39:S40" si="38">DEC2HEX(R39)</f>
         <v>313110</v>
       </c>
-      <c r="T39" s="69">
+      <c r="T39" s="61">
         <f>T37+O37</f>
         <v>70016</v>
       </c>
@@ -7821,7 +7821,7 @@
         <f t="shared" si="36"/>
         <v>41472</v>
       </c>
-      <c r="P40" s="63">
+      <c r="P40" s="55">
         <f>R44</f>
         <v>3288720</v>
       </c>
@@ -7829,7 +7829,7 @@
         <f t="shared" si="37"/>
         <v>322E90</v>
       </c>
-      <c r="R40" s="69">
+      <c r="R40" s="61">
         <f>R39+K39</f>
         <v>3256272</v>
       </c>
@@ -7837,7 +7837,7 @@
         <f t="shared" si="38"/>
         <v>31AFD0</v>
       </c>
-      <c r="T40" s="69">
+      <c r="T40" s="61">
         <f>T39+O39</f>
         <v>74624</v>
       </c>
@@ -7890,11 +7890,11 @@
       <c r="M41" s="36"/>
       <c r="N41" s="36"/>
       <c r="O41" s="37"/>
-      <c r="P41" s="64"/>
+      <c r="P41" s="56"/>
       <c r="Q41" s="20"/>
-      <c r="R41" s="70"/>
+      <c r="R41" s="62"/>
       <c r="S41" s="20"/>
-      <c r="T41" s="70"/>
+      <c r="T41" s="62"/>
       <c r="U41" s="20"/>
       <c r="V41" s="47"/>
       <c r="W41" s="47"/>
@@ -7925,11 +7925,11 @@
       <c r="M42" s="36"/>
       <c r="N42" s="36"/>
       <c r="O42" s="37"/>
-      <c r="P42" s="64"/>
+      <c r="P42" s="56"/>
       <c r="Q42" s="20"/>
-      <c r="R42" s="70"/>
+      <c r="R42" s="62"/>
       <c r="S42" s="20"/>
-      <c r="T42" s="70"/>
+      <c r="T42" s="62"/>
       <c r="U42" s="20"/>
       <c r="V42" s="47"/>
       <c r="W42" s="47"/>
@@ -7964,11 +7964,11 @@
       <c r="M43" s="32"/>
       <c r="N43" s="32"/>
       <c r="O43" s="33"/>
-      <c r="P43" s="62"/>
+      <c r="P43" s="54"/>
       <c r="Q43" s="16"/>
-      <c r="R43" s="68"/>
+      <c r="R43" s="60"/>
       <c r="S43" s="16"/>
-      <c r="T43" s="68"/>
+      <c r="T43" s="60"/>
       <c r="U43" s="16"/>
       <c r="V43" s="43"/>
       <c r="W43" s="43"/>
@@ -8030,7 +8030,7 @@
         <f>_xlfn.CEILING.MATH(D44^2*E44/2)*F44</f>
         <v>9216</v>
       </c>
-      <c r="P44" s="63">
+      <c r="P44" s="55">
         <f>R46</f>
         <v>3296832</v>
       </c>
@@ -8038,7 +8038,7 @@
         <f>DEC2HEX(P44)</f>
         <v>324E40</v>
       </c>
-      <c r="R44" s="69">
+      <c r="R44" s="61">
         <f>R40+K40</f>
         <v>3288720</v>
       </c>
@@ -8046,7 +8046,7 @@
         <f>DEC2HEX(R44)</f>
         <v>322E90</v>
       </c>
-      <c r="T44" s="69">
+      <c r="T44" s="61">
         <f>T40+O40</f>
         <v>116096</v>
       </c>
@@ -8099,11 +8099,11 @@
       <c r="M45" s="36"/>
       <c r="N45" s="36"/>
       <c r="O45" s="37"/>
-      <c r="P45" s="64"/>
+      <c r="P45" s="56"/>
       <c r="Q45" s="20"/>
-      <c r="R45" s="70"/>
+      <c r="R45" s="62"/>
       <c r="S45" s="20"/>
-      <c r="T45" s="70"/>
+      <c r="T45" s="62"/>
       <c r="U45" s="20"/>
       <c r="V45" s="47"/>
       <c r="W45" s="47"/>
@@ -8165,7 +8165,7 @@
         <f t="shared" ref="O46:O47" si="44">_xlfn.CEILING.MATH(D46^2*E46/2)*F46</f>
         <v>4608</v>
       </c>
-      <c r="P46" s="63">
+      <c r="P46" s="55">
         <f>R47</f>
         <v>3329280</v>
       </c>
@@ -8173,7 +8173,7 @@
         <f t="shared" ref="Q46:Q47" si="45">DEC2HEX(P46)</f>
         <v>32CD00</v>
       </c>
-      <c r="R46" s="69">
+      <c r="R46" s="61">
         <f>R44+K44</f>
         <v>3296832</v>
       </c>
@@ -8181,7 +8181,7 @@
         <f t="shared" ref="S46:S47" si="46">DEC2HEX(R46)</f>
         <v>324E40</v>
       </c>
-      <c r="T46" s="69">
+      <c r="T46" s="61">
         <f>T44+O44</f>
         <v>125312</v>
       </c>
@@ -8265,7 +8265,7 @@
         <f t="shared" si="44"/>
         <v>41472</v>
       </c>
-      <c r="P47" s="63">
+      <c r="P47" s="55">
         <f>R51</f>
         <v>3361728</v>
       </c>
@@ -8273,7 +8273,7 @@
         <f t="shared" si="45"/>
         <v>334BC0</v>
       </c>
-      <c r="R47" s="69">
+      <c r="R47" s="61">
         <f>R46+K46</f>
         <v>3329280</v>
       </c>
@@ -8281,7 +8281,7 @@
         <f t="shared" si="46"/>
         <v>32CD00</v>
       </c>
-      <c r="T47" s="69">
+      <c r="T47" s="61">
         <f>T46+O46</f>
         <v>129920</v>
       </c>
@@ -8334,11 +8334,11 @@
       <c r="M48" s="36"/>
       <c r="N48" s="36"/>
       <c r="O48" s="37"/>
-      <c r="P48" s="64"/>
+      <c r="P48" s="56"/>
       <c r="Q48" s="20"/>
-      <c r="R48" s="70"/>
+      <c r="R48" s="62"/>
       <c r="S48" s="20"/>
-      <c r="T48" s="70"/>
+      <c r="T48" s="62"/>
       <c r="U48" s="20"/>
       <c r="V48" s="47"/>
       <c r="W48" s="47"/>
@@ -8369,11 +8369,11 @@
       <c r="M49" s="36"/>
       <c r="N49" s="36"/>
       <c r="O49" s="37"/>
-      <c r="P49" s="64"/>
+      <c r="P49" s="56"/>
       <c r="Q49" s="20"/>
-      <c r="R49" s="70"/>
+      <c r="R49" s="62"/>
       <c r="S49" s="20"/>
-      <c r="T49" s="70"/>
+      <c r="T49" s="62"/>
       <c r="U49" s="20"/>
       <c r="V49" s="47"/>
       <c r="W49" s="47"/>
@@ -8408,11 +8408,11 @@
       <c r="M50" s="32"/>
       <c r="N50" s="32"/>
       <c r="O50" s="33"/>
-      <c r="P50" s="62"/>
+      <c r="P50" s="54"/>
       <c r="Q50" s="16"/>
-      <c r="R50" s="68"/>
+      <c r="R50" s="60"/>
       <c r="S50" s="16"/>
-      <c r="T50" s="68"/>
+      <c r="T50" s="60"/>
       <c r="U50" s="16"/>
       <c r="V50" s="43"/>
       <c r="W50" s="43"/>
@@ -8474,7 +8474,7 @@
         <f>_xlfn.CEILING.MATH(D51^2*E51/2)*F51</f>
         <v>12288</v>
       </c>
-      <c r="P51" s="63">
+      <c r="P51" s="55">
         <f>R53</f>
         <v>3372544</v>
       </c>
@@ -8482,7 +8482,7 @@
         <f>DEC2HEX(P51)</f>
         <v>337600</v>
       </c>
-      <c r="R51" s="69">
+      <c r="R51" s="61">
         <f>R47+K47</f>
         <v>3361728</v>
       </c>
@@ -8490,7 +8490,7 @@
         <f>DEC2HEX(R51)</f>
         <v>334BC0</v>
       </c>
-      <c r="T51" s="69">
+      <c r="T51" s="61">
         <f>T47+O47</f>
         <v>171392</v>
       </c>
@@ -8543,11 +8543,11 @@
       <c r="M52" s="36"/>
       <c r="N52" s="36"/>
       <c r="O52" s="37"/>
-      <c r="P52" s="64"/>
+      <c r="P52" s="56"/>
       <c r="Q52" s="20"/>
-      <c r="R52" s="70"/>
+      <c r="R52" s="62"/>
       <c r="S52" s="20"/>
-      <c r="T52" s="70"/>
+      <c r="T52" s="62"/>
       <c r="U52" s="20"/>
       <c r="V52" s="47"/>
       <c r="W52" s="47"/>
@@ -8609,7 +8609,7 @@
         <f t="shared" ref="O53:O54" si="52">_xlfn.CEILING.MATH(D53^2*E53/2)*F53</f>
         <v>8192</v>
       </c>
-      <c r="P53" s="63">
+      <c r="P53" s="55">
         <f>R54</f>
         <v>3415808</v>
       </c>
@@ -8617,7 +8617,7 @@
         <f t="shared" ref="Q53:Q54" si="53">DEC2HEX(P53)</f>
         <v>341F00</v>
       </c>
-      <c r="R53" s="69">
+      <c r="R53" s="61">
         <f>R51+K51</f>
         <v>3372544</v>
       </c>
@@ -8625,7 +8625,7 @@
         <f t="shared" ref="S53:S54" si="54">DEC2HEX(R53)</f>
         <v>337600</v>
       </c>
-      <c r="T53" s="69">
+      <c r="T53" s="61">
         <f>T51+O51</f>
         <v>183680</v>
       </c>
@@ -8709,7 +8709,7 @@
         <f t="shared" si="52"/>
         <v>73728</v>
       </c>
-      <c r="P54" s="63">
+      <c r="P54" s="55">
         <f>R58</f>
         <v>3459072</v>
       </c>
@@ -8717,7 +8717,7 @@
         <f t="shared" si="53"/>
         <v>34C800</v>
       </c>
-      <c r="R54" s="69">
+      <c r="R54" s="61">
         <f>R53+K53</f>
         <v>3415808</v>
       </c>
@@ -8725,7 +8725,7 @@
         <f t="shared" si="54"/>
         <v>341F00</v>
       </c>
-      <c r="T54" s="69">
+      <c r="T54" s="61">
         <f>T53+O53</f>
         <v>191872</v>
       </c>
@@ -8778,11 +8778,11 @@
       <c r="M55" s="36"/>
       <c r="N55" s="36"/>
       <c r="O55" s="37"/>
-      <c r="P55" s="64"/>
+      <c r="P55" s="56"/>
       <c r="Q55" s="20"/>
-      <c r="R55" s="70"/>
+      <c r="R55" s="62"/>
       <c r="S55" s="20"/>
-      <c r="T55" s="70"/>
+      <c r="T55" s="62"/>
       <c r="U55" s="20"/>
       <c r="V55" s="47"/>
       <c r="W55" s="47"/>
@@ -8813,11 +8813,11 @@
       <c r="M56" s="36"/>
       <c r="N56" s="36"/>
       <c r="O56" s="37"/>
-      <c r="P56" s="64"/>
+      <c r="P56" s="56"/>
       <c r="Q56" s="20"/>
-      <c r="R56" s="70"/>
+      <c r="R56" s="62"/>
       <c r="S56" s="20"/>
-      <c r="T56" s="70"/>
+      <c r="T56" s="62"/>
       <c r="U56" s="20"/>
       <c r="V56" s="47"/>
       <c r="W56" s="47"/>
@@ -8852,11 +8852,11 @@
       <c r="M57" s="32"/>
       <c r="N57" s="32"/>
       <c r="O57" s="33"/>
-      <c r="P57" s="62"/>
+      <c r="P57" s="54"/>
       <c r="Q57" s="16"/>
-      <c r="R57" s="68"/>
+      <c r="R57" s="60"/>
       <c r="S57" s="16"/>
-      <c r="T57" s="68"/>
+      <c r="T57" s="60"/>
       <c r="U57" s="16"/>
       <c r="V57" s="43"/>
       <c r="W57" s="43"/>
@@ -8918,7 +8918,7 @@
         <f>_xlfn.CEILING.MATH(D58^2*E58/2)*F58</f>
         <v>16384</v>
       </c>
-      <c r="P58" s="63">
+      <c r="P58" s="55">
         <f>R60</f>
         <v>3469888</v>
       </c>
@@ -8926,7 +8926,7 @@
         <f>DEC2HEX(P58)</f>
         <v>34F240</v>
       </c>
-      <c r="R58" s="69">
+      <c r="R58" s="61">
         <f>R54+K54</f>
         <v>3459072</v>
       </c>
@@ -8934,7 +8934,7 @@
         <f>DEC2HEX(R58)</f>
         <v>34C800</v>
       </c>
-      <c r="T58" s="69">
+      <c r="T58" s="61">
         <f>T54+O54</f>
         <v>265600</v>
       </c>
@@ -8987,11 +8987,11 @@
       <c r="M59" s="36"/>
       <c r="N59" s="36"/>
       <c r="O59" s="37"/>
-      <c r="P59" s="64"/>
+      <c r="P59" s="56"/>
       <c r="Q59" s="20"/>
-      <c r="R59" s="70"/>
+      <c r="R59" s="62"/>
       <c r="S59" s="20"/>
-      <c r="T59" s="70"/>
+      <c r="T59" s="62"/>
       <c r="U59" s="20"/>
       <c r="V59" s="47"/>
       <c r="W59" s="47"/>
@@ -9053,7 +9053,7 @@
         <f t="shared" ref="O60:O61" si="60">_xlfn.CEILING.MATH(D60^2*E60/2)*F60</f>
         <v>8192</v>
       </c>
-      <c r="P60" s="63">
+      <c r="P60" s="55">
         <f>R61</f>
         <v>3513152</v>
       </c>
@@ -9061,7 +9061,7 @@
         <f t="shared" ref="Q60:Q61" si="61">DEC2HEX(P60)</f>
         <v>359B40</v>
       </c>
-      <c r="R60" s="69">
+      <c r="R60" s="61">
         <f>R58+K58</f>
         <v>3469888</v>
       </c>
@@ -9069,7 +9069,7 @@
         <f t="shared" ref="S60:S61" si="62">DEC2HEX(R60)</f>
         <v>34F240</v>
       </c>
-      <c r="T60" s="69">
+      <c r="T60" s="61">
         <f>T58+O58</f>
         <v>281984</v>
       </c>
@@ -9153,7 +9153,7 @@
         <f t="shared" si="60"/>
         <v>73728</v>
       </c>
-      <c r="P61" s="63">
+      <c r="P61" s="55">
         <f>R66</f>
         <v>3556416</v>
       </c>
@@ -9161,7 +9161,7 @@
         <f t="shared" si="61"/>
         <v>364440</v>
       </c>
-      <c r="R61" s="69">
+      <c r="R61" s="61">
         <f>R60+K60</f>
         <v>3513152</v>
       </c>
@@ -9169,7 +9169,7 @@
         <f t="shared" si="62"/>
         <v>359B40</v>
       </c>
-      <c r="T61" s="69">
+      <c r="T61" s="61">
         <f>T60+O60</f>
         <v>290176</v>
       </c>
@@ -9222,11 +9222,11 @@
       <c r="M62" s="36"/>
       <c r="N62" s="36"/>
       <c r="O62" s="37"/>
-      <c r="P62" s="64"/>
+      <c r="P62" s="56"/>
       <c r="Q62" s="20"/>
-      <c r="R62" s="70"/>
+      <c r="R62" s="62"/>
       <c r="S62" s="20"/>
-      <c r="T62" s="70"/>
+      <c r="T62" s="62"/>
       <c r="U62" s="20"/>
       <c r="V62" s="47"/>
       <c r="W62" s="47"/>
@@ -9257,11 +9257,11 @@
       <c r="M63" s="36"/>
       <c r="N63" s="36"/>
       <c r="O63" s="37"/>
-      <c r="P63" s="64"/>
+      <c r="P63" s="56"/>
       <c r="Q63" s="20"/>
-      <c r="R63" s="70"/>
+      <c r="R63" s="62"/>
       <c r="S63" s="20"/>
-      <c r="T63" s="70"/>
+      <c r="T63" s="62"/>
       <c r="U63" s="20"/>
       <c r="V63" s="47"/>
       <c r="W63" s="47"/>
@@ -9296,11 +9296,11 @@
       <c r="M64" s="32"/>
       <c r="N64" s="32"/>
       <c r="O64" s="33"/>
-      <c r="P64" s="62"/>
+      <c r="P64" s="54"/>
       <c r="Q64" s="16"/>
-      <c r="R64" s="68"/>
+      <c r="R64" s="60"/>
       <c r="S64" s="16"/>
-      <c r="T64" s="68"/>
+      <c r="T64" s="60"/>
       <c r="U64" s="16"/>
       <c r="V64" s="43"/>
       <c r="W64" s="43"/>
@@ -9331,11 +9331,11 @@
       <c r="M65" s="36"/>
       <c r="N65" s="36"/>
       <c r="O65" s="37"/>
-      <c r="P65" s="64"/>
+      <c r="P65" s="56"/>
       <c r="Q65" s="20"/>
-      <c r="R65" s="70"/>
+      <c r="R65" s="62"/>
       <c r="S65" s="20"/>
-      <c r="T65" s="70"/>
+      <c r="T65" s="62"/>
       <c r="U65" s="20"/>
       <c r="V65" s="47"/>
       <c r="W65" s="47"/>
@@ -9397,7 +9397,7 @@
         <f>_xlfn.CEILING.MATH(D66^2*E66/2)*F66</f>
         <v>256000</v>
       </c>
-      <c r="P66" s="63">
+      <c r="P66" s="55">
         <f>R68</f>
         <v>3725416</v>
       </c>
@@ -9405,7 +9405,7 @@
         <f>DEC2HEX(P66)</f>
         <v>38D868</v>
       </c>
-      <c r="R66" s="69">
+      <c r="R66" s="61">
         <f>R61+K61</f>
         <v>3556416</v>
       </c>
@@ -9413,7 +9413,7 @@
         <f>DEC2HEX(R66)</f>
         <v>364440</v>
       </c>
-      <c r="T66" s="69">
+      <c r="T66" s="61">
         <f>T61+O61</f>
         <v>363904</v>
       </c>
@@ -9466,11 +9466,11 @@
       <c r="M67" s="36"/>
       <c r="N67" s="36"/>
       <c r="O67" s="37"/>
-      <c r="P67" s="64"/>
+      <c r="P67" s="56"/>
       <c r="Q67" s="20"/>
-      <c r="R67" s="70"/>
+      <c r="R67" s="62"/>
       <c r="S67" s="20"/>
-      <c r="T67" s="70"/>
+      <c r="T67" s="62"/>
       <c r="U67" s="20"/>
       <c r="V67" s="47"/>
       <c r="W67" s="47"/>
@@ -9519,7 +9519,7 @@
       <c r="M68" s="38"/>
       <c r="N68" s="38"/>
       <c r="O68" s="39"/>
-      <c r="P68" s="65">
+      <c r="P68" s="57">
         <f>R69</f>
         <v>3726416</v>
       </c>
@@ -9527,7 +9527,7 @@
         <f>DEC2HEX(P68)</f>
         <v>38DC50</v>
       </c>
-      <c r="R68" s="71">
+      <c r="R68" s="63">
         <f>R66+K66</f>
         <v>3725416</v>
       </c>
@@ -9535,7 +9535,7 @@
         <f>DEC2HEX(R68)</f>
         <v>38D868</v>
       </c>
-      <c r="T68" s="71"/>
+      <c r="T68" s="63"/>
       <c r="U68" s="22" t="s">
         <v>150</v>
       </c>
@@ -9584,14 +9584,14 @@
       <c r="M69" s="32"/>
       <c r="N69" s="32"/>
       <c r="O69" s="33"/>
-      <c r="P69" s="62"/>
+      <c r="P69" s="54"/>
       <c r="Q69" s="16"/>
-      <c r="R69" s="68">
+      <c r="R69" s="60">
         <f>R68+L68</f>
         <v>3726416</v>
       </c>
       <c r="S69" s="16"/>
-      <c r="T69" s="68"/>
+      <c r="T69" s="60"/>
       <c r="U69" s="16"/>
       <c r="V69" s="43"/>
       <c r="W69" s="43"/>
@@ -9630,11 +9630,11 @@
         <f>SUM(O4:O69)</f>
         <v>615808</v>
       </c>
-      <c r="P70" s="66"/>
+      <c r="P70" s="58"/>
       <c r="Q70" s="24"/>
-      <c r="R70" s="72"/>
+      <c r="R70" s="64"/>
       <c r="S70" s="24"/>
-      <c r="T70" s="72"/>
+      <c r="T70" s="64"/>
       <c r="U70" s="24"/>
       <c r="V70" s="14"/>
       <c r="W70" s="14"/>
@@ -9676,11 +9676,11 @@
         <v>1235496</v>
       </c>
       <c r="O71" s="31"/>
-      <c r="P71" s="66"/>
+      <c r="P71" s="58"/>
       <c r="Q71" s="24"/>
-      <c r="R71" s="72"/>
+      <c r="R71" s="64"/>
       <c r="S71" s="24"/>
-      <c r="T71" s="72"/>
+      <c r="T71" s="64"/>
       <c r="U71" s="24"/>
       <c r="V71" s="14"/>
       <c r="W71" s="14"/>

</xml_diff>

<commit_message>
Move dma enable logic from csb to engine, fix memory access time estimation
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A01F76A-E7AE-4EAF-863A-EE77608D3C57}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933EB47A-C77E-4367-9A6B-ACE2E37896DE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7860" activeTab="1" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
   <sheets>
     <sheet name="SqueezeNet @ 100MHz + 312.5MHz" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -5168,8 +5169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80B23C6-EAEB-43B1-B045-456C36085CFA}">
   <dimension ref="A1:AC71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AA6" sqref="AA6:AA71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5370,8 +5371,8 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
       <c r="AA3" s="3">
-        <f>0.0000032*K3</f>
-        <v>0.4816896</v>
+        <f>K3/64*0.97</f>
+        <v>2281.44</v>
       </c>
       <c r="AB3" s="3"/>
       <c r="AC3" s="26" t="s">
@@ -5468,8 +5469,8 @@
         <v>1</v>
       </c>
       <c r="AA4" s="4">
-        <f>0.0000032*M4+0.0000064*K4</f>
-        <v>5.0522111999999995</v>
+        <f>K4/64*0.97</f>
+        <v>11951.369999999999</v>
       </c>
       <c r="AB4" s="4">
         <f>L4*Y4*Z4</f>
@@ -5586,8 +5587,8 @@
         <v>1</v>
       </c>
       <c r="AA6" s="6">
-        <f>0.0000064*K6</f>
-        <v>1.2390399999999999</v>
+        <f>K6/64*0.97</f>
+        <v>2934.25</v>
       </c>
       <c r="AB6" s="6">
         <f>L6*Y6*Z6</f>
@@ -5686,8 +5687,8 @@
         <v>1</v>
       </c>
       <c r="AA7" s="4">
-        <f>0.0000032*M7+0.0000064*K7</f>
-        <v>0.3130368</v>
+        <f>K7/64*0.97</f>
+        <v>733.5625</v>
       </c>
       <c r="AB7" s="4">
         <f>L7*Y7*Z7</f>
@@ -5821,8 +5822,8 @@
         <v>0</v>
       </c>
       <c r="AA9" s="4">
-        <f>0.0000032*M9+0.0000064*K9</f>
-        <v>1.2423168</v>
+        <f t="shared" ref="AA9:AA10" si="8">K9/64*0.97</f>
+        <v>2934.25</v>
       </c>
       <c r="AB9" s="4">
         <f>L9*Y9*Z9</f>
@@ -5921,8 +5922,8 @@
         <v>1</v>
       </c>
       <c r="AA10" s="4">
-        <f>0.0000032*M10+0.0000064*K10</f>
-        <v>1.2685312</v>
+        <f t="shared" si="8"/>
+        <v>2934.25</v>
       </c>
       <c r="AB10" s="4">
         <f>L10*Y10*Z10</f>
@@ -6130,8 +6131,8 @@
         <v>1</v>
       </c>
       <c r="AA14" s="4">
-        <f>0.0000032*M14+0.0000064*K14</f>
-        <v>0.31631359999999997</v>
+        <f>K14/64*0.97</f>
+        <v>733.5625</v>
       </c>
       <c r="AB14" s="4">
         <f>L14*Y14*Z14</f>
@@ -6206,23 +6207,23 @@
         <v>55</v>
       </c>
       <c r="K16" s="34">
-        <f t="shared" ref="K16:K17" si="8">J16^2*F16</f>
+        <f t="shared" ref="K16:K17" si="9">J16^2*F16</f>
         <v>193600</v>
       </c>
       <c r="L16" s="34">
-        <f t="shared" ref="L16:L17" si="9">J16^2*E16</f>
+        <f t="shared" ref="L16:L17" si="10">J16^2*E16</f>
         <v>48400</v>
       </c>
       <c r="M16" s="34">
-        <f t="shared" ref="M16:M17" si="10">D16^2*E16*F16</f>
+        <f t="shared" ref="M16:M17" si="11">D16^2*E16*F16</f>
         <v>1024</v>
       </c>
       <c r="N16" s="34">
-        <f t="shared" ref="N16:N17" si="11">F16</f>
+        <f t="shared" ref="N16:N17" si="12">F16</f>
         <v>64</v>
       </c>
       <c r="O16" s="35">
-        <f t="shared" ref="O16:O17" si="12">_xlfn.CEILING.MATH(D16^2*E16/2)*F16</f>
+        <f t="shared" ref="O16:O17" si="13">_xlfn.CEILING.MATH(D16^2*E16/2)*F16</f>
         <v>512</v>
       </c>
       <c r="P16" s="55">
@@ -6230,7 +6231,7 @@
         <v>2465632</v>
       </c>
       <c r="Q16" s="18" t="str">
-        <f t="shared" ref="Q16:Q17" si="13">DEC2HEX(P16)</f>
+        <f t="shared" ref="Q16:Q17" si="14">DEC2HEX(P16)</f>
         <v>259F60</v>
       </c>
       <c r="R16" s="61">
@@ -6238,7 +6239,7 @@
         <v>2272032</v>
       </c>
       <c r="S16" s="18" t="str">
-        <f t="shared" ref="S16:S17" si="14">DEC2HEX(R16)</f>
+        <f t="shared" ref="S16:S17" si="15">DEC2HEX(R16)</f>
         <v>22AB20</v>
       </c>
       <c r="T16" s="61">
@@ -6246,7 +6247,7 @@
         <v>11648</v>
       </c>
       <c r="U16" s="18" t="str">
-        <f t="shared" ref="U16:U17" si="15">DEC2HEX(T16)</f>
+        <f t="shared" ref="U16:U17" si="16">DEC2HEX(T16)</f>
         <v>2D80</v>
       </c>
       <c r="V16" s="45" t="s">
@@ -6265,8 +6266,8 @@
         <v>0</v>
       </c>
       <c r="AA16" s="4">
-        <f>0.0000032*M16+0.0000064*K16</f>
-        <v>1.2423168</v>
+        <f t="shared" ref="AA16:AA17" si="17">K16/64*0.97</f>
+        <v>2934.25</v>
       </c>
       <c r="AB16" s="4">
         <f>L16*Y16*Z16</f>
@@ -6306,23 +6307,23 @@
         <v>55</v>
       </c>
       <c r="K17" s="34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>193600</v>
       </c>
       <c r="L17" s="34">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>48400</v>
       </c>
       <c r="M17" s="34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9216</v>
       </c>
       <c r="N17" s="34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>64</v>
       </c>
       <c r="O17" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4608</v>
       </c>
       <c r="P17" s="55">
@@ -6330,7 +6331,7 @@
         <v>2659232</v>
       </c>
       <c r="Q17" s="18" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2893A0</v>
       </c>
       <c r="R17" s="61">
@@ -6338,7 +6339,7 @@
         <v>2465632</v>
       </c>
       <c r="S17" s="18" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>259F60</v>
       </c>
       <c r="T17" s="61">
@@ -6346,7 +6347,7 @@
         <v>12160</v>
       </c>
       <c r="U17" s="18" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2F80</v>
       </c>
       <c r="V17" s="45" t="s">
@@ -6365,8 +6366,8 @@
         <v>1</v>
       </c>
       <c r="AA17" s="4">
-        <f>0.0000032*M17+0.0000064*K17</f>
-        <v>1.2685312</v>
+        <f t="shared" si="17"/>
+        <v>2934.25</v>
       </c>
       <c r="AB17" s="4">
         <f>L17*Y17*Z17</f>
@@ -6557,8 +6558,8 @@
         <v>1</v>
       </c>
       <c r="AA21" s="6">
-        <f>0.0000064*K21</f>
-        <v>0.59719679999999997</v>
+        <f>K21/64*0.97</f>
+        <v>1414.26</v>
       </c>
       <c r="AB21" s="6">
         <f>L21*Y21*Z21</f>
@@ -6657,8 +6658,8 @@
         <v>1</v>
       </c>
       <c r="AA22" s="4">
-        <f>0.0000032*M22+0.0000064*K22</f>
-        <v>0.16240640000000001</v>
+        <f>K22/64*0.97</f>
+        <v>353.565</v>
       </c>
       <c r="AB22" s="4">
         <f>L22*Y22*Z22</f>
@@ -6733,23 +6734,23 @@
         <v>27</v>
       </c>
       <c r="K24" s="34">
-        <f t="shared" ref="K24:K25" si="16">J24^2*F24</f>
+        <f t="shared" ref="K24:K25" si="18">J24^2*F24</f>
         <v>93312</v>
       </c>
       <c r="L24" s="34">
-        <f t="shared" ref="L24:L25" si="17">J24^2*E24</f>
+        <f t="shared" ref="L24:L25" si="19">J24^2*E24</f>
         <v>23328</v>
       </c>
       <c r="M24" s="34">
-        <f t="shared" ref="M24:M25" si="18">D24^2*E24*F24</f>
+        <f t="shared" ref="M24:M25" si="20">D24^2*E24*F24</f>
         <v>4096</v>
       </c>
       <c r="N24" s="34">
-        <f t="shared" ref="N24:N25" si="19">F24</f>
+        <f t="shared" ref="N24:N25" si="21">F24</f>
         <v>128</v>
       </c>
       <c r="O24" s="35">
-        <f t="shared" ref="O24:O25" si="20">_xlfn.CEILING.MATH(D24^2*E24/2)*F24</f>
+        <f t="shared" ref="O24:O25" si="22">_xlfn.CEILING.MATH(D24^2*E24/2)*F24</f>
         <v>2048</v>
       </c>
       <c r="P24" s="55">
@@ -6757,7 +6758,7 @@
         <v>2869184</v>
       </c>
       <c r="Q24" s="18" t="str">
-        <f t="shared" ref="Q24:Q25" si="21">DEC2HEX(P24)</f>
+        <f t="shared" ref="Q24:Q25" si="23">DEC2HEX(P24)</f>
         <v>2BC7C0</v>
       </c>
       <c r="R24" s="61">
@@ -6765,7 +6766,7 @@
         <v>2775872</v>
       </c>
       <c r="S24" s="18" t="str">
-        <f t="shared" ref="S24:S25" si="22">DEC2HEX(R24)</f>
+        <f t="shared" ref="S24:S25" si="24">DEC2HEX(R24)</f>
         <v>2A5B40</v>
       </c>
       <c r="T24" s="61">
@@ -6773,7 +6774,7 @@
         <v>18816</v>
       </c>
       <c r="U24" s="18" t="str">
-        <f t="shared" ref="U24:U25" si="23">DEC2HEX(T24)</f>
+        <f t="shared" ref="U24:U25" si="25">DEC2HEX(T24)</f>
         <v>4980</v>
       </c>
       <c r="V24" s="45" t="s">
@@ -6792,8 +6793,8 @@
         <v>0</v>
       </c>
       <c r="AA24" s="4">
-        <f>0.0000032*M24+0.0000064*K24</f>
-        <v>0.61030399999999996</v>
+        <f t="shared" ref="AA24:AA25" si="26">K24/64*0.97</f>
+        <v>1414.26</v>
       </c>
       <c r="AB24" s="4">
         <f>L24*Y24*Z24</f>
@@ -6833,23 +6834,23 @@
         <v>27</v>
       </c>
       <c r="K25" s="34">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>93312</v>
       </c>
       <c r="L25" s="34">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>23328</v>
       </c>
       <c r="M25" s="34">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>36864</v>
       </c>
       <c r="N25" s="34">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>128</v>
       </c>
       <c r="O25" s="35">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>18432</v>
       </c>
       <c r="P25" s="55">
@@ -6857,7 +6858,7 @@
         <v>2962496</v>
       </c>
       <c r="Q25" s="18" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>2D3440</v>
       </c>
       <c r="R25" s="61">
@@ -6865,7 +6866,7 @@
         <v>2869184</v>
       </c>
       <c r="S25" s="18" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>2BC7C0</v>
       </c>
       <c r="T25" s="61">
@@ -6873,7 +6874,7 @@
         <v>20864</v>
       </c>
       <c r="U25" s="18" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>5180</v>
       </c>
       <c r="V25" s="45" t="s">
@@ -6892,8 +6893,8 @@
         <v>1</v>
       </c>
       <c r="AA25" s="4">
-        <f>0.0000032*M25+0.0000064*K25</f>
-        <v>0.71516159999999995</v>
+        <f t="shared" si="26"/>
+        <v>1414.26</v>
       </c>
       <c r="AB25" s="4">
         <f>L25*Y25*Z25</f>
@@ -7101,8 +7102,8 @@
         <v>1</v>
       </c>
       <c r="AA29" s="4">
-        <f>0.0000032*M29+0.0000064*K29</f>
-        <v>0.17551359999999999</v>
+        <f>K29/64*0.97</f>
+        <v>353.565</v>
       </c>
       <c r="AB29" s="4">
         <f>L29*Y29*Z29</f>
@@ -7177,23 +7178,23 @@
         <v>27</v>
       </c>
       <c r="K31" s="34">
-        <f t="shared" ref="K31:K32" si="24">J31^2*F31</f>
+        <f t="shared" ref="K31:K32" si="27">J31^2*F31</f>
         <v>93312</v>
       </c>
       <c r="L31" s="34">
-        <f t="shared" ref="L31:L32" si="25">J31^2*E31</f>
+        <f t="shared" ref="L31:L32" si="28">J31^2*E31</f>
         <v>23328</v>
       </c>
       <c r="M31" s="34">
-        <f t="shared" ref="M31:M32" si="26">D31^2*E31*F31</f>
+        <f t="shared" ref="M31:M32" si="29">D31^2*E31*F31</f>
         <v>4096</v>
       </c>
       <c r="N31" s="34">
-        <f t="shared" ref="N31:N32" si="27">F31</f>
+        <f t="shared" ref="N31:N32" si="30">F31</f>
         <v>128</v>
       </c>
       <c r="O31" s="35">
-        <f t="shared" ref="O31:O32" si="28">_xlfn.CEILING.MATH(D31^2*E31/2)*F31</f>
+        <f t="shared" ref="O31:O32" si="31">_xlfn.CEILING.MATH(D31^2*E31/2)*F31</f>
         <v>2048</v>
       </c>
       <c r="P31" s="55">
@@ -7201,7 +7202,7 @@
         <v>3079136</v>
       </c>
       <c r="Q31" s="18" t="str">
-        <f t="shared" ref="Q31:Q32" si="29">DEC2HEX(P31)</f>
+        <f t="shared" ref="Q31:Q32" si="32">DEC2HEX(P31)</f>
         <v>2EFBE0</v>
       </c>
       <c r="R31" s="61">
@@ -7209,7 +7210,7 @@
         <v>2985824</v>
       </c>
       <c r="S31" s="18" t="str">
-        <f t="shared" ref="S31:S32" si="30">DEC2HEX(R31)</f>
+        <f t="shared" ref="S31:S32" si="33">DEC2HEX(R31)</f>
         <v>2D8F60</v>
       </c>
       <c r="T31" s="61">
@@ -7217,7 +7218,7 @@
         <v>43392</v>
       </c>
       <c r="U31" s="18" t="str">
-        <f t="shared" ref="U31:U32" si="31">DEC2HEX(T31)</f>
+        <f t="shared" ref="U31:U32" si="34">DEC2HEX(T31)</f>
         <v>A980</v>
       </c>
       <c r="V31" s="45" t="s">
@@ -7236,8 +7237,8 @@
         <v>0</v>
       </c>
       <c r="AA31" s="4">
-        <f>0.0000032*M31+0.0000064*K31</f>
-        <v>0.61030399999999996</v>
+        <f t="shared" ref="AA31:AA32" si="35">K31/64*0.97</f>
+        <v>1414.26</v>
       </c>
       <c r="AB31" s="4">
         <f>L31*Y31*Z31</f>
@@ -7277,23 +7278,23 @@
         <v>27</v>
       </c>
       <c r="K32" s="34">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>93312</v>
       </c>
       <c r="L32" s="34">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>23328</v>
       </c>
       <c r="M32" s="34">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>36864</v>
       </c>
       <c r="N32" s="34">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>128</v>
       </c>
       <c r="O32" s="35">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>18432</v>
       </c>
       <c r="P32" s="55">
@@ -7301,7 +7302,7 @@
         <v>3172448</v>
       </c>
       <c r="Q32" s="18" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>306860</v>
       </c>
       <c r="R32" s="61">
@@ -7309,7 +7310,7 @@
         <v>3079136</v>
       </c>
       <c r="S32" s="18" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>2EFBE0</v>
       </c>
       <c r="T32" s="61">
@@ -7317,7 +7318,7 @@
         <v>45440</v>
       </c>
       <c r="U32" s="18" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>B180</v>
       </c>
       <c r="V32" s="45" t="s">
@@ -7336,8 +7337,8 @@
         <v>1</v>
       </c>
       <c r="AA32" s="4">
-        <f>0.0000032*M32+0.0000064*K32</f>
-        <v>0.71516159999999995</v>
+        <f t="shared" si="35"/>
+        <v>1414.26</v>
       </c>
       <c r="AB32" s="4">
         <f>L32*Y32*Z32</f>
@@ -7526,8 +7527,8 @@
         <v>1</v>
       </c>
       <c r="AA36" s="6">
-        <f>0.0000064*K36</f>
-        <v>0.27688960000000001</v>
+        <f>K36/64*0.97</f>
+        <v>655.72</v>
       </c>
       <c r="AB36" s="6">
         <f>L36*Y36*Z36</f>
@@ -7626,8 +7627,8 @@
         <v>1</v>
       </c>
       <c r="AA37" s="4">
-        <f>0.0000032*M37+0.0000064*K37</f>
-        <v>9.1238399999999997E-2</v>
+        <f>K37/64*0.97</f>
+        <v>122.94749999999999</v>
       </c>
       <c r="AB37" s="4">
         <f>L37*Y37*Z37</f>
@@ -7702,23 +7703,23 @@
         <v>13</v>
       </c>
       <c r="K39" s="34">
-        <f t="shared" ref="K39:K40" si="32">J39^2*F39</f>
+        <f t="shared" ref="K39:K40" si="36">J39^2*F39</f>
         <v>32448</v>
       </c>
       <c r="L39" s="34">
-        <f t="shared" ref="L39:L40" si="33">J39^2*E39</f>
+        <f t="shared" ref="L39:L40" si="37">J39^2*E39</f>
         <v>8112</v>
       </c>
       <c r="M39" s="34">
-        <f t="shared" ref="M39:M40" si="34">D39^2*E39*F39</f>
+        <f t="shared" ref="M39:M40" si="38">D39^2*E39*F39</f>
         <v>9216</v>
       </c>
       <c r="N39" s="34">
-        <f t="shared" ref="N39:N40" si="35">F39</f>
+        <f t="shared" ref="N39:N40" si="39">F39</f>
         <v>192</v>
       </c>
       <c r="O39" s="35">
-        <f t="shared" ref="O39:O40" si="36">_xlfn.CEILING.MATH(D39^2*E39/2)*F39</f>
+        <f t="shared" ref="O39:O40" si="40">_xlfn.CEILING.MATH(D39^2*E39/2)*F39</f>
         <v>4608</v>
       </c>
       <c r="P39" s="55">
@@ -7726,7 +7727,7 @@
         <v>3256272</v>
       </c>
       <c r="Q39" s="18" t="str">
-        <f t="shared" ref="Q39:Q40" si="37">DEC2HEX(P39)</f>
+        <f t="shared" ref="Q39:Q40" si="41">DEC2HEX(P39)</f>
         <v>31AFD0</v>
       </c>
       <c r="R39" s="61">
@@ -7734,7 +7735,7 @@
         <v>3223824</v>
       </c>
       <c r="S39" s="18" t="str">
-        <f t="shared" ref="S39:S40" si="38">DEC2HEX(R39)</f>
+        <f t="shared" ref="S39:S40" si="42">DEC2HEX(R39)</f>
         <v>313110</v>
       </c>
       <c r="T39" s="61">
@@ -7742,7 +7743,7 @@
         <v>70016</v>
       </c>
       <c r="U39" s="18" t="str">
-        <f t="shared" ref="U39:U40" si="39">DEC2HEX(T39)</f>
+        <f t="shared" ref="U39:U40" si="43">DEC2HEX(T39)</f>
         <v>11180</v>
       </c>
       <c r="V39" s="45" t="s">
@@ -7761,8 +7762,8 @@
         <v>0</v>
       </c>
       <c r="AA39" s="4">
-        <f>0.0000032*M39+0.0000064*K39</f>
-        <v>0.23715839999999999</v>
+        <f t="shared" ref="AA39:AA40" si="44">K39/64*0.97</f>
+        <v>491.78999999999996</v>
       </c>
       <c r="AB39" s="4">
         <f>L39*Y39*Z39</f>
@@ -7802,23 +7803,23 @@
         <v>13</v>
       </c>
       <c r="K40" s="34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>32448</v>
       </c>
       <c r="L40" s="34">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>8112</v>
       </c>
       <c r="M40" s="34">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>82944</v>
       </c>
       <c r="N40" s="34">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>192</v>
       </c>
       <c r="O40" s="35">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>41472</v>
       </c>
       <c r="P40" s="55">
@@ -7826,7 +7827,7 @@
         <v>3288720</v>
       </c>
       <c r="Q40" s="18" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>322E90</v>
       </c>
       <c r="R40" s="61">
@@ -7834,7 +7835,7 @@
         <v>3256272</v>
       </c>
       <c r="S40" s="18" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>31AFD0</v>
       </c>
       <c r="T40" s="61">
@@ -7842,7 +7843,7 @@
         <v>74624</v>
       </c>
       <c r="U40" s="18" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>12380</v>
       </c>
       <c r="V40" s="45" t="s">
@@ -7861,8 +7862,8 @@
         <v>1</v>
       </c>
       <c r="AA40" s="4">
-        <f>0.0000032*M40+0.0000064*K40</f>
-        <v>0.47308800000000001</v>
+        <f t="shared" si="44"/>
+        <v>491.78999999999996</v>
       </c>
       <c r="AB40" s="4">
         <f>L40*Y40*Z40</f>
@@ -8070,8 +8071,8 @@
         <v>1</v>
       </c>
       <c r="AA44" s="4">
-        <f>0.0000032*M44+0.0000064*K44</f>
-        <v>0.1108992</v>
+        <f>K44/64*0.97</f>
+        <v>122.94749999999999</v>
       </c>
       <c r="AB44" s="4">
         <f>L44*Y44*Z44</f>
@@ -8146,23 +8147,23 @@
         <v>13</v>
       </c>
       <c r="K46" s="34">
-        <f t="shared" ref="K46:K47" si="40">J46^2*F46</f>
+        <f t="shared" ref="K46:K47" si="45">J46^2*F46</f>
         <v>32448</v>
       </c>
       <c r="L46" s="34">
-        <f t="shared" ref="L46:L47" si="41">J46^2*E46</f>
+        <f t="shared" ref="L46:L47" si="46">J46^2*E46</f>
         <v>8112</v>
       </c>
       <c r="M46" s="34">
-        <f t="shared" ref="M46:M47" si="42">D46^2*E46*F46</f>
+        <f t="shared" ref="M46:M47" si="47">D46^2*E46*F46</f>
         <v>9216</v>
       </c>
       <c r="N46" s="34">
-        <f t="shared" ref="N46:N47" si="43">F46</f>
+        <f t="shared" ref="N46:N47" si="48">F46</f>
         <v>192</v>
       </c>
       <c r="O46" s="35">
-        <f t="shared" ref="O46:O47" si="44">_xlfn.CEILING.MATH(D46^2*E46/2)*F46</f>
+        <f t="shared" ref="O46:O47" si="49">_xlfn.CEILING.MATH(D46^2*E46/2)*F46</f>
         <v>4608</v>
       </c>
       <c r="P46" s="55">
@@ -8170,7 +8171,7 @@
         <v>3329280</v>
       </c>
       <c r="Q46" s="18" t="str">
-        <f t="shared" ref="Q46:Q47" si="45">DEC2HEX(P46)</f>
+        <f t="shared" ref="Q46:Q47" si="50">DEC2HEX(P46)</f>
         <v>32CD00</v>
       </c>
       <c r="R46" s="61">
@@ -8178,7 +8179,7 @@
         <v>3296832</v>
       </c>
       <c r="S46" s="18" t="str">
-        <f t="shared" ref="S46:S47" si="46">DEC2HEX(R46)</f>
+        <f t="shared" ref="S46:S47" si="51">DEC2HEX(R46)</f>
         <v>324E40</v>
       </c>
       <c r="T46" s="61">
@@ -8186,7 +8187,7 @@
         <v>125312</v>
       </c>
       <c r="U46" s="18" t="str">
-        <f t="shared" ref="U46:U47" si="47">DEC2HEX(T46)</f>
+        <f t="shared" ref="U46:U47" si="52">DEC2HEX(T46)</f>
         <v>1E980</v>
       </c>
       <c r="V46" s="45" t="s">
@@ -8205,8 +8206,8 @@
         <v>0</v>
       </c>
       <c r="AA46" s="4">
-        <f>0.0000032*M46+0.0000064*K46</f>
-        <v>0.23715839999999999</v>
+        <f t="shared" ref="AA46:AA47" si="53">K46/64*0.97</f>
+        <v>491.78999999999996</v>
       </c>
       <c r="AB46" s="4">
         <f>L46*Y46*Z46</f>
@@ -8246,23 +8247,23 @@
         <v>13</v>
       </c>
       <c r="K47" s="34">
-        <f t="shared" si="40"/>
+        <f t="shared" si="45"/>
         <v>32448</v>
       </c>
       <c r="L47" s="34">
-        <f t="shared" si="41"/>
+        <f t="shared" si="46"/>
         <v>8112</v>
       </c>
       <c r="M47" s="34">
-        <f t="shared" si="42"/>
+        <f t="shared" si="47"/>
         <v>82944</v>
       </c>
       <c r="N47" s="34">
-        <f t="shared" si="43"/>
+        <f t="shared" si="48"/>
         <v>192</v>
       </c>
       <c r="O47" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="49"/>
         <v>41472</v>
       </c>
       <c r="P47" s="55">
@@ -8270,7 +8271,7 @@
         <v>3361728</v>
       </c>
       <c r="Q47" s="18" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="50"/>
         <v>334BC0</v>
       </c>
       <c r="R47" s="61">
@@ -8278,7 +8279,7 @@
         <v>3329280</v>
       </c>
       <c r="S47" s="18" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="51"/>
         <v>32CD00</v>
       </c>
       <c r="T47" s="61">
@@ -8286,7 +8287,7 @@
         <v>129920</v>
       </c>
       <c r="U47" s="18" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="52"/>
         <v>1FB80</v>
       </c>
       <c r="V47" s="45" t="s">
@@ -8305,8 +8306,8 @@
         <v>1</v>
       </c>
       <c r="AA47" s="4">
-        <f>0.0000032*M47+0.0000064*K47</f>
-        <v>0.47308800000000001</v>
+        <f t="shared" si="53"/>
+        <v>491.78999999999996</v>
       </c>
       <c r="AB47" s="4">
         <f>L47*Y47*Z47</f>
@@ -8514,8 +8515,8 @@
         <v>1</v>
       </c>
       <c r="AA51" s="4">
-        <f>0.0000032*M51+0.0000064*K51</f>
-        <v>0.14786559999999999</v>
+        <f>K51/64*0.97</f>
+        <v>163.93</v>
       </c>
       <c r="AB51" s="4">
         <f>L51*Y51*Z51</f>
@@ -8590,23 +8591,23 @@
         <v>13</v>
       </c>
       <c r="K53" s="34">
-        <f t="shared" ref="K53:K54" si="48">J53^2*F53</f>
+        <f t="shared" ref="K53:K54" si="54">J53^2*F53</f>
         <v>43264</v>
       </c>
       <c r="L53" s="34">
-        <f t="shared" ref="L53:L54" si="49">J53^2*E53</f>
+        <f t="shared" ref="L53:L54" si="55">J53^2*E53</f>
         <v>10816</v>
       </c>
       <c r="M53" s="34">
-        <f t="shared" ref="M53:M54" si="50">D53^2*E53*F53</f>
+        <f t="shared" ref="M53:M54" si="56">D53^2*E53*F53</f>
         <v>16384</v>
       </c>
       <c r="N53" s="34">
-        <f t="shared" ref="N53:N54" si="51">F53</f>
+        <f t="shared" ref="N53:N54" si="57">F53</f>
         <v>256</v>
       </c>
       <c r="O53" s="35">
-        <f t="shared" ref="O53:O54" si="52">_xlfn.CEILING.MATH(D53^2*E53/2)*F53</f>
+        <f t="shared" ref="O53:O54" si="58">_xlfn.CEILING.MATH(D53^2*E53/2)*F53</f>
         <v>8192</v>
       </c>
       <c r="P53" s="55">
@@ -8614,7 +8615,7 @@
         <v>3415808</v>
       </c>
       <c r="Q53" s="18" t="str">
-        <f t="shared" ref="Q53:Q54" si="53">DEC2HEX(P53)</f>
+        <f t="shared" ref="Q53:Q54" si="59">DEC2HEX(P53)</f>
         <v>341F00</v>
       </c>
       <c r="R53" s="61">
@@ -8622,7 +8623,7 @@
         <v>3372544</v>
       </c>
       <c r="S53" s="18" t="str">
-        <f t="shared" ref="S53:S54" si="54">DEC2HEX(R53)</f>
+        <f t="shared" ref="S53:S54" si="60">DEC2HEX(R53)</f>
         <v>337600</v>
       </c>
       <c r="T53" s="61">
@@ -8630,7 +8631,7 @@
         <v>183680</v>
       </c>
       <c r="U53" s="18" t="str">
-        <f t="shared" ref="U53:U54" si="55">DEC2HEX(T53)</f>
+        <f t="shared" ref="U53:U54" si="61">DEC2HEX(T53)</f>
         <v>2CD80</v>
       </c>
       <c r="V53" s="45" t="s">
@@ -8649,8 +8650,8 @@
         <v>0</v>
       </c>
       <c r="AA53" s="4">
-        <f>0.0000032*M53+0.0000064*K53</f>
-        <v>0.32931840000000001</v>
+        <f t="shared" ref="AA53:AA54" si="62">K53/64*0.97</f>
+        <v>655.72</v>
       </c>
       <c r="AB53" s="4">
         <f>L53*Y53*Z53</f>
@@ -8690,23 +8691,23 @@
         <v>13</v>
       </c>
       <c r="K54" s="34">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>43264</v>
       </c>
       <c r="L54" s="34">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>10816</v>
       </c>
       <c r="M54" s="34">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>147456</v>
       </c>
       <c r="N54" s="34">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>256</v>
       </c>
       <c r="O54" s="35">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>73728</v>
       </c>
       <c r="P54" s="55">
@@ -8714,7 +8715,7 @@
         <v>3459072</v>
       </c>
       <c r="Q54" s="18" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="59"/>
         <v>34C800</v>
       </c>
       <c r="R54" s="61">
@@ -8722,7 +8723,7 @@
         <v>3415808</v>
       </c>
       <c r="S54" s="18" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="60"/>
         <v>341F00</v>
       </c>
       <c r="T54" s="61">
@@ -8730,7 +8731,7 @@
         <v>191872</v>
       </c>
       <c r="U54" s="18" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="61"/>
         <v>2ED80</v>
       </c>
       <c r="V54" s="45" t="s">
@@ -8749,8 +8750,8 @@
         <v>1</v>
       </c>
       <c r="AA54" s="4">
-        <f>0.0000032*M54+0.0000064*K54</f>
-        <v>0.74874879999999999</v>
+        <f t="shared" si="62"/>
+        <v>655.72</v>
       </c>
       <c r="AB54" s="4">
         <f>L54*Y54*Z54</f>
@@ -8958,8 +8959,8 @@
         <v>1</v>
       </c>
       <c r="AA58" s="4">
-        <f>0.0000032*M58+0.0000064*K58</f>
-        <v>0.17408000000000001</v>
+        <f>K58/64*0.97</f>
+        <v>163.93</v>
       </c>
       <c r="AB58" s="4">
         <f>L58*Y58*Z58</f>
@@ -9034,23 +9035,23 @@
         <v>13</v>
       </c>
       <c r="K60" s="34">
-        <f t="shared" ref="K60:K61" si="56">J60^2*F60</f>
+        <f t="shared" ref="K60:K61" si="63">J60^2*F60</f>
         <v>43264</v>
       </c>
       <c r="L60" s="34">
-        <f t="shared" ref="L60:L61" si="57">J60^2*E60</f>
+        <f t="shared" ref="L60:L61" si="64">J60^2*E60</f>
         <v>10816</v>
       </c>
       <c r="M60" s="34">
-        <f t="shared" ref="M60:M61" si="58">D60^2*E60*F60</f>
+        <f t="shared" ref="M60:M61" si="65">D60^2*E60*F60</f>
         <v>16384</v>
       </c>
       <c r="N60" s="34">
-        <f t="shared" ref="N60:N61" si="59">F60</f>
+        <f t="shared" ref="N60:N61" si="66">F60</f>
         <v>256</v>
       </c>
       <c r="O60" s="35">
-        <f t="shared" ref="O60:O61" si="60">_xlfn.CEILING.MATH(D60^2*E60/2)*F60</f>
+        <f t="shared" ref="O60:O61" si="67">_xlfn.CEILING.MATH(D60^2*E60/2)*F60</f>
         <v>8192</v>
       </c>
       <c r="P60" s="55">
@@ -9058,7 +9059,7 @@
         <v>3513152</v>
       </c>
       <c r="Q60" s="18" t="str">
-        <f t="shared" ref="Q60:Q61" si="61">DEC2HEX(P60)</f>
+        <f t="shared" ref="Q60:Q61" si="68">DEC2HEX(P60)</f>
         <v>359B40</v>
       </c>
       <c r="R60" s="61">
@@ -9066,7 +9067,7 @@
         <v>3469888</v>
       </c>
       <c r="S60" s="18" t="str">
-        <f t="shared" ref="S60:S61" si="62">DEC2HEX(R60)</f>
+        <f t="shared" ref="S60:S61" si="69">DEC2HEX(R60)</f>
         <v>34F240</v>
       </c>
       <c r="T60" s="61">
@@ -9074,7 +9075,7 @@
         <v>281984</v>
       </c>
       <c r="U60" s="18" t="str">
-        <f t="shared" ref="U60:U61" si="63">DEC2HEX(T60)</f>
+        <f t="shared" ref="U60:U61" si="70">DEC2HEX(T60)</f>
         <v>44D80</v>
       </c>
       <c r="V60" s="45" t="s">
@@ -9093,8 +9094,8 @@
         <v>0</v>
       </c>
       <c r="AA60" s="4">
-        <f>0.0000032*M60+0.0000064*K60</f>
-        <v>0.32931840000000001</v>
+        <f t="shared" ref="AA60:AA61" si="71">K60/64*0.97</f>
+        <v>655.72</v>
       </c>
       <c r="AB60" s="4">
         <f>L60*Y60*Z60</f>
@@ -9134,23 +9135,23 @@
         <v>13</v>
       </c>
       <c r="K61" s="34">
-        <f t="shared" si="56"/>
+        <f t="shared" si="63"/>
         <v>43264</v>
       </c>
       <c r="L61" s="34">
-        <f t="shared" si="57"/>
+        <f t="shared" si="64"/>
         <v>10816</v>
       </c>
       <c r="M61" s="34">
-        <f t="shared" si="58"/>
+        <f t="shared" si="65"/>
         <v>147456</v>
       </c>
       <c r="N61" s="34">
-        <f t="shared" si="59"/>
+        <f t="shared" si="66"/>
         <v>256</v>
       </c>
       <c r="O61" s="35">
-        <f t="shared" si="60"/>
+        <f t="shared" si="67"/>
         <v>73728</v>
       </c>
       <c r="P61" s="55">
@@ -9158,7 +9159,7 @@
         <v>3556416</v>
       </c>
       <c r="Q61" s="18" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="68"/>
         <v>364440</v>
       </c>
       <c r="R61" s="61">
@@ -9166,7 +9167,7 @@
         <v>3513152</v>
       </c>
       <c r="S61" s="18" t="str">
-        <f t="shared" si="62"/>
+        <f t="shared" si="69"/>
         <v>359B40</v>
       </c>
       <c r="T61" s="61">
@@ -9174,7 +9175,7 @@
         <v>290176</v>
       </c>
       <c r="U61" s="18" t="str">
-        <f t="shared" si="63"/>
+        <f t="shared" si="70"/>
         <v>46D80</v>
       </c>
       <c r="V61" s="45" t="s">
@@ -9193,8 +9194,8 @@
         <v>1</v>
       </c>
       <c r="AA61" s="4">
-        <f>0.0000032*M61+0.0000064*K61</f>
-        <v>0.74874879999999999</v>
+        <f t="shared" si="71"/>
+        <v>655.72</v>
       </c>
       <c r="AB61" s="4">
         <f>L61*Y61*Z61</f>
@@ -9437,8 +9438,8 @@
         <v>1</v>
       </c>
       <c r="AA66" s="4">
-        <f>0.0000032*M66+0.0000064*K66</f>
-        <v>2.7199999999999998</v>
+        <f>K66/64*0.97</f>
+        <v>2561.40625</v>
       </c>
       <c r="AB66" s="4">
         <f>L66*Y66*Z66</f>
@@ -9555,8 +9556,8 @@
         <v>1</v>
       </c>
       <c r="AA68" s="6">
-        <f>0.0000064*K68</f>
-        <v>6.3999999999999994E-3</v>
+        <f>K68/64*0.97</f>
+        <v>15.15625</v>
       </c>
       <c r="AB68" s="6">
         <f>L68*Y68*Z68</f>
@@ -9643,10 +9644,10 @@
       <c r="Z70" s="26"/>
       <c r="AA70" s="26">
         <f>SUM(AA3:AA69)</f>
-        <v>23.114035199999996</v>
+        <v>46545.692500000019</v>
       </c>
       <c r="AB70" s="26">
-        <f t="shared" ref="AB70" si="64">SUM(AB4:AB69)</f>
+        <f t="shared" ref="AB70" si="72">SUM(AB4:AB69)</f>
         <v>388579.16000000003</v>
       </c>
       <c r="AC70" s="26"/>

</xml_diff>

<commit_message>
Dropout layer is diabled in test/inference
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933EB47A-C77E-4367-9A6B-ACE2E37896DE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C18A31-827D-4AA1-A5A0-594E52357ED4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
@@ -600,7 +600,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -632,6 +632,14 @@
     <font>
       <b/>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Ubuntu Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Ubuntu Mono"/>
@@ -731,7 +739,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -940,6 +948,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5169,8 +5183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80B23C6-EAEB-43B1-B045-456C36085CFA}">
   <dimension ref="A1:AC71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AA6" sqref="AA6:AA71"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9313,10 +9327,10 @@
       <c r="AC64" s="26"/>
     </row>
     <row r="65" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A65" s="11" t="s">
+      <c r="A65" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="B65" s="36" t="s">
+      <c r="B65" s="79" t="s">
         <v>75</v>
       </c>
       <c r="C65" s="36"/>

</xml_diff>

<commit_message>
Update memory access address for commands
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C4B9B6-A1C5-41DC-918C-76508AD64412}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7657A6C0-5B99-4259-BDC6-6CA98DA00C81}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
   <sheets>
     <sheet name="SqueezeNet v2 MEC Parallel Ch" sheetId="2" r:id="rId1"/>
@@ -382,9 +382,6 @@
     <t>Bias</t>
   </si>
   <si>
-    <t>2B Aligned</t>
-  </si>
-  <si>
     <t>0040_0040</t>
   </si>
   <si>
@@ -466,48 +463,30 @@
     <t>00400_101</t>
   </si>
   <si>
-    <t>00001380</t>
-  </si>
-  <si>
     <t>001CA81B</t>
   </si>
   <si>
     <t>00400_103</t>
   </si>
   <si>
-    <t>00001580</t>
-  </si>
-  <si>
     <t>001FB81B</t>
   </si>
   <si>
     <t>02400_113</t>
   </si>
   <si>
-    <t>00001780</t>
-  </si>
-  <si>
     <t>0022C81B</t>
   </si>
   <si>
     <t>00800_101</t>
   </si>
   <si>
-    <t>00002980</t>
-  </si>
-  <si>
     <t>00238C1B</t>
   </si>
   <si>
-    <t>00002D80</t>
-  </si>
-  <si>
     <t>00269C1B</t>
   </si>
   <si>
-    <t>00002F80</t>
-  </si>
-  <si>
     <t>0029AC1B</t>
   </si>
   <si>
@@ -517,48 +496,30 @@
     <t>01000_101</t>
   </si>
   <si>
-    <t>00004180</t>
-  </si>
-  <si>
     <t>002B961B</t>
   </si>
   <si>
     <t>01000_103</t>
   </si>
   <si>
-    <t>00004980</t>
-  </si>
-  <si>
     <t>002D1E1B</t>
   </si>
   <si>
     <t>09000_113</t>
   </si>
   <si>
-    <t>00005180</t>
-  </si>
-  <si>
     <t>002EA61B</t>
   </si>
   <si>
     <t>02000_101</t>
   </si>
   <si>
-    <t>00009980</t>
-  </si>
-  <si>
     <t>002F081B</t>
   </si>
   <si>
-    <t>0000A980</t>
-  </si>
-  <si>
     <t>0030901B</t>
   </si>
   <si>
-    <t>0000B180</t>
-  </si>
-  <si>
     <t>0032181B</t>
   </si>
   <si>
@@ -568,9 +529,6 @@
     <t>03000_101</t>
   </si>
   <si>
-    <t>0000F980</t>
-  </si>
-  <si>
     <t>003300DB</t>
   </si>
   <si>
@@ -580,87 +538,54 @@
     <t>00C0_0030</t>
   </si>
   <si>
-    <t>00011180</t>
-  </si>
-  <si>
     <t>003393DB</t>
   </si>
   <si>
     <t>14400_113</t>
   </si>
   <si>
-    <t>00012380</t>
-  </si>
-  <si>
     <t>003426DB</t>
   </si>
   <si>
     <t>04800_101</t>
   </si>
   <si>
-    <t>0001C580</t>
-  </si>
-  <si>
     <t>00344B9B</t>
   </si>
   <si>
-    <t>0001E980</t>
-  </si>
-  <si>
     <t>0034DE9B</t>
   </si>
   <si>
-    <t>0001FB80</t>
-  </si>
-  <si>
     <t>0035719B</t>
   </si>
   <si>
     <t>06000_101</t>
   </si>
   <si>
-    <t>00029D80</t>
-  </si>
-  <si>
     <t>0035A29B</t>
   </si>
   <si>
     <t>04000_103</t>
   </si>
   <si>
-    <t>0002CD80</t>
-  </si>
-  <si>
     <t>0036669B</t>
   </si>
   <si>
     <t>24000_113</t>
   </si>
   <si>
-    <t>0002ED80</t>
-  </si>
-  <si>
     <t>00372A9B</t>
   </si>
   <si>
     <t>08000_101</t>
   </si>
   <si>
-    <t>00040D80</t>
-  </si>
-  <si>
     <t>00375B9B</t>
   </si>
   <si>
-    <t>00044D80</t>
-  </si>
-  <si>
     <t>00381F9B</t>
   </si>
   <si>
-    <t>00046D80</t>
-  </si>
-  <si>
     <t>0038E39B</t>
   </si>
   <si>
@@ -670,18 +595,12 @@
     <t>03E8_0200</t>
   </si>
   <si>
-    <t>00058D80</t>
-  </si>
-  <si>
     <t>003BE13B</t>
   </si>
   <si>
     <t>03E8_03E8</t>
   </si>
   <si>
-    <t>003BE523</t>
-  </si>
-  <si>
     <t>result addr</t>
   </si>
   <si>
@@ -719,6 +638,87 @@
   </si>
   <si>
     <t>0001_010E</t>
+  </si>
+  <si>
+    <t>Conv Weight</t>
+  </si>
+  <si>
+    <t>000A0000</t>
+  </si>
+  <si>
+    <t>00001700</t>
+  </si>
+  <si>
+    <t>00001B10</t>
+  </si>
+  <si>
+    <t>00001F50</t>
+  </si>
+  <si>
+    <t>00004390</t>
+  </si>
+  <si>
+    <t>00004BA0</t>
+  </si>
+  <si>
+    <t>00004FE0</t>
+  </si>
+  <si>
+    <t>00007420</t>
+  </si>
+  <si>
+    <t>00008440</t>
+  </si>
+  <si>
+    <t>000094C0</t>
+  </si>
+  <si>
+    <t>00012540</t>
+  </si>
+  <si>
+    <t>00014560</t>
+  </si>
+  <si>
+    <t>000155E0</t>
+  </si>
+  <si>
+    <t>0001E660</t>
+  </si>
+  <si>
+    <t>00021690</t>
+  </si>
+  <si>
+    <t>00023B50</t>
+  </si>
+  <si>
+    <t>00038010</t>
+  </si>
+  <si>
+    <t>0003C840</t>
+  </si>
+  <si>
+    <t>0003ED00</t>
+  </si>
+  <si>
+    <t>000531C0</t>
+  </si>
+  <si>
+    <t>00059200</t>
+  </si>
+  <si>
+    <t>0005D300</t>
+  </si>
+  <si>
+    <t>00081400</t>
+  </si>
+  <si>
+    <t>00089440</t>
+  </si>
+  <si>
+    <t>0008D540</t>
+  </si>
+  <si>
+    <t>000B1640</t>
   </si>
 </sst>
 </file>
@@ -1350,7 +1350,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AD71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="G10" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Y4" activeCellId="3" sqref="Q4:S68 U4:U68 W4:W68 Y4:Y68"/>
     </sheetView>
   </sheetViews>
@@ -1368,11 +1368,11 @@
     <col min="13" max="13" width="10.85546875" style="30" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.85546875" style="30" customWidth="1"/>
     <col min="15" max="15" width="7.85546875" style="30" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" style="30" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="27.140625" style="49" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.85546875" style="31" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.85546875" style="37" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.140625" style="37" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="8.85546875" style="31" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="7.85546875" style="37" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="8.85546875" style="31" bestFit="1" customWidth="1"/>
@@ -1433,7 +1433,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D2" s="52" t="s">
         <v>77</v>
@@ -1460,22 +1460,22 @@
         <v>91</v>
       </c>
       <c r="N2" s="24" t="s">
-        <v>85</v>
+        <v>201</v>
       </c>
       <c r="O2" s="24" t="s">
         <v>114</v>
       </c>
       <c r="P2" s="40" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="Q2" s="41" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="R2" s="42" t="s">
         <v>96</v>
       </c>
       <c r="S2" s="18" t="s">
-        <v>217</v>
+        <v>190</v>
       </c>
       <c r="T2" s="58" t="s">
         <v>95</v>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="W2" s="58"/>
       <c r="X2" s="58" t="s">
-        <v>215</v>
+        <v>188</v>
       </c>
       <c r="Y2" s="59"/>
       <c r="Z2" s="20" t="s">
@@ -1522,7 +1522,7 @@
       <c r="H3" s="25"/>
       <c r="I3" s="25"/>
       <c r="J3" s="25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K3" s="25">
         <v>227</v>
@@ -1540,21 +1540,10 @@
       <c r="S3" s="10"/>
       <c r="T3" s="32"/>
       <c r="U3" s="10"/>
-      <c r="V3" s="32">
-        <v>655360</v>
-      </c>
-      <c r="W3" s="10" t="str">
-        <f>DEC2HEX(V3,8)</f>
-        <v>000A0000</v>
-      </c>
-      <c r="X3" s="32">
-        <f>V4</f>
-        <v>809947</v>
-      </c>
-      <c r="Y3" s="11" t="str">
-        <f>DEC2HEX(X3,8)</f>
-        <v>000C5BDB</v>
-      </c>
+      <c r="V3" s="32"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="32"/>
+      <c r="Y3" s="11"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1">
@@ -1595,7 +1584,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K4" s="26">
         <v>113</v>
@@ -1617,8 +1606,8 @@
         <v>64</v>
       </c>
       <c r="P4" s="26">
-        <f>_xlfn.CEILING.MATH(E4^2*F4/2)*G4</f>
-        <v>896</v>
+        <f>N4+O4</f>
+        <v>1792</v>
       </c>
       <c r="Q4" s="45" t="str">
         <f>DEC2HEX(N4,5)&amp;"_"&amp;DEC2HEX(H4,1)&amp;DEC2HEX(I4,1)&amp;DEC2HEX(C4,1)</f>
@@ -1640,20 +1629,19 @@
         <v>00001000</v>
       </c>
       <c r="V4" s="33">
-        <f>V3+L3</f>
-        <v>809947</v>
+        <v>655360</v>
       </c>
       <c r="W4" s="12" t="str">
         <f>DEC2HEX(V4,8)</f>
-        <v>000C5BDB</v>
+        <v>000A0000</v>
       </c>
       <c r="X4" s="33">
-        <f>V6</f>
-        <v>1627163</v>
+        <f>V4+L3</f>
+        <v>809947</v>
       </c>
       <c r="Y4" s="13" t="str">
         <f>DEC2HEX(X4,8)</f>
-        <v>0018D41B</v>
+        <v>000C5BDB</v>
       </c>
       <c r="Z4" s="2">
         <v>0.2</v>
@@ -1736,7 +1724,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K6" s="28">
         <v>56</v>
@@ -1770,20 +1758,20 @@
         <v>00000000</v>
       </c>
       <c r="V6" s="35">
-        <f>V4+L4</f>
-        <v>1627163</v>
+        <f>X4</f>
+        <v>809947</v>
       </c>
       <c r="W6" s="16" t="str">
         <f>DEC2HEX(V6,8)</f>
-        <v>0018D41B</v>
+        <v>000C5BDB</v>
       </c>
       <c r="X6" s="35">
-        <f>V7</f>
-        <v>1827867</v>
+        <f>V6+L4</f>
+        <v>1627163</v>
       </c>
       <c r="Y6" s="17" t="str">
         <f>DEC2HEX(X6,8)</f>
-        <v>001BE41B</v>
+        <v>0018D41B</v>
       </c>
       <c r="Z6" s="4">
         <v>0.31</v>
@@ -1830,7 +1818,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K7" s="26">
         <v>56</v>
@@ -1852,8 +1840,8 @@
         <v>16</v>
       </c>
       <c r="P7" s="26">
-        <f>_xlfn.CEILING.MATH(E7^2*F7/2)*G7</f>
-        <v>512</v>
+        <f>N7+O7</f>
+        <v>1040</v>
       </c>
       <c r="Q7" s="45" t="str">
         <f>DEC2HEX(N7,5)&amp;"_"&amp;DEC2HEX(H7,1)&amp;DEC2HEX(I7,1)&amp;DEC2HEX(C7,1)</f>
@@ -1869,27 +1857,27 @@
       </c>
       <c r="T7" s="33">
         <f>T4+P4</f>
-        <v>4992</v>
+        <v>5888</v>
       </c>
       <c r="U7" s="12" t="str">
         <f>DEC2HEX(T7,8)</f>
-        <v>00001380</v>
+        <v>00001700</v>
       </c>
       <c r="V7" s="33">
-        <f>V6+L6</f>
-        <v>1827867</v>
+        <f>X6</f>
+        <v>1627163</v>
       </c>
       <c r="W7" s="12" t="str">
         <f>DEC2HEX(V7,8)</f>
-        <v>001BE41B</v>
+        <v>0018D41B</v>
       </c>
       <c r="X7" s="33">
-        <f>V9</f>
-        <v>1878043</v>
+        <f>V7+L6</f>
+        <v>1827867</v>
       </c>
       <c r="Y7" s="13" t="str">
         <f>DEC2HEX(X7,8)</f>
-        <v>001CA81B</v>
+        <v>001BE41B</v>
       </c>
       <c r="Z7" s="2">
         <v>0.2</v>
@@ -1972,7 +1960,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K9" s="26">
         <v>56</v>
@@ -1994,8 +1982,8 @@
         <v>64</v>
       </c>
       <c r="P9" s="26">
-        <f t="shared" ref="P9:P10" si="4">_xlfn.CEILING.MATH(E9^2*F9/2)*G9</f>
-        <v>512</v>
+        <f t="shared" ref="P9:P10" si="4">N9+O9</f>
+        <v>1088</v>
       </c>
       <c r="Q9" s="45" t="str">
         <f>DEC2HEX(N9,5)&amp;"_"&amp;DEC2HEX(H9,1)&amp;DEC2HEX(I9,1)&amp;DEC2HEX(C9,1)</f>
@@ -2011,27 +1999,27 @@
       </c>
       <c r="T9" s="33">
         <f>T7+P7</f>
-        <v>5504</v>
+        <v>6928</v>
       </c>
       <c r="U9" s="12" t="str">
         <f t="shared" ref="U9:U10" si="6">DEC2HEX(T9,8)</f>
-        <v>00001580</v>
+        <v>00001B10</v>
       </c>
       <c r="V9" s="33">
-        <f>V7+L7</f>
-        <v>1878043</v>
+        <f>X7</f>
+        <v>1827867</v>
       </c>
       <c r="W9" s="12" t="str">
         <f t="shared" ref="W9:W10" si="7">DEC2HEX(V9,8)</f>
-        <v>001CA81B</v>
+        <v>001BE41B</v>
       </c>
       <c r="X9" s="33">
-        <f>V10</f>
-        <v>2078747</v>
+        <f>V9+L7</f>
+        <v>1878043</v>
       </c>
       <c r="Y9" s="13" t="str">
         <f t="shared" ref="Y9:Y10" si="8">DEC2HEX(X9,8)</f>
-        <v>001FB81B</v>
+        <v>001CA81B</v>
       </c>
       <c r="Z9" s="2">
         <v>0.2</v>
@@ -2078,7 +2066,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K10" s="26">
         <v>56</v>
@@ -2101,7 +2089,7 @@
       </c>
       <c r="P10" s="26">
         <f t="shared" si="4"/>
-        <v>4608</v>
+        <v>9280</v>
       </c>
       <c r="Q10" s="45" t="str">
         <f>DEC2HEX(N10,5)&amp;"_"&amp;DEC2HEX(H10,1)&amp;DEC2HEX(I10,1)&amp;DEC2HEX(C10,1)</f>
@@ -2117,27 +2105,27 @@
       </c>
       <c r="T10" s="33">
         <f>T9+P9</f>
-        <v>6016</v>
+        <v>8016</v>
       </c>
       <c r="U10" s="12" t="str">
         <f t="shared" si="6"/>
-        <v>00001780</v>
+        <v>00001F50</v>
       </c>
       <c r="V10" s="33">
-        <f>V9+L9</f>
-        <v>2078747</v>
+        <f>X7</f>
+        <v>1827867</v>
       </c>
       <c r="W10" s="12" t="str">
         <f t="shared" si="7"/>
-        <v>001FB81B</v>
+        <v>001BE41B</v>
       </c>
       <c r="X10" s="33">
-        <f>V14</f>
-        <v>2279451</v>
+        <f>V10++L7+L9</f>
+        <v>2078747</v>
       </c>
       <c r="Y10" s="13" t="str">
         <f t="shared" si="8"/>
-        <v>0022C81B</v>
+        <v>001FB81B</v>
       </c>
       <c r="Z10" s="2">
         <v>0.2</v>
@@ -2242,7 +2230,7 @@
       <c r="H13" s="25"/>
       <c r="I13" s="25"/>
       <c r="J13" s="25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K13" s="25">
         <v>56</v>
@@ -2296,7 +2284,7 @@
         <v>0</v>
       </c>
       <c r="J14" s="26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K14" s="26">
         <v>56</v>
@@ -2318,8 +2306,8 @@
         <v>16</v>
       </c>
       <c r="P14" s="26">
-        <f>_xlfn.CEILING.MATH(E14^2*F14/2)*G14</f>
-        <v>1024</v>
+        <f>N14+O14</f>
+        <v>2064</v>
       </c>
       <c r="Q14" s="45" t="str">
         <f>DEC2HEX(N14,5)&amp;"_"&amp;DEC2HEX(H14,1)&amp;DEC2HEX(I14,1)&amp;DEC2HEX(C14,1)</f>
@@ -2335,27 +2323,27 @@
       </c>
       <c r="T14" s="33">
         <f>T10+P10</f>
-        <v>10624</v>
+        <v>17296</v>
       </c>
       <c r="U14" s="12" t="str">
         <f>DEC2HEX(T14,8)</f>
-        <v>00002980</v>
+        <v>00004390</v>
       </c>
       <c r="V14" s="33">
-        <f>V10+L10</f>
-        <v>2279451</v>
+        <f>X10</f>
+        <v>2078747</v>
       </c>
       <c r="W14" s="12" t="str">
         <f>DEC2HEX(V14,8)</f>
-        <v>0022C81B</v>
+        <v>001FB81B</v>
       </c>
       <c r="X14" s="33">
-        <f>V16</f>
-        <v>2329627</v>
+        <f>V14+L10</f>
+        <v>2279451</v>
       </c>
       <c r="Y14" s="13" t="str">
         <f>DEC2HEX(X14,8)</f>
-        <v>00238C1B</v>
+        <v>0022C81B</v>
       </c>
       <c r="Z14" s="2">
         <v>0.2</v>
@@ -2438,7 +2426,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K16" s="26">
         <v>56</v>
@@ -2460,8 +2448,8 @@
         <v>64</v>
       </c>
       <c r="P16" s="26">
-        <f t="shared" ref="P16:P17" si="13">_xlfn.CEILING.MATH(E16^2*F16/2)*G16</f>
-        <v>512</v>
+        <f t="shared" ref="P16:P17" si="13">N16+O16</f>
+        <v>1088</v>
       </c>
       <c r="Q16" s="45" t="str">
         <f>DEC2HEX(N16,5)&amp;"_"&amp;DEC2HEX(H16,1)&amp;DEC2HEX(I16,1)&amp;DEC2HEX(C16,1)</f>
@@ -2477,27 +2465,27 @@
       </c>
       <c r="T16" s="33">
         <f>T14+P14</f>
-        <v>11648</v>
+        <v>19360</v>
       </c>
       <c r="U16" s="12" t="str">
         <f t="shared" ref="U16:U17" si="15">DEC2HEX(T16,8)</f>
-        <v>00002D80</v>
+        <v>00004BA0</v>
       </c>
       <c r="V16" s="33">
-        <f>V14+L14</f>
-        <v>2329627</v>
+        <f>X14</f>
+        <v>2279451</v>
       </c>
       <c r="W16" s="12" t="str">
         <f t="shared" ref="W16:W17" si="16">DEC2HEX(V16,8)</f>
-        <v>00238C1B</v>
+        <v>0022C81B</v>
       </c>
       <c r="X16" s="33">
-        <f>V17</f>
-        <v>2530331</v>
+        <f>V16+L14</f>
+        <v>2329627</v>
       </c>
       <c r="Y16" s="13" t="str">
         <f t="shared" ref="Y16:Y17" si="17">DEC2HEX(X16,8)</f>
-        <v>00269C1B</v>
+        <v>00238C1B</v>
       </c>
       <c r="Z16" s="2">
         <v>0.2</v>
@@ -2544,7 +2532,7 @@
         <v>1</v>
       </c>
       <c r="J17" s="26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K17" s="26">
         <v>56</v>
@@ -2567,7 +2555,7 @@
       </c>
       <c r="P17" s="26">
         <f t="shared" si="13"/>
-        <v>4608</v>
+        <v>9280</v>
       </c>
       <c r="Q17" s="45" t="str">
         <f>DEC2HEX(N17,5)&amp;"_"&amp;DEC2HEX(H17,1)&amp;DEC2HEX(I17,1)&amp;DEC2HEX(C17,1)</f>
@@ -2583,27 +2571,27 @@
       </c>
       <c r="T17" s="33">
         <f>T16+P16</f>
-        <v>12160</v>
+        <v>20448</v>
       </c>
       <c r="U17" s="12" t="str">
         <f t="shared" si="15"/>
-        <v>00002F80</v>
+        <v>00004FE0</v>
       </c>
       <c r="V17" s="33">
-        <f>V16+L16</f>
-        <v>2530331</v>
+        <f>X14</f>
+        <v>2279451</v>
       </c>
       <c r="W17" s="12" t="str">
         <f t="shared" si="16"/>
-        <v>00269C1B</v>
+        <v>0022C81B</v>
       </c>
       <c r="X17" s="33">
-        <f>V21</f>
-        <v>2731035</v>
+        <f>V17++L14+L16</f>
+        <v>2530331</v>
       </c>
       <c r="Y17" s="13" t="str">
         <f t="shared" si="17"/>
-        <v>0029AC1B</v>
+        <v>00269C1B</v>
       </c>
       <c r="Z17" s="2">
         <v>0.2</v>
@@ -2708,7 +2696,7 @@
       <c r="H20" s="25"/>
       <c r="I20" s="25"/>
       <c r="J20" s="25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K20" s="25">
         <v>56</v>
@@ -2796,20 +2784,20 @@
         <v>00000000</v>
       </c>
       <c r="V21" s="35">
-        <f>V17+L17</f>
-        <v>2731035</v>
+        <f>X17</f>
+        <v>2530331</v>
       </c>
       <c r="W21" s="16" t="str">
         <f>DEC2HEX(V21,8)</f>
-        <v>0029AC1B</v>
+        <v>00269C1B</v>
       </c>
       <c r="X21" s="35">
-        <f>V22</f>
-        <v>2831387</v>
+        <f>V21+L17</f>
+        <v>2731035</v>
       </c>
       <c r="Y21" s="17" t="str">
         <f>DEC2HEX(X21,8)</f>
-        <v>002B341B</v>
+        <v>0029AC1B</v>
       </c>
       <c r="Z21" s="4">
         <v>0.31</v>
@@ -2856,7 +2844,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K22" s="26">
         <v>28</v>
@@ -2878,8 +2866,8 @@
         <v>32</v>
       </c>
       <c r="P22" s="26">
-        <f>_xlfn.CEILING.MATH(E22^2*F22/2)*G22</f>
-        <v>2048</v>
+        <f>N22+O22</f>
+        <v>4128</v>
       </c>
       <c r="Q22" s="45" t="str">
         <f>DEC2HEX(N22,5)&amp;"_"&amp;DEC2HEX(H22,1)&amp;DEC2HEX(I22,1)&amp;DEC2HEX(C22,1)</f>
@@ -2895,27 +2883,27 @@
       </c>
       <c r="T22" s="33">
         <f>T17+P17</f>
-        <v>16768</v>
+        <v>29728</v>
       </c>
       <c r="U22" s="12" t="str">
         <f>DEC2HEX(T22,8)</f>
-        <v>00004180</v>
+        <v>00007420</v>
       </c>
       <c r="V22" s="33">
-        <f>V21+L21</f>
-        <v>2831387</v>
+        <f>X21</f>
+        <v>2731035</v>
       </c>
       <c r="W22" s="12" t="str">
         <f>DEC2HEX(V22,8)</f>
-        <v>002B341B</v>
+        <v>0029AC1B</v>
       </c>
       <c r="X22" s="33">
-        <f>V24</f>
-        <v>2856475</v>
+        <f>V22+L21</f>
+        <v>2831387</v>
       </c>
       <c r="Y22" s="13" t="str">
         <f>DEC2HEX(X22,8)</f>
-        <v>002B961B</v>
+        <v>002B341B</v>
       </c>
       <c r="Z22" s="2">
         <v>0.2</v>
@@ -2998,7 +2986,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K24" s="26">
         <v>28</v>
@@ -3020,8 +3008,8 @@
         <v>128</v>
       </c>
       <c r="P24" s="26">
-        <f t="shared" ref="P24:P25" si="22">_xlfn.CEILING.MATH(E24^2*F24/2)*G24</f>
-        <v>2048</v>
+        <f t="shared" ref="P24:P25" si="22">N24+O24</f>
+        <v>4224</v>
       </c>
       <c r="Q24" s="45" t="str">
         <f>DEC2HEX(N24,5)&amp;"_"&amp;DEC2HEX(H24,1)&amp;DEC2HEX(I24,1)&amp;DEC2HEX(C24,1)</f>
@@ -3037,27 +3025,27 @@
       </c>
       <c r="T24" s="33">
         <f>T22+P22</f>
-        <v>18816</v>
+        <v>33856</v>
       </c>
       <c r="U24" s="12" t="str">
         <f t="shared" ref="U24:U25" si="24">DEC2HEX(T24,8)</f>
-        <v>00004980</v>
+        <v>00008440</v>
       </c>
       <c r="V24" s="33">
-        <f>V22+L22</f>
-        <v>2856475</v>
+        <f>X22</f>
+        <v>2831387</v>
       </c>
       <c r="W24" s="12" t="str">
         <f t="shared" ref="W24:W25" si="25">DEC2HEX(V24,8)</f>
-        <v>002B961B</v>
+        <v>002B341B</v>
       </c>
       <c r="X24" s="33">
-        <f>V25</f>
-        <v>2956827</v>
+        <f>V24+L22</f>
+        <v>2856475</v>
       </c>
       <c r="Y24" s="13" t="str">
         <f t="shared" ref="Y24:Y25" si="26">DEC2HEX(X24,8)</f>
-        <v>002D1E1B</v>
+        <v>002B961B</v>
       </c>
       <c r="Z24" s="2">
         <v>0.2</v>
@@ -3104,7 +3092,7 @@
         <v>1</v>
       </c>
       <c r="J25" s="26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K25" s="26">
         <v>28</v>
@@ -3127,7 +3115,7 @@
       </c>
       <c r="P25" s="26">
         <f t="shared" si="22"/>
-        <v>18432</v>
+        <v>36992</v>
       </c>
       <c r="Q25" s="45" t="str">
         <f>DEC2HEX(N25,5)&amp;"_"&amp;DEC2HEX(H25,1)&amp;DEC2HEX(I25,1)&amp;DEC2HEX(C25,1)</f>
@@ -3143,27 +3131,27 @@
       </c>
       <c r="T25" s="33">
         <f>T24+P24</f>
-        <v>20864</v>
+        <v>38080</v>
       </c>
       <c r="U25" s="12" t="str">
         <f t="shared" si="24"/>
-        <v>00005180</v>
+        <v>000094C0</v>
       </c>
       <c r="V25" s="33">
-        <f>V24+L24</f>
-        <v>2956827</v>
+        <f>X22</f>
+        <v>2831387</v>
       </c>
       <c r="W25" s="12" t="str">
         <f t="shared" si="25"/>
-        <v>002D1E1B</v>
+        <v>002B341B</v>
       </c>
       <c r="X25" s="33">
-        <f>V29</f>
-        <v>3057179</v>
+        <f>V25++L22+L24</f>
+        <v>2956827</v>
       </c>
       <c r="Y25" s="13" t="str">
         <f t="shared" si="26"/>
-        <v>002EA61B</v>
+        <v>002D1E1B</v>
       </c>
       <c r="Z25" s="2">
         <v>0.2</v>
@@ -3268,7 +3256,7 @@
       <c r="H28" s="25"/>
       <c r="I28" s="25"/>
       <c r="J28" s="25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K28" s="25">
         <v>28</v>
@@ -3322,7 +3310,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K29" s="26">
         <v>28</v>
@@ -3344,8 +3332,8 @@
         <v>32</v>
       </c>
       <c r="P29" s="26">
-        <f>_xlfn.CEILING.MATH(E29^2*F29/2)*G29</f>
-        <v>4096</v>
+        <f>N29+O29</f>
+        <v>8224</v>
       </c>
       <c r="Q29" s="45" t="str">
         <f>DEC2HEX(N29,5)&amp;"_"&amp;DEC2HEX(H29,1)&amp;DEC2HEX(I29,1)&amp;DEC2HEX(C29,1)</f>
@@ -3361,27 +3349,27 @@
       </c>
       <c r="T29" s="33">
         <f>T25+P25</f>
-        <v>39296</v>
+        <v>75072</v>
       </c>
       <c r="U29" s="12" t="str">
         <f>DEC2HEX(T29,8)</f>
-        <v>00009980</v>
+        <v>00012540</v>
       </c>
       <c r="V29" s="33">
-        <f>V25+L25</f>
-        <v>3057179</v>
+        <f>X25</f>
+        <v>2956827</v>
       </c>
       <c r="W29" s="12" t="str">
         <f>DEC2HEX(V29,8)</f>
-        <v>002EA61B</v>
+        <v>002D1E1B</v>
       </c>
       <c r="X29" s="33">
-        <f>V31</f>
-        <v>3082267</v>
+        <f>V29+L25</f>
+        <v>3057179</v>
       </c>
       <c r="Y29" s="13" t="str">
         <f>DEC2HEX(X29,8)</f>
-        <v>002F081B</v>
+        <v>002EA61B</v>
       </c>
       <c r="Z29" s="2">
         <v>0.2</v>
@@ -3464,7 +3452,7 @@
         <v>0</v>
       </c>
       <c r="J31" s="26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K31" s="26">
         <v>28</v>
@@ -3486,8 +3474,8 @@
         <v>128</v>
       </c>
       <c r="P31" s="26">
-        <f t="shared" ref="P31:P32" si="31">_xlfn.CEILING.MATH(E31^2*F31/2)*G31</f>
-        <v>2048</v>
+        <f t="shared" ref="P31:P32" si="31">N31+O31</f>
+        <v>4224</v>
       </c>
       <c r="Q31" s="45" t="str">
         <f>DEC2HEX(N31,5)&amp;"_"&amp;DEC2HEX(H31,1)&amp;DEC2HEX(I31,1)&amp;DEC2HEX(C31,1)</f>
@@ -3503,27 +3491,27 @@
       </c>
       <c r="T31" s="33">
         <f>T29+P29</f>
-        <v>43392</v>
+        <v>83296</v>
       </c>
       <c r="U31" s="12" t="str">
         <f t="shared" ref="U31:U32" si="33">DEC2HEX(T31,8)</f>
-        <v>0000A980</v>
+        <v>00014560</v>
       </c>
       <c r="V31" s="33">
-        <f>V29+L29</f>
-        <v>3082267</v>
+        <f>X29</f>
+        <v>3057179</v>
       </c>
       <c r="W31" s="12" t="str">
         <f t="shared" ref="W31:W32" si="34">DEC2HEX(V31,8)</f>
-        <v>002F081B</v>
+        <v>002EA61B</v>
       </c>
       <c r="X31" s="33">
-        <f>V32</f>
-        <v>3182619</v>
+        <f>V31+L29</f>
+        <v>3082267</v>
       </c>
       <c r="Y31" s="13" t="str">
         <f t="shared" ref="Y31:Y32" si="35">DEC2HEX(X31,8)</f>
-        <v>0030901B</v>
+        <v>002F081B</v>
       </c>
       <c r="Z31" s="2">
         <v>0.2</v>
@@ -3570,7 +3558,7 @@
         <v>1</v>
       </c>
       <c r="J32" s="26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K32" s="26">
         <v>28</v>
@@ -3593,7 +3581,7 @@
       </c>
       <c r="P32" s="26">
         <f t="shared" si="31"/>
-        <v>18432</v>
+        <v>36992</v>
       </c>
       <c r="Q32" s="45" t="str">
         <f>DEC2HEX(N32,5)&amp;"_"&amp;DEC2HEX(H32,1)&amp;DEC2HEX(I32,1)&amp;DEC2HEX(C32,1)</f>
@@ -3609,27 +3597,27 @@
       </c>
       <c r="T32" s="33">
         <f>T31+P31</f>
-        <v>45440</v>
+        <v>87520</v>
       </c>
       <c r="U32" s="12" t="str">
         <f t="shared" si="33"/>
-        <v>0000B180</v>
+        <v>000155E0</v>
       </c>
       <c r="V32" s="33">
-        <f>V31+L31</f>
-        <v>3182619</v>
+        <f>X29</f>
+        <v>3057179</v>
       </c>
       <c r="W32" s="12" t="str">
         <f t="shared" si="34"/>
-        <v>0030901B</v>
+        <v>002EA61B</v>
       </c>
       <c r="X32" s="33">
-        <f>V36</f>
-        <v>3282971</v>
+        <f>V32+L29+L31</f>
+        <v>3182619</v>
       </c>
       <c r="Y32" s="13" t="str">
         <f t="shared" si="35"/>
-        <v>0032181B</v>
+        <v>0030901B</v>
       </c>
       <c r="Z32" s="2">
         <v>0.2</v>
@@ -3734,7 +3722,7 @@
       <c r="H35" s="25"/>
       <c r="I35" s="25"/>
       <c r="J35" s="25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K35" s="25"/>
       <c r="L35" s="25"/>
@@ -3786,7 +3774,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K36" s="28">
         <v>14</v>
@@ -3820,20 +3808,20 @@
         <v>00000000</v>
       </c>
       <c r="V36" s="35">
-        <f>V32+L32</f>
-        <v>3282971</v>
+        <f>X32</f>
+        <v>3182619</v>
       </c>
       <c r="W36" s="16" t="str">
         <f>DEC2HEX(V36,8)</f>
-        <v>0032181B</v>
+        <v>0030901B</v>
       </c>
       <c r="X36" s="35">
-        <f>V37</f>
-        <v>3333147</v>
+        <f>V36+L32</f>
+        <v>3282971</v>
       </c>
       <c r="Y36" s="17" t="str">
         <f>DEC2HEX(X36,8)</f>
-        <v>0032DC1B</v>
+        <v>0032181B</v>
       </c>
       <c r="Z36" s="4">
         <v>0.31</v>
@@ -3880,7 +3868,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K37" s="26">
         <v>14</v>
@@ -3902,8 +3890,8 @@
         <v>48</v>
       </c>
       <c r="P37" s="26">
-        <f>_xlfn.CEILING.MATH(E37^2*F37/2)*G37</f>
-        <v>6144</v>
+        <f>N37+O37</f>
+        <v>12336</v>
       </c>
       <c r="Q37" s="45" t="str">
         <f>DEC2HEX(N37,5)&amp;"_"&amp;DEC2HEX(H37,1)&amp;DEC2HEX(I37,1)&amp;DEC2HEX(C37,1)</f>
@@ -3919,27 +3907,27 @@
       </c>
       <c r="T37" s="33">
         <f>T32+P32</f>
-        <v>63872</v>
+        <v>124512</v>
       </c>
       <c r="U37" s="12" t="str">
         <f>DEC2HEX(T37,8)</f>
-        <v>0000F980</v>
+        <v>0001E660</v>
       </c>
       <c r="V37" s="33">
-        <f>V36+L36</f>
-        <v>3333147</v>
+        <f>X36</f>
+        <v>3282971</v>
       </c>
       <c r="W37" s="12" t="str">
         <f>DEC2HEX(V37,8)</f>
-        <v>0032DC1B</v>
+        <v>0032181B</v>
       </c>
       <c r="X37" s="33">
-        <f>V39</f>
-        <v>3342555</v>
+        <f>V37+L36</f>
+        <v>3333147</v>
       </c>
       <c r="Y37" s="13" t="str">
         <f>DEC2HEX(X37,8)</f>
-        <v>003300DB</v>
+        <v>0032DC1B</v>
       </c>
       <c r="Z37" s="2">
         <v>0.2</v>
@@ -4022,7 +4010,7 @@
         <v>0</v>
       </c>
       <c r="J39" s="26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K39" s="26">
         <v>14</v>
@@ -4044,8 +4032,8 @@
         <v>192</v>
       </c>
       <c r="P39" s="26">
-        <f t="shared" ref="P39:P40" si="40">_xlfn.CEILING.MATH(E39^2*F39/2)*G39</f>
-        <v>4608</v>
+        <f t="shared" ref="P39:P40" si="40">N39+O39</f>
+        <v>9408</v>
       </c>
       <c r="Q39" s="45" t="str">
         <f>DEC2HEX(N39,5)&amp;"_"&amp;DEC2HEX(H39,1)&amp;DEC2HEX(I39,1)&amp;DEC2HEX(C39,1)</f>
@@ -4061,27 +4049,27 @@
       </c>
       <c r="T39" s="33">
         <f>T37+P37</f>
-        <v>70016</v>
+        <v>136848</v>
       </c>
       <c r="U39" s="12" t="str">
         <f t="shared" ref="U39:U40" si="42">DEC2HEX(T39,8)</f>
-        <v>00011180</v>
+        <v>00021690</v>
       </c>
       <c r="V39" s="33">
-        <f>V37+L37</f>
-        <v>3342555</v>
+        <f>X37</f>
+        <v>3333147</v>
       </c>
       <c r="W39" s="12" t="str">
         <f t="shared" ref="W39:W40" si="43">DEC2HEX(V39,8)</f>
-        <v>003300DB</v>
+        <v>0032DC1B</v>
       </c>
       <c r="X39" s="33">
-        <f>V40</f>
-        <v>3380187</v>
+        <f>V39+L37</f>
+        <v>3342555</v>
       </c>
       <c r="Y39" s="13" t="str">
         <f t="shared" ref="Y39:Y40" si="44">DEC2HEX(X39,8)</f>
-        <v>003393DB</v>
+        <v>003300DB</v>
       </c>
       <c r="Z39" s="2">
         <v>0.2</v>
@@ -4128,7 +4116,7 @@
         <v>1</v>
       </c>
       <c r="J40" s="26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K40" s="26">
         <v>14</v>
@@ -4151,7 +4139,7 @@
       </c>
       <c r="P40" s="26">
         <f t="shared" si="40"/>
-        <v>41472</v>
+        <v>83136</v>
       </c>
       <c r="Q40" s="45" t="str">
         <f>DEC2HEX(N40,5)&amp;"_"&amp;DEC2HEX(H40,1)&amp;DEC2HEX(I40,1)&amp;DEC2HEX(C40,1)</f>
@@ -4167,27 +4155,27 @@
       </c>
       <c r="T40" s="33">
         <f>T39+P39</f>
-        <v>74624</v>
+        <v>146256</v>
       </c>
       <c r="U40" s="12" t="str">
         <f t="shared" si="42"/>
-        <v>00012380</v>
+        <v>00023B50</v>
       </c>
       <c r="V40" s="33">
-        <f>V39+L39</f>
-        <v>3380187</v>
+        <f>X37</f>
+        <v>3333147</v>
       </c>
       <c r="W40" s="12" t="str">
         <f t="shared" si="43"/>
-        <v>003393DB</v>
+        <v>0032DC1B</v>
       </c>
       <c r="X40" s="33">
-        <f>V44</f>
-        <v>3417819</v>
+        <f>V40+L37+L39</f>
+        <v>3380187</v>
       </c>
       <c r="Y40" s="13" t="str">
         <f t="shared" si="44"/>
-        <v>003426DB</v>
+        <v>003393DB</v>
       </c>
       <c r="Z40" s="2">
         <v>0.2</v>
@@ -4292,7 +4280,7 @@
       <c r="H43" s="25"/>
       <c r="I43" s="25"/>
       <c r="J43" s="25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K43" s="25">
         <v>14</v>
@@ -4346,7 +4334,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K44" s="26">
         <v>14</v>
@@ -4368,8 +4356,8 @@
         <v>48</v>
       </c>
       <c r="P44" s="26">
-        <f>_xlfn.CEILING.MATH(E44^2*F44/2)*G44</f>
-        <v>9216</v>
+        <f>N44+O44</f>
+        <v>18480</v>
       </c>
       <c r="Q44" s="45" t="str">
         <f>DEC2HEX(N44,5)&amp;"_"&amp;DEC2HEX(H44,1)&amp;DEC2HEX(I44,1)&amp;DEC2HEX(C44,1)</f>
@@ -4385,27 +4373,27 @@
       </c>
       <c r="T44" s="33">
         <f>T40+P40</f>
-        <v>116096</v>
+        <v>229392</v>
       </c>
       <c r="U44" s="12" t="str">
         <f>DEC2HEX(T44,8)</f>
-        <v>0001C580</v>
+        <v>00038010</v>
       </c>
       <c r="V44" s="33">
-        <f>V40+L40</f>
-        <v>3417819</v>
+        <f>X40</f>
+        <v>3380187</v>
       </c>
       <c r="W44" s="12" t="str">
         <f>DEC2HEX(V44,8)</f>
-        <v>003426DB</v>
+        <v>003393DB</v>
       </c>
       <c r="X44" s="33">
-        <f>V46</f>
-        <v>3427227</v>
+        <f>V44+L40</f>
+        <v>3417819</v>
       </c>
       <c r="Y44" s="13" t="str">
         <f>DEC2HEX(X44,8)</f>
-        <v>00344B9B</v>
+        <v>003426DB</v>
       </c>
       <c r="Z44" s="2">
         <v>0.2</v>
@@ -4488,7 +4476,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K46" s="26">
         <v>14</v>
@@ -4510,8 +4498,8 @@
         <v>192</v>
       </c>
       <c r="P46" s="26">
-        <f t="shared" ref="P46:P47" si="49">_xlfn.CEILING.MATH(E46^2*F46/2)*G46</f>
-        <v>4608</v>
+        <f t="shared" ref="P46:P47" si="49">N46+O46</f>
+        <v>9408</v>
       </c>
       <c r="Q46" s="45" t="str">
         <f>DEC2HEX(N46,5)&amp;"_"&amp;DEC2HEX(H46,1)&amp;DEC2HEX(I46,1)&amp;DEC2HEX(C46,1)</f>
@@ -4527,27 +4515,27 @@
       </c>
       <c r="T46" s="33">
         <f>T44+P44</f>
-        <v>125312</v>
+        <v>247872</v>
       </c>
       <c r="U46" s="12" t="str">
         <f t="shared" ref="U46:U47" si="51">DEC2HEX(T46,8)</f>
-        <v>0001E980</v>
+        <v>0003C840</v>
       </c>
       <c r="V46" s="33">
-        <f>V44+L44</f>
-        <v>3427227</v>
+        <f>X44</f>
+        <v>3417819</v>
       </c>
       <c r="W46" s="12" t="str">
         <f t="shared" ref="W46:W47" si="52">DEC2HEX(V46,8)</f>
-        <v>00344B9B</v>
+        <v>003426DB</v>
       </c>
       <c r="X46" s="33">
-        <f>V47</f>
-        <v>3464859</v>
+        <f>V46+L44</f>
+        <v>3427227</v>
       </c>
       <c r="Y46" s="13" t="str">
         <f t="shared" ref="Y46:Y47" si="53">DEC2HEX(X46,8)</f>
-        <v>0034DE9B</v>
+        <v>00344B9B</v>
       </c>
       <c r="Z46" s="2">
         <v>0.2</v>
@@ -4594,7 +4582,7 @@
         <v>1</v>
       </c>
       <c r="J47" s="26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K47" s="26">
         <v>14</v>
@@ -4617,7 +4605,7 @@
       </c>
       <c r="P47" s="26">
         <f t="shared" si="49"/>
-        <v>41472</v>
+        <v>83136</v>
       </c>
       <c r="Q47" s="45" t="str">
         <f>DEC2HEX(N47,5)&amp;"_"&amp;DEC2HEX(H47,1)&amp;DEC2HEX(I47,1)&amp;DEC2HEX(C47,1)</f>
@@ -4633,27 +4621,27 @@
       </c>
       <c r="T47" s="33">
         <f>T46+P46</f>
-        <v>129920</v>
+        <v>257280</v>
       </c>
       <c r="U47" s="12" t="str">
         <f t="shared" si="51"/>
-        <v>0001FB80</v>
+        <v>0003ED00</v>
       </c>
       <c r="V47" s="33">
-        <f>V46+L46</f>
-        <v>3464859</v>
+        <f>X44</f>
+        <v>3417819</v>
       </c>
       <c r="W47" s="12" t="str">
         <f t="shared" si="52"/>
-        <v>0034DE9B</v>
+        <v>003426DB</v>
       </c>
       <c r="X47" s="33">
-        <f>V51</f>
-        <v>3502491</v>
+        <f>V47+L44+L46</f>
+        <v>3464859</v>
       </c>
       <c r="Y47" s="13" t="str">
         <f t="shared" si="53"/>
-        <v>0035719B</v>
+        <v>0034DE9B</v>
       </c>
       <c r="Z47" s="2">
         <v>0.2</v>
@@ -4758,7 +4746,7 @@
       <c r="H50" s="25"/>
       <c r="I50" s="25"/>
       <c r="J50" s="25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K50" s="25">
         <v>14</v>
@@ -4812,7 +4800,7 @@
         <v>0</v>
       </c>
       <c r="J51" s="26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K51" s="26">
         <v>14</v>
@@ -4834,8 +4822,8 @@
         <v>64</v>
       </c>
       <c r="P51" s="26">
-        <f>_xlfn.CEILING.MATH(E51^2*F51/2)*G51</f>
-        <v>12288</v>
+        <f>N51+O51</f>
+        <v>24640</v>
       </c>
       <c r="Q51" s="45" t="str">
         <f>DEC2HEX(N51,5)&amp;"_"&amp;DEC2HEX(H51,1)&amp;DEC2HEX(I51,1)&amp;DEC2HEX(C51,1)</f>
@@ -4851,27 +4839,27 @@
       </c>
       <c r="T51" s="33">
         <f>T47+P47</f>
-        <v>171392</v>
+        <v>340416</v>
       </c>
       <c r="U51" s="12" t="str">
         <f>DEC2HEX(T51,8)</f>
-        <v>00029D80</v>
+        <v>000531C0</v>
       </c>
       <c r="V51" s="33">
-        <f>V47+L47</f>
-        <v>3502491</v>
+        <f>X47</f>
+        <v>3464859</v>
       </c>
       <c r="W51" s="12" t="str">
         <f>DEC2HEX(V51,8)</f>
-        <v>0035719B</v>
+        <v>0034DE9B</v>
       </c>
       <c r="X51" s="33">
-        <f>V53</f>
-        <v>3515035</v>
+        <f>V51+L47</f>
+        <v>3502491</v>
       </c>
       <c r="Y51" s="13" t="str">
         <f>DEC2HEX(X51,8)</f>
-        <v>0035A29B</v>
+        <v>0035719B</v>
       </c>
       <c r="Z51" s="2">
         <v>0.2</v>
@@ -4954,7 +4942,7 @@
         <v>0</v>
       </c>
       <c r="J53" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K53" s="26">
         <v>14</v>
@@ -4976,8 +4964,8 @@
         <v>256</v>
       </c>
       <c r="P53" s="26">
-        <f t="shared" ref="P53:P54" si="58">_xlfn.CEILING.MATH(E53^2*F53/2)*G53</f>
-        <v>8192</v>
+        <f t="shared" ref="P53:P54" si="58">N53+O53</f>
+        <v>16640</v>
       </c>
       <c r="Q53" s="45" t="str">
         <f>DEC2HEX(N53,5)&amp;"_"&amp;DEC2HEX(H53,1)&amp;DEC2HEX(I53,1)&amp;DEC2HEX(C53,1)</f>
@@ -4993,27 +4981,27 @@
       </c>
       <c r="T53" s="33">
         <f>T51+P51</f>
-        <v>183680</v>
+        <v>365056</v>
       </c>
       <c r="U53" s="12" t="str">
         <f t="shared" ref="U53:U54" si="60">DEC2HEX(T53,8)</f>
-        <v>0002CD80</v>
+        <v>00059200</v>
       </c>
       <c r="V53" s="33">
-        <f>V51+L51</f>
-        <v>3515035</v>
+        <f>X51</f>
+        <v>3502491</v>
       </c>
       <c r="W53" s="12" t="str">
         <f t="shared" ref="W53:W54" si="61">DEC2HEX(V53,8)</f>
-        <v>0035A29B</v>
+        <v>0035719B</v>
       </c>
       <c r="X53" s="33">
-        <f>V54</f>
-        <v>3565211</v>
+        <f>V53+L51</f>
+        <v>3515035</v>
       </c>
       <c r="Y53" s="13" t="str">
         <f t="shared" ref="Y53:Y54" si="62">DEC2HEX(X53,8)</f>
-        <v>0036669B</v>
+        <v>0035A29B</v>
       </c>
       <c r="Z53" s="2">
         <v>0.2</v>
@@ -5060,7 +5048,7 @@
         <v>1</v>
       </c>
       <c r="J54" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K54" s="26">
         <v>14</v>
@@ -5083,7 +5071,7 @@
       </c>
       <c r="P54" s="26">
         <f t="shared" si="58"/>
-        <v>73728</v>
+        <v>147712</v>
       </c>
       <c r="Q54" s="45" t="str">
         <f>DEC2HEX(N54,5)&amp;"_"&amp;DEC2HEX(H54,1)&amp;DEC2HEX(I54,1)&amp;DEC2HEX(C54,1)</f>
@@ -5099,27 +5087,27 @@
       </c>
       <c r="T54" s="33">
         <f>T53+P53</f>
-        <v>191872</v>
+        <v>381696</v>
       </c>
       <c r="U54" s="12" t="str">
         <f t="shared" si="60"/>
-        <v>0002ED80</v>
+        <v>0005D300</v>
       </c>
       <c r="V54" s="33">
-        <f>V53+L53</f>
-        <v>3565211</v>
+        <f>X51</f>
+        <v>3502491</v>
       </c>
       <c r="W54" s="12" t="str">
         <f t="shared" si="61"/>
-        <v>0036669B</v>
+        <v>0035719B</v>
       </c>
       <c r="X54" s="33">
-        <f>V58</f>
-        <v>3615387</v>
+        <f>V54+L51+L53</f>
+        <v>3565211</v>
       </c>
       <c r="Y54" s="13" t="str">
         <f t="shared" si="62"/>
-        <v>00372A9B</v>
+        <v>0036669B</v>
       </c>
       <c r="Z54" s="2">
         <v>0.2</v>
@@ -5224,7 +5212,7 @@
       <c r="H57" s="25"/>
       <c r="I57" s="25"/>
       <c r="J57" s="25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K57" s="25">
         <v>14</v>
@@ -5278,7 +5266,7 @@
         <v>0</v>
       </c>
       <c r="J58" s="26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K58" s="26">
         <v>14</v>
@@ -5300,8 +5288,8 @@
         <v>64</v>
       </c>
       <c r="P58" s="26">
-        <f>_xlfn.CEILING.MATH(E58^2*F58/2)*G58</f>
-        <v>16384</v>
+        <f>N58+O58</f>
+        <v>32832</v>
       </c>
       <c r="Q58" s="45" t="str">
         <f>DEC2HEX(N58,5)&amp;"_"&amp;DEC2HEX(H58,1)&amp;DEC2HEX(I58,1)&amp;DEC2HEX(C58,1)</f>
@@ -5317,27 +5305,27 @@
       </c>
       <c r="T58" s="33">
         <f>T54+P54</f>
-        <v>265600</v>
+        <v>529408</v>
       </c>
       <c r="U58" s="12" t="str">
         <f>DEC2HEX(T58,8)</f>
-        <v>00040D80</v>
+        <v>00081400</v>
       </c>
       <c r="V58" s="33">
-        <f>V54+L54</f>
-        <v>3615387</v>
+        <f>X54</f>
+        <v>3565211</v>
       </c>
       <c r="W58" s="12" t="str">
         <f>DEC2HEX(V58,8)</f>
-        <v>00372A9B</v>
+        <v>0036669B</v>
       </c>
       <c r="X58" s="33">
-        <f>V60</f>
-        <v>3627931</v>
+        <f>V58+L54</f>
+        <v>3615387</v>
       </c>
       <c r="Y58" s="13" t="str">
         <f>DEC2HEX(X58,8)</f>
-        <v>00375B9B</v>
+        <v>00372A9B</v>
       </c>
       <c r="Z58" s="2">
         <v>0.2</v>
@@ -5420,7 +5408,7 @@
         <v>0</v>
       </c>
       <c r="J60" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K60" s="26">
         <v>14</v>
@@ -5442,8 +5430,8 @@
         <v>256</v>
       </c>
       <c r="P60" s="26">
-        <f t="shared" ref="P60:P61" si="67">_xlfn.CEILING.MATH(E60^2*F60/2)*G60</f>
-        <v>8192</v>
+        <f t="shared" ref="P60:P61" si="67">N60+O60</f>
+        <v>16640</v>
       </c>
       <c r="Q60" s="45" t="str">
         <f>DEC2HEX(N60,5)&amp;"_"&amp;DEC2HEX(H60,1)&amp;DEC2HEX(I60,1)&amp;DEC2HEX(C60,1)</f>
@@ -5459,27 +5447,27 @@
       </c>
       <c r="T60" s="33">
         <f>T58+P58</f>
-        <v>281984</v>
+        <v>562240</v>
       </c>
       <c r="U60" s="12" t="str">
         <f t="shared" ref="U60:U61" si="69">DEC2HEX(T60,8)</f>
-        <v>00044D80</v>
+        <v>00089440</v>
       </c>
       <c r="V60" s="33">
-        <f>V58+L58</f>
-        <v>3627931</v>
+        <f>X58</f>
+        <v>3615387</v>
       </c>
       <c r="W60" s="12" t="str">
         <f t="shared" ref="W60:W61" si="70">DEC2HEX(V60,8)</f>
-        <v>00375B9B</v>
+        <v>00372A9B</v>
       </c>
       <c r="X60" s="33">
-        <f>V61</f>
-        <v>3678107</v>
+        <f>V60+L58</f>
+        <v>3627931</v>
       </c>
       <c r="Y60" s="13" t="str">
         <f t="shared" ref="Y60:Y61" si="71">DEC2HEX(X60,8)</f>
-        <v>00381F9B</v>
+        <v>00375B9B</v>
       </c>
       <c r="Z60" s="2">
         <v>0.2</v>
@@ -5526,7 +5514,7 @@
         <v>1</v>
       </c>
       <c r="J61" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K61" s="26">
         <v>14</v>
@@ -5549,7 +5537,7 @@
       </c>
       <c r="P61" s="26">
         <f t="shared" si="67"/>
-        <v>73728</v>
+        <v>147712</v>
       </c>
       <c r="Q61" s="45" t="str">
         <f>DEC2HEX(N61,5)&amp;"_"&amp;DEC2HEX(H61,1)&amp;DEC2HEX(I61,1)&amp;DEC2HEX(C61,1)</f>
@@ -5565,27 +5553,27 @@
       </c>
       <c r="T61" s="33">
         <f>T60+P60</f>
-        <v>290176</v>
+        <v>578880</v>
       </c>
       <c r="U61" s="12" t="str">
         <f t="shared" si="69"/>
-        <v>00046D80</v>
+        <v>0008D540</v>
       </c>
       <c r="V61" s="33">
-        <f>V60+L60</f>
-        <v>3678107</v>
+        <f>X58</f>
+        <v>3615387</v>
       </c>
       <c r="W61" s="12" t="str">
         <f t="shared" si="70"/>
-        <v>00381F9B</v>
+        <v>00372A9B</v>
       </c>
       <c r="X61" s="33">
-        <f>V66</f>
-        <v>3728283</v>
+        <f>V61+L58+L60</f>
+        <v>3678107</v>
       </c>
       <c r="Y61" s="13" t="str">
         <f t="shared" si="71"/>
-        <v>0038E39B</v>
+        <v>00381F9B</v>
       </c>
       <c r="Z61" s="2">
         <v>0.2</v>
@@ -5690,7 +5678,7 @@
       <c r="H64" s="25"/>
       <c r="I64" s="25"/>
       <c r="J64" s="25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K64" s="25">
         <v>14</v>
@@ -5780,7 +5768,7 @@
         <v>0</v>
       </c>
       <c r="J66" s="26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K66" s="26">
         <v>14</v>
@@ -5802,8 +5790,8 @@
         <v>1000</v>
       </c>
       <c r="P66" s="26">
-        <f>_xlfn.CEILING.MATH(E66^2*F66/2)*G66</f>
-        <v>256000</v>
+        <f>N66+O66</f>
+        <v>513000</v>
       </c>
       <c r="Q66" s="45" t="str">
         <f>DEC2HEX(N66,5)&amp;"_"&amp;DEC2HEX(H66,1)&amp;DEC2HEX(I66,1)&amp;DEC2HEX(C66,1)</f>
@@ -5819,27 +5807,27 @@
       </c>
       <c r="T66" s="33">
         <f>T61+P61</f>
-        <v>363904</v>
+        <v>726592</v>
       </c>
       <c r="U66" s="12" t="str">
         <f>DEC2HEX(T66,8)</f>
-        <v>00058D80</v>
+        <v>000B1640</v>
       </c>
       <c r="V66" s="33">
-        <f>V61+L61</f>
-        <v>3728283</v>
+        <f>X61</f>
+        <v>3678107</v>
       </c>
       <c r="W66" s="12" t="str">
         <f>DEC2HEX(V66,8)</f>
-        <v>0038E39B</v>
+        <v>00381F9B</v>
       </c>
       <c r="X66" s="33">
-        <f>V68</f>
-        <v>3924283</v>
+        <f>V66+L61</f>
+        <v>3728283</v>
       </c>
       <c r="Y66" s="13" t="str">
         <f>DEC2HEX(X66,8)</f>
-        <v>003BE13B</v>
+        <v>0038E39B</v>
       </c>
       <c r="Z66" s="2">
         <v>0.2</v>
@@ -5904,7 +5892,7 @@
         <v>5</v>
       </c>
       <c r="D68" s="28" t="s">
-        <v>216</v>
+        <v>189</v>
       </c>
       <c r="E68" s="28">
         <v>14</v>
@@ -5956,20 +5944,20 @@
         <v>00000000</v>
       </c>
       <c r="V68" s="35">
-        <f>V66+L66</f>
-        <v>3924283</v>
+        <f>X66</f>
+        <v>3728283</v>
       </c>
       <c r="W68" s="16" t="str">
         <f>DEC2HEX(V68,8)</f>
-        <v>003BE13B</v>
+        <v>0038E39B</v>
       </c>
       <c r="X68" s="35">
-        <f>V69</f>
-        <v>3925283</v>
+        <f>V68+L66</f>
+        <v>3924283</v>
       </c>
       <c r="Y68" s="17" t="str">
         <f>DEC2HEX(X68,8)</f>
-        <v>003BE523</v>
+        <v>003BE13B</v>
       </c>
       <c r="Z68" s="4">
         <v>1.2</v>
@@ -6013,10 +6001,7 @@
       <c r="S69" s="10"/>
       <c r="T69" s="32"/>
       <c r="U69" s="10"/>
-      <c r="V69" s="32">
-        <f>V68+M68</f>
-        <v>3925283</v>
-      </c>
+      <c r="V69" s="32"/>
       <c r="W69" s="10"/>
       <c r="X69" s="32"/>
       <c r="Y69" s="11"/>
@@ -6053,7 +6038,7 @@
       </c>
       <c r="P70" s="40">
         <f>SUM(P4:P69)</f>
-        <v>615808</v>
+        <v>1235496</v>
       </c>
       <c r="Q70" s="48"/>
       <c r="R70" s="18"/>
@@ -6141,7 +6126,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="V4:V66 X3:X72" formula="1"/>
+    <ignoredError sqref="X70:X72 V7:V68 X4:X68" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -6150,8 +6135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E501AE-4D2D-491C-85E4-0C34FDA03C89}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:M30"/>
+    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
+      <selection sqref="A1:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6166,22 +6151,22 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>97</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>218</v>
+        <v>191</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>137</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>139</v>
       </c>
       <c r="H1" t="str">
         <f>LEFT(SUBSTITUTE(A1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A1,"_",),4)</f>
@@ -6201,31 +6186,31 @@
       </c>
       <c r="L1" t="str">
         <f t="shared" si="0"/>
-        <v>000C 5BDB</v>
+        <v>000A 0000</v>
       </c>
       <c r="M1" t="str">
         <f t="shared" si="0"/>
-        <v>0018 D41B</v>
+        <v>000C 5BDB</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
-        <v>219</v>
+        <v>192</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>220</v>
+        <v>193</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H2" t="str">
         <f t="shared" ref="H2:H30" si="1">LEFT(SUBSTITUTE(A2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A2,"_",),4)</f>
@@ -6245,31 +6230,31 @@
       </c>
       <c r="L2" t="str">
         <f t="shared" ref="L2:L30" si="5">LEFT(SUBSTITUTE(E2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E2,"_",),4)</f>
-        <v>0018 D41B</v>
+        <v>000C 5BDB</v>
       </c>
       <c r="M2" t="str">
         <f t="shared" ref="M2:M30" si="6">LEFT(SUBSTITUTE(F2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F2,"_",),4)</f>
-        <v>001B E41B</v>
+        <v>0018 D41B</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="45" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>98</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>221</v>
+        <v>194</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>143</v>
+        <v>203</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" si="1"/>
@@ -6285,35 +6270,35 @@
       </c>
       <c r="K3" t="str">
         <f t="shared" si="4"/>
-        <v>0000 1380</v>
+        <v>0000 1700</v>
       </c>
       <c r="L3" t="str">
         <f t="shared" si="5"/>
-        <v>001B E41B</v>
+        <v>0018 D41B</v>
       </c>
       <c r="M3" t="str">
         <f t="shared" si="6"/>
-        <v>001C A81B</v>
+        <v>001B E41B</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="45" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>99</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>221</v>
+        <v>194</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>146</v>
+        <v>204</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="1"/>
@@ -6329,35 +6314,35 @@
       </c>
       <c r="K4" t="str">
         <f t="shared" si="4"/>
-        <v>0000 1580</v>
+        <v>0000 1B10</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" si="5"/>
-        <v>001C A81B</v>
+        <v>001B E41B</v>
       </c>
       <c r="M4" t="str">
         <f t="shared" si="6"/>
-        <v>001F B81B</v>
+        <v>001C A81B</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="45" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>99</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>220</v>
+        <v>193</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>149</v>
+        <v>205</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="1"/>
@@ -6373,35 +6358,35 @@
       </c>
       <c r="K5" t="str">
         <f t="shared" si="4"/>
-        <v>0000 1780</v>
+        <v>0000 1F50</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" si="5"/>
-        <v>001F B81B</v>
+        <v>001B E41B</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" si="6"/>
-        <v>0022 C81B</v>
+        <v>001F B81B</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="45" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>100</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>221</v>
+        <v>194</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>152</v>
+        <v>206</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="1"/>
@@ -6417,35 +6402,35 @@
       </c>
       <c r="K6" t="str">
         <f t="shared" si="4"/>
-        <v>0000 2980</v>
+        <v>0000 4390</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="5"/>
-        <v>0022 C81B</v>
+        <v>001F B81B</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" si="6"/>
-        <v>0023 8C1B</v>
+        <v>0022 C81B</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="45" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>99</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>221</v>
+        <v>194</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>154</v>
+        <v>207</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="1"/>
@@ -6461,35 +6446,35 @@
       </c>
       <c r="K7" t="str">
         <f t="shared" si="4"/>
-        <v>0000 2D80</v>
+        <v>0000 4BA0</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="5"/>
-        <v>0023 8C1B</v>
+        <v>0022 C81B</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="6"/>
-        <v>0026 9C1B</v>
+        <v>0023 8C1B</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="45" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>99</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>220</v>
+        <v>193</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>156</v>
+        <v>208</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="1"/>
@@ -6505,35 +6490,35 @@
       </c>
       <c r="K8" t="str">
         <f t="shared" si="4"/>
-        <v>0000 2F80</v>
+        <v>0000 4FE0</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="5"/>
-        <v>0026 9C1B</v>
+        <v>0022 C81B</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" si="6"/>
-        <v>0029 AC1B</v>
+        <v>0026 9C1B</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
-        <v>219</v>
+        <v>192</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>222</v>
+        <v>195</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="1"/>
@@ -6553,31 +6538,31 @@
       </c>
       <c r="L9" t="str">
         <f t="shared" si="5"/>
-        <v>0029 AC1B</v>
+        <v>0026 9C1B</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" si="6"/>
-        <v>002B 341B</v>
+        <v>0029 AC1B</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="45" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>101</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>223</v>
+        <v>196</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>160</v>
+        <v>209</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="1"/>
@@ -6593,35 +6578,35 @@
       </c>
       <c r="K10" t="str">
         <f t="shared" si="4"/>
-        <v>0000 4180</v>
+        <v>0000 7420</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="5"/>
-        <v>002B 341B</v>
+        <v>0029 AC1B</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" si="6"/>
-        <v>002B 961B</v>
+        <v>002B 341B</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="45" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>223</v>
+        <v>196</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>163</v>
+        <v>210</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="1"/>
@@ -6637,35 +6622,35 @@
       </c>
       <c r="K11" t="str">
         <f t="shared" si="4"/>
-        <v>0000 4980</v>
+        <v>0000 8440</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="5"/>
-        <v>002B 961B</v>
+        <v>002B 341B</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" si="6"/>
-        <v>002D 1E1B</v>
+        <v>002B 961B</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="45" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>222</v>
+        <v>195</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>166</v>
+        <v>211</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="1"/>
@@ -6681,35 +6666,35 @@
       </c>
       <c r="K12" t="str">
         <f t="shared" si="4"/>
-        <v>0000 5180</v>
+        <v>0000 94C0</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="5"/>
-        <v>002D 1E1B</v>
+        <v>002B 341B</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" si="6"/>
-        <v>002E A61B</v>
+        <v>002D 1E1B</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="45" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>102</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>223</v>
+        <v>196</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>169</v>
+        <v>212</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="1"/>
@@ -6725,35 +6710,35 @@
       </c>
       <c r="K13" t="str">
         <f t="shared" si="4"/>
-        <v>0000 9980</v>
+        <v>0001 2540</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="5"/>
-        <v>002E A61B</v>
+        <v>002D 1E1B</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="6"/>
-        <v>002F 081B</v>
+        <v>002E A61B</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="45" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>223</v>
+        <v>196</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>171</v>
+        <v>213</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="1"/>
@@ -6769,35 +6754,35 @@
       </c>
       <c r="K14" t="str">
         <f t="shared" si="4"/>
-        <v>0000 A980</v>
+        <v>0001 4560</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="5"/>
-        <v>002F 081B</v>
+        <v>002E A61B</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="6"/>
-        <v>0030 901B</v>
+        <v>002F 081B</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="45" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>222</v>
+        <v>195</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>173</v>
+        <v>214</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="1"/>
@@ -6813,35 +6798,35 @@
       </c>
       <c r="K15" t="str">
         <f t="shared" si="4"/>
-        <v>0000 B180</v>
+        <v>0001 55E0</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="5"/>
-        <v>0030 901B</v>
+        <v>002E A61B</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="6"/>
-        <v>0032 181B</v>
+        <v>0030 901B</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="47" t="s">
-        <v>219</v>
+        <v>192</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>224</v>
+        <v>197</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="1"/>
@@ -6861,31 +6846,31 @@
       </c>
       <c r="L16" t="str">
         <f t="shared" si="5"/>
-        <v>0032 181B</v>
+        <v>0030 901B</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="6"/>
-        <v>0032 DC1B</v>
+        <v>0032 181B</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="45" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>104</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>225</v>
+        <v>198</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>177</v>
+        <v>215</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="1"/>
@@ -6901,35 +6886,35 @@
       </c>
       <c r="K17" t="str">
         <f t="shared" si="4"/>
-        <v>0000 F980</v>
+        <v>0001 E660</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="5"/>
-        <v>0032 DC1B</v>
+        <v>0032 181B</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="6"/>
-        <v>0033 00DB</v>
+        <v>0032 DC1B</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="45" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>225</v>
+        <v>198</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>181</v>
+        <v>216</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="1"/>
@@ -6945,35 +6930,35 @@
       </c>
       <c r="K18" t="str">
         <f t="shared" si="4"/>
-        <v>0001 1180</v>
+        <v>0002 1690</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="5"/>
-        <v>0033 00DB</v>
+        <v>0032 DC1B</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" si="6"/>
-        <v>0033 93DB</v>
+        <v>0033 00DB</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="45" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>224</v>
+        <v>197</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>184</v>
+        <v>217</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="1"/>
@@ -6989,35 +6974,35 @@
       </c>
       <c r="K19" t="str">
         <f t="shared" si="4"/>
-        <v>0001 2380</v>
+        <v>0002 3B50</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" si="5"/>
-        <v>0033 93DB</v>
+        <v>0032 DC1B</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="6"/>
-        <v>0034 26DB</v>
+        <v>0033 93DB</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="45" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>105</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>225</v>
+        <v>198</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>187</v>
+        <v>218</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="1"/>
@@ -7033,35 +7018,35 @@
       </c>
       <c r="K20" t="str">
         <f t="shared" si="4"/>
-        <v>0001 C580</v>
+        <v>0003 8010</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="5"/>
-        <v>0034 26DB</v>
+        <v>0033 93DB</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="6"/>
-        <v>0034 4B9B</v>
+        <v>0034 26DB</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="45" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>225</v>
+        <v>198</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="1"/>
@@ -7077,35 +7062,35 @@
       </c>
       <c r="K21" t="str">
         <f t="shared" si="4"/>
-        <v>0001 E980</v>
+        <v>0003 C840</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" si="5"/>
-        <v>0034 4B9B</v>
+        <v>0034 26DB</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="6"/>
-        <v>0034 DE9B</v>
+        <v>0034 4B9B</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="45" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>224</v>
+        <v>197</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>191</v>
+        <v>220</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="1"/>
@@ -7121,35 +7106,35 @@
       </c>
       <c r="K22" t="str">
         <f t="shared" si="4"/>
-        <v>0001 FB80</v>
+        <v>0003 ED00</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" si="5"/>
-        <v>0034 DE9B</v>
+        <v>0034 26DB</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="6"/>
-        <v>0035 719B</v>
+        <v>0034 DE9B</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="45" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>106</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>225</v>
+        <v>198</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>194</v>
+        <v>221</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="1"/>
@@ -7165,35 +7150,35 @@
       </c>
       <c r="K23" t="str">
         <f t="shared" si="4"/>
-        <v>0002 9D80</v>
+        <v>0005 31C0</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" si="5"/>
-        <v>0035 719B</v>
+        <v>0034 DE9B</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" si="6"/>
-        <v>0035 A29B</v>
+        <v>0035 719B</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="45" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>107</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>225</v>
+        <v>198</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>197</v>
+        <v>222</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>198</v>
+        <v>175</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="1"/>
@@ -7209,35 +7194,35 @@
       </c>
       <c r="K24" t="str">
         <f t="shared" si="4"/>
-        <v>0002 CD80</v>
+        <v>0005 9200</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" si="5"/>
-        <v>0035 A29B</v>
+        <v>0035 719B</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" si="6"/>
-        <v>0036 669B</v>
+        <v>0035 A29B</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="45" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>107</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>224</v>
+        <v>197</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>200</v>
+        <v>223</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>198</v>
+        <v>173</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="1"/>
@@ -7253,35 +7238,35 @@
       </c>
       <c r="K25" t="str">
         <f t="shared" si="4"/>
-        <v>0002 ED80</v>
+        <v>0005 D300</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" si="5"/>
-        <v>0036 669B</v>
+        <v>0035 719B</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" si="6"/>
-        <v>0037 2A9B</v>
+        <v>0036 669B</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="45" t="s">
-        <v>202</v>
+        <v>180</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>108</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>225</v>
+        <v>198</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>203</v>
+        <v>224</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>204</v>
+        <v>179</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="1"/>
@@ -7297,35 +7282,35 @@
       </c>
       <c r="K26" t="str">
         <f t="shared" si="4"/>
-        <v>0004 0D80</v>
+        <v>0008 1400</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" si="5"/>
-        <v>0037 2A9B</v>
+        <v>0036 669B</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" si="6"/>
-        <v>0037 5B9B</v>
+        <v>0037 2A9B</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="45" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>107</v>
       </c>
       <c r="C27" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="D27" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="D27" s="12" t="s">
-        <v>205</v>
-      </c>
       <c r="E27" s="12" t="s">
-        <v>204</v>
+        <v>179</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="1"/>
@@ -7341,35 +7326,35 @@
       </c>
       <c r="K27" t="str">
         <f t="shared" si="4"/>
-        <v>0004 4D80</v>
+        <v>0008 9440</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" si="5"/>
-        <v>0037 5B9B</v>
+        <v>0037 2A9B</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" si="6"/>
-        <v>0038 1F9B</v>
+        <v>0037 5B9B</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="45" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>107</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>224</v>
+        <v>197</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>207</v>
+        <v>226</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>206</v>
+        <v>179</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>208</v>
+        <v>182</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="1"/>
@@ -7385,35 +7370,35 @@
       </c>
       <c r="K28" t="str">
         <f t="shared" si="4"/>
-        <v>0004 6D80</v>
+        <v>0008 D540</v>
       </c>
       <c r="L28" t="str">
         <f t="shared" si="5"/>
-        <v>0038 1F9B</v>
+        <v>0037 2A9B</v>
       </c>
       <c r="M28" t="str">
         <f t="shared" si="6"/>
-        <v>0038 E39B</v>
+        <v>0038 1F9B</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="45" t="s">
-        <v>209</v>
+        <v>184</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>225</v>
+        <v>198</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>208</v>
+        <v>182</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>212</v>
+        <v>183</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="1"/>
@@ -7429,35 +7414,35 @@
       </c>
       <c r="K29" t="str">
         <f t="shared" si="4"/>
-        <v>0005 8D80</v>
+        <v>000B 1640</v>
       </c>
       <c r="L29" t="str">
         <f t="shared" si="5"/>
-        <v>0038 E39B</v>
+        <v>0038 1F9B</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" si="6"/>
-        <v>003B E13B</v>
+        <v>0038 E39B</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="47" t="s">
-        <v>226</v>
+        <v>199</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>213</v>
+        <v>187</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>227</v>
+        <v>200</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>212</v>
+        <v>183</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="1"/>
@@ -7477,11 +7462,11 @@
       </c>
       <c r="L30" t="str">
         <f t="shared" si="5"/>
-        <v>003B E13B</v>
+        <v>0038 E39B</v>
       </c>
       <c r="M30" t="str">
         <f t="shared" si="6"/>
-        <v>003B E523</v>
+        <v>003B E13B</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update side in commands and remove kernel size for IMG2COL conv
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7657A6C0-5B99-4259-BDC6-6CA98DA00C81}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B2FF0A-75F6-4546-9799-094F2568F573}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
   <sheets>
     <sheet name="SqueezeNet v2 MEC Parallel Ch" sheetId="2" r:id="rId1"/>
@@ -325,9 +325,6 @@
     <t>wgt staddr</t>
   </si>
   <si>
-    <t>oichsize</t>
-  </si>
-  <si>
     <t>0040_0003</t>
   </si>
   <si>
@@ -607,33 +604,9 @@
     <t>14x14</t>
   </si>
   <si>
-    <t>osurf, oiknsize</t>
-  </si>
-  <si>
-    <t>31E1_7103</t>
-  </si>
-  <si>
     <t>00009_204</t>
   </si>
   <si>
-    <t>0C40_3803</t>
-  </si>
-  <si>
-    <t>0C40_3801</t>
-  </si>
-  <si>
-    <t>0310_1C03</t>
-  </si>
-  <si>
-    <t>0310_1C01</t>
-  </si>
-  <si>
-    <t>00C4_0E03</t>
-  </si>
-  <si>
-    <t>00C4_0E01</t>
-  </si>
-  <si>
     <t>000C4_105</t>
   </si>
   <si>
@@ -719,6 +692,33 @@
   </si>
   <si>
     <t>000B1640</t>
+  </si>
+  <si>
+    <t>osurf, oiside</t>
+  </si>
+  <si>
+    <t>oichannel</t>
+  </si>
+  <si>
+    <t>31E1_71E3</t>
+  </si>
+  <si>
+    <t>0C40_3871</t>
+  </si>
+  <si>
+    <t>0C40_3838</t>
+  </si>
+  <si>
+    <t>0310_1C38</t>
+  </si>
+  <si>
+    <t>0310_1C1C</t>
+  </si>
+  <si>
+    <t>00C4_0E1C</t>
+  </si>
+  <si>
+    <t>00C4_0E0E</t>
   </si>
 </sst>
 </file>
@@ -1347,44 +1347,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80B23C6-EAEB-43B1-B045-456C36085CFA}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AD71"/>
   <sheetViews>
-    <sheetView topLeftCell="G10" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y4" activeCellId="3" sqref="Q4:S68 U4:U68 W4:W68 Y4:Y68"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="30" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.85546875" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="8.7109375" style="30"/>
-    <col min="10" max="10" width="10.85546875" style="30" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.85546875" style="30" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" style="30"/>
-    <col min="13" max="13" width="10.85546875" style="30" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" style="30" customWidth="1"/>
-    <col min="15" max="15" width="7.85546875" style="30" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="27.140625" style="49" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" style="31" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.140625" style="37" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.85546875" style="31" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.85546875" style="37" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.85546875" style="31" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.85546875" style="37" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.85546875" style="43" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1796875" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" style="30" customWidth="1"/>
+    <col min="3" max="3" width="7.81640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.81640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.81640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="8.7265625" style="30"/>
+    <col min="10" max="10" width="10.81640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.81640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7265625" style="30"/>
+    <col min="13" max="13" width="10.81640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.81640625" style="30" customWidth="1"/>
+    <col min="15" max="15" width="7.81640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.26953125" style="30" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.1796875" style="49" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.81640625" style="31" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.1796875" style="31" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.1796875" style="37" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.81640625" style="31" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.81640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.81640625" style="31" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.81640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.81640625" style="43" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A1" s="21"/>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -1399,7 +1396,7 @@
       <c r="H1" s="22"/>
       <c r="I1" s="22"/>
       <c r="J1" s="52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K1" s="52"/>
       <c r="L1" s="52"/>
@@ -1419,13 +1416,13 @@
       <c r="X1" s="56"/>
       <c r="Y1" s="57"/>
       <c r="Z1" s="50" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AA1" s="51"/>
       <c r="AB1" s="51"/>
       <c r="AC1" s="51"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
@@ -1433,7 +1430,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D2" s="52" t="s">
         <v>77</v>
@@ -1460,22 +1457,22 @@
         <v>91</v>
       </c>
       <c r="N2" s="24" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="O2" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P2" s="40" t="s">
         <v>85</v>
       </c>
       <c r="Q2" s="41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="R2" s="42" t="s">
-        <v>96</v>
+        <v>220</v>
       </c>
       <c r="S2" s="18" t="s">
-        <v>190</v>
+        <v>219</v>
       </c>
       <c r="T2" s="58" t="s">
         <v>95</v>
@@ -1486,26 +1483,26 @@
       </c>
       <c r="W2" s="58"/>
       <c r="X2" s="58" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="Y2" s="59"/>
       <c r="Z2" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AA2" s="20" t="s">
         <v>89</v>
       </c>
       <c r="AB2" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC2" s="20" t="s">
         <v>111</v>
-      </c>
-      <c r="AC2" s="20" t="s">
-        <v>112</v>
       </c>
       <c r="AD2" s="20" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1522,7 +1519,7 @@
       <c r="H3" s="25"/>
       <c r="I3" s="25"/>
       <c r="J3" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K3" s="25">
         <v>227</v>
@@ -1555,7 +1552,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -1584,7 +1581,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K4" s="26">
         <v>113</v>
@@ -1618,8 +1615,8 @@
         <v>0040_0003</v>
       </c>
       <c r="S4" s="12" t="str">
-        <f>DEC2HEX(K4^2,4)&amp;"_"&amp;DEC2HEX(K4,2)&amp;DEC2HEX(E4,2)</f>
-        <v>31E1_7103</v>
+        <f>DEC2HEX(K4^2,4)&amp;"_"&amp;DEC2HEX(K4,2)&amp;DEC2HEX(K3,2)</f>
+        <v>31E1_71E3</v>
       </c>
       <c r="T4" s="33">
         <v>4096</v>
@@ -1659,7 +1656,7 @@
       </c>
       <c r="AD4" s="20"/>
     </row>
-    <row r="5" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
@@ -1695,7 +1692,7 @@
       <c r="AC5" s="3"/>
       <c r="AD5" s="20"/>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
@@ -1724,7 +1721,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K6" s="28">
         <v>56</v>
@@ -1749,8 +1746,8 @@
         <v>0040_0040</v>
       </c>
       <c r="S6" s="16" t="str">
-        <f>DEC2HEX(K6^2,4)&amp;"_"&amp;DEC2HEX(K6,2)&amp;DEC2HEX(E6,2)</f>
-        <v>0C40_3803</v>
+        <f>DEC2HEX(K6^2,4)&amp;"_"&amp;DEC2HEX(K6,2)&amp;DEC2HEX(K4,2)</f>
+        <v>0C40_3871</v>
       </c>
       <c r="T6" s="35"/>
       <c r="U6" s="16" t="str">
@@ -1789,7 +1786,7 @@
       </c>
       <c r="AD6" s="20"/>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1818,7 +1815,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K7" s="26">
         <v>56</v>
@@ -1852,8 +1849,8 @@
         <v>0010_0040</v>
       </c>
       <c r="S7" s="12" t="str">
-        <f>DEC2HEX(K7^2,4)&amp;"_"&amp;DEC2HEX(K7,2)&amp;DEC2HEX(E7,2)</f>
-        <v>0C40_3801</v>
+        <f>DEC2HEX(K7^2,4)&amp;"_"&amp;DEC2HEX(K7,2)&amp;DEC2HEX(K6,2)</f>
+        <v>0C40_3838</v>
       </c>
       <c r="T7" s="33">
         <f>T4+P4</f>
@@ -1895,7 +1892,7 @@
       </c>
       <c r="AD7" s="20"/>
     </row>
-    <row r="8" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
@@ -1931,7 +1928,7 @@
       <c r="AC8" s="3"/>
       <c r="AD8" s="20"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -1960,7 +1957,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K9" s="26">
         <v>56</v>
@@ -1994,15 +1991,15 @@
         <v>0040_0010</v>
       </c>
       <c r="S9" s="12" t="str">
-        <f t="shared" ref="S9:S10" si="5">DEC2HEX(K9^2,4)&amp;"_"&amp;DEC2HEX(K9,2)&amp;DEC2HEX(E9,2)</f>
-        <v>0C40_3801</v>
+        <f>DEC2HEX(K9^2,4)&amp;"_"&amp;DEC2HEX(K9,2)&amp;DEC2HEX(K7,2)</f>
+        <v>0C40_3838</v>
       </c>
       <c r="T9" s="33">
         <f>T7+P7</f>
         <v>6928</v>
       </c>
       <c r="U9" s="12" t="str">
-        <f t="shared" ref="U9:U10" si="6">DEC2HEX(T9,8)</f>
+        <f t="shared" ref="U9:U10" si="5">DEC2HEX(T9,8)</f>
         <v>00001B10</v>
       </c>
       <c r="V9" s="33">
@@ -2010,7 +2007,7 @@
         <v>1827867</v>
       </c>
       <c r="W9" s="12" t="str">
-        <f t="shared" ref="W9:W10" si="7">DEC2HEX(V9,8)</f>
+        <f t="shared" ref="W9:W10" si="6">DEC2HEX(V9,8)</f>
         <v>001BE41B</v>
       </c>
       <c r="X9" s="33">
@@ -2018,7 +2015,7 @@
         <v>1878043</v>
       </c>
       <c r="Y9" s="13" t="str">
-        <f t="shared" ref="Y9:Y10" si="8">DEC2HEX(X9,8)</f>
+        <f t="shared" ref="Y9:Y10" si="7">DEC2HEX(X9,8)</f>
         <v>001CA81B</v>
       </c>
       <c r="Z9" s="2">
@@ -2037,7 +2034,7 @@
       </c>
       <c r="AD9" s="20"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -2066,7 +2063,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K10" s="26">
         <v>56</v>
@@ -2100,15 +2097,15 @@
         <v>0040_0010</v>
       </c>
       <c r="S10" s="12" t="str">
-        <f t="shared" si="5"/>
-        <v>0C40_3803</v>
+        <f>DEC2HEX(K10^2,4)&amp;"_"&amp;DEC2HEX(K10,2)&amp;DEC2HEX(K7,2)</f>
+        <v>0C40_3838</v>
       </c>
       <c r="T10" s="33">
         <f>T9+P9</f>
         <v>8016</v>
       </c>
       <c r="U10" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>00001F50</v>
       </c>
       <c r="V10" s="33">
@@ -2116,7 +2113,7 @@
         <v>1827867</v>
       </c>
       <c r="W10" s="12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>001BE41B</v>
       </c>
       <c r="X10" s="33">
@@ -2124,7 +2121,7 @@
         <v>2078747</v>
       </c>
       <c r="Y10" s="13" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>001FB81B</v>
       </c>
       <c r="Z10" s="2">
@@ -2143,7 +2140,7 @@
       </c>
       <c r="AD10" s="20"/>
     </row>
-    <row r="11" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
@@ -2179,7 +2176,7 @@
       <c r="AC11" s="3"/>
       <c r="AD11" s="20"/>
     </row>
-    <row r="12" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>12</v>
       </c>
@@ -2215,7 +2212,7 @@
       <c r="AC12" s="3"/>
       <c r="AD12" s="20"/>
     </row>
-    <row r="13" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>19</v>
       </c>
@@ -2230,7 +2227,7 @@
       <c r="H13" s="25"/>
       <c r="I13" s="25"/>
       <c r="J13" s="25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K13" s="25">
         <v>56</v>
@@ -2255,7 +2252,7 @@
       <c r="AC13" s="1"/>
       <c r="AD13" s="20"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>13</v>
       </c>
@@ -2284,7 +2281,7 @@
         <v>0</v>
       </c>
       <c r="J14" s="26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K14" s="26">
         <v>56</v>
@@ -2318,8 +2315,8 @@
         <v>0010_0080</v>
       </c>
       <c r="S14" s="12" t="str">
-        <f>DEC2HEX(K14^2,4)&amp;"_"&amp;DEC2HEX(K14,2)&amp;DEC2HEX(E14,2)</f>
-        <v>0C40_3801</v>
+        <f>DEC2HEX(K14^2,4)&amp;"_"&amp;DEC2HEX(K14,2)&amp;DEC2HEX(K9,2)</f>
+        <v>0C40_3838</v>
       </c>
       <c r="T14" s="33">
         <f>T10+P10</f>
@@ -2361,7 +2358,7 @@
       </c>
       <c r="AD14" s="20"/>
     </row>
-    <row r="15" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>14</v>
       </c>
@@ -2397,7 +2394,7 @@
       <c r="AC15" s="3"/>
       <c r="AD15" s="20"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
@@ -2426,29 +2423,29 @@
         <v>0</v>
       </c>
       <c r="J16" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K16" s="26">
         <v>56</v>
       </c>
       <c r="L16" s="26">
-        <f t="shared" ref="L16:L17" si="9">K16^2*G16</f>
+        <f t="shared" ref="L16:L17" si="8">K16^2*G16</f>
         <v>200704</v>
       </c>
       <c r="M16" s="26">
-        <f t="shared" ref="M16:M17" si="10">K16^2*F16</f>
+        <f t="shared" ref="M16:M17" si="9">K16^2*F16</f>
         <v>50176</v>
       </c>
       <c r="N16" s="26">
-        <f t="shared" ref="N16:N17" si="11">E16^2*F16*G16</f>
+        <f t="shared" ref="N16:N17" si="10">E16^2*F16*G16</f>
         <v>1024</v>
       </c>
       <c r="O16" s="26">
-        <f t="shared" ref="O16:O17" si="12">G16</f>
+        <f t="shared" ref="O16:O17" si="11">G16</f>
         <v>64</v>
       </c>
       <c r="P16" s="26">
-        <f t="shared" ref="P16:P17" si="13">N16+O16</f>
+        <f t="shared" ref="P16:P17" si="12">N16+O16</f>
         <v>1088</v>
       </c>
       <c r="Q16" s="45" t="str">
@@ -2460,15 +2457,15 @@
         <v>0040_0010</v>
       </c>
       <c r="S16" s="12" t="str">
-        <f t="shared" ref="S16:S17" si="14">DEC2HEX(K16^2,4)&amp;"_"&amp;DEC2HEX(K16,2)&amp;DEC2HEX(E16,2)</f>
-        <v>0C40_3801</v>
+        <f>DEC2HEX(K16^2,4)&amp;"_"&amp;DEC2HEX(K16,2)&amp;DEC2HEX(K14,2)</f>
+        <v>0C40_3838</v>
       </c>
       <c r="T16" s="33">
         <f>T14+P14</f>
         <v>19360</v>
       </c>
       <c r="U16" s="12" t="str">
-        <f t="shared" ref="U16:U17" si="15">DEC2HEX(T16,8)</f>
+        <f t="shared" ref="U16:U17" si="13">DEC2HEX(T16,8)</f>
         <v>00004BA0</v>
       </c>
       <c r="V16" s="33">
@@ -2476,7 +2473,7 @@
         <v>2279451</v>
       </c>
       <c r="W16" s="12" t="str">
-        <f t="shared" ref="W16:W17" si="16">DEC2HEX(V16,8)</f>
+        <f t="shared" ref="W16:W17" si="14">DEC2HEX(V16,8)</f>
         <v>0022C81B</v>
       </c>
       <c r="X16" s="33">
@@ -2484,7 +2481,7 @@
         <v>2329627</v>
       </c>
       <c r="Y16" s="13" t="str">
-        <f t="shared" ref="Y16:Y17" si="17">DEC2HEX(X16,8)</f>
+        <f t="shared" ref="Y16:Y17" si="15">DEC2HEX(X16,8)</f>
         <v>00238C1B</v>
       </c>
       <c r="Z16" s="2">
@@ -2503,7 +2500,7 @@
       </c>
       <c r="AD16" s="20"/>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
@@ -2532,29 +2529,29 @@
         <v>1</v>
       </c>
       <c r="J17" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K17" s="26">
         <v>56</v>
       </c>
       <c r="L17" s="26">
+        <f t="shared" si="8"/>
+        <v>200704</v>
+      </c>
+      <c r="M17" s="26">
         <f t="shared" si="9"/>
-        <v>200704</v>
-      </c>
-      <c r="M17" s="26">
+        <v>50176</v>
+      </c>
+      <c r="N17" s="26">
         <f t="shared" si="10"/>
-        <v>50176</v>
-      </c>
-      <c r="N17" s="26">
+        <v>9216</v>
+      </c>
+      <c r="O17" s="26">
         <f t="shared" si="11"/>
-        <v>9216</v>
-      </c>
-      <c r="O17" s="26">
+        <v>64</v>
+      </c>
+      <c r="P17" s="26">
         <f t="shared" si="12"/>
-        <v>64</v>
-      </c>
-      <c r="P17" s="26">
-        <f t="shared" si="13"/>
         <v>9280</v>
       </c>
       <c r="Q17" s="45" t="str">
@@ -2566,15 +2563,15 @@
         <v>0040_0010</v>
       </c>
       <c r="S17" s="12" t="str">
-        <f t="shared" si="14"/>
-        <v>0C40_3803</v>
+        <f>DEC2HEX(K17^2,4)&amp;"_"&amp;DEC2HEX(K17,2)&amp;DEC2HEX(K14,2)</f>
+        <v>0C40_3838</v>
       </c>
       <c r="T17" s="33">
         <f>T16+P16</f>
         <v>20448</v>
       </c>
       <c r="U17" s="12" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>00004FE0</v>
       </c>
       <c r="V17" s="33">
@@ -2582,7 +2579,7 @@
         <v>2279451</v>
       </c>
       <c r="W17" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0022C81B</v>
       </c>
       <c r="X17" s="33">
@@ -2590,7 +2587,7 @@
         <v>2530331</v>
       </c>
       <c r="Y17" s="13" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>00269C1B</v>
       </c>
       <c r="Z17" s="2">
@@ -2609,7 +2606,7 @@
       </c>
       <c r="AD17" s="20"/>
     </row>
-    <row r="18" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>17</v>
       </c>
@@ -2645,7 +2642,7 @@
       <c r="AC18" s="3"/>
       <c r="AD18" s="20"/>
     </row>
-    <row r="19" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>18</v>
       </c>
@@ -2681,7 +2678,7 @@
       <c r="AC19" s="3"/>
       <c r="AD19" s="20"/>
     </row>
-    <row r="20" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>20</v>
       </c>
@@ -2696,7 +2693,7 @@
       <c r="H20" s="25"/>
       <c r="I20" s="25"/>
       <c r="J20" s="25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K20" s="25">
         <v>56</v>
@@ -2721,7 +2718,7 @@
       <c r="AC20" s="1"/>
       <c r="AD20" s="20"/>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
         <v>21</v>
       </c>
@@ -2775,8 +2772,8 @@
         <v>0080_0080</v>
       </c>
       <c r="S21" s="16" t="str">
-        <f>DEC2HEX(K21^2,4)&amp;"_"&amp;DEC2HEX(K21,2)&amp;DEC2HEX(E21,2)</f>
-        <v>0310_1C03</v>
+        <f>DEC2HEX(K21^2,4)&amp;"_"&amp;DEC2HEX(K21,2)&amp;DEC2HEX(K16,2)</f>
+        <v>0310_1C38</v>
       </c>
       <c r="T21" s="35"/>
       <c r="U21" s="16" t="str">
@@ -2815,7 +2812,7 @@
       </c>
       <c r="AD21" s="20"/>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
@@ -2844,7 +2841,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K22" s="26">
         <v>28</v>
@@ -2878,8 +2875,8 @@
         <v>0020_0080</v>
       </c>
       <c r="S22" s="12" t="str">
-        <f>DEC2HEX(K22^2,4)&amp;"_"&amp;DEC2HEX(K22,2)&amp;DEC2HEX(E22,2)</f>
-        <v>0310_1C01</v>
+        <f>DEC2HEX(K22^2,4)&amp;"_"&amp;DEC2HEX(K22,2)&amp;DEC2HEX(K21,2)</f>
+        <v>0310_1C1C</v>
       </c>
       <c r="T22" s="33">
         <f>T17+P17</f>
@@ -2921,7 +2918,7 @@
       </c>
       <c r="AD22" s="20"/>
     </row>
-    <row r="23" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>23</v>
       </c>
@@ -2957,7 +2954,7 @@
       <c r="AC23" s="3"/>
       <c r="AD23" s="20"/>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>24</v>
       </c>
@@ -2986,29 +2983,29 @@
         <v>0</v>
       </c>
       <c r="J24" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K24" s="26">
         <v>28</v>
       </c>
       <c r="L24" s="26">
-        <f t="shared" ref="L24:L25" si="18">K24^2*G24</f>
+        <f t="shared" ref="L24:L25" si="16">K24^2*G24</f>
         <v>100352</v>
       </c>
       <c r="M24" s="26">
-        <f t="shared" ref="M24:M25" si="19">K24^2*F24</f>
+        <f t="shared" ref="M24:M25" si="17">K24^2*F24</f>
         <v>25088</v>
       </c>
       <c r="N24" s="26">
-        <f t="shared" ref="N24:N25" si="20">E24^2*F24*G24</f>
+        <f t="shared" ref="N24:N25" si="18">E24^2*F24*G24</f>
         <v>4096</v>
       </c>
       <c r="O24" s="26">
-        <f t="shared" ref="O24:O25" si="21">G24</f>
+        <f t="shared" ref="O24:O25" si="19">G24</f>
         <v>128</v>
       </c>
       <c r="P24" s="26">
-        <f t="shared" ref="P24:P25" si="22">N24+O24</f>
+        <f t="shared" ref="P24:P25" si="20">N24+O24</f>
         <v>4224</v>
       </c>
       <c r="Q24" s="45" t="str">
@@ -3020,15 +3017,15 @@
         <v>0080_0020</v>
       </c>
       <c r="S24" s="12" t="str">
-        <f t="shared" ref="S24:S25" si="23">DEC2HEX(K24^2,4)&amp;"_"&amp;DEC2HEX(K24,2)&amp;DEC2HEX(E24,2)</f>
-        <v>0310_1C01</v>
+        <f>DEC2HEX(K24^2,4)&amp;"_"&amp;DEC2HEX(K24,2)&amp;DEC2HEX(K22,2)</f>
+        <v>0310_1C1C</v>
       </c>
       <c r="T24" s="33">
         <f>T22+P22</f>
         <v>33856</v>
       </c>
       <c r="U24" s="12" t="str">
-        <f t="shared" ref="U24:U25" si="24">DEC2HEX(T24,8)</f>
+        <f t="shared" ref="U24:U25" si="21">DEC2HEX(T24,8)</f>
         <v>00008440</v>
       </c>
       <c r="V24" s="33">
@@ -3036,7 +3033,7 @@
         <v>2831387</v>
       </c>
       <c r="W24" s="12" t="str">
-        <f t="shared" ref="W24:W25" si="25">DEC2HEX(V24,8)</f>
+        <f t="shared" ref="W24:W25" si="22">DEC2HEX(V24,8)</f>
         <v>002B341B</v>
       </c>
       <c r="X24" s="33">
@@ -3044,7 +3041,7 @@
         <v>2856475</v>
       </c>
       <c r="Y24" s="13" t="str">
-        <f t="shared" ref="Y24:Y25" si="26">DEC2HEX(X24,8)</f>
+        <f t="shared" ref="Y24:Y25" si="23">DEC2HEX(X24,8)</f>
         <v>002B961B</v>
       </c>
       <c r="Z24" s="2">
@@ -3063,7 +3060,7 @@
       </c>
       <c r="AD24" s="20"/>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>25</v>
       </c>
@@ -3092,29 +3089,29 @@
         <v>1</v>
       </c>
       <c r="J25" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K25" s="26">
         <v>28</v>
       </c>
       <c r="L25" s="26">
+        <f t="shared" si="16"/>
+        <v>100352</v>
+      </c>
+      <c r="M25" s="26">
+        <f t="shared" si="17"/>
+        <v>25088</v>
+      </c>
+      <c r="N25" s="26">
         <f t="shared" si="18"/>
-        <v>100352</v>
-      </c>
-      <c r="M25" s="26">
+        <v>36864</v>
+      </c>
+      <c r="O25" s="26">
         <f t="shared" si="19"/>
-        <v>25088</v>
-      </c>
-      <c r="N25" s="26">
+        <v>128</v>
+      </c>
+      <c r="P25" s="26">
         <f t="shared" si="20"/>
-        <v>36864</v>
-      </c>
-      <c r="O25" s="26">
-        <f t="shared" si="21"/>
-        <v>128</v>
-      </c>
-      <c r="P25" s="26">
-        <f t="shared" si="22"/>
         <v>36992</v>
       </c>
       <c r="Q25" s="45" t="str">
@@ -3126,15 +3123,15 @@
         <v>0080_0020</v>
       </c>
       <c r="S25" s="12" t="str">
-        <f t="shared" si="23"/>
-        <v>0310_1C03</v>
+        <f>DEC2HEX(K25^2,4)&amp;"_"&amp;DEC2HEX(K25,2)&amp;DEC2HEX(K22,2)</f>
+        <v>0310_1C1C</v>
       </c>
       <c r="T25" s="33">
         <f>T24+P24</f>
         <v>38080</v>
       </c>
       <c r="U25" s="12" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>000094C0</v>
       </c>
       <c r="V25" s="33">
@@ -3142,7 +3139,7 @@
         <v>2831387</v>
       </c>
       <c r="W25" s="12" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v>002B341B</v>
       </c>
       <c r="X25" s="33">
@@ -3150,7 +3147,7 @@
         <v>2956827</v>
       </c>
       <c r="Y25" s="13" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>002D1E1B</v>
       </c>
       <c r="Z25" s="2">
@@ -3169,7 +3166,7 @@
       </c>
       <c r="AD25" s="20"/>
     </row>
-    <row r="26" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>26</v>
       </c>
@@ -3205,7 +3202,7 @@
       <c r="AC26" s="3"/>
       <c r="AD26" s="20"/>
     </row>
-    <row r="27" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>27</v>
       </c>
@@ -3241,7 +3238,7 @@
       <c r="AC27" s="3"/>
       <c r="AD27" s="20"/>
     </row>
-    <row r="28" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>28</v>
       </c>
@@ -3256,7 +3253,7 @@
       <c r="H28" s="25"/>
       <c r="I28" s="25"/>
       <c r="J28" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K28" s="25">
         <v>28</v>
@@ -3281,7 +3278,7 @@
       <c r="AC28" s="1"/>
       <c r="AD28" s="20"/>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
         <v>29</v>
       </c>
@@ -3310,7 +3307,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K29" s="26">
         <v>28</v>
@@ -3344,8 +3341,8 @@
         <v>0020_0100</v>
       </c>
       <c r="S29" s="12" t="str">
-        <f>DEC2HEX(K29^2,4)&amp;"_"&amp;DEC2HEX(K29,2)&amp;DEC2HEX(E29,2)</f>
-        <v>0310_1C01</v>
+        <f>DEC2HEX(K29^2,4)&amp;"_"&amp;DEC2HEX(K29,2)&amp;DEC2HEX(K24,2)</f>
+        <v>0310_1C1C</v>
       </c>
       <c r="T29" s="33">
         <f>T25+P25</f>
@@ -3387,7 +3384,7 @@
       </c>
       <c r="AD29" s="20"/>
     </row>
-    <row r="30" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>30</v>
       </c>
@@ -3423,7 +3420,7 @@
       <c r="AC30" s="3"/>
       <c r="AD30" s="20"/>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
         <v>31</v>
       </c>
@@ -3452,29 +3449,29 @@
         <v>0</v>
       </c>
       <c r="J31" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K31" s="26">
         <v>28</v>
       </c>
       <c r="L31" s="26">
-        <f t="shared" ref="L31:L32" si="27">K31^2*G31</f>
+        <f t="shared" ref="L31:L32" si="24">K31^2*G31</f>
         <v>100352</v>
       </c>
       <c r="M31" s="26">
-        <f t="shared" ref="M31:M32" si="28">K31^2*F31</f>
+        <f t="shared" ref="M31:M32" si="25">K31^2*F31</f>
         <v>25088</v>
       </c>
       <c r="N31" s="26">
-        <f t="shared" ref="N31:N32" si="29">E31^2*F31*G31</f>
+        <f t="shared" ref="N31:N32" si="26">E31^2*F31*G31</f>
         <v>4096</v>
       </c>
       <c r="O31" s="26">
-        <f t="shared" ref="O31:O32" si="30">G31</f>
+        <f t="shared" ref="O31:O32" si="27">G31</f>
         <v>128</v>
       </c>
       <c r="P31" s="26">
-        <f t="shared" ref="P31:P32" si="31">N31+O31</f>
+        <f t="shared" ref="P31:P32" si="28">N31+O31</f>
         <v>4224</v>
       </c>
       <c r="Q31" s="45" t="str">
@@ -3486,15 +3483,15 @@
         <v>0080_0020</v>
       </c>
       <c r="S31" s="12" t="str">
-        <f t="shared" ref="S31:S32" si="32">DEC2HEX(K31^2,4)&amp;"_"&amp;DEC2HEX(K31,2)&amp;DEC2HEX(E31,2)</f>
-        <v>0310_1C01</v>
+        <f>DEC2HEX(K31^2,4)&amp;"_"&amp;DEC2HEX(K31,2)&amp;DEC2HEX(K29,2)</f>
+        <v>0310_1C1C</v>
       </c>
       <c r="T31" s="33">
         <f>T29+P29</f>
         <v>83296</v>
       </c>
       <c r="U31" s="12" t="str">
-        <f t="shared" ref="U31:U32" si="33">DEC2HEX(T31,8)</f>
+        <f t="shared" ref="U31:U32" si="29">DEC2HEX(T31,8)</f>
         <v>00014560</v>
       </c>
       <c r="V31" s="33">
@@ -3502,7 +3499,7 @@
         <v>3057179</v>
       </c>
       <c r="W31" s="12" t="str">
-        <f t="shared" ref="W31:W32" si="34">DEC2HEX(V31,8)</f>
+        <f t="shared" ref="W31:W32" si="30">DEC2HEX(V31,8)</f>
         <v>002EA61B</v>
       </c>
       <c r="X31" s="33">
@@ -3510,7 +3507,7 @@
         <v>3082267</v>
       </c>
       <c r="Y31" s="13" t="str">
-        <f t="shared" ref="Y31:Y32" si="35">DEC2HEX(X31,8)</f>
+        <f t="shared" ref="Y31:Y32" si="31">DEC2HEX(X31,8)</f>
         <v>002F081B</v>
       </c>
       <c r="Z31" s="2">
@@ -3529,7 +3526,7 @@
       </c>
       <c r="AD31" s="20"/>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
         <v>32</v>
       </c>
@@ -3558,29 +3555,29 @@
         <v>1</v>
       </c>
       <c r="J32" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K32" s="26">
         <v>28</v>
       </c>
       <c r="L32" s="26">
+        <f t="shared" si="24"/>
+        <v>100352</v>
+      </c>
+      <c r="M32" s="26">
+        <f t="shared" si="25"/>
+        <v>25088</v>
+      </c>
+      <c r="N32" s="26">
+        <f t="shared" si="26"/>
+        <v>36864</v>
+      </c>
+      <c r="O32" s="26">
         <f t="shared" si="27"/>
-        <v>100352</v>
-      </c>
-      <c r="M32" s="26">
+        <v>128</v>
+      </c>
+      <c r="P32" s="26">
         <f t="shared" si="28"/>
-        <v>25088</v>
-      </c>
-      <c r="N32" s="26">
-        <f t="shared" si="29"/>
-        <v>36864</v>
-      </c>
-      <c r="O32" s="26">
-        <f t="shared" si="30"/>
-        <v>128</v>
-      </c>
-      <c r="P32" s="26">
-        <f t="shared" si="31"/>
         <v>36992</v>
       </c>
       <c r="Q32" s="45" t="str">
@@ -3592,15 +3589,15 @@
         <v>0080_0020</v>
       </c>
       <c r="S32" s="12" t="str">
-        <f t="shared" si="32"/>
-        <v>0310_1C03</v>
+        <f>DEC2HEX(K32^2,4)&amp;"_"&amp;DEC2HEX(K32,2)&amp;DEC2HEX(K29,2)</f>
+        <v>0310_1C1C</v>
       </c>
       <c r="T32" s="33">
         <f>T31+P31</f>
         <v>87520</v>
       </c>
       <c r="U32" s="12" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="29"/>
         <v>000155E0</v>
       </c>
       <c r="V32" s="33">
@@ -3608,7 +3605,7 @@
         <v>3057179</v>
       </c>
       <c r="W32" s="12" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="30"/>
         <v>002EA61B</v>
       </c>
       <c r="X32" s="33">
@@ -3616,7 +3613,7 @@
         <v>3182619</v>
       </c>
       <c r="Y32" s="13" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="31"/>
         <v>0030901B</v>
       </c>
       <c r="Z32" s="2">
@@ -3635,7 +3632,7 @@
       </c>
       <c r="AD32" s="20"/>
     </row>
-    <row r="33" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>33</v>
       </c>
@@ -3671,7 +3668,7 @@
       <c r="AC33" s="3"/>
       <c r="AD33" s="20"/>
     </row>
-    <row r="34" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
         <v>34</v>
       </c>
@@ -3707,7 +3704,7 @@
       <c r="AC34" s="3"/>
       <c r="AD34" s="20"/>
     </row>
-    <row r="35" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>35</v>
       </c>
@@ -3722,7 +3719,7 @@
       <c r="H35" s="25"/>
       <c r="I35" s="25"/>
       <c r="J35" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K35" s="25"/>
       <c r="L35" s="25"/>
@@ -3745,7 +3742,7 @@
       <c r="AC35" s="1"/>
       <c r="AD35" s="20"/>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A36" s="8" t="s">
         <v>36</v>
       </c>
@@ -3774,7 +3771,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K36" s="28">
         <v>14</v>
@@ -3799,8 +3796,8 @@
         <v>0100_0100</v>
       </c>
       <c r="S36" s="16" t="str">
-        <f>DEC2HEX(K36^2,4)&amp;"_"&amp;DEC2HEX(K36,2)&amp;DEC2HEX(E36,2)</f>
-        <v>00C4_0E03</v>
+        <f>DEC2HEX(K36^2,4)&amp;"_"&amp;DEC2HEX(K36,2)&amp;DEC2HEX(K31,2)</f>
+        <v>00C4_0E1C</v>
       </c>
       <c r="T36" s="35"/>
       <c r="U36" s="16" t="str">
@@ -3839,7 +3836,7 @@
       </c>
       <c r="AD36" s="20"/>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
         <v>37</v>
       </c>
@@ -3868,7 +3865,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K37" s="26">
         <v>14</v>
@@ -3902,8 +3899,8 @@
         <v>0030_0100</v>
       </c>
       <c r="S37" s="12" t="str">
-        <f>DEC2HEX(K37^2,4)&amp;"_"&amp;DEC2HEX(K37,2)&amp;DEC2HEX(E37,2)</f>
-        <v>00C4_0E01</v>
+        <f>DEC2HEX(K37^2,4)&amp;"_"&amp;DEC2HEX(K37,2)&amp;DEC2HEX(K36,2)</f>
+        <v>00C4_0E0E</v>
       </c>
       <c r="T37" s="33">
         <f>T32+P32</f>
@@ -3945,7 +3942,7 @@
       </c>
       <c r="AD37" s="20"/>
     </row>
-    <row r="38" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
         <v>38</v>
       </c>
@@ -3981,7 +3978,7 @@
       <c r="AC38" s="3"/>
       <c r="AD38" s="20"/>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A39" s="6" t="s">
         <v>39</v>
       </c>
@@ -4010,29 +4007,29 @@
         <v>0</v>
       </c>
       <c r="J39" s="26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K39" s="26">
         <v>14</v>
       </c>
       <c r="L39" s="26">
-        <f t="shared" ref="L39:L40" si="36">K39^2*G39</f>
+        <f t="shared" ref="L39:L40" si="32">K39^2*G39</f>
         <v>37632</v>
       </c>
       <c r="M39" s="26">
-        <f t="shared" ref="M39:M40" si="37">K39^2*F39</f>
+        <f t="shared" ref="M39:M40" si="33">K39^2*F39</f>
         <v>9408</v>
       </c>
       <c r="N39" s="26">
-        <f t="shared" ref="N39:N40" si="38">E39^2*F39*G39</f>
+        <f t="shared" ref="N39:N40" si="34">E39^2*F39*G39</f>
         <v>9216</v>
       </c>
       <c r="O39" s="26">
-        <f t="shared" ref="O39:O40" si="39">G39</f>
+        <f t="shared" ref="O39:O40" si="35">G39</f>
         <v>192</v>
       </c>
       <c r="P39" s="26">
-        <f t="shared" ref="P39:P40" si="40">N39+O39</f>
+        <f t="shared" ref="P39:P40" si="36">N39+O39</f>
         <v>9408</v>
       </c>
       <c r="Q39" s="45" t="str">
@@ -4044,15 +4041,15 @@
         <v>00C0_0030</v>
       </c>
       <c r="S39" s="12" t="str">
-        <f t="shared" ref="S39:S40" si="41">DEC2HEX(K39^2,4)&amp;"_"&amp;DEC2HEX(K39,2)&amp;DEC2HEX(E39,2)</f>
-        <v>00C4_0E01</v>
+        <f>DEC2HEX(K39^2,4)&amp;"_"&amp;DEC2HEX(K39,2)&amp;DEC2HEX(K37,2)</f>
+        <v>00C4_0E0E</v>
       </c>
       <c r="T39" s="33">
         <f>T37+P37</f>
         <v>136848</v>
       </c>
       <c r="U39" s="12" t="str">
-        <f t="shared" ref="U39:U40" si="42">DEC2HEX(T39,8)</f>
+        <f t="shared" ref="U39:U40" si="37">DEC2HEX(T39,8)</f>
         <v>00021690</v>
       </c>
       <c r="V39" s="33">
@@ -4060,7 +4057,7 @@
         <v>3333147</v>
       </c>
       <c r="W39" s="12" t="str">
-        <f t="shared" ref="W39:W40" si="43">DEC2HEX(V39,8)</f>
+        <f t="shared" ref="W39:W40" si="38">DEC2HEX(V39,8)</f>
         <v>0032DC1B</v>
       </c>
       <c r="X39" s="33">
@@ -4068,7 +4065,7 @@
         <v>3342555</v>
       </c>
       <c r="Y39" s="13" t="str">
-        <f t="shared" ref="Y39:Y40" si="44">DEC2HEX(X39,8)</f>
+        <f t="shared" ref="Y39:Y40" si="39">DEC2HEX(X39,8)</f>
         <v>003300DB</v>
       </c>
       <c r="Z39" s="2">
@@ -4087,7 +4084,7 @@
       </c>
       <c r="AD39" s="20"/>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A40" s="6" t="s">
         <v>40</v>
       </c>
@@ -4116,29 +4113,29 @@
         <v>1</v>
       </c>
       <c r="J40" s="26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K40" s="26">
         <v>14</v>
       </c>
       <c r="L40" s="26">
+        <f t="shared" si="32"/>
+        <v>37632</v>
+      </c>
+      <c r="M40" s="26">
+        <f t="shared" si="33"/>
+        <v>9408</v>
+      </c>
+      <c r="N40" s="26">
+        <f t="shared" si="34"/>
+        <v>82944</v>
+      </c>
+      <c r="O40" s="26">
+        <f t="shared" si="35"/>
+        <v>192</v>
+      </c>
+      <c r="P40" s="26">
         <f t="shared" si="36"/>
-        <v>37632</v>
-      </c>
-      <c r="M40" s="26">
-        <f t="shared" si="37"/>
-        <v>9408</v>
-      </c>
-      <c r="N40" s="26">
-        <f t="shared" si="38"/>
-        <v>82944</v>
-      </c>
-      <c r="O40" s="26">
-        <f t="shared" si="39"/>
-        <v>192</v>
-      </c>
-      <c r="P40" s="26">
-        <f t="shared" si="40"/>
         <v>83136</v>
       </c>
       <c r="Q40" s="45" t="str">
@@ -4150,15 +4147,15 @@
         <v>00C0_0030</v>
       </c>
       <c r="S40" s="12" t="str">
-        <f t="shared" si="41"/>
-        <v>00C4_0E03</v>
+        <f>DEC2HEX(K40^2,4)&amp;"_"&amp;DEC2HEX(K40,2)&amp;DEC2HEX(K37,2)</f>
+        <v>00C4_0E0E</v>
       </c>
       <c r="T40" s="33">
         <f>T39+P39</f>
         <v>146256</v>
       </c>
       <c r="U40" s="12" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="37"/>
         <v>00023B50</v>
       </c>
       <c r="V40" s="33">
@@ -4166,7 +4163,7 @@
         <v>3333147</v>
       </c>
       <c r="W40" s="12" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="38"/>
         <v>0032DC1B</v>
       </c>
       <c r="X40" s="33">
@@ -4174,7 +4171,7 @@
         <v>3380187</v>
       </c>
       <c r="Y40" s="13" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="39"/>
         <v>003393DB</v>
       </c>
       <c r="Z40" s="2">
@@ -4193,7 +4190,7 @@
       </c>
       <c r="AD40" s="20"/>
     </row>
-    <row r="41" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>41</v>
       </c>
@@ -4229,7 +4226,7 @@
       <c r="AC41" s="3"/>
       <c r="AD41" s="20"/>
     </row>
-    <row r="42" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>42</v>
       </c>
@@ -4265,7 +4262,7 @@
       <c r="AC42" s="3"/>
       <c r="AD42" s="20"/>
     </row>
-    <row r="43" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>43</v>
       </c>
@@ -4280,7 +4277,7 @@
       <c r="H43" s="25"/>
       <c r="I43" s="25"/>
       <c r="J43" s="25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K43" s="25">
         <v>14</v>
@@ -4305,7 +4302,7 @@
       <c r="AC43" s="1"/>
       <c r="AD43" s="20"/>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A44" s="6" t="s">
         <v>44</v>
       </c>
@@ -4334,7 +4331,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K44" s="26">
         <v>14</v>
@@ -4368,8 +4365,8 @@
         <v>0030_0180</v>
       </c>
       <c r="S44" s="12" t="str">
-        <f>DEC2HEX(K44^2,4)&amp;"_"&amp;DEC2HEX(K44,2)&amp;DEC2HEX(E44,2)</f>
-        <v>00C4_0E01</v>
+        <f>DEC2HEX(K44^2,4)&amp;"_"&amp;DEC2HEX(K44,2)&amp;DEC2HEX(K39,2)</f>
+        <v>00C4_0E0E</v>
       </c>
       <c r="T44" s="33">
         <f>T40+P40</f>
@@ -4411,7 +4408,7 @@
       </c>
       <c r="AD44" s="20"/>
     </row>
-    <row r="45" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
         <v>45</v>
       </c>
@@ -4447,7 +4444,7 @@
       <c r="AC45" s="3"/>
       <c r="AD45" s="20"/>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A46" s="6" t="s">
         <v>46</v>
       </c>
@@ -4476,29 +4473,29 @@
         <v>0</v>
       </c>
       <c r="J46" s="26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K46" s="26">
         <v>14</v>
       </c>
       <c r="L46" s="26">
-        <f t="shared" ref="L46:L47" si="45">K46^2*G46</f>
+        <f t="shared" ref="L46:L47" si="40">K46^2*G46</f>
         <v>37632</v>
       </c>
       <c r="M46" s="26">
-        <f t="shared" ref="M46:M47" si="46">K46^2*F46</f>
+        <f t="shared" ref="M46:M47" si="41">K46^2*F46</f>
         <v>9408</v>
       </c>
       <c r="N46" s="26">
-        <f t="shared" ref="N46:N47" si="47">E46^2*F46*G46</f>
+        <f t="shared" ref="N46:N47" si="42">E46^2*F46*G46</f>
         <v>9216</v>
       </c>
       <c r="O46" s="26">
-        <f t="shared" ref="O46:O47" si="48">G46</f>
+        <f t="shared" ref="O46:O47" si="43">G46</f>
         <v>192</v>
       </c>
       <c r="P46" s="26">
-        <f t="shared" ref="P46:P47" si="49">N46+O46</f>
+        <f t="shared" ref="P46:P47" si="44">N46+O46</f>
         <v>9408</v>
       </c>
       <c r="Q46" s="45" t="str">
@@ -4510,15 +4507,15 @@
         <v>00C0_0030</v>
       </c>
       <c r="S46" s="12" t="str">
-        <f t="shared" ref="S46:S47" si="50">DEC2HEX(K46^2,4)&amp;"_"&amp;DEC2HEX(K46,2)&amp;DEC2HEX(E46,2)</f>
-        <v>00C4_0E01</v>
+        <f>DEC2HEX(K46^2,4)&amp;"_"&amp;DEC2HEX(K46,2)&amp;DEC2HEX(K44,2)</f>
+        <v>00C4_0E0E</v>
       </c>
       <c r="T46" s="33">
         <f>T44+P44</f>
         <v>247872</v>
       </c>
       <c r="U46" s="12" t="str">
-        <f t="shared" ref="U46:U47" si="51">DEC2HEX(T46,8)</f>
+        <f t="shared" ref="U46:U47" si="45">DEC2HEX(T46,8)</f>
         <v>0003C840</v>
       </c>
       <c r="V46" s="33">
@@ -4526,7 +4523,7 @@
         <v>3417819</v>
       </c>
       <c r="W46" s="12" t="str">
-        <f t="shared" ref="W46:W47" si="52">DEC2HEX(V46,8)</f>
+        <f t="shared" ref="W46:W47" si="46">DEC2HEX(V46,8)</f>
         <v>003426DB</v>
       </c>
       <c r="X46" s="33">
@@ -4534,7 +4531,7 @@
         <v>3427227</v>
       </c>
       <c r="Y46" s="13" t="str">
-        <f t="shared" ref="Y46:Y47" si="53">DEC2HEX(X46,8)</f>
+        <f t="shared" ref="Y46:Y47" si="47">DEC2HEX(X46,8)</f>
         <v>00344B9B</v>
       </c>
       <c r="Z46" s="2">
@@ -4553,7 +4550,7 @@
       </c>
       <c r="AD46" s="20"/>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A47" s="6" t="s">
         <v>47</v>
       </c>
@@ -4582,29 +4579,29 @@
         <v>1</v>
       </c>
       <c r="J47" s="26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K47" s="26">
         <v>14</v>
       </c>
       <c r="L47" s="26">
-        <f t="shared" si="45"/>
+        <f t="shared" si="40"/>
         <v>37632</v>
       </c>
       <c r="M47" s="26">
-        <f t="shared" si="46"/>
+        <f t="shared" si="41"/>
         <v>9408</v>
       </c>
       <c r="N47" s="26">
-        <f t="shared" si="47"/>
+        <f t="shared" si="42"/>
         <v>82944</v>
       </c>
       <c r="O47" s="26">
-        <f t="shared" si="48"/>
+        <f t="shared" si="43"/>
         <v>192</v>
       </c>
       <c r="P47" s="26">
-        <f t="shared" si="49"/>
+        <f t="shared" si="44"/>
         <v>83136</v>
       </c>
       <c r="Q47" s="45" t="str">
@@ -4616,15 +4613,15 @@
         <v>00C0_0030</v>
       </c>
       <c r="S47" s="12" t="str">
-        <f t="shared" si="50"/>
-        <v>00C4_0E03</v>
+        <f>DEC2HEX(K47^2,4)&amp;"_"&amp;DEC2HEX(K47,2)&amp;DEC2HEX(K44,2)</f>
+        <v>00C4_0E0E</v>
       </c>
       <c r="T47" s="33">
         <f>T46+P46</f>
         <v>257280</v>
       </c>
       <c r="U47" s="12" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="45"/>
         <v>0003ED00</v>
       </c>
       <c r="V47" s="33">
@@ -4632,7 +4629,7 @@
         <v>3417819</v>
       </c>
       <c r="W47" s="12" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="46"/>
         <v>003426DB</v>
       </c>
       <c r="X47" s="33">
@@ -4640,7 +4637,7 @@
         <v>3464859</v>
       </c>
       <c r="Y47" s="13" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="47"/>
         <v>0034DE9B</v>
       </c>
       <c r="Z47" s="2">
@@ -4659,7 +4656,7 @@
       </c>
       <c r="AD47" s="20"/>
     </row>
-    <row r="48" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
         <v>48</v>
       </c>
@@ -4695,7 +4692,7 @@
       <c r="AC48" s="3"/>
       <c r="AD48" s="20"/>
     </row>
-    <row r="49" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
         <v>49</v>
       </c>
@@ -4731,7 +4728,7 @@
       <c r="AC49" s="3"/>
       <c r="AD49" s="20"/>
     </row>
-    <row r="50" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>50</v>
       </c>
@@ -4746,7 +4743,7 @@
       <c r="H50" s="25"/>
       <c r="I50" s="25"/>
       <c r="J50" s="25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K50" s="25">
         <v>14</v>
@@ -4771,7 +4768,7 @@
       <c r="AC50" s="1"/>
       <c r="AD50" s="20"/>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
         <v>51</v>
       </c>
@@ -4800,7 +4797,7 @@
         <v>0</v>
       </c>
       <c r="J51" s="26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K51" s="26">
         <v>14</v>
@@ -4834,8 +4831,8 @@
         <v>0040_0180</v>
       </c>
       <c r="S51" s="12" t="str">
-        <f>DEC2HEX(K51^2,4)&amp;"_"&amp;DEC2HEX(K51,2)&amp;DEC2HEX(E51,2)</f>
-        <v>00C4_0E01</v>
+        <f>DEC2HEX(K51^2,4)&amp;"_"&amp;DEC2HEX(K51,2)&amp;DEC2HEX(K46,2)</f>
+        <v>00C4_0E0E</v>
       </c>
       <c r="T51" s="33">
         <f>T47+P47</f>
@@ -4877,7 +4874,7 @@
       </c>
       <c r="AD51" s="20"/>
     </row>
-    <row r="52" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A52" s="7" t="s">
         <v>52</v>
       </c>
@@ -4913,7 +4910,7 @@
       <c r="AC52" s="3"/>
       <c r="AD52" s="20"/>
     </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
         <v>53</v>
       </c>
@@ -4942,29 +4939,29 @@
         <v>0</v>
       </c>
       <c r="J53" s="26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K53" s="26">
         <v>14</v>
       </c>
       <c r="L53" s="26">
-        <f t="shared" ref="L53:L54" si="54">K53^2*G53</f>
+        <f t="shared" ref="L53:L54" si="48">K53^2*G53</f>
         <v>50176</v>
       </c>
       <c r="M53" s="26">
-        <f t="shared" ref="M53:M54" si="55">K53^2*F53</f>
+        <f t="shared" ref="M53:M54" si="49">K53^2*F53</f>
         <v>12544</v>
       </c>
       <c r="N53" s="26">
-        <f t="shared" ref="N53:N54" si="56">E53^2*F53*G53</f>
+        <f t="shared" ref="N53:N54" si="50">E53^2*F53*G53</f>
         <v>16384</v>
       </c>
       <c r="O53" s="26">
-        <f t="shared" ref="O53:O54" si="57">G53</f>
+        <f t="shared" ref="O53:O54" si="51">G53</f>
         <v>256</v>
       </c>
       <c r="P53" s="26">
-        <f t="shared" ref="P53:P54" si="58">N53+O53</f>
+        <f t="shared" ref="P53:P54" si="52">N53+O53</f>
         <v>16640</v>
       </c>
       <c r="Q53" s="45" t="str">
@@ -4976,15 +4973,15 @@
         <v>0100_0040</v>
       </c>
       <c r="S53" s="12" t="str">
-        <f t="shared" ref="S53:S54" si="59">DEC2HEX(K53^2,4)&amp;"_"&amp;DEC2HEX(K53,2)&amp;DEC2HEX(E53,2)</f>
-        <v>00C4_0E01</v>
+        <f>DEC2HEX(K53^2,4)&amp;"_"&amp;DEC2HEX(K53,2)&amp;DEC2HEX(K51,2)</f>
+        <v>00C4_0E0E</v>
       </c>
       <c r="T53" s="33">
         <f>T51+P51</f>
         <v>365056</v>
       </c>
       <c r="U53" s="12" t="str">
-        <f t="shared" ref="U53:U54" si="60">DEC2HEX(T53,8)</f>
+        <f t="shared" ref="U53:U54" si="53">DEC2HEX(T53,8)</f>
         <v>00059200</v>
       </c>
       <c r="V53" s="33">
@@ -4992,7 +4989,7 @@
         <v>3502491</v>
       </c>
       <c r="W53" s="12" t="str">
-        <f t="shared" ref="W53:W54" si="61">DEC2HEX(V53,8)</f>
+        <f t="shared" ref="W53:W54" si="54">DEC2HEX(V53,8)</f>
         <v>0035719B</v>
       </c>
       <c r="X53" s="33">
@@ -5000,7 +4997,7 @@
         <v>3515035</v>
       </c>
       <c r="Y53" s="13" t="str">
-        <f t="shared" ref="Y53:Y54" si="62">DEC2HEX(X53,8)</f>
+        <f t="shared" ref="Y53:Y54" si="55">DEC2HEX(X53,8)</f>
         <v>0035A29B</v>
       </c>
       <c r="Z53" s="2">
@@ -5019,7 +5016,7 @@
       </c>
       <c r="AD53" s="20"/>
     </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
         <v>54</v>
       </c>
@@ -5048,29 +5045,29 @@
         <v>1</v>
       </c>
       <c r="J54" s="26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K54" s="26">
         <v>14</v>
       </c>
       <c r="L54" s="26">
-        <f t="shared" si="54"/>
+        <f t="shared" si="48"/>
         <v>50176</v>
       </c>
       <c r="M54" s="26">
-        <f t="shared" si="55"/>
+        <f t="shared" si="49"/>
         <v>12544</v>
       </c>
       <c r="N54" s="26">
-        <f t="shared" si="56"/>
+        <f t="shared" si="50"/>
         <v>147456</v>
       </c>
       <c r="O54" s="26">
-        <f t="shared" si="57"/>
+        <f t="shared" si="51"/>
         <v>256</v>
       </c>
       <c r="P54" s="26">
-        <f t="shared" si="58"/>
+        <f t="shared" si="52"/>
         <v>147712</v>
       </c>
       <c r="Q54" s="45" t="str">
@@ -5082,15 +5079,15 @@
         <v>0100_0040</v>
       </c>
       <c r="S54" s="12" t="str">
-        <f t="shared" si="59"/>
-        <v>00C4_0E03</v>
+        <f>DEC2HEX(K54^2,4)&amp;"_"&amp;DEC2HEX(K54,2)&amp;DEC2HEX(K51,2)</f>
+        <v>00C4_0E0E</v>
       </c>
       <c r="T54" s="33">
         <f>T53+P53</f>
         <v>381696</v>
       </c>
       <c r="U54" s="12" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="53"/>
         <v>0005D300</v>
       </c>
       <c r="V54" s="33">
@@ -5098,7 +5095,7 @@
         <v>3502491</v>
       </c>
       <c r="W54" s="12" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="54"/>
         <v>0035719B</v>
       </c>
       <c r="X54" s="33">
@@ -5106,7 +5103,7 @@
         <v>3565211</v>
       </c>
       <c r="Y54" s="13" t="str">
-        <f t="shared" si="62"/>
+        <f t="shared" si="55"/>
         <v>0036669B</v>
       </c>
       <c r="Z54" s="2">
@@ -5125,7 +5122,7 @@
       </c>
       <c r="AD54" s="20"/>
     </row>
-    <row r="55" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
         <v>55</v>
       </c>
@@ -5161,7 +5158,7 @@
       <c r="AC55" s="3"/>
       <c r="AD55" s="20"/>
     </row>
-    <row r="56" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
         <v>56</v>
       </c>
@@ -5197,7 +5194,7 @@
       <c r="AC56" s="3"/>
       <c r="AD56" s="20"/>
     </row>
-    <row r="57" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>57</v>
       </c>
@@ -5212,7 +5209,7 @@
       <c r="H57" s="25"/>
       <c r="I57" s="25"/>
       <c r="J57" s="25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K57" s="25">
         <v>14</v>
@@ -5237,7 +5234,7 @@
       <c r="AC57" s="1"/>
       <c r="AD57" s="20"/>
     </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A58" s="6" t="s">
         <v>58</v>
       </c>
@@ -5266,7 +5263,7 @@
         <v>0</v>
       </c>
       <c r="J58" s="26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K58" s="26">
         <v>14</v>
@@ -5300,8 +5297,8 @@
         <v>0040_0200</v>
       </c>
       <c r="S58" s="12" t="str">
-        <f>DEC2HEX(K58^2,4)&amp;"_"&amp;DEC2HEX(K58,2)&amp;DEC2HEX(E58,2)</f>
-        <v>00C4_0E01</v>
+        <f>DEC2HEX(K58^2,4)&amp;"_"&amp;DEC2HEX(K58,2)&amp;DEC2HEX(K53,2)</f>
+        <v>00C4_0E0E</v>
       </c>
       <c r="T58" s="33">
         <f>T54+P54</f>
@@ -5343,7 +5340,7 @@
       </c>
       <c r="AD58" s="20"/>
     </row>
-    <row r="59" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A59" s="7" t="s">
         <v>59</v>
       </c>
@@ -5379,7 +5376,7 @@
       <c r="AC59" s="3"/>
       <c r="AD59" s="20"/>
     </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A60" s="6" t="s">
         <v>60</v>
       </c>
@@ -5408,29 +5405,29 @@
         <v>0</v>
       </c>
       <c r="J60" s="26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K60" s="26">
         <v>14</v>
       </c>
       <c r="L60" s="26">
-        <f t="shared" ref="L60:L61" si="63">K60^2*G60</f>
+        <f t="shared" ref="L60:L61" si="56">K60^2*G60</f>
         <v>50176</v>
       </c>
       <c r="M60" s="26">
-        <f t="shared" ref="M60:M61" si="64">K60^2*F60</f>
+        <f t="shared" ref="M60:M61" si="57">K60^2*F60</f>
         <v>12544</v>
       </c>
       <c r="N60" s="26">
-        <f t="shared" ref="N60:N61" si="65">E60^2*F60*G60</f>
+        <f t="shared" ref="N60:N61" si="58">E60^2*F60*G60</f>
         <v>16384</v>
       </c>
       <c r="O60" s="26">
-        <f t="shared" ref="O60:O61" si="66">G60</f>
+        <f t="shared" ref="O60:O61" si="59">G60</f>
         <v>256</v>
       </c>
       <c r="P60" s="26">
-        <f t="shared" ref="P60:P61" si="67">N60+O60</f>
+        <f t="shared" ref="P60:P61" si="60">N60+O60</f>
         <v>16640</v>
       </c>
       <c r="Q60" s="45" t="str">
@@ -5442,15 +5439,15 @@
         <v>0100_0040</v>
       </c>
       <c r="S60" s="12" t="str">
-        <f t="shared" ref="S60:S61" si="68">DEC2HEX(K60^2,4)&amp;"_"&amp;DEC2HEX(K60,2)&amp;DEC2HEX(E60,2)</f>
-        <v>00C4_0E01</v>
+        <f>DEC2HEX(K60^2,4)&amp;"_"&amp;DEC2HEX(K60,2)&amp;DEC2HEX(K58,2)</f>
+        <v>00C4_0E0E</v>
       </c>
       <c r="T60" s="33">
         <f>T58+P58</f>
         <v>562240</v>
       </c>
       <c r="U60" s="12" t="str">
-        <f t="shared" ref="U60:U61" si="69">DEC2HEX(T60,8)</f>
+        <f t="shared" ref="U60:U61" si="61">DEC2HEX(T60,8)</f>
         <v>00089440</v>
       </c>
       <c r="V60" s="33">
@@ -5458,7 +5455,7 @@
         <v>3615387</v>
       </c>
       <c r="W60" s="12" t="str">
-        <f t="shared" ref="W60:W61" si="70">DEC2HEX(V60,8)</f>
+        <f t="shared" ref="W60:W61" si="62">DEC2HEX(V60,8)</f>
         <v>00372A9B</v>
       </c>
       <c r="X60" s="33">
@@ -5466,7 +5463,7 @@
         <v>3627931</v>
       </c>
       <c r="Y60" s="13" t="str">
-        <f t="shared" ref="Y60:Y61" si="71">DEC2HEX(X60,8)</f>
+        <f t="shared" ref="Y60:Y61" si="63">DEC2HEX(X60,8)</f>
         <v>00375B9B</v>
       </c>
       <c r="Z60" s="2">
@@ -5485,7 +5482,7 @@
       </c>
       <c r="AD60" s="20"/>
     </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A61" s="6" t="s">
         <v>61</v>
       </c>
@@ -5514,29 +5511,29 @@
         <v>1</v>
       </c>
       <c r="J61" s="26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K61" s="26">
         <v>14</v>
       </c>
       <c r="L61" s="26">
-        <f t="shared" si="63"/>
+        <f t="shared" si="56"/>
         <v>50176</v>
       </c>
       <c r="M61" s="26">
-        <f t="shared" si="64"/>
+        <f t="shared" si="57"/>
         <v>12544</v>
       </c>
       <c r="N61" s="26">
-        <f t="shared" si="65"/>
+        <f t="shared" si="58"/>
         <v>147456</v>
       </c>
       <c r="O61" s="26">
-        <f t="shared" si="66"/>
+        <f t="shared" si="59"/>
         <v>256</v>
       </c>
       <c r="P61" s="26">
-        <f t="shared" si="67"/>
+        <f t="shared" si="60"/>
         <v>147712</v>
       </c>
       <c r="Q61" s="45" t="str">
@@ -5548,15 +5545,15 @@
         <v>0100_0040</v>
       </c>
       <c r="S61" s="12" t="str">
-        <f t="shared" si="68"/>
-        <v>00C4_0E03</v>
+        <f>DEC2HEX(K61^2,4)&amp;"_"&amp;DEC2HEX(K61,2)&amp;DEC2HEX(K58,2)</f>
+        <v>00C4_0E0E</v>
       </c>
       <c r="T61" s="33">
         <f>T60+P60</f>
         <v>578880</v>
       </c>
       <c r="U61" s="12" t="str">
-        <f t="shared" si="69"/>
+        <f t="shared" si="61"/>
         <v>0008D540</v>
       </c>
       <c r="V61" s="33">
@@ -5564,7 +5561,7 @@
         <v>3615387</v>
       </c>
       <c r="W61" s="12" t="str">
-        <f t="shared" si="70"/>
+        <f t="shared" si="62"/>
         <v>00372A9B</v>
       </c>
       <c r="X61" s="33">
@@ -5572,7 +5569,7 @@
         <v>3678107</v>
       </c>
       <c r="Y61" s="13" t="str">
-        <f t="shared" si="71"/>
+        <f t="shared" si="63"/>
         <v>00381F9B</v>
       </c>
       <c r="Z61" s="2">
@@ -5591,7 +5588,7 @@
       </c>
       <c r="AD61" s="20"/>
     </row>
-    <row r="62" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
         <v>62</v>
       </c>
@@ -5627,7 +5624,7 @@
       <c r="AC62" s="3"/>
       <c r="AD62" s="20"/>
     </row>
-    <row r="63" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A63" s="7" t="s">
         <v>63</v>
       </c>
@@ -5663,7 +5660,7 @@
       <c r="AC63" s="3"/>
       <c r="AD63" s="20"/>
     </row>
-    <row r="64" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>64</v>
       </c>
@@ -5678,7 +5675,7 @@
       <c r="H64" s="25"/>
       <c r="I64" s="25"/>
       <c r="J64" s="25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K64" s="25">
         <v>14</v>
@@ -5703,7 +5700,7 @@
       <c r="AC64" s="1"/>
       <c r="AD64" s="20"/>
     </row>
-    <row r="65" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A65" s="38" t="s">
         <v>65</v>
       </c>
@@ -5739,7 +5736,7 @@
       <c r="AC65" s="3"/>
       <c r="AD65" s="20"/>
     </row>
-    <row r="66" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A66" s="6" t="s">
         <v>66</v>
       </c>
@@ -5768,7 +5765,7 @@
         <v>0</v>
       </c>
       <c r="J66" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K66" s="26">
         <v>14</v>
@@ -5802,8 +5799,8 @@
         <v>03E8_0200</v>
       </c>
       <c r="S66" s="12" t="str">
-        <f>DEC2HEX(K66^2,4)&amp;"_"&amp;DEC2HEX(K66,2)&amp;DEC2HEX(E66,2)</f>
-        <v>00C4_0E01</v>
+        <f>DEC2HEX(K66^2,4)&amp;"_"&amp;DEC2HEX(K66,2)&amp;DEC2HEX(K60,2)</f>
+        <v>00C4_0E0E</v>
       </c>
       <c r="T66" s="33">
         <f>T61+P61</f>
@@ -5845,7 +5842,7 @@
       </c>
       <c r="AD66" s="20"/>
     </row>
-    <row r="67" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A67" s="7" t="s">
         <v>67</v>
       </c>
@@ -5881,7 +5878,7 @@
       <c r="AC67" s="3"/>
       <c r="AD67" s="20"/>
     </row>
-    <row r="68" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A68" s="8" t="s">
         <v>68</v>
       </c>
@@ -5892,7 +5889,7 @@
         <v>5</v>
       </c>
       <c r="D68" s="28" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E68" s="28">
         <v>14</v>
@@ -5935,7 +5932,7 @@
         <v>03E8_03E8</v>
       </c>
       <c r="S68" s="16" t="str">
-        <f>DEC2HEX(K68^2,4)&amp;"_"&amp;DEC2HEX(K68,2)&amp;DEC2HEX(E68,2)</f>
+        <f>DEC2HEX(K68^2,4)&amp;"_"&amp;DEC2HEX(K68,2)&amp;DEC2HEX(K66,2)</f>
         <v>0001_010E</v>
       </c>
       <c r="T68" s="35"/>
@@ -5975,7 +5972,7 @@
       </c>
       <c r="AD68" s="20"/>
     </row>
-    <row r="69" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>69</v>
       </c>
@@ -6011,7 +6008,7 @@
       <c r="AC69" s="1"/>
       <c r="AD69" s="20"/>
     </row>
-    <row r="70" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A70" s="9"/>
       <c r="B70" s="24"/>
       <c r="C70" s="40"/>
@@ -6056,12 +6053,12 @@
         <v>49559.770468750008</v>
       </c>
       <c r="AC70" s="20">
-        <f t="shared" ref="AC70" si="72">SUM(AC4:AC69)</f>
+        <f t="shared" ref="AC70" si="64">SUM(AC4:AC69)</f>
         <v>417544.91999999993</v>
       </c>
       <c r="AD70" s="20"/>
     </row>
-    <row r="71" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A71" s="9"/>
       <c r="B71" s="24"/>
       <c r="C71" s="40"/>
@@ -6103,15 +6100,7 @@
       <c r="AD71" s="20"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:B71" xr:uid="{009522EF-F8DC-42BE-8F4B-D751FC8B03E1}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="AVE Pooling"/>
-        <filter val="Convolution"/>
-        <filter val="MAX Pooling"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B2:B71" xr:uid="{009522EF-F8DC-42BE-8F4B-D751FC8B03E1}"/>
   <mergeCells count="9">
     <mergeCell ref="Z1:AC1"/>
     <mergeCell ref="J1:P1"/>
@@ -6135,38 +6124,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E501AE-4D2D-491C-85E4-0C34FDA03C89}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
+    <sheetView zoomScale="76" workbookViewId="0">
       <selection sqref="A1:F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>136</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>137</v>
       </c>
       <c r="H1" t="str">
         <f>LEFT(SUBSTITUTE(A1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A1,"_",),4)</f>
@@ -6178,7 +6167,7 @@
       </c>
       <c r="J1" t="str">
         <f t="shared" si="0"/>
-        <v>31E1 7103</v>
+        <v>31E1 71E3</v>
       </c>
       <c r="K1" t="str">
         <f t="shared" si="0"/>
@@ -6193,24 +6182,24 @@
         <v>000C 5BDB</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="47" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>193</v>
+        <v>222</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E2" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>137</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>138</v>
       </c>
       <c r="H2" t="str">
         <f t="shared" ref="H2:H30" si="1">LEFT(SUBSTITUTE(A2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A2,"_",),4)</f>
@@ -6222,7 +6211,7 @@
       </c>
       <c r="J2" t="str">
         <f t="shared" ref="J2:J30" si="3">LEFT(SUBSTITUTE(C2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C2,"_",),4)</f>
-        <v>0C40 3803</v>
+        <v>0C40 3871</v>
       </c>
       <c r="K2" t="str">
         <f t="shared" ref="K2:K30" si="4">LEFT(SUBSTITUTE(D2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D2,"_",),4)</f>
@@ -6237,24 +6226,24 @@
         <v>0018 D41B</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="45" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>203</v>
-      </c>
       <c r="E3" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" si="1"/>
@@ -6266,7 +6255,7 @@
       </c>
       <c r="J3" t="str">
         <f t="shared" si="3"/>
-        <v>0C40 3801</v>
+        <v>0C40 3838</v>
       </c>
       <c r="K3" t="str">
         <f t="shared" si="4"/>
@@ -6281,24 +6270,24 @@
         <v>001B E41B</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="45" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>194</v>
+        <v>223</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="1"/>
@@ -6310,7 +6299,7 @@
       </c>
       <c r="J4" t="str">
         <f t="shared" si="3"/>
-        <v>0C40 3801</v>
+        <v>0C40 3838</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" si="4"/>
@@ -6325,24 +6314,24 @@
         <v>001C A81B</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="45" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>193</v>
+        <v>223</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="1"/>
@@ -6354,7 +6343,7 @@
       </c>
       <c r="J5" t="str">
         <f t="shared" si="3"/>
-        <v>0C40 3803</v>
+        <v>0C40 3838</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="4"/>
@@ -6369,24 +6358,24 @@
         <v>001F B81B</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="45" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>194</v>
+        <v>223</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="1"/>
@@ -6398,7 +6387,7 @@
       </c>
       <c r="J6" t="str">
         <f t="shared" si="3"/>
-        <v>0C40 3801</v>
+        <v>0C40 3838</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="4"/>
@@ -6413,24 +6402,24 @@
         <v>0022 C81B</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="45" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>194</v>
+        <v>223</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="1"/>
@@ -6442,7 +6431,7 @@
       </c>
       <c r="J7" t="str">
         <f t="shared" si="3"/>
-        <v>0C40 3801</v>
+        <v>0C40 3838</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="4"/>
@@ -6457,24 +6446,24 @@
         <v>0023 8C1B</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="45" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>146</v>
-      </c>
       <c r="F8" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="1"/>
@@ -6486,7 +6475,7 @@
       </c>
       <c r="J8" t="str">
         <f t="shared" si="3"/>
-        <v>0C40 3803</v>
+        <v>0C40 3838</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="4"/>
@@ -6501,24 +6490,24 @@
         <v>0026 9C1B</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="47" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>195</v>
+        <v>224</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E9" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="F9" s="17" t="s">
         <v>149</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>150</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="1"/>
@@ -6530,7 +6519,7 @@
       </c>
       <c r="J9" t="str">
         <f t="shared" si="3"/>
-        <v>0310 1C03</v>
+        <v>0310 1C38</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="4"/>
@@ -6545,24 +6534,24 @@
         <v>0029 AC1B</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="45" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>196</v>
+        <v>225</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="E10" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F10" s="13" t="s">
         <v>150</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>151</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="1"/>
@@ -6574,7 +6563,7 @@
       </c>
       <c r="J10" t="str">
         <f t="shared" si="3"/>
-        <v>0310 1C01</v>
+        <v>0310 1C1C</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="4"/>
@@ -6589,24 +6578,24 @@
         <v>002B 341B</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="45" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>196</v>
+        <v>225</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="1"/>
@@ -6618,7 +6607,7 @@
       </c>
       <c r="J11" t="str">
         <f t="shared" si="3"/>
-        <v>0310 1C01</v>
+        <v>0310 1C1C</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="4"/>
@@ -6633,24 +6622,24 @@
         <v>002B 961B</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="45" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>195</v>
+        <v>225</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="1"/>
@@ -6662,7 +6651,7 @@
       </c>
       <c r="J12" t="str">
         <f t="shared" si="3"/>
-        <v>0310 1C03</v>
+        <v>0310 1C1C</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="4"/>
@@ -6677,24 +6666,24 @@
         <v>002D 1E1B</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="45" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>196</v>
+        <v>225</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="1"/>
@@ -6706,7 +6695,7 @@
       </c>
       <c r="J13" t="str">
         <f t="shared" si="3"/>
-        <v>0310 1C01</v>
+        <v>0310 1C1C</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="4"/>
@@ -6721,24 +6710,24 @@
         <v>002E A61B</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="45" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>196</v>
+        <v>225</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="1"/>
@@ -6750,7 +6739,7 @@
       </c>
       <c r="J14" t="str">
         <f t="shared" si="3"/>
-        <v>0310 1C01</v>
+        <v>0310 1C1C</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="4"/>
@@ -6765,24 +6754,24 @@
         <v>002F 081B</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="E15" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>157</v>
-      </c>
       <c r="F15" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="1"/>
@@ -6794,7 +6783,7 @@
       </c>
       <c r="J15" t="str">
         <f t="shared" si="3"/>
-        <v>0310 1C03</v>
+        <v>0310 1C1C</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="4"/>
@@ -6809,24 +6798,24 @@
         <v>0030 901B</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="47" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>197</v>
+        <v>226</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E16" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="F16" s="17" t="s">
         <v>160</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>161</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="1"/>
@@ -6838,7 +6827,7 @@
       </c>
       <c r="J16" t="str">
         <f t="shared" si="3"/>
-        <v>00C4 0E03</v>
+        <v>00C4 0E1C</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="4"/>
@@ -6853,24 +6842,24 @@
         <v>0032 181B</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="45" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>198</v>
+        <v>227</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="E17" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="F17" s="13" t="s">
         <v>161</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>162</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="1"/>
@@ -6882,7 +6871,7 @@
       </c>
       <c r="J17" t="str">
         <f t="shared" si="3"/>
-        <v>00C4 0E01</v>
+        <v>00C4 0E0E</v>
       </c>
       <c r="K17" t="str">
         <f t="shared" si="4"/>
@@ -6897,24 +6886,24 @@
         <v>0032 DC1B</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>166</v>
-      </c>
       <c r="C18" s="12" t="s">
-        <v>198</v>
+        <v>227</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="1"/>
@@ -6926,7 +6915,7 @@
       </c>
       <c r="J18" t="str">
         <f t="shared" si="3"/>
-        <v>00C4 0E01</v>
+        <v>00C4 0E0E</v>
       </c>
       <c r="K18" t="str">
         <f t="shared" si="4"/>
@@ -6941,24 +6930,24 @@
         <v>0033 00DB</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="45" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B19" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="F19" s="13" t="s">
         <v>166</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>167</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="1"/>
@@ -6970,7 +6959,7 @@
       </c>
       <c r="J19" t="str">
         <f t="shared" si="3"/>
-        <v>00C4 0E03</v>
+        <v>00C4 0E0E</v>
       </c>
       <c r="K19" t="str">
         <f t="shared" si="4"/>
@@ -6985,24 +6974,24 @@
         <v>0033 93DB</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="45" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>198</v>
+        <v>227</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="1"/>
@@ -7014,7 +7003,7 @@
       </c>
       <c r="J20" t="str">
         <f t="shared" si="3"/>
-        <v>00C4 0E01</v>
+        <v>00C4 0E0E</v>
       </c>
       <c r="K20" t="str">
         <f t="shared" si="4"/>
@@ -7029,24 +7018,24 @@
         <v>0034 26DB</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="B21" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>166</v>
-      </c>
       <c r="C21" s="12" t="s">
-        <v>198</v>
+        <v>227</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="1"/>
@@ -7058,7 +7047,7 @@
       </c>
       <c r="J21" t="str">
         <f t="shared" si="3"/>
-        <v>00C4 0E01</v>
+        <v>00C4 0E0E</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" si="4"/>
@@ -7073,24 +7062,24 @@
         <v>0034 4B9B</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="45" t="s">
+        <v>167</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="E22" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>169</v>
-      </c>
       <c r="F22" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="1"/>
@@ -7102,7 +7091,7 @@
       </c>
       <c r="J22" t="str">
         <f t="shared" si="3"/>
-        <v>00C4 0E03</v>
+        <v>00C4 0E0E</v>
       </c>
       <c r="K22" t="str">
         <f t="shared" si="4"/>
@@ -7117,24 +7106,24 @@
         <v>0034 DE9B</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="45" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>198</v>
+        <v>227</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="E23" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="F23" s="13" t="s">
         <v>172</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>173</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="1"/>
@@ -7146,7 +7135,7 @@
       </c>
       <c r="J23" t="str">
         <f t="shared" si="3"/>
-        <v>00C4 0E01</v>
+        <v>00C4 0E0E</v>
       </c>
       <c r="K23" t="str">
         <f t="shared" si="4"/>
@@ -7161,24 +7150,24 @@
         <v>0035 719B</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="45" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>198</v>
+        <v>227</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="1"/>
@@ -7190,7 +7179,7 @@
       </c>
       <c r="J24" t="str">
         <f t="shared" si="3"/>
-        <v>00C4 0E01</v>
+        <v>00C4 0E0E</v>
       </c>
       <c r="K24" t="str">
         <f t="shared" si="4"/>
@@ -7205,24 +7194,24 @@
         <v>0035 A29B</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="45" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>197</v>
+        <v>227</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="1"/>
@@ -7234,7 +7223,7 @@
       </c>
       <c r="J25" t="str">
         <f t="shared" si="3"/>
-        <v>00C4 0E03</v>
+        <v>00C4 0E0E</v>
       </c>
       <c r="K25" t="str">
         <f t="shared" si="4"/>
@@ -7249,24 +7238,24 @@
         <v>0036 669B</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="45" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>198</v>
+        <v>227</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="1"/>
@@ -7278,7 +7267,7 @@
       </c>
       <c r="J26" t="str">
         <f t="shared" si="3"/>
-        <v>00C4 0E01</v>
+        <v>00C4 0E0E</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" si="4"/>
@@ -7293,24 +7282,24 @@
         <v>0037 2A9B</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="45" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>198</v>
+        <v>227</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="1"/>
@@ -7322,7 +7311,7 @@
       </c>
       <c r="J27" t="str">
         <f t="shared" si="3"/>
-        <v>00C4 0E01</v>
+        <v>00C4 0E0E</v>
       </c>
       <c r="K27" t="str">
         <f t="shared" si="4"/>
@@ -7337,24 +7326,24 @@
         <v>0037 5B9B</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="E28" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="B28" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>179</v>
-      </c>
       <c r="F28" s="13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="1"/>
@@ -7366,7 +7355,7 @@
       </c>
       <c r="J28" t="str">
         <f t="shared" si="3"/>
-        <v>00C4 0E03</v>
+        <v>00C4 0E0E</v>
       </c>
       <c r="K28" t="str">
         <f t="shared" si="4"/>
@@ -7381,24 +7370,24 @@
         <v>0038 1F9B</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="45" t="s">
+        <v>183</v>
+      </c>
+      <c r="B29" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>185</v>
-      </c>
       <c r="C29" s="12" t="s">
-        <v>198</v>
+        <v>227</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="E29" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="F29" s="13" t="s">
         <v>182</v>
-      </c>
-      <c r="F29" s="13" t="s">
-        <v>183</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="1"/>
@@ -7410,7 +7399,7 @@
       </c>
       <c r="J29" t="str">
         <f t="shared" si="3"/>
-        <v>00C4 0E01</v>
+        <v>00C4 0E0E</v>
       </c>
       <c r="K29" t="str">
         <f t="shared" si="4"/>
@@ -7425,24 +7414,24 @@
         <v>0038 E39B</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="47" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Update some variable names
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86E0EC2-CD07-4D84-AE28-9102EF8A929D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7E5844-8295-42BB-99D7-961A1BB5F0FC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="248">
   <si>
     <t>INPUT</t>
   </si>
@@ -298,9 +298,6 @@
     <t>1x1</t>
   </si>
   <si>
-    <t>27x27x128</t>
-  </si>
-  <si>
     <t>1x1x1000</t>
   </si>
   <si>
@@ -547,9 +544,6 @@
     <t>14x14</t>
   </si>
   <si>
-    <t>0001_010E</t>
-  </si>
-  <si>
     <t>Conv Weight</t>
   </si>
   <si>
@@ -634,27 +628,6 @@
     <t>oichannel</t>
   </si>
   <si>
-    <t>31E1_71E3</t>
-  </si>
-  <si>
-    <t>0C40_3871</t>
-  </si>
-  <si>
-    <t>0C40_3838</t>
-  </si>
-  <si>
-    <t>0310_1C38</t>
-  </si>
-  <si>
-    <t>0310_1C1C</t>
-  </si>
-  <si>
-    <t>00C4_0E1C</t>
-  </si>
-  <si>
-    <t>00C4_0E0E</t>
-  </si>
-  <si>
     <t>op_num</t>
   </si>
   <si>
@@ -752,6 +725,60 @@
   </si>
   <si>
     <t>kernel, oiside</t>
+  </si>
+  <si>
+    <t>0003_71E3</t>
+  </si>
+  <si>
+    <t>31E1_C949</t>
+  </si>
+  <si>
+    <t>0009_3871</t>
+  </si>
+  <si>
+    <t>0C40_31E1</t>
+  </si>
+  <si>
+    <t>0001_3838</t>
+  </si>
+  <si>
+    <t>0C40_0C40</t>
+  </si>
+  <si>
+    <t>0003_3838</t>
+  </si>
+  <si>
+    <t>0003_1C38</t>
+  </si>
+  <si>
+    <t>0310_0C40</t>
+  </si>
+  <si>
+    <t>0001_1C1C</t>
+  </si>
+  <si>
+    <t>0310_0310</t>
+  </si>
+  <si>
+    <t>0003_1C1C</t>
+  </si>
+  <si>
+    <t>0003_0E1C</t>
+  </si>
+  <si>
+    <t>00C4_0310</t>
+  </si>
+  <si>
+    <t>0001_0E0E</t>
+  </si>
+  <si>
+    <t>0003_0E0E</t>
+  </si>
+  <si>
+    <t>000E_010E</t>
+  </si>
+  <si>
+    <t>0001_00C4</t>
   </si>
 </sst>
 </file>
@@ -1388,8 +1415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80B23C6-EAEB-43B1-B045-456C36085CFA}">
   <dimension ref="A1:AG71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I50" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V69" sqref="V69"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1413,7 +1440,7 @@
     <col min="19" max="19" width="18" style="31" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9.81640625" style="31" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.90625" style="31" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.90625" style="31" customWidth="1"/>
+    <col min="22" max="22" width="9.81640625" style="31" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="6.81640625" style="37" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="8.81640625" style="31" customWidth="1"/>
     <col min="25" max="25" width="7.81640625" style="37" bestFit="1" customWidth="1"/>
@@ -1431,18 +1458,18 @@
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
       <c r="D1" s="56" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E1" s="56"/>
       <c r="F1" s="56"/>
       <c r="G1" s="56"/>
       <c r="H1" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I1" s="22"/>
       <c r="J1" s="22"/>
       <c r="K1" s="54" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L1" s="54"/>
       <c r="M1" s="54"/>
@@ -1451,7 +1478,7 @@
       <c r="P1" s="54"/>
       <c r="Q1" s="55"/>
       <c r="R1" s="57" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="S1" s="58"/>
       <c r="T1" s="58"/>
@@ -1464,7 +1491,7 @@
       <c r="AA1" s="58"/>
       <c r="AB1" s="59"/>
       <c r="AC1" s="52" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AD1" s="53"/>
       <c r="AE1" s="53"/>
@@ -1478,7 +1505,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D2" s="54" t="s">
         <v>77</v>
@@ -1488,7 +1515,7 @@
         <v>83</v>
       </c>
       <c r="G2" s="50" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="H2" s="24" t="s">
         <v>84</v>
@@ -1505,55 +1532,55 @@
       <c r="L2" s="54"/>
       <c r="M2" s="54"/>
       <c r="N2" s="24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O2" s="24" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P2" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q2" s="40" t="s">
         <v>85</v>
       </c>
       <c r="R2" s="41" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="S2" s="51" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="T2" s="42" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="U2" s="18" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="V2" s="18" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="W2" s="60" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="X2" s="60"/>
       <c r="Y2" s="60" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z2" s="60"/>
       <c r="AA2" s="60" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AB2" s="61"/>
       <c r="AC2" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AD2" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AE2" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AF2" s="20" t="s">
         <v>110</v>
-      </c>
-      <c r="AF2" s="20" t="s">
-        <v>111</v>
       </c>
       <c r="AG2" s="20" t="s">
         <v>80</v>
@@ -1577,7 +1604,7 @@
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
       <c r="K3" s="25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L3" s="25">
         <v>227</v>
@@ -1645,7 +1672,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L4" s="26">
         <v>113</v>
@@ -1800,7 +1827,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L6" s="28">
         <v>56</v>
@@ -1906,7 +1933,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L7" s="26">
         <v>56</v>
@@ -2038,7 +2065,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="26" t="s">
         <v>86</v>
@@ -2063,7 +2090,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L9" s="26">
         <v>56</v>
@@ -2090,7 +2117,7 @@
       </c>
       <c r="R9" s="45" t="str">
         <f t="shared" ref="R9:R10" si="6">DEC2HEX(G9,4)&amp;"_0"&amp;DEC2HEX(I9,1)&amp;DEC2HEX(J9,1)&amp;DEC2HEX(C9,1)</f>
-        <v>0010_0102</v>
+        <v>0010_0101</v>
       </c>
       <c r="S9" s="12" t="str">
         <f t="shared" ref="S9:S10" si="7">IF(J9=0,DEC2HEX(G9,4)&amp;"_"&amp;DEC2HEX(G9,4), DEC2HEX(G9/9*6,4)&amp;"_"&amp;DEC2HEX(G9/9*4,4))</f>
@@ -2156,7 +2183,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>82</v>
@@ -2181,7 +2208,7 @@
         <v>1</v>
       </c>
       <c r="K10" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L10" s="26">
         <v>56</v>
@@ -2208,7 +2235,7 @@
       </c>
       <c r="R10" s="45" t="str">
         <f t="shared" si="6"/>
-        <v>0090_0111</v>
+        <v>0090_0112</v>
       </c>
       <c r="S10" s="12" t="str">
         <f t="shared" si="7"/>
@@ -2360,7 +2387,7 @@
       <c r="I13" s="25"/>
       <c r="J13" s="25"/>
       <c r="K13" s="25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L13" s="25">
         <v>56</v>
@@ -2420,7 +2447,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L14" s="26">
         <v>56</v>
@@ -2552,7 +2579,7 @@
         <v>8</v>
       </c>
       <c r="C16" s="26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" s="26" t="s">
         <v>86</v>
@@ -2577,7 +2604,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L16" s="26">
         <v>56</v>
@@ -2604,7 +2631,7 @@
       </c>
       <c r="R16" s="45" t="str">
         <f t="shared" ref="R16:R17" si="17">DEC2HEX(G16,4)&amp;"_0"&amp;DEC2HEX(I16,1)&amp;DEC2HEX(J16,1)&amp;DEC2HEX(C16,1)</f>
-        <v>0010_0102</v>
+        <v>0010_0101</v>
       </c>
       <c r="S16" s="12" t="str">
         <f t="shared" ref="S16:S17" si="18">IF(J16=0,DEC2HEX(G16,4)&amp;"_"&amp;DEC2HEX(G16,4), DEC2HEX(G16/9*6,4)&amp;"_"&amp;DEC2HEX(G16/9*4,4))</f>
@@ -2670,7 +2697,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="26" t="s">
         <v>82</v>
@@ -2695,7 +2722,7 @@
         <v>1</v>
       </c>
       <c r="K17" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L17" s="26">
         <v>56</v>
@@ -2722,7 +2749,7 @@
       </c>
       <c r="R17" s="45" t="str">
         <f t="shared" si="17"/>
-        <v>0090_0111</v>
+        <v>0090_0112</v>
       </c>
       <c r="S17" s="12" t="str">
         <f t="shared" si="18"/>
@@ -2874,7 +2901,7 @@
       <c r="I20" s="25"/>
       <c r="J20" s="25"/>
       <c r="K20" s="25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L20" s="25">
         <v>56</v>
@@ -2934,7 +2961,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="28" t="s">
-        <v>87</v>
+        <v>122</v>
       </c>
       <c r="L21" s="28">
         <v>28</v>
@@ -3040,7 +3067,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L22" s="26">
         <v>28</v>
@@ -3172,7 +3199,7 @@
         <v>8</v>
       </c>
       <c r="C24" s="26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24" s="26" t="s">
         <v>86</v>
@@ -3197,7 +3224,7 @@
         <v>0</v>
       </c>
       <c r="K24" s="26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L24" s="26">
         <v>28</v>
@@ -3224,7 +3251,7 @@
       </c>
       <c r="R24" s="45" t="str">
         <f t="shared" ref="R24:R25" si="28">DEC2HEX(G24,4)&amp;"_0"&amp;DEC2HEX(I24,1)&amp;DEC2HEX(J24,1)&amp;DEC2HEX(C24,1)</f>
-        <v>0020_0102</v>
+        <v>0020_0101</v>
       </c>
       <c r="S24" s="12" t="str">
         <f t="shared" ref="S24:S25" si="29">IF(J24=0,DEC2HEX(G24,4)&amp;"_"&amp;DEC2HEX(G24,4), DEC2HEX(G24/9*6,4)&amp;"_"&amp;DEC2HEX(G24/9*4,4))</f>
@@ -3290,7 +3317,7 @@
         <v>8</v>
       </c>
       <c r="C25" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" s="26" t="s">
         <v>82</v>
@@ -3315,7 +3342,7 @@
         <v>1</v>
       </c>
       <c r="K25" s="26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L25" s="26">
         <v>28</v>
@@ -3342,7 +3369,7 @@
       </c>
       <c r="R25" s="45" t="str">
         <f t="shared" si="28"/>
-        <v>0120_0111</v>
+        <v>0120_0112</v>
       </c>
       <c r="S25" s="12" t="str">
         <f t="shared" si="29"/>
@@ -3494,7 +3521,7 @@
       <c r="I28" s="25"/>
       <c r="J28" s="25"/>
       <c r="K28" s="25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L28" s="25">
         <v>28</v>
@@ -3554,7 +3581,7 @@
         <v>0</v>
       </c>
       <c r="K29" s="26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L29" s="26">
         <v>28</v>
@@ -3686,7 +3713,7 @@
         <v>8</v>
       </c>
       <c r="C31" s="26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D31" s="26" t="s">
         <v>86</v>
@@ -3711,7 +3738,7 @@
         <v>0</v>
       </c>
       <c r="K31" s="26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L31" s="26">
         <v>28</v>
@@ -3738,7 +3765,7 @@
       </c>
       <c r="R31" s="45" t="str">
         <f t="shared" ref="R31:R32" si="39">DEC2HEX(G31,4)&amp;"_0"&amp;DEC2HEX(I31,1)&amp;DEC2HEX(J31,1)&amp;DEC2HEX(C31,1)</f>
-        <v>0020_0102</v>
+        <v>0020_0101</v>
       </c>
       <c r="S31" s="12" t="str">
         <f t="shared" ref="S31:S32" si="40">IF(J31=0,DEC2HEX(G31,4)&amp;"_"&amp;DEC2HEX(G31,4), DEC2HEX(G31/9*6,4)&amp;"_"&amp;DEC2HEX(G31/9*4,4))</f>
@@ -3804,7 +3831,7 @@
         <v>8</v>
       </c>
       <c r="C32" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32" s="26" t="s">
         <v>82</v>
@@ -3829,7 +3856,7 @@
         <v>1</v>
       </c>
       <c r="K32" s="26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L32" s="26">
         <v>28</v>
@@ -3856,7 +3883,7 @@
       </c>
       <c r="R32" s="45" t="str">
         <f t="shared" si="39"/>
-        <v>0120_0111</v>
+        <v>0120_0112</v>
       </c>
       <c r="S32" s="12" t="str">
         <f t="shared" si="40"/>
@@ -4008,7 +4035,7 @@
       <c r="I35" s="25"/>
       <c r="J35" s="25"/>
       <c r="K35" s="25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L35" s="25"/>
       <c r="M35" s="25"/>
@@ -4066,7 +4093,7 @@
         <v>0</v>
       </c>
       <c r="K36" s="28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L36" s="28">
         <v>14</v>
@@ -4172,7 +4199,7 @@
         <v>0</v>
       </c>
       <c r="K37" s="26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L37" s="26">
         <v>14</v>
@@ -4304,7 +4331,7 @@
         <v>8</v>
       </c>
       <c r="C39" s="26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D39" s="26" t="s">
         <v>86</v>
@@ -4329,7 +4356,7 @@
         <v>0</v>
       </c>
       <c r="K39" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L39" s="26">
         <v>14</v>
@@ -4356,7 +4383,7 @@
       </c>
       <c r="R39" s="45" t="str">
         <f t="shared" ref="R39:R40" si="50">DEC2HEX(G39,4)&amp;"_0"&amp;DEC2HEX(I39,1)&amp;DEC2HEX(J39,1)&amp;DEC2HEX(C39,1)</f>
-        <v>0030_0102</v>
+        <v>0030_0101</v>
       </c>
       <c r="S39" s="12" t="str">
         <f t="shared" ref="S39:S40" si="51">IF(J39=0,DEC2HEX(G39,4)&amp;"_"&amp;DEC2HEX(G39,4), DEC2HEX(G39/9*6,4)&amp;"_"&amp;DEC2HEX(G39/9*4,4))</f>
@@ -4422,7 +4449,7 @@
         <v>8</v>
       </c>
       <c r="C40" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D40" s="26" t="s">
         <v>82</v>
@@ -4447,7 +4474,7 @@
         <v>1</v>
       </c>
       <c r="K40" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L40" s="26">
         <v>14</v>
@@ -4474,7 +4501,7 @@
       </c>
       <c r="R40" s="45" t="str">
         <f t="shared" si="50"/>
-        <v>01B0_0111</v>
+        <v>01B0_0112</v>
       </c>
       <c r="S40" s="12" t="str">
         <f t="shared" si="51"/>
@@ -4626,7 +4653,7 @@
       <c r="I43" s="25"/>
       <c r="J43" s="25"/>
       <c r="K43" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L43" s="25">
         <v>14</v>
@@ -4686,7 +4713,7 @@
         <v>0</v>
       </c>
       <c r="K44" s="26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L44" s="26">
         <v>14</v>
@@ -4818,7 +4845,7 @@
         <v>8</v>
       </c>
       <c r="C46" s="26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D46" s="26" t="s">
         <v>86</v>
@@ -4843,7 +4870,7 @@
         <v>0</v>
       </c>
       <c r="K46" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L46" s="26">
         <v>14</v>
@@ -4870,7 +4897,7 @@
       </c>
       <c r="R46" s="45" t="str">
         <f t="shared" ref="R46:R47" si="61">DEC2HEX(G46,4)&amp;"_0"&amp;DEC2HEX(I46,1)&amp;DEC2HEX(J46,1)&amp;DEC2HEX(C46,1)</f>
-        <v>0030_0102</v>
+        <v>0030_0101</v>
       </c>
       <c r="S46" s="12" t="str">
         <f t="shared" ref="S46:S47" si="62">IF(J46=0,DEC2HEX(G46,4)&amp;"_"&amp;DEC2HEX(G46,4), DEC2HEX(G46/9*6,4)&amp;"_"&amp;DEC2HEX(G46/9*4,4))</f>
@@ -4936,7 +4963,7 @@
         <v>8</v>
       </c>
       <c r="C47" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D47" s="26" t="s">
         <v>82</v>
@@ -4961,7 +4988,7 @@
         <v>1</v>
       </c>
       <c r="K47" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L47" s="26">
         <v>14</v>
@@ -4988,7 +5015,7 @@
       </c>
       <c r="R47" s="45" t="str">
         <f t="shared" si="61"/>
-        <v>01B0_0111</v>
+        <v>01B0_0112</v>
       </c>
       <c r="S47" s="12" t="str">
         <f t="shared" si="62"/>
@@ -5140,7 +5167,7 @@
       <c r="I50" s="25"/>
       <c r="J50" s="25"/>
       <c r="K50" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L50" s="25">
         <v>14</v>
@@ -5200,7 +5227,7 @@
         <v>0</v>
       </c>
       <c r="K51" s="26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L51" s="26">
         <v>14</v>
@@ -5332,7 +5359,7 @@
         <v>8</v>
       </c>
       <c r="C53" s="26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D53" s="26" t="s">
         <v>86</v>
@@ -5357,7 +5384,7 @@
         <v>0</v>
       </c>
       <c r="K53" s="26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L53" s="26">
         <v>14</v>
@@ -5384,7 +5411,7 @@
       </c>
       <c r="R53" s="45" t="str">
         <f t="shared" ref="R53:R54" si="72">DEC2HEX(G53,4)&amp;"_0"&amp;DEC2HEX(I53,1)&amp;DEC2HEX(J53,1)&amp;DEC2HEX(C53,1)</f>
-        <v>0040_0102</v>
+        <v>0040_0101</v>
       </c>
       <c r="S53" s="12" t="str">
         <f t="shared" ref="S53:S54" si="73">IF(J53=0,DEC2HEX(G53,4)&amp;"_"&amp;DEC2HEX(G53,4), DEC2HEX(G53/9*6,4)&amp;"_"&amp;DEC2HEX(G53/9*4,4))</f>
@@ -5450,7 +5477,7 @@
         <v>8</v>
       </c>
       <c r="C54" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D54" s="26" t="s">
         <v>82</v>
@@ -5475,7 +5502,7 @@
         <v>1</v>
       </c>
       <c r="K54" s="26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L54" s="26">
         <v>14</v>
@@ -5502,7 +5529,7 @@
       </c>
       <c r="R54" s="45" t="str">
         <f t="shared" si="72"/>
-        <v>0240_0111</v>
+        <v>0240_0112</v>
       </c>
       <c r="S54" s="12" t="str">
         <f t="shared" si="73"/>
@@ -5654,7 +5681,7 @@
       <c r="I57" s="25"/>
       <c r="J57" s="25"/>
       <c r="K57" s="25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L57" s="25">
         <v>14</v>
@@ -5714,7 +5741,7 @@
         <v>0</v>
       </c>
       <c r="K58" s="26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L58" s="26">
         <v>14</v>
@@ -5846,7 +5873,7 @@
         <v>8</v>
       </c>
       <c r="C60" s="26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D60" s="26" t="s">
         <v>86</v>
@@ -5871,7 +5898,7 @@
         <v>0</v>
       </c>
       <c r="K60" s="26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L60" s="26">
         <v>14</v>
@@ -5898,7 +5925,7 @@
       </c>
       <c r="R60" s="45" t="str">
         <f t="shared" ref="R60:R61" si="83">DEC2HEX(G60,4)&amp;"_0"&amp;DEC2HEX(I60,1)&amp;DEC2HEX(J60,1)&amp;DEC2HEX(C60,1)</f>
-        <v>0040_0102</v>
+        <v>0040_0101</v>
       </c>
       <c r="S60" s="12" t="str">
         <f t="shared" ref="S60:S61" si="84">IF(J60=0,DEC2HEX(G60,4)&amp;"_"&amp;DEC2HEX(G60,4), DEC2HEX(G60/9*6,4)&amp;"_"&amp;DEC2HEX(G60/9*4,4))</f>
@@ -5964,7 +5991,7 @@
         <v>8</v>
       </c>
       <c r="C61" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D61" s="26" t="s">
         <v>82</v>
@@ -5989,7 +6016,7 @@
         <v>1</v>
       </c>
       <c r="K61" s="26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L61" s="26">
         <v>14</v>
@@ -6016,7 +6043,7 @@
       </c>
       <c r="R61" s="45" t="str">
         <f t="shared" si="83"/>
-        <v>0240_0111</v>
+        <v>0240_0112</v>
       </c>
       <c r="S61" s="12" t="str">
         <f t="shared" si="84"/>
@@ -6168,7 +6195,7 @@
       <c r="I64" s="25"/>
       <c r="J64" s="25"/>
       <c r="K64" s="25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L64" s="25">
         <v>14</v>
@@ -6267,7 +6294,7 @@
         <v>0</v>
       </c>
       <c r="K66" s="26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L66" s="26">
         <v>14</v>
@@ -6402,7 +6429,7 @@
         <v>5</v>
       </c>
       <c r="D68" s="28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E68" s="28">
         <v>14</v>
@@ -6424,7 +6451,7 @@
         <v>0</v>
       </c>
       <c r="K68" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L68" s="28">
         <v>1</v>
@@ -6656,10 +6683,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E501AE-4D2D-491C-85E4-0C34FDA03C89}">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView zoomScale="76" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="J1" sqref="J1:Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6667,1539 +6694,1747 @@
     <col min="1" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="45" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>199</v>
+        <v>230</v>
       </c>
       <c r="E1" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="H1" t="str">
+      <c r="J1" t="str">
         <f>LEFT(SUBSTITUTE(A1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A1,"_",),4)</f>
         <v>001B 0202</v>
       </c>
-      <c r="I1" t="str">
-        <f t="shared" ref="I1:N1" si="0">LEFT(SUBSTITUTE(B1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B1,"_",),4)</f>
+      <c r="K1" t="str">
+        <f t="shared" ref="K1:Q1" si="0">LEFT(SUBSTITUTE(B1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B1,"_",),4)</f>
         <v>001B 001B</v>
       </c>
-      <c r="J1" t="str">
+      <c r="L1" t="str">
         <f t="shared" si="0"/>
         <v>0040 0003</v>
       </c>
-      <c r="K1" t="str">
+      <c r="M1" t="str">
         <f t="shared" si="0"/>
-        <v>31E1 71E3</v>
-      </c>
-      <c r="L1" t="str">
+        <v>0003 71E3</v>
+      </c>
+      <c r="N1" t="str">
+        <f t="shared" si="0"/>
+        <v>31E1 C949</v>
+      </c>
+      <c r="O1" t="str">
         <f t="shared" si="0"/>
         <v>0000 1000</v>
       </c>
-      <c r="M1" t="str">
+      <c r="P1" t="str">
         <f t="shared" si="0"/>
         <v>000A 0000</v>
       </c>
-      <c r="N1" t="str">
+      <c r="Q1" t="str">
         <f t="shared" si="0"/>
         <v>000C 5BDB</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="47" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>200</v>
+        <v>232</v>
       </c>
       <c r="E2" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="J2" t="str">
+        <f t="shared" ref="J2:J30" si="1">LEFT(SUBSTITUTE(A2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A2,"_",),4)</f>
+        <v>0009 0204</v>
+      </c>
+      <c r="K2" t="str">
+        <f t="shared" ref="K2:K30" si="2">LEFT(SUBSTITUTE(B2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B2,"_",),4)</f>
+        <v>0009 0009</v>
+      </c>
+      <c r="L2" t="str">
+        <f t="shared" ref="L2:L30" si="3">LEFT(SUBSTITUTE(C2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C2,"_",),4)</f>
+        <v>0040 0040</v>
+      </c>
+      <c r="M2" t="str">
+        <f t="shared" ref="M2:M30" si="4">LEFT(SUBSTITUTE(D2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D2,"_",),4)</f>
+        <v>0009 3871</v>
+      </c>
+      <c r="N2" t="str">
+        <f t="shared" ref="N2:N30" si="5">LEFT(SUBSTITUTE(E2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E2,"_",),4)</f>
+        <v>0C40 31E1</v>
+      </c>
+      <c r="O2" t="str">
+        <f t="shared" ref="O2:O30" si="6">LEFT(SUBSTITUTE(F2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F2,"_",),4)</f>
+        <v>0000 0000</v>
+      </c>
+      <c r="P2" t="str">
+        <f t="shared" ref="P2:P30" si="7">LEFT(SUBSTITUTE(G2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(G2,"_",),4)</f>
+        <v>000C 5BDB</v>
+      </c>
+      <c r="Q2" t="str">
+        <f t="shared" ref="Q2:Q30" si="8">LEFT(SUBSTITUTE(H2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(H2,"_",),4)</f>
+        <v>0018 D41B</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" s="45" t="s">
+        <v>204</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="H3" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="F2" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="H2" t="str">
-        <f t="shared" ref="H2:H30" si="1">LEFT(SUBSTITUTE(A2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A2,"_",),4)</f>
-        <v>0009 0204</v>
-      </c>
-      <c r="I2" t="str">
-        <f t="shared" ref="I2:I30" si="2">LEFT(SUBSTITUTE(B2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B2,"_",),4)</f>
-        <v>0009 0009</v>
-      </c>
-      <c r="J2" t="str">
-        <f t="shared" ref="J2:J30" si="3">LEFT(SUBSTITUTE(C2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C2,"_",),4)</f>
-        <v>0040 0040</v>
-      </c>
-      <c r="K2" t="str">
-        <f t="shared" ref="K2:K30" si="4">LEFT(SUBSTITUTE(D2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D2,"_",),4)</f>
-        <v>0C40 3871</v>
-      </c>
-      <c r="L2" t="str">
-        <f t="shared" ref="L2:L30" si="5">LEFT(SUBSTITUTE(E2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E2,"_",),4)</f>
-        <v>0000 0000</v>
-      </c>
-      <c r="M2" t="str">
-        <f t="shared" ref="M2:N30" si="6">LEFT(SUBSTITUTE(F2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F2,"_",),4)</f>
-        <v>000C 5BDB</v>
-      </c>
-      <c r="N2" t="str">
-        <f t="shared" si="6"/>
-        <v>0018 D41B</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="45" t="s">
-        <v>213</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="H3" t="str">
+      <c r="J3" t="str">
         <f t="shared" si="1"/>
         <v>0040 0101</v>
       </c>
-      <c r="I3" t="str">
+      <c r="K3" t="str">
         <f t="shared" si="2"/>
         <v>0040 0040</v>
       </c>
-      <c r="J3" t="str">
+      <c r="L3" t="str">
         <f t="shared" si="3"/>
         <v>0010 0040</v>
       </c>
-      <c r="K3" t="str">
+      <c r="M3" t="str">
         <f t="shared" si="4"/>
-        <v>0C40 3838</v>
-      </c>
-      <c r="L3" t="str">
+        <v>0001 3838</v>
+      </c>
+      <c r="N3" t="str">
         <f t="shared" si="5"/>
+        <v>0C40 0C40</v>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" si="6"/>
         <v>0000 1700</v>
       </c>
-      <c r="M3" t="str">
-        <f t="shared" si="6"/>
+      <c r="P3" t="str">
+        <f t="shared" si="7"/>
         <v>0018 D41B</v>
       </c>
-      <c r="N3" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q3" t="str">
+        <f t="shared" si="8"/>
         <v>001B E41B</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="45" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>201</v>
+        <v>234</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>174</v>
+        <v>235</v>
       </c>
       <c r="F4" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="H4" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="G4" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="H4" t="str">
+      <c r="J4" t="str">
         <f t="shared" si="1"/>
         <v>0010 0102</v>
       </c>
-      <c r="I4" t="str">
+      <c r="K4" t="str">
         <f t="shared" si="2"/>
         <v>0010 0010</v>
       </c>
-      <c r="J4" t="str">
+      <c r="L4" t="str">
         <f t="shared" si="3"/>
         <v>0040 0010</v>
       </c>
-      <c r="K4" t="str">
+      <c r="M4" t="str">
         <f t="shared" si="4"/>
-        <v>0C40 3838</v>
-      </c>
-      <c r="L4" t="str">
+        <v>0001 3838</v>
+      </c>
+      <c r="N4" t="str">
         <f t="shared" si="5"/>
+        <v>0C40 0C40</v>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" si="6"/>
         <v>0000 1B10</v>
       </c>
-      <c r="M4" t="str">
-        <f t="shared" si="6"/>
+      <c r="P4" t="str">
+        <f t="shared" si="7"/>
         <v>001B E41B</v>
       </c>
-      <c r="N4" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q4" t="str">
+        <f t="shared" si="8"/>
         <v>001C A81B</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="45" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>201</v>
+        <v>236</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>175</v>
+        <v>235</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="H5" t="str">
+        <v>173</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="J5" t="str">
         <f t="shared" si="1"/>
         <v>0090 0111</v>
       </c>
-      <c r="I5" t="str">
+      <c r="K5" t="str">
         <f t="shared" si="2"/>
         <v>0060 0040</v>
       </c>
-      <c r="J5" t="str">
+      <c r="L5" t="str">
         <f t="shared" si="3"/>
         <v>0040 0010</v>
       </c>
-      <c r="K5" t="str">
+      <c r="M5" t="str">
         <f t="shared" si="4"/>
-        <v>0C40 3838</v>
-      </c>
-      <c r="L5" t="str">
+        <v>0003 3838</v>
+      </c>
+      <c r="N5" t="str">
         <f t="shared" si="5"/>
+        <v>0C40 0C40</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="6"/>
         <v>0000 1F50</v>
       </c>
-      <c r="M5" t="str">
-        <f t="shared" si="6"/>
+      <c r="P5" t="str">
+        <f t="shared" si="7"/>
         <v>001B E41B</v>
       </c>
-      <c r="N5" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q5" t="str">
+        <f t="shared" si="8"/>
         <v>001F B81B</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="45" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>201</v>
+        <v>234</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>176</v>
+        <v>235</v>
       </c>
       <c r="F6" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="H6" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="G6" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="H6" t="str">
+      <c r="J6" t="str">
         <f t="shared" si="1"/>
         <v>0080 0101</v>
       </c>
-      <c r="I6" t="str">
+      <c r="K6" t="str">
         <f t="shared" si="2"/>
         <v>0080 0080</v>
       </c>
-      <c r="J6" t="str">
+      <c r="L6" t="str">
         <f t="shared" si="3"/>
         <v>0010 0080</v>
       </c>
-      <c r="K6" t="str">
+      <c r="M6" t="str">
         <f t="shared" si="4"/>
-        <v>0C40 3838</v>
-      </c>
-      <c r="L6" t="str">
+        <v>0001 3838</v>
+      </c>
+      <c r="N6" t="str">
         <f t="shared" si="5"/>
+        <v>0C40 0C40</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="6"/>
         <v>0000 4390</v>
       </c>
-      <c r="M6" t="str">
-        <f t="shared" si="6"/>
+      <c r="P6" t="str">
+        <f t="shared" si="7"/>
         <v>001F B81B</v>
       </c>
-      <c r="N6" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q6" t="str">
+        <f t="shared" si="8"/>
         <v>0022 C81B</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="45" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>201</v>
+        <v>234</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>177</v>
+        <v>235</v>
       </c>
       <c r="F7" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="H7" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="G7" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="H7" t="str">
+      <c r="J7" t="str">
         <f t="shared" si="1"/>
         <v>0010 0102</v>
       </c>
-      <c r="I7" t="str">
+      <c r="K7" t="str">
         <f t="shared" si="2"/>
         <v>0010 0010</v>
       </c>
-      <c r="J7" t="str">
+      <c r="L7" t="str">
         <f t="shared" si="3"/>
         <v>0040 0010</v>
       </c>
-      <c r="K7" t="str">
+      <c r="M7" t="str">
         <f t="shared" si="4"/>
-        <v>0C40 3838</v>
-      </c>
-      <c r="L7" t="str">
+        <v>0001 3838</v>
+      </c>
+      <c r="N7" t="str">
         <f t="shared" si="5"/>
+        <v>0C40 0C40</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="6"/>
         <v>0000 4BA0</v>
       </c>
-      <c r="M7" t="str">
-        <f t="shared" si="6"/>
+      <c r="P7" t="str">
+        <f t="shared" si="7"/>
         <v>0022 C81B</v>
       </c>
-      <c r="N7" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q7" t="str">
+        <f t="shared" si="8"/>
         <v>0023 8C1B</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="45" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>201</v>
+        <v>236</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>178</v>
+        <v>235</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="H8" t="str">
+        <v>176</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="J8" t="str">
         <f t="shared" si="1"/>
         <v>0090 0111</v>
       </c>
-      <c r="I8" t="str">
+      <c r="K8" t="str">
         <f t="shared" si="2"/>
         <v>0060 0040</v>
       </c>
-      <c r="J8" t="str">
+      <c r="L8" t="str">
         <f t="shared" si="3"/>
         <v>0040 0010</v>
       </c>
-      <c r="K8" t="str">
+      <c r="M8" t="str">
         <f t="shared" si="4"/>
-        <v>0C40 3838</v>
-      </c>
-      <c r="L8" t="str">
+        <v>0003 3838</v>
+      </c>
+      <c r="N8" t="str">
         <f t="shared" si="5"/>
+        <v>0C40 0C40</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="6"/>
         <v>0000 4FE0</v>
       </c>
-      <c r="M8" t="str">
-        <f t="shared" si="6"/>
+      <c r="P8" t="str">
+        <f t="shared" si="7"/>
         <v>0022 C81B</v>
       </c>
-      <c r="N8" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q8" t="str">
+        <f t="shared" si="8"/>
         <v>0026 9C1B</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="47" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>202</v>
+        <v>237</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>136</v>
+        <v>238</v>
       </c>
       <c r="F9" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="H9" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="G9" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="H9" t="str">
+      <c r="J9" t="str">
         <f t="shared" si="1"/>
         <v>0009 0204</v>
       </c>
-      <c r="I9" t="str">
+      <c r="K9" t="str">
         <f t="shared" si="2"/>
         <v>0009 0009</v>
       </c>
-      <c r="J9" t="str">
+      <c r="L9" t="str">
         <f t="shared" si="3"/>
         <v>0080 0080</v>
       </c>
-      <c r="K9" t="str">
+      <c r="M9" t="str">
         <f t="shared" si="4"/>
-        <v>0310 1C38</v>
-      </c>
-      <c r="L9" t="str">
+        <v>0003 1C38</v>
+      </c>
+      <c r="N9" t="str">
         <f t="shared" si="5"/>
+        <v>0310 0C40</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="6"/>
         <v>0000 0000</v>
       </c>
-      <c r="M9" t="str">
-        <f t="shared" si="6"/>
+      <c r="P9" t="str">
+        <f t="shared" si="7"/>
         <v>0026 9C1B</v>
       </c>
-      <c r="N9" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q9" t="str">
+        <f t="shared" si="8"/>
         <v>0029 AC1B</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="45" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>203</v>
+        <v>239</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>179</v>
+        <v>240</v>
       </c>
       <c r="F10" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="H10" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="G10" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="H10" t="str">
+      <c r="J10" t="str">
         <f t="shared" si="1"/>
         <v>0080 0101</v>
       </c>
-      <c r="I10" t="str">
+      <c r="K10" t="str">
         <f t="shared" si="2"/>
         <v>0080 0080</v>
       </c>
-      <c r="J10" t="str">
+      <c r="L10" t="str">
         <f t="shared" si="3"/>
         <v>0020 0080</v>
       </c>
-      <c r="K10" t="str">
+      <c r="M10" t="str">
         <f t="shared" si="4"/>
-        <v>0310 1C1C</v>
-      </c>
-      <c r="L10" t="str">
+        <v>0001 1C1C</v>
+      </c>
+      <c r="N10" t="str">
         <f t="shared" si="5"/>
+        <v>0310 0310</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="6"/>
         <v>0000 7420</v>
       </c>
-      <c r="M10" t="str">
-        <f t="shared" si="6"/>
+      <c r="P10" t="str">
+        <f t="shared" si="7"/>
         <v>0029 AC1B</v>
       </c>
-      <c r="N10" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q10" t="str">
+        <f t="shared" si="8"/>
         <v>002B 341B</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="45" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>203</v>
+        <v>239</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="F11" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="H11" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="G11" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="H11" t="str">
+      <c r="J11" t="str">
         <f t="shared" si="1"/>
         <v>0020 0102</v>
       </c>
-      <c r="I11" t="str">
+      <c r="K11" t="str">
         <f t="shared" si="2"/>
         <v>0020 0020</v>
       </c>
-      <c r="J11" t="str">
+      <c r="L11" t="str">
         <f t="shared" si="3"/>
         <v>0080 0020</v>
       </c>
-      <c r="K11" t="str">
+      <c r="M11" t="str">
         <f t="shared" si="4"/>
-        <v>0310 1C1C</v>
-      </c>
-      <c r="L11" t="str">
+        <v>0001 1C1C</v>
+      </c>
+      <c r="N11" t="str">
         <f t="shared" si="5"/>
+        <v>0310 0310</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="6"/>
         <v>0000 8440</v>
       </c>
-      <c r="M11" t="str">
-        <f t="shared" si="6"/>
+      <c r="P11" t="str">
+        <f t="shared" si="7"/>
         <v>002B 341B</v>
       </c>
-      <c r="N11" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q11" t="str">
+        <f t="shared" si="8"/>
         <v>002B 961B</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="45" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>203</v>
+        <v>241</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>181</v>
+        <v>240</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="H12" t="str">
+        <v>179</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="J12" t="str">
         <f t="shared" si="1"/>
         <v>0120 0111</v>
       </c>
-      <c r="I12" t="str">
+      <c r="K12" t="str">
         <f t="shared" si="2"/>
         <v>00C0 0080</v>
       </c>
-      <c r="J12" t="str">
+      <c r="L12" t="str">
         <f t="shared" si="3"/>
         <v>0080 0020</v>
       </c>
-      <c r="K12" t="str">
+      <c r="M12" t="str">
         <f t="shared" si="4"/>
-        <v>0310 1C1C</v>
-      </c>
-      <c r="L12" t="str">
+        <v>0003 1C1C</v>
+      </c>
+      <c r="N12" t="str">
         <f t="shared" si="5"/>
+        <v>0310 0310</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="6"/>
         <v>0000 94C0</v>
       </c>
-      <c r="M12" t="str">
-        <f t="shared" si="6"/>
+      <c r="P12" t="str">
+        <f t="shared" si="7"/>
         <v>002B 341B</v>
       </c>
-      <c r="N12" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q12" t="str">
+        <f t="shared" si="8"/>
         <v>002D 1E1B</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="45" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>203</v>
+        <v>239</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>182</v>
+        <v>240</v>
       </c>
       <c r="F13" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="H13" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="G13" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="H13" t="str">
+      <c r="J13" t="str">
         <f t="shared" si="1"/>
         <v>0100 0101</v>
       </c>
-      <c r="I13" t="str">
+      <c r="K13" t="str">
         <f t="shared" si="2"/>
         <v>0100 0100</v>
       </c>
-      <c r="J13" t="str">
+      <c r="L13" t="str">
         <f t="shared" si="3"/>
         <v>0020 0100</v>
       </c>
-      <c r="K13" t="str">
+      <c r="M13" t="str">
         <f t="shared" si="4"/>
-        <v>0310 1C1C</v>
-      </c>
-      <c r="L13" t="str">
+        <v>0001 1C1C</v>
+      </c>
+      <c r="N13" t="str">
         <f t="shared" si="5"/>
+        <v>0310 0310</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="6"/>
         <v>0001 2540</v>
       </c>
-      <c r="M13" t="str">
-        <f t="shared" si="6"/>
+      <c r="P13" t="str">
+        <f t="shared" si="7"/>
         <v>002D 1E1B</v>
       </c>
-      <c r="N13" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q13" t="str">
+        <f t="shared" si="8"/>
         <v>002E A61B</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="45" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>203</v>
+        <v>239</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>183</v>
+        <v>240</v>
       </c>
       <c r="F14" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="H14" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="G14" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="H14" t="str">
+      <c r="J14" t="str">
         <f t="shared" si="1"/>
         <v>0020 0102</v>
       </c>
-      <c r="I14" t="str">
+      <c r="K14" t="str">
         <f t="shared" si="2"/>
         <v>0020 0020</v>
       </c>
-      <c r="J14" t="str">
+      <c r="L14" t="str">
         <f t="shared" si="3"/>
         <v>0080 0020</v>
       </c>
-      <c r="K14" t="str">
+      <c r="M14" t="str">
         <f t="shared" si="4"/>
-        <v>0310 1C1C</v>
-      </c>
-      <c r="L14" t="str">
+        <v>0001 1C1C</v>
+      </c>
+      <c r="N14" t="str">
         <f t="shared" si="5"/>
+        <v>0310 0310</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="6"/>
         <v>0001 4560</v>
       </c>
-      <c r="M14" t="str">
-        <f t="shared" si="6"/>
+      <c r="P14" t="str">
+        <f t="shared" si="7"/>
         <v>002E A61B</v>
       </c>
-      <c r="N14" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q14" t="str">
+        <f t="shared" si="8"/>
         <v>002F 081B</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="45" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>203</v>
+        <v>241</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>184</v>
+        <v>240</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="H15" t="str">
+        <v>182</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="J15" t="str">
         <f t="shared" si="1"/>
         <v>0120 0111</v>
       </c>
-      <c r="I15" t="str">
+      <c r="K15" t="str">
         <f t="shared" si="2"/>
         <v>00C0 0080</v>
       </c>
-      <c r="J15" t="str">
+      <c r="L15" t="str">
         <f t="shared" si="3"/>
         <v>0080 0020</v>
       </c>
-      <c r="K15" t="str">
+      <c r="M15" t="str">
         <f t="shared" si="4"/>
-        <v>0310 1C1C</v>
-      </c>
-      <c r="L15" t="str">
+        <v>0003 1C1C</v>
+      </c>
+      <c r="N15" t="str">
         <f t="shared" si="5"/>
+        <v>0310 0310</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="6"/>
         <v>0001 55E0</v>
       </c>
-      <c r="M15" t="str">
-        <f t="shared" si="6"/>
+      <c r="P15" t="str">
+        <f t="shared" si="7"/>
         <v>002E A61B</v>
       </c>
-      <c r="N15" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q15" t="str">
+        <f t="shared" si="8"/>
         <v>0030 901B</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="47" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>204</v>
+        <v>242</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>136</v>
+        <v>243</v>
       </c>
       <c r="F16" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="H16" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="G16" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="H16" t="str">
+      <c r="J16" t="str">
         <f t="shared" si="1"/>
         <v>0009 0204</v>
       </c>
-      <c r="I16" t="str">
+      <c r="K16" t="str">
         <f t="shared" si="2"/>
         <v>0009 0009</v>
       </c>
-      <c r="J16" t="str">
+      <c r="L16" t="str">
         <f t="shared" si="3"/>
         <v>0100 0100</v>
       </c>
-      <c r="K16" t="str">
+      <c r="M16" t="str">
         <f t="shared" si="4"/>
-        <v>00C4 0E1C</v>
-      </c>
-      <c r="L16" t="str">
+        <v>0003 0E1C</v>
+      </c>
+      <c r="N16" t="str">
         <f t="shared" si="5"/>
+        <v>00C4 0310</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="6"/>
         <v>0000 0000</v>
       </c>
-      <c r="M16" t="str">
-        <f t="shared" si="6"/>
+      <c r="P16" t="str">
+        <f t="shared" si="7"/>
         <v>0030 901B</v>
       </c>
-      <c r="N16" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q16" t="str">
+        <f t="shared" si="8"/>
         <v>0032 181B</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="45" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>205</v>
+        <v>244</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>185</v>
+        <v>227</v>
       </c>
       <c r="F17" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="H17" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="G17" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="H17" t="str">
+      <c r="J17" t="str">
         <f t="shared" si="1"/>
         <v>0100 0101</v>
       </c>
-      <c r="I17" t="str">
+      <c r="K17" t="str">
         <f t="shared" si="2"/>
         <v>0100 0100</v>
       </c>
-      <c r="J17" t="str">
+      <c r="L17" t="str">
         <f t="shared" si="3"/>
         <v>0030 0100</v>
       </c>
-      <c r="K17" t="str">
+      <c r="M17" t="str">
         <f t="shared" si="4"/>
-        <v>00C4 0E0E</v>
-      </c>
-      <c r="L17" t="str">
+        <v>0001 0E0E</v>
+      </c>
+      <c r="N17" t="str">
         <f t="shared" si="5"/>
+        <v>00C4 00C4</v>
+      </c>
+      <c r="O17" t="str">
+        <f t="shared" si="6"/>
         <v>0001 E660</v>
       </c>
-      <c r="M17" t="str">
-        <f t="shared" si="6"/>
+      <c r="P17" t="str">
+        <f t="shared" si="7"/>
         <v>0032 181B</v>
       </c>
-      <c r="N17" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q17" t="str">
+        <f t="shared" si="8"/>
         <v>0032 DC1B</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="45" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>205</v>
+        <v>244</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="F18" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="H18" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="G18" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="H18" t="str">
+      <c r="J18" t="str">
         <f t="shared" si="1"/>
         <v>0030 0102</v>
       </c>
-      <c r="I18" t="str">
+      <c r="K18" t="str">
         <f t="shared" si="2"/>
         <v>0030 0030</v>
       </c>
-      <c r="J18" t="str">
+      <c r="L18" t="str">
         <f t="shared" si="3"/>
         <v>00C0 0030</v>
       </c>
-      <c r="K18" t="str">
+      <c r="M18" t="str">
         <f t="shared" si="4"/>
-        <v>00C4 0E0E</v>
-      </c>
-      <c r="L18" t="str">
+        <v>0001 0E0E</v>
+      </c>
+      <c r="N18" t="str">
         <f t="shared" si="5"/>
+        <v>00C4 00C4</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="6"/>
         <v>0002 1690</v>
       </c>
-      <c r="M18" t="str">
-        <f t="shared" si="6"/>
+      <c r="P18" t="str">
+        <f t="shared" si="7"/>
         <v>0032 DC1B</v>
       </c>
-      <c r="N18" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q18" t="str">
+        <f t="shared" si="8"/>
         <v>0033 00DB</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="45" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="B19" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="E19" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="F19" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="H19" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="H19" t="str">
+      <c r="J19" t="str">
         <f t="shared" si="1"/>
         <v>01B0 0111</v>
       </c>
-      <c r="I19" t="str">
+      <c r="K19" t="str">
         <f t="shared" si="2"/>
         <v>0120 00C0</v>
       </c>
-      <c r="J19" t="str">
+      <c r="L19" t="str">
         <f t="shared" si="3"/>
         <v>00C0 0030</v>
       </c>
-      <c r="K19" t="str">
+      <c r="M19" t="str">
         <f t="shared" si="4"/>
-        <v>00C4 0E0E</v>
-      </c>
-      <c r="L19" t="str">
+        <v>0003 0E0E</v>
+      </c>
+      <c r="N19" t="str">
         <f t="shared" si="5"/>
+        <v>00C4 00C4</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="6"/>
         <v>0002 3B50</v>
       </c>
-      <c r="M19" t="str">
-        <f t="shared" si="6"/>
+      <c r="P19" t="str">
+        <f t="shared" si="7"/>
         <v>0032 DC1B</v>
       </c>
-      <c r="N19" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q19" t="str">
+        <f t="shared" si="8"/>
         <v>0033 93DB</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="45" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>205</v>
+        <v>244</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>188</v>
+        <v>227</v>
       </c>
       <c r="F20" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="H20" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="G20" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="H20" t="str">
+      <c r="J20" t="str">
         <f t="shared" si="1"/>
         <v>0180 0101</v>
       </c>
-      <c r="I20" t="str">
+      <c r="K20" t="str">
         <f t="shared" si="2"/>
         <v>0180 0180</v>
       </c>
-      <c r="J20" t="str">
+      <c r="L20" t="str">
         <f t="shared" si="3"/>
         <v>0030 0180</v>
       </c>
-      <c r="K20" t="str">
+      <c r="M20" t="str">
         <f t="shared" si="4"/>
-        <v>00C4 0E0E</v>
-      </c>
-      <c r="L20" t="str">
+        <v>0001 0E0E</v>
+      </c>
+      <c r="N20" t="str">
         <f t="shared" si="5"/>
+        <v>00C4 00C4</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="6"/>
         <v>0003 8010</v>
       </c>
-      <c r="M20" t="str">
-        <f t="shared" si="6"/>
+      <c r="P20" t="str">
+        <f t="shared" si="7"/>
         <v>0033 93DB</v>
       </c>
-      <c r="N20" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q20" t="str">
+        <f t="shared" si="8"/>
         <v>0034 26DB</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="45" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>205</v>
+        <v>244</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>189</v>
+        <v>227</v>
       </c>
       <c r="F21" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="H21" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="G21" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="H21" t="str">
+      <c r="J21" t="str">
         <f t="shared" si="1"/>
         <v>0030 0102</v>
       </c>
-      <c r="I21" t="str">
+      <c r="K21" t="str">
         <f t="shared" si="2"/>
         <v>0030 0030</v>
       </c>
-      <c r="J21" t="str">
+      <c r="L21" t="str">
         <f t="shared" si="3"/>
         <v>00C0 0030</v>
       </c>
-      <c r="K21" t="str">
+      <c r="M21" t="str">
         <f t="shared" si="4"/>
-        <v>00C4 0E0E</v>
-      </c>
-      <c r="L21" t="str">
+        <v>0001 0E0E</v>
+      </c>
+      <c r="N21" t="str">
         <f t="shared" si="5"/>
+        <v>00C4 00C4</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="6"/>
         <v>0003 C840</v>
       </c>
-      <c r="M21" t="str">
-        <f t="shared" si="6"/>
+      <c r="P21" t="str">
+        <f t="shared" si="7"/>
         <v>0034 26DB</v>
       </c>
-      <c r="N21" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q21" t="str">
+        <f t="shared" si="8"/>
         <v>0034 4B9B</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="45" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="B22" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="E22" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>190</v>
-      </c>
       <c r="F22" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="H22" t="str">
+        <v>188</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="J22" t="str">
         <f t="shared" si="1"/>
         <v>01B0 0111</v>
       </c>
-      <c r="I22" t="str">
+      <c r="K22" t="str">
         <f t="shared" si="2"/>
         <v>0120 00C0</v>
       </c>
-      <c r="J22" t="str">
+      <c r="L22" t="str">
         <f t="shared" si="3"/>
         <v>00C0 0030</v>
       </c>
-      <c r="K22" t="str">
+      <c r="M22" t="str">
         <f t="shared" si="4"/>
-        <v>00C4 0E0E</v>
-      </c>
-      <c r="L22" t="str">
+        <v>0003 0E0E</v>
+      </c>
+      <c r="N22" t="str">
         <f t="shared" si="5"/>
+        <v>00C4 00C4</v>
+      </c>
+      <c r="O22" t="str">
+        <f t="shared" si="6"/>
         <v>0003 ED00</v>
       </c>
-      <c r="M22" t="str">
-        <f t="shared" si="6"/>
+      <c r="P22" t="str">
+        <f t="shared" si="7"/>
         <v>0034 26DB</v>
       </c>
-      <c r="N22" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q22" t="str">
+        <f t="shared" si="8"/>
         <v>0034 DE9B</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="45" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>205</v>
+        <v>244</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>191</v>
+        <v>227</v>
       </c>
       <c r="F23" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="H23" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="G23" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="H23" t="str">
+      <c r="J23" t="str">
         <f t="shared" si="1"/>
         <v>0180 0101</v>
       </c>
-      <c r="I23" t="str">
+      <c r="K23" t="str">
         <f t="shared" si="2"/>
         <v>0180 0180</v>
       </c>
-      <c r="J23" t="str">
+      <c r="L23" t="str">
         <f t="shared" si="3"/>
         <v>0040 0180</v>
       </c>
-      <c r="K23" t="str">
+      <c r="M23" t="str">
         <f t="shared" si="4"/>
-        <v>00C4 0E0E</v>
-      </c>
-      <c r="L23" t="str">
+        <v>0001 0E0E</v>
+      </c>
+      <c r="N23" t="str">
         <f t="shared" si="5"/>
+        <v>00C4 00C4</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="6"/>
         <v>0005 31C0</v>
       </c>
-      <c r="M23" t="str">
-        <f t="shared" si="6"/>
+      <c r="P23" t="str">
+        <f t="shared" si="7"/>
         <v>0034 DE9B</v>
       </c>
-      <c r="N23" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q23" t="str">
+        <f t="shared" si="8"/>
         <v>0035 719B</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="45" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>205</v>
+        <v>244</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>192</v>
+        <v>227</v>
       </c>
       <c r="F24" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="H24" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="G24" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="H24" t="str">
+      <c r="J24" t="str">
         <f t="shared" si="1"/>
         <v>0040 0102</v>
       </c>
-      <c r="I24" t="str">
+      <c r="K24" t="str">
         <f t="shared" si="2"/>
         <v>0040 0040</v>
       </c>
-      <c r="J24" t="str">
+      <c r="L24" t="str">
         <f t="shared" si="3"/>
         <v>0100 0040</v>
       </c>
-      <c r="K24" t="str">
+      <c r="M24" t="str">
         <f t="shared" si="4"/>
-        <v>00C4 0E0E</v>
-      </c>
-      <c r="L24" t="str">
+        <v>0001 0E0E</v>
+      </c>
+      <c r="N24" t="str">
         <f t="shared" si="5"/>
+        <v>00C4 00C4</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="6"/>
         <v>0005 9200</v>
       </c>
-      <c r="M24" t="str">
-        <f t="shared" si="6"/>
+      <c r="P24" t="str">
+        <f t="shared" si="7"/>
         <v>0035 719B</v>
       </c>
-      <c r="N24" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q24" t="str">
+        <f t="shared" si="8"/>
         <v>0035 A29B</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="45" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>205</v>
+        <v>245</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>193</v>
+        <v>227</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="H25" t="str">
+        <v>191</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="J25" t="str">
         <f t="shared" si="1"/>
         <v>0240 0111</v>
       </c>
-      <c r="I25" t="str">
+      <c r="K25" t="str">
         <f t="shared" si="2"/>
         <v>0180 0100</v>
       </c>
-      <c r="J25" t="str">
+      <c r="L25" t="str">
         <f t="shared" si="3"/>
         <v>0100 0040</v>
       </c>
-      <c r="K25" t="str">
+      <c r="M25" t="str">
         <f t="shared" si="4"/>
-        <v>00C4 0E0E</v>
-      </c>
-      <c r="L25" t="str">
+        <v>0003 0E0E</v>
+      </c>
+      <c r="N25" t="str">
         <f t="shared" si="5"/>
+        <v>00C4 00C4</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="6"/>
         <v>0005 D300</v>
       </c>
-      <c r="M25" t="str">
-        <f t="shared" si="6"/>
+      <c r="P25" t="str">
+        <f t="shared" si="7"/>
         <v>0035 719B</v>
       </c>
-      <c r="N25" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q25" t="str">
+        <f t="shared" si="8"/>
         <v>0036 669B</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="45" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>205</v>
+        <v>244</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>194</v>
+        <v>227</v>
       </c>
       <c r="F26" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="H26" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="G26" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="H26" t="str">
+      <c r="J26" t="str">
         <f t="shared" si="1"/>
         <v>0200 0101</v>
       </c>
-      <c r="I26" t="str">
+      <c r="K26" t="str">
         <f t="shared" si="2"/>
         <v>0200 0200</v>
       </c>
-      <c r="J26" t="str">
+      <c r="L26" t="str">
         <f t="shared" si="3"/>
         <v>0040 0200</v>
       </c>
-      <c r="K26" t="str">
+      <c r="M26" t="str">
         <f t="shared" si="4"/>
-        <v>00C4 0E0E</v>
-      </c>
-      <c r="L26" t="str">
+        <v>0001 0E0E</v>
+      </c>
+      <c r="N26" t="str">
         <f t="shared" si="5"/>
+        <v>00C4 00C4</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="6"/>
         <v>0008 1400</v>
       </c>
-      <c r="M26" t="str">
-        <f t="shared" si="6"/>
+      <c r="P26" t="str">
+        <f t="shared" si="7"/>
         <v>0036 669B</v>
       </c>
-      <c r="N26" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q26" t="str">
+        <f t="shared" si="8"/>
         <v>0037 2A9B</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="45" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>205</v>
+        <v>244</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>195</v>
+        <v>227</v>
       </c>
       <c r="F27" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="H27" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="G27" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="H27" t="str">
+      <c r="J27" t="str">
         <f t="shared" si="1"/>
         <v>0040 0102</v>
       </c>
-      <c r="I27" t="str">
+      <c r="K27" t="str">
         <f t="shared" si="2"/>
         <v>0040 0040</v>
       </c>
-      <c r="J27" t="str">
+      <c r="L27" t="str">
         <f t="shared" si="3"/>
         <v>0100 0040</v>
       </c>
-      <c r="K27" t="str">
+      <c r="M27" t="str">
         <f t="shared" si="4"/>
-        <v>00C4 0E0E</v>
-      </c>
-      <c r="L27" t="str">
+        <v>0001 0E0E</v>
+      </c>
+      <c r="N27" t="str">
         <f t="shared" si="5"/>
+        <v>00C4 00C4</v>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="6"/>
         <v>0008 9440</v>
       </c>
-      <c r="M27" t="str">
-        <f t="shared" si="6"/>
+      <c r="P27" t="str">
+        <f t="shared" si="7"/>
         <v>0037 2A9B</v>
       </c>
-      <c r="N27" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q27" t="str">
+        <f t="shared" si="8"/>
         <v>0037 5B9B</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="45" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>205</v>
+        <v>245</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>196</v>
+        <v>227</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="H28" t="str">
+        <v>194</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="J28" t="str">
         <f t="shared" si="1"/>
         <v>0240 0111</v>
       </c>
-      <c r="I28" t="str">
+      <c r="K28" t="str">
         <f t="shared" si="2"/>
         <v>0180 0100</v>
       </c>
-      <c r="J28" t="str">
+      <c r="L28" t="str">
         <f t="shared" si="3"/>
         <v>0100 0040</v>
       </c>
-      <c r="K28" t="str">
+      <c r="M28" t="str">
         <f t="shared" si="4"/>
-        <v>00C4 0E0E</v>
-      </c>
-      <c r="L28" t="str">
+        <v>0003 0E0E</v>
+      </c>
+      <c r="N28" t="str">
         <f t="shared" si="5"/>
+        <v>00C4 00C4</v>
+      </c>
+      <c r="O28" t="str">
+        <f t="shared" si="6"/>
         <v>0008 D540</v>
       </c>
-      <c r="M28" t="str">
-        <f t="shared" si="6"/>
+      <c r="P28" t="str">
+        <f t="shared" si="7"/>
         <v>0037 2A9B</v>
       </c>
-      <c r="N28" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q28" t="str">
+        <f t="shared" si="8"/>
         <v>0038 1F9B</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="45" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>205</v>
+        <v>244</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>197</v>
+        <v>227</v>
       </c>
       <c r="F29" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="H29" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="G29" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="H29" t="str">
+      <c r="J29" t="str">
         <f t="shared" si="1"/>
         <v>0200 0101</v>
       </c>
-      <c r="I29" t="str">
+      <c r="K29" t="str">
         <f t="shared" si="2"/>
         <v>0200 0200</v>
       </c>
-      <c r="J29" t="str">
+      <c r="L29" t="str">
         <f t="shared" si="3"/>
         <v>03E8 0200</v>
       </c>
-      <c r="K29" t="str">
+      <c r="M29" t="str">
         <f t="shared" si="4"/>
-        <v>00C4 0E0E</v>
-      </c>
-      <c r="L29" t="str">
+        <v>0001 0E0E</v>
+      </c>
+      <c r="N29" t="str">
         <f t="shared" si="5"/>
+        <v>00C4 00C4</v>
+      </c>
+      <c r="O29" t="str">
+        <f t="shared" si="6"/>
         <v>000B 1640</v>
       </c>
-      <c r="M29" t="str">
-        <f t="shared" si="6"/>
+      <c r="P29" t="str">
+        <f t="shared" si="7"/>
         <v>0038 1F9B</v>
       </c>
-      <c r="N29" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q29" t="str">
+        <f t="shared" si="8"/>
         <v>0038 E39B</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="47" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>170</v>
+        <v>246</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>136</v>
+        <v>247</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="G30" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="H30" t="str">
+        <v>135</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="H30" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="J30" t="str">
         <f t="shared" si="1"/>
         <v>00C4 0105</v>
       </c>
-      <c r="I30" t="str">
+      <c r="K30" t="str">
         <f t="shared" si="2"/>
         <v>00C4 00C4</v>
       </c>
-      <c r="J30" t="str">
+      <c r="L30" t="str">
         <f t="shared" si="3"/>
         <v>03E8 03E8</v>
       </c>
-      <c r="K30" t="str">
+      <c r="M30" t="str">
         <f t="shared" si="4"/>
-        <v>0001 010E</v>
-      </c>
-      <c r="L30" t="str">
+        <v>000E 010E</v>
+      </c>
+      <c r="N30" t="str">
         <f t="shared" si="5"/>
+        <v>0001 00C4</v>
+      </c>
+      <c r="O30" t="str">
+        <f t="shared" si="6"/>
         <v>0000 0000</v>
       </c>
-      <c r="M30" t="str">
-        <f t="shared" si="6"/>
+      <c r="P30" t="str">
+        <f t="shared" si="7"/>
         <v>0038 E39B</v>
       </c>
-      <c r="N30" t="str">
-        <f t="shared" si="6"/>
+      <c r="Q30" t="str">
+        <f t="shared" si="8"/>
         <v>003B E13B</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Optimize cmac, sacc and scmp, calculation in 1 cycle, not synthesized
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1ACE564-8279-4FC1-8858-C10647F65CAF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B084B7-49E8-4C7D-9E3C-726BD20C7A66}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
   <sheets>
     <sheet name="SqueezeNet v2 MEC Parallel Ch" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="248">
   <si>
     <t>INPUT</t>
   </si>
@@ -776,6 +776,9 @@
   </si>
   <si>
     <t>0001_00C4</t>
+  </si>
+  <si>
+    <t>Operation Time</t>
   </si>
 </sst>
 </file>
@@ -1060,10 +1063,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1410,10 +1413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80B23C6-EAEB-43B1-B045-456C36085CFA}">
-  <dimension ref="A1:AF71"/>
+  <dimension ref="A1:AG71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R34" zoomScale="77" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AD4" sqref="AD4"/>
+    <sheetView tabSelected="1" topLeftCell="K49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AF71" sqref="AF71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1444,12 +1447,14 @@
     <col min="26" max="26" width="7.81640625" style="37" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="8.81640625" style="43" customWidth="1"/>
     <col min="28" max="28" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" s="21"/>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -1485,14 +1490,15 @@
       <c r="Y1" s="57"/>
       <c r="Z1" s="57"/>
       <c r="AA1" s="58"/>
-      <c r="AB1" s="52" t="s">
+      <c r="AB1" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AC1" s="54"/>
+      <c r="AD1" s="54"/>
+      <c r="AE1" s="54"/>
+      <c r="AF1" s="54"/>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
@@ -1569,16 +1575,19 @@
         <v>88</v>
       </c>
       <c r="AD2" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE2" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="AE2" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="AF2" s="20" t="s">
+      <c r="AF2" s="52" t="s">
+        <v>247</v>
+      </c>
+      <c r="AG2" s="20" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1621,16 +1630,14 @@
       <c r="AA3" s="11"/>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
-      <c r="AD3" s="1">
-        <f>M3/64*0.97</f>
-        <v>2342.9592187499998</v>
-      </c>
+      <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
-      <c r="AF3" s="20" t="s">
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="20" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -1727,22 +1734,26 @@
         <v>000C5BDB</v>
       </c>
       <c r="AB4" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC4" s="2">
         <v>6.25E-2</v>
       </c>
       <c r="AD4" s="2">
+        <f>M4*G4</f>
+        <v>22064832</v>
+      </c>
+      <c r="AE4" s="2">
         <f>M4*G4*0.03</f>
         <v>661944.96</v>
       </c>
-      <c r="AE4" s="2">
+      <c r="AF4" s="2">
         <f>M4*G4*AB4*AC4</f>
-        <v>275810.40000000002</v>
-      </c>
-      <c r="AF4" s="20"/>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+        <v>13790.52</v>
+      </c>
+      <c r="AG4" s="20"/>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
@@ -1778,9 +1789,10 @@
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
       <c r="AE5" s="3"/>
-      <c r="AF5" s="20"/>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="20"/>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
@@ -1867,22 +1879,26 @@
         <v>0018D41B</v>
       </c>
       <c r="AB6" s="4">
-        <v>0.31</v>
+        <v>0.1</v>
       </c>
       <c r="AC6" s="4">
         <v>6.25E-2</v>
       </c>
       <c r="AD6" s="4">
+        <f>M6*G6</f>
+        <v>1806336</v>
+      </c>
+      <c r="AE6" s="4">
         <f>M6*G6*0.03</f>
         <v>54190.079999999994</v>
       </c>
-      <c r="AE6" s="4">
-        <f>M6*G6*AC6</f>
-        <v>112896</v>
-      </c>
-      <c r="AF6" s="20"/>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF6" s="4">
+        <f>M6*G6*AB6*AC6</f>
+        <v>11289.6</v>
+      </c>
+      <c r="AG6" s="20"/>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1981,22 +1997,26 @@
         <v>001BE41B</v>
       </c>
       <c r="AB7" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC7" s="2">
         <v>6.25E-2</v>
       </c>
       <c r="AD7" s="2">
+        <f>M7*G7</f>
+        <v>3211264</v>
+      </c>
+      <c r="AE7" s="2">
         <f>M7*G7*0.03</f>
         <v>96337.919999999998</v>
       </c>
-      <c r="AE7" s="2">
+      <c r="AF7" s="2">
         <f>M7*G7*AB7*AC7</f>
-        <v>40140.800000000003</v>
-      </c>
-      <c r="AF7" s="20"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
+        <v>2007.04</v>
+      </c>
+      <c r="AG7" s="20"/>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
@@ -2032,9 +2052,10 @@
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
       <c r="AE8" s="3"/>
-      <c r="AF8" s="20"/>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF8" s="3"/>
+      <c r="AG8" s="20"/>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -2133,22 +2154,26 @@
         <v>001CA81B</v>
       </c>
       <c r="AB9" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC9" s="2">
         <v>0</v>
       </c>
       <c r="AD9" s="2">
-        <f t="shared" ref="AD9:AD10" si="6">M9*G9*0.03</f>
+        <f>M9*G9</f>
+        <v>3211264</v>
+      </c>
+      <c r="AE9" s="2">
+        <f t="shared" ref="AE9:AE10" si="6">M9*G9*0.03</f>
         <v>96337.919999999998</v>
       </c>
-      <c r="AE9" s="2">
-        <f>M9*G9*AB9*AC9</f>
+      <c r="AF9" s="2">
+        <f t="shared" ref="AF9:AF10" si="7">M9*G9*AB9*AC9</f>
         <v>0</v>
       </c>
-      <c r="AF9" s="20"/>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG9" s="20"/>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -2247,22 +2272,26 @@
         <v>001FB81B</v>
       </c>
       <c r="AB10" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC10" s="2">
         <v>6.25E-2</v>
       </c>
       <c r="AD10" s="2">
+        <f>M10*G10</f>
+        <v>28901376</v>
+      </c>
+      <c r="AE10" s="2">
         <f t="shared" si="6"/>
         <v>867041.27999999991</v>
       </c>
-      <c r="AE10" s="2">
-        <f>M10*G10*AB10*AC10</f>
-        <v>361267.20000000001</v>
-      </c>
-      <c r="AF10" s="20"/>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF10" s="2">
+        <f t="shared" si="7"/>
+        <v>18063.36</v>
+      </c>
+      <c r="AG10" s="20"/>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
@@ -2298,9 +2327,10 @@
       <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
       <c r="AE11" s="3"/>
-      <c r="AF11" s="20"/>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF11" s="3"/>
+      <c r="AG11" s="20"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>12</v>
       </c>
@@ -2336,9 +2366,10 @@
       <c r="AC12" s="3"/>
       <c r="AD12" s="3"/>
       <c r="AE12" s="3"/>
-      <c r="AF12" s="20"/>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF12" s="3"/>
+      <c r="AG12" s="20"/>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>19</v>
       </c>
@@ -2378,9 +2409,10 @@
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
       <c r="AE13" s="1"/>
-      <c r="AF13" s="20"/>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF13" s="1"/>
+      <c r="AG13" s="20"/>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>13</v>
       </c>
@@ -2479,22 +2511,26 @@
         <v>0022C81B</v>
       </c>
       <c r="AB14" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC14" s="2">
         <v>6.25E-2</v>
       </c>
       <c r="AD14" s="2">
+        <f>M14*G14</f>
+        <v>6422528</v>
+      </c>
+      <c r="AE14" s="2">
         <f>M14*G14*0.03</f>
         <v>192675.84</v>
       </c>
-      <c r="AE14" s="2">
+      <c r="AF14" s="2">
         <f>M14*G14*AB14*AC14</f>
-        <v>80281.600000000006</v>
-      </c>
-      <c r="AF14" s="20"/>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
+        <v>4014.08</v>
+      </c>
+      <c r="AG14" s="20"/>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>14</v>
       </c>
@@ -2530,9 +2566,10 @@
       <c r="AC15" s="3"/>
       <c r="AD15" s="3"/>
       <c r="AE15" s="3"/>
-      <c r="AF15" s="20"/>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF15" s="3"/>
+      <c r="AG15" s="20"/>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
@@ -2552,7 +2589,7 @@
         <v>16</v>
       </c>
       <c r="G16" s="26">
-        <f t="shared" ref="G16:G17" si="7">E16^2*F16</f>
+        <f t="shared" ref="G16:G17" si="8">E16^2*F16</f>
         <v>16</v>
       </c>
       <c r="H16" s="26">
@@ -2571,7 +2608,7 @@
         <v>56</v>
       </c>
       <c r="M16" s="26">
-        <f t="shared" ref="M16:M17" si="8">L16^2*H16</f>
+        <f t="shared" ref="M16:M17" si="9">L16^2*H16</f>
         <v>200704</v>
       </c>
       <c r="N16" s="26">
@@ -2583,7 +2620,7 @@
         <v>64</v>
       </c>
       <c r="P16" s="26">
-        <f t="shared" ref="P16:P17" si="9">N16+O16</f>
+        <f t="shared" ref="P16:P17" si="10">N16+O16</f>
         <v>1088</v>
       </c>
       <c r="Q16" s="45" t="str">
@@ -2611,7 +2648,7 @@
         <v>19360</v>
       </c>
       <c r="W16" s="12" t="str">
-        <f t="shared" ref="W16:W17" si="10">DEC2HEX(V16,8)</f>
+        <f t="shared" ref="W16:W17" si="11">DEC2HEX(V16,8)</f>
         <v>00004BA0</v>
       </c>
       <c r="X16" s="33">
@@ -2619,7 +2656,7 @@
         <v>2279451</v>
       </c>
       <c r="Y16" s="12" t="str">
-        <f t="shared" ref="Y16:Y17" si="11">DEC2HEX(X16,8)</f>
+        <f t="shared" ref="Y16:Y17" si="12">DEC2HEX(X16,8)</f>
         <v>0022C81B</v>
       </c>
       <c r="Z16" s="33">
@@ -2627,26 +2664,30 @@
         <v>2329627</v>
       </c>
       <c r="AA16" s="13" t="str">
-        <f t="shared" ref="AA16:AA17" si="12">DEC2HEX(Z16,8)</f>
+        <f t="shared" ref="AA16:AA17" si="13">DEC2HEX(Z16,8)</f>
         <v>00238C1B</v>
       </c>
       <c r="AB16" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC16" s="2">
         <v>0</v>
       </c>
       <c r="AD16" s="2">
-        <f t="shared" ref="AD16:AD17" si="13">M16*G16*0.03</f>
+        <f>M16*G16</f>
+        <v>3211264</v>
+      </c>
+      <c r="AE16" s="2">
+        <f t="shared" ref="AE16:AE17" si="14">M16*G16*0.03</f>
         <v>96337.919999999998</v>
       </c>
-      <c r="AE16" s="2">
-        <f>M16*G16*AB16*AC16</f>
+      <c r="AF16" s="2">
+        <f t="shared" ref="AF16:AF17" si="15">M16*G16*AB16*AC16</f>
         <v>0</v>
       </c>
-      <c r="AF16" s="20"/>
-    </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG16" s="20"/>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
@@ -2666,7 +2707,7 @@
         <v>16</v>
       </c>
       <c r="G17" s="26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>144</v>
       </c>
       <c r="H17" s="26">
@@ -2685,7 +2726,7 @@
         <v>56</v>
       </c>
       <c r="M17" s="26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>200704</v>
       </c>
       <c r="N17" s="26">
@@ -2697,7 +2738,7 @@
         <v>64</v>
       </c>
       <c r="P17" s="26">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>9280</v>
       </c>
       <c r="Q17" s="45" t="str">
@@ -2725,7 +2766,7 @@
         <v>20448</v>
       </c>
       <c r="W17" s="12" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>00004FE0</v>
       </c>
       <c r="X17" s="33">
@@ -2733,7 +2774,7 @@
         <v>2279451</v>
       </c>
       <c r="Y17" s="12" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0022C81B</v>
       </c>
       <c r="Z17" s="33">
@@ -2741,26 +2782,30 @@
         <v>2530331</v>
       </c>
       <c r="AA17" s="13" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>00269C1B</v>
       </c>
       <c r="AB17" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC17" s="2">
         <v>6.25E-2</v>
       </c>
       <c r="AD17" s="2">
-        <f t="shared" si="13"/>
+        <f>M17*G17</f>
+        <v>28901376</v>
+      </c>
+      <c r="AE17" s="2">
+        <f t="shared" si="14"/>
         <v>867041.27999999991</v>
       </c>
-      <c r="AE17" s="2">
-        <f>M17*G17*AB17*AC17</f>
-        <v>361267.20000000001</v>
-      </c>
-      <c r="AF17" s="20"/>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF17" s="2">
+        <f t="shared" si="15"/>
+        <v>18063.36</v>
+      </c>
+      <c r="AG17" s="20"/>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>17</v>
       </c>
@@ -2796,9 +2841,10 @@
       <c r="AC18" s="3"/>
       <c r="AD18" s="3"/>
       <c r="AE18" s="3"/>
-      <c r="AF18" s="20"/>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF18" s="3"/>
+      <c r="AG18" s="20"/>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>18</v>
       </c>
@@ -2834,9 +2880,10 @@
       <c r="AC19" s="3"/>
       <c r="AD19" s="3"/>
       <c r="AE19" s="3"/>
-      <c r="AF19" s="20"/>
-    </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF19" s="3"/>
+      <c r="AG19" s="20"/>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>20</v>
       </c>
@@ -2876,9 +2923,10 @@
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
       <c r="AE20" s="1"/>
-      <c r="AF20" s="20"/>
-    </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF20" s="1"/>
+      <c r="AG20" s="20"/>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
         <v>21</v>
       </c>
@@ -2965,22 +3013,26 @@
         <v>0029AC1B</v>
       </c>
       <c r="AB21" s="4">
-        <v>0.31</v>
+        <v>0.1</v>
       </c>
       <c r="AC21" s="4">
         <v>6.25E-2</v>
       </c>
       <c r="AD21" s="4">
+        <f>M21*G21</f>
+        <v>903168</v>
+      </c>
+      <c r="AE21" s="4">
         <f>M21*G21*0.03</f>
         <v>27095.039999999997</v>
       </c>
-      <c r="AE21" s="4">
-        <f>M21*G21*AC21</f>
-        <v>56448</v>
-      </c>
-      <c r="AF21" s="20"/>
-    </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF21" s="4">
+        <f>M21*G21*AB21*AC21</f>
+        <v>5644.8</v>
+      </c>
+      <c r="AG21" s="20"/>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
@@ -3079,22 +3131,26 @@
         <v>002B341B</v>
       </c>
       <c r="AB22" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC22" s="2">
         <v>6.25E-2</v>
       </c>
       <c r="AD22" s="2">
+        <f>M22*G22</f>
+        <v>3211264</v>
+      </c>
+      <c r="AE22" s="2">
         <f>M22*G22*0.03</f>
         <v>96337.919999999998</v>
       </c>
-      <c r="AE22" s="2">
+      <c r="AF22" s="2">
         <f>M22*G22*AB22*AC22</f>
-        <v>40140.800000000003</v>
-      </c>
-      <c r="AF22" s="20"/>
-    </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.35">
+        <v>2007.04</v>
+      </c>
+      <c r="AG22" s="20"/>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>23</v>
       </c>
@@ -3130,9 +3186,10 @@
       <c r="AC23" s="3"/>
       <c r="AD23" s="3"/>
       <c r="AE23" s="3"/>
-      <c r="AF23" s="20"/>
-    </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF23" s="3"/>
+      <c r="AG23" s="20"/>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>24</v>
       </c>
@@ -3152,7 +3209,7 @@
         <v>32</v>
       </c>
       <c r="G24" s="26">
-        <f t="shared" ref="G24:G25" si="14">E24^2*F24</f>
+        <f t="shared" ref="G24:G25" si="16">E24^2*F24</f>
         <v>32</v>
       </c>
       <c r="H24" s="26">
@@ -3171,7 +3228,7 @@
         <v>28</v>
       </c>
       <c r="M24" s="26">
-        <f t="shared" ref="M24:M25" si="15">L24^2*H24</f>
+        <f t="shared" ref="M24:M25" si="17">L24^2*H24</f>
         <v>100352</v>
       </c>
       <c r="N24" s="26">
@@ -3183,7 +3240,7 @@
         <v>128</v>
       </c>
       <c r="P24" s="26">
-        <f t="shared" ref="P24:P25" si="16">N24+O24</f>
+        <f t="shared" ref="P24:P25" si="18">N24+O24</f>
         <v>4224</v>
       </c>
       <c r="Q24" s="45" t="str">
@@ -3211,7 +3268,7 @@
         <v>33856</v>
       </c>
       <c r="W24" s="12" t="str">
-        <f t="shared" ref="W24:W25" si="17">DEC2HEX(V24,8)</f>
+        <f t="shared" ref="W24:W25" si="19">DEC2HEX(V24,8)</f>
         <v>00008440</v>
       </c>
       <c r="X24" s="33">
@@ -3219,7 +3276,7 @@
         <v>2831387</v>
       </c>
       <c r="Y24" s="12" t="str">
-        <f t="shared" ref="Y24:Y25" si="18">DEC2HEX(X24,8)</f>
+        <f t="shared" ref="Y24:Y25" si="20">DEC2HEX(X24,8)</f>
         <v>002B341B</v>
       </c>
       <c r="Z24" s="33">
@@ -3227,26 +3284,30 @@
         <v>2856475</v>
       </c>
       <c r="AA24" s="13" t="str">
-        <f t="shared" ref="AA24:AA25" si="19">DEC2HEX(Z24,8)</f>
+        <f t="shared" ref="AA24:AA25" si="21">DEC2HEX(Z24,8)</f>
         <v>002B961B</v>
       </c>
       <c r="AB24" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC24" s="2">
         <v>0</v>
       </c>
       <c r="AD24" s="2">
-        <f t="shared" ref="AD24:AD25" si="20">M24*G24*0.03</f>
+        <f>M24*G24</f>
+        <v>3211264</v>
+      </c>
+      <c r="AE24" s="2">
+        <f t="shared" ref="AE24:AE25" si="22">M24*G24*0.03</f>
         <v>96337.919999999998</v>
       </c>
-      <c r="AE24" s="2">
-        <f>M24*G24*AB24*AC24</f>
+      <c r="AF24" s="2">
+        <f t="shared" ref="AF24:AF25" si="23">M24*G24*AB24*AC24</f>
         <v>0</v>
       </c>
-      <c r="AF24" s="20"/>
-    </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG24" s="20"/>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>25</v>
       </c>
@@ -3266,7 +3327,7 @@
         <v>32</v>
       </c>
       <c r="G25" s="26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>288</v>
       </c>
       <c r="H25" s="26">
@@ -3285,7 +3346,7 @@
         <v>28</v>
       </c>
       <c r="M25" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>100352</v>
       </c>
       <c r="N25" s="26">
@@ -3297,7 +3358,7 @@
         <v>128</v>
       </c>
       <c r="P25" s="26">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>36992</v>
       </c>
       <c r="Q25" s="45" t="str">
@@ -3325,7 +3386,7 @@
         <v>38080</v>
       </c>
       <c r="W25" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>000094C0</v>
       </c>
       <c r="X25" s="33">
@@ -3333,7 +3394,7 @@
         <v>2831387</v>
       </c>
       <c r="Y25" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>002B341B</v>
       </c>
       <c r="Z25" s="33">
@@ -3341,26 +3402,30 @@
         <v>2956827</v>
       </c>
       <c r="AA25" s="13" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>002D1E1B</v>
       </c>
       <c r="AB25" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC25" s="2">
         <v>6.25E-2</v>
       </c>
       <c r="AD25" s="2">
-        <f t="shared" si="20"/>
+        <f>M25*G25</f>
+        <v>28901376</v>
+      </c>
+      <c r="AE25" s="2">
+        <f t="shared" si="22"/>
         <v>867041.27999999991</v>
       </c>
-      <c r="AE25" s="2">
-        <f>M25*G25*AB25*AC25</f>
-        <v>361267.20000000001</v>
-      </c>
-      <c r="AF25" s="20"/>
-    </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF25" s="2">
+        <f t="shared" si="23"/>
+        <v>18063.36</v>
+      </c>
+      <c r="AG25" s="20"/>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>26</v>
       </c>
@@ -3396,9 +3461,10 @@
       <c r="AC26" s="3"/>
       <c r="AD26" s="3"/>
       <c r="AE26" s="3"/>
-      <c r="AF26" s="20"/>
-    </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF26" s="3"/>
+      <c r="AG26" s="20"/>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>27</v>
       </c>
@@ -3434,9 +3500,10 @@
       <c r="AC27" s="3"/>
       <c r="AD27" s="3"/>
       <c r="AE27" s="3"/>
-      <c r="AF27" s="20"/>
-    </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF27" s="3"/>
+      <c r="AG27" s="20"/>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>28</v>
       </c>
@@ -3476,9 +3543,10 @@
       <c r="AC28" s="1"/>
       <c r="AD28" s="1"/>
       <c r="AE28" s="1"/>
-      <c r="AF28" s="20"/>
-    </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF28" s="1"/>
+      <c r="AG28" s="20"/>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
         <v>29</v>
       </c>
@@ -3577,22 +3645,26 @@
         <v>002EA61B</v>
       </c>
       <c r="AB29" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC29" s="2">
         <v>6.25E-2</v>
       </c>
       <c r="AD29" s="2">
+        <f>M29*G29</f>
+        <v>6422528</v>
+      </c>
+      <c r="AE29" s="2">
         <f>M29*G29*0.03</f>
         <v>192675.84</v>
       </c>
-      <c r="AE29" s="2">
+      <c r="AF29" s="2">
         <f>M29*G29*AB29*AC29</f>
-        <v>80281.600000000006</v>
-      </c>
-      <c r="AF29" s="20"/>
-    </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.35">
+        <v>4014.08</v>
+      </c>
+      <c r="AG29" s="20"/>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>30</v>
       </c>
@@ -3628,9 +3700,10 @@
       <c r="AC30" s="3"/>
       <c r="AD30" s="3"/>
       <c r="AE30" s="3"/>
-      <c r="AF30" s="20"/>
-    </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF30" s="3"/>
+      <c r="AG30" s="20"/>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
         <v>31</v>
       </c>
@@ -3650,7 +3723,7 @@
         <v>32</v>
       </c>
       <c r="G31" s="26">
-        <f t="shared" ref="G31:G32" si="21">E31^2*F31</f>
+        <f t="shared" ref="G31:G32" si="24">E31^2*F31</f>
         <v>32</v>
       </c>
       <c r="H31" s="26">
@@ -3669,7 +3742,7 @@
         <v>28</v>
       </c>
       <c r="M31" s="26">
-        <f t="shared" ref="M31:M32" si="22">L31^2*H31</f>
+        <f t="shared" ref="M31:M32" si="25">L31^2*H31</f>
         <v>100352</v>
       </c>
       <c r="N31" s="26">
@@ -3681,7 +3754,7 @@
         <v>128</v>
       </c>
       <c r="P31" s="26">
-        <f t="shared" ref="P31:P32" si="23">N31+O31</f>
+        <f t="shared" ref="P31:P32" si="26">N31+O31</f>
         <v>4224</v>
       </c>
       <c r="Q31" s="45" t="str">
@@ -3709,7 +3782,7 @@
         <v>83296</v>
       </c>
       <c r="W31" s="12" t="str">
-        <f t="shared" ref="W31:W32" si="24">DEC2HEX(V31,8)</f>
+        <f t="shared" ref="W31:W32" si="27">DEC2HEX(V31,8)</f>
         <v>00014560</v>
       </c>
       <c r="X31" s="33">
@@ -3717,7 +3790,7 @@
         <v>3057179</v>
       </c>
       <c r="Y31" s="12" t="str">
-        <f t="shared" ref="Y31:Y32" si="25">DEC2HEX(X31,8)</f>
+        <f t="shared" ref="Y31:Y32" si="28">DEC2HEX(X31,8)</f>
         <v>002EA61B</v>
       </c>
       <c r="Z31" s="33">
@@ -3725,26 +3798,30 @@
         <v>3082267</v>
       </c>
       <c r="AA31" s="13" t="str">
-        <f t="shared" ref="AA31:AA32" si="26">DEC2HEX(Z31,8)</f>
+        <f t="shared" ref="AA31:AA32" si="29">DEC2HEX(Z31,8)</f>
         <v>002F081B</v>
       </c>
       <c r="AB31" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC31" s="2">
         <v>0</v>
       </c>
       <c r="AD31" s="2">
-        <f t="shared" ref="AD31:AD32" si="27">M31*G31*0.03</f>
+        <f>M31*G31</f>
+        <v>3211264</v>
+      </c>
+      <c r="AE31" s="2">
+        <f t="shared" ref="AE31:AE32" si="30">M31*G31*0.03</f>
         <v>96337.919999999998</v>
       </c>
-      <c r="AE31" s="2">
-        <f>M31*G31*AB31*AC31</f>
+      <c r="AF31" s="2">
+        <f t="shared" ref="AF31:AF32" si="31">M31*G31*AB31*AC31</f>
         <v>0</v>
       </c>
-      <c r="AF31" s="20"/>
-    </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG31" s="20"/>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
         <v>32</v>
       </c>
@@ -3764,7 +3841,7 @@
         <v>32</v>
       </c>
       <c r="G32" s="26">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>288</v>
       </c>
       <c r="H32" s="26">
@@ -3783,7 +3860,7 @@
         <v>28</v>
       </c>
       <c r="M32" s="26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>100352</v>
       </c>
       <c r="N32" s="26">
@@ -3795,7 +3872,7 @@
         <v>128</v>
       </c>
       <c r="P32" s="26">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>36992</v>
       </c>
       <c r="Q32" s="45" t="str">
@@ -3823,7 +3900,7 @@
         <v>87520</v>
       </c>
       <c r="W32" s="12" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>000155E0</v>
       </c>
       <c r="X32" s="33">
@@ -3831,7 +3908,7 @@
         <v>3057179</v>
       </c>
       <c r="Y32" s="12" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>002EA61B</v>
       </c>
       <c r="Z32" s="33">
@@ -3839,26 +3916,30 @@
         <v>3182619</v>
       </c>
       <c r="AA32" s="13" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>0030901B</v>
       </c>
       <c r="AB32" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC32" s="2">
         <v>6.25E-2</v>
       </c>
       <c r="AD32" s="2">
-        <f t="shared" si="27"/>
+        <f>M32*G32</f>
+        <v>28901376</v>
+      </c>
+      <c r="AE32" s="2">
+        <f t="shared" si="30"/>
         <v>867041.27999999991</v>
       </c>
-      <c r="AE32" s="2">
-        <f>M32*G32*AB32*AC32</f>
-        <v>361267.20000000001</v>
-      </c>
-      <c r="AF32" s="20"/>
-    </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF32" s="2">
+        <f t="shared" si="31"/>
+        <v>18063.36</v>
+      </c>
+      <c r="AG32" s="20"/>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>33</v>
       </c>
@@ -3894,9 +3975,10 @@
       <c r="AC33" s="3"/>
       <c r="AD33" s="3"/>
       <c r="AE33" s="3"/>
-      <c r="AF33" s="20"/>
-    </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF33" s="3"/>
+      <c r="AG33" s="20"/>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
         <v>34</v>
       </c>
@@ -3932,9 +4014,10 @@
       <c r="AC34" s="3"/>
       <c r="AD34" s="3"/>
       <c r="AE34" s="3"/>
-      <c r="AF34" s="20"/>
-    </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF34" s="3"/>
+      <c r="AG34" s="20"/>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>35</v>
       </c>
@@ -3972,9 +4055,10 @@
       <c r="AC35" s="1"/>
       <c r="AD35" s="1"/>
       <c r="AE35" s="1"/>
-      <c r="AF35" s="20"/>
-    </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF35" s="1"/>
+      <c r="AG35" s="20"/>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A36" s="8" t="s">
         <v>36</v>
       </c>
@@ -4061,22 +4145,26 @@
         <v>0032181B</v>
       </c>
       <c r="AB36" s="4">
-        <v>0.31</v>
+        <v>0.1</v>
       </c>
       <c r="AC36" s="4">
         <v>6.25E-2</v>
       </c>
       <c r="AD36" s="4">
+        <f>M36*G36</f>
+        <v>451584</v>
+      </c>
+      <c r="AE36" s="4">
         <f>M36*G36*0.03</f>
         <v>13547.519999999999</v>
       </c>
-      <c r="AE36" s="4">
-        <f>M36*G36*AC36</f>
-        <v>28224</v>
-      </c>
-      <c r="AF36" s="20"/>
-    </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF36" s="4">
+        <f>M36*G36*AB36*AC36</f>
+        <v>2822.4</v>
+      </c>
+      <c r="AG36" s="20"/>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
         <v>37</v>
       </c>
@@ -4175,22 +4263,26 @@
         <v>0032DC1B</v>
       </c>
       <c r="AB37" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC37" s="2">
         <v>6.25E-2</v>
       </c>
       <c r="AD37" s="2">
+        <f>M37*G37</f>
+        <v>2408448</v>
+      </c>
+      <c r="AE37" s="2">
         <f>M37*G37*0.03</f>
         <v>72253.440000000002</v>
       </c>
-      <c r="AE37" s="2">
+      <c r="AF37" s="2">
         <f>M37*G37*AB37*AC37</f>
-        <v>30105.600000000002</v>
-      </c>
-      <c r="AF37" s="20"/>
-    </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.35">
+        <v>1505.28</v>
+      </c>
+      <c r="AG37" s="20"/>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
         <v>38</v>
       </c>
@@ -4226,9 +4318,10 @@
       <c r="AC38" s="3"/>
       <c r="AD38" s="3"/>
       <c r="AE38" s="3"/>
-      <c r="AF38" s="20"/>
-    </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF38" s="3"/>
+      <c r="AG38" s="20"/>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A39" s="6" t="s">
         <v>39</v>
       </c>
@@ -4248,7 +4341,7 @@
         <v>48</v>
       </c>
       <c r="G39" s="26">
-        <f t="shared" ref="G39:G40" si="28">E39^2*F39</f>
+        <f t="shared" ref="G39:G40" si="32">E39^2*F39</f>
         <v>48</v>
       </c>
       <c r="H39" s="26">
@@ -4267,7 +4360,7 @@
         <v>14</v>
       </c>
       <c r="M39" s="26">
-        <f t="shared" ref="M39:M40" si="29">L39^2*H39</f>
+        <f t="shared" ref="M39:M40" si="33">L39^2*H39</f>
         <v>37632</v>
       </c>
       <c r="N39" s="26">
@@ -4279,7 +4372,7 @@
         <v>192</v>
       </c>
       <c r="P39" s="26">
-        <f t="shared" ref="P39:P40" si="30">N39+O39</f>
+        <f t="shared" ref="P39:P40" si="34">N39+O39</f>
         <v>9408</v>
       </c>
       <c r="Q39" s="45" t="str">
@@ -4307,7 +4400,7 @@
         <v>136848</v>
       </c>
       <c r="W39" s="12" t="str">
-        <f t="shared" ref="W39:W40" si="31">DEC2HEX(V39,8)</f>
+        <f t="shared" ref="W39:W40" si="35">DEC2HEX(V39,8)</f>
         <v>00021690</v>
       </c>
       <c r="X39" s="33">
@@ -4315,7 +4408,7 @@
         <v>3333147</v>
       </c>
       <c r="Y39" s="12" t="str">
-        <f t="shared" ref="Y39:Y40" si="32">DEC2HEX(X39,8)</f>
+        <f t="shared" ref="Y39:Y40" si="36">DEC2HEX(X39,8)</f>
         <v>0032DC1B</v>
       </c>
       <c r="Z39" s="33">
@@ -4323,26 +4416,30 @@
         <v>3342555</v>
       </c>
       <c r="AA39" s="13" t="str">
-        <f t="shared" ref="AA39:AA40" si="33">DEC2HEX(Z39,8)</f>
+        <f t="shared" ref="AA39:AA40" si="37">DEC2HEX(Z39,8)</f>
         <v>003300DB</v>
       </c>
       <c r="AB39" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC39" s="2">
         <v>0</v>
       </c>
       <c r="AD39" s="2">
-        <f t="shared" ref="AD39:AD40" si="34">M39*G39*0.03</f>
+        <f>M39*G39</f>
+        <v>1806336</v>
+      </c>
+      <c r="AE39" s="2">
+        <f t="shared" ref="AE39:AE40" si="38">M39*G39*0.03</f>
         <v>54190.079999999994</v>
       </c>
-      <c r="AE39" s="2">
-        <f>M39*G39*AB39*AC39</f>
+      <c r="AF39" s="2">
+        <f t="shared" ref="AF39:AF40" si="39">M39*G39*AB39*AC39</f>
         <v>0</v>
       </c>
-      <c r="AF39" s="20"/>
-    </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG39" s="20"/>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A40" s="6" t="s">
         <v>40</v>
       </c>
@@ -4362,7 +4459,7 @@
         <v>48</v>
       </c>
       <c r="G40" s="26">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>432</v>
       </c>
       <c r="H40" s="26">
@@ -4381,7 +4478,7 @@
         <v>14</v>
       </c>
       <c r="M40" s="26">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>37632</v>
       </c>
       <c r="N40" s="26">
@@ -4393,7 +4490,7 @@
         <v>192</v>
       </c>
       <c r="P40" s="26">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>83136</v>
       </c>
       <c r="Q40" s="45" t="str">
@@ -4421,7 +4518,7 @@
         <v>146256</v>
       </c>
       <c r="W40" s="12" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>00023B50</v>
       </c>
       <c r="X40" s="33">
@@ -4429,7 +4526,7 @@
         <v>3333147</v>
       </c>
       <c r="Y40" s="12" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0032DC1B</v>
       </c>
       <c r="Z40" s="33">
@@ -4437,26 +4534,30 @@
         <v>3380187</v>
       </c>
       <c r="AA40" s="13" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>003393DB</v>
       </c>
       <c r="AB40" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC40" s="2">
         <v>6.25E-2</v>
       </c>
       <c r="AD40" s="2">
-        <f t="shared" si="34"/>
+        <f>M40*G40</f>
+        <v>16257024</v>
+      </c>
+      <c r="AE40" s="2">
+        <f t="shared" si="38"/>
         <v>487710.71999999997</v>
       </c>
-      <c r="AE40" s="2">
-        <f>M40*G40*AB40*AC40</f>
-        <v>203212.80000000002</v>
-      </c>
-      <c r="AF40" s="20"/>
-    </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF40" s="2">
+        <f t="shared" si="39"/>
+        <v>10160.64</v>
+      </c>
+      <c r="AG40" s="20"/>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>41</v>
       </c>
@@ -4492,9 +4593,10 @@
       <c r="AC41" s="3"/>
       <c r="AD41" s="3"/>
       <c r="AE41" s="3"/>
-      <c r="AF41" s="20"/>
-    </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF41" s="3"/>
+      <c r="AG41" s="20"/>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>42</v>
       </c>
@@ -4530,9 +4632,10 @@
       <c r="AC42" s="3"/>
       <c r="AD42" s="3"/>
       <c r="AE42" s="3"/>
-      <c r="AF42" s="20"/>
-    </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF42" s="3"/>
+      <c r="AG42" s="20"/>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>43</v>
       </c>
@@ -4572,9 +4675,10 @@
       <c r="AC43" s="1"/>
       <c r="AD43" s="1"/>
       <c r="AE43" s="1"/>
-      <c r="AF43" s="20"/>
-    </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF43" s="1"/>
+      <c r="AG43" s="20"/>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A44" s="6" t="s">
         <v>44</v>
       </c>
@@ -4673,22 +4777,26 @@
         <v>003426DB</v>
       </c>
       <c r="AB44" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC44" s="2">
         <v>6.25E-2</v>
       </c>
       <c r="AD44" s="2">
+        <f>M44*G44</f>
+        <v>3612672</v>
+      </c>
+      <c r="AE44" s="2">
         <f>M44*G44*0.03</f>
         <v>108380.15999999999</v>
       </c>
-      <c r="AE44" s="2">
+      <c r="AF44" s="2">
         <f>M44*G44*AB44*AC44</f>
-        <v>45158.400000000001</v>
-      </c>
-      <c r="AF44" s="20"/>
-    </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.35">
+        <v>2257.92</v>
+      </c>
+      <c r="AG44" s="20"/>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
         <v>45</v>
       </c>
@@ -4724,9 +4832,10 @@
       <c r="AC45" s="3"/>
       <c r="AD45" s="3"/>
       <c r="AE45" s="3"/>
-      <c r="AF45" s="20"/>
-    </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF45" s="3"/>
+      <c r="AG45" s="20"/>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A46" s="6" t="s">
         <v>46</v>
       </c>
@@ -4746,7 +4855,7 @@
         <v>48</v>
       </c>
       <c r="G46" s="26">
-        <f t="shared" ref="G46:G47" si="35">E46^2*F46</f>
+        <f t="shared" ref="G46:G47" si="40">E46^2*F46</f>
         <v>48</v>
       </c>
       <c r="H46" s="26">
@@ -4765,7 +4874,7 @@
         <v>14</v>
       </c>
       <c r="M46" s="26">
-        <f t="shared" ref="M46:M47" si="36">L46^2*H46</f>
+        <f t="shared" ref="M46:M47" si="41">L46^2*H46</f>
         <v>37632</v>
       </c>
       <c r="N46" s="26">
@@ -4777,7 +4886,7 @@
         <v>192</v>
       </c>
       <c r="P46" s="26">
-        <f t="shared" ref="P46:P47" si="37">N46+O46</f>
+        <f t="shared" ref="P46:P47" si="42">N46+O46</f>
         <v>9408</v>
       </c>
       <c r="Q46" s="45" t="str">
@@ -4805,7 +4914,7 @@
         <v>247872</v>
       </c>
       <c r="W46" s="12" t="str">
-        <f t="shared" ref="W46:W47" si="38">DEC2HEX(V46,8)</f>
+        <f t="shared" ref="W46:W47" si="43">DEC2HEX(V46,8)</f>
         <v>0003C840</v>
       </c>
       <c r="X46" s="33">
@@ -4813,7 +4922,7 @@
         <v>3417819</v>
       </c>
       <c r="Y46" s="12" t="str">
-        <f t="shared" ref="Y46:Y47" si="39">DEC2HEX(X46,8)</f>
+        <f t="shared" ref="Y46:Y47" si="44">DEC2HEX(X46,8)</f>
         <v>003426DB</v>
       </c>
       <c r="Z46" s="33">
@@ -4821,26 +4930,30 @@
         <v>3427227</v>
       </c>
       <c r="AA46" s="13" t="str">
-        <f t="shared" ref="AA46:AA47" si="40">DEC2HEX(Z46,8)</f>
+        <f t="shared" ref="AA46:AA47" si="45">DEC2HEX(Z46,8)</f>
         <v>00344B9B</v>
       </c>
       <c r="AB46" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC46" s="2">
         <v>0</v>
       </c>
       <c r="AD46" s="2">
-        <f t="shared" ref="AD46:AD47" si="41">M46*G46*0.03</f>
+        <f>M46*G46</f>
+        <v>1806336</v>
+      </c>
+      <c r="AE46" s="2">
+        <f t="shared" ref="AE46:AE47" si="46">M46*G46*0.03</f>
         <v>54190.079999999994</v>
       </c>
-      <c r="AE46" s="2">
-        <f>M46*G46*AB46*AC46</f>
+      <c r="AF46" s="2">
+        <f t="shared" ref="AF46:AF47" si="47">M46*G46*AB46*AC46</f>
         <v>0</v>
       </c>
-      <c r="AF46" s="20"/>
-    </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG46" s="20"/>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A47" s="6" t="s">
         <v>47</v>
       </c>
@@ -4860,7 +4973,7 @@
         <v>48</v>
       </c>
       <c r="G47" s="26">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>432</v>
       </c>
       <c r="H47" s="26">
@@ -4879,7 +4992,7 @@
         <v>14</v>
       </c>
       <c r="M47" s="26">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>37632</v>
       </c>
       <c r="N47" s="26">
@@ -4891,7 +5004,7 @@
         <v>192</v>
       </c>
       <c r="P47" s="26">
-        <f t="shared" si="37"/>
+        <f t="shared" si="42"/>
         <v>83136</v>
       </c>
       <c r="Q47" s="45" t="str">
@@ -4919,7 +5032,7 @@
         <v>257280</v>
       </c>
       <c r="W47" s="12" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="43"/>
         <v>0003ED00</v>
       </c>
       <c r="X47" s="33">
@@ -4927,7 +5040,7 @@
         <v>3417819</v>
       </c>
       <c r="Y47" s="12" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="44"/>
         <v>003426DB</v>
       </c>
       <c r="Z47" s="33">
@@ -4935,26 +5048,30 @@
         <v>3464859</v>
       </c>
       <c r="AA47" s="13" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="45"/>
         <v>0034DE9B</v>
       </c>
       <c r="AB47" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC47" s="2">
         <v>6.25E-2</v>
       </c>
       <c r="AD47" s="2">
-        <f t="shared" si="41"/>
+        <f>M47*G47</f>
+        <v>16257024</v>
+      </c>
+      <c r="AE47" s="2">
+        <f t="shared" si="46"/>
         <v>487710.71999999997</v>
       </c>
-      <c r="AE47" s="2">
-        <f>M47*G47*AB47*AC47</f>
-        <v>203212.80000000002</v>
-      </c>
-      <c r="AF47" s="20"/>
-    </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF47" s="2">
+        <f t="shared" si="47"/>
+        <v>10160.64</v>
+      </c>
+      <c r="AG47" s="20"/>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
         <v>48</v>
       </c>
@@ -4990,9 +5107,10 @@
       <c r="AC48" s="3"/>
       <c r="AD48" s="3"/>
       <c r="AE48" s="3"/>
-      <c r="AF48" s="20"/>
-    </row>
-    <row r="49" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF48" s="3"/>
+      <c r="AG48" s="20"/>
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
         <v>49</v>
       </c>
@@ -5028,9 +5146,10 @@
       <c r="AC49" s="3"/>
       <c r="AD49" s="3"/>
       <c r="AE49" s="3"/>
-      <c r="AF49" s="20"/>
-    </row>
-    <row r="50" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF49" s="3"/>
+      <c r="AG49" s="20"/>
+    </row>
+    <row r="50" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>50</v>
       </c>
@@ -5070,9 +5189,10 @@
       <c r="AC50" s="1"/>
       <c r="AD50" s="1"/>
       <c r="AE50" s="1"/>
-      <c r="AF50" s="20"/>
-    </row>
-    <row r="51" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF50" s="1"/>
+      <c r="AG50" s="20"/>
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
         <v>51</v>
       </c>
@@ -5171,22 +5291,26 @@
         <v>0035719B</v>
       </c>
       <c r="AB51" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC51" s="2">
         <v>6.25E-2</v>
       </c>
       <c r="AD51" s="2">
+        <f>M51*G51</f>
+        <v>4816896</v>
+      </c>
+      <c r="AE51" s="2">
         <f>M51*G51*0.03</f>
         <v>144506.88</v>
       </c>
-      <c r="AE51" s="2">
+      <c r="AF51" s="2">
         <f>M51*G51*AB51*AC51</f>
-        <v>60211.200000000004</v>
-      </c>
-      <c r="AF51" s="20"/>
-    </row>
-    <row r="52" spans="1:32" x14ac:dyDescent="0.35">
+        <v>3010.56</v>
+      </c>
+      <c r="AG51" s="20"/>
+    </row>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A52" s="7" t="s">
         <v>52</v>
       </c>
@@ -5222,9 +5346,10 @@
       <c r="AC52" s="3"/>
       <c r="AD52" s="3"/>
       <c r="AE52" s="3"/>
-      <c r="AF52" s="20"/>
-    </row>
-    <row r="53" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF52" s="3"/>
+      <c r="AG52" s="20"/>
+    </row>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
         <v>53</v>
       </c>
@@ -5244,7 +5369,7 @@
         <v>64</v>
       </c>
       <c r="G53" s="26">
-        <f t="shared" ref="G53:G54" si="42">E53^2*F53</f>
+        <f t="shared" ref="G53:G54" si="48">E53^2*F53</f>
         <v>64</v>
       </c>
       <c r="H53" s="26">
@@ -5263,7 +5388,7 @@
         <v>14</v>
       </c>
       <c r="M53" s="26">
-        <f t="shared" ref="M53:M54" si="43">L53^2*H53</f>
+        <f t="shared" ref="M53:M54" si="49">L53^2*H53</f>
         <v>50176</v>
       </c>
       <c r="N53" s="26">
@@ -5275,7 +5400,7 @@
         <v>256</v>
       </c>
       <c r="P53" s="26">
-        <f t="shared" ref="P53:P54" si="44">N53+O53</f>
+        <f t="shared" ref="P53:P54" si="50">N53+O53</f>
         <v>16640</v>
       </c>
       <c r="Q53" s="45" t="str">
@@ -5303,7 +5428,7 @@
         <v>365056</v>
       </c>
       <c r="W53" s="12" t="str">
-        <f t="shared" ref="W53:W54" si="45">DEC2HEX(V53,8)</f>
+        <f t="shared" ref="W53:W54" si="51">DEC2HEX(V53,8)</f>
         <v>00059200</v>
       </c>
       <c r="X53" s="33">
@@ -5311,7 +5436,7 @@
         <v>3502491</v>
       </c>
       <c r="Y53" s="12" t="str">
-        <f t="shared" ref="Y53:Y54" si="46">DEC2HEX(X53,8)</f>
+        <f t="shared" ref="Y53:Y54" si="52">DEC2HEX(X53,8)</f>
         <v>0035719B</v>
       </c>
       <c r="Z53" s="33">
@@ -5319,26 +5444,30 @@
         <v>3515035</v>
       </c>
       <c r="AA53" s="13" t="str">
-        <f t="shared" ref="AA53:AA54" si="47">DEC2HEX(Z53,8)</f>
+        <f t="shared" ref="AA53:AA54" si="53">DEC2HEX(Z53,8)</f>
         <v>0035A29B</v>
       </c>
       <c r="AB53" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC53" s="2">
         <v>0</v>
       </c>
       <c r="AD53" s="2">
-        <f t="shared" ref="AD53:AD54" si="48">M53*G53*0.03</f>
+        <f>M53*G53</f>
+        <v>3211264</v>
+      </c>
+      <c r="AE53" s="2">
+        <f t="shared" ref="AE53:AE54" si="54">M53*G53*0.03</f>
         <v>96337.919999999998</v>
       </c>
-      <c r="AE53" s="2">
-        <f>M53*G53*AB53*AC53</f>
+      <c r="AF53" s="2">
+        <f t="shared" ref="AF53:AF54" si="55">M53*G53*AB53*AC53</f>
         <v>0</v>
       </c>
-      <c r="AF53" s="20"/>
-    </row>
-    <row r="54" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG53" s="20"/>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
         <v>54</v>
       </c>
@@ -5358,7 +5487,7 @@
         <v>64</v>
       </c>
       <c r="G54" s="26">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>576</v>
       </c>
       <c r="H54" s="26">
@@ -5377,7 +5506,7 @@
         <v>14</v>
       </c>
       <c r="M54" s="26">
-        <f t="shared" si="43"/>
+        <f t="shared" si="49"/>
         <v>50176</v>
       </c>
       <c r="N54" s="26">
@@ -5389,7 +5518,7 @@
         <v>256</v>
       </c>
       <c r="P54" s="26">
-        <f t="shared" si="44"/>
+        <f t="shared" si="50"/>
         <v>147712</v>
       </c>
       <c r="Q54" s="45" t="str">
@@ -5417,7 +5546,7 @@
         <v>381696</v>
       </c>
       <c r="W54" s="12" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="51"/>
         <v>0005D300</v>
       </c>
       <c r="X54" s="33">
@@ -5425,7 +5554,7 @@
         <v>3502491</v>
       </c>
       <c r="Y54" s="12" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="52"/>
         <v>0035719B</v>
       </c>
       <c r="Z54" s="33">
@@ -5433,26 +5562,30 @@
         <v>3565211</v>
       </c>
       <c r="AA54" s="13" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="53"/>
         <v>0036669B</v>
       </c>
       <c r="AB54" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC54" s="2">
         <v>6.25E-2</v>
       </c>
       <c r="AD54" s="2">
-        <f t="shared" si="48"/>
+        <f>M54*G54</f>
+        <v>28901376</v>
+      </c>
+      <c r="AE54" s="2">
+        <f t="shared" si="54"/>
         <v>867041.27999999991</v>
       </c>
-      <c r="AE54" s="2">
-        <f>M54*G54*AB54*AC54</f>
-        <v>361267.20000000001</v>
-      </c>
-      <c r="AF54" s="20"/>
-    </row>
-    <row r="55" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF54" s="2">
+        <f t="shared" si="55"/>
+        <v>18063.36</v>
+      </c>
+      <c r="AG54" s="20"/>
+    </row>
+    <row r="55" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
         <v>55</v>
       </c>
@@ -5488,9 +5621,10 @@
       <c r="AC55" s="3"/>
       <c r="AD55" s="3"/>
       <c r="AE55" s="3"/>
-      <c r="AF55" s="20"/>
-    </row>
-    <row r="56" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF55" s="3"/>
+      <c r="AG55" s="20"/>
+    </row>
+    <row r="56" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
         <v>56</v>
       </c>
@@ -5526,9 +5660,10 @@
       <c r="AC56" s="3"/>
       <c r="AD56" s="3"/>
       <c r="AE56" s="3"/>
-      <c r="AF56" s="20"/>
-    </row>
-    <row r="57" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF56" s="3"/>
+      <c r="AG56" s="20"/>
+    </row>
+    <row r="57" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>57</v>
       </c>
@@ -5568,9 +5703,10 @@
       <c r="AC57" s="1"/>
       <c r="AD57" s="1"/>
       <c r="AE57" s="1"/>
-      <c r="AF57" s="20"/>
-    </row>
-    <row r="58" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF57" s="1"/>
+      <c r="AG57" s="20"/>
+    </row>
+    <row r="58" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A58" s="6" t="s">
         <v>58</v>
       </c>
@@ -5669,22 +5805,26 @@
         <v>00372A9B</v>
       </c>
       <c r="AB58" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC58" s="2">
         <v>6.25E-2</v>
       </c>
       <c r="AD58" s="2">
+        <f>M58*G58</f>
+        <v>6422528</v>
+      </c>
+      <c r="AE58" s="2">
         <f>M58*G58*0.03</f>
         <v>192675.84</v>
       </c>
-      <c r="AE58" s="2">
+      <c r="AF58" s="2">
         <f>M58*G58*AB58*AC58</f>
-        <v>80281.600000000006</v>
-      </c>
-      <c r="AF58" s="20"/>
-    </row>
-    <row r="59" spans="1:32" x14ac:dyDescent="0.35">
+        <v>4014.08</v>
+      </c>
+      <c r="AG58" s="20"/>
+    </row>
+    <row r="59" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A59" s="7" t="s">
         <v>59</v>
       </c>
@@ -5720,9 +5860,10 @@
       <c r="AC59" s="3"/>
       <c r="AD59" s="3"/>
       <c r="AE59" s="3"/>
-      <c r="AF59" s="20"/>
-    </row>
-    <row r="60" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF59" s="3"/>
+      <c r="AG59" s="20"/>
+    </row>
+    <row r="60" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A60" s="6" t="s">
         <v>60</v>
       </c>
@@ -5742,7 +5883,7 @@
         <v>64</v>
       </c>
       <c r="G60" s="26">
-        <f t="shared" ref="G60:G61" si="49">E60^2*F60</f>
+        <f t="shared" ref="G60:G61" si="56">E60^2*F60</f>
         <v>64</v>
       </c>
       <c r="H60" s="26">
@@ -5761,7 +5902,7 @@
         <v>14</v>
       </c>
       <c r="M60" s="26">
-        <f t="shared" ref="M60:M61" si="50">L60^2*H60</f>
+        <f t="shared" ref="M60:M61" si="57">L60^2*H60</f>
         <v>50176</v>
       </c>
       <c r="N60" s="26">
@@ -5773,7 +5914,7 @@
         <v>256</v>
       </c>
       <c r="P60" s="26">
-        <f t="shared" ref="P60:P61" si="51">N60+O60</f>
+        <f t="shared" ref="P60:P61" si="58">N60+O60</f>
         <v>16640</v>
       </c>
       <c r="Q60" s="45" t="str">
@@ -5801,7 +5942,7 @@
         <v>562240</v>
       </c>
       <c r="W60" s="12" t="str">
-        <f t="shared" ref="W60:W61" si="52">DEC2HEX(V60,8)</f>
+        <f t="shared" ref="W60:W61" si="59">DEC2HEX(V60,8)</f>
         <v>00089440</v>
       </c>
       <c r="X60" s="33">
@@ -5809,7 +5950,7 @@
         <v>3615387</v>
       </c>
       <c r="Y60" s="12" t="str">
-        <f t="shared" ref="Y60:Y61" si="53">DEC2HEX(X60,8)</f>
+        <f t="shared" ref="Y60:Y61" si="60">DEC2HEX(X60,8)</f>
         <v>00372A9B</v>
       </c>
       <c r="Z60" s="33">
@@ -5817,26 +5958,30 @@
         <v>3627931</v>
       </c>
       <c r="AA60" s="13" t="str">
-        <f t="shared" ref="AA60:AA61" si="54">DEC2HEX(Z60,8)</f>
+        <f t="shared" ref="AA60:AA61" si="61">DEC2HEX(Z60,8)</f>
         <v>00375B9B</v>
       </c>
       <c r="AB60" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC60" s="2">
         <v>0</v>
       </c>
       <c r="AD60" s="2">
-        <f t="shared" ref="AD60:AD61" si="55">M60*G60*0.03</f>
+        <f>M60*G60</f>
+        <v>3211264</v>
+      </c>
+      <c r="AE60" s="2">
+        <f t="shared" ref="AE60:AE61" si="62">M60*G60*0.03</f>
         <v>96337.919999999998</v>
       </c>
-      <c r="AE60" s="2">
-        <f>M60*G60*AB60*AC60</f>
+      <c r="AF60" s="2">
+        <f t="shared" ref="AF60:AF61" si="63">M60*G60*AB60*AC60</f>
         <v>0</v>
       </c>
-      <c r="AF60" s="20"/>
-    </row>
-    <row r="61" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG60" s="20"/>
+    </row>
+    <row r="61" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A61" s="6" t="s">
         <v>61</v>
       </c>
@@ -5856,7 +6001,7 @@
         <v>64</v>
       </c>
       <c r="G61" s="26">
-        <f t="shared" si="49"/>
+        <f t="shared" si="56"/>
         <v>576</v>
       </c>
       <c r="H61" s="26">
@@ -5875,7 +6020,7 @@
         <v>14</v>
       </c>
       <c r="M61" s="26">
-        <f t="shared" si="50"/>
+        <f t="shared" si="57"/>
         <v>50176</v>
       </c>
       <c r="N61" s="26">
@@ -5887,7 +6032,7 @@
         <v>256</v>
       </c>
       <c r="P61" s="26">
-        <f t="shared" si="51"/>
+        <f t="shared" si="58"/>
         <v>147712</v>
       </c>
       <c r="Q61" s="45" t="str">
@@ -5915,7 +6060,7 @@
         <v>578880</v>
       </c>
       <c r="W61" s="12" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="59"/>
         <v>0008D540</v>
       </c>
       <c r="X61" s="33">
@@ -5923,7 +6068,7 @@
         <v>3615387</v>
       </c>
       <c r="Y61" s="12" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="60"/>
         <v>00372A9B</v>
       </c>
       <c r="Z61" s="33">
@@ -5931,26 +6076,30 @@
         <v>3678107</v>
       </c>
       <c r="AA61" s="13" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="61"/>
         <v>00381F9B</v>
       </c>
       <c r="AB61" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC61" s="2">
         <v>6.25E-2</v>
       </c>
       <c r="AD61" s="2">
-        <f t="shared" si="55"/>
+        <f>M61*G61</f>
+        <v>28901376</v>
+      </c>
+      <c r="AE61" s="2">
+        <f t="shared" si="62"/>
         <v>867041.27999999991</v>
       </c>
-      <c r="AE61" s="2">
-        <f>M61*G61*AB61*AC61</f>
-        <v>361267.20000000001</v>
-      </c>
-      <c r="AF61" s="20"/>
-    </row>
-    <row r="62" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF61" s="2">
+        <f t="shared" si="63"/>
+        <v>18063.36</v>
+      </c>
+      <c r="AG61" s="20"/>
+    </row>
+    <row r="62" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
         <v>62</v>
       </c>
@@ -5986,9 +6135,10 @@
       <c r="AC62" s="3"/>
       <c r="AD62" s="3"/>
       <c r="AE62" s="3"/>
-      <c r="AF62" s="20"/>
-    </row>
-    <row r="63" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF62" s="3"/>
+      <c r="AG62" s="20"/>
+    </row>
+    <row r="63" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A63" s="7" t="s">
         <v>63</v>
       </c>
@@ -6024,9 +6174,10 @@
       <c r="AC63" s="3"/>
       <c r="AD63" s="3"/>
       <c r="AE63" s="3"/>
-      <c r="AF63" s="20"/>
-    </row>
-    <row r="64" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF63" s="3"/>
+      <c r="AG63" s="20"/>
+    </row>
+    <row r="64" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>64</v>
       </c>
@@ -6066,9 +6217,10 @@
       <c r="AC64" s="1"/>
       <c r="AD64" s="1"/>
       <c r="AE64" s="1"/>
-      <c r="AF64" s="20"/>
-    </row>
-    <row r="65" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF64" s="1"/>
+      <c r="AG64" s="20"/>
+    </row>
+    <row r="65" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A65" s="38" t="s">
         <v>65</v>
       </c>
@@ -6104,9 +6256,10 @@
       <c r="AC65" s="3"/>
       <c r="AD65" s="3"/>
       <c r="AE65" s="3"/>
-      <c r="AF65" s="20"/>
-    </row>
-    <row r="66" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF65" s="3"/>
+      <c r="AG65" s="20"/>
+    </row>
+    <row r="66" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A66" s="6" t="s">
         <v>66</v>
       </c>
@@ -6205,22 +6358,26 @@
         <v>0038E39B</v>
       </c>
       <c r="AB66" s="2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="AC66" s="2">
         <v>6.25E-2</v>
       </c>
       <c r="AD66" s="2">
+        <f>M66*G66</f>
+        <v>100352000</v>
+      </c>
+      <c r="AE66" s="2">
         <f>M66*G66*0.03</f>
         <v>3010560</v>
       </c>
-      <c r="AE66" s="2">
+      <c r="AF66" s="2">
         <f>M66*G66*AB66*AC66</f>
-        <v>1254400</v>
-      </c>
-      <c r="AF66" s="20"/>
-    </row>
-    <row r="67" spans="1:32" x14ac:dyDescent="0.35">
+        <v>62720</v>
+      </c>
+      <c r="AG66" s="20"/>
+    </row>
+    <row r="67" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A67" s="7" t="s">
         <v>67</v>
       </c>
@@ -6256,9 +6413,10 @@
       <c r="AC67" s="3"/>
       <c r="AD67" s="3"/>
       <c r="AE67" s="3"/>
-      <c r="AF67" s="20"/>
-    </row>
-    <row r="68" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF67" s="3"/>
+      <c r="AG67" s="20"/>
+    </row>
+    <row r="68" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A68" s="8" t="s">
         <v>68</v>
       </c>
@@ -6345,22 +6503,26 @@
         <v>003BE13B</v>
       </c>
       <c r="AB68" s="4">
-        <v>1.2</v>
+        <v>0.1</v>
       </c>
       <c r="AC68" s="4">
         <v>6.25E-2</v>
       </c>
       <c r="AD68" s="4">
+        <f>M68*G68</f>
+        <v>196000</v>
+      </c>
+      <c r="AE68" s="4">
         <f>M68*G68*0.03</f>
         <v>5880</v>
       </c>
-      <c r="AE68" s="4">
-        <f>M68*G68*AC68</f>
-        <v>12250</v>
-      </c>
-      <c r="AF68" s="20"/>
-    </row>
-    <row r="69" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF68" s="4">
+        <f>M68*G68*AB68*AC68</f>
+        <v>1225</v>
+      </c>
+      <c r="AG68" s="20"/>
+    </row>
+    <row r="69" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>69</v>
       </c>
@@ -6396,9 +6558,10 @@
       <c r="AC69" s="1"/>
       <c r="AD69" s="1"/>
       <c r="AE69" s="1"/>
-      <c r="AF69" s="20"/>
-    </row>
-    <row r="70" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AF69" s="1"/>
+      <c r="AG69" s="20"/>
+    </row>
+    <row r="70" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A70" s="9"/>
       <c r="B70" s="24"/>
       <c r="C70" s="40"/>
@@ -6441,16 +6604,20 @@
       <c r="AB70" s="20"/>
       <c r="AC70" s="20"/>
       <c r="AD70" s="20">
-        <f>SUM(AD3:AD69)</f>
-        <v>11735481.19921875</v>
+        <f t="shared" ref="AD70" si="64">SUM(AD4:AD69)</f>
+        <v>391104608</v>
       </c>
       <c r="AE70" s="20">
-        <f t="shared" ref="AE70" si="56">SUM(AE4:AE69)</f>
-        <v>4770658.8000000007</v>
-      </c>
-      <c r="AF70" s="20"/>
-    </row>
-    <row r="71" spans="1:32" x14ac:dyDescent="0.35">
+        <f>SUM(AE3:AE69)</f>
+        <v>11733138.239999998</v>
+      </c>
+      <c r="AF70" s="52">
+        <f>SUM(AF3:AF69)</f>
+        <v>249023.83999999997</v>
+      </c>
+      <c r="AG70" s="20"/>
+    </row>
+    <row r="71" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A71" s="9"/>
       <c r="B71" s="24"/>
       <c r="C71" s="40"/>
@@ -6491,12 +6658,12 @@
       <c r="AC71" s="20"/>
       <c r="AD71" s="20"/>
       <c r="AE71" s="20"/>
-      <c r="AF71" s="20"/>
+      <c r="AF71" s="52"/>
+      <c r="AG71" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="B2:B71" xr:uid="{009522EF-F8DC-42BE-8F4B-D751FC8B03E1}"/>
   <mergeCells count="9">
-    <mergeCell ref="AB1:AE1"/>
     <mergeCell ref="K1:P1"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="K2:M2"/>
@@ -6505,6 +6672,7 @@
     <mergeCell ref="X2:Y2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="D1:G1"/>
+    <mergeCell ref="AB1:AF1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Move gemm counters to output(sum) side. fix counter logic and io errors. use macros instead of paras
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA29FF1-EEB1-458B-8187-D6EB7A71F907}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7CF654-6BEC-42C9-8646-78096A42FCE4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
   <sheets>
     <sheet name="SqueezeNet v2 MEC Parallel Ch" sheetId="2" r:id="rId1"/>
@@ -992,10 +992,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1014,15 +1023,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1347,92 +1347,92 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80B23C6-EAEB-43B1-B045-456C36085CFA}">
   <dimension ref="A1:AH71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q39" sqref="Q39"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AF10" sqref="AF10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.1796875" style="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" style="30" customWidth="1"/>
-    <col min="3" max="3" width="7.81640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.81640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="7.81640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="6.81640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.81640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.81640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.81640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7265625" style="30"/>
-    <col min="13" max="13" width="8.81640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="7.81640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.1796875" style="47" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="9.81640625" style="31" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.81640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.81640625" style="31" customWidth="1"/>
-    <col min="21" max="21" width="7.81640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.81640625" style="31" customWidth="1"/>
-    <col min="23" max="23" width="7.81640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.81640625" style="41" customWidth="1"/>
-    <col min="25" max="25" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.81640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.81640625" style="29" customWidth="1"/>
-    <col min="32" max="32" width="13.90625" style="30" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.90625" style="59" customWidth="1"/>
-    <col min="34" max="34" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="30" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="7.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="6.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="30"/>
+    <col min="13" max="13" width="8.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="7.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="9.85546875" style="31" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.85546875" style="37" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.85546875" style="31" customWidth="1"/>
+    <col min="21" max="21" width="7.85546875" style="37" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" style="31" customWidth="1"/>
+    <col min="23" max="23" width="7.85546875" style="37" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.85546875" style="41" customWidth="1"/>
+    <col min="25" max="25" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.85546875" style="29" customWidth="1"/>
+    <col min="32" max="32" width="13.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.85546875" style="59" customWidth="1"/>
+    <col min="34" max="34" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="21"/>
       <c r="B1" s="22"/>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="67" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
       <c r="F1" s="23"/>
       <c r="G1" s="54"/>
       <c r="H1" s="22"/>
       <c r="I1" s="22"/>
-      <c r="J1" s="66" t="s">
+      <c r="J1" s="69" t="s">
         <v>192</v>
       </c>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
       <c r="M1" s="52"/>
       <c r="N1" s="52"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="67" t="s">
+      <c r="O1" s="65"/>
+      <c r="P1" s="70" t="s">
         <v>80</v>
       </c>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="68"/>
-      <c r="W1" s="68"/>
-      <c r="X1" s="69"/>
+      <c r="Q1" s="71"/>
+      <c r="R1" s="71"/>
+      <c r="S1" s="71"/>
+      <c r="T1" s="71"/>
+      <c r="U1" s="71"/>
+      <c r="V1" s="71"/>
+      <c r="W1" s="71"/>
+      <c r="X1" s="72"/>
       <c r="Z1" s="52"/>
-      <c r="AA1" s="72"/>
-      <c r="AB1" s="66" t="s">
+      <c r="AA1" s="64"/>
+      <c r="AB1" s="69" t="s">
         <v>181</v>
       </c>
-      <c r="AC1" s="66"/>
-      <c r="AD1" s="66"/>
-      <c r="AE1" s="64" t="s">
+      <c r="AC1" s="69"/>
+      <c r="AD1" s="69"/>
+      <c r="AE1" s="68" t="s">
         <v>182</v>
       </c>
-      <c r="AF1" s="65"/>
+      <c r="AF1" s="67"/>
       <c r="AG1" s="63"/>
       <c r="AH1" s="20" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
@@ -1460,7 +1460,7 @@
       <c r="I2" s="24" t="s">
         <v>191</v>
       </c>
-      <c r="J2" s="74" t="s">
+      <c r="J2" s="66" t="s">
         <v>197</v>
       </c>
       <c r="M2" s="24" t="s">
@@ -1481,18 +1481,18 @@
       <c r="R2" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="S2" s="70" t="s">
+      <c r="S2" s="73" t="s">
         <v>82</v>
       </c>
-      <c r="T2" s="70"/>
-      <c r="U2" s="70" t="s">
+      <c r="T2" s="73"/>
+      <c r="U2" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="V2" s="70"/>
-      <c r="W2" s="70" t="s">
+      <c r="V2" s="73"/>
+      <c r="W2" s="73" t="s">
         <v>151</v>
       </c>
-      <c r="X2" s="71"/>
+      <c r="X2" s="74"/>
       <c r="Y2" s="20" t="s">
         <v>95</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -1686,8 +1686,8 @@
         <v>230859</v>
       </c>
       <c r="AF4" s="26">
-        <f>AE4*0.03*Z4</f>
-        <v>432.86062499999997</v>
+        <f>AE4*0.03</f>
+        <v>6925.7699999999995</v>
       </c>
       <c r="AG4" s="56">
         <f>D4*J3</f>
@@ -1698,7 +1698,7 @@
         <v>95.57709251101322</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
@@ -1738,7 +1738,7 @@
       <c r="AG5" s="57"/>
       <c r="AH5" s="20"/>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
@@ -1839,8 +1839,8 @@
         <v>1214976</v>
       </c>
       <c r="AF6" s="28">
-        <f>AE6*0.03*Z6</f>
-        <v>2278.08</v>
+        <f>AE6*0.03</f>
+        <v>36449.279999999999</v>
       </c>
       <c r="AG6" s="58">
         <f>D6*J4</f>
@@ -1851,7 +1851,7 @@
         <v>1.4867256637168142</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1964,8 +1964,8 @@
         <v>200704</v>
       </c>
       <c r="AF7" s="26">
-        <f>AE7*0.03*Z7</f>
-        <v>376.32</v>
+        <f>AE7*0.03</f>
+        <v>6021.12</v>
       </c>
       <c r="AG7" s="56">
         <f>D7*J6</f>
@@ -1976,7 +1976,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
@@ -2016,7 +2016,7 @@
       <c r="AG8" s="57"/>
       <c r="AH8" s="20"/>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -2129,19 +2129,19 @@
         <v>50176</v>
       </c>
       <c r="AF9" s="26">
-        <f t="shared" ref="AF9:AF10" si="5">AE9*0.03*Z9</f>
-        <v>94.08</v>
+        <f>AE9*0.03</f>
+        <v>1505.28</v>
       </c>
       <c r="AG9" s="56">
         <f>D9*J7</f>
         <v>56</v>
       </c>
       <c r="AH9" s="49">
-        <f t="shared" ref="AH9:AH10" si="6">AB9/AE9</f>
+        <f t="shared" ref="AH9:AH10" si="5">AB9/AE9</f>
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -2254,19 +2254,19 @@
         <v>150528</v>
       </c>
       <c r="AF10" s="26">
-        <f t="shared" si="5"/>
-        <v>282.24</v>
+        <f>AE10*0.03</f>
+        <v>4515.84</v>
       </c>
       <c r="AG10" s="56">
         <f>D10*J7</f>
         <v>168</v>
       </c>
       <c r="AH10" s="49">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
@@ -2306,7 +2306,7 @@
       <c r="AG11" s="57"/>
       <c r="AH11" s="20"/>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>12</v>
       </c>
@@ -2346,7 +2346,7 @@
       <c r="AG12" s="57"/>
       <c r="AH12" s="20"/>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>19</v>
       </c>
@@ -2392,7 +2392,7 @@
       <c r="AG13" s="55"/>
       <c r="AH13" s="20"/>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>13</v>
       </c>
@@ -2505,8 +2505,8 @@
         <v>401408</v>
       </c>
       <c r="AF14" s="26">
-        <f>AE14*0.03*Z14</f>
-        <v>752.64</v>
+        <f>AE14*0.03</f>
+        <v>12042.24</v>
       </c>
       <c r="AG14" s="56">
         <f>D14*J13</f>
@@ -2517,7 +2517,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>14</v>
       </c>
@@ -2557,7 +2557,7 @@
       <c r="AG15" s="57"/>
       <c r="AH15" s="20"/>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>64</v>
       </c>
       <c r="O16" s="26">
-        <f t="shared" ref="O16:O17" si="7">M16+N16</f>
+        <f t="shared" ref="O16:O17" si="6">M16+N16</f>
         <v>1088</v>
       </c>
       <c r="P16" s="43" t="str">
@@ -2624,7 +2624,7 @@
         <v>19360</v>
       </c>
       <c r="T16" s="12" t="str">
-        <f t="shared" ref="T16:T17" si="8">DEC2HEX(S16,8)</f>
+        <f t="shared" ref="T16:T17" si="7">DEC2HEX(S16,8)</f>
         <v>00004BA0</v>
       </c>
       <c r="U16" s="33">
@@ -2632,7 +2632,7 @@
         <v>2279451</v>
       </c>
       <c r="V16" s="12" t="str">
-        <f t="shared" ref="V16:V17" si="9">DEC2HEX(U16,8)</f>
+        <f t="shared" ref="V16:V17" si="8">DEC2HEX(U16,8)</f>
         <v>0022C81B</v>
       </c>
       <c r="W16" s="33">
@@ -2640,7 +2640,7 @@
         <v>2329627</v>
       </c>
       <c r="X16" s="13" t="str">
-        <f t="shared" ref="X16:X17" si="10">DEC2HEX(W16,8)</f>
+        <f t="shared" ref="X16:X17" si="9">DEC2HEX(W16,8)</f>
         <v>00238C1B</v>
       </c>
       <c r="Y16" s="2">
@@ -2670,19 +2670,19 @@
         <v>50176</v>
       </c>
       <c r="AF16" s="26">
-        <f t="shared" ref="AF16:AF17" si="11">AE16*0.03*Z16</f>
-        <v>94.08</v>
+        <f>AE16*0.03</f>
+        <v>1505.28</v>
       </c>
       <c r="AG16" s="56">
         <f>D16*J14</f>
         <v>56</v>
       </c>
       <c r="AH16" s="49">
-        <f t="shared" ref="AH16:AH17" si="12">AB16/AE16</f>
+        <f t="shared" ref="AH16:AH17" si="10">AB16/AE16</f>
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>64</v>
       </c>
       <c r="O17" s="26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>9280</v>
       </c>
       <c r="P17" s="43" t="str">
@@ -2749,7 +2749,7 @@
         <v>20448</v>
       </c>
       <c r="T17" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>00004FE0</v>
       </c>
       <c r="U17" s="33">
@@ -2757,7 +2757,7 @@
         <v>2279451</v>
       </c>
       <c r="V17" s="12" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0022C81B</v>
       </c>
       <c r="W17" s="33">
@@ -2765,7 +2765,7 @@
         <v>2530331</v>
       </c>
       <c r="X17" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>00269C1B</v>
       </c>
       <c r="Y17" s="2">
@@ -2795,19 +2795,19 @@
         <v>150528</v>
       </c>
       <c r="AF17" s="26">
-        <f t="shared" si="11"/>
-        <v>282.24</v>
+        <f>AE17*0.03</f>
+        <v>4515.84</v>
       </c>
       <c r="AG17" s="56">
         <f>D17*J14</f>
         <v>168</v>
       </c>
       <c r="AH17" s="49">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>17</v>
       </c>
@@ -2847,7 +2847,7 @@
       <c r="AG18" s="57"/>
       <c r="AH18" s="20"/>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>18</v>
       </c>
@@ -2887,7 +2887,7 @@
       <c r="AG19" s="57"/>
       <c r="AH19" s="20"/>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>20</v>
       </c>
@@ -2933,7 +2933,7 @@
       <c r="AG20" s="55"/>
       <c r="AH20" s="20"/>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>21</v>
       </c>
@@ -3034,19 +3034,19 @@
         <v>602112</v>
       </c>
       <c r="AF21" s="28">
-        <f>AE21*0.03*Z21</f>
-        <v>1128.96</v>
+        <f>AE21*0.03</f>
+        <v>18063.36</v>
       </c>
       <c r="AG21" s="58">
         <f>D21*J20</f>
         <v>168</v>
       </c>
       <c r="AH21" s="49">
-        <f t="shared" ref="AH21:AH22" si="13">AB21/AE21</f>
+        <f t="shared" ref="AH21:AH22" si="11">AB21/AE21</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
@@ -3159,19 +3159,19 @@
         <v>100352</v>
       </c>
       <c r="AF22" s="26">
-        <f>AE22*0.03*Z22</f>
-        <v>188.16</v>
+        <f>AE22*0.03</f>
+        <v>3010.56</v>
       </c>
       <c r="AG22" s="56">
         <f>D22*J21</f>
         <v>28</v>
       </c>
       <c r="AH22" s="49">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>23</v>
       </c>
@@ -3211,7 +3211,7 @@
       <c r="AG23" s="57"/>
       <c r="AH23" s="20"/>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>24</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>128</v>
       </c>
       <c r="O24" s="26">
-        <f t="shared" ref="O24:O25" si="14">M24+N24</f>
+        <f t="shared" ref="O24:O25" si="12">M24+N24</f>
         <v>4224</v>
       </c>
       <c r="P24" s="43" t="str">
@@ -3278,7 +3278,7 @@
         <v>33856</v>
       </c>
       <c r="T24" s="12" t="str">
-        <f t="shared" ref="T24:T25" si="15">DEC2HEX(S24,8)</f>
+        <f t="shared" ref="T24:T25" si="13">DEC2HEX(S24,8)</f>
         <v>00008440</v>
       </c>
       <c r="U24" s="33">
@@ -3286,7 +3286,7 @@
         <v>2831387</v>
       </c>
       <c r="V24" s="12" t="str">
-        <f t="shared" ref="V24:V25" si="16">DEC2HEX(U24,8)</f>
+        <f t="shared" ref="V24:V25" si="14">DEC2HEX(U24,8)</f>
         <v>002B341B</v>
       </c>
       <c r="W24" s="33">
@@ -3294,7 +3294,7 @@
         <v>2856475</v>
       </c>
       <c r="X24" s="13" t="str">
-        <f t="shared" ref="X24:X25" si="17">DEC2HEX(W24,8)</f>
+        <f t="shared" ref="X24:X25" si="15">DEC2HEX(W24,8)</f>
         <v>002B961B</v>
       </c>
       <c r="Y24" s="2">
@@ -3324,19 +3324,19 @@
         <v>25088</v>
       </c>
       <c r="AF24" s="26">
-        <f t="shared" ref="AF24:AF25" si="18">AE24*0.03*Z24</f>
-        <v>47.04</v>
+        <f>AE24*0.03</f>
+        <v>752.64</v>
       </c>
       <c r="AG24" s="56">
         <f>D24*J22</f>
         <v>28</v>
       </c>
       <c r="AH24" s="49">
-        <f t="shared" ref="AH24:AH25" si="19">AB24/AE24</f>
+        <f t="shared" ref="AH24:AH25" si="16">AB24/AE24</f>
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>25</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>128</v>
       </c>
       <c r="O25" s="26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>36992</v>
       </c>
       <c r="P25" s="43" t="str">
@@ -3403,7 +3403,7 @@
         <v>38080</v>
       </c>
       <c r="T25" s="12" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>000094C0</v>
       </c>
       <c r="U25" s="33">
@@ -3411,7 +3411,7 @@
         <v>2831387</v>
       </c>
       <c r="V25" s="12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>002B341B</v>
       </c>
       <c r="W25" s="33">
@@ -3419,7 +3419,7 @@
         <v>2956827</v>
       </c>
       <c r="X25" s="13" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>002D1E1B</v>
       </c>
       <c r="Y25" s="2">
@@ -3449,19 +3449,19 @@
         <v>75264</v>
       </c>
       <c r="AF25" s="26">
-        <f t="shared" si="18"/>
-        <v>141.12</v>
+        <f>AE25*0.03</f>
+        <v>2257.92</v>
       </c>
       <c r="AG25" s="56">
         <f>D25*J22</f>
         <v>84</v>
       </c>
       <c r="AH25" s="49">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>384</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>26</v>
       </c>
@@ -3501,7 +3501,7 @@
       <c r="AG26" s="57"/>
       <c r="AH26" s="20"/>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>27</v>
       </c>
@@ -3541,7 +3541,7 @@
       <c r="AG27" s="57"/>
       <c r="AH27" s="20"/>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>28</v>
       </c>
@@ -3587,7 +3587,7 @@
       <c r="AG28" s="55"/>
       <c r="AH28" s="20"/>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>29</v>
       </c>
@@ -3700,8 +3700,8 @@
         <v>200704</v>
       </c>
       <c r="AF29" s="26">
-        <f>AE29*0.03*Z29</f>
-        <v>376.32</v>
+        <f>AE29*0.03</f>
+        <v>6021.12</v>
       </c>
       <c r="AG29" s="56">
         <f>D29*J28</f>
@@ -3712,7 +3712,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>30</v>
       </c>
@@ -3752,7 +3752,7 @@
       <c r="AG30" s="57"/>
       <c r="AH30" s="20"/>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>31</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>128</v>
       </c>
       <c r="O31" s="26">
-        <f t="shared" ref="O31:O32" si="20">M31+N31</f>
+        <f t="shared" ref="O31:O32" si="17">M31+N31</f>
         <v>4224</v>
       </c>
       <c r="P31" s="43" t="str">
@@ -3819,7 +3819,7 @@
         <v>83296</v>
       </c>
       <c r="T31" s="12" t="str">
-        <f t="shared" ref="T31:T32" si="21">DEC2HEX(S31,8)</f>
+        <f t="shared" ref="T31:T32" si="18">DEC2HEX(S31,8)</f>
         <v>00014560</v>
       </c>
       <c r="U31" s="33">
@@ -3827,7 +3827,7 @@
         <v>3057179</v>
       </c>
       <c r="V31" s="12" t="str">
-        <f t="shared" ref="V31:V32" si="22">DEC2HEX(U31,8)</f>
+        <f t="shared" ref="V31:V32" si="19">DEC2HEX(U31,8)</f>
         <v>002EA61B</v>
       </c>
       <c r="W31" s="33">
@@ -3835,7 +3835,7 @@
         <v>3082267</v>
       </c>
       <c r="X31" s="13" t="str">
-        <f t="shared" ref="X31:X32" si="23">DEC2HEX(W31,8)</f>
+        <f t="shared" ref="X31:X32" si="20">DEC2HEX(W31,8)</f>
         <v>002F081B</v>
       </c>
       <c r="Y31" s="2">
@@ -3865,19 +3865,19 @@
         <v>25088</v>
       </c>
       <c r="AF31" s="26">
-        <f t="shared" ref="AF31:AF32" si="24">AE31*0.03*Z31</f>
-        <v>47.04</v>
+        <f>AE31*0.03</f>
+        <v>752.64</v>
       </c>
       <c r="AG31" s="56">
         <f>D31*J29</f>
         <v>28</v>
       </c>
       <c r="AH31" s="49">
-        <f t="shared" ref="AH31:AH32" si="25">AB31/AE31</f>
+        <f t="shared" ref="AH31:AH32" si="21">AB31/AE31</f>
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>32</v>
       </c>
@@ -3924,7 +3924,7 @@
         <v>128</v>
       </c>
       <c r="O32" s="26">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>36992</v>
       </c>
       <c r="P32" s="43" t="str">
@@ -3944,7 +3944,7 @@
         <v>87520</v>
       </c>
       <c r="T32" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>000155E0</v>
       </c>
       <c r="U32" s="33">
@@ -3952,7 +3952,7 @@
         <v>3057179</v>
       </c>
       <c r="V32" s="12" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>002EA61B</v>
       </c>
       <c r="W32" s="33">
@@ -3960,7 +3960,7 @@
         <v>3182619</v>
       </c>
       <c r="X32" s="13" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>0030901B</v>
       </c>
       <c r="Y32" s="2">
@@ -3990,19 +3990,19 @@
         <v>75264</v>
       </c>
       <c r="AF32" s="26">
-        <f t="shared" si="24"/>
-        <v>141.12</v>
+        <f>AE32*0.03</f>
+        <v>2257.92</v>
       </c>
       <c r="AG32" s="56">
         <f>D32*J29</f>
         <v>84</v>
       </c>
       <c r="AH32" s="49">
-        <f t="shared" si="25"/>
+        <f t="shared" si="21"/>
         <v>384</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>33</v>
       </c>
@@ -4042,7 +4042,7 @@
       <c r="AG33" s="57"/>
       <c r="AH33" s="20"/>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>34</v>
       </c>
@@ -4082,7 +4082,7 @@
       <c r="AG34" s="57"/>
       <c r="AH34" s="20"/>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>35</v>
       </c>
@@ -4128,7 +4128,7 @@
       <c r="AG35" s="55"/>
       <c r="AH35" s="20"/>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>36</v>
       </c>
@@ -4229,19 +4229,19 @@
         <v>301056</v>
       </c>
       <c r="AF36" s="28">
-        <f>AE36*0.03*Z36</f>
-        <v>564.48</v>
+        <f>AE36*0.03</f>
+        <v>9031.68</v>
       </c>
       <c r="AG36" s="58">
         <f>D36*J35</f>
         <v>84</v>
       </c>
       <c r="AH36" s="49">
-        <f t="shared" ref="AH36:AH37" si="26">AB36/AE36</f>
+        <f t="shared" ref="AH36:AH37" si="22">AB36/AE36</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>37</v>
       </c>
@@ -4354,19 +4354,19 @@
         <v>50176</v>
       </c>
       <c r="AF37" s="26">
-        <f>AE37*0.03*Z37</f>
-        <v>94.08</v>
+        <f>AE37*0.03</f>
+        <v>1505.28</v>
       </c>
       <c r="AG37" s="56">
         <f>D37*J36</f>
         <v>14</v>
       </c>
       <c r="AH37" s="49">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>38</v>
       </c>
@@ -4406,7 +4406,7 @@
       <c r="AG38" s="57"/>
       <c r="AH38" s="20"/>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>39</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>192</v>
       </c>
       <c r="O39" s="26">
-        <f t="shared" ref="O39:O40" si="27">M39+N39</f>
+        <f t="shared" ref="O39:O40" si="23">M39+N39</f>
         <v>9408</v>
       </c>
       <c r="P39" s="43" t="str">
@@ -4473,7 +4473,7 @@
         <v>136848</v>
       </c>
       <c r="T39" s="12" t="str">
-        <f t="shared" ref="T39:T40" si="28">DEC2HEX(S39,8)</f>
+        <f t="shared" ref="T39:T40" si="24">DEC2HEX(S39,8)</f>
         <v>00021690</v>
       </c>
       <c r="U39" s="33">
@@ -4481,7 +4481,7 @@
         <v>3333147</v>
       </c>
       <c r="V39" s="12" t="str">
-        <f t="shared" ref="V39:V40" si="29">DEC2HEX(U39,8)</f>
+        <f t="shared" ref="V39:V40" si="25">DEC2HEX(U39,8)</f>
         <v>0032DC1B</v>
       </c>
       <c r="W39" s="33">
@@ -4489,7 +4489,7 @@
         <v>3342555</v>
       </c>
       <c r="X39" s="13" t="str">
-        <f t="shared" ref="X39:X40" si="30">DEC2HEX(W39,8)</f>
+        <f t="shared" ref="X39:X40" si="26">DEC2HEX(W39,8)</f>
         <v>003300DB</v>
       </c>
       <c r="Y39" s="2">
@@ -4519,19 +4519,19 @@
         <v>9408</v>
       </c>
       <c r="AF39" s="26">
-        <f t="shared" ref="AF39:AF40" si="31">AE39*0.03*Z39</f>
-        <v>17.64</v>
+        <f>AE39*0.03</f>
+        <v>282.24</v>
       </c>
       <c r="AG39" s="56">
         <f>D39*J37</f>
         <v>14</v>
       </c>
       <c r="AH39" s="49">
-        <f t="shared" ref="AH39:AH40" si="32">AB39/AE39</f>
+        <f t="shared" ref="AH39:AH40" si="27">AB39/AE39</f>
         <v>192</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>40</v>
       </c>
@@ -4578,7 +4578,7 @@
         <v>192</v>
       </c>
       <c r="O40" s="26">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>83136</v>
       </c>
       <c r="P40" s="43" t="str">
@@ -4598,7 +4598,7 @@
         <v>146256</v>
       </c>
       <c r="T40" s="12" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="24"/>
         <v>00023B50</v>
       </c>
       <c r="U40" s="33">
@@ -4606,7 +4606,7 @@
         <v>3333147</v>
       </c>
       <c r="V40" s="12" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="25"/>
         <v>0032DC1B</v>
       </c>
       <c r="W40" s="33">
@@ -4614,7 +4614,7 @@
         <v>3380187</v>
       </c>
       <c r="X40" s="13" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="26"/>
         <v>003393DB</v>
       </c>
       <c r="Y40" s="2">
@@ -4644,19 +4644,19 @@
         <v>28224</v>
       </c>
       <c r="AF40" s="26">
-        <f t="shared" si="31"/>
-        <v>52.919999999999995</v>
+        <f>AE40*0.03</f>
+        <v>846.71999999999991</v>
       </c>
       <c r="AG40" s="56">
         <f>D40*J37</f>
         <v>42</v>
       </c>
       <c r="AH40" s="49">
-        <f t="shared" si="32"/>
+        <f t="shared" si="27"/>
         <v>576</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>41</v>
       </c>
@@ -4696,7 +4696,7 @@
       <c r="AG41" s="57"/>
       <c r="AH41" s="20"/>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>42</v>
       </c>
@@ -4736,7 +4736,7 @@
       <c r="AG42" s="57"/>
       <c r="AH42" s="20"/>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>43</v>
       </c>
@@ -4782,7 +4782,7 @@
       <c r="AG43" s="55"/>
       <c r="AH43" s="20"/>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>44</v>
       </c>
@@ -4895,8 +4895,8 @@
         <v>75264</v>
       </c>
       <c r="AF44" s="26">
-        <f>AE44*0.03*Z44</f>
-        <v>141.12</v>
+        <f>AE44*0.03</f>
+        <v>2257.92</v>
       </c>
       <c r="AG44" s="56">
         <f>D44*J43</f>
@@ -4907,7 +4907,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>45</v>
       </c>
@@ -4947,7 +4947,7 @@
       <c r="AG45" s="57"/>
       <c r="AH45" s="20"/>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>46</v>
       </c>
@@ -4994,7 +4994,7 @@
         <v>192</v>
       </c>
       <c r="O46" s="26">
-        <f t="shared" ref="O46:O47" si="33">M46+N46</f>
+        <f t="shared" ref="O46:O47" si="28">M46+N46</f>
         <v>9408</v>
       </c>
       <c r="P46" s="43" t="str">
@@ -5014,7 +5014,7 @@
         <v>247872</v>
       </c>
       <c r="T46" s="12" t="str">
-        <f t="shared" ref="T46:T47" si="34">DEC2HEX(S46,8)</f>
+        <f t="shared" ref="T46:T47" si="29">DEC2HEX(S46,8)</f>
         <v>0003C840</v>
       </c>
       <c r="U46" s="33">
@@ -5022,7 +5022,7 @@
         <v>3417819</v>
       </c>
       <c r="V46" s="12" t="str">
-        <f t="shared" ref="V46:V47" si="35">DEC2HEX(U46,8)</f>
+        <f t="shared" ref="V46:V47" si="30">DEC2HEX(U46,8)</f>
         <v>003426DB</v>
       </c>
       <c r="W46" s="33">
@@ -5030,7 +5030,7 @@
         <v>3427227</v>
       </c>
       <c r="X46" s="13" t="str">
-        <f t="shared" ref="X46:X47" si="36">DEC2HEX(W46,8)</f>
+        <f t="shared" ref="X46:X47" si="31">DEC2HEX(W46,8)</f>
         <v>00344B9B</v>
       </c>
       <c r="Y46" s="2">
@@ -5060,19 +5060,19 @@
         <v>9408</v>
       </c>
       <c r="AF46" s="26">
-        <f t="shared" ref="AF46:AF47" si="37">AE46*0.03*Z46</f>
-        <v>17.64</v>
+        <f>AE46*0.03</f>
+        <v>282.24</v>
       </c>
       <c r="AG46" s="56">
         <f>D46*J44</f>
         <v>14</v>
       </c>
       <c r="AH46" s="49">
-        <f t="shared" ref="AH46:AH47" si="38">AB46/AE46</f>
+        <f t="shared" ref="AH46:AH47" si="32">AB46/AE46</f>
         <v>192</v>
       </c>
     </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>47</v>
       </c>
@@ -5119,7 +5119,7 @@
         <v>192</v>
       </c>
       <c r="O47" s="26">
-        <f t="shared" si="33"/>
+        <f t="shared" si="28"/>
         <v>83136</v>
       </c>
       <c r="P47" s="43" t="str">
@@ -5139,7 +5139,7 @@
         <v>257280</v>
       </c>
       <c r="T47" s="12" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="29"/>
         <v>0003ED00</v>
       </c>
       <c r="U47" s="33">
@@ -5147,7 +5147,7 @@
         <v>3417819</v>
       </c>
       <c r="V47" s="12" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="30"/>
         <v>003426DB</v>
       </c>
       <c r="W47" s="33">
@@ -5155,7 +5155,7 @@
         <v>3464859</v>
       </c>
       <c r="X47" s="13" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="31"/>
         <v>0034DE9B</v>
       </c>
       <c r="Y47" s="2">
@@ -5185,19 +5185,19 @@
         <v>28224</v>
       </c>
       <c r="AF47" s="26">
-        <f t="shared" si="37"/>
-        <v>52.919999999999995</v>
+        <f>AE47*0.03</f>
+        <v>846.71999999999991</v>
       </c>
       <c r="AG47" s="56">
         <f>D47*J44</f>
         <v>42</v>
       </c>
       <c r="AH47" s="49">
-        <f t="shared" si="38"/>
+        <f t="shared" si="32"/>
         <v>576</v>
       </c>
     </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>48</v>
       </c>
@@ -5237,7 +5237,7 @@
       <c r="AG48" s="57"/>
       <c r="AH48" s="20"/>
     </row>
-    <row r="49" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>49</v>
       </c>
@@ -5277,7 +5277,7 @@
       <c r="AG49" s="57"/>
       <c r="AH49" s="20"/>
     </row>
-    <row r="50" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>50</v>
       </c>
@@ -5323,7 +5323,7 @@
       <c r="AG50" s="55"/>
       <c r="AH50" s="20"/>
     </row>
-    <row r="51" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>51</v>
       </c>
@@ -5436,8 +5436,8 @@
         <v>75264</v>
       </c>
       <c r="AF51" s="26">
-        <f>AE51*0.03*Z51</f>
-        <v>141.12</v>
+        <f>AE51*0.03</f>
+        <v>2257.92</v>
       </c>
       <c r="AG51" s="56">
         <f>D51*J50</f>
@@ -5448,7 +5448,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>52</v>
       </c>
@@ -5488,7 +5488,7 @@
       <c r="AG52" s="57"/>
       <c r="AH52" s="20"/>
     </row>
-    <row r="53" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>53</v>
       </c>
@@ -5535,7 +5535,7 @@
         <v>256</v>
       </c>
       <c r="O53" s="26">
-        <f t="shared" ref="O53:O54" si="39">M53+N53</f>
+        <f t="shared" ref="O53:O54" si="33">M53+N53</f>
         <v>16640</v>
       </c>
       <c r="P53" s="43" t="str">
@@ -5555,7 +5555,7 @@
         <v>365056</v>
       </c>
       <c r="T53" s="12" t="str">
-        <f t="shared" ref="T53:T54" si="40">DEC2HEX(S53,8)</f>
+        <f t="shared" ref="T53:T54" si="34">DEC2HEX(S53,8)</f>
         <v>00059200</v>
       </c>
       <c r="U53" s="33">
@@ -5563,7 +5563,7 @@
         <v>3502491</v>
       </c>
       <c r="V53" s="12" t="str">
-        <f t="shared" ref="V53:V54" si="41">DEC2HEX(U53,8)</f>
+        <f t="shared" ref="V53:V54" si="35">DEC2HEX(U53,8)</f>
         <v>0035719B</v>
       </c>
       <c r="W53" s="33">
@@ -5571,7 +5571,7 @@
         <v>3515035</v>
       </c>
       <c r="X53" s="13" t="str">
-        <f t="shared" ref="X53:X54" si="42">DEC2HEX(W53,8)</f>
+        <f t="shared" ref="X53:X54" si="36">DEC2HEX(W53,8)</f>
         <v>0035A29B</v>
       </c>
       <c r="Y53" s="2">
@@ -5601,19 +5601,19 @@
         <v>12544</v>
       </c>
       <c r="AF53" s="26">
-        <f t="shared" ref="AF53:AF54" si="43">AE53*0.03*Z53</f>
-        <v>23.52</v>
+        <f>AE53*0.03</f>
+        <v>376.32</v>
       </c>
       <c r="AG53" s="56">
         <f>D53*J51</f>
         <v>14</v>
       </c>
       <c r="AH53" s="49">
-        <f t="shared" ref="AH53:AH54" si="44">AB53/AE53</f>
+        <f t="shared" ref="AH53:AH54" si="37">AB53/AE53</f>
         <v>256</v>
       </c>
     </row>
-    <row r="54" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>54</v>
       </c>
@@ -5660,7 +5660,7 @@
         <v>256</v>
       </c>
       <c r="O54" s="26">
-        <f t="shared" si="39"/>
+        <f t="shared" si="33"/>
         <v>147712</v>
       </c>
       <c r="P54" s="43" t="str">
@@ -5680,7 +5680,7 @@
         <v>381696</v>
       </c>
       <c r="T54" s="12" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="34"/>
         <v>0005D300</v>
       </c>
       <c r="U54" s="33">
@@ -5688,7 +5688,7 @@
         <v>3502491</v>
       </c>
       <c r="V54" s="12" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="35"/>
         <v>0035719B</v>
       </c>
       <c r="W54" s="33">
@@ -5696,7 +5696,7 @@
         <v>3565211</v>
       </c>
       <c r="X54" s="13" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="36"/>
         <v>0036669B</v>
       </c>
       <c r="Y54" s="2">
@@ -5726,19 +5726,19 @@
         <v>37632</v>
       </c>
       <c r="AF54" s="26">
-        <f t="shared" si="43"/>
-        <v>70.56</v>
+        <f>AE54*0.03</f>
+        <v>1128.96</v>
       </c>
       <c r="AG54" s="56">
         <f>D54*J51</f>
         <v>42</v>
       </c>
       <c r="AH54" s="49">
-        <f t="shared" si="44"/>
+        <f t="shared" si="37"/>
         <v>768</v>
       </c>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>55</v>
       </c>
@@ -5778,7 +5778,7 @@
       <c r="AG55" s="57"/>
       <c r="AH55" s="20"/>
     </row>
-    <row r="56" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>56</v>
       </c>
@@ -5818,7 +5818,7 @@
       <c r="AG56" s="57"/>
       <c r="AH56" s="20"/>
     </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>57</v>
       </c>
@@ -5864,7 +5864,7 @@
       <c r="AG57" s="55"/>
       <c r="AH57" s="20"/>
     </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>58</v>
       </c>
@@ -5977,8 +5977,8 @@
         <v>100352</v>
       </c>
       <c r="AF58" s="26">
-        <f>AE58*0.03*Z58</f>
-        <v>188.16</v>
+        <f>AE58*0.03</f>
+        <v>3010.56</v>
       </c>
       <c r="AG58" s="56">
         <f>D58*J57</f>
@@ -5989,7 +5989,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>59</v>
       </c>
@@ -6029,7 +6029,7 @@
       <c r="AG59" s="57"/>
       <c r="AH59" s="20"/>
     </row>
-    <row r="60" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>60</v>
       </c>
@@ -6076,7 +6076,7 @@
         <v>256</v>
       </c>
       <c r="O60" s="26">
-        <f t="shared" ref="O60:O61" si="45">M60+N60</f>
+        <f t="shared" ref="O60:O61" si="38">M60+N60</f>
         <v>16640</v>
       </c>
       <c r="P60" s="43" t="str">
@@ -6096,7 +6096,7 @@
         <v>562240</v>
       </c>
       <c r="T60" s="12" t="str">
-        <f t="shared" ref="T60:T61" si="46">DEC2HEX(S60,8)</f>
+        <f t="shared" ref="T60:T61" si="39">DEC2HEX(S60,8)</f>
         <v>00089440</v>
       </c>
       <c r="U60" s="33">
@@ -6104,7 +6104,7 @@
         <v>3615387</v>
       </c>
       <c r="V60" s="12" t="str">
-        <f t="shared" ref="V60:V61" si="47">DEC2HEX(U60,8)</f>
+        <f t="shared" ref="V60:V61" si="40">DEC2HEX(U60,8)</f>
         <v>00372A9B</v>
       </c>
       <c r="W60" s="33">
@@ -6112,7 +6112,7 @@
         <v>3627931</v>
       </c>
       <c r="X60" s="13" t="str">
-        <f t="shared" ref="X60:X61" si="48">DEC2HEX(W60,8)</f>
+        <f t="shared" ref="X60:X61" si="41">DEC2HEX(W60,8)</f>
         <v>00375B9B</v>
       </c>
       <c r="Y60" s="2">
@@ -6142,19 +6142,19 @@
         <v>12544</v>
       </c>
       <c r="AF60" s="26">
-        <f t="shared" ref="AF60:AF61" si="49">AE60*0.03*Z60</f>
-        <v>23.52</v>
+        <f>AE60*0.03</f>
+        <v>376.32</v>
       </c>
       <c r="AG60" s="56">
         <f>D60*J58</f>
         <v>14</v>
       </c>
       <c r="AH60" s="49">
-        <f t="shared" ref="AH60:AH61" si="50">AB60/AE60</f>
+        <f t="shared" ref="AH60:AH61" si="42">AB60/AE60</f>
         <v>256</v>
       </c>
     </row>
-    <row r="61" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>61</v>
       </c>
@@ -6201,7 +6201,7 @@
         <v>256</v>
       </c>
       <c r="O61" s="26">
-        <f t="shared" si="45"/>
+        <f t="shared" si="38"/>
         <v>147712</v>
       </c>
       <c r="P61" s="43" t="str">
@@ -6221,7 +6221,7 @@
         <v>578880</v>
       </c>
       <c r="T61" s="12" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="39"/>
         <v>0008D540</v>
       </c>
       <c r="U61" s="33">
@@ -6229,7 +6229,7 @@
         <v>3615387</v>
       </c>
       <c r="V61" s="12" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="40"/>
         <v>00372A9B</v>
       </c>
       <c r="W61" s="33">
@@ -6237,7 +6237,7 @@
         <v>3678107</v>
       </c>
       <c r="X61" s="13" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="41"/>
         <v>00381F9B</v>
       </c>
       <c r="Y61" s="2">
@@ -6267,19 +6267,19 @@
         <v>37632</v>
       </c>
       <c r="AF61" s="26">
-        <f t="shared" si="49"/>
-        <v>70.56</v>
+        <f>AE61*0.03</f>
+        <v>1128.96</v>
       </c>
       <c r="AG61" s="56">
         <f>D61*J58</f>
         <v>42</v>
       </c>
       <c r="AH61" s="49">
-        <f t="shared" si="50"/>
+        <f t="shared" si="42"/>
         <v>768</v>
       </c>
     </row>
-    <row r="62" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>62</v>
       </c>
@@ -6319,7 +6319,7 @@
       <c r="AG62" s="57"/>
       <c r="AH62" s="20"/>
     </row>
-    <row r="63" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>63</v>
       </c>
@@ -6359,7 +6359,7 @@
       <c r="AG63" s="57"/>
       <c r="AH63" s="20"/>
     </row>
-    <row r="64" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>64</v>
       </c>
@@ -6405,7 +6405,7 @@
       <c r="AG64" s="55"/>
       <c r="AH64" s="20"/>
     </row>
-    <row r="65" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A65" s="38" t="s">
         <v>65</v>
       </c>
@@ -6445,7 +6445,7 @@
       <c r="AG65" s="57"/>
       <c r="AH65" s="20"/>
     </row>
-    <row r="66" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>66</v>
       </c>
@@ -6558,8 +6558,8 @@
         <v>100352</v>
       </c>
       <c r="AF66" s="26">
-        <f>AE66*0.03*Z66</f>
-        <v>188.16</v>
+        <f>AE66*0.03</f>
+        <v>3010.56</v>
       </c>
       <c r="AG66" s="56">
         <f>D66*J64</f>
@@ -6570,7 +6570,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="67" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>67</v>
       </c>
@@ -6610,7 +6610,7 @@
       <c r="AG67" s="57"/>
       <c r="AH67" s="20"/>
     </row>
-    <row r="68" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>68</v>
       </c>
@@ -6711,8 +6711,8 @@
         <v>196000</v>
       </c>
       <c r="AF68" s="28">
-        <f>AE68*0.03*Z68</f>
-        <v>367.5</v>
+        <f>AE68*0.03</f>
+        <v>5880</v>
       </c>
       <c r="AG68" s="58">
         <f>D68*J66</f>
@@ -6723,7 +6723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>69</v>
       </c>
@@ -6762,7 +6762,7 @@
       <c r="AF69" s="25"/>
       <c r="AG69" s="55"/>
     </row>
-    <row r="70" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A70" s="9"/>
       <c r="B70" s="24"/>
       <c r="C70" s="40"/>
@@ -6803,7 +6803,7 @@
       <c r="Z70" s="20"/>
       <c r="AA70" s="48"/>
       <c r="AB70" s="20">
-        <f t="shared" ref="AB70" si="51">SUM(AB4:AB69)</f>
+        <f t="shared" ref="AB70" si="43">SUM(AB4:AB69)</f>
         <v>391104608</v>
       </c>
       <c r="AC70" s="20">
@@ -6820,15 +6820,15 @@
       </c>
       <c r="AF70" s="62">
         <f>SUM(AF4:AF69)</f>
-        <v>8676.2006250000013</v>
+        <v>138819.21000000002</v>
       </c>
       <c r="AG70" s="61"/>
       <c r="AH70" s="20">
         <f>AC70/AF70/16</f>
-        <v>84.520998498694794</v>
-      </c>
-    </row>
-    <row r="71" spans="1:34" x14ac:dyDescent="0.35">
+        <v>5.2825624061684247</v>
+      </c>
+    </row>
+    <row r="71" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A71" s="9"/>
       <c r="B71" s="24"/>
       <c r="C71" s="40"/>
@@ -6876,14 +6876,14 @@
   </sheetData>
   <autoFilter ref="B2:B71" xr:uid="{009522EF-F8DC-42BE-8F4B-D751FC8B03E1}"/>
   <mergeCells count="8">
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="S2:T2"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AB1:AD1"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="P1:X1"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="S2:T2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6901,15 +6901,15 @@
       <selection activeCell="H1" sqref="H1:M30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="43" t="s">
         <v>200</v>
       </c>
@@ -6929,31 +6929,31 @@
         <v>117</v>
       </c>
       <c r="H1" t="str">
-        <f>LEFT(SUBSTITUTE(A1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A1,"_",),4)</f>
+        <f t="shared" ref="H1:H30" si="0">LEFT(SUBSTITUTE(A1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A1,"_",),4)</f>
         <v>0003 0202</v>
       </c>
       <c r="I1" t="str">
-        <f>LEFT(SUBSTITUTE(B1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B1,"_",),4)</f>
+        <f t="shared" ref="I1:I30" si="1">LEFT(SUBSTITUTE(B1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B1,"_",),4)</f>
         <v>0040 0003</v>
       </c>
       <c r="J1" t="str">
-        <f>LEFT(SUBSTITUTE(C1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C1,"_",),4)</f>
+        <f t="shared" ref="J1:J30" si="2">LEFT(SUBSTITUTE(C1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C1,"_",),4)</f>
         <v>0000 71E3</v>
       </c>
       <c r="K1" t="str">
-        <f>LEFT(SUBSTITUTE(D1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D1,"_",),4)</f>
+        <f t="shared" ref="K1:K30" si="3">LEFT(SUBSTITUTE(D1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D1,"_",),4)</f>
         <v>0000 1000</v>
       </c>
       <c r="L1" t="str">
-        <f>LEFT(SUBSTITUTE(E1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E1,"_",),4)</f>
+        <f t="shared" ref="L1:L30" si="4">LEFT(SUBSTITUTE(E1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E1,"_",),4)</f>
         <v>000A 0000</v>
       </c>
       <c r="M1" t="str">
-        <f>LEFT(SUBSTITUTE(F1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F1,"_",),4)</f>
+        <f t="shared" ref="M1:M30" si="5">LEFT(SUBSTITUTE(F1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F1,"_",),4)</f>
         <v>000C 5BDB</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
         <v>202</v>
       </c>
@@ -6973,31 +6973,31 @@
         <v>118</v>
       </c>
       <c r="H2" t="str">
-        <f>LEFT(SUBSTITUTE(A2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A2,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0003 0204</v>
       </c>
       <c r="I2" t="str">
-        <f>LEFT(SUBSTITUTE(B2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B2,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>0040 0040</v>
       </c>
       <c r="J2" t="str">
-        <f>LEFT(SUBSTITUTE(C2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C2,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 3871</v>
       </c>
       <c r="K2" t="str">
-        <f>LEFT(SUBSTITUTE(D2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D2,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0000 0000</v>
       </c>
       <c r="L2" t="str">
-        <f>LEFT(SUBSTITUTE(E2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E2,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>000C 5BDB</v>
       </c>
       <c r="M2" t="str">
-        <f>LEFT(SUBSTITUTE(F2,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F2,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>0018 D41B</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
         <v>204</v>
       </c>
@@ -7017,31 +7017,31 @@
         <v>120</v>
       </c>
       <c r="H3" t="str">
-        <f>LEFT(SUBSTITUTE(A3,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A3,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0001 0101</v>
       </c>
       <c r="I3" t="str">
-        <f>LEFT(SUBSTITUTE(B3,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B3,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>0010 0040</v>
       </c>
       <c r="J3" t="str">
-        <f>LEFT(SUBSTITUTE(C3,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C3,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 3838</v>
       </c>
       <c r="K3" t="str">
-        <f>LEFT(SUBSTITUTE(D3,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D3,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0000 1700</v>
       </c>
       <c r="L3" t="str">
-        <f>LEFT(SUBSTITUTE(E3,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E3,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>0018 D41B</v>
       </c>
       <c r="M3" t="str">
-        <f>LEFT(SUBSTITUTE(F3,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F3,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>001B E41B</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
         <v>204</v>
       </c>
@@ -7061,31 +7061,31 @@
         <v>121</v>
       </c>
       <c r="H4" t="str">
-        <f>LEFT(SUBSTITUTE(A4,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A4,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0001 0101</v>
       </c>
       <c r="I4" t="str">
-        <f>LEFT(SUBSTITUTE(B4,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B4,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>0040 0010</v>
       </c>
       <c r="J4" t="str">
-        <f>LEFT(SUBSTITUTE(C4,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C4,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 3838</v>
       </c>
       <c r="K4" t="str">
-        <f>LEFT(SUBSTITUTE(D4,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D4,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0000 1B10</v>
       </c>
       <c r="L4" t="str">
-        <f>LEFT(SUBSTITUTE(E4,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E4,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>001B E41B</v>
       </c>
       <c r="M4" t="str">
-        <f>LEFT(SUBSTITUTE(F4,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F4,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>001C A81B</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
         <v>206</v>
       </c>
@@ -7105,31 +7105,31 @@
         <v>122</v>
       </c>
       <c r="H5" t="str">
-        <f>LEFT(SUBSTITUTE(A5,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A5,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0003 0112</v>
       </c>
       <c r="I5" t="str">
-        <f>LEFT(SUBSTITUTE(B5,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B5,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>0040 0010</v>
       </c>
       <c r="J5" t="str">
-        <f>LEFT(SUBSTITUTE(C5,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C5,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 3838</v>
       </c>
       <c r="K5" t="str">
-        <f>LEFT(SUBSTITUTE(D5,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D5,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0000 1F50</v>
       </c>
       <c r="L5" t="str">
-        <f>LEFT(SUBSTITUTE(E5,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E5,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>001B E41B</v>
       </c>
       <c r="M5" t="str">
-        <f>LEFT(SUBSTITUTE(F5,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F5,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>001F B81B</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
         <v>204</v>
       </c>
@@ -7149,31 +7149,31 @@
         <v>123</v>
       </c>
       <c r="H6" t="str">
-        <f>LEFT(SUBSTITUTE(A6,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A6,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0001 0101</v>
       </c>
       <c r="I6" t="str">
-        <f>LEFT(SUBSTITUTE(B6,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B6,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>0010 0080</v>
       </c>
       <c r="J6" t="str">
-        <f>LEFT(SUBSTITUTE(C6,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C6,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 3838</v>
       </c>
       <c r="K6" t="str">
-        <f>LEFT(SUBSTITUTE(D6,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D6,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0000 4390</v>
       </c>
       <c r="L6" t="str">
-        <f>LEFT(SUBSTITUTE(E6,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E6,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>001F B81B</v>
       </c>
       <c r="M6" t="str">
-        <f>LEFT(SUBSTITUTE(F6,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F6,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>0022 C81B</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="43" t="s">
         <v>204</v>
       </c>
@@ -7193,31 +7193,31 @@
         <v>124</v>
       </c>
       <c r="H7" t="str">
-        <f>LEFT(SUBSTITUTE(A7,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A7,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0001 0101</v>
       </c>
       <c r="I7" t="str">
-        <f>LEFT(SUBSTITUTE(B7,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B7,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>0040 0010</v>
       </c>
       <c r="J7" t="str">
-        <f>LEFT(SUBSTITUTE(C7,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C7,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 3838</v>
       </c>
       <c r="K7" t="str">
-        <f>LEFT(SUBSTITUTE(D7,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D7,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0000 4BA0</v>
       </c>
       <c r="L7" t="str">
-        <f>LEFT(SUBSTITUTE(E7,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E7,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>0022 C81B</v>
       </c>
       <c r="M7" t="str">
-        <f>LEFT(SUBSTITUTE(F7,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F7,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>0023 8C1B</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
         <v>206</v>
       </c>
@@ -7237,31 +7237,31 @@
         <v>125</v>
       </c>
       <c r="H8" t="str">
-        <f>LEFT(SUBSTITUTE(A8,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A8,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0003 0112</v>
       </c>
       <c r="I8" t="str">
-        <f>LEFT(SUBSTITUTE(B8,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B8,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>0040 0010</v>
       </c>
       <c r="J8" t="str">
-        <f>LEFT(SUBSTITUTE(C8,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C8,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 3838</v>
       </c>
       <c r="K8" t="str">
-        <f>LEFT(SUBSTITUTE(D8,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D8,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0000 4FE0</v>
       </c>
       <c r="L8" t="str">
-        <f>LEFT(SUBSTITUTE(E8,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E8,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>0022 C81B</v>
       </c>
       <c r="M8" t="str">
-        <f>LEFT(SUBSTITUTE(F8,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F8,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>0026 9C1B</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="45" t="s">
         <v>202</v>
       </c>
@@ -7281,31 +7281,31 @@
         <v>126</v>
       </c>
       <c r="H9" t="str">
-        <f>LEFT(SUBSTITUTE(A9,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A9,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0003 0204</v>
       </c>
       <c r="I9" t="str">
-        <f>LEFT(SUBSTITUTE(B9,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B9,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>0080 0080</v>
       </c>
       <c r="J9" t="str">
-        <f>LEFT(SUBSTITUTE(C9,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C9,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 1C38</v>
       </c>
       <c r="K9" t="str">
-        <f>LEFT(SUBSTITUTE(D9,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D9,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0000 0000</v>
       </c>
       <c r="L9" t="str">
-        <f>LEFT(SUBSTITUTE(E9,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E9,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>0026 9C1B</v>
       </c>
       <c r="M9" t="str">
-        <f>LEFT(SUBSTITUTE(F9,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F9,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>0029 AC1B</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="43" t="s">
         <v>204</v>
       </c>
@@ -7325,31 +7325,31 @@
         <v>127</v>
       </c>
       <c r="H10" t="str">
-        <f>LEFT(SUBSTITUTE(A10,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A10,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0001 0101</v>
       </c>
       <c r="I10" t="str">
-        <f>LEFT(SUBSTITUTE(B10,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B10,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>0020 0080</v>
       </c>
       <c r="J10" t="str">
-        <f>LEFT(SUBSTITUTE(C10,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C10,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 1C1C</v>
       </c>
       <c r="K10" t="str">
-        <f>LEFT(SUBSTITUTE(D10,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D10,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0000 7420</v>
       </c>
       <c r="L10" t="str">
-        <f>LEFT(SUBSTITUTE(E10,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E10,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>0029 AC1B</v>
       </c>
       <c r="M10" t="str">
-        <f>LEFT(SUBSTITUTE(F10,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F10,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>002B 341B</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="43" t="s">
         <v>204</v>
       </c>
@@ -7369,31 +7369,31 @@
         <v>128</v>
       </c>
       <c r="H11" t="str">
-        <f>LEFT(SUBSTITUTE(A11,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A11,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0001 0101</v>
       </c>
       <c r="I11" t="str">
-        <f>LEFT(SUBSTITUTE(B11,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B11,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>0080 0020</v>
       </c>
       <c r="J11" t="str">
-        <f>LEFT(SUBSTITUTE(C11,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C11,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 1C1C</v>
       </c>
       <c r="K11" t="str">
-        <f>LEFT(SUBSTITUTE(D11,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D11,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0000 8440</v>
       </c>
       <c r="L11" t="str">
-        <f>LEFT(SUBSTITUTE(E11,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E11,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>002B 341B</v>
       </c>
       <c r="M11" t="str">
-        <f>LEFT(SUBSTITUTE(F11,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F11,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>002B 961B</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="43" t="s">
         <v>206</v>
       </c>
@@ -7413,31 +7413,31 @@
         <v>129</v>
       </c>
       <c r="H12" t="str">
-        <f>LEFT(SUBSTITUTE(A12,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A12,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0003 0112</v>
       </c>
       <c r="I12" t="str">
-        <f>LEFT(SUBSTITUTE(B12,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B12,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>0080 0020</v>
       </c>
       <c r="J12" t="str">
-        <f>LEFT(SUBSTITUTE(C12,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C12,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 1C1C</v>
       </c>
       <c r="K12" t="str">
-        <f>LEFT(SUBSTITUTE(D12,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D12,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0000 94C0</v>
       </c>
       <c r="L12" t="str">
-        <f>LEFT(SUBSTITUTE(E12,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E12,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>002B 341B</v>
       </c>
       <c r="M12" t="str">
-        <f>LEFT(SUBSTITUTE(F12,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F12,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>002D 1E1B</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="43" t="s">
         <v>204</v>
       </c>
@@ -7457,31 +7457,31 @@
         <v>130</v>
       </c>
       <c r="H13" t="str">
-        <f>LEFT(SUBSTITUTE(A13,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A13,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0001 0101</v>
       </c>
       <c r="I13" t="str">
-        <f>LEFT(SUBSTITUTE(B13,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B13,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>0020 0100</v>
       </c>
       <c r="J13" t="str">
-        <f>LEFT(SUBSTITUTE(C13,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C13,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 1C1C</v>
       </c>
       <c r="K13" t="str">
-        <f>LEFT(SUBSTITUTE(D13,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D13,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0001 2540</v>
       </c>
       <c r="L13" t="str">
-        <f>LEFT(SUBSTITUTE(E13,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E13,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>002D 1E1B</v>
       </c>
       <c r="M13" t="str">
-        <f>LEFT(SUBSTITUTE(F13,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F13,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>002E A61B</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="43" t="s">
         <v>204</v>
       </c>
@@ -7501,31 +7501,31 @@
         <v>131</v>
       </c>
       <c r="H14" t="str">
-        <f>LEFT(SUBSTITUTE(A14,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A14,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0001 0101</v>
       </c>
       <c r="I14" t="str">
-        <f>LEFT(SUBSTITUTE(B14,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B14,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>0080 0020</v>
       </c>
       <c r="J14" t="str">
-        <f>LEFT(SUBSTITUTE(C14,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C14,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 1C1C</v>
       </c>
       <c r="K14" t="str">
-        <f>LEFT(SUBSTITUTE(D14,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D14,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0001 4560</v>
       </c>
       <c r="L14" t="str">
-        <f>LEFT(SUBSTITUTE(E14,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E14,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>002E A61B</v>
       </c>
       <c r="M14" t="str">
-        <f>LEFT(SUBSTITUTE(F14,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F14,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>002F 081B</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="43" t="s">
         <v>206</v>
       </c>
@@ -7545,31 +7545,31 @@
         <v>132</v>
       </c>
       <c r="H15" t="str">
-        <f>LEFT(SUBSTITUTE(A15,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A15,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0003 0112</v>
       </c>
       <c r="I15" t="str">
-        <f>LEFT(SUBSTITUTE(B15,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B15,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>0080 0020</v>
       </c>
       <c r="J15" t="str">
-        <f>LEFT(SUBSTITUTE(C15,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C15,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 1C1C</v>
       </c>
       <c r="K15" t="str">
-        <f>LEFT(SUBSTITUTE(D15,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D15,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0001 55E0</v>
       </c>
       <c r="L15" t="str">
-        <f>LEFT(SUBSTITUTE(E15,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E15,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>002E A61B</v>
       </c>
       <c r="M15" t="str">
-        <f>LEFT(SUBSTITUTE(F15,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F15,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>0030 901B</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="45" t="s">
         <v>202</v>
       </c>
@@ -7589,31 +7589,31 @@
         <v>133</v>
       </c>
       <c r="H16" t="str">
-        <f>LEFT(SUBSTITUTE(A16,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A16,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0003 0204</v>
       </c>
       <c r="I16" t="str">
-        <f>LEFT(SUBSTITUTE(B16,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B16,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>0100 0100</v>
       </c>
       <c r="J16" t="str">
-        <f>LEFT(SUBSTITUTE(C16,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C16,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 0E1C</v>
       </c>
       <c r="K16" t="str">
-        <f>LEFT(SUBSTITUTE(D16,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D16,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0000 0000</v>
       </c>
       <c r="L16" t="str">
-        <f>LEFT(SUBSTITUTE(E16,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E16,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>0030 901B</v>
       </c>
       <c r="M16" t="str">
-        <f>LEFT(SUBSTITUTE(F16,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F16,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>0032 181B</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="43" t="s">
         <v>204</v>
       </c>
@@ -7633,31 +7633,31 @@
         <v>134</v>
       </c>
       <c r="H17" t="str">
-        <f>LEFT(SUBSTITUTE(A17,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A17,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0001 0101</v>
       </c>
       <c r="I17" t="str">
-        <f>LEFT(SUBSTITUTE(B17,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B17,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>0030 0100</v>
       </c>
       <c r="J17" t="str">
-        <f>LEFT(SUBSTITUTE(C17,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C17,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 0E0E</v>
       </c>
       <c r="K17" t="str">
-        <f>LEFT(SUBSTITUTE(D17,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D17,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0001 E660</v>
       </c>
       <c r="L17" t="str">
-        <f>LEFT(SUBSTITUTE(E17,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E17,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>0032 181B</v>
       </c>
       <c r="M17" t="str">
-        <f>LEFT(SUBSTITUTE(F17,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F17,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>0032 DC1B</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="43" t="s">
         <v>204</v>
       </c>
@@ -7677,31 +7677,31 @@
         <v>135</v>
       </c>
       <c r="H18" t="str">
-        <f>LEFT(SUBSTITUTE(A18,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A18,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0001 0101</v>
       </c>
       <c r="I18" t="str">
-        <f>LEFT(SUBSTITUTE(B18,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B18,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>00C0 0030</v>
       </c>
       <c r="J18" t="str">
-        <f>LEFT(SUBSTITUTE(C18,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C18,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 0E0E</v>
       </c>
       <c r="K18" t="str">
-        <f>LEFT(SUBSTITUTE(D18,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D18,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0002 1690</v>
       </c>
       <c r="L18" t="str">
-        <f>LEFT(SUBSTITUTE(E18,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E18,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>0032 DC1B</v>
       </c>
       <c r="M18" t="str">
-        <f>LEFT(SUBSTITUTE(F18,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F18,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>0033 00DB</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="43" t="s">
         <v>206</v>
       </c>
@@ -7721,31 +7721,31 @@
         <v>137</v>
       </c>
       <c r="H19" t="str">
-        <f>LEFT(SUBSTITUTE(A19,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A19,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0003 0112</v>
       </c>
       <c r="I19" t="str">
-        <f>LEFT(SUBSTITUTE(B19,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B19,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>00C0 0030</v>
       </c>
       <c r="J19" t="str">
-        <f>LEFT(SUBSTITUTE(C19,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C19,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 0E0E</v>
       </c>
       <c r="K19" t="str">
-        <f>LEFT(SUBSTITUTE(D19,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D19,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0002 3B50</v>
       </c>
       <c r="L19" t="str">
-        <f>LEFT(SUBSTITUTE(E19,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E19,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>0032 DC1B</v>
       </c>
       <c r="M19" t="str">
-        <f>LEFT(SUBSTITUTE(F19,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F19,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>0033 93DB</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="43" t="s">
         <v>204</v>
       </c>
@@ -7765,31 +7765,31 @@
         <v>138</v>
       </c>
       <c r="H20" t="str">
-        <f>LEFT(SUBSTITUTE(A20,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A20,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0001 0101</v>
       </c>
       <c r="I20" t="str">
-        <f>LEFT(SUBSTITUTE(B20,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B20,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>0030 0180</v>
       </c>
       <c r="J20" t="str">
-        <f>LEFT(SUBSTITUTE(C20,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C20,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 0E0E</v>
       </c>
       <c r="K20" t="str">
-        <f>LEFT(SUBSTITUTE(D20,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D20,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0003 8010</v>
       </c>
       <c r="L20" t="str">
-        <f>LEFT(SUBSTITUTE(E20,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E20,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>0033 93DB</v>
       </c>
       <c r="M20" t="str">
-        <f>LEFT(SUBSTITUTE(F20,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F20,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>0034 26DB</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="43" t="s">
         <v>204</v>
       </c>
@@ -7809,31 +7809,31 @@
         <v>139</v>
       </c>
       <c r="H21" t="str">
-        <f>LEFT(SUBSTITUTE(A21,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A21,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0001 0101</v>
       </c>
       <c r="I21" t="str">
-        <f>LEFT(SUBSTITUTE(B21,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B21,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>00C0 0030</v>
       </c>
       <c r="J21" t="str">
-        <f>LEFT(SUBSTITUTE(C21,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C21,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 0E0E</v>
       </c>
       <c r="K21" t="str">
-        <f>LEFT(SUBSTITUTE(D21,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D21,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0003 C840</v>
       </c>
       <c r="L21" t="str">
-        <f>LEFT(SUBSTITUTE(E21,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E21,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>0034 26DB</v>
       </c>
       <c r="M21" t="str">
-        <f>LEFT(SUBSTITUTE(F21,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F21,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>0034 4B9B</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="43" t="s">
         <v>206</v>
       </c>
@@ -7853,31 +7853,31 @@
         <v>140</v>
       </c>
       <c r="H22" t="str">
-        <f>LEFT(SUBSTITUTE(A22,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A22,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0003 0112</v>
       </c>
       <c r="I22" t="str">
-        <f>LEFT(SUBSTITUTE(B22,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B22,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>00C0 0030</v>
       </c>
       <c r="J22" t="str">
-        <f>LEFT(SUBSTITUTE(C22,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C22,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 0E0E</v>
       </c>
       <c r="K22" t="str">
-        <f>LEFT(SUBSTITUTE(D22,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D22,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0003 ED00</v>
       </c>
       <c r="L22" t="str">
-        <f>LEFT(SUBSTITUTE(E22,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E22,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>0034 26DB</v>
       </c>
       <c r="M22" t="str">
-        <f>LEFT(SUBSTITUTE(F22,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F22,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>0034 DE9B</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="43" t="s">
         <v>204</v>
       </c>
@@ -7897,31 +7897,31 @@
         <v>141</v>
       </c>
       <c r="H23" t="str">
-        <f>LEFT(SUBSTITUTE(A23,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A23,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0001 0101</v>
       </c>
       <c r="I23" t="str">
-        <f>LEFT(SUBSTITUTE(B23,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B23,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>0040 0180</v>
       </c>
       <c r="J23" t="str">
-        <f>LEFT(SUBSTITUTE(C23,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C23,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 0E0E</v>
       </c>
       <c r="K23" t="str">
-        <f>LEFT(SUBSTITUTE(D23,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D23,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0005 31C0</v>
       </c>
       <c r="L23" t="str">
-        <f>LEFT(SUBSTITUTE(E23,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E23,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>0034 DE9B</v>
       </c>
       <c r="M23" t="str">
-        <f>LEFT(SUBSTITUTE(F23,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F23,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>0035 719B</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="43" t="s">
         <v>204</v>
       </c>
@@ -7941,31 +7941,31 @@
         <v>142</v>
       </c>
       <c r="H24" t="str">
-        <f>LEFT(SUBSTITUTE(A24,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A24,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0001 0101</v>
       </c>
       <c r="I24" t="str">
-        <f>LEFT(SUBSTITUTE(B24,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B24,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>0100 0040</v>
       </c>
       <c r="J24" t="str">
-        <f>LEFT(SUBSTITUTE(C24,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C24,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 0E0E</v>
       </c>
       <c r="K24" t="str">
-        <f>LEFT(SUBSTITUTE(D24,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D24,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0005 9200</v>
       </c>
       <c r="L24" t="str">
-        <f>LEFT(SUBSTITUTE(E24,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E24,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>0035 719B</v>
       </c>
       <c r="M24" t="str">
-        <f>LEFT(SUBSTITUTE(F24,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F24,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>0035 A29B</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="43" t="s">
         <v>206</v>
       </c>
@@ -7985,31 +7985,31 @@
         <v>143</v>
       </c>
       <c r="H25" t="str">
-        <f>LEFT(SUBSTITUTE(A25,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A25,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0003 0112</v>
       </c>
       <c r="I25" t="str">
-        <f>LEFT(SUBSTITUTE(B25,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B25,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>0100 0040</v>
       </c>
       <c r="J25" t="str">
-        <f>LEFT(SUBSTITUTE(C25,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C25,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 0E0E</v>
       </c>
       <c r="K25" t="str">
-        <f>LEFT(SUBSTITUTE(D25,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D25,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0005 D300</v>
       </c>
       <c r="L25" t="str">
-        <f>LEFT(SUBSTITUTE(E25,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E25,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>0035 719B</v>
       </c>
       <c r="M25" t="str">
-        <f>LEFT(SUBSTITUTE(F25,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F25,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>0036 669B</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="43" t="s">
         <v>204</v>
       </c>
@@ -8029,31 +8029,31 @@
         <v>144</v>
       </c>
       <c r="H26" t="str">
-        <f>LEFT(SUBSTITUTE(A26,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A26,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0001 0101</v>
       </c>
       <c r="I26" t="str">
-        <f>LEFT(SUBSTITUTE(B26,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B26,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>0040 0200</v>
       </c>
       <c r="J26" t="str">
-        <f>LEFT(SUBSTITUTE(C26,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C26,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 0E0E</v>
       </c>
       <c r="K26" t="str">
-        <f>LEFT(SUBSTITUTE(D26,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D26,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0008 1400</v>
       </c>
       <c r="L26" t="str">
-        <f>LEFT(SUBSTITUTE(E26,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E26,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>0036 669B</v>
       </c>
       <c r="M26" t="str">
-        <f>LEFT(SUBSTITUTE(F26,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F26,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>0037 2A9B</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="43" t="s">
         <v>204</v>
       </c>
@@ -8073,31 +8073,31 @@
         <v>145</v>
       </c>
       <c r="H27" t="str">
-        <f>LEFT(SUBSTITUTE(A27,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A27,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0001 0101</v>
       </c>
       <c r="I27" t="str">
-        <f>LEFT(SUBSTITUTE(B27,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B27,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>0100 0040</v>
       </c>
       <c r="J27" t="str">
-        <f>LEFT(SUBSTITUTE(C27,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C27,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 0E0E</v>
       </c>
       <c r="K27" t="str">
-        <f>LEFT(SUBSTITUTE(D27,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D27,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0008 9440</v>
       </c>
       <c r="L27" t="str">
-        <f>LEFT(SUBSTITUTE(E27,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E27,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>0037 2A9B</v>
       </c>
       <c r="M27" t="str">
-        <f>LEFT(SUBSTITUTE(F27,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F27,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>0037 5B9B</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="43" t="s">
         <v>206</v>
       </c>
@@ -8117,31 +8117,31 @@
         <v>146</v>
       </c>
       <c r="H28" t="str">
-        <f>LEFT(SUBSTITUTE(A28,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A28,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0003 0112</v>
       </c>
       <c r="I28" t="str">
-        <f>LEFT(SUBSTITUTE(B28,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B28,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>0100 0040</v>
       </c>
       <c r="J28" t="str">
-        <f>LEFT(SUBSTITUTE(C28,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C28,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 0E0E</v>
       </c>
       <c r="K28" t="str">
-        <f>LEFT(SUBSTITUTE(D28,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D28,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0008 D540</v>
       </c>
       <c r="L28" t="str">
-        <f>LEFT(SUBSTITUTE(E28,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E28,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>0037 2A9B</v>
       </c>
       <c r="M28" t="str">
-        <f>LEFT(SUBSTITUTE(F28,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F28,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>0038 1F9B</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="43" t="s">
         <v>204</v>
       </c>
@@ -8161,31 +8161,31 @@
         <v>147</v>
       </c>
       <c r="H29" t="str">
-        <f>LEFT(SUBSTITUTE(A29,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A29,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0001 0101</v>
       </c>
       <c r="I29" t="str">
-        <f>LEFT(SUBSTITUTE(B29,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B29,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>03E8 0200</v>
       </c>
       <c r="J29" t="str">
-        <f>LEFT(SUBSTITUTE(C29,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C29,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 0E0E</v>
       </c>
       <c r="K29" t="str">
-        <f>LEFT(SUBSTITUTE(D29,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D29,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>000B 1640</v>
       </c>
       <c r="L29" t="str">
-        <f>LEFT(SUBSTITUTE(E29,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E29,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>0038 1F9B</v>
       </c>
       <c r="M29" t="str">
-        <f>LEFT(SUBSTITUTE(F29,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F29,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>0038 E39B</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="45" t="s">
         <v>211</v>
       </c>
@@ -8205,27 +8205,27 @@
         <v>149</v>
       </c>
       <c r="H30" t="str">
-        <f>LEFT(SUBSTITUTE(A30,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A30,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>000E 0105</v>
       </c>
       <c r="I30" t="str">
-        <f>LEFT(SUBSTITUTE(B30,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B30,"_",),4)</f>
+        <f t="shared" si="1"/>
         <v>03E8 03E8</v>
       </c>
       <c r="J30" t="str">
-        <f>LEFT(SUBSTITUTE(C30,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C30,"_",),4)</f>
+        <f t="shared" si="2"/>
         <v>0000 010E</v>
       </c>
       <c r="K30" t="str">
-        <f>LEFT(SUBSTITUTE(D30,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D30,"_",),4)</f>
+        <f t="shared" si="3"/>
         <v>0000 0000</v>
       </c>
       <c r="L30" t="str">
-        <f>LEFT(SUBSTITUTE(E30,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E30,"_",),4)</f>
+        <f t="shared" si="4"/>
         <v>0038 E39B</v>
       </c>
       <c r="M30" t="str">
-        <f>LEFT(SUBSTITUTE(F30,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F30,"_",),4)</f>
+        <f t="shared" si="5"/>
         <v>003B E13B</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update weight reshape and split code. Fix bytearray, endian and blob conversion. Use binaries to store weights.
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53776427-256C-4A4D-AABF-1067838E9BE9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405C8E9D-9159-44CD-9396-442CEE6A2BA3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="231">
   <si>
     <t>INPUT</t>
   </si>
@@ -565,27 +565,18 @@
     <t>71E3_0322</t>
   </si>
   <si>
-    <t>0006_0009</t>
-  </si>
-  <si>
     <t>3871_0324</t>
   </si>
   <si>
     <t>3838_0111</t>
   </si>
   <si>
-    <t>0001_0001</t>
-  </si>
-  <si>
     <t>023B_0000</t>
   </si>
   <si>
     <t>3838_0312</t>
   </si>
   <si>
-    <t>0003_0009</t>
-  </si>
-  <si>
     <t>001D732B</t>
   </si>
   <si>
@@ -712,9 +703,6 @@
     <t>010E_0E15</t>
   </si>
   <si>
-    <t>000E_00C4</t>
-  </si>
-  <si>
     <t>003F0E7B</t>
   </si>
   <si>
@@ -725,6 +713,21 @@
   </si>
   <si>
     <t>stride2|ksize|result_mask</t>
+  </si>
+  <si>
+    <t>0006_0901</t>
+  </si>
+  <si>
+    <t>0001_0103</t>
+  </si>
+  <si>
+    <t>0001_0101</t>
+  </si>
+  <si>
+    <t>0003_0901</t>
+  </si>
+  <si>
+    <t>000E_C401</t>
   </si>
 </sst>
 </file>
@@ -1310,8 +1313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80B23C6-EAEB-43B1-B045-456C36085CFA}">
   <dimension ref="A1:AL71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J39" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S69" sqref="S69"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1456,7 +1459,7 @@
         <v>151</v>
       </c>
       <c r="S2" s="14" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="T2" s="38" t="s">
         <v>82</v>
@@ -1467,11 +1470,11 @@
       </c>
       <c r="W2" s="38"/>
       <c r="X2" s="38" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="Y2" s="38"/>
       <c r="Z2" s="38" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="AA2" s="38"/>
       <c r="AB2" s="28" t="s">
@@ -1531,8 +1534,8 @@
         <v>101</v>
       </c>
       <c r="L3" s="1">
-        <f>J3^2*F3</f>
-        <v>154587</v>
+        <f>J3^2*8</f>
+        <v>412232</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -1603,8 +1606,8 @@
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2">
-        <f>D4^2*E4*F4</f>
-        <v>1728</v>
+        <f>D4^2*8*F4</f>
+        <v>4608</v>
       </c>
       <c r="O4" s="2">
         <f>F4</f>
@@ -1612,7 +1615,7 @@
       </c>
       <c r="P4" s="2">
         <f>N4+O4</f>
-        <v>1792</v>
+        <v>4672</v>
       </c>
       <c r="Q4" s="6" t="str">
         <f>DEC2HEX(J4,2)&amp;DEC2HEX(G4,2)&amp;"_"&amp;DEC2HEX(D4,2)&amp;DEC2HEX(H4,1)&amp;DEC2HEX(C4,1)</f>
@@ -1634,20 +1637,20 @@
         <v>00001000</v>
       </c>
       <c r="V4" s="20">
-        <f>640*1024</f>
-        <v>655360</v>
+        <f>2048*1024</f>
+        <v>2097152</v>
       </c>
       <c r="W4" s="2" t="str">
         <f>DEC2HEX(V4,8)</f>
-        <v>000A0000</v>
+        <v>00200000</v>
       </c>
       <c r="X4" s="20">
         <f>V4+L3</f>
-        <v>809947</v>
+        <v>2509384</v>
       </c>
       <c r="Y4" s="2" t="str">
         <f>DEC2HEX(X4,8)</f>
-        <v>000C5BDB</v>
+        <v>00264A48</v>
       </c>
       <c r="Z4" s="20"/>
       <c r="AA4" s="2" t="str">
@@ -1801,19 +1804,19 @@
       </c>
       <c r="V6" s="22">
         <f>X4</f>
-        <v>809947</v>
+        <v>2509384</v>
       </c>
       <c r="W6" s="4" t="str">
         <f>DEC2HEX(V6,8)</f>
-        <v>000C5BDB</v>
+        <v>00264A48</v>
       </c>
       <c r="X6" s="22">
         <f>V6+L4</f>
-        <v>1627163</v>
+        <v>3326600</v>
       </c>
       <c r="Y6" s="4" t="str">
         <f>DEC2HEX(X6,8)</f>
-        <v>0018D41B</v>
+        <v>0032C288</v>
       </c>
       <c r="Z6" s="22"/>
       <c r="AA6" s="4" t="str">
@@ -1930,35 +1933,35 @@
       </c>
       <c r="T7" s="20">
         <f>T4+P4</f>
-        <v>5888</v>
+        <v>8768</v>
       </c>
       <c r="U7" s="2" t="str">
         <f>DEC2HEX(T7,8)</f>
-        <v>00001700</v>
+        <v>00002240</v>
       </c>
       <c r="V7" s="20">
         <f>X6</f>
-        <v>1627163</v>
+        <v>3326600</v>
       </c>
       <c r="W7" s="2" t="str">
         <f>DEC2HEX(V7,8)</f>
-        <v>0018D41B</v>
+        <v>0032C288</v>
       </c>
       <c r="X7" s="20">
         <f>V7+L6</f>
-        <v>1827867</v>
+        <v>3527304</v>
       </c>
       <c r="Y7" s="2" t="str">
         <f>DEC2HEX(X7,8)</f>
-        <v>001BE41B</v>
+        <v>0035D288</v>
       </c>
       <c r="Z7" s="20">
         <f>X7+L7</f>
-        <v>1878043</v>
+        <v>3577480</v>
       </c>
       <c r="AA7" s="2" t="str">
         <f>DEC2HEX(Z7,8)</f>
-        <v>001CA81B</v>
+        <v>00369688</v>
       </c>
       <c r="AB7" s="11" t="str">
         <f>DEC2HEX(I10*2,2)&amp;DEC2HEX(I10*(G10+3),2)&amp;"_"&amp;DEC2HEX(I9*2,2)&amp;DEC2HEX(I9*(G9+3),2)</f>
@@ -2112,27 +2115,27 @@
       </c>
       <c r="T9" s="20">
         <f>T7+P7</f>
-        <v>6928</v>
+        <v>9808</v>
       </c>
       <c r="U9" s="2" t="str">
         <f t="shared" ref="U9:U10" si="3">DEC2HEX(T9,8)</f>
-        <v>00001B10</v>
+        <v>00002650</v>
       </c>
       <c r="V9" s="20">
         <f>X7</f>
-        <v>1827867</v>
+        <v>3527304</v>
       </c>
       <c r="W9" s="2" t="str">
         <f t="shared" ref="W9:W10" si="4">DEC2HEX(V9,8)</f>
-        <v>001BE41B</v>
+        <v>0035D288</v>
       </c>
       <c r="X9" s="20">
         <f>Z7+M7</f>
-        <v>1930027</v>
+        <v>3629464</v>
       </c>
       <c r="Y9" s="2" t="str">
         <f>DEC2HEX(X9,8)</f>
-        <v>001D732B</v>
+        <v>00376198</v>
       </c>
       <c r="Z9" s="20"/>
       <c r="AA9" s="2" t="str">
@@ -2246,27 +2249,27 @@
       </c>
       <c r="T10" s="20">
         <f>T9+P9</f>
-        <v>8016</v>
+        <v>10896</v>
       </c>
       <c r="U10" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>00001F50</v>
+        <v>00002A90</v>
       </c>
       <c r="V10" s="20">
         <f>Z7</f>
-        <v>1878043</v>
+        <v>3577480</v>
       </c>
       <c r="W10" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>001CA81B</v>
+        <v>00369688</v>
       </c>
       <c r="X10" s="20">
         <f>X9+L9</f>
-        <v>2130731</v>
+        <v>3830168</v>
       </c>
       <c r="Y10" s="2" t="str">
         <f>DEC2HEX(X10,8)</f>
-        <v>0020832B</v>
+        <v>003A7198</v>
       </c>
       <c r="Z10" s="20"/>
       <c r="AA10" s="2" t="str">
@@ -2521,35 +2524,35 @@
       </c>
       <c r="T14" s="20">
         <f>T10+P10</f>
-        <v>17296</v>
+        <v>20176</v>
       </c>
       <c r="U14" s="2" t="str">
         <f>DEC2HEX(T14,8)</f>
-        <v>00004390</v>
+        <v>00004ED0</v>
       </c>
       <c r="V14" s="20">
         <f>X9</f>
-        <v>1930027</v>
+        <v>3629464</v>
       </c>
       <c r="W14" s="2" t="str">
         <f>DEC2HEX(V14,8)</f>
-        <v>001D732B</v>
+        <v>00376198</v>
       </c>
       <c r="X14" s="20">
         <f>X10+L10</f>
-        <v>2331435</v>
+        <v>4030872</v>
       </c>
       <c r="Y14" s="2" t="str">
         <f>DEC2HEX(X14,8)</f>
-        <v>0023932B</v>
+        <v>003D8198</v>
       </c>
       <c r="Z14" s="20">
         <f>X14+L14</f>
-        <v>2381611</v>
+        <v>4081048</v>
       </c>
       <c r="AA14" s="2" t="str">
         <f>DEC2HEX(Z14,8)</f>
-        <v>0024572B</v>
+        <v>003E4598</v>
       </c>
       <c r="AB14" s="11" t="str">
         <f>DEC2HEX(I17*2,2)&amp;DEC2HEX(I17*(G17+3),2)&amp;"_"&amp;DEC2HEX(I16*2,2)&amp;DEC2HEX(I16*(G16+3),2)</f>
@@ -2703,27 +2706,27 @@
       </c>
       <c r="T16" s="20">
         <f>T14+P14</f>
-        <v>19360</v>
+        <v>22240</v>
       </c>
       <c r="U16" s="2" t="str">
         <f t="shared" ref="U16:U17" si="9">DEC2HEX(T16,8)</f>
-        <v>00004BA0</v>
+        <v>000056E0</v>
       </c>
       <c r="V16" s="20">
         <f>X14</f>
-        <v>2331435</v>
+        <v>4030872</v>
       </c>
       <c r="W16" s="2" t="str">
         <f t="shared" ref="W16:W17" si="10">DEC2HEX(V16,8)</f>
-        <v>0023932B</v>
+        <v>003D8198</v>
       </c>
       <c r="X16" s="20">
         <f>Z14+M14</f>
-        <v>2433595</v>
+        <v>4133032</v>
       </c>
       <c r="Y16" s="2" t="str">
         <f>DEC2HEX(X16,8)</f>
-        <v>0025223B</v>
+        <v>003F10A8</v>
       </c>
       <c r="Z16" s="20"/>
       <c r="AA16" s="2" t="str">
@@ -2837,27 +2840,27 @@
       </c>
       <c r="T17" s="20">
         <f>T16+P16</f>
-        <v>20448</v>
+        <v>23328</v>
       </c>
       <c r="U17" s="2" t="str">
         <f t="shared" si="9"/>
-        <v>00004FE0</v>
+        <v>00005B20</v>
       </c>
       <c r="V17" s="20">
         <f>Z14</f>
-        <v>2381611</v>
+        <v>4081048</v>
       </c>
       <c r="W17" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>0024572B</v>
+        <v>003E4598</v>
       </c>
       <c r="X17" s="20">
         <f>X16+L16</f>
-        <v>2634299</v>
+        <v>4333736</v>
       </c>
       <c r="Y17" s="2" t="str">
         <f>DEC2HEX(X17,8)</f>
-        <v>0028323B</v>
+        <v>004220A8</v>
       </c>
       <c r="Z17" s="20"/>
       <c r="AA17" s="2" t="str">
@@ -3105,19 +3108,19 @@
       </c>
       <c r="V21" s="22">
         <f>X16</f>
-        <v>2433595</v>
+        <v>4133032</v>
       </c>
       <c r="W21" s="4" t="str">
         <f>DEC2HEX(V21,8)</f>
-        <v>0025223B</v>
+        <v>003F10A8</v>
       </c>
       <c r="X21" s="22">
         <f>X17+L17</f>
-        <v>2835003</v>
+        <v>4534440</v>
       </c>
       <c r="Y21" s="4" t="str">
         <f>DEC2HEX(X21,8)</f>
-        <v>002B423B</v>
+        <v>004530A8</v>
       </c>
       <c r="Z21" s="22"/>
       <c r="AA21" s="4" t="str">
@@ -3234,35 +3237,35 @@
       </c>
       <c r="T22" s="20">
         <f>T17+P17</f>
-        <v>29728</v>
+        <v>32608</v>
       </c>
       <c r="U22" s="2" t="str">
         <f>DEC2HEX(T22,8)</f>
-        <v>00007420</v>
+        <v>00007F60</v>
       </c>
       <c r="V22" s="20">
         <f>X21</f>
-        <v>2835003</v>
+        <v>4534440</v>
       </c>
       <c r="W22" s="2" t="str">
         <f>DEC2HEX(V22,8)</f>
-        <v>002B423B</v>
+        <v>004530A8</v>
       </c>
       <c r="X22" s="20">
         <f>X21+L21</f>
-        <v>2935355</v>
+        <v>4634792</v>
       </c>
       <c r="Y22" s="2" t="str">
         <f>DEC2HEX(X22,8)</f>
-        <v>002CCA3B</v>
+        <v>0046B8A8</v>
       </c>
       <c r="Z22" s="20">
         <f>X22+L22</f>
-        <v>2960443</v>
+        <v>4659880</v>
       </c>
       <c r="AA22" s="2" t="str">
         <f>DEC2HEX(Z22,8)</f>
-        <v>002D2C3B</v>
+        <v>00471AA8</v>
       </c>
       <c r="AB22" s="11" t="str">
         <f>DEC2HEX(I25*2,2)&amp;DEC2HEX(I25*(G25+3),2)&amp;"_"&amp;DEC2HEX(I24*2,2)&amp;DEC2HEX(I24*(G24+3),2)</f>
@@ -3416,27 +3419,27 @@
       </c>
       <c r="T24" s="20">
         <f>T22+P22</f>
-        <v>33856</v>
+        <v>36736</v>
       </c>
       <c r="U24" s="2" t="str">
         <f t="shared" ref="U24:U25" si="16">DEC2HEX(T24,8)</f>
-        <v>00008440</v>
+        <v>00008F80</v>
       </c>
       <c r="V24" s="20">
         <f>X22</f>
-        <v>2935355</v>
+        <v>4634792</v>
       </c>
       <c r="W24" s="2" t="str">
         <f t="shared" ref="W24:W25" si="17">DEC2HEX(V24,8)</f>
-        <v>002CCA3B</v>
+        <v>0046B8A8</v>
       </c>
       <c r="X24" s="20">
         <f>Z22+M22</f>
-        <v>2987355</v>
+        <v>4686792</v>
       </c>
       <c r="Y24" s="2" t="str">
         <f>DEC2HEX(X24,8)</f>
-        <v>002D955B</v>
+        <v>004783C8</v>
       </c>
       <c r="Z24" s="20"/>
       <c r="AA24" s="2" t="str">
@@ -3550,27 +3553,27 @@
       </c>
       <c r="T25" s="20">
         <f>T24+P24</f>
-        <v>38080</v>
+        <v>40960</v>
       </c>
       <c r="U25" s="2" t="str">
         <f t="shared" si="16"/>
-        <v>000094C0</v>
+        <v>0000A000</v>
       </c>
       <c r="V25" s="20">
         <f>Z22</f>
-        <v>2960443</v>
+        <v>4659880</v>
       </c>
       <c r="W25" s="2" t="str">
         <f t="shared" si="17"/>
-        <v>002D2C3B</v>
+        <v>00471AA8</v>
       </c>
       <c r="X25" s="20">
         <f>X24+L24</f>
-        <v>3087707</v>
+        <v>4787144</v>
       </c>
       <c r="Y25" s="2" t="str">
         <f>DEC2HEX(X25,8)</f>
-        <v>002F1D5B</v>
+        <v>00490BC8</v>
       </c>
       <c r="Z25" s="20"/>
       <c r="AA25" s="2" t="str">
@@ -3825,35 +3828,35 @@
       </c>
       <c r="T29" s="20">
         <f>T25+P25</f>
-        <v>75072</v>
+        <v>77952</v>
       </c>
       <c r="U29" s="2" t="str">
         <f>DEC2HEX(T29,8)</f>
-        <v>00012540</v>
+        <v>00013080</v>
       </c>
       <c r="V29" s="20">
         <f>X24</f>
-        <v>2987355</v>
+        <v>4686792</v>
       </c>
       <c r="W29" s="2" t="str">
         <f>DEC2HEX(V29,8)</f>
-        <v>002D955B</v>
+        <v>004783C8</v>
       </c>
       <c r="X29" s="20">
         <f>X25+L25</f>
-        <v>3188059</v>
+        <v>4887496</v>
       </c>
       <c r="Y29" s="2" t="str">
         <f>DEC2HEX(X29,8)</f>
-        <v>0030A55B</v>
+        <v>004A93C8</v>
       </c>
       <c r="Z29" s="20">
         <f>X29+L29</f>
-        <v>3213147</v>
+        <v>4912584</v>
       </c>
       <c r="AA29" s="2" t="str">
         <f>DEC2HEX(Z29,8)</f>
-        <v>0031075B</v>
+        <v>004AF5C8</v>
       </c>
       <c r="AB29" s="11" t="str">
         <f>DEC2HEX(I32*2,2)&amp;DEC2HEX(I32*(G32+3),2)&amp;"_"&amp;DEC2HEX(I31*2,2)&amp;DEC2HEX(I31*(G31+3),2)</f>
@@ -4007,27 +4010,27 @@
       </c>
       <c r="T31" s="20">
         <f>T29+P29</f>
-        <v>83296</v>
+        <v>86176</v>
       </c>
       <c r="U31" s="2" t="str">
         <f t="shared" ref="U31:U32" si="22">DEC2HEX(T31,8)</f>
-        <v>00014560</v>
+        <v>000150A0</v>
       </c>
       <c r="V31" s="20">
         <f>X29</f>
-        <v>3188059</v>
+        <v>4887496</v>
       </c>
       <c r="W31" s="2" t="str">
         <f t="shared" ref="W31:W32" si="23">DEC2HEX(V31,8)</f>
-        <v>0030A55B</v>
+        <v>004A93C8</v>
       </c>
       <c r="X31" s="20">
         <f>Z29+M29</f>
-        <v>3240059</v>
+        <v>4939496</v>
       </c>
       <c r="Y31" s="2" t="str">
         <f>DEC2HEX(X31,8)</f>
-        <v>0031707B</v>
+        <v>004B5EE8</v>
       </c>
       <c r="Z31" s="20"/>
       <c r="AA31" s="2" t="str">
@@ -4141,27 +4144,27 @@
       </c>
       <c r="T32" s="20">
         <f>T31+P31</f>
-        <v>87520</v>
+        <v>90400</v>
       </c>
       <c r="U32" s="2" t="str">
         <f t="shared" si="22"/>
-        <v>000155E0</v>
+        <v>00016120</v>
       </c>
       <c r="V32" s="20">
         <f>Z29</f>
-        <v>3213147</v>
+        <v>4912584</v>
       </c>
       <c r="W32" s="2" t="str">
         <f t="shared" si="23"/>
-        <v>0031075B</v>
+        <v>004AF5C8</v>
       </c>
       <c r="X32" s="20">
         <f>X31+L31</f>
-        <v>3340411</v>
+        <v>5039848</v>
       </c>
       <c r="Y32" s="2" t="str">
         <f>DEC2HEX(X32,8)</f>
-        <v>0032F87B</v>
+        <v>004CE6E8</v>
       </c>
       <c r="Z32" s="20"/>
       <c r="AA32" s="2" t="str">
@@ -4409,19 +4412,19 @@
       </c>
       <c r="V36" s="22">
         <f>X31</f>
-        <v>3240059</v>
+        <v>4939496</v>
       </c>
       <c r="W36" s="4" t="str">
         <f>DEC2HEX(V36,8)</f>
-        <v>0031707B</v>
+        <v>004B5EE8</v>
       </c>
       <c r="X36" s="22">
         <f>X32+L32</f>
-        <v>3440763</v>
+        <v>5140200</v>
       </c>
       <c r="Y36" s="4" t="str">
         <f>DEC2HEX(X36,8)</f>
-        <v>0034807B</v>
+        <v>004E6EE8</v>
       </c>
       <c r="Z36" s="22"/>
       <c r="AA36" s="4" t="str">
@@ -4538,35 +4541,35 @@
       </c>
       <c r="T37" s="20">
         <f>T32+P32</f>
-        <v>124512</v>
+        <v>127392</v>
       </c>
       <c r="U37" s="2" t="str">
         <f>DEC2HEX(T37,8)</f>
-        <v>0001E660</v>
+        <v>0001F1A0</v>
       </c>
       <c r="V37" s="20">
         <f>X36</f>
-        <v>3440763</v>
+        <v>5140200</v>
       </c>
       <c r="W37" s="2" t="str">
         <f>DEC2HEX(V37,8)</f>
-        <v>0034807B</v>
+        <v>004E6EE8</v>
       </c>
       <c r="X37" s="20">
         <f>X36+L36</f>
-        <v>3490939</v>
+        <v>5190376</v>
       </c>
       <c r="Y37" s="2" t="str">
         <f>DEC2HEX(X37,8)</f>
-        <v>0035447B</v>
+        <v>004F32E8</v>
       </c>
       <c r="Z37" s="20">
         <f>X37+L37</f>
-        <v>3500347</v>
+        <v>5199784</v>
       </c>
       <c r="AA37" s="2" t="str">
         <f>DEC2HEX(Z37,8)</f>
-        <v>0035693B</v>
+        <v>004F57A8</v>
       </c>
       <c r="AB37" s="11" t="str">
         <f>DEC2HEX(I40*2,2)&amp;DEC2HEX(I40*(G40+3),2)&amp;"_"&amp;DEC2HEX(I39*2,2)&amp;DEC2HEX(I39*(G39+3),2)</f>
@@ -4720,27 +4723,27 @@
       </c>
       <c r="T39" s="20">
         <f>T37+P37</f>
-        <v>136848</v>
+        <v>139728</v>
       </c>
       <c r="U39" s="2" t="str">
         <f t="shared" ref="U39:U40" si="29">DEC2HEX(T39,8)</f>
-        <v>00021690</v>
+        <v>000221D0</v>
       </c>
       <c r="V39" s="20">
         <f>X37</f>
-        <v>3490939</v>
+        <v>5190376</v>
       </c>
       <c r="W39" s="2" t="str">
         <f t="shared" ref="W39:W40" si="30">DEC2HEX(V39,8)</f>
-        <v>0035447B</v>
+        <v>004F32E8</v>
       </c>
       <c r="X39" s="20">
         <f>Z37+M37</f>
-        <v>3511147</v>
+        <v>5210584</v>
       </c>
       <c r="Y39" s="2" t="str">
         <f>DEC2HEX(X39,8)</f>
-        <v>0035936B</v>
+        <v>004F81D8</v>
       </c>
       <c r="Z39" s="20"/>
       <c r="AA39" s="2" t="str">
@@ -4854,27 +4857,27 @@
       </c>
       <c r="T40" s="20">
         <f>T39+P39</f>
-        <v>146256</v>
+        <v>149136</v>
       </c>
       <c r="U40" s="2" t="str">
         <f t="shared" si="29"/>
-        <v>00023B50</v>
+        <v>00024690</v>
       </c>
       <c r="V40" s="20">
         <f>Z37</f>
-        <v>3500347</v>
+        <v>5199784</v>
       </c>
       <c r="W40" s="2" t="str">
         <f t="shared" si="30"/>
-        <v>0035693B</v>
+        <v>004F57A8</v>
       </c>
       <c r="X40" s="20">
         <f>X39+L39</f>
-        <v>3548779</v>
+        <v>5248216</v>
       </c>
       <c r="Y40" s="2" t="str">
         <f>DEC2HEX(X40,8)</f>
-        <v>0036266B</v>
+        <v>005014D8</v>
       </c>
       <c r="Z40" s="20"/>
       <c r="AA40" s="2" t="str">
@@ -5129,35 +5132,35 @@
       </c>
       <c r="T44" s="20">
         <f>T40+P40</f>
-        <v>229392</v>
+        <v>232272</v>
       </c>
       <c r="U44" s="2" t="str">
         <f>DEC2HEX(T44,8)</f>
-        <v>00038010</v>
+        <v>00038B50</v>
       </c>
       <c r="V44" s="20">
         <f>X39</f>
-        <v>3511147</v>
+        <v>5210584</v>
       </c>
       <c r="W44" s="2" t="str">
         <f>DEC2HEX(V44,8)</f>
-        <v>0035936B</v>
+        <v>004F81D8</v>
       </c>
       <c r="X44" s="20">
         <f>X40+L40</f>
-        <v>3586411</v>
+        <v>5285848</v>
       </c>
       <c r="Y44" s="2" t="str">
         <f>DEC2HEX(X44,8)</f>
-        <v>0036B96B</v>
+        <v>0050A7D8</v>
       </c>
       <c r="Z44" s="20">
         <f>X44+L44</f>
-        <v>3595819</v>
+        <v>5295256</v>
       </c>
       <c r="AA44" s="2" t="str">
         <f>DEC2HEX(Z44,8)</f>
-        <v>0036DE2B</v>
+        <v>0050CC98</v>
       </c>
       <c r="AB44" s="11" t="str">
         <f>DEC2HEX(I47*2,2)&amp;DEC2HEX(I47*(G47+3),2)&amp;"_"&amp;DEC2HEX(I46*2,2)&amp;DEC2HEX(I46*(G46+3),2)</f>
@@ -5311,27 +5314,27 @@
       </c>
       <c r="T46" s="20">
         <f>T44+P44</f>
-        <v>247872</v>
+        <v>250752</v>
       </c>
       <c r="U46" s="2" t="str">
         <f t="shared" ref="U46:U47" si="35">DEC2HEX(T46,8)</f>
-        <v>0003C840</v>
+        <v>0003D380</v>
       </c>
       <c r="V46" s="20">
         <f>X44</f>
-        <v>3586411</v>
+        <v>5285848</v>
       </c>
       <c r="W46" s="2" t="str">
         <f t="shared" ref="W46:W47" si="36">DEC2HEX(V46,8)</f>
-        <v>0036B96B</v>
+        <v>0050A7D8</v>
       </c>
       <c r="X46" s="20">
         <f>Z44+M44</f>
-        <v>3606619</v>
+        <v>5306056</v>
       </c>
       <c r="Y46" s="2" t="str">
         <f>DEC2HEX(X46,8)</f>
-        <v>0037085B</v>
+        <v>0050F6C8</v>
       </c>
       <c r="Z46" s="20"/>
       <c r="AA46" s="2" t="str">
@@ -5445,27 +5448,27 @@
       </c>
       <c r="T47" s="20">
         <f>T46+P46</f>
-        <v>257280</v>
+        <v>260160</v>
       </c>
       <c r="U47" s="2" t="str">
         <f t="shared" si="35"/>
-        <v>0003ED00</v>
+        <v>0003F840</v>
       </c>
       <c r="V47" s="20">
         <f>Z44</f>
-        <v>3595819</v>
+        <v>5295256</v>
       </c>
       <c r="W47" s="2" t="str">
         <f t="shared" si="36"/>
-        <v>0036DE2B</v>
+        <v>0050CC98</v>
       </c>
       <c r="X47" s="20">
         <f>X46+L46</f>
-        <v>3644251</v>
+        <v>5343688</v>
       </c>
       <c r="Y47" s="2" t="str">
         <f>DEC2HEX(X47,8)</f>
-        <v>00379B5B</v>
+        <v>005189C8</v>
       </c>
       <c r="Z47" s="20"/>
       <c r="AA47" s="2" t="str">
@@ -5720,35 +5723,35 @@
       </c>
       <c r="T51" s="20">
         <f>T47+P47</f>
-        <v>340416</v>
+        <v>343296</v>
       </c>
       <c r="U51" s="2" t="str">
         <f>DEC2HEX(T51,8)</f>
-        <v>000531C0</v>
+        <v>00053D00</v>
       </c>
       <c r="V51" s="20">
         <f>X46</f>
-        <v>3606619</v>
+        <v>5306056</v>
       </c>
       <c r="W51" s="2" t="str">
         <f>DEC2HEX(V51,8)</f>
-        <v>0037085B</v>
+        <v>0050F6C8</v>
       </c>
       <c r="X51" s="20">
         <f>X47+L47</f>
-        <v>3681883</v>
+        <v>5381320</v>
       </c>
       <c r="Y51" s="2" t="str">
         <f>DEC2HEX(X51,8)</f>
-        <v>00382E5B</v>
+        <v>00521CC8</v>
       </c>
       <c r="Z51" s="20">
         <f>X51+L51</f>
-        <v>3694427</v>
+        <v>5393864</v>
       </c>
       <c r="AA51" s="2" t="str">
         <f>DEC2HEX(Z51,8)</f>
-        <v>00385F5B</v>
+        <v>00524DC8</v>
       </c>
       <c r="AB51" s="11" t="str">
         <f>DEC2HEX(I54*2,2)&amp;DEC2HEX(I54*(G54+3),2)&amp;"_"&amp;DEC2HEX(I53*2,2)&amp;DEC2HEX(I53*(G53+3),2)</f>
@@ -5902,27 +5905,27 @@
       </c>
       <c r="T53" s="20">
         <f>T51+P51</f>
-        <v>365056</v>
+        <v>367936</v>
       </c>
       <c r="U53" s="2" t="str">
         <f t="shared" ref="U53:U54" si="41">DEC2HEX(T53,8)</f>
-        <v>00059200</v>
+        <v>00059D40</v>
       </c>
       <c r="V53" s="20">
         <f>X51</f>
-        <v>3681883</v>
+        <v>5381320</v>
       </c>
       <c r="W53" s="2" t="str">
         <f t="shared" ref="W53:W54" si="42">DEC2HEX(V53,8)</f>
-        <v>00382E5B</v>
+        <v>00521CC8</v>
       </c>
       <c r="X53" s="20">
         <f>Z51+M51</f>
-        <v>3708827</v>
+        <v>5408264</v>
       </c>
       <c r="Y53" s="2" t="str">
         <f>DEC2HEX(X53,8)</f>
-        <v>0038979B</v>
+        <v>00528608</v>
       </c>
       <c r="Z53" s="20"/>
       <c r="AA53" s="2" t="str">
@@ -6036,27 +6039,27 @@
       </c>
       <c r="T54" s="20">
         <f>T53+P53</f>
-        <v>381696</v>
+        <v>384576</v>
       </c>
       <c r="U54" s="2" t="str">
         <f t="shared" si="41"/>
-        <v>0005D300</v>
+        <v>0005DE40</v>
       </c>
       <c r="V54" s="20">
         <f>Z51</f>
-        <v>3694427</v>
+        <v>5393864</v>
       </c>
       <c r="W54" s="2" t="str">
         <f t="shared" si="42"/>
-        <v>00385F5B</v>
+        <v>00524DC8</v>
       </c>
       <c r="X54" s="20">
         <f>X53+L53</f>
-        <v>3759003</v>
+        <v>5458440</v>
       </c>
       <c r="Y54" s="2" t="str">
         <f>DEC2HEX(X54,8)</f>
-        <v>00395B9B</v>
+        <v>00534A08</v>
       </c>
       <c r="Z54" s="20"/>
       <c r="AA54" s="2" t="str">
@@ -6311,35 +6314,35 @@
       </c>
       <c r="T58" s="20">
         <f>T54+P54</f>
-        <v>529408</v>
+        <v>532288</v>
       </c>
       <c r="U58" s="2" t="str">
         <f>DEC2HEX(T58,8)</f>
-        <v>00081400</v>
+        <v>00081F40</v>
       </c>
       <c r="V58" s="20">
         <f>X54</f>
-        <v>3759003</v>
+        <v>5458440</v>
       </c>
       <c r="W58" s="2" t="str">
         <f>DEC2HEX(V58,8)</f>
-        <v>00395B9B</v>
+        <v>00534A08</v>
       </c>
       <c r="X58" s="20">
         <f>X54+L54</f>
-        <v>3809179</v>
+        <v>5508616</v>
       </c>
       <c r="Y58" s="2" t="str">
         <f>DEC2HEX(X58,8)</f>
-        <v>003A1F9B</v>
+        <v>00540E08</v>
       </c>
       <c r="Z58" s="20">
         <f>X58+L58</f>
-        <v>3821723</v>
+        <v>5521160</v>
       </c>
       <c r="AA58" s="2" t="str">
         <f>DEC2HEX(Z58,8)</f>
-        <v>003A509B</v>
+        <v>00543F08</v>
       </c>
       <c r="AB58" s="11" t="str">
         <f>DEC2HEX(I61*2,2)&amp;DEC2HEX(I61*(G61+3),2)&amp;"_"&amp;DEC2HEX(I60*2,2)&amp;DEC2HEX(I60*(G60+3),2)</f>
@@ -6493,27 +6496,27 @@
       </c>
       <c r="T60" s="20">
         <f>T58+P58</f>
-        <v>562240</v>
+        <v>565120</v>
       </c>
       <c r="U60" s="2" t="str">
         <f t="shared" ref="U60:U61" si="47">DEC2HEX(T60,8)</f>
-        <v>00089440</v>
+        <v>00089F80</v>
       </c>
       <c r="V60" s="20">
         <f>X58</f>
-        <v>3809179</v>
+        <v>5508616</v>
       </c>
       <c r="W60" s="2" t="str">
         <f t="shared" ref="W60:W61" si="48">DEC2HEX(V60,8)</f>
-        <v>003A1F9B</v>
+        <v>00540E08</v>
       </c>
       <c r="X60" s="20">
         <f>Z58+M58</f>
-        <v>3836123</v>
+        <v>5535560</v>
       </c>
       <c r="Y60" s="2" t="str">
         <f>DEC2HEX(X60,8)</f>
-        <v>003A88DB</v>
+        <v>00547748</v>
       </c>
       <c r="Z60" s="20"/>
       <c r="AA60" s="2" t="str">
@@ -6627,27 +6630,27 @@
       </c>
       <c r="T61" s="20">
         <f>T60+P60</f>
-        <v>578880</v>
+        <v>581760</v>
       </c>
       <c r="U61" s="2" t="str">
         <f t="shared" si="47"/>
-        <v>0008D540</v>
+        <v>0008E080</v>
       </c>
       <c r="V61" s="20">
         <f>Z58</f>
-        <v>3821723</v>
+        <v>5521160</v>
       </c>
       <c r="W61" s="2" t="str">
         <f t="shared" si="48"/>
-        <v>003A509B</v>
+        <v>00543F08</v>
       </c>
       <c r="X61" s="20">
         <f>X60+L60</f>
-        <v>3886299</v>
+        <v>5585736</v>
       </c>
       <c r="Y61" s="2" t="str">
         <f>DEC2HEX(X61,8)</f>
-        <v>003B4CDB</v>
+        <v>00553B48</v>
       </c>
       <c r="Z61" s="20"/>
       <c r="AA61" s="2" t="str">
@@ -6943,27 +6946,27 @@
       </c>
       <c r="T66" s="20">
         <f>T61+P61</f>
-        <v>726592</v>
+        <v>729472</v>
       </c>
       <c r="U66" s="2" t="str">
         <f>DEC2HEX(T66,8)</f>
-        <v>000B1640</v>
+        <v>000B2180</v>
       </c>
       <c r="V66" s="20">
         <f>X60</f>
-        <v>3836123</v>
+        <v>5535560</v>
       </c>
       <c r="W66" s="2" t="str">
         <f>DEC2HEX(V66,8)</f>
-        <v>003A88DB</v>
+        <v>00547748</v>
       </c>
       <c r="X66" s="20">
         <f>X61+L61</f>
-        <v>3936475</v>
+        <v>5635912</v>
       </c>
       <c r="Y66" s="2" t="str">
         <f>DEC2HEX(X66,8)</f>
-        <v>003C10DB</v>
+        <v>0055FF48</v>
       </c>
       <c r="Z66" s="20"/>
       <c r="AA66" s="2" t="str">
@@ -7117,19 +7120,19 @@
       </c>
       <c r="V68" s="22">
         <f>X66</f>
-        <v>3936475</v>
+        <v>5635912</v>
       </c>
       <c r="W68" s="4" t="str">
         <f>DEC2HEX(V68,8)</f>
-        <v>003C10DB</v>
+        <v>0055FF48</v>
       </c>
       <c r="X68" s="22">
         <f>X66+L66</f>
-        <v>4132475</v>
+        <v>5831912</v>
       </c>
       <c r="Y68" s="4" t="str">
         <f>DEC2HEX(X68,8)</f>
-        <v>003F0E7B</v>
+        <v>0058FCE8</v>
       </c>
       <c r="Z68" s="22"/>
       <c r="AA68" s="4" t="str">
@@ -7235,12 +7238,12 @@
       <c r="K70" s="14"/>
       <c r="L70" s="14">
         <f>SUM(L3:L69)</f>
-        <v>3269923</v>
+        <v>3527568</v>
       </c>
       <c r="M70" s="14"/>
       <c r="N70" s="14">
         <f>SUM(N4:N69)</f>
-        <v>1231552</v>
+        <v>1234432</v>
       </c>
       <c r="O70" s="14">
         <f>SUM(O4:O69)</f>
@@ -7248,7 +7251,7 @@
       </c>
       <c r="P70" s="14">
         <f>SUM(P4:P69)</f>
-        <v>1235496</v>
+        <v>1238376</v>
       </c>
       <c r="Q70" s="9"/>
       <c r="R70" s="14"/>
@@ -7305,16 +7308,16 @@
       <c r="K71" s="14"/>
       <c r="L71" s="14">
         <f>L70*16/1024/8</f>
-        <v>6386.568359375</v>
+        <v>6889.78125</v>
       </c>
       <c r="M71" s="14"/>
       <c r="N71" s="14">
         <f>N70*16/1024/8</f>
-        <v>2405.375</v>
+        <v>2411</v>
       </c>
       <c r="O71" s="14">
         <f>N70+O70</f>
-        <v>1235496</v>
+        <v>1238376</v>
       </c>
       <c r="P71" s="14"/>
       <c r="Q71" s="9"/>
@@ -7366,7 +7369,7 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView zoomScale="76" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7386,7 +7389,7 @@
         <v>83</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>176</v>
+        <v>226</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>116</v>
@@ -7413,7 +7416,7 @@
       </c>
       <c r="K1" t="str">
         <f t="shared" ref="K1:K30" si="2">LEFT(SUBSTITUTE(C1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C1,"_",),4)</f>
-        <v>0006 0009</v>
+        <v>0006 0901</v>
       </c>
       <c r="L1" t="str">
         <f t="shared" ref="L1:L30" si="3">LEFT(SUBSTITUTE(D1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D1,"_",),4)</f>
@@ -7438,13 +7441,13 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>176</v>
+        <v>226</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>119</v>
@@ -7471,7 +7474,7 @@
       </c>
       <c r="K2" t="str">
         <f t="shared" si="2"/>
-        <v>0006 0009</v>
+        <v>0006 0901</v>
       </c>
       <c r="L2" t="str">
         <f t="shared" si="3"/>
@@ -7496,13 +7499,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>84</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>179</v>
+        <v>227</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>126</v>
@@ -7517,7 +7520,7 @@
         <v>121</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I3" t="str">
         <f t="shared" si="0"/>
@@ -7529,7 +7532,7 @@
       </c>
       <c r="K3" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0103</v>
       </c>
       <c r="L3" t="str">
         <f t="shared" si="3"/>
@@ -7554,13 +7557,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>179</v>
+        <v>228</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>127</v>
@@ -7569,7 +7572,7 @@
         <v>120</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>119</v>
@@ -7587,7 +7590,7 @@
       </c>
       <c r="K4" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0101</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" si="3"/>
@@ -7612,13 +7615,13 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>128</v>
@@ -7627,7 +7630,7 @@
         <v>121</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>119</v>
@@ -7645,7 +7648,7 @@
       </c>
       <c r="K5" t="str">
         <f t="shared" si="2"/>
-        <v>0003 0009</v>
+        <v>0003 0901</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" si="3"/>
@@ -7670,28 +7673,28 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>86</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>179</v>
+        <v>227</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>129</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>186</v>
-      </c>
       <c r="H6" s="11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
@@ -7703,7 +7706,7 @@
       </c>
       <c r="K6" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0103</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="3"/>
@@ -7728,22 +7731,22 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>179</v>
+        <v>228</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>130</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>119</v>
@@ -7761,7 +7764,7 @@
       </c>
       <c r="K7" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0101</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="3"/>
@@ -7786,22 +7789,22 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>131</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>119</v>
@@ -7819,7 +7822,7 @@
       </c>
       <c r="K8" t="str">
         <f t="shared" si="2"/>
-        <v>0003 0009</v>
+        <v>0003 0901</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="3"/>
@@ -7844,22 +7847,22 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>99</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>176</v>
+        <v>226</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>119</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>119</v>
@@ -7877,7 +7880,7 @@
       </c>
       <c r="K9" t="str">
         <f t="shared" si="2"/>
-        <v>0006 0009</v>
+        <v>0006 0901</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="3"/>
@@ -7902,28 +7905,28 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>179</v>
+        <v>227</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="H10" s="11" t="s">
         <v>191</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>194</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
@@ -7935,7 +7938,7 @@
       </c>
       <c r="K10" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0103</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="3"/>
@@ -7960,22 +7963,22 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>179</v>
+        <v>228</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>133</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>119</v>
@@ -7993,7 +7996,7 @@
       </c>
       <c r="K11" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0101</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="3"/>
@@ -8018,22 +8021,22 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>134</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>119</v>
@@ -8051,7 +8054,7 @@
       </c>
       <c r="K12" t="str">
         <f t="shared" si="2"/>
-        <v>0003 0009</v>
+        <v>0003 0901</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="3"/>
@@ -8076,28 +8079,28 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>179</v>
+        <v>227</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>135</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>199</v>
-      </c>
       <c r="H13" s="11" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="0"/>
@@ -8109,7 +8112,7 @@
       </c>
       <c r="K13" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0103</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="3"/>
@@ -8134,22 +8137,22 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>179</v>
+        <v>228</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>136</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>119</v>
@@ -8167,7 +8170,7 @@
       </c>
       <c r="K14" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0101</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="3"/>
@@ -8192,22 +8195,22 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>137</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>119</v>
@@ -8225,7 +8228,7 @@
       </c>
       <c r="K15" t="str">
         <f t="shared" si="2"/>
-        <v>0003 0009</v>
+        <v>0003 0901</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="3"/>
@@ -8250,22 +8253,22 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>100</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>176</v>
+        <v>226</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>119</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>119</v>
@@ -8283,7 +8286,7 @@
       </c>
       <c r="K16" t="str">
         <f t="shared" si="2"/>
-        <v>0006 0009</v>
+        <v>0006 0901</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="3"/>
@@ -8308,28 +8311,28 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>179</v>
+        <v>227</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>138</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="H17" s="11" t="s">
         <v>204</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>207</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" si="0"/>
@@ -8341,7 +8344,7 @@
       </c>
       <c r="K17" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0103</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="3"/>
@@ -8366,22 +8369,22 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>179</v>
+        <v>228</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>139</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>119</v>
@@ -8399,7 +8402,7 @@
       </c>
       <c r="K18" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0101</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="3"/>
@@ -8424,22 +8427,22 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>140</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>119</v>
@@ -8457,7 +8460,7 @@
       </c>
       <c r="K19" t="str">
         <f t="shared" si="2"/>
-        <v>0003 0009</v>
+        <v>0003 0901</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" si="3"/>
@@ -8482,28 +8485,28 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>179</v>
+        <v>227</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>212</v>
-      </c>
       <c r="H20" s="11" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="0"/>
@@ -8515,7 +8518,7 @@
       </c>
       <c r="K20" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0103</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="3"/>
@@ -8540,22 +8543,22 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>179</v>
+        <v>228</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>142</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>119</v>
@@ -8573,7 +8576,7 @@
       </c>
       <c r="K21" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0101</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" si="3"/>
@@ -8598,22 +8601,22 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>143</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>119</v>
@@ -8631,7 +8634,7 @@
       </c>
       <c r="K22" t="str">
         <f t="shared" si="2"/>
-        <v>0003 0009</v>
+        <v>0003 0901</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" si="3"/>
@@ -8656,28 +8659,28 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>179</v>
+        <v>227</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>144</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>216</v>
-      </c>
       <c r="H23" s="11" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="0"/>
@@ -8689,7 +8692,7 @@
       </c>
       <c r="K23" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0103</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" si="3"/>
@@ -8714,22 +8717,22 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>179</v>
+        <v>228</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>145</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>119</v>
@@ -8747,7 +8750,7 @@
       </c>
       <c r="K24" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0101</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" si="3"/>
@@ -8772,22 +8775,22 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>146</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>119</v>
@@ -8805,7 +8808,7 @@
       </c>
       <c r="K25" t="str">
         <f t="shared" si="2"/>
-        <v>0003 0009</v>
+        <v>0003 0901</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" si="3"/>
@@ -8830,28 +8833,28 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>94</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>179</v>
+        <v>227</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>147</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="0"/>
@@ -8863,7 +8866,7 @@
       </c>
       <c r="K26" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0103</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" si="3"/>
@@ -8888,22 +8891,22 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>179</v>
+        <v>228</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>148</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>119</v>
@@ -8921,7 +8924,7 @@
       </c>
       <c r="K27" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0101</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" si="3"/>
@@ -8946,22 +8949,22 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>149</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>119</v>
@@ -8979,7 +8982,7 @@
       </c>
       <c r="K28" t="str">
         <f t="shared" si="2"/>
-        <v>0003 0009</v>
+        <v>0003 0901</v>
       </c>
       <c r="L28" t="str">
         <f t="shared" si="3"/>
@@ -9004,22 +9007,22 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>123</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>179</v>
+        <v>228</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>150</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>119</v>
@@ -9037,7 +9040,7 @@
       </c>
       <c r="K29" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0101</v>
       </c>
       <c r="L29" t="str">
         <f t="shared" si="3"/>
@@ -9062,22 +9065,22 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>124</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>119</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>119</v>
@@ -9095,7 +9098,7 @@
       </c>
       <c r="K30" t="str">
         <f t="shared" si="2"/>
-        <v>000E 00C4</v>
+        <v>000E C401</v>
       </c>
       <c r="L30" t="str">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Fix bytearray, endian and blob conversion
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53776427-256C-4A4D-AABF-1067838E9BE9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405C8E9D-9159-44CD-9396-442CEE6A2BA3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="231">
   <si>
     <t>INPUT</t>
   </si>
@@ -565,27 +565,18 @@
     <t>71E3_0322</t>
   </si>
   <si>
-    <t>0006_0009</t>
-  </si>
-  <si>
     <t>3871_0324</t>
   </si>
   <si>
     <t>3838_0111</t>
   </si>
   <si>
-    <t>0001_0001</t>
-  </si>
-  <si>
     <t>023B_0000</t>
   </si>
   <si>
     <t>3838_0312</t>
   </si>
   <si>
-    <t>0003_0009</t>
-  </si>
-  <si>
     <t>001D732B</t>
   </si>
   <si>
@@ -712,9 +703,6 @@
     <t>010E_0E15</t>
   </si>
   <si>
-    <t>000E_00C4</t>
-  </si>
-  <si>
     <t>003F0E7B</t>
   </si>
   <si>
@@ -725,6 +713,21 @@
   </si>
   <si>
     <t>stride2|ksize|result_mask</t>
+  </si>
+  <si>
+    <t>0006_0901</t>
+  </si>
+  <si>
+    <t>0001_0103</t>
+  </si>
+  <si>
+    <t>0001_0101</t>
+  </si>
+  <si>
+    <t>0003_0901</t>
+  </si>
+  <si>
+    <t>000E_C401</t>
   </si>
 </sst>
 </file>
@@ -1310,8 +1313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80B23C6-EAEB-43B1-B045-456C36085CFA}">
   <dimension ref="A1:AL71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J39" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S69" sqref="S69"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1456,7 +1459,7 @@
         <v>151</v>
       </c>
       <c r="S2" s="14" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="T2" s="38" t="s">
         <v>82</v>
@@ -1467,11 +1470,11 @@
       </c>
       <c r="W2" s="38"/>
       <c r="X2" s="38" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="Y2" s="38"/>
       <c r="Z2" s="38" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="AA2" s="38"/>
       <c r="AB2" s="28" t="s">
@@ -1531,8 +1534,8 @@
         <v>101</v>
       </c>
       <c r="L3" s="1">
-        <f>J3^2*F3</f>
-        <v>154587</v>
+        <f>J3^2*8</f>
+        <v>412232</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -1603,8 +1606,8 @@
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2">
-        <f>D4^2*E4*F4</f>
-        <v>1728</v>
+        <f>D4^2*8*F4</f>
+        <v>4608</v>
       </c>
       <c r="O4" s="2">
         <f>F4</f>
@@ -1612,7 +1615,7 @@
       </c>
       <c r="P4" s="2">
         <f>N4+O4</f>
-        <v>1792</v>
+        <v>4672</v>
       </c>
       <c r="Q4" s="6" t="str">
         <f>DEC2HEX(J4,2)&amp;DEC2HEX(G4,2)&amp;"_"&amp;DEC2HEX(D4,2)&amp;DEC2HEX(H4,1)&amp;DEC2HEX(C4,1)</f>
@@ -1634,20 +1637,20 @@
         <v>00001000</v>
       </c>
       <c r="V4" s="20">
-        <f>640*1024</f>
-        <v>655360</v>
+        <f>2048*1024</f>
+        <v>2097152</v>
       </c>
       <c r="W4" s="2" t="str">
         <f>DEC2HEX(V4,8)</f>
-        <v>000A0000</v>
+        <v>00200000</v>
       </c>
       <c r="X4" s="20">
         <f>V4+L3</f>
-        <v>809947</v>
+        <v>2509384</v>
       </c>
       <c r="Y4" s="2" t="str">
         <f>DEC2HEX(X4,8)</f>
-        <v>000C5BDB</v>
+        <v>00264A48</v>
       </c>
       <c r="Z4" s="20"/>
       <c r="AA4" s="2" t="str">
@@ -1801,19 +1804,19 @@
       </c>
       <c r="V6" s="22">
         <f>X4</f>
-        <v>809947</v>
+        <v>2509384</v>
       </c>
       <c r="W6" s="4" t="str">
         <f>DEC2HEX(V6,8)</f>
-        <v>000C5BDB</v>
+        <v>00264A48</v>
       </c>
       <c r="X6" s="22">
         <f>V6+L4</f>
-        <v>1627163</v>
+        <v>3326600</v>
       </c>
       <c r="Y6" s="4" t="str">
         <f>DEC2HEX(X6,8)</f>
-        <v>0018D41B</v>
+        <v>0032C288</v>
       </c>
       <c r="Z6" s="22"/>
       <c r="AA6" s="4" t="str">
@@ -1930,35 +1933,35 @@
       </c>
       <c r="T7" s="20">
         <f>T4+P4</f>
-        <v>5888</v>
+        <v>8768</v>
       </c>
       <c r="U7" s="2" t="str">
         <f>DEC2HEX(T7,8)</f>
-        <v>00001700</v>
+        <v>00002240</v>
       </c>
       <c r="V7" s="20">
         <f>X6</f>
-        <v>1627163</v>
+        <v>3326600</v>
       </c>
       <c r="W7" s="2" t="str">
         <f>DEC2HEX(V7,8)</f>
-        <v>0018D41B</v>
+        <v>0032C288</v>
       </c>
       <c r="X7" s="20">
         <f>V7+L6</f>
-        <v>1827867</v>
+        <v>3527304</v>
       </c>
       <c r="Y7" s="2" t="str">
         <f>DEC2HEX(X7,8)</f>
-        <v>001BE41B</v>
+        <v>0035D288</v>
       </c>
       <c r="Z7" s="20">
         <f>X7+L7</f>
-        <v>1878043</v>
+        <v>3577480</v>
       </c>
       <c r="AA7" s="2" t="str">
         <f>DEC2HEX(Z7,8)</f>
-        <v>001CA81B</v>
+        <v>00369688</v>
       </c>
       <c r="AB7" s="11" t="str">
         <f>DEC2HEX(I10*2,2)&amp;DEC2HEX(I10*(G10+3),2)&amp;"_"&amp;DEC2HEX(I9*2,2)&amp;DEC2HEX(I9*(G9+3),2)</f>
@@ -2112,27 +2115,27 @@
       </c>
       <c r="T9" s="20">
         <f>T7+P7</f>
-        <v>6928</v>
+        <v>9808</v>
       </c>
       <c r="U9" s="2" t="str">
         <f t="shared" ref="U9:U10" si="3">DEC2HEX(T9,8)</f>
-        <v>00001B10</v>
+        <v>00002650</v>
       </c>
       <c r="V9" s="20">
         <f>X7</f>
-        <v>1827867</v>
+        <v>3527304</v>
       </c>
       <c r="W9" s="2" t="str">
         <f t="shared" ref="W9:W10" si="4">DEC2HEX(V9,8)</f>
-        <v>001BE41B</v>
+        <v>0035D288</v>
       </c>
       <c r="X9" s="20">
         <f>Z7+M7</f>
-        <v>1930027</v>
+        <v>3629464</v>
       </c>
       <c r="Y9" s="2" t="str">
         <f>DEC2HEX(X9,8)</f>
-        <v>001D732B</v>
+        <v>00376198</v>
       </c>
       <c r="Z9" s="20"/>
       <c r="AA9" s="2" t="str">
@@ -2246,27 +2249,27 @@
       </c>
       <c r="T10" s="20">
         <f>T9+P9</f>
-        <v>8016</v>
+        <v>10896</v>
       </c>
       <c r="U10" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>00001F50</v>
+        <v>00002A90</v>
       </c>
       <c r="V10" s="20">
         <f>Z7</f>
-        <v>1878043</v>
+        <v>3577480</v>
       </c>
       <c r="W10" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>001CA81B</v>
+        <v>00369688</v>
       </c>
       <c r="X10" s="20">
         <f>X9+L9</f>
-        <v>2130731</v>
+        <v>3830168</v>
       </c>
       <c r="Y10" s="2" t="str">
         <f>DEC2HEX(X10,8)</f>
-        <v>0020832B</v>
+        <v>003A7198</v>
       </c>
       <c r="Z10" s="20"/>
       <c r="AA10" s="2" t="str">
@@ -2521,35 +2524,35 @@
       </c>
       <c r="T14" s="20">
         <f>T10+P10</f>
-        <v>17296</v>
+        <v>20176</v>
       </c>
       <c r="U14" s="2" t="str">
         <f>DEC2HEX(T14,8)</f>
-        <v>00004390</v>
+        <v>00004ED0</v>
       </c>
       <c r="V14" s="20">
         <f>X9</f>
-        <v>1930027</v>
+        <v>3629464</v>
       </c>
       <c r="W14" s="2" t="str">
         <f>DEC2HEX(V14,8)</f>
-        <v>001D732B</v>
+        <v>00376198</v>
       </c>
       <c r="X14" s="20">
         <f>X10+L10</f>
-        <v>2331435</v>
+        <v>4030872</v>
       </c>
       <c r="Y14" s="2" t="str">
         <f>DEC2HEX(X14,8)</f>
-        <v>0023932B</v>
+        <v>003D8198</v>
       </c>
       <c r="Z14" s="20">
         <f>X14+L14</f>
-        <v>2381611</v>
+        <v>4081048</v>
       </c>
       <c r="AA14" s="2" t="str">
         <f>DEC2HEX(Z14,8)</f>
-        <v>0024572B</v>
+        <v>003E4598</v>
       </c>
       <c r="AB14" s="11" t="str">
         <f>DEC2HEX(I17*2,2)&amp;DEC2HEX(I17*(G17+3),2)&amp;"_"&amp;DEC2HEX(I16*2,2)&amp;DEC2HEX(I16*(G16+3),2)</f>
@@ -2703,27 +2706,27 @@
       </c>
       <c r="T16" s="20">
         <f>T14+P14</f>
-        <v>19360</v>
+        <v>22240</v>
       </c>
       <c r="U16" s="2" t="str">
         <f t="shared" ref="U16:U17" si="9">DEC2HEX(T16,8)</f>
-        <v>00004BA0</v>
+        <v>000056E0</v>
       </c>
       <c r="V16" s="20">
         <f>X14</f>
-        <v>2331435</v>
+        <v>4030872</v>
       </c>
       <c r="W16" s="2" t="str">
         <f t="shared" ref="W16:W17" si="10">DEC2HEX(V16,8)</f>
-        <v>0023932B</v>
+        <v>003D8198</v>
       </c>
       <c r="X16" s="20">
         <f>Z14+M14</f>
-        <v>2433595</v>
+        <v>4133032</v>
       </c>
       <c r="Y16" s="2" t="str">
         <f>DEC2HEX(X16,8)</f>
-        <v>0025223B</v>
+        <v>003F10A8</v>
       </c>
       <c r="Z16" s="20"/>
       <c r="AA16" s="2" t="str">
@@ -2837,27 +2840,27 @@
       </c>
       <c r="T17" s="20">
         <f>T16+P16</f>
-        <v>20448</v>
+        <v>23328</v>
       </c>
       <c r="U17" s="2" t="str">
         <f t="shared" si="9"/>
-        <v>00004FE0</v>
+        <v>00005B20</v>
       </c>
       <c r="V17" s="20">
         <f>Z14</f>
-        <v>2381611</v>
+        <v>4081048</v>
       </c>
       <c r="W17" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>0024572B</v>
+        <v>003E4598</v>
       </c>
       <c r="X17" s="20">
         <f>X16+L16</f>
-        <v>2634299</v>
+        <v>4333736</v>
       </c>
       <c r="Y17" s="2" t="str">
         <f>DEC2HEX(X17,8)</f>
-        <v>0028323B</v>
+        <v>004220A8</v>
       </c>
       <c r="Z17" s="20"/>
       <c r="AA17" s="2" t="str">
@@ -3105,19 +3108,19 @@
       </c>
       <c r="V21" s="22">
         <f>X16</f>
-        <v>2433595</v>
+        <v>4133032</v>
       </c>
       <c r="W21" s="4" t="str">
         <f>DEC2HEX(V21,8)</f>
-        <v>0025223B</v>
+        <v>003F10A8</v>
       </c>
       <c r="X21" s="22">
         <f>X17+L17</f>
-        <v>2835003</v>
+        <v>4534440</v>
       </c>
       <c r="Y21" s="4" t="str">
         <f>DEC2HEX(X21,8)</f>
-        <v>002B423B</v>
+        <v>004530A8</v>
       </c>
       <c r="Z21" s="22"/>
       <c r="AA21" s="4" t="str">
@@ -3234,35 +3237,35 @@
       </c>
       <c r="T22" s="20">
         <f>T17+P17</f>
-        <v>29728</v>
+        <v>32608</v>
       </c>
       <c r="U22" s="2" t="str">
         <f>DEC2HEX(T22,8)</f>
-        <v>00007420</v>
+        <v>00007F60</v>
       </c>
       <c r="V22" s="20">
         <f>X21</f>
-        <v>2835003</v>
+        <v>4534440</v>
       </c>
       <c r="W22" s="2" t="str">
         <f>DEC2HEX(V22,8)</f>
-        <v>002B423B</v>
+        <v>004530A8</v>
       </c>
       <c r="X22" s="20">
         <f>X21+L21</f>
-        <v>2935355</v>
+        <v>4634792</v>
       </c>
       <c r="Y22" s="2" t="str">
         <f>DEC2HEX(X22,8)</f>
-        <v>002CCA3B</v>
+        <v>0046B8A8</v>
       </c>
       <c r="Z22" s="20">
         <f>X22+L22</f>
-        <v>2960443</v>
+        <v>4659880</v>
       </c>
       <c r="AA22" s="2" t="str">
         <f>DEC2HEX(Z22,8)</f>
-        <v>002D2C3B</v>
+        <v>00471AA8</v>
       </c>
       <c r="AB22" s="11" t="str">
         <f>DEC2HEX(I25*2,2)&amp;DEC2HEX(I25*(G25+3),2)&amp;"_"&amp;DEC2HEX(I24*2,2)&amp;DEC2HEX(I24*(G24+3),2)</f>
@@ -3416,27 +3419,27 @@
       </c>
       <c r="T24" s="20">
         <f>T22+P22</f>
-        <v>33856</v>
+        <v>36736</v>
       </c>
       <c r="U24" s="2" t="str">
         <f t="shared" ref="U24:U25" si="16">DEC2HEX(T24,8)</f>
-        <v>00008440</v>
+        <v>00008F80</v>
       </c>
       <c r="V24" s="20">
         <f>X22</f>
-        <v>2935355</v>
+        <v>4634792</v>
       </c>
       <c r="W24" s="2" t="str">
         <f t="shared" ref="W24:W25" si="17">DEC2HEX(V24,8)</f>
-        <v>002CCA3B</v>
+        <v>0046B8A8</v>
       </c>
       <c r="X24" s="20">
         <f>Z22+M22</f>
-        <v>2987355</v>
+        <v>4686792</v>
       </c>
       <c r="Y24" s="2" t="str">
         <f>DEC2HEX(X24,8)</f>
-        <v>002D955B</v>
+        <v>004783C8</v>
       </c>
       <c r="Z24" s="20"/>
       <c r="AA24" s="2" t="str">
@@ -3550,27 +3553,27 @@
       </c>
       <c r="T25" s="20">
         <f>T24+P24</f>
-        <v>38080</v>
+        <v>40960</v>
       </c>
       <c r="U25" s="2" t="str">
         <f t="shared" si="16"/>
-        <v>000094C0</v>
+        <v>0000A000</v>
       </c>
       <c r="V25" s="20">
         <f>Z22</f>
-        <v>2960443</v>
+        <v>4659880</v>
       </c>
       <c r="W25" s="2" t="str">
         <f t="shared" si="17"/>
-        <v>002D2C3B</v>
+        <v>00471AA8</v>
       </c>
       <c r="X25" s="20">
         <f>X24+L24</f>
-        <v>3087707</v>
+        <v>4787144</v>
       </c>
       <c r="Y25" s="2" t="str">
         <f>DEC2HEX(X25,8)</f>
-        <v>002F1D5B</v>
+        <v>00490BC8</v>
       </c>
       <c r="Z25" s="20"/>
       <c r="AA25" s="2" t="str">
@@ -3825,35 +3828,35 @@
       </c>
       <c r="T29" s="20">
         <f>T25+P25</f>
-        <v>75072</v>
+        <v>77952</v>
       </c>
       <c r="U29" s="2" t="str">
         <f>DEC2HEX(T29,8)</f>
-        <v>00012540</v>
+        <v>00013080</v>
       </c>
       <c r="V29" s="20">
         <f>X24</f>
-        <v>2987355</v>
+        <v>4686792</v>
       </c>
       <c r="W29" s="2" t="str">
         <f>DEC2HEX(V29,8)</f>
-        <v>002D955B</v>
+        <v>004783C8</v>
       </c>
       <c r="X29" s="20">
         <f>X25+L25</f>
-        <v>3188059</v>
+        <v>4887496</v>
       </c>
       <c r="Y29" s="2" t="str">
         <f>DEC2HEX(X29,8)</f>
-        <v>0030A55B</v>
+        <v>004A93C8</v>
       </c>
       <c r="Z29" s="20">
         <f>X29+L29</f>
-        <v>3213147</v>
+        <v>4912584</v>
       </c>
       <c r="AA29" s="2" t="str">
         <f>DEC2HEX(Z29,8)</f>
-        <v>0031075B</v>
+        <v>004AF5C8</v>
       </c>
       <c r="AB29" s="11" t="str">
         <f>DEC2HEX(I32*2,2)&amp;DEC2HEX(I32*(G32+3),2)&amp;"_"&amp;DEC2HEX(I31*2,2)&amp;DEC2HEX(I31*(G31+3),2)</f>
@@ -4007,27 +4010,27 @@
       </c>
       <c r="T31" s="20">
         <f>T29+P29</f>
-        <v>83296</v>
+        <v>86176</v>
       </c>
       <c r="U31" s="2" t="str">
         <f t="shared" ref="U31:U32" si="22">DEC2HEX(T31,8)</f>
-        <v>00014560</v>
+        <v>000150A0</v>
       </c>
       <c r="V31" s="20">
         <f>X29</f>
-        <v>3188059</v>
+        <v>4887496</v>
       </c>
       <c r="W31" s="2" t="str">
         <f t="shared" ref="W31:W32" si="23">DEC2HEX(V31,8)</f>
-        <v>0030A55B</v>
+        <v>004A93C8</v>
       </c>
       <c r="X31" s="20">
         <f>Z29+M29</f>
-        <v>3240059</v>
+        <v>4939496</v>
       </c>
       <c r="Y31" s="2" t="str">
         <f>DEC2HEX(X31,8)</f>
-        <v>0031707B</v>
+        <v>004B5EE8</v>
       </c>
       <c r="Z31" s="20"/>
       <c r="AA31" s="2" t="str">
@@ -4141,27 +4144,27 @@
       </c>
       <c r="T32" s="20">
         <f>T31+P31</f>
-        <v>87520</v>
+        <v>90400</v>
       </c>
       <c r="U32" s="2" t="str">
         <f t="shared" si="22"/>
-        <v>000155E0</v>
+        <v>00016120</v>
       </c>
       <c r="V32" s="20">
         <f>Z29</f>
-        <v>3213147</v>
+        <v>4912584</v>
       </c>
       <c r="W32" s="2" t="str">
         <f t="shared" si="23"/>
-        <v>0031075B</v>
+        <v>004AF5C8</v>
       </c>
       <c r="X32" s="20">
         <f>X31+L31</f>
-        <v>3340411</v>
+        <v>5039848</v>
       </c>
       <c r="Y32" s="2" t="str">
         <f>DEC2HEX(X32,8)</f>
-        <v>0032F87B</v>
+        <v>004CE6E8</v>
       </c>
       <c r="Z32" s="20"/>
       <c r="AA32" s="2" t="str">
@@ -4409,19 +4412,19 @@
       </c>
       <c r="V36" s="22">
         <f>X31</f>
-        <v>3240059</v>
+        <v>4939496</v>
       </c>
       <c r="W36" s="4" t="str">
         <f>DEC2HEX(V36,8)</f>
-        <v>0031707B</v>
+        <v>004B5EE8</v>
       </c>
       <c r="X36" s="22">
         <f>X32+L32</f>
-        <v>3440763</v>
+        <v>5140200</v>
       </c>
       <c r="Y36" s="4" t="str">
         <f>DEC2HEX(X36,8)</f>
-        <v>0034807B</v>
+        <v>004E6EE8</v>
       </c>
       <c r="Z36" s="22"/>
       <c r="AA36" s="4" t="str">
@@ -4538,35 +4541,35 @@
       </c>
       <c r="T37" s="20">
         <f>T32+P32</f>
-        <v>124512</v>
+        <v>127392</v>
       </c>
       <c r="U37" s="2" t="str">
         <f>DEC2HEX(T37,8)</f>
-        <v>0001E660</v>
+        <v>0001F1A0</v>
       </c>
       <c r="V37" s="20">
         <f>X36</f>
-        <v>3440763</v>
+        <v>5140200</v>
       </c>
       <c r="W37" s="2" t="str">
         <f>DEC2HEX(V37,8)</f>
-        <v>0034807B</v>
+        <v>004E6EE8</v>
       </c>
       <c r="X37" s="20">
         <f>X36+L36</f>
-        <v>3490939</v>
+        <v>5190376</v>
       </c>
       <c r="Y37" s="2" t="str">
         <f>DEC2HEX(X37,8)</f>
-        <v>0035447B</v>
+        <v>004F32E8</v>
       </c>
       <c r="Z37" s="20">
         <f>X37+L37</f>
-        <v>3500347</v>
+        <v>5199784</v>
       </c>
       <c r="AA37" s="2" t="str">
         <f>DEC2HEX(Z37,8)</f>
-        <v>0035693B</v>
+        <v>004F57A8</v>
       </c>
       <c r="AB37" s="11" t="str">
         <f>DEC2HEX(I40*2,2)&amp;DEC2HEX(I40*(G40+3),2)&amp;"_"&amp;DEC2HEX(I39*2,2)&amp;DEC2HEX(I39*(G39+3),2)</f>
@@ -4720,27 +4723,27 @@
       </c>
       <c r="T39" s="20">
         <f>T37+P37</f>
-        <v>136848</v>
+        <v>139728</v>
       </c>
       <c r="U39" s="2" t="str">
         <f t="shared" ref="U39:U40" si="29">DEC2HEX(T39,8)</f>
-        <v>00021690</v>
+        <v>000221D0</v>
       </c>
       <c r="V39" s="20">
         <f>X37</f>
-        <v>3490939</v>
+        <v>5190376</v>
       </c>
       <c r="W39" s="2" t="str">
         <f t="shared" ref="W39:W40" si="30">DEC2HEX(V39,8)</f>
-        <v>0035447B</v>
+        <v>004F32E8</v>
       </c>
       <c r="X39" s="20">
         <f>Z37+M37</f>
-        <v>3511147</v>
+        <v>5210584</v>
       </c>
       <c r="Y39" s="2" t="str">
         <f>DEC2HEX(X39,8)</f>
-        <v>0035936B</v>
+        <v>004F81D8</v>
       </c>
       <c r="Z39" s="20"/>
       <c r="AA39" s="2" t="str">
@@ -4854,27 +4857,27 @@
       </c>
       <c r="T40" s="20">
         <f>T39+P39</f>
-        <v>146256</v>
+        <v>149136</v>
       </c>
       <c r="U40" s="2" t="str">
         <f t="shared" si="29"/>
-        <v>00023B50</v>
+        <v>00024690</v>
       </c>
       <c r="V40" s="20">
         <f>Z37</f>
-        <v>3500347</v>
+        <v>5199784</v>
       </c>
       <c r="W40" s="2" t="str">
         <f t="shared" si="30"/>
-        <v>0035693B</v>
+        <v>004F57A8</v>
       </c>
       <c r="X40" s="20">
         <f>X39+L39</f>
-        <v>3548779</v>
+        <v>5248216</v>
       </c>
       <c r="Y40" s="2" t="str">
         <f>DEC2HEX(X40,8)</f>
-        <v>0036266B</v>
+        <v>005014D8</v>
       </c>
       <c r="Z40" s="20"/>
       <c r="AA40" s="2" t="str">
@@ -5129,35 +5132,35 @@
       </c>
       <c r="T44" s="20">
         <f>T40+P40</f>
-        <v>229392</v>
+        <v>232272</v>
       </c>
       <c r="U44" s="2" t="str">
         <f>DEC2HEX(T44,8)</f>
-        <v>00038010</v>
+        <v>00038B50</v>
       </c>
       <c r="V44" s="20">
         <f>X39</f>
-        <v>3511147</v>
+        <v>5210584</v>
       </c>
       <c r="W44" s="2" t="str">
         <f>DEC2HEX(V44,8)</f>
-        <v>0035936B</v>
+        <v>004F81D8</v>
       </c>
       <c r="X44" s="20">
         <f>X40+L40</f>
-        <v>3586411</v>
+        <v>5285848</v>
       </c>
       <c r="Y44" s="2" t="str">
         <f>DEC2HEX(X44,8)</f>
-        <v>0036B96B</v>
+        <v>0050A7D8</v>
       </c>
       <c r="Z44" s="20">
         <f>X44+L44</f>
-        <v>3595819</v>
+        <v>5295256</v>
       </c>
       <c r="AA44" s="2" t="str">
         <f>DEC2HEX(Z44,8)</f>
-        <v>0036DE2B</v>
+        <v>0050CC98</v>
       </c>
       <c r="AB44" s="11" t="str">
         <f>DEC2HEX(I47*2,2)&amp;DEC2HEX(I47*(G47+3),2)&amp;"_"&amp;DEC2HEX(I46*2,2)&amp;DEC2HEX(I46*(G46+3),2)</f>
@@ -5311,27 +5314,27 @@
       </c>
       <c r="T46" s="20">
         <f>T44+P44</f>
-        <v>247872</v>
+        <v>250752</v>
       </c>
       <c r="U46" s="2" t="str">
         <f t="shared" ref="U46:U47" si="35">DEC2HEX(T46,8)</f>
-        <v>0003C840</v>
+        <v>0003D380</v>
       </c>
       <c r="V46" s="20">
         <f>X44</f>
-        <v>3586411</v>
+        <v>5285848</v>
       </c>
       <c r="W46" s="2" t="str">
         <f t="shared" ref="W46:W47" si="36">DEC2HEX(V46,8)</f>
-        <v>0036B96B</v>
+        <v>0050A7D8</v>
       </c>
       <c r="X46" s="20">
         <f>Z44+M44</f>
-        <v>3606619</v>
+        <v>5306056</v>
       </c>
       <c r="Y46" s="2" t="str">
         <f>DEC2HEX(X46,8)</f>
-        <v>0037085B</v>
+        <v>0050F6C8</v>
       </c>
       <c r="Z46" s="20"/>
       <c r="AA46" s="2" t="str">
@@ -5445,27 +5448,27 @@
       </c>
       <c r="T47" s="20">
         <f>T46+P46</f>
-        <v>257280</v>
+        <v>260160</v>
       </c>
       <c r="U47" s="2" t="str">
         <f t="shared" si="35"/>
-        <v>0003ED00</v>
+        <v>0003F840</v>
       </c>
       <c r="V47" s="20">
         <f>Z44</f>
-        <v>3595819</v>
+        <v>5295256</v>
       </c>
       <c r="W47" s="2" t="str">
         <f t="shared" si="36"/>
-        <v>0036DE2B</v>
+        <v>0050CC98</v>
       </c>
       <c r="X47" s="20">
         <f>X46+L46</f>
-        <v>3644251</v>
+        <v>5343688</v>
       </c>
       <c r="Y47" s="2" t="str">
         <f>DEC2HEX(X47,8)</f>
-        <v>00379B5B</v>
+        <v>005189C8</v>
       </c>
       <c r="Z47" s="20"/>
       <c r="AA47" s="2" t="str">
@@ -5720,35 +5723,35 @@
       </c>
       <c r="T51" s="20">
         <f>T47+P47</f>
-        <v>340416</v>
+        <v>343296</v>
       </c>
       <c r="U51" s="2" t="str">
         <f>DEC2HEX(T51,8)</f>
-        <v>000531C0</v>
+        <v>00053D00</v>
       </c>
       <c r="V51" s="20">
         <f>X46</f>
-        <v>3606619</v>
+        <v>5306056</v>
       </c>
       <c r="W51" s="2" t="str">
         <f>DEC2HEX(V51,8)</f>
-        <v>0037085B</v>
+        <v>0050F6C8</v>
       </c>
       <c r="X51" s="20">
         <f>X47+L47</f>
-        <v>3681883</v>
+        <v>5381320</v>
       </c>
       <c r="Y51" s="2" t="str">
         <f>DEC2HEX(X51,8)</f>
-        <v>00382E5B</v>
+        <v>00521CC8</v>
       </c>
       <c r="Z51" s="20">
         <f>X51+L51</f>
-        <v>3694427</v>
+        <v>5393864</v>
       </c>
       <c r="AA51" s="2" t="str">
         <f>DEC2HEX(Z51,8)</f>
-        <v>00385F5B</v>
+        <v>00524DC8</v>
       </c>
       <c r="AB51" s="11" t="str">
         <f>DEC2HEX(I54*2,2)&amp;DEC2HEX(I54*(G54+3),2)&amp;"_"&amp;DEC2HEX(I53*2,2)&amp;DEC2HEX(I53*(G53+3),2)</f>
@@ -5902,27 +5905,27 @@
       </c>
       <c r="T53" s="20">
         <f>T51+P51</f>
-        <v>365056</v>
+        <v>367936</v>
       </c>
       <c r="U53" s="2" t="str">
         <f t="shared" ref="U53:U54" si="41">DEC2HEX(T53,8)</f>
-        <v>00059200</v>
+        <v>00059D40</v>
       </c>
       <c r="V53" s="20">
         <f>X51</f>
-        <v>3681883</v>
+        <v>5381320</v>
       </c>
       <c r="W53" s="2" t="str">
         <f t="shared" ref="W53:W54" si="42">DEC2HEX(V53,8)</f>
-        <v>00382E5B</v>
+        <v>00521CC8</v>
       </c>
       <c r="X53" s="20">
         <f>Z51+M51</f>
-        <v>3708827</v>
+        <v>5408264</v>
       </c>
       <c r="Y53" s="2" t="str">
         <f>DEC2HEX(X53,8)</f>
-        <v>0038979B</v>
+        <v>00528608</v>
       </c>
       <c r="Z53" s="20"/>
       <c r="AA53" s="2" t="str">
@@ -6036,27 +6039,27 @@
       </c>
       <c r="T54" s="20">
         <f>T53+P53</f>
-        <v>381696</v>
+        <v>384576</v>
       </c>
       <c r="U54" s="2" t="str">
         <f t="shared" si="41"/>
-        <v>0005D300</v>
+        <v>0005DE40</v>
       </c>
       <c r="V54" s="20">
         <f>Z51</f>
-        <v>3694427</v>
+        <v>5393864</v>
       </c>
       <c r="W54" s="2" t="str">
         <f t="shared" si="42"/>
-        <v>00385F5B</v>
+        <v>00524DC8</v>
       </c>
       <c r="X54" s="20">
         <f>X53+L53</f>
-        <v>3759003</v>
+        <v>5458440</v>
       </c>
       <c r="Y54" s="2" t="str">
         <f>DEC2HEX(X54,8)</f>
-        <v>00395B9B</v>
+        <v>00534A08</v>
       </c>
       <c r="Z54" s="20"/>
       <c r="AA54" s="2" t="str">
@@ -6311,35 +6314,35 @@
       </c>
       <c r="T58" s="20">
         <f>T54+P54</f>
-        <v>529408</v>
+        <v>532288</v>
       </c>
       <c r="U58" s="2" t="str">
         <f>DEC2HEX(T58,8)</f>
-        <v>00081400</v>
+        <v>00081F40</v>
       </c>
       <c r="V58" s="20">
         <f>X54</f>
-        <v>3759003</v>
+        <v>5458440</v>
       </c>
       <c r="W58" s="2" t="str">
         <f>DEC2HEX(V58,8)</f>
-        <v>00395B9B</v>
+        <v>00534A08</v>
       </c>
       <c r="X58" s="20">
         <f>X54+L54</f>
-        <v>3809179</v>
+        <v>5508616</v>
       </c>
       <c r="Y58" s="2" t="str">
         <f>DEC2HEX(X58,8)</f>
-        <v>003A1F9B</v>
+        <v>00540E08</v>
       </c>
       <c r="Z58" s="20">
         <f>X58+L58</f>
-        <v>3821723</v>
+        <v>5521160</v>
       </c>
       <c r="AA58" s="2" t="str">
         <f>DEC2HEX(Z58,8)</f>
-        <v>003A509B</v>
+        <v>00543F08</v>
       </c>
       <c r="AB58" s="11" t="str">
         <f>DEC2HEX(I61*2,2)&amp;DEC2HEX(I61*(G61+3),2)&amp;"_"&amp;DEC2HEX(I60*2,2)&amp;DEC2HEX(I60*(G60+3),2)</f>
@@ -6493,27 +6496,27 @@
       </c>
       <c r="T60" s="20">
         <f>T58+P58</f>
-        <v>562240</v>
+        <v>565120</v>
       </c>
       <c r="U60" s="2" t="str">
         <f t="shared" ref="U60:U61" si="47">DEC2HEX(T60,8)</f>
-        <v>00089440</v>
+        <v>00089F80</v>
       </c>
       <c r="V60" s="20">
         <f>X58</f>
-        <v>3809179</v>
+        <v>5508616</v>
       </c>
       <c r="W60" s="2" t="str">
         <f t="shared" ref="W60:W61" si="48">DEC2HEX(V60,8)</f>
-        <v>003A1F9B</v>
+        <v>00540E08</v>
       </c>
       <c r="X60" s="20">
         <f>Z58+M58</f>
-        <v>3836123</v>
+        <v>5535560</v>
       </c>
       <c r="Y60" s="2" t="str">
         <f>DEC2HEX(X60,8)</f>
-        <v>003A88DB</v>
+        <v>00547748</v>
       </c>
       <c r="Z60" s="20"/>
       <c r="AA60" s="2" t="str">
@@ -6627,27 +6630,27 @@
       </c>
       <c r="T61" s="20">
         <f>T60+P60</f>
-        <v>578880</v>
+        <v>581760</v>
       </c>
       <c r="U61" s="2" t="str">
         <f t="shared" si="47"/>
-        <v>0008D540</v>
+        <v>0008E080</v>
       </c>
       <c r="V61" s="20">
         <f>Z58</f>
-        <v>3821723</v>
+        <v>5521160</v>
       </c>
       <c r="W61" s="2" t="str">
         <f t="shared" si="48"/>
-        <v>003A509B</v>
+        <v>00543F08</v>
       </c>
       <c r="X61" s="20">
         <f>X60+L60</f>
-        <v>3886299</v>
+        <v>5585736</v>
       </c>
       <c r="Y61" s="2" t="str">
         <f>DEC2HEX(X61,8)</f>
-        <v>003B4CDB</v>
+        <v>00553B48</v>
       </c>
       <c r="Z61" s="20"/>
       <c r="AA61" s="2" t="str">
@@ -6943,27 +6946,27 @@
       </c>
       <c r="T66" s="20">
         <f>T61+P61</f>
-        <v>726592</v>
+        <v>729472</v>
       </c>
       <c r="U66" s="2" t="str">
         <f>DEC2HEX(T66,8)</f>
-        <v>000B1640</v>
+        <v>000B2180</v>
       </c>
       <c r="V66" s="20">
         <f>X60</f>
-        <v>3836123</v>
+        <v>5535560</v>
       </c>
       <c r="W66" s="2" t="str">
         <f>DEC2HEX(V66,8)</f>
-        <v>003A88DB</v>
+        <v>00547748</v>
       </c>
       <c r="X66" s="20">
         <f>X61+L61</f>
-        <v>3936475</v>
+        <v>5635912</v>
       </c>
       <c r="Y66" s="2" t="str">
         <f>DEC2HEX(X66,8)</f>
-        <v>003C10DB</v>
+        <v>0055FF48</v>
       </c>
       <c r="Z66" s="20"/>
       <c r="AA66" s="2" t="str">
@@ -7117,19 +7120,19 @@
       </c>
       <c r="V68" s="22">
         <f>X66</f>
-        <v>3936475</v>
+        <v>5635912</v>
       </c>
       <c r="W68" s="4" t="str">
         <f>DEC2HEX(V68,8)</f>
-        <v>003C10DB</v>
+        <v>0055FF48</v>
       </c>
       <c r="X68" s="22">
         <f>X66+L66</f>
-        <v>4132475</v>
+        <v>5831912</v>
       </c>
       <c r="Y68" s="4" t="str">
         <f>DEC2HEX(X68,8)</f>
-        <v>003F0E7B</v>
+        <v>0058FCE8</v>
       </c>
       <c r="Z68" s="22"/>
       <c r="AA68" s="4" t="str">
@@ -7235,12 +7238,12 @@
       <c r="K70" s="14"/>
       <c r="L70" s="14">
         <f>SUM(L3:L69)</f>
-        <v>3269923</v>
+        <v>3527568</v>
       </c>
       <c r="M70" s="14"/>
       <c r="N70" s="14">
         <f>SUM(N4:N69)</f>
-        <v>1231552</v>
+        <v>1234432</v>
       </c>
       <c r="O70" s="14">
         <f>SUM(O4:O69)</f>
@@ -7248,7 +7251,7 @@
       </c>
       <c r="P70" s="14">
         <f>SUM(P4:P69)</f>
-        <v>1235496</v>
+        <v>1238376</v>
       </c>
       <c r="Q70" s="9"/>
       <c r="R70" s="14"/>
@@ -7305,16 +7308,16 @@
       <c r="K71" s="14"/>
       <c r="L71" s="14">
         <f>L70*16/1024/8</f>
-        <v>6386.568359375</v>
+        <v>6889.78125</v>
       </c>
       <c r="M71" s="14"/>
       <c r="N71" s="14">
         <f>N70*16/1024/8</f>
-        <v>2405.375</v>
+        <v>2411</v>
       </c>
       <c r="O71" s="14">
         <f>N70+O70</f>
-        <v>1235496</v>
+        <v>1238376</v>
       </c>
       <c r="P71" s="14"/>
       <c r="Q71" s="9"/>
@@ -7366,7 +7369,7 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView zoomScale="76" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7386,7 +7389,7 @@
         <v>83</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>176</v>
+        <v>226</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>116</v>
@@ -7413,7 +7416,7 @@
       </c>
       <c r="K1" t="str">
         <f t="shared" ref="K1:K30" si="2">LEFT(SUBSTITUTE(C1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C1,"_",),4)</f>
-        <v>0006 0009</v>
+        <v>0006 0901</v>
       </c>
       <c r="L1" t="str">
         <f t="shared" ref="L1:L30" si="3">LEFT(SUBSTITUTE(D1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D1,"_",),4)</f>
@@ -7438,13 +7441,13 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>176</v>
+        <v>226</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>119</v>
@@ -7471,7 +7474,7 @@
       </c>
       <c r="K2" t="str">
         <f t="shared" si="2"/>
-        <v>0006 0009</v>
+        <v>0006 0901</v>
       </c>
       <c r="L2" t="str">
         <f t="shared" si="3"/>
@@ -7496,13 +7499,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>84</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>179</v>
+        <v>227</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>126</v>
@@ -7517,7 +7520,7 @@
         <v>121</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I3" t="str">
         <f t="shared" si="0"/>
@@ -7529,7 +7532,7 @@
       </c>
       <c r="K3" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0103</v>
       </c>
       <c r="L3" t="str">
         <f t="shared" si="3"/>
@@ -7554,13 +7557,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>179</v>
+        <v>228</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>127</v>
@@ -7569,7 +7572,7 @@
         <v>120</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>119</v>
@@ -7587,7 +7590,7 @@
       </c>
       <c r="K4" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0101</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" si="3"/>
@@ -7612,13 +7615,13 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>128</v>
@@ -7627,7 +7630,7 @@
         <v>121</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>119</v>
@@ -7645,7 +7648,7 @@
       </c>
       <c r="K5" t="str">
         <f t="shared" si="2"/>
-        <v>0003 0009</v>
+        <v>0003 0901</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" si="3"/>
@@ -7670,28 +7673,28 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>86</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>179</v>
+        <v>227</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>129</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>186</v>
-      </c>
       <c r="H6" s="11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
@@ -7703,7 +7706,7 @@
       </c>
       <c r="K6" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0103</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="3"/>
@@ -7728,22 +7731,22 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>179</v>
+        <v>228</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>130</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>119</v>
@@ -7761,7 +7764,7 @@
       </c>
       <c r="K7" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0101</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="3"/>
@@ -7786,22 +7789,22 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>131</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>119</v>
@@ -7819,7 +7822,7 @@
       </c>
       <c r="K8" t="str">
         <f t="shared" si="2"/>
-        <v>0003 0009</v>
+        <v>0003 0901</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="3"/>
@@ -7844,22 +7847,22 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>99</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>176</v>
+        <v>226</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>119</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>119</v>
@@ -7877,7 +7880,7 @@
       </c>
       <c r="K9" t="str">
         <f t="shared" si="2"/>
-        <v>0006 0009</v>
+        <v>0006 0901</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="3"/>
@@ -7902,28 +7905,28 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>179</v>
+        <v>227</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="H10" s="11" t="s">
         <v>191</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>194</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
@@ -7935,7 +7938,7 @@
       </c>
       <c r="K10" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0103</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="3"/>
@@ -7960,22 +7963,22 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>179</v>
+        <v>228</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>133</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>119</v>
@@ -7993,7 +7996,7 @@
       </c>
       <c r="K11" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0101</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="3"/>
@@ -8018,22 +8021,22 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>134</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>119</v>
@@ -8051,7 +8054,7 @@
       </c>
       <c r="K12" t="str">
         <f t="shared" si="2"/>
-        <v>0003 0009</v>
+        <v>0003 0901</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="3"/>
@@ -8076,28 +8079,28 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>179</v>
+        <v>227</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>135</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>199</v>
-      </c>
       <c r="H13" s="11" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="0"/>
@@ -8109,7 +8112,7 @@
       </c>
       <c r="K13" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0103</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="3"/>
@@ -8134,22 +8137,22 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>179</v>
+        <v>228</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>136</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>119</v>
@@ -8167,7 +8170,7 @@
       </c>
       <c r="K14" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0101</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="3"/>
@@ -8192,22 +8195,22 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>137</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>119</v>
@@ -8225,7 +8228,7 @@
       </c>
       <c r="K15" t="str">
         <f t="shared" si="2"/>
-        <v>0003 0009</v>
+        <v>0003 0901</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="3"/>
@@ -8250,22 +8253,22 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>100</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>176</v>
+        <v>226</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>119</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>119</v>
@@ -8283,7 +8286,7 @@
       </c>
       <c r="K16" t="str">
         <f t="shared" si="2"/>
-        <v>0006 0009</v>
+        <v>0006 0901</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="3"/>
@@ -8308,28 +8311,28 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>179</v>
+        <v>227</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>138</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="H17" s="11" t="s">
         <v>204</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>207</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" si="0"/>
@@ -8341,7 +8344,7 @@
       </c>
       <c r="K17" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0103</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="3"/>
@@ -8366,22 +8369,22 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>179</v>
+        <v>228</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>139</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>119</v>
@@ -8399,7 +8402,7 @@
       </c>
       <c r="K18" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0101</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="3"/>
@@ -8424,22 +8427,22 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>140</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>119</v>
@@ -8457,7 +8460,7 @@
       </c>
       <c r="K19" t="str">
         <f t="shared" si="2"/>
-        <v>0003 0009</v>
+        <v>0003 0901</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" si="3"/>
@@ -8482,28 +8485,28 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>179</v>
+        <v>227</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>141</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>212</v>
-      </c>
       <c r="H20" s="11" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="0"/>
@@ -8515,7 +8518,7 @@
       </c>
       <c r="K20" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0103</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="3"/>
@@ -8540,22 +8543,22 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>179</v>
+        <v>228</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>142</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>119</v>
@@ -8573,7 +8576,7 @@
       </c>
       <c r="K21" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0101</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" si="3"/>
@@ -8598,22 +8601,22 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>143</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>119</v>
@@ -8631,7 +8634,7 @@
       </c>
       <c r="K22" t="str">
         <f t="shared" si="2"/>
-        <v>0003 0009</v>
+        <v>0003 0901</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" si="3"/>
@@ -8656,28 +8659,28 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>179</v>
+        <v>227</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>144</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>216</v>
-      </c>
       <c r="H23" s="11" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="0"/>
@@ -8689,7 +8692,7 @@
       </c>
       <c r="K23" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0103</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" si="3"/>
@@ -8714,22 +8717,22 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>179</v>
+        <v>228</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>145</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>119</v>
@@ -8747,7 +8750,7 @@
       </c>
       <c r="K24" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0101</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" si="3"/>
@@ -8772,22 +8775,22 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>146</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>119</v>
@@ -8805,7 +8808,7 @@
       </c>
       <c r="K25" t="str">
         <f t="shared" si="2"/>
-        <v>0003 0009</v>
+        <v>0003 0901</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" si="3"/>
@@ -8830,28 +8833,28 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>94</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>179</v>
+        <v>227</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>147</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="0"/>
@@ -8863,7 +8866,7 @@
       </c>
       <c r="K26" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0103</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" si="3"/>
@@ -8888,22 +8891,22 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>179</v>
+        <v>228</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>148</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>119</v>
@@ -8921,7 +8924,7 @@
       </c>
       <c r="K27" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0101</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" si="3"/>
@@ -8946,22 +8949,22 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>149</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>119</v>
@@ -8979,7 +8982,7 @@
       </c>
       <c r="K28" t="str">
         <f t="shared" si="2"/>
-        <v>0003 0009</v>
+        <v>0003 0901</v>
       </c>
       <c r="L28" t="str">
         <f t="shared" si="3"/>
@@ -9004,22 +9007,22 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>123</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>179</v>
+        <v>228</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>150</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>119</v>
@@ -9037,7 +9040,7 @@
       </c>
       <c r="K29" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0001</v>
+        <v>0001 0101</v>
       </c>
       <c r="L29" t="str">
         <f t="shared" si="3"/>
@@ -9062,22 +9065,22 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>124</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>119</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>119</v>
@@ -9095,7 +9098,7 @@
       </c>
       <c r="K30" t="str">
         <f t="shared" si="2"/>
-        <v>000E 00C4</v>
+        <v>000E C401</v>
       </c>
       <c r="L30" t="str">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Update readout and sanity logic in host
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405C8E9D-9159-44CD-9396-442CEE6A2BA3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0BD1AC-34F1-4238-8E22-9A64E9275559}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
@@ -388,21 +388,9 @@
     <t>00001000</t>
   </si>
   <si>
-    <t>000C5BDB</t>
-  </si>
-  <si>
-    <t>0018D41B</t>
-  </si>
-  <si>
     <t>00000000</t>
   </si>
   <si>
-    <t>001BE41B</t>
-  </si>
-  <si>
-    <t>001CA81B</t>
-  </si>
-  <si>
     <t>00C0_0030</t>
   </si>
   <si>
@@ -412,84 +400,6 @@
     <t>03E8_03E8</t>
   </si>
   <si>
-    <t>000A0000</t>
-  </si>
-  <si>
-    <t>00001700</t>
-  </si>
-  <si>
-    <t>00001B10</t>
-  </si>
-  <si>
-    <t>00001F50</t>
-  </si>
-  <si>
-    <t>00004390</t>
-  </si>
-  <si>
-    <t>00004BA0</t>
-  </si>
-  <si>
-    <t>00004FE0</t>
-  </si>
-  <si>
-    <t>00007420</t>
-  </si>
-  <si>
-    <t>00008440</t>
-  </si>
-  <si>
-    <t>000094C0</t>
-  </si>
-  <si>
-    <t>00012540</t>
-  </si>
-  <si>
-    <t>00014560</t>
-  </si>
-  <si>
-    <t>000155E0</t>
-  </si>
-  <si>
-    <t>0001E660</t>
-  </si>
-  <si>
-    <t>00021690</t>
-  </si>
-  <si>
-    <t>00023B50</t>
-  </si>
-  <si>
-    <t>00038010</t>
-  </si>
-  <si>
-    <t>0003C840</t>
-  </si>
-  <si>
-    <t>0003ED00</t>
-  </si>
-  <si>
-    <t>000531C0</t>
-  </si>
-  <si>
-    <t>00059200</t>
-  </si>
-  <si>
-    <t>0005D300</t>
-  </si>
-  <si>
-    <t>00081400</t>
-  </si>
-  <si>
-    <t>00089440</t>
-  </si>
-  <si>
-    <t>0008D540</t>
-  </si>
-  <si>
-    <t>000B1640</t>
-  </si>
-  <si>
     <t>oichannel</t>
   </si>
   <si>
@@ -577,135 +487,33 @@
     <t>3838_0312</t>
   </si>
   <si>
-    <t>001D732B</t>
-  </si>
-  <si>
-    <t>0020832B</t>
-  </si>
-  <si>
-    <t>0023932B</t>
-  </si>
-  <si>
-    <t>0024572B</t>
-  </si>
-  <si>
-    <t>0025223B</t>
-  </si>
-  <si>
-    <t>0028323B</t>
-  </si>
-  <si>
     <t>1C38_0324</t>
   </si>
   <si>
     <t>1C1C_0111</t>
   </si>
   <si>
-    <t>002B423B</t>
-  </si>
-  <si>
-    <t>002CCA3B</t>
-  </si>
-  <si>
-    <t>002D2C3B</t>
-  </si>
-  <si>
     <t>021F_0000</t>
   </si>
   <si>
     <t>1C1C_0312</t>
   </si>
   <si>
-    <t>002D955B</t>
-  </si>
-  <si>
-    <t>002F1D5B</t>
-  </si>
-  <si>
-    <t>0030A55B</t>
-  </si>
-  <si>
-    <t>0031075B</t>
-  </si>
-  <si>
-    <t>0031707B</t>
-  </si>
-  <si>
-    <t>0032F87B</t>
-  </si>
-  <si>
     <t>0E1C_0324</t>
   </si>
   <si>
     <t>0E0E_0111</t>
   </si>
   <si>
-    <t>0034807B</t>
-  </si>
-  <si>
-    <t>0035447B</t>
-  </si>
-  <si>
-    <t>0035693B</t>
-  </si>
-  <si>
     <t>0211_0000</t>
   </si>
   <si>
     <t>0E0E_0312</t>
   </si>
   <si>
-    <t>0035936B</t>
-  </si>
-  <si>
-    <t>0036266B</t>
-  </si>
-  <si>
-    <t>0036B96B</t>
-  </si>
-  <si>
-    <t>0036DE2B</t>
-  </si>
-  <si>
-    <t>0037085B</t>
-  </si>
-  <si>
-    <t>00379B5B</t>
-  </si>
-  <si>
-    <t>00382E5B</t>
-  </si>
-  <si>
-    <t>00385F5B</t>
-  </si>
-  <si>
-    <t>0038979B</t>
-  </si>
-  <si>
-    <t>00395B9B</t>
-  </si>
-  <si>
-    <t>003A1F9B</t>
-  </si>
-  <si>
-    <t>003A509B</t>
-  </si>
-  <si>
-    <t>003A88DB</t>
-  </si>
-  <si>
-    <t>003B4CDB</t>
-  </si>
-  <si>
-    <t>003C10DB</t>
-  </si>
-  <si>
     <t>010E_0E15</t>
   </si>
   <si>
-    <t>003F0E7B</t>
-  </si>
-  <si>
     <t>p0_result staddr</t>
   </si>
   <si>
@@ -728,6 +536,198 @@
   </si>
   <si>
     <t>000E_C401</t>
+  </si>
+  <si>
+    <t>00200000</t>
+  </si>
+  <si>
+    <t>00264A48</t>
+  </si>
+  <si>
+    <t>00002240</t>
+  </si>
+  <si>
+    <t>0032C288</t>
+  </si>
+  <si>
+    <t>0035D288</t>
+  </si>
+  <si>
+    <t>00369688</t>
+  </si>
+  <si>
+    <t>00002650</t>
+  </si>
+  <si>
+    <t>00002A90</t>
+  </si>
+  <si>
+    <t>00376198</t>
+  </si>
+  <si>
+    <t>003A7198</t>
+  </si>
+  <si>
+    <t>00004ED0</t>
+  </si>
+  <si>
+    <t>003D8198</t>
+  </si>
+  <si>
+    <t>003E4598</t>
+  </si>
+  <si>
+    <t>000056E0</t>
+  </si>
+  <si>
+    <t>00005B20</t>
+  </si>
+  <si>
+    <t>003F10A8</t>
+  </si>
+  <si>
+    <t>004220A8</t>
+  </si>
+  <si>
+    <t>00007F60</t>
+  </si>
+  <si>
+    <t>004530A8</t>
+  </si>
+  <si>
+    <t>0046B8A8</t>
+  </si>
+  <si>
+    <t>00471AA8</t>
+  </si>
+  <si>
+    <t>00008F80</t>
+  </si>
+  <si>
+    <t>0000A000</t>
+  </si>
+  <si>
+    <t>004783C8</t>
+  </si>
+  <si>
+    <t>00490BC8</t>
+  </si>
+  <si>
+    <t>00013080</t>
+  </si>
+  <si>
+    <t>004A93C8</t>
+  </si>
+  <si>
+    <t>004AF5C8</t>
+  </si>
+  <si>
+    <t>000150A0</t>
+  </si>
+  <si>
+    <t>00016120</t>
+  </si>
+  <si>
+    <t>004B5EE8</t>
+  </si>
+  <si>
+    <t>004CE6E8</t>
+  </si>
+  <si>
+    <t>0001F1A0</t>
+  </si>
+  <si>
+    <t>004E6EE8</t>
+  </si>
+  <si>
+    <t>004F32E8</t>
+  </si>
+  <si>
+    <t>004F57A8</t>
+  </si>
+  <si>
+    <t>000221D0</t>
+  </si>
+  <si>
+    <t>00024690</t>
+  </si>
+  <si>
+    <t>004F81D8</t>
+  </si>
+  <si>
+    <t>005014D8</t>
+  </si>
+  <si>
+    <t>00038B50</t>
+  </si>
+  <si>
+    <t>0050A7D8</t>
+  </si>
+  <si>
+    <t>0050CC98</t>
+  </si>
+  <si>
+    <t>0003D380</t>
+  </si>
+  <si>
+    <t>0003F840</t>
+  </si>
+  <si>
+    <t>0050F6C8</t>
+  </si>
+  <si>
+    <t>005189C8</t>
+  </si>
+  <si>
+    <t>00053D00</t>
+  </si>
+  <si>
+    <t>00521CC8</t>
+  </si>
+  <si>
+    <t>00524DC8</t>
+  </si>
+  <si>
+    <t>00059D40</t>
+  </si>
+  <si>
+    <t>0005DE40</t>
+  </si>
+  <si>
+    <t>00528608</t>
+  </si>
+  <si>
+    <t>00534A08</t>
+  </si>
+  <si>
+    <t>00081F40</t>
+  </si>
+  <si>
+    <t>00540E08</t>
+  </si>
+  <si>
+    <t>00543F08</t>
+  </si>
+  <si>
+    <t>00089F80</t>
+  </si>
+  <si>
+    <t>0008E080</t>
+  </si>
+  <si>
+    <t>00547748</t>
+  </si>
+  <si>
+    <t>00553B48</t>
+  </si>
+  <si>
+    <t>000B2180</t>
+  </si>
+  <si>
+    <t>0055FF48</t>
+  </si>
+  <si>
+    <t>0058FCE8</t>
   </si>
 </sst>
 </file>
@@ -1313,8 +1313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80B23C6-EAEB-43B1-B045-456C36085CFA}">
   <dimension ref="A1:AL71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="J40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y68" sqref="Y68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1336,12 +1336,12 @@
     <col min="19" max="19" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="6.88671875" style="24" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.88671875" style="24" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.21875" style="24" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8" style="24" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8" style="24" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.21875" style="24" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.21875" style="24" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="10" style="27" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="13.88671875" bestFit="1" customWidth="1"/>
@@ -1368,7 +1368,7 @@
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
       <c r="J1" s="38" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="K1" s="38"/>
       <c r="L1" s="38"/>
@@ -1393,17 +1393,17 @@
       <c r="AD1" s="29"/>
       <c r="AE1" s="33"/>
       <c r="AF1" s="38" t="s">
-        <v>154</v>
+        <v>124</v>
       </c>
       <c r="AG1" s="38"/>
       <c r="AH1" s="38"/>
       <c r="AI1" s="40" t="s">
-        <v>155</v>
+        <v>125</v>
       </c>
       <c r="AJ1" s="39"/>
       <c r="AK1" s="32"/>
       <c r="AL1" s="14" t="s">
-        <v>157</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.3">
@@ -1414,52 +1414,52 @@
         <v>10</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="E2" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="S2" s="14" t="s">
         <v>161</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="Q2" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="R2" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="S2" s="14" t="s">
-        <v>225</v>
       </c>
       <c r="T2" s="38" t="s">
         <v>82</v>
@@ -1470,15 +1470,15 @@
       </c>
       <c r="W2" s="38"/>
       <c r="X2" s="38" t="s">
-        <v>223</v>
+        <v>159</v>
       </c>
       <c r="Y2" s="38"/>
       <c r="Z2" s="38" t="s">
-        <v>224</v>
+        <v>160</v>
       </c>
       <c r="AA2" s="38"/>
       <c r="AB2" s="28" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="AC2" s="14" t="s">
         <v>95</v>
@@ -1487,7 +1487,7 @@
         <v>79</v>
       </c>
       <c r="AE2" s="14" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="AF2" s="14" t="s">
         <v>97</v>
@@ -1496,16 +1496,16 @@
         <v>96</v>
       </c>
       <c r="AH2" s="14" t="s">
-        <v>153</v>
+        <v>123</v>
       </c>
       <c r="AI2" s="9" t="s">
-        <v>156</v>
+        <v>126</v>
       </c>
       <c r="AJ2" s="14" t="s">
         <v>96</v>
       </c>
       <c r="AK2" s="28" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
       <c r="AL2" s="14" t="s">
         <v>76</v>
@@ -1658,7 +1658,7 @@
         <v>00000000</v>
       </c>
       <c r="AB4" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC4" s="2">
         <v>0.01</v>
@@ -1824,7 +1824,7 @@
         <v>00000000</v>
       </c>
       <c r="AB6" s="13" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC6" s="4">
         <v>0.01</v>
@@ -2143,7 +2143,7 @@
         <v>00000000</v>
       </c>
       <c r="AB9" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC9" s="2">
         <v>0.01</v>
@@ -2277,7 +2277,7 @@
         <v>00000000</v>
       </c>
       <c r="AB10" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC10" s="2">
         <v>0.01</v>
@@ -2734,7 +2734,7 @@
         <v>00000000</v>
       </c>
       <c r="AB16" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC16" s="2">
         <v>0.01</v>
@@ -2868,7 +2868,7 @@
         <v>00000000</v>
       </c>
       <c r="AB17" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC17" s="2">
         <v>0.01</v>
@@ -3128,7 +3128,7 @@
         <v>00000000</v>
       </c>
       <c r="AB21" s="13" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC21" s="4">
         <v>0.01</v>
@@ -3447,7 +3447,7 @@
         <v>00000000</v>
       </c>
       <c r="AB24" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC24" s="2">
         <v>0.01</v>
@@ -3581,7 +3581,7 @@
         <v>00000000</v>
       </c>
       <c r="AB25" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC25" s="2">
         <v>0.01</v>
@@ -4038,7 +4038,7 @@
         <v>00000000</v>
       </c>
       <c r="AB31" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC31" s="2">
         <v>0.01</v>
@@ -4172,7 +4172,7 @@
         <v>00000000</v>
       </c>
       <c r="AB32" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC32" s="2">
         <v>0.01</v>
@@ -4432,7 +4432,7 @@
         <v>00000000</v>
       </c>
       <c r="AB36" s="13" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC36" s="4">
         <v>0.01</v>
@@ -4751,7 +4751,7 @@
         <v>00000000</v>
       </c>
       <c r="AB39" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC39" s="2">
         <v>0.01</v>
@@ -4885,7 +4885,7 @@
         <v>00000000</v>
       </c>
       <c r="AB40" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC40" s="2">
         <v>0.01</v>
@@ -5342,7 +5342,7 @@
         <v>00000000</v>
       </c>
       <c r="AB46" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC46" s="2">
         <v>0.01</v>
@@ -5476,7 +5476,7 @@
         <v>00000000</v>
       </c>
       <c r="AB47" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC47" s="2">
         <v>0.01</v>
@@ -5933,7 +5933,7 @@
         <v>00000000</v>
       </c>
       <c r="AB53" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC53" s="2">
         <v>0.01</v>
@@ -6067,7 +6067,7 @@
         <v>00000000</v>
       </c>
       <c r="AB54" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC54" s="2">
         <v>0.01</v>
@@ -6524,7 +6524,7 @@
         <v>00000000</v>
       </c>
       <c r="AB60" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC60" s="2">
         <v>0.01</v>
@@ -6658,7 +6658,7 @@
         <v>00000000</v>
       </c>
       <c r="AB61" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC61" s="2">
         <v>0.01</v>
@@ -6974,7 +6974,7 @@
         <v>00000000</v>
       </c>
       <c r="AB66" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC66" s="2">
         <v>0.01</v>
@@ -7140,7 +7140,7 @@
         <v>00000000</v>
       </c>
       <c r="AB68" s="13" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC68" s="4">
         <v>0.01</v>
@@ -7369,7 +7369,7 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView zoomScale="76" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="I1" sqref="I1:P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7383,28 +7383,28 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>175</v>
+        <v>145</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>83</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>226</v>
+        <v>162</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>116</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>125</v>
+        <v>167</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="H1" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="I1" t="str">
         <f t="shared" ref="I1:I30" si="0">LEFT(SUBSTITUTE(A1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A1,"_",),4)</f>
@@ -7424,11 +7424,11 @@
       </c>
       <c r="M1" t="str">
         <f t="shared" ref="M1:M30" si="4">LEFT(SUBSTITUTE(E1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E1,"_",),4)</f>
-        <v>000A 0000</v>
+        <v>0020 0000</v>
       </c>
       <c r="N1" t="str">
         <f t="shared" ref="N1:N30" si="5">LEFT(SUBSTITUTE(F1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F1,"_",),4)</f>
-        <v>000C 5BDB</v>
+        <v>0026 4A48</v>
       </c>
       <c r="O1" t="str">
         <f t="shared" ref="O1:O30" si="6">LEFT(SUBSTITUTE(G1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(G1,"_",),4)</f>
@@ -7441,28 +7441,28 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>176</v>
+        <v>146</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>226</v>
+        <v>162</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>119</v>
-      </c>
       <c r="H2" s="13" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="I2" t="str">
         <f t="shared" si="0"/>
@@ -7482,11 +7482,11 @@
       </c>
       <c r="M2" t="str">
         <f t="shared" si="4"/>
-        <v>000C 5BDB</v>
+        <v>0026 4A48</v>
       </c>
       <c r="N2" t="str">
         <f t="shared" si="5"/>
-        <v>0018 D41B</v>
+        <v>0032 C288</v>
       </c>
       <c r="O2" t="str">
         <f t="shared" si="6"/>
@@ -7499,28 +7499,28 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>84</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>227</v>
+        <v>163</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>126</v>
+        <v>169</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>118</v>
+        <v>170</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>120</v>
+        <v>171</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>121</v>
+        <v>172</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>178</v>
+        <v>148</v>
       </c>
       <c r="I3" t="str">
         <f t="shared" si="0"/>
@@ -7536,19 +7536,19 @@
       </c>
       <c r="L3" t="str">
         <f t="shared" si="3"/>
-        <v>0000 1700</v>
+        <v>0000 2240</v>
       </c>
       <c r="M3" t="str">
         <f t="shared" si="4"/>
-        <v>0018 D41B</v>
+        <v>0032 C288</v>
       </c>
       <c r="N3" t="str">
         <f t="shared" si="5"/>
-        <v>001B E41B</v>
+        <v>0035 D288</v>
       </c>
       <c r="O3" t="str">
         <f t="shared" si="6"/>
-        <v>001C A81B</v>
+        <v>0036 9688</v>
       </c>
       <c r="P3" t="str">
         <f t="shared" si="7"/>
@@ -7557,28 +7557,28 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>228</v>
+        <v>164</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>127</v>
+        <v>173</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>120</v>
+        <v>171</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" si="0"/>
@@ -7594,15 +7594,15 @@
       </c>
       <c r="L4" t="str">
         <f t="shared" si="3"/>
-        <v>0000 1B10</v>
+        <v>0000 2650</v>
       </c>
       <c r="M4" t="str">
         <f t="shared" si="4"/>
-        <v>001B E41B</v>
+        <v>0035 D288</v>
       </c>
       <c r="N4" t="str">
         <f t="shared" si="5"/>
-        <v>001D 732B</v>
+        <v>0037 6198</v>
       </c>
       <c r="O4" t="str">
         <f t="shared" si="6"/>
@@ -7615,28 +7615,28 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>179</v>
+        <v>149</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>229</v>
+        <v>165</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>128</v>
+        <v>174</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>121</v>
+        <v>172</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="0"/>
@@ -7652,15 +7652,15 @@
       </c>
       <c r="L5" t="str">
         <f t="shared" si="3"/>
-        <v>0000 1F50</v>
+        <v>0000 2A90</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" si="4"/>
-        <v>001C A81B</v>
+        <v>0036 9688</v>
       </c>
       <c r="N5" t="str">
         <f t="shared" si="5"/>
-        <v>0020 832B</v>
+        <v>003A 7198</v>
       </c>
       <c r="O5" t="str">
         <f t="shared" si="6"/>
@@ -7673,28 +7673,28 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>86</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>227</v>
+        <v>163</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>129</v>
+        <v>177</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>178</v>
+        <v>148</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
@@ -7710,19 +7710,19 @@
       </c>
       <c r="L6" t="str">
         <f t="shared" si="3"/>
-        <v>0000 4390</v>
+        <v>0000 4ED0</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" si="4"/>
-        <v>001D 732B</v>
+        <v>0037 6198</v>
       </c>
       <c r="N6" t="str">
         <f t="shared" si="5"/>
-        <v>0023 932B</v>
+        <v>003D 8198</v>
       </c>
       <c r="O6" t="str">
         <f t="shared" si="6"/>
-        <v>0024 572B</v>
+        <v>003E 4598</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" si="7"/>
@@ -7731,28 +7731,28 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>228</v>
+        <v>164</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>130</v>
+        <v>180</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>184</v>
-      </c>
       <c r="G7" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
@@ -7768,15 +7768,15 @@
       </c>
       <c r="L7" t="str">
         <f t="shared" si="3"/>
-        <v>0000 4BA0</v>
+        <v>0000 56E0</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="4"/>
-        <v>0023 932B</v>
+        <v>003D 8198</v>
       </c>
       <c r="N7" t="str">
         <f t="shared" si="5"/>
-        <v>0025 223B</v>
+        <v>003F 10A8</v>
       </c>
       <c r="O7" t="str">
         <f t="shared" si="6"/>
@@ -7789,28 +7789,28 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>179</v>
+        <v>149</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>229</v>
+        <v>165</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>131</v>
+        <v>181</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>185</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
@@ -7826,15 +7826,15 @@
       </c>
       <c r="L8" t="str">
         <f t="shared" si="3"/>
-        <v>0000 4FE0</v>
+        <v>0000 5B20</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" si="4"/>
-        <v>0024 572B</v>
+        <v>003E 4598</v>
       </c>
       <c r="N8" t="str">
         <f t="shared" si="5"/>
-        <v>0028 323B</v>
+        <v>0042 20A8</v>
       </c>
       <c r="O8" t="str">
         <f t="shared" si="6"/>
@@ -7847,28 +7847,28 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>186</v>
+        <v>150</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>99</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>226</v>
+        <v>162</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
@@ -7888,11 +7888,11 @@
       </c>
       <c r="M9" t="str">
         <f t="shared" si="4"/>
-        <v>0025 223B</v>
+        <v>003F 10A8</v>
       </c>
       <c r="N9" t="str">
         <f t="shared" si="5"/>
-        <v>002B 423B</v>
+        <v>0045 30A8</v>
       </c>
       <c r="O9" t="str">
         <f t="shared" si="6"/>
@@ -7905,28 +7905,28 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>187</v>
+        <v>151</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>227</v>
+        <v>163</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>132</v>
+        <v>184</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>191</v>
+        <v>152</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
@@ -7942,19 +7942,19 @@
       </c>
       <c r="L10" t="str">
         <f t="shared" si="3"/>
-        <v>0000 7420</v>
+        <v>0000 7F60</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" si="4"/>
-        <v>002B 423B</v>
+        <v>0045 30A8</v>
       </c>
       <c r="N10" t="str">
         <f t="shared" si="5"/>
-        <v>002C CA3B</v>
+        <v>0046 B8A8</v>
       </c>
       <c r="O10" t="str">
         <f t="shared" si="6"/>
-        <v>002D 2C3B</v>
+        <v>0047 1AA8</v>
       </c>
       <c r="P10" t="str">
         <f t="shared" si="7"/>
@@ -7963,28 +7963,28 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>187</v>
+        <v>151</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>228</v>
+        <v>164</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>133</v>
+        <v>188</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="0"/>
@@ -8000,15 +8000,15 @@
       </c>
       <c r="L11" t="str">
         <f t="shared" si="3"/>
-        <v>0000 8440</v>
+        <v>0000 8F80</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" si="4"/>
-        <v>002C CA3B</v>
+        <v>0046 B8A8</v>
       </c>
       <c r="N11" t="str">
         <f t="shared" si="5"/>
-        <v>002D 955B</v>
+        <v>0047 83C8</v>
       </c>
       <c r="O11" t="str">
         <f t="shared" si="6"/>
@@ -8021,28 +8021,28 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>192</v>
+        <v>153</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>229</v>
+        <v>165</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>134</v>
+        <v>189</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="0"/>
@@ -8058,15 +8058,15 @@
       </c>
       <c r="L12" t="str">
         <f t="shared" si="3"/>
-        <v>0000 94C0</v>
+        <v>0000 A000</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" si="4"/>
-        <v>002D 2C3B</v>
+        <v>0047 1AA8</v>
       </c>
       <c r="N12" t="str">
         <f t="shared" si="5"/>
-        <v>002F 1D5B</v>
+        <v>0049 0BC8</v>
       </c>
       <c r="O12" t="str">
         <f t="shared" si="6"/>
@@ -8079,28 +8079,28 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>187</v>
+        <v>151</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>227</v>
+        <v>163</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>135</v>
+        <v>192</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>195</v>
-      </c>
       <c r="G13" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>191</v>
+        <v>152</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="0"/>
@@ -8116,19 +8116,19 @@
       </c>
       <c r="L13" t="str">
         <f t="shared" si="3"/>
-        <v>0001 2540</v>
+        <v>0001 3080</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="4"/>
-        <v>002D 955B</v>
+        <v>0047 83C8</v>
       </c>
       <c r="N13" t="str">
         <f t="shared" si="5"/>
-        <v>0030 A55B</v>
+        <v>004A 93C8</v>
       </c>
       <c r="O13" t="str">
         <f t="shared" si="6"/>
-        <v>0031 075B</v>
+        <v>004A F5C8</v>
       </c>
       <c r="P13" t="str">
         <f t="shared" si="7"/>
@@ -8137,28 +8137,28 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>187</v>
+        <v>151</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>228</v>
+        <v>164</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>136</v>
+        <v>195</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>197</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="0"/>
@@ -8174,15 +8174,15 @@
       </c>
       <c r="L14" t="str">
         <f t="shared" si="3"/>
-        <v>0001 4560</v>
+        <v>0001 50A0</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="4"/>
-        <v>0030 A55B</v>
+        <v>004A 93C8</v>
       </c>
       <c r="N14" t="str">
         <f t="shared" si="5"/>
-        <v>0031 707B</v>
+        <v>004B 5EE8</v>
       </c>
       <c r="O14" t="str">
         <f t="shared" si="6"/>
@@ -8195,28 +8195,28 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>192</v>
+        <v>153</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>229</v>
+        <v>165</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>137</v>
+        <v>196</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>198</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="0"/>
@@ -8232,15 +8232,15 @@
       </c>
       <c r="L15" t="str">
         <f t="shared" si="3"/>
-        <v>0001 55E0</v>
+        <v>0001 6120</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="4"/>
-        <v>0031 075B</v>
+        <v>004A F5C8</v>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="5"/>
-        <v>0032 F87B</v>
+        <v>004C E6E8</v>
       </c>
       <c r="O15" t="str">
         <f t="shared" si="6"/>
@@ -8253,28 +8253,28 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>199</v>
+        <v>154</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>100</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>226</v>
+        <v>162</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>197</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" si="0"/>
@@ -8294,11 +8294,11 @@
       </c>
       <c r="M16" t="str">
         <f t="shared" si="4"/>
-        <v>0031 707B</v>
+        <v>004B 5EE8</v>
       </c>
       <c r="N16" t="str">
         <f t="shared" si="5"/>
-        <v>0034 807B</v>
+        <v>004E 6EE8</v>
       </c>
       <c r="O16" t="str">
         <f t="shared" si="6"/>
@@ -8311,28 +8311,28 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>200</v>
+        <v>155</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>227</v>
+        <v>163</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>138</v>
+        <v>199</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>203</v>
-      </c>
       <c r="H17" s="11" t="s">
-        <v>204</v>
+        <v>156</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" si="0"/>
@@ -8348,19 +8348,19 @@
       </c>
       <c r="L17" t="str">
         <f t="shared" si="3"/>
-        <v>0001 E660</v>
+        <v>0001 F1A0</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="4"/>
-        <v>0034 807B</v>
+        <v>004E 6EE8</v>
       </c>
       <c r="N17" t="str">
         <f t="shared" si="5"/>
-        <v>0035 447B</v>
+        <v>004F 32E8</v>
       </c>
       <c r="O17" t="str">
         <f t="shared" si="6"/>
-        <v>0035 693B</v>
+        <v>004F 57A8</v>
       </c>
       <c r="P17" t="str">
         <f t="shared" si="7"/>
@@ -8369,28 +8369,28 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>200</v>
+        <v>155</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>228</v>
+        <v>164</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>139</v>
+        <v>203</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" si="0"/>
@@ -8406,15 +8406,15 @@
       </c>
       <c r="L18" t="str">
         <f t="shared" si="3"/>
-        <v>0002 1690</v>
+        <v>0002 21D0</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" si="4"/>
-        <v>0035 447B</v>
+        <v>004F 32E8</v>
       </c>
       <c r="N18" t="str">
         <f t="shared" si="5"/>
-        <v>0035 936B</v>
+        <v>004F 81D8</v>
       </c>
       <c r="O18" t="str">
         <f t="shared" si="6"/>
@@ -8427,28 +8427,28 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>205</v>
+        <v>157</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>229</v>
+        <v>165</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>140</v>
+        <v>204</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" si="0"/>
@@ -8464,15 +8464,15 @@
       </c>
       <c r="L19" t="str">
         <f t="shared" si="3"/>
-        <v>0002 3B50</v>
+        <v>0002 4690</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="4"/>
-        <v>0035 693B</v>
+        <v>004F 57A8</v>
       </c>
       <c r="N19" t="str">
         <f t="shared" si="5"/>
-        <v>0036 266B</v>
+        <v>0050 14D8</v>
       </c>
       <c r="O19" t="str">
         <f t="shared" si="6"/>
@@ -8485,19 +8485,19 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>200</v>
+        <v>155</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>227</v>
+        <v>163</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>141</v>
+        <v>207</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>208</v>
@@ -8506,7 +8506,7 @@
         <v>209</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>204</v>
+        <v>156</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="0"/>
@@ -8522,19 +8522,19 @@
       </c>
       <c r="L20" t="str">
         <f t="shared" si="3"/>
-        <v>0003 8010</v>
+        <v>0003 8B50</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="4"/>
-        <v>0035 936B</v>
+        <v>004F 81D8</v>
       </c>
       <c r="N20" t="str">
         <f t="shared" si="5"/>
-        <v>0036 B96B</v>
+        <v>0050 A7D8</v>
       </c>
       <c r="O20" t="str">
         <f t="shared" si="6"/>
-        <v>0036 DE2B</v>
+        <v>0050 CC98</v>
       </c>
       <c r="P20" t="str">
         <f t="shared" si="7"/>
@@ -8543,28 +8543,28 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>200</v>
+        <v>155</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>228</v>
+        <v>164</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>142</v>
+        <v>210</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>208</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" si="0"/>
@@ -8580,15 +8580,15 @@
       </c>
       <c r="L21" t="str">
         <f t="shared" si="3"/>
-        <v>0003 C840</v>
+        <v>0003 D380</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="4"/>
-        <v>0036 B96B</v>
+        <v>0050 A7D8</v>
       </c>
       <c r="N21" t="str">
         <f t="shared" si="5"/>
-        <v>0037 085B</v>
+        <v>0050 F6C8</v>
       </c>
       <c r="O21" t="str">
         <f t="shared" si="6"/>
@@ -8601,28 +8601,28 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>205</v>
+        <v>157</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>229</v>
+        <v>165</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>143</v>
+        <v>211</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>209</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" si="0"/>
@@ -8638,15 +8638,15 @@
       </c>
       <c r="L22" t="str">
         <f t="shared" si="3"/>
-        <v>0003 ED00</v>
+        <v>0003 F840</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="4"/>
-        <v>0036 DE2B</v>
+        <v>0050 CC98</v>
       </c>
       <c r="N22" t="str">
         <f t="shared" si="5"/>
-        <v>0037 9B5B</v>
+        <v>0051 89C8</v>
       </c>
       <c r="O22" t="str">
         <f t="shared" si="6"/>
@@ -8659,28 +8659,28 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>200</v>
+        <v>155</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>227</v>
+        <v>163</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>144</v>
+        <v>214</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>204</v>
+        <v>156</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="0"/>
@@ -8696,19 +8696,19 @@
       </c>
       <c r="L23" t="str">
         <f t="shared" si="3"/>
-        <v>0005 31C0</v>
+        <v>0005 3D00</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" si="4"/>
-        <v>0037 085B</v>
+        <v>0050 F6C8</v>
       </c>
       <c r="N23" t="str">
         <f t="shared" si="5"/>
-        <v>0038 2E5B</v>
+        <v>0052 1CC8</v>
       </c>
       <c r="O23" t="str">
         <f t="shared" si="6"/>
-        <v>0038 5F5B</v>
+        <v>0052 4DC8</v>
       </c>
       <c r="P23" t="str">
         <f t="shared" si="7"/>
@@ -8717,28 +8717,28 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>200</v>
+        <v>155</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>228</v>
+        <v>164</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>145</v>
+        <v>217</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="0"/>
@@ -8754,15 +8754,15 @@
       </c>
       <c r="L24" t="str">
         <f t="shared" si="3"/>
-        <v>0005 9200</v>
+        <v>0005 9D40</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" si="4"/>
-        <v>0038 2E5B</v>
+        <v>0052 1CC8</v>
       </c>
       <c r="N24" t="str">
         <f t="shared" si="5"/>
-        <v>0038 979B</v>
+        <v>0052 8608</v>
       </c>
       <c r="O24" t="str">
         <f t="shared" si="6"/>
@@ -8775,28 +8775,28 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>205</v>
+        <v>157</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>229</v>
+        <v>165</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>146</v>
+        <v>218</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="I25" t="str">
         <f t="shared" si="0"/>
@@ -8812,15 +8812,15 @@
       </c>
       <c r="L25" t="str">
         <f t="shared" si="3"/>
-        <v>0005 D300</v>
+        <v>0005 DE40</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" si="4"/>
-        <v>0038 5F5B</v>
+        <v>0052 4DC8</v>
       </c>
       <c r="N25" t="str">
         <f t="shared" si="5"/>
-        <v>0039 5B9B</v>
+        <v>0053 4A08</v>
       </c>
       <c r="O25" t="str">
         <f t="shared" si="6"/>
@@ -8833,28 +8833,28 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>200</v>
+        <v>155</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>94</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>227</v>
+        <v>163</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>147</v>
+        <v>221</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>204</v>
+        <v>156</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="0"/>
@@ -8870,19 +8870,19 @@
       </c>
       <c r="L26" t="str">
         <f t="shared" si="3"/>
-        <v>0008 1400</v>
+        <v>0008 1F40</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" si="4"/>
-        <v>0039 5B9B</v>
+        <v>0053 4A08</v>
       </c>
       <c r="N26" t="str">
         <f t="shared" si="5"/>
-        <v>003A 1F9B</v>
+        <v>0054 0E08</v>
       </c>
       <c r="O26" t="str">
         <f t="shared" si="6"/>
-        <v>003A 509B</v>
+        <v>0054 3F08</v>
       </c>
       <c r="P26" t="str">
         <f t="shared" si="7"/>
@@ -8891,28 +8891,28 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>200</v>
+        <v>155</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>228</v>
+        <v>164</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>148</v>
+        <v>224</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="I27" t="str">
         <f t="shared" si="0"/>
@@ -8928,15 +8928,15 @@
       </c>
       <c r="L27" t="str">
         <f t="shared" si="3"/>
-        <v>0008 9440</v>
+        <v>0008 9F80</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" si="4"/>
-        <v>003A 1F9B</v>
+        <v>0054 0E08</v>
       </c>
       <c r="N27" t="str">
         <f t="shared" si="5"/>
-        <v>003A 88DB</v>
+        <v>0054 7748</v>
       </c>
       <c r="O27" t="str">
         <f t="shared" si="6"/>
@@ -8949,28 +8949,28 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>205</v>
+        <v>157</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>229</v>
+        <v>165</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>149</v>
+        <v>225</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="I28" t="str">
         <f t="shared" si="0"/>
@@ -8986,15 +8986,15 @@
       </c>
       <c r="L28" t="str">
         <f t="shared" si="3"/>
-        <v>0008 D540</v>
+        <v>0008 E080</v>
       </c>
       <c r="M28" t="str">
         <f t="shared" si="4"/>
-        <v>003A 509B</v>
+        <v>0054 3F08</v>
       </c>
       <c r="N28" t="str">
         <f t="shared" si="5"/>
-        <v>003B 4CDB</v>
+        <v>0055 3B48</v>
       </c>
       <c r="O28" t="str">
         <f t="shared" si="6"/>
@@ -9007,28 +9007,28 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>200</v>
+        <v>155</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="E29" s="2" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="I29" t="str">
         <f t="shared" si="0"/>
@@ -9044,15 +9044,15 @@
       </c>
       <c r="L29" t="str">
         <f t="shared" si="3"/>
-        <v>000B 1640</v>
+        <v>000B 2180</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" si="4"/>
-        <v>003A 88DB</v>
+        <v>0054 7748</v>
       </c>
       <c r="N29" t="str">
         <f t="shared" si="5"/>
-        <v>003C 10DB</v>
+        <v>0055 FF48</v>
       </c>
       <c r="O29" t="str">
         <f t="shared" si="6"/>
@@ -9065,28 +9065,28 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>221</v>
+        <v>158</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C30" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="F30" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>222</v>
-      </c>
       <c r="G30" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="I30" t="str">
         <f t="shared" si="0"/>
@@ -9106,11 +9106,11 @@
       </c>
       <c r="M30" t="str">
         <f t="shared" si="4"/>
-        <v>003C 10DB</v>
+        <v>0055 FF48</v>
       </c>
       <c r="N30" t="str">
         <f t="shared" si="5"/>
-        <v>003F 0E7B</v>
+        <v>0058 FCE8</v>
       </c>
       <c r="O30" t="str">
         <f t="shared" si="6"/>

</xml_diff>

<commit_message>
Update readout and sanity logic in host, fix finish state issue and endian, fix issues leading to system halt
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405C8E9D-9159-44CD-9396-442CEE6A2BA3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0EDA27-467F-4C3D-9C18-EADD3A3580C4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
   <sheets>
     <sheet name="SqueezeNet v2 MEC Parallel Ch" sheetId="2" r:id="rId1"/>
@@ -388,21 +388,9 @@
     <t>00001000</t>
   </si>
   <si>
-    <t>000C5BDB</t>
-  </si>
-  <si>
-    <t>0018D41B</t>
-  </si>
-  <si>
     <t>00000000</t>
   </si>
   <si>
-    <t>001BE41B</t>
-  </si>
-  <si>
-    <t>001CA81B</t>
-  </si>
-  <si>
     <t>00C0_0030</t>
   </si>
   <si>
@@ -412,84 +400,6 @@
     <t>03E8_03E8</t>
   </si>
   <si>
-    <t>000A0000</t>
-  </si>
-  <si>
-    <t>00001700</t>
-  </si>
-  <si>
-    <t>00001B10</t>
-  </si>
-  <si>
-    <t>00001F50</t>
-  </si>
-  <si>
-    <t>00004390</t>
-  </si>
-  <si>
-    <t>00004BA0</t>
-  </si>
-  <si>
-    <t>00004FE0</t>
-  </si>
-  <si>
-    <t>00007420</t>
-  </si>
-  <si>
-    <t>00008440</t>
-  </si>
-  <si>
-    <t>000094C0</t>
-  </si>
-  <si>
-    <t>00012540</t>
-  </si>
-  <si>
-    <t>00014560</t>
-  </si>
-  <si>
-    <t>000155E0</t>
-  </si>
-  <si>
-    <t>0001E660</t>
-  </si>
-  <si>
-    <t>00021690</t>
-  </si>
-  <si>
-    <t>00023B50</t>
-  </si>
-  <si>
-    <t>00038010</t>
-  </si>
-  <si>
-    <t>0003C840</t>
-  </si>
-  <si>
-    <t>0003ED00</t>
-  </si>
-  <si>
-    <t>000531C0</t>
-  </si>
-  <si>
-    <t>00059200</t>
-  </si>
-  <si>
-    <t>0005D300</t>
-  </si>
-  <si>
-    <t>00081400</t>
-  </si>
-  <si>
-    <t>00089440</t>
-  </si>
-  <si>
-    <t>0008D540</t>
-  </si>
-  <si>
-    <t>000B1640</t>
-  </si>
-  <si>
     <t>oichannel</t>
   </si>
   <si>
@@ -562,150 +472,24 @@
     <t>0000_0000</t>
   </si>
   <si>
-    <t>71E3_0322</t>
-  </si>
-  <si>
-    <t>3871_0324</t>
-  </si>
-  <si>
     <t>3838_0111</t>
   </si>
   <si>
     <t>023B_0000</t>
   </si>
   <si>
-    <t>3838_0312</t>
-  </si>
-  <si>
-    <t>001D732B</t>
-  </si>
-  <si>
-    <t>0020832B</t>
-  </si>
-  <si>
-    <t>0023932B</t>
-  </si>
-  <si>
-    <t>0024572B</t>
-  </si>
-  <si>
-    <t>0025223B</t>
-  </si>
-  <si>
-    <t>0028323B</t>
-  </si>
-  <si>
-    <t>1C38_0324</t>
-  </si>
-  <si>
     <t>1C1C_0111</t>
   </si>
   <si>
-    <t>002B423B</t>
-  </si>
-  <si>
-    <t>002CCA3B</t>
-  </si>
-  <si>
-    <t>002D2C3B</t>
-  </si>
-  <si>
     <t>021F_0000</t>
   </si>
   <si>
-    <t>1C1C_0312</t>
-  </si>
-  <si>
-    <t>002D955B</t>
-  </si>
-  <si>
-    <t>002F1D5B</t>
-  </si>
-  <si>
-    <t>0030A55B</t>
-  </si>
-  <si>
-    <t>0031075B</t>
-  </si>
-  <si>
-    <t>0031707B</t>
-  </si>
-  <si>
-    <t>0032F87B</t>
-  </si>
-  <si>
-    <t>0E1C_0324</t>
-  </si>
-  <si>
     <t>0E0E_0111</t>
   </si>
   <si>
-    <t>0034807B</t>
-  </si>
-  <si>
-    <t>0035447B</t>
-  </si>
-  <si>
-    <t>0035693B</t>
-  </si>
-  <si>
     <t>0211_0000</t>
   </si>
   <si>
-    <t>0E0E_0312</t>
-  </si>
-  <si>
-    <t>0035936B</t>
-  </si>
-  <si>
-    <t>0036266B</t>
-  </si>
-  <si>
-    <t>0036B96B</t>
-  </si>
-  <si>
-    <t>0036DE2B</t>
-  </si>
-  <si>
-    <t>0037085B</t>
-  </si>
-  <si>
-    <t>00379B5B</t>
-  </si>
-  <si>
-    <t>00382E5B</t>
-  </si>
-  <si>
-    <t>00385F5B</t>
-  </si>
-  <si>
-    <t>0038979B</t>
-  </si>
-  <si>
-    <t>00395B9B</t>
-  </si>
-  <si>
-    <t>003A1F9B</t>
-  </si>
-  <si>
-    <t>003A509B</t>
-  </si>
-  <si>
-    <t>003A88DB</t>
-  </si>
-  <si>
-    <t>003B4CDB</t>
-  </si>
-  <si>
-    <t>003C10DB</t>
-  </si>
-  <si>
-    <t>010E_0E15</t>
-  </si>
-  <si>
-    <t>003F0E7B</t>
-  </si>
-  <si>
     <t>p0_result staddr</t>
   </si>
   <si>
@@ -728,6 +512,222 @@
   </si>
   <si>
     <t>000E_C401</t>
+  </si>
+  <si>
+    <t>00200000</t>
+  </si>
+  <si>
+    <t>00264A48</t>
+  </si>
+  <si>
+    <t>00002240</t>
+  </si>
+  <si>
+    <t>0032C288</t>
+  </si>
+  <si>
+    <t>0035D288</t>
+  </si>
+  <si>
+    <t>00369688</t>
+  </si>
+  <si>
+    <t>00002650</t>
+  </si>
+  <si>
+    <t>00002A90</t>
+  </si>
+  <si>
+    <t>00376198</t>
+  </si>
+  <si>
+    <t>003A7198</t>
+  </si>
+  <si>
+    <t>00004ED0</t>
+  </si>
+  <si>
+    <t>003D8198</t>
+  </si>
+  <si>
+    <t>003E4598</t>
+  </si>
+  <si>
+    <t>000056E0</t>
+  </si>
+  <si>
+    <t>00005B20</t>
+  </si>
+  <si>
+    <t>003F10A8</t>
+  </si>
+  <si>
+    <t>004220A8</t>
+  </si>
+  <si>
+    <t>00007F60</t>
+  </si>
+  <si>
+    <t>004530A8</t>
+  </si>
+  <si>
+    <t>0046B8A8</t>
+  </si>
+  <si>
+    <t>00471AA8</t>
+  </si>
+  <si>
+    <t>00008F80</t>
+  </si>
+  <si>
+    <t>0000A000</t>
+  </si>
+  <si>
+    <t>004783C8</t>
+  </si>
+  <si>
+    <t>00490BC8</t>
+  </si>
+  <si>
+    <t>00013080</t>
+  </si>
+  <si>
+    <t>004A93C8</t>
+  </si>
+  <si>
+    <t>004AF5C8</t>
+  </si>
+  <si>
+    <t>000150A0</t>
+  </si>
+  <si>
+    <t>00016120</t>
+  </si>
+  <si>
+    <t>004B5EE8</t>
+  </si>
+  <si>
+    <t>004CE6E8</t>
+  </si>
+  <si>
+    <t>0001F1A0</t>
+  </si>
+  <si>
+    <t>004E6EE8</t>
+  </si>
+  <si>
+    <t>004F32E8</t>
+  </si>
+  <si>
+    <t>004F57A8</t>
+  </si>
+  <si>
+    <t>000221D0</t>
+  </si>
+  <si>
+    <t>00024690</t>
+  </si>
+  <si>
+    <t>004F81D8</t>
+  </si>
+  <si>
+    <t>005014D8</t>
+  </si>
+  <si>
+    <t>00038B50</t>
+  </si>
+  <si>
+    <t>0050A7D8</t>
+  </si>
+  <si>
+    <t>0050CC98</t>
+  </si>
+  <si>
+    <t>0003D380</t>
+  </si>
+  <si>
+    <t>0003F840</t>
+  </si>
+  <si>
+    <t>0050F6C8</t>
+  </si>
+  <si>
+    <t>005189C8</t>
+  </si>
+  <si>
+    <t>00053D00</t>
+  </si>
+  <si>
+    <t>00521CC8</t>
+  </si>
+  <si>
+    <t>00524DC8</t>
+  </si>
+  <si>
+    <t>00059D40</t>
+  </si>
+  <si>
+    <t>0005DE40</t>
+  </si>
+  <si>
+    <t>00528608</t>
+  </si>
+  <si>
+    <t>00534A08</t>
+  </si>
+  <si>
+    <t>00081F40</t>
+  </si>
+  <si>
+    <t>00540E08</t>
+  </si>
+  <si>
+    <t>00543F08</t>
+  </si>
+  <si>
+    <t>00089F80</t>
+  </si>
+  <si>
+    <t>0008E080</t>
+  </si>
+  <si>
+    <t>00547748</t>
+  </si>
+  <si>
+    <t>00553B48</t>
+  </si>
+  <si>
+    <t>000B2180</t>
+  </si>
+  <si>
+    <t>0055FF48</t>
+  </si>
+  <si>
+    <t>0058FCE8</t>
+  </si>
+  <si>
+    <t>71E3_0321</t>
+  </si>
+  <si>
+    <t>3871_0322</t>
+  </si>
+  <si>
+    <t>3838_0311</t>
+  </si>
+  <si>
+    <t>1C38_0322</t>
+  </si>
+  <si>
+    <t>1C1C_0311</t>
+  </si>
+  <si>
+    <t>0E1C_0322</t>
+  </si>
+  <si>
+    <t>0E0E_0311</t>
+  </si>
+  <si>
+    <t>010E_0E13</t>
   </si>
 </sst>
 </file>
@@ -1313,8 +1313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80B23C6-EAEB-43B1-B045-456C36085CFA}">
   <dimension ref="A1:AL71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1336,12 +1336,12 @@
     <col min="19" max="19" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="6.88671875" style="24" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.88671875" style="24" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.21875" style="24" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8" style="24" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8" style="24" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.21875" style="24" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.21875" style="24" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="10" style="27" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="13.88671875" bestFit="1" customWidth="1"/>
@@ -1368,7 +1368,7 @@
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
       <c r="J1" s="38" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="K1" s="38"/>
       <c r="L1" s="38"/>
@@ -1393,17 +1393,17 @@
       <c r="AD1" s="29"/>
       <c r="AE1" s="33"/>
       <c r="AF1" s="38" t="s">
-        <v>154</v>
+        <v>124</v>
       </c>
       <c r="AG1" s="38"/>
       <c r="AH1" s="38"/>
       <c r="AI1" s="40" t="s">
-        <v>155</v>
+        <v>125</v>
       </c>
       <c r="AJ1" s="39"/>
       <c r="AK1" s="32"/>
       <c r="AL1" s="14" t="s">
-        <v>157</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.3">
@@ -1414,52 +1414,52 @@
         <v>10</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>161</v>
+        <v>131</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>166</v>
+        <v>136</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>173</v>
+        <v>143</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>167</v>
+        <v>137</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>165</v>
+        <v>135</v>
       </c>
       <c r="P2" s="14" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
       <c r="R2" s="14" t="s">
-        <v>151</v>
+        <v>121</v>
       </c>
       <c r="S2" s="14" t="s">
-        <v>225</v>
+        <v>153</v>
       </c>
       <c r="T2" s="38" t="s">
         <v>82</v>
@@ -1470,15 +1470,15 @@
       </c>
       <c r="W2" s="38"/>
       <c r="X2" s="38" t="s">
-        <v>223</v>
+        <v>151</v>
       </c>
       <c r="Y2" s="38"/>
       <c r="Z2" s="38" t="s">
-        <v>224</v>
+        <v>152</v>
       </c>
       <c r="AA2" s="38"/>
       <c r="AB2" s="28" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="AC2" s="14" t="s">
         <v>95</v>
@@ -1487,7 +1487,7 @@
         <v>79</v>
       </c>
       <c r="AE2" s="14" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="AF2" s="14" t="s">
         <v>97</v>
@@ -1496,16 +1496,16 @@
         <v>96</v>
       </c>
       <c r="AH2" s="14" t="s">
-        <v>153</v>
+        <v>123</v>
       </c>
       <c r="AI2" s="9" t="s">
-        <v>156</v>
+        <v>126</v>
       </c>
       <c r="AJ2" s="14" t="s">
         <v>96</v>
       </c>
       <c r="AK2" s="28" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
       <c r="AL2" s="14" t="s">
         <v>76</v>
@@ -1574,7 +1574,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2">
         <v>3</v>
@@ -1619,7 +1619,7 @@
       </c>
       <c r="Q4" s="6" t="str">
         <f>DEC2HEX(J4,2)&amp;DEC2HEX(G4,2)&amp;"_"&amp;DEC2HEX(D4,2)&amp;DEC2HEX(H4,1)&amp;DEC2HEX(C4,1)</f>
-        <v>71E3_0322</v>
+        <v>71E3_0321</v>
       </c>
       <c r="R4" s="2" t="str">
         <f>DEC2HEX(F4,4)&amp;"_"&amp;DEC2HEX(E4,4)</f>
@@ -1658,7 +1658,7 @@
         <v>00000000</v>
       </c>
       <c r="AB4" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC4" s="2">
         <v>0.01</v>
@@ -1751,7 +1751,7 @@
         <v>71</v>
       </c>
       <c r="C6" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D6" s="4">
         <v>3</v>
@@ -1787,7 +1787,7 @@
       <c r="P6" s="4"/>
       <c r="Q6" s="8" t="str">
         <f>DEC2HEX(J6,2)&amp;DEC2HEX(G6,2)&amp;"_"&amp;DEC2HEX(D6,2)&amp;DEC2HEX(H6,1)&amp;DEC2HEX(C6,1)</f>
-        <v>3871_0324</v>
+        <v>3871_0322</v>
       </c>
       <c r="R6" s="4" t="str">
         <f>DEC2HEX(F6,4)&amp;"_"&amp;DEC2HEX(F6,4)</f>
@@ -1824,7 +1824,7 @@
         <v>00000000</v>
       </c>
       <c r="AB6" s="13" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC6" s="4">
         <v>0.01</v>
@@ -2143,7 +2143,7 @@
         <v>00000000</v>
       </c>
       <c r="AB9" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC9" s="2">
         <v>0.01</v>
@@ -2192,7 +2192,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2">
         <v>3</v>
@@ -2237,7 +2237,7 @@
       </c>
       <c r="Q10" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>3838_0312</v>
+        <v>3838_0311</v>
       </c>
       <c r="R10" s="2" t="str">
         <f>DEC2HEX(F10,4)&amp;"_"&amp;DEC2HEX(E10,4)</f>
@@ -2277,7 +2277,7 @@
         <v>00000000</v>
       </c>
       <c r="AB10" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC10" s="2">
         <v>0.01</v>
@@ -2734,7 +2734,7 @@
         <v>00000000</v>
       </c>
       <c r="AB16" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC16" s="2">
         <v>0.01</v>
@@ -2783,7 +2783,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2">
         <v>3</v>
@@ -2828,7 +2828,7 @@
       </c>
       <c r="Q17" s="6" t="str">
         <f t="shared" si="8"/>
-        <v>3838_0312</v>
+        <v>3838_0311</v>
       </c>
       <c r="R17" s="2" t="str">
         <f>DEC2HEX(F17,4)&amp;"_"&amp;DEC2HEX(E17,4)</f>
@@ -2868,7 +2868,7 @@
         <v>00000000</v>
       </c>
       <c r="AB17" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC17" s="2">
         <v>0.01</v>
@@ -3055,7 +3055,7 @@
         <v>71</v>
       </c>
       <c r="C21" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D21" s="4">
         <v>3</v>
@@ -3091,7 +3091,7 @@
       <c r="P21" s="4"/>
       <c r="Q21" s="8" t="str">
         <f>DEC2HEX(J21,2)&amp;DEC2HEX(G21,2)&amp;"_"&amp;DEC2HEX(D21,2)&amp;DEC2HEX(H21,1)&amp;DEC2HEX(C21,1)</f>
-        <v>1C38_0324</v>
+        <v>1C38_0322</v>
       </c>
       <c r="R21" s="4" t="str">
         <f>DEC2HEX(F21,4)&amp;"_"&amp;DEC2HEX(F21,4)</f>
@@ -3128,7 +3128,7 @@
         <v>00000000</v>
       </c>
       <c r="AB21" s="13" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC21" s="4">
         <v>0.01</v>
@@ -3447,7 +3447,7 @@
         <v>00000000</v>
       </c>
       <c r="AB24" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC24" s="2">
         <v>0.01</v>
@@ -3496,7 +3496,7 @@
         <v>8</v>
       </c>
       <c r="C25" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" s="2">
         <v>3</v>
@@ -3541,7 +3541,7 @@
       </c>
       <c r="Q25" s="6" t="str">
         <f t="shared" si="15"/>
-        <v>1C1C_0312</v>
+        <v>1C1C_0311</v>
       </c>
       <c r="R25" s="2" t="str">
         <f>DEC2HEX(F25,4)&amp;"_"&amp;DEC2HEX(E25,4)</f>
@@ -3581,7 +3581,7 @@
         <v>00000000</v>
       </c>
       <c r="AB25" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC25" s="2">
         <v>0.01</v>
@@ -4038,7 +4038,7 @@
         <v>00000000</v>
       </c>
       <c r="AB31" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC31" s="2">
         <v>0.01</v>
@@ -4087,7 +4087,7 @@
         <v>8</v>
       </c>
       <c r="C32" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D32" s="2">
         <v>3</v>
@@ -4132,7 +4132,7 @@
       </c>
       <c r="Q32" s="6" t="str">
         <f t="shared" si="21"/>
-        <v>1C1C_0312</v>
+        <v>1C1C_0311</v>
       </c>
       <c r="R32" s="2" t="str">
         <f>DEC2HEX(F32,4)&amp;"_"&amp;DEC2HEX(E32,4)</f>
@@ -4172,7 +4172,7 @@
         <v>00000000</v>
       </c>
       <c r="AB32" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC32" s="2">
         <v>0.01</v>
@@ -4359,7 +4359,7 @@
         <v>71</v>
       </c>
       <c r="C36" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D36" s="4">
         <v>3</v>
@@ -4395,7 +4395,7 @@
       <c r="P36" s="4"/>
       <c r="Q36" s="8" t="str">
         <f>DEC2HEX(J36,2)&amp;DEC2HEX(G36,2)&amp;"_"&amp;DEC2HEX(D36,2)&amp;DEC2HEX(H36,1)&amp;DEC2HEX(C36,1)</f>
-        <v>0E1C_0324</v>
+        <v>0E1C_0322</v>
       </c>
       <c r="R36" s="4" t="str">
         <f>DEC2HEX(F36,4)&amp;"_"&amp;DEC2HEX(F36,4)</f>
@@ -4432,7 +4432,7 @@
         <v>00000000</v>
       </c>
       <c r="AB36" s="13" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC36" s="4">
         <v>0.01</v>
@@ -4751,7 +4751,7 @@
         <v>00000000</v>
       </c>
       <c r="AB39" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC39" s="2">
         <v>0.01</v>
@@ -4800,7 +4800,7 @@
         <v>8</v>
       </c>
       <c r="C40" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D40" s="2">
         <v>3</v>
@@ -4845,7 +4845,7 @@
       </c>
       <c r="Q40" s="6" t="str">
         <f t="shared" si="28"/>
-        <v>0E0E_0312</v>
+        <v>0E0E_0311</v>
       </c>
       <c r="R40" s="2" t="str">
         <f>DEC2HEX(F40,4)&amp;"_"&amp;DEC2HEX(E40,4)</f>
@@ -4885,7 +4885,7 @@
         <v>00000000</v>
       </c>
       <c r="AB40" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC40" s="2">
         <v>0.01</v>
@@ -5342,7 +5342,7 @@
         <v>00000000</v>
       </c>
       <c r="AB46" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC46" s="2">
         <v>0.01</v>
@@ -5391,7 +5391,7 @@
         <v>8</v>
       </c>
       <c r="C47" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D47" s="2">
         <v>3</v>
@@ -5436,7 +5436,7 @@
       </c>
       <c r="Q47" s="6" t="str">
         <f t="shared" si="34"/>
-        <v>0E0E_0312</v>
+        <v>0E0E_0311</v>
       </c>
       <c r="R47" s="2" t="str">
         <f>DEC2HEX(F47,4)&amp;"_"&amp;DEC2HEX(E47,4)</f>
@@ -5476,7 +5476,7 @@
         <v>00000000</v>
       </c>
       <c r="AB47" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC47" s="2">
         <v>0.01</v>
@@ -5933,7 +5933,7 @@
         <v>00000000</v>
       </c>
       <c r="AB53" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC53" s="2">
         <v>0.01</v>
@@ -5982,7 +5982,7 @@
         <v>8</v>
       </c>
       <c r="C54" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D54" s="2">
         <v>3</v>
@@ -6027,7 +6027,7 @@
       </c>
       <c r="Q54" s="6" t="str">
         <f t="shared" si="40"/>
-        <v>0E0E_0312</v>
+        <v>0E0E_0311</v>
       </c>
       <c r="R54" s="2" t="str">
         <f>DEC2HEX(F54,4)&amp;"_"&amp;DEC2HEX(E54,4)</f>
@@ -6067,7 +6067,7 @@
         <v>00000000</v>
       </c>
       <c r="AB54" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC54" s="2">
         <v>0.01</v>
@@ -6524,7 +6524,7 @@
         <v>00000000</v>
       </c>
       <c r="AB60" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC60" s="2">
         <v>0.01</v>
@@ -6573,7 +6573,7 @@
         <v>8</v>
       </c>
       <c r="C61" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D61" s="2">
         <v>3</v>
@@ -6618,7 +6618,7 @@
       </c>
       <c r="Q61" s="6" t="str">
         <f t="shared" si="46"/>
-        <v>0E0E_0312</v>
+        <v>0E0E_0311</v>
       </c>
       <c r="R61" s="2" t="str">
         <f>DEC2HEX(F61,4)&amp;"_"&amp;DEC2HEX(E61,4)</f>
@@ -6658,7 +6658,7 @@
         <v>00000000</v>
       </c>
       <c r="AB61" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC61" s="2">
         <v>0.01</v>
@@ -6974,7 +6974,7 @@
         <v>00000000</v>
       </c>
       <c r="AB66" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC66" s="2">
         <v>0.01</v>
@@ -7067,7 +7067,7 @@
         <v>72</v>
       </c>
       <c r="C68" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D68" s="4">
         <v>14</v>
@@ -7103,7 +7103,7 @@
       <c r="P68" s="4"/>
       <c r="Q68" s="8" t="str">
         <f>DEC2HEX(J68,2)&amp;DEC2HEX(G68,2)&amp;"_"&amp;DEC2HEX(D68,2)&amp;DEC2HEX(H68,1)&amp;DEC2HEX(C68,1)</f>
-        <v>010E_0E15</v>
+        <v>010E_0E13</v>
       </c>
       <c r="R68" s="4" t="str">
         <f>DEC2HEX(F68,4)&amp;"_"&amp;DEC2HEX(F68,4)</f>
@@ -7140,7 +7140,7 @@
         <v>00000000</v>
       </c>
       <c r="AB68" s="13" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="AC68" s="4">
         <v>0.01</v>
@@ -7368,8 +7368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E501AE-4D2D-491C-85E4-0C34FDA03C89}">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView zoomScale="76" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7383,1741 +7383,1741 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>175</v>
+        <v>223</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>83</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>226</v>
+        <v>154</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>116</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>125</v>
+        <v>159</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="H1" s="11" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="I1" t="str">
-        <f t="shared" ref="I1:I30" si="0">LEFT(SUBSTITUTE(A1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A1,"_",),4)</f>
-        <v>71E3 0322</v>
+        <f>RIGHT(SUBSTITUTE(A1,"_",),2)&amp;MID(SUBSTITUTE(A1,"_",),5,2)&amp;" "&amp;MID(SUBSTITUTE(A1,"_",),3,2)&amp;LEFT(SUBSTITUTE(A1,"_",),2)</f>
+        <v>2103 E371</v>
       </c>
       <c r="J1" t="str">
-        <f t="shared" ref="J1:J30" si="1">LEFT(SUBSTITUTE(B1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B1,"_",),4)</f>
-        <v>0040 0003</v>
+        <f t="shared" ref="J1:P16" si="0">RIGHT(SUBSTITUTE(B1,"_",),2)&amp;MID(SUBSTITUTE(B1,"_",),5,2)&amp;" "&amp;MID(SUBSTITUTE(B1,"_",),3,2)&amp;LEFT(SUBSTITUTE(B1,"_",),2)</f>
+        <v>0300 4000</v>
       </c>
       <c r="K1" t="str">
-        <f t="shared" ref="K1:K30" si="2">LEFT(SUBSTITUTE(C1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C1,"_",),4)</f>
-        <v>0006 0901</v>
+        <f t="shared" si="0"/>
+        <v>0109 0600</v>
       </c>
       <c r="L1" t="str">
-        <f t="shared" ref="L1:L30" si="3">LEFT(SUBSTITUTE(D1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D1,"_",),4)</f>
-        <v>0000 1000</v>
+        <f t="shared" si="0"/>
+        <v>0010 0000</v>
       </c>
       <c r="M1" t="str">
-        <f t="shared" ref="M1:M30" si="4">LEFT(SUBSTITUTE(E1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E1,"_",),4)</f>
-        <v>000A 0000</v>
+        <f t="shared" si="0"/>
+        <v>0000 2000</v>
       </c>
       <c r="N1" t="str">
-        <f t="shared" ref="N1:N30" si="5">LEFT(SUBSTITUTE(F1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F1,"_",),4)</f>
-        <v>000C 5BDB</v>
+        <f t="shared" si="0"/>
+        <v>484A 2600</v>
       </c>
       <c r="O1" t="str">
-        <f t="shared" ref="O1:O30" si="6">LEFT(SUBSTITUTE(G1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(G1,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0000 0000</v>
       </c>
       <c r="P1" t="str">
-        <f t="shared" ref="P1:P30" si="7">LEFT(SUBSTITUTE(H1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(H1,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0000 0000</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>176</v>
+        <v>224</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="I2" t="str">
+        <f t="shared" ref="I2:I30" si="1">RIGHT(SUBSTITUTE(A2,"_",),2)&amp;MID(SUBSTITUTE(A2,"_",),5,2)&amp;" "&amp;MID(SUBSTITUTE(A2,"_",),3,2)&amp;LEFT(SUBSTITUTE(A2,"_",),2)</f>
+        <v>2203 7138</v>
+      </c>
+      <c r="J2" t="str">
+        <f t="shared" si="0"/>
+        <v>4000 4000</v>
+      </c>
+      <c r="K2" t="str">
+        <f t="shared" si="0"/>
+        <v>0109 0600</v>
+      </c>
+      <c r="L2" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="M2" t="str">
+        <f t="shared" si="0"/>
+        <v>484A 2600</v>
+      </c>
+      <c r="N2" t="str">
+        <f t="shared" si="0"/>
+        <v>88C2 3200</v>
+      </c>
+      <c r="O2" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="P2" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" si="1"/>
+        <v>1101 3838</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" si="0"/>
+        <v>4000 1000</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" si="0"/>
+        <v>0301 0100</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" si="0"/>
+        <v>4022 0000</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" si="0"/>
+        <v>88C2 3200</v>
+      </c>
+      <c r="N3" t="str">
+        <f t="shared" si="0"/>
+        <v>88D2 3500</v>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" si="0"/>
+        <v>8896 3600</v>
+      </c>
+      <c r="P3" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 3B02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="1"/>
+        <v>1101 3838</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>1000 4000</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="0"/>
+        <v>0101 0100</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="0"/>
+        <v>5026 0000</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="0"/>
+        <v>88D2 3500</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" si="0"/>
+        <v>9861 3700</v>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="P4" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="1"/>
+        <v>1103 3838</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>1000 4000</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v>0109 0300</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="0"/>
+        <v>902A 0000</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="0"/>
+        <v>8896 3600</v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" si="0"/>
+        <v>9871 3A00</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="P5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="1"/>
+        <v>1101 3838</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>8000 1000</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v>0301 0100</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="0"/>
+        <v>D04E 0000</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="0"/>
+        <v>9861 3700</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="0"/>
+        <v>9881 3D00</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="0"/>
+        <v>9845 3E00</v>
+      </c>
+      <c r="P6" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 3B02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="1"/>
+        <v>1101 3838</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>1000 4000</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>0101 0100</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="0"/>
+        <v>E056 0000</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="0"/>
+        <v>9881 3D00</v>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" si="0"/>
+        <v>A810 3F00</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="1"/>
+        <v>1103 3838</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>1000 4000</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v>0109 0300</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="0"/>
+        <v>205B 0000</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="0"/>
+        <v>9845 3E00</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="0"/>
+        <v>A820 4200</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="B9" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="E9" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="1"/>
+        <v>2203 381C</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>8000 8000</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v>0109 0600</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="0"/>
+        <v>A810 3F00</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="0"/>
+        <v>A830 4500</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="1"/>
+        <v>1101 1C1C</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>8000 2000</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v>0301 0100</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="0"/>
+        <v>607F 0000</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="0"/>
+        <v>A830 4500</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" si="0"/>
+        <v>A8B8 4600</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="0"/>
+        <v>A81A 4700</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 1F02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="1"/>
+        <v>1101 1C1C</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="0"/>
+        <v>2000 8000</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v>0101 0100</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="0"/>
+        <v>808F 0000</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="0"/>
+        <v>A8B8 4600</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="0"/>
+        <v>C883 4700</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="1"/>
+        <v>1103 1C1C</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="0"/>
+        <v>2000 8000</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v>0109 0300</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="0"/>
+        <v>00A0 0000</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="0"/>
+        <v>A81A 4700</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="0"/>
+        <v>C80B 4900</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="1"/>
+        <v>1101 1C1C</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="0"/>
+        <v>0001 2000</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v>0301 0100</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="0"/>
+        <v>8030 0100</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="0"/>
+        <v>C883 4700</v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" si="0"/>
+        <v>C893 4A00</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="0"/>
+        <v>C8F5 4A00</v>
+      </c>
+      <c r="P13" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 1F02</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="1"/>
+        <v>1101 1C1C</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="0"/>
+        <v>2000 8000</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="0"/>
+        <v>0101 0100</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="0"/>
+        <v>A050 0100</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="0"/>
+        <v>C893 4A00</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="0"/>
+        <v>E85E 4B00</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="P14" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="1"/>
+        <v>1103 1C1C</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="0"/>
+        <v>2000 8000</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="0"/>
+        <v>0109 0300</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="0"/>
+        <v>2061 0100</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="0"/>
+        <v>C8F5 4A00</v>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" si="0"/>
+        <v>E8E6 4C00</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="P15" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="1"/>
+        <v>2203 1C0E</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="0"/>
+        <v>0001 0001</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="0"/>
+        <v>0109 0600</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="0"/>
+        <v>E85E 4B00</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" si="0"/>
+        <v>E86E 4E00</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="P16" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="1"/>
+        <v>1101 0E0E</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" ref="J17:J30" si="2">RIGHT(SUBSTITUTE(B17,"_",),2)&amp;MID(SUBSTITUTE(B17,"_",),5,2)&amp;" "&amp;MID(SUBSTITUTE(B17,"_",),3,2)&amp;LEFT(SUBSTITUTE(B17,"_",),2)</f>
+        <v>0001 3000</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" ref="K17:K30" si="3">RIGHT(SUBSTITUTE(C17,"_",),2)&amp;MID(SUBSTITUTE(C17,"_",),5,2)&amp;" "&amp;MID(SUBSTITUTE(C17,"_",),3,2)&amp;LEFT(SUBSTITUTE(C17,"_",),2)</f>
+        <v>0301 0100</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" ref="L17:L30" si="4">RIGHT(SUBSTITUTE(D17,"_",),2)&amp;MID(SUBSTITUTE(D17,"_",),5,2)&amp;" "&amp;MID(SUBSTITUTE(D17,"_",),3,2)&amp;LEFT(SUBSTITUTE(D17,"_",),2)</f>
+        <v>A0F1 0100</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" ref="M17:M30" si="5">RIGHT(SUBSTITUTE(E17,"_",),2)&amp;MID(SUBSTITUTE(E17,"_",),5,2)&amp;" "&amp;MID(SUBSTITUTE(E17,"_",),3,2)&amp;LEFT(SUBSTITUTE(E17,"_",),2)</f>
+        <v>E86E 4E00</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" ref="N17:N30" si="6">RIGHT(SUBSTITUTE(F17,"_",),2)&amp;MID(SUBSTITUTE(F17,"_",),5,2)&amp;" "&amp;MID(SUBSTITUTE(F17,"_",),3,2)&amp;LEFT(SUBSTITUTE(F17,"_",),2)</f>
+        <v>E832 4F00</v>
+      </c>
+      <c r="O17" t="str">
+        <f t="shared" ref="O17:O30" si="7">RIGHT(SUBSTITUTE(G17,"_",),2)&amp;MID(SUBSTITUTE(G17,"_",),5,2)&amp;" "&amp;MID(SUBSTITUTE(G17,"_",),3,2)&amp;LEFT(SUBSTITUTE(G17,"_",),2)</f>
+        <v>A857 4F00</v>
+      </c>
+      <c r="P17" t="str">
+        <f t="shared" ref="P17:P30" si="8">RIGHT(SUBSTITUTE(H17,"_",),2)&amp;MID(SUBSTITUTE(H17,"_",),5,2)&amp;" "&amp;MID(SUBSTITUTE(H17,"_",),3,2)&amp;LEFT(SUBSTITUTE(H17,"_",),2)</f>
+        <v>0000 1102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="I2" t="str">
-        <f t="shared" si="0"/>
-        <v>3871 0324</v>
-      </c>
-      <c r="J2" t="str">
+      <c r="C18" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I18" t="str">
         <f t="shared" si="1"/>
-        <v>0040 0040</v>
-      </c>
-      <c r="K2" t="str">
+        <v>1101 0E0E</v>
+      </c>
+      <c r="J18" t="str">
         <f t="shared" si="2"/>
-        <v>0006 0901</v>
-      </c>
-      <c r="L2" t="str">
+        <v>3000 C000</v>
+      </c>
+      <c r="K18" t="str">
         <f t="shared" si="3"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="M2" t="str">
+        <v>0101 0100</v>
+      </c>
+      <c r="L18" t="str">
         <f t="shared" si="4"/>
-        <v>000C 5BDB</v>
-      </c>
-      <c r="N2" t="str">
+        <v>D021 0200</v>
+      </c>
+      <c r="M18" t="str">
         <f t="shared" si="5"/>
-        <v>0018 D41B</v>
-      </c>
-      <c r="O2" t="str">
+        <v>E832 4F00</v>
+      </c>
+      <c r="N18" t="str">
         <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P2" t="str">
+        <v>D881 4F00</v>
+      </c>
+      <c r="O18" t="str">
         <f t="shared" si="7"/>
         <v>0000 0000</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="P18" t="str">
+        <f t="shared" si="8"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="I3" t="str">
-        <f t="shared" si="0"/>
-        <v>3838 0111</v>
-      </c>
-      <c r="J3" t="str">
+      <c r="C19" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I19" t="str">
         <f t="shared" si="1"/>
-        <v>0010 0040</v>
-      </c>
-      <c r="K3" t="str">
+        <v>1103 0E0E</v>
+      </c>
+      <c r="J19" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0103</v>
-      </c>
-      <c r="L3" t="str">
+        <v>3000 C000</v>
+      </c>
+      <c r="K19" t="str">
         <f t="shared" si="3"/>
-        <v>0000 1700</v>
-      </c>
-      <c r="M3" t="str">
+        <v>0109 0300</v>
+      </c>
+      <c r="L19" t="str">
         <f t="shared" si="4"/>
-        <v>0018 D41B</v>
-      </c>
-      <c r="N3" t="str">
+        <v>9046 0200</v>
+      </c>
+      <c r="M19" t="str">
         <f t="shared" si="5"/>
-        <v>001B E41B</v>
-      </c>
-      <c r="O3" t="str">
+        <v>A857 4F00</v>
+      </c>
+      <c r="N19" t="str">
         <f t="shared" si="6"/>
-        <v>001C A81B</v>
-      </c>
-      <c r="P3" t="str">
-        <f t="shared" si="7"/>
-        <v>023B 0000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="I4" t="str">
-        <f t="shared" si="0"/>
-        <v>3838 0111</v>
-      </c>
-      <c r="J4" t="str">
-        <f t="shared" si="1"/>
-        <v>0040 0010</v>
-      </c>
-      <c r="K4" t="str">
-        <f t="shared" si="2"/>
-        <v>0001 0101</v>
-      </c>
-      <c r="L4" t="str">
-        <f t="shared" si="3"/>
-        <v>0000 1B10</v>
-      </c>
-      <c r="M4" t="str">
-        <f t="shared" si="4"/>
-        <v>001B E41B</v>
-      </c>
-      <c r="N4" t="str">
-        <f t="shared" si="5"/>
-        <v>001D 732B</v>
-      </c>
-      <c r="O4" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P4" t="str">
+        <v>D814 5000</v>
+      </c>
+      <c r="O19" t="str">
         <f t="shared" si="7"/>
         <v>0000 0000</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="I5" t="str">
-        <f t="shared" si="0"/>
-        <v>3838 0312</v>
-      </c>
-      <c r="J5" t="str">
+      <c r="P19" t="str">
+        <f t="shared" si="8"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="I20" t="str">
         <f t="shared" si="1"/>
-        <v>0040 0010</v>
-      </c>
-      <c r="K5" t="str">
+        <v>1101 0E0E</v>
+      </c>
+      <c r="J20" t="str">
         <f t="shared" si="2"/>
-        <v>0003 0901</v>
-      </c>
-      <c r="L5" t="str">
+        <v>8001 3000</v>
+      </c>
+      <c r="K20" t="str">
         <f t="shared" si="3"/>
-        <v>0000 1F50</v>
-      </c>
-      <c r="M5" t="str">
+        <v>0301 0100</v>
+      </c>
+      <c r="L20" t="str">
         <f t="shared" si="4"/>
-        <v>001C A81B</v>
-      </c>
-      <c r="N5" t="str">
+        <v>508B 0300</v>
+      </c>
+      <c r="M20" t="str">
         <f t="shared" si="5"/>
-        <v>0020 832B</v>
-      </c>
-      <c r="O5" t="str">
+        <v>D881 4F00</v>
+      </c>
+      <c r="N20" t="str">
         <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P5" t="str">
+        <v>D8A7 5000</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="7"/>
+        <v>98CC 5000</v>
+      </c>
+      <c r="P20" t="str">
+        <f t="shared" si="8"/>
+        <v>0000 1102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="1"/>
+        <v>1101 0E0E</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="2"/>
+        <v>3000 C000</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="3"/>
+        <v>0101 0100</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="4"/>
+        <v>80D3 0300</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="5"/>
+        <v>D8A7 5000</v>
+      </c>
+      <c r="N21" t="str">
+        <f t="shared" si="6"/>
+        <v>C8F6 5000</v>
+      </c>
+      <c r="O21" t="str">
         <f t="shared" si="7"/>
         <v>0000 0000</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="I6" t="str">
-        <f t="shared" si="0"/>
-        <v>3838 0111</v>
-      </c>
-      <c r="J6" t="str">
+      <c r="P21" t="str">
+        <f t="shared" si="8"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I22" t="str">
         <f t="shared" si="1"/>
-        <v>0010 0080</v>
-      </c>
-      <c r="K6" t="str">
+        <v>1103 0E0E</v>
+      </c>
+      <c r="J22" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0103</v>
-      </c>
-      <c r="L6" t="str">
+        <v>3000 C000</v>
+      </c>
+      <c r="K22" t="str">
         <f t="shared" si="3"/>
-        <v>0000 4390</v>
-      </c>
-      <c r="M6" t="str">
+        <v>0109 0300</v>
+      </c>
+      <c r="L22" t="str">
         <f t="shared" si="4"/>
-        <v>001D 732B</v>
-      </c>
-      <c r="N6" t="str">
+        <v>40F8 0300</v>
+      </c>
+      <c r="M22" t="str">
         <f t="shared" si="5"/>
-        <v>0023 932B</v>
-      </c>
-      <c r="O6" t="str">
+        <v>98CC 5000</v>
+      </c>
+      <c r="N22" t="str">
         <f t="shared" si="6"/>
-        <v>0024 572B</v>
-      </c>
-      <c r="P6" t="str">
-        <f t="shared" si="7"/>
-        <v>023B 0000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="I7" t="str">
-        <f t="shared" si="0"/>
-        <v>3838 0111</v>
-      </c>
-      <c r="J7" t="str">
-        <f t="shared" si="1"/>
-        <v>0040 0010</v>
-      </c>
-      <c r="K7" t="str">
-        <f t="shared" si="2"/>
-        <v>0001 0101</v>
-      </c>
-      <c r="L7" t="str">
-        <f t="shared" si="3"/>
-        <v>0000 4BA0</v>
-      </c>
-      <c r="M7" t="str">
-        <f t="shared" si="4"/>
-        <v>0023 932B</v>
-      </c>
-      <c r="N7" t="str">
-        <f t="shared" si="5"/>
-        <v>0025 223B</v>
-      </c>
-      <c r="O7" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P7" t="str">
+        <v>C889 5100</v>
+      </c>
+      <c r="O22" t="str">
         <f t="shared" si="7"/>
         <v>0000 0000</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="I8" t="str">
-        <f t="shared" si="0"/>
-        <v>3838 0312</v>
-      </c>
-      <c r="J8" t="str">
+      <c r="P22" t="str">
+        <f t="shared" si="8"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="I23" t="str">
         <f t="shared" si="1"/>
-        <v>0040 0010</v>
-      </c>
-      <c r="K8" t="str">
+        <v>1101 0E0E</v>
+      </c>
+      <c r="J23" t="str">
         <f t="shared" si="2"/>
-        <v>0003 0901</v>
-      </c>
-      <c r="L8" t="str">
+        <v>8001 4000</v>
+      </c>
+      <c r="K23" t="str">
         <f t="shared" si="3"/>
-        <v>0000 4FE0</v>
-      </c>
-      <c r="M8" t="str">
+        <v>0301 0100</v>
+      </c>
+      <c r="L23" t="str">
         <f t="shared" si="4"/>
-        <v>0024 572B</v>
-      </c>
-      <c r="N8" t="str">
+        <v>003D 0500</v>
+      </c>
+      <c r="M23" t="str">
         <f t="shared" si="5"/>
-        <v>0028 323B</v>
-      </c>
-      <c r="O8" t="str">
+        <v>C8F6 5000</v>
+      </c>
+      <c r="N23" t="str">
         <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P8" t="str">
+        <v>C81C 5200</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="7"/>
+        <v>C84D 5200</v>
+      </c>
+      <c r="P23" t="str">
+        <f t="shared" si="8"/>
+        <v>0000 1102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="1"/>
+        <v>1101 0E0E</v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="2"/>
+        <v>4000 0001</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="3"/>
+        <v>0101 0100</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="4"/>
+        <v>409D 0500</v>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" si="5"/>
+        <v>C81C 5200</v>
+      </c>
+      <c r="N24" t="str">
+        <f t="shared" si="6"/>
+        <v>0886 5200</v>
+      </c>
+      <c r="O24" t="str">
         <f t="shared" si="7"/>
         <v>0000 0000</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="I9" t="str">
-        <f t="shared" si="0"/>
-        <v>1C38 0324</v>
-      </c>
-      <c r="J9" t="str">
+      <c r="P24" t="str">
+        <f t="shared" si="8"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I25" t="str">
         <f t="shared" si="1"/>
-        <v>0080 0080</v>
-      </c>
-      <c r="K9" t="str">
+        <v>1103 0E0E</v>
+      </c>
+      <c r="J25" t="str">
         <f t="shared" si="2"/>
-        <v>0006 0901</v>
-      </c>
-      <c r="L9" t="str">
+        <v>4000 0001</v>
+      </c>
+      <c r="K25" t="str">
         <f t="shared" si="3"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="M9" t="str">
+        <v>0109 0300</v>
+      </c>
+      <c r="L25" t="str">
         <f t="shared" si="4"/>
-        <v>0025 223B</v>
-      </c>
-      <c r="N9" t="str">
+        <v>40DE 0500</v>
+      </c>
+      <c r="M25" t="str">
         <f t="shared" si="5"/>
-        <v>002B 423B</v>
-      </c>
-      <c r="O9" t="str">
+        <v>C84D 5200</v>
+      </c>
+      <c r="N25" t="str">
         <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P9" t="str">
+        <v>084A 5300</v>
+      </c>
+      <c r="O25" t="str">
         <f t="shared" si="7"/>
         <v>0000 0000</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="I10" t="str">
-        <f t="shared" si="0"/>
-        <v>1C1C 0111</v>
-      </c>
-      <c r="J10" t="str">
+      <c r="P25" t="str">
+        <f t="shared" si="8"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="I26" t="str">
         <f t="shared" si="1"/>
-        <v>0020 0080</v>
-      </c>
-      <c r="K10" t="str">
+        <v>1101 0E0E</v>
+      </c>
+      <c r="J26" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0103</v>
-      </c>
-      <c r="L10" t="str">
+        <v>0002 4000</v>
+      </c>
+      <c r="K26" t="str">
         <f t="shared" si="3"/>
-        <v>0000 7420</v>
-      </c>
-      <c r="M10" t="str">
+        <v>0301 0100</v>
+      </c>
+      <c r="L26" t="str">
         <f t="shared" si="4"/>
-        <v>002B 423B</v>
-      </c>
-      <c r="N10" t="str">
+        <v>401F 0800</v>
+      </c>
+      <c r="M26" t="str">
         <f t="shared" si="5"/>
-        <v>002C CA3B</v>
-      </c>
-      <c r="O10" t="str">
+        <v>084A 5300</v>
+      </c>
+      <c r="N26" t="str">
         <f t="shared" si="6"/>
-        <v>002D 2C3B</v>
-      </c>
-      <c r="P10" t="str">
+        <v>080E 5400</v>
+      </c>
+      <c r="O26" t="str">
         <f t="shared" si="7"/>
-        <v>021F 0000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="I11" t="str">
-        <f t="shared" si="0"/>
-        <v>1C1C 0111</v>
-      </c>
-      <c r="J11" t="str">
+        <v>083F 5400</v>
+      </c>
+      <c r="P26" t="str">
+        <f t="shared" si="8"/>
+        <v>0000 1102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I27" t="str">
         <f t="shared" si="1"/>
-        <v>0080 0020</v>
-      </c>
-      <c r="K11" t="str">
+        <v>1101 0E0E</v>
+      </c>
+      <c r="J27" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0101</v>
-      </c>
-      <c r="L11" t="str">
+        <v>4000 0001</v>
+      </c>
+      <c r="K27" t="str">
         <f t="shared" si="3"/>
-        <v>0000 8440</v>
-      </c>
-      <c r="M11" t="str">
+        <v>0101 0100</v>
+      </c>
+      <c r="L27" t="str">
         <f t="shared" si="4"/>
-        <v>002C CA3B</v>
-      </c>
-      <c r="N11" t="str">
+        <v>809F 0800</v>
+      </c>
+      <c r="M27" t="str">
         <f t="shared" si="5"/>
-        <v>002D 955B</v>
-      </c>
-      <c r="O11" t="str">
+        <v>080E 5400</v>
+      </c>
+      <c r="N27" t="str">
         <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P11" t="str">
+        <v>4877 5400</v>
+      </c>
+      <c r="O27" t="str">
         <f t="shared" si="7"/>
         <v>0000 0000</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="P27" t="str">
+        <f t="shared" si="8"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="I12" t="str">
-        <f t="shared" si="0"/>
-        <v>1C1C 0312</v>
-      </c>
-      <c r="J12" t="str">
+      <c r="B28" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I28" t="str">
         <f t="shared" si="1"/>
-        <v>0080 0020</v>
-      </c>
-      <c r="K12" t="str">
+        <v>1103 0E0E</v>
+      </c>
+      <c r="J28" t="str">
         <f t="shared" si="2"/>
-        <v>0003 0901</v>
-      </c>
-      <c r="L12" t="str">
+        <v>4000 0001</v>
+      </c>
+      <c r="K28" t="str">
         <f t="shared" si="3"/>
-        <v>0000 94C0</v>
-      </c>
-      <c r="M12" t="str">
+        <v>0109 0300</v>
+      </c>
+      <c r="L28" t="str">
         <f t="shared" si="4"/>
-        <v>002D 2C3B</v>
-      </c>
-      <c r="N12" t="str">
+        <v>80E0 0800</v>
+      </c>
+      <c r="M28" t="str">
         <f t="shared" si="5"/>
-        <v>002F 1D5B</v>
-      </c>
-      <c r="O12" t="str">
+        <v>083F 5400</v>
+      </c>
+      <c r="N28" t="str">
         <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P12" t="str">
+        <v>483B 5500</v>
+      </c>
+      <c r="O28" t="str">
         <f t="shared" si="7"/>
         <v>0000 0000</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="I13" t="str">
-        <f t="shared" si="0"/>
-        <v>1C1C 0111</v>
-      </c>
-      <c r="J13" t="str">
+      <c r="P28" t="str">
+        <f t="shared" si="8"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I29" t="str">
         <f t="shared" si="1"/>
-        <v>0020 0100</v>
-      </c>
-      <c r="K13" t="str">
+        <v>1101 0E0E</v>
+      </c>
+      <c r="J29" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0103</v>
-      </c>
-      <c r="L13" t="str">
+        <v>0002 E803</v>
+      </c>
+      <c r="K29" t="str">
         <f t="shared" si="3"/>
-        <v>0001 2540</v>
-      </c>
-      <c r="M13" t="str">
+        <v>0101 0100</v>
+      </c>
+      <c r="L29" t="str">
         <f t="shared" si="4"/>
-        <v>002D 955B</v>
-      </c>
-      <c r="N13" t="str">
+        <v>8021 0B00</v>
+      </c>
+      <c r="M29" t="str">
         <f t="shared" si="5"/>
-        <v>0030 A55B</v>
-      </c>
-      <c r="O13" t="str">
+        <v>4877 5400</v>
+      </c>
+      <c r="N29" t="str">
         <f t="shared" si="6"/>
-        <v>0031 075B</v>
-      </c>
-      <c r="P13" t="str">
-        <f t="shared" si="7"/>
-        <v>021F 0000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="I14" t="str">
-        <f t="shared" si="0"/>
-        <v>1C1C 0111</v>
-      </c>
-      <c r="J14" t="str">
-        <f t="shared" si="1"/>
-        <v>0080 0020</v>
-      </c>
-      <c r="K14" t="str">
-        <f t="shared" si="2"/>
-        <v>0001 0101</v>
-      </c>
-      <c r="L14" t="str">
-        <f t="shared" si="3"/>
-        <v>0001 4560</v>
-      </c>
-      <c r="M14" t="str">
-        <f t="shared" si="4"/>
-        <v>0030 A55B</v>
-      </c>
-      <c r="N14" t="str">
-        <f t="shared" si="5"/>
-        <v>0031 707B</v>
-      </c>
-      <c r="O14" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P14" t="str">
+        <v>48FF 5500</v>
+      </c>
+      <c r="O29" t="str">
         <f t="shared" si="7"/>
         <v>0000 0000</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="I15" t="str">
-        <f t="shared" si="0"/>
-        <v>1C1C 0312</v>
-      </c>
-      <c r="J15" t="str">
+      <c r="P29" t="str">
+        <f t="shared" si="8"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="I30" t="str">
         <f t="shared" si="1"/>
-        <v>0080 0020</v>
-      </c>
-      <c r="K15" t="str">
+        <v>130E 0E01</v>
+      </c>
+      <c r="J30" t="str">
         <f t="shared" si="2"/>
-        <v>0003 0901</v>
-      </c>
-      <c r="L15" t="str">
+        <v>E803 E803</v>
+      </c>
+      <c r="K30" t="str">
         <f t="shared" si="3"/>
-        <v>0001 55E0</v>
-      </c>
-      <c r="M15" t="str">
+        <v>01C4 0E00</v>
+      </c>
+      <c r="L30" t="str">
         <f t="shared" si="4"/>
-        <v>0031 075B</v>
-      </c>
-      <c r="N15" t="str">
+        <v>0000 0000</v>
+      </c>
+      <c r="M30" t="str">
         <f t="shared" si="5"/>
-        <v>0032 F87B</v>
-      </c>
-      <c r="O15" t="str">
+        <v>48FF 5500</v>
+      </c>
+      <c r="N30" t="str">
         <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P15" t="str">
+        <v>E8FC 5800</v>
+      </c>
+      <c r="O30" t="str">
         <f t="shared" si="7"/>
         <v>0000 0000</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="I16" t="str">
-        <f t="shared" si="0"/>
-        <v>0E1C 0324</v>
-      </c>
-      <c r="J16" t="str">
-        <f t="shared" si="1"/>
-        <v>0100 0100</v>
-      </c>
-      <c r="K16" t="str">
-        <f t="shared" si="2"/>
-        <v>0006 0901</v>
-      </c>
-      <c r="L16" t="str">
-        <f t="shared" si="3"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="M16" t="str">
-        <f t="shared" si="4"/>
-        <v>0031 707B</v>
-      </c>
-      <c r="N16" t="str">
-        <f t="shared" si="5"/>
-        <v>0034 807B</v>
-      </c>
-      <c r="O16" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P16" t="str">
-        <f t="shared" si="7"/>
-        <v>0000 0000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="I17" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0111</v>
-      </c>
-      <c r="J17" t="str">
-        <f t="shared" si="1"/>
-        <v>0030 0100</v>
-      </c>
-      <c r="K17" t="str">
-        <f t="shared" si="2"/>
-        <v>0001 0103</v>
-      </c>
-      <c r="L17" t="str">
-        <f t="shared" si="3"/>
-        <v>0001 E660</v>
-      </c>
-      <c r="M17" t="str">
-        <f t="shared" si="4"/>
-        <v>0034 807B</v>
-      </c>
-      <c r="N17" t="str">
-        <f t="shared" si="5"/>
-        <v>0035 447B</v>
-      </c>
-      <c r="O17" t="str">
-        <f t="shared" si="6"/>
-        <v>0035 693B</v>
-      </c>
-      <c r="P17" t="str">
-        <f t="shared" si="7"/>
-        <v>0211 0000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="I18" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0111</v>
-      </c>
-      <c r="J18" t="str">
-        <f t="shared" si="1"/>
-        <v>00C0 0030</v>
-      </c>
-      <c r="K18" t="str">
-        <f t="shared" si="2"/>
-        <v>0001 0101</v>
-      </c>
-      <c r="L18" t="str">
-        <f t="shared" si="3"/>
-        <v>0002 1690</v>
-      </c>
-      <c r="M18" t="str">
-        <f t="shared" si="4"/>
-        <v>0035 447B</v>
-      </c>
-      <c r="N18" t="str">
-        <f t="shared" si="5"/>
-        <v>0035 936B</v>
-      </c>
-      <c r="O18" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P18" t="str">
-        <f t="shared" si="7"/>
-        <v>0000 0000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="I19" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0312</v>
-      </c>
-      <c r="J19" t="str">
-        <f t="shared" si="1"/>
-        <v>00C0 0030</v>
-      </c>
-      <c r="K19" t="str">
-        <f t="shared" si="2"/>
-        <v>0003 0901</v>
-      </c>
-      <c r="L19" t="str">
-        <f t="shared" si="3"/>
-        <v>0002 3B50</v>
-      </c>
-      <c r="M19" t="str">
-        <f t="shared" si="4"/>
-        <v>0035 693B</v>
-      </c>
-      <c r="N19" t="str">
-        <f t="shared" si="5"/>
-        <v>0036 266B</v>
-      </c>
-      <c r="O19" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P19" t="str">
-        <f t="shared" si="7"/>
-        <v>0000 0000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="I20" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0111</v>
-      </c>
-      <c r="J20" t="str">
-        <f t="shared" si="1"/>
-        <v>0030 0180</v>
-      </c>
-      <c r="K20" t="str">
-        <f t="shared" si="2"/>
-        <v>0001 0103</v>
-      </c>
-      <c r="L20" t="str">
-        <f t="shared" si="3"/>
-        <v>0003 8010</v>
-      </c>
-      <c r="M20" t="str">
-        <f t="shared" si="4"/>
-        <v>0035 936B</v>
-      </c>
-      <c r="N20" t="str">
-        <f t="shared" si="5"/>
-        <v>0036 B96B</v>
-      </c>
-      <c r="O20" t="str">
-        <f t="shared" si="6"/>
-        <v>0036 DE2B</v>
-      </c>
-      <c r="P20" t="str">
-        <f t="shared" si="7"/>
-        <v>0211 0000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="I21" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0111</v>
-      </c>
-      <c r="J21" t="str">
-        <f t="shared" si="1"/>
-        <v>00C0 0030</v>
-      </c>
-      <c r="K21" t="str">
-        <f t="shared" si="2"/>
-        <v>0001 0101</v>
-      </c>
-      <c r="L21" t="str">
-        <f t="shared" si="3"/>
-        <v>0003 C840</v>
-      </c>
-      <c r="M21" t="str">
-        <f t="shared" si="4"/>
-        <v>0036 B96B</v>
-      </c>
-      <c r="N21" t="str">
-        <f t="shared" si="5"/>
-        <v>0037 085B</v>
-      </c>
-      <c r="O21" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P21" t="str">
-        <f t="shared" si="7"/>
-        <v>0000 0000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="I22" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0312</v>
-      </c>
-      <c r="J22" t="str">
-        <f t="shared" si="1"/>
-        <v>00C0 0030</v>
-      </c>
-      <c r="K22" t="str">
-        <f t="shared" si="2"/>
-        <v>0003 0901</v>
-      </c>
-      <c r="L22" t="str">
-        <f t="shared" si="3"/>
-        <v>0003 ED00</v>
-      </c>
-      <c r="M22" t="str">
-        <f t="shared" si="4"/>
-        <v>0036 DE2B</v>
-      </c>
-      <c r="N22" t="str">
-        <f t="shared" si="5"/>
-        <v>0037 9B5B</v>
-      </c>
-      <c r="O22" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P22" t="str">
-        <f t="shared" si="7"/>
-        <v>0000 0000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="I23" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0111</v>
-      </c>
-      <c r="J23" t="str">
-        <f t="shared" si="1"/>
-        <v>0040 0180</v>
-      </c>
-      <c r="K23" t="str">
-        <f t="shared" si="2"/>
-        <v>0001 0103</v>
-      </c>
-      <c r="L23" t="str">
-        <f t="shared" si="3"/>
-        <v>0005 31C0</v>
-      </c>
-      <c r="M23" t="str">
-        <f t="shared" si="4"/>
-        <v>0037 085B</v>
-      </c>
-      <c r="N23" t="str">
-        <f t="shared" si="5"/>
-        <v>0038 2E5B</v>
-      </c>
-      <c r="O23" t="str">
-        <f t="shared" si="6"/>
-        <v>0038 5F5B</v>
-      </c>
-      <c r="P23" t="str">
-        <f t="shared" si="7"/>
-        <v>0211 0000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="I24" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0111</v>
-      </c>
-      <c r="J24" t="str">
-        <f t="shared" si="1"/>
-        <v>0100 0040</v>
-      </c>
-      <c r="K24" t="str">
-        <f t="shared" si="2"/>
-        <v>0001 0101</v>
-      </c>
-      <c r="L24" t="str">
-        <f t="shared" si="3"/>
-        <v>0005 9200</v>
-      </c>
-      <c r="M24" t="str">
-        <f t="shared" si="4"/>
-        <v>0038 2E5B</v>
-      </c>
-      <c r="N24" t="str">
-        <f t="shared" si="5"/>
-        <v>0038 979B</v>
-      </c>
-      <c r="O24" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P24" t="str">
-        <f t="shared" si="7"/>
-        <v>0000 0000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="I25" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0312</v>
-      </c>
-      <c r="J25" t="str">
-        <f t="shared" si="1"/>
-        <v>0100 0040</v>
-      </c>
-      <c r="K25" t="str">
-        <f t="shared" si="2"/>
-        <v>0003 0901</v>
-      </c>
-      <c r="L25" t="str">
-        <f t="shared" si="3"/>
-        <v>0005 D300</v>
-      </c>
-      <c r="M25" t="str">
-        <f t="shared" si="4"/>
-        <v>0038 5F5B</v>
-      </c>
-      <c r="N25" t="str">
-        <f t="shared" si="5"/>
-        <v>0039 5B9B</v>
-      </c>
-      <c r="O25" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P25" t="str">
-        <f t="shared" si="7"/>
-        <v>0000 0000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="H26" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="I26" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0111</v>
-      </c>
-      <c r="J26" t="str">
-        <f t="shared" si="1"/>
-        <v>0040 0200</v>
-      </c>
-      <c r="K26" t="str">
-        <f t="shared" si="2"/>
-        <v>0001 0103</v>
-      </c>
-      <c r="L26" t="str">
-        <f t="shared" si="3"/>
-        <v>0008 1400</v>
-      </c>
-      <c r="M26" t="str">
-        <f t="shared" si="4"/>
-        <v>0039 5B9B</v>
-      </c>
-      <c r="N26" t="str">
-        <f t="shared" si="5"/>
-        <v>003A 1F9B</v>
-      </c>
-      <c r="O26" t="str">
-        <f t="shared" si="6"/>
-        <v>003A 509B</v>
-      </c>
-      <c r="P26" t="str">
-        <f t="shared" si="7"/>
-        <v>0211 0000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="I27" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0111</v>
-      </c>
-      <c r="J27" t="str">
-        <f t="shared" si="1"/>
-        <v>0100 0040</v>
-      </c>
-      <c r="K27" t="str">
-        <f t="shared" si="2"/>
-        <v>0001 0101</v>
-      </c>
-      <c r="L27" t="str">
-        <f t="shared" si="3"/>
-        <v>0008 9440</v>
-      </c>
-      <c r="M27" t="str">
-        <f t="shared" si="4"/>
-        <v>003A 1F9B</v>
-      </c>
-      <c r="N27" t="str">
-        <f t="shared" si="5"/>
-        <v>003A 88DB</v>
-      </c>
-      <c r="O27" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P27" t="str">
-        <f t="shared" si="7"/>
-        <v>0000 0000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H28" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="I28" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0312</v>
-      </c>
-      <c r="J28" t="str">
-        <f t="shared" si="1"/>
-        <v>0100 0040</v>
-      </c>
-      <c r="K28" t="str">
-        <f t="shared" si="2"/>
-        <v>0003 0901</v>
-      </c>
-      <c r="L28" t="str">
-        <f t="shared" si="3"/>
-        <v>0008 D540</v>
-      </c>
-      <c r="M28" t="str">
-        <f t="shared" si="4"/>
-        <v>003A 509B</v>
-      </c>
-      <c r="N28" t="str">
-        <f t="shared" si="5"/>
-        <v>003B 4CDB</v>
-      </c>
-      <c r="O28" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P28" t="str">
-        <f t="shared" si="7"/>
-        <v>0000 0000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H29" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="I29" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0111</v>
-      </c>
-      <c r="J29" t="str">
-        <f t="shared" si="1"/>
-        <v>03E8 0200</v>
-      </c>
-      <c r="K29" t="str">
-        <f t="shared" si="2"/>
-        <v>0001 0101</v>
-      </c>
-      <c r="L29" t="str">
-        <f t="shared" si="3"/>
-        <v>000B 1640</v>
-      </c>
-      <c r="M29" t="str">
-        <f t="shared" si="4"/>
-        <v>003A 88DB</v>
-      </c>
-      <c r="N29" t="str">
-        <f t="shared" si="5"/>
-        <v>003C 10DB</v>
-      </c>
-      <c r="O29" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P29" t="str">
-        <f t="shared" si="7"/>
-        <v>0000 0000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="H30" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="I30" t="str">
-        <f t="shared" si="0"/>
-        <v>010E 0E15</v>
-      </c>
-      <c r="J30" t="str">
-        <f t="shared" si="1"/>
-        <v>03E8 03E8</v>
-      </c>
-      <c r="K30" t="str">
-        <f t="shared" si="2"/>
-        <v>000E C401</v>
-      </c>
-      <c r="L30" t="str">
-        <f t="shared" si="3"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="M30" t="str">
-        <f t="shared" si="4"/>
-        <v>003C 10DB</v>
-      </c>
-      <c r="N30" t="str">
-        <f t="shared" si="5"/>
-        <v>003F 0E7B</v>
-      </c>
-      <c r="O30" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
       <c r="P30" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0000 0000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update some issues related to run
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0BD1AC-34F1-4238-8E22-9A64E9275559}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06378805-EFCE-4ADE-94DB-5ACE81C79A7C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
@@ -1313,8 +1313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80B23C6-EAEB-43B1-B045-456C36085CFA}">
   <dimension ref="A1:AL71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y68" sqref="Y68"/>
+    <sheetView tabSelected="1" topLeftCell="H36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1574,7 +1574,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2">
         <v>3</v>
@@ -1619,7 +1619,7 @@
       </c>
       <c r="Q4" s="6" t="str">
         <f>DEC2HEX(J4,2)&amp;DEC2HEX(G4,2)&amp;"_"&amp;DEC2HEX(D4,2)&amp;DEC2HEX(H4,1)&amp;DEC2HEX(C4,1)</f>
-        <v>71E3_0322</v>
+        <v>71E3_0321</v>
       </c>
       <c r="R4" s="2" t="str">
         <f>DEC2HEX(F4,4)&amp;"_"&amp;DEC2HEX(E4,4)</f>
@@ -1751,7 +1751,7 @@
         <v>71</v>
       </c>
       <c r="C6" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D6" s="4">
         <v>3</v>
@@ -1787,7 +1787,7 @@
       <c r="P6" s="4"/>
       <c r="Q6" s="8" t="str">
         <f>DEC2HEX(J6,2)&amp;DEC2HEX(G6,2)&amp;"_"&amp;DEC2HEX(D6,2)&amp;DEC2HEX(H6,1)&amp;DEC2HEX(C6,1)</f>
-        <v>3871_0324</v>
+        <v>3871_0322</v>
       </c>
       <c r="R6" s="4" t="str">
         <f>DEC2HEX(F6,4)&amp;"_"&amp;DEC2HEX(F6,4)</f>
@@ -2192,7 +2192,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2">
         <v>3</v>
@@ -2237,7 +2237,7 @@
       </c>
       <c r="Q10" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>3838_0312</v>
+        <v>3838_0311</v>
       </c>
       <c r="R10" s="2" t="str">
         <f>DEC2HEX(F10,4)&amp;"_"&amp;DEC2HEX(E10,4)</f>
@@ -2783,7 +2783,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2">
         <v>3</v>
@@ -2828,7 +2828,7 @@
       </c>
       <c r="Q17" s="6" t="str">
         <f t="shared" si="8"/>
-        <v>3838_0312</v>
+        <v>3838_0311</v>
       </c>
       <c r="R17" s="2" t="str">
         <f>DEC2HEX(F17,4)&amp;"_"&amp;DEC2HEX(E17,4)</f>
@@ -3055,7 +3055,7 @@
         <v>71</v>
       </c>
       <c r="C21" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D21" s="4">
         <v>3</v>
@@ -3091,7 +3091,7 @@
       <c r="P21" s="4"/>
       <c r="Q21" s="8" t="str">
         <f>DEC2HEX(J21,2)&amp;DEC2HEX(G21,2)&amp;"_"&amp;DEC2HEX(D21,2)&amp;DEC2HEX(H21,1)&amp;DEC2HEX(C21,1)</f>
-        <v>1C38_0324</v>
+        <v>1C38_0322</v>
       </c>
       <c r="R21" s="4" t="str">
         <f>DEC2HEX(F21,4)&amp;"_"&amp;DEC2HEX(F21,4)</f>
@@ -3496,7 +3496,7 @@
         <v>8</v>
       </c>
       <c r="C25" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" s="2">
         <v>3</v>
@@ -3541,7 +3541,7 @@
       </c>
       <c r="Q25" s="6" t="str">
         <f t="shared" si="15"/>
-        <v>1C1C_0312</v>
+        <v>1C1C_0311</v>
       </c>
       <c r="R25" s="2" t="str">
         <f>DEC2HEX(F25,4)&amp;"_"&amp;DEC2HEX(E25,4)</f>
@@ -4087,7 +4087,7 @@
         <v>8</v>
       </c>
       <c r="C32" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D32" s="2">
         <v>3</v>
@@ -4132,7 +4132,7 @@
       </c>
       <c r="Q32" s="6" t="str">
         <f t="shared" si="21"/>
-        <v>1C1C_0312</v>
+        <v>1C1C_0311</v>
       </c>
       <c r="R32" s="2" t="str">
         <f>DEC2HEX(F32,4)&amp;"_"&amp;DEC2HEX(E32,4)</f>
@@ -4359,7 +4359,7 @@
         <v>71</v>
       </c>
       <c r="C36" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D36" s="4">
         <v>3</v>
@@ -4395,7 +4395,7 @@
       <c r="P36" s="4"/>
       <c r="Q36" s="8" t="str">
         <f>DEC2HEX(J36,2)&amp;DEC2HEX(G36,2)&amp;"_"&amp;DEC2HEX(D36,2)&amp;DEC2HEX(H36,1)&amp;DEC2HEX(C36,1)</f>
-        <v>0E1C_0324</v>
+        <v>0E1C_0322</v>
       </c>
       <c r="R36" s="4" t="str">
         <f>DEC2HEX(F36,4)&amp;"_"&amp;DEC2HEX(F36,4)</f>
@@ -4800,7 +4800,7 @@
         <v>8</v>
       </c>
       <c r="C40" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D40" s="2">
         <v>3</v>
@@ -4845,7 +4845,7 @@
       </c>
       <c r="Q40" s="6" t="str">
         <f t="shared" si="28"/>
-        <v>0E0E_0312</v>
+        <v>0E0E_0311</v>
       </c>
       <c r="R40" s="2" t="str">
         <f>DEC2HEX(F40,4)&amp;"_"&amp;DEC2HEX(E40,4)</f>
@@ -5391,7 +5391,7 @@
         <v>8</v>
       </c>
       <c r="C47" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D47" s="2">
         <v>3</v>
@@ -5436,7 +5436,7 @@
       </c>
       <c r="Q47" s="6" t="str">
         <f t="shared" si="34"/>
-        <v>0E0E_0312</v>
+        <v>0E0E_0311</v>
       </c>
       <c r="R47" s="2" t="str">
         <f>DEC2HEX(F47,4)&amp;"_"&amp;DEC2HEX(E47,4)</f>
@@ -5982,7 +5982,7 @@
         <v>8</v>
       </c>
       <c r="C54" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D54" s="2">
         <v>3</v>
@@ -6027,7 +6027,7 @@
       </c>
       <c r="Q54" s="6" t="str">
         <f t="shared" si="40"/>
-        <v>0E0E_0312</v>
+        <v>0E0E_0311</v>
       </c>
       <c r="R54" s="2" t="str">
         <f>DEC2HEX(F54,4)&amp;"_"&amp;DEC2HEX(E54,4)</f>
@@ -6573,7 +6573,7 @@
         <v>8</v>
       </c>
       <c r="C61" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D61" s="2">
         <v>3</v>
@@ -6618,7 +6618,7 @@
       </c>
       <c r="Q61" s="6" t="str">
         <f t="shared" si="46"/>
-        <v>0E0E_0312</v>
+        <v>0E0E_0311</v>
       </c>
       <c r="R61" s="2" t="str">
         <f>DEC2HEX(F61,4)&amp;"_"&amp;DEC2HEX(E61,4)</f>
@@ -7067,7 +7067,7 @@
         <v>72</v>
       </c>
       <c r="C68" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D68" s="4">
         <v>14</v>
@@ -7103,7 +7103,7 @@
       <c r="P68" s="4"/>
       <c r="Q68" s="8" t="str">
         <f>DEC2HEX(J68,2)&amp;DEC2HEX(G68,2)&amp;"_"&amp;DEC2HEX(D68,2)&amp;DEC2HEX(H68,1)&amp;DEC2HEX(C68,1)</f>
-        <v>010E_0E15</v>
+        <v>010E_0E13</v>
       </c>
       <c r="R68" s="4" t="str">
         <f>DEC2HEX(F68,4)&amp;"_"&amp;DEC2HEX(F68,4)</f>

</xml_diff>

<commit_message>
Fix typos and endians
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06378805-EFCE-4ADE-94DB-5ACE81C79A7C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0EDA27-467F-4C3D-9C18-EADD3A3580C4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
   <sheets>
     <sheet name="SqueezeNet v2 MEC Parallel Ch" sheetId="2" r:id="rId1"/>
@@ -472,48 +472,24 @@
     <t>0000_0000</t>
   </si>
   <si>
-    <t>71E3_0322</t>
-  </si>
-  <si>
-    <t>3871_0324</t>
-  </si>
-  <si>
     <t>3838_0111</t>
   </si>
   <si>
     <t>023B_0000</t>
   </si>
   <si>
-    <t>3838_0312</t>
-  </si>
-  <si>
-    <t>1C38_0324</t>
-  </si>
-  <si>
     <t>1C1C_0111</t>
   </si>
   <si>
     <t>021F_0000</t>
   </si>
   <si>
-    <t>1C1C_0312</t>
-  </si>
-  <si>
-    <t>0E1C_0324</t>
-  </si>
-  <si>
     <t>0E0E_0111</t>
   </si>
   <si>
     <t>0211_0000</t>
   </si>
   <si>
-    <t>0E0E_0312</t>
-  </si>
-  <si>
-    <t>010E_0E15</t>
-  </si>
-  <si>
     <t>p0_result staddr</t>
   </si>
   <si>
@@ -728,6 +704,30 @@
   </si>
   <si>
     <t>0058FCE8</t>
+  </si>
+  <si>
+    <t>71E3_0321</t>
+  </si>
+  <si>
+    <t>3871_0322</t>
+  </si>
+  <si>
+    <t>3838_0311</t>
+  </si>
+  <si>
+    <t>1C38_0322</t>
+  </si>
+  <si>
+    <t>1C1C_0311</t>
+  </si>
+  <si>
+    <t>0E1C_0322</t>
+  </si>
+  <si>
+    <t>0E0E_0311</t>
+  </si>
+  <si>
+    <t>010E_0E13</t>
   </si>
 </sst>
 </file>
@@ -1313,8 +1313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80B23C6-EAEB-43B1-B045-456C36085CFA}">
   <dimension ref="A1:AL71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1459,7 +1459,7 @@
         <v>121</v>
       </c>
       <c r="S2" s="14" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="T2" s="38" t="s">
         <v>82</v>
@@ -1470,11 +1470,11 @@
       </c>
       <c r="W2" s="38"/>
       <c r="X2" s="38" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="Y2" s="38"/>
       <c r="Z2" s="38" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="AA2" s="38"/>
       <c r="AB2" s="28" t="s">
@@ -7368,7 +7368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E501AE-4D2D-491C-85E4-0C34FDA03C89}">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView zoomScale="76" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
       <selection activeCell="I1" sqref="I1:P30"/>
     </sheetView>
   </sheetViews>
@@ -7383,22 +7383,22 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>145</v>
+        <v>223</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>83</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>116</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>117</v>
@@ -7407,56 +7407,56 @@
         <v>144</v>
       </c>
       <c r="I1" t="str">
-        <f t="shared" ref="I1:I30" si="0">LEFT(SUBSTITUTE(A1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(A1,"_",),4)</f>
-        <v>71E3 0322</v>
+        <f>RIGHT(SUBSTITUTE(A1,"_",),2)&amp;MID(SUBSTITUTE(A1,"_",),5,2)&amp;" "&amp;MID(SUBSTITUTE(A1,"_",),3,2)&amp;LEFT(SUBSTITUTE(A1,"_",),2)</f>
+        <v>2103 E371</v>
       </c>
       <c r="J1" t="str">
-        <f t="shared" ref="J1:J30" si="1">LEFT(SUBSTITUTE(B1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(B1,"_",),4)</f>
-        <v>0040 0003</v>
+        <f t="shared" ref="J1:P16" si="0">RIGHT(SUBSTITUTE(B1,"_",),2)&amp;MID(SUBSTITUTE(B1,"_",),5,2)&amp;" "&amp;MID(SUBSTITUTE(B1,"_",),3,2)&amp;LEFT(SUBSTITUTE(B1,"_",),2)</f>
+        <v>0300 4000</v>
       </c>
       <c r="K1" t="str">
-        <f t="shared" ref="K1:K30" si="2">LEFT(SUBSTITUTE(C1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(C1,"_",),4)</f>
-        <v>0006 0901</v>
+        <f t="shared" si="0"/>
+        <v>0109 0600</v>
       </c>
       <c r="L1" t="str">
-        <f t="shared" ref="L1:L30" si="3">LEFT(SUBSTITUTE(D1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(D1,"_",),4)</f>
-        <v>0000 1000</v>
+        <f t="shared" si="0"/>
+        <v>0010 0000</v>
       </c>
       <c r="M1" t="str">
-        <f t="shared" ref="M1:M30" si="4">LEFT(SUBSTITUTE(E1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(E1,"_",),4)</f>
-        <v>0020 0000</v>
+        <f t="shared" si="0"/>
+        <v>0000 2000</v>
       </c>
       <c r="N1" t="str">
-        <f t="shared" ref="N1:N30" si="5">LEFT(SUBSTITUTE(F1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(F1,"_",),4)</f>
-        <v>0026 4A48</v>
+        <f t="shared" si="0"/>
+        <v>484A 2600</v>
       </c>
       <c r="O1" t="str">
-        <f t="shared" ref="O1:O30" si="6">LEFT(SUBSTITUTE(G1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(G1,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0000 0000</v>
       </c>
       <c r="P1" t="str">
-        <f t="shared" ref="P1:P30" si="7">LEFT(SUBSTITUTE(H1,"_",),4)&amp;" "&amp;RIGHT(SUBSTITUTE(H1,"_",),4)</f>
+        <f t="shared" si="0"/>
         <v>0000 0000</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>146</v>
+        <v>224</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>117</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>117</v>
@@ -7465,1659 +7465,1659 @@
         <v>144</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" si="0"/>
-        <v>3871 0324</v>
+        <f t="shared" ref="I2:I30" si="1">RIGHT(SUBSTITUTE(A2,"_",),2)&amp;MID(SUBSTITUTE(A2,"_",),5,2)&amp;" "&amp;MID(SUBSTITUTE(A2,"_",),3,2)&amp;LEFT(SUBSTITUTE(A2,"_",),2)</f>
+        <v>2203 7138</v>
       </c>
       <c r="J2" t="str">
+        <f t="shared" si="0"/>
+        <v>4000 4000</v>
+      </c>
+      <c r="K2" t="str">
+        <f t="shared" si="0"/>
+        <v>0109 0600</v>
+      </c>
+      <c r="L2" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="M2" t="str">
+        <f t="shared" si="0"/>
+        <v>484A 2600</v>
+      </c>
+      <c r="N2" t="str">
+        <f t="shared" si="0"/>
+        <v>88C2 3200</v>
+      </c>
+      <c r="O2" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="P2" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="I3" t="str">
         <f t="shared" si="1"/>
-        <v>0040 0040</v>
-      </c>
-      <c r="K2" t="str">
+        <v>1101 3838</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" si="0"/>
+        <v>4000 1000</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" si="0"/>
+        <v>0301 0100</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" si="0"/>
+        <v>4022 0000</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" si="0"/>
+        <v>88C2 3200</v>
+      </c>
+      <c r="N3" t="str">
+        <f t="shared" si="0"/>
+        <v>88D2 3500</v>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" si="0"/>
+        <v>8896 3600</v>
+      </c>
+      <c r="P3" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 3B02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="1"/>
+        <v>1101 3838</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>1000 4000</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="0"/>
+        <v>0101 0100</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="0"/>
+        <v>5026 0000</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="0"/>
+        <v>88D2 3500</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" si="0"/>
+        <v>9861 3700</v>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="P4" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="1"/>
+        <v>1103 3838</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>1000 4000</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v>0109 0300</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="0"/>
+        <v>902A 0000</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="0"/>
+        <v>8896 3600</v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" si="0"/>
+        <v>9871 3A00</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="P5" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="1"/>
+        <v>1101 3838</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>8000 1000</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v>0301 0100</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="0"/>
+        <v>D04E 0000</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="0"/>
+        <v>9861 3700</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="0"/>
+        <v>9881 3D00</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="0"/>
+        <v>9845 3E00</v>
+      </c>
+      <c r="P6" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 3B02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="1"/>
+        <v>1101 3838</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>1000 4000</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>0101 0100</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="0"/>
+        <v>E056 0000</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="0"/>
+        <v>9881 3D00</v>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" si="0"/>
+        <v>A810 3F00</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="1"/>
+        <v>1103 3838</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>1000 4000</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v>0109 0300</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="0"/>
+        <v>205B 0000</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="0"/>
+        <v>9845 3E00</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="0"/>
+        <v>A820 4200</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="1"/>
+        <v>2203 381C</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>8000 8000</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v>0109 0600</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="0"/>
+        <v>A810 3F00</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="0"/>
+        <v>A830 4500</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="1"/>
+        <v>1101 1C1C</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>8000 2000</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v>0301 0100</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="0"/>
+        <v>607F 0000</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="0"/>
+        <v>A830 4500</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" si="0"/>
+        <v>A8B8 4600</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="0"/>
+        <v>A81A 4700</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 1F02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="1"/>
+        <v>1101 1C1C</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="0"/>
+        <v>2000 8000</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v>0101 0100</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="0"/>
+        <v>808F 0000</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="0"/>
+        <v>A8B8 4600</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="0"/>
+        <v>C883 4700</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="1"/>
+        <v>1103 1C1C</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="0"/>
+        <v>2000 8000</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v>0109 0300</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="0"/>
+        <v>00A0 0000</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="0"/>
+        <v>A81A 4700</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="0"/>
+        <v>C80B 4900</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="1"/>
+        <v>1101 1C1C</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="0"/>
+        <v>0001 2000</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v>0301 0100</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="0"/>
+        <v>8030 0100</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="0"/>
+        <v>C883 4700</v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" si="0"/>
+        <v>C893 4A00</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="0"/>
+        <v>C8F5 4A00</v>
+      </c>
+      <c r="P13" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 1F02</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="1"/>
+        <v>1101 1C1C</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="0"/>
+        <v>2000 8000</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="0"/>
+        <v>0101 0100</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="0"/>
+        <v>A050 0100</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="0"/>
+        <v>C893 4A00</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="0"/>
+        <v>E85E 4B00</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="P14" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="1"/>
+        <v>1103 1C1C</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="0"/>
+        <v>2000 8000</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="0"/>
+        <v>0109 0300</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="0"/>
+        <v>2061 0100</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="0"/>
+        <v>C8F5 4A00</v>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" si="0"/>
+        <v>E8E6 4C00</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="P15" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="1"/>
+        <v>2203 1C0E</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="0"/>
+        <v>0001 0001</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="0"/>
+        <v>0109 0600</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="0"/>
+        <v>E85E 4B00</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" si="0"/>
+        <v>E86E 4E00</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+      <c r="P16" t="str">
+        <f t="shared" si="0"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="1"/>
+        <v>1101 0E0E</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" ref="J17:J30" si="2">RIGHT(SUBSTITUTE(B17,"_",),2)&amp;MID(SUBSTITUTE(B17,"_",),5,2)&amp;" "&amp;MID(SUBSTITUTE(B17,"_",),3,2)&amp;LEFT(SUBSTITUTE(B17,"_",),2)</f>
+        <v>0001 3000</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" ref="K17:K30" si="3">RIGHT(SUBSTITUTE(C17,"_",),2)&amp;MID(SUBSTITUTE(C17,"_",),5,2)&amp;" "&amp;MID(SUBSTITUTE(C17,"_",),3,2)&amp;LEFT(SUBSTITUTE(C17,"_",),2)</f>
+        <v>0301 0100</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" ref="L17:L30" si="4">RIGHT(SUBSTITUTE(D17,"_",),2)&amp;MID(SUBSTITUTE(D17,"_",),5,2)&amp;" "&amp;MID(SUBSTITUTE(D17,"_",),3,2)&amp;LEFT(SUBSTITUTE(D17,"_",),2)</f>
+        <v>A0F1 0100</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" ref="M17:M30" si="5">RIGHT(SUBSTITUTE(E17,"_",),2)&amp;MID(SUBSTITUTE(E17,"_",),5,2)&amp;" "&amp;MID(SUBSTITUTE(E17,"_",),3,2)&amp;LEFT(SUBSTITUTE(E17,"_",),2)</f>
+        <v>E86E 4E00</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" ref="N17:N30" si="6">RIGHT(SUBSTITUTE(F17,"_",),2)&amp;MID(SUBSTITUTE(F17,"_",),5,2)&amp;" "&amp;MID(SUBSTITUTE(F17,"_",),3,2)&amp;LEFT(SUBSTITUTE(F17,"_",),2)</f>
+        <v>E832 4F00</v>
+      </c>
+      <c r="O17" t="str">
+        <f t="shared" ref="O17:O30" si="7">RIGHT(SUBSTITUTE(G17,"_",),2)&amp;MID(SUBSTITUTE(G17,"_",),5,2)&amp;" "&amp;MID(SUBSTITUTE(G17,"_",),3,2)&amp;LEFT(SUBSTITUTE(G17,"_",),2)</f>
+        <v>A857 4F00</v>
+      </c>
+      <c r="P17" t="str">
+        <f t="shared" ref="P17:P30" si="8">RIGHT(SUBSTITUTE(H17,"_",),2)&amp;MID(SUBSTITUTE(H17,"_",),5,2)&amp;" "&amp;MID(SUBSTITUTE(H17,"_",),3,2)&amp;LEFT(SUBSTITUTE(H17,"_",),2)</f>
+        <v>0000 1102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="1"/>
+        <v>1101 0E0E</v>
+      </c>
+      <c r="J18" t="str">
         <f t="shared" si="2"/>
-        <v>0006 0901</v>
-      </c>
-      <c r="L2" t="str">
+        <v>3000 C000</v>
+      </c>
+      <c r="K18" t="str">
         <f t="shared" si="3"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="M2" t="str">
+        <v>0101 0100</v>
+      </c>
+      <c r="L18" t="str">
         <f t="shared" si="4"/>
-        <v>0026 4A48</v>
-      </c>
-      <c r="N2" t="str">
+        <v>D021 0200</v>
+      </c>
+      <c r="M18" t="str">
         <f t="shared" si="5"/>
-        <v>0032 C288</v>
-      </c>
-      <c r="O2" t="str">
+        <v>E832 4F00</v>
+      </c>
+      <c r="N18" t="str">
         <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P2" t="str">
+        <v>D881 4F00</v>
+      </c>
+      <c r="O18" t="str">
         <f t="shared" si="7"/>
         <v>0000 0000</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="I3" t="str">
-        <f t="shared" si="0"/>
-        <v>3838 0111</v>
-      </c>
-      <c r="J3" t="str">
+      <c r="P18" t="str">
+        <f t="shared" si="8"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I19" t="str">
         <f t="shared" si="1"/>
-        <v>0010 0040</v>
-      </c>
-      <c r="K3" t="str">
+        <v>1103 0E0E</v>
+      </c>
+      <c r="J19" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0103</v>
-      </c>
-      <c r="L3" t="str">
+        <v>3000 C000</v>
+      </c>
+      <c r="K19" t="str">
         <f t="shared" si="3"/>
-        <v>0000 2240</v>
-      </c>
-      <c r="M3" t="str">
+        <v>0109 0300</v>
+      </c>
+      <c r="L19" t="str">
         <f t="shared" si="4"/>
-        <v>0032 C288</v>
-      </c>
-      <c r="N3" t="str">
+        <v>9046 0200</v>
+      </c>
+      <c r="M19" t="str">
         <f t="shared" si="5"/>
-        <v>0035 D288</v>
-      </c>
-      <c r="O3" t="str">
+        <v>A857 4F00</v>
+      </c>
+      <c r="N19" t="str">
         <f t="shared" si="6"/>
-        <v>0036 9688</v>
-      </c>
-      <c r="P3" t="str">
-        <f t="shared" si="7"/>
-        <v>023B 0000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="I4" t="str">
-        <f t="shared" si="0"/>
-        <v>3838 0111</v>
-      </c>
-      <c r="J4" t="str">
-        <f t="shared" si="1"/>
-        <v>0040 0010</v>
-      </c>
-      <c r="K4" t="str">
-        <f t="shared" si="2"/>
-        <v>0001 0101</v>
-      </c>
-      <c r="L4" t="str">
-        <f t="shared" si="3"/>
-        <v>0000 2650</v>
-      </c>
-      <c r="M4" t="str">
-        <f t="shared" si="4"/>
-        <v>0035 D288</v>
-      </c>
-      <c r="N4" t="str">
-        <f t="shared" si="5"/>
-        <v>0037 6198</v>
-      </c>
-      <c r="O4" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P4" t="str">
+        <v>D814 5000</v>
+      </c>
+      <c r="O19" t="str">
         <f t="shared" si="7"/>
         <v>0000 0000</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="P19" t="str">
+        <f t="shared" si="8"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="G5" s="2" t="s">
+      <c r="B20" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="1"/>
+        <v>1101 0E0E</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="2"/>
+        <v>8001 3000</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="3"/>
+        <v>0301 0100</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="4"/>
+        <v>508B 0300</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="5"/>
+        <v>D881 4F00</v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" si="6"/>
+        <v>D8A7 5000</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="7"/>
+        <v>98CC 5000</v>
+      </c>
+      <c r="P20" t="str">
+        <f t="shared" si="8"/>
+        <v>0000 1102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H21" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="I5" t="str">
-        <f t="shared" si="0"/>
-        <v>3838 0312</v>
-      </c>
-      <c r="J5" t="str">
+      <c r="I21" t="str">
         <f t="shared" si="1"/>
-        <v>0040 0010</v>
-      </c>
-      <c r="K5" t="str">
+        <v>1101 0E0E</v>
+      </c>
+      <c r="J21" t="str">
         <f t="shared" si="2"/>
-        <v>0003 0901</v>
-      </c>
-      <c r="L5" t="str">
+        <v>3000 C000</v>
+      </c>
+      <c r="K21" t="str">
         <f t="shared" si="3"/>
-        <v>0000 2A90</v>
-      </c>
-      <c r="M5" t="str">
+        <v>0101 0100</v>
+      </c>
+      <c r="L21" t="str">
         <f t="shared" si="4"/>
-        <v>0036 9688</v>
-      </c>
-      <c r="N5" t="str">
+        <v>80D3 0300</v>
+      </c>
+      <c r="M21" t="str">
         <f t="shared" si="5"/>
-        <v>003A 7198</v>
-      </c>
-      <c r="O5" t="str">
+        <v>D8A7 5000</v>
+      </c>
+      <c r="N21" t="str">
         <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P5" t="str">
+        <v>C8F6 5000</v>
+      </c>
+      <c r="O21" t="str">
         <f t="shared" si="7"/>
         <v>0000 0000</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="I6" t="str">
-        <f t="shared" si="0"/>
-        <v>3838 0111</v>
-      </c>
-      <c r="J6" t="str">
+      <c r="P21" t="str">
+        <f t="shared" si="8"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I22" t="str">
         <f t="shared" si="1"/>
-        <v>0010 0080</v>
-      </c>
-      <c r="K6" t="str">
+        <v>1103 0E0E</v>
+      </c>
+      <c r="J22" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0103</v>
-      </c>
-      <c r="L6" t="str">
+        <v>3000 C000</v>
+      </c>
+      <c r="K22" t="str">
         <f t="shared" si="3"/>
-        <v>0000 4ED0</v>
-      </c>
-      <c r="M6" t="str">
+        <v>0109 0300</v>
+      </c>
+      <c r="L22" t="str">
         <f t="shared" si="4"/>
-        <v>0037 6198</v>
-      </c>
-      <c r="N6" t="str">
+        <v>40F8 0300</v>
+      </c>
+      <c r="M22" t="str">
         <f t="shared" si="5"/>
-        <v>003D 8198</v>
-      </c>
-      <c r="O6" t="str">
+        <v>98CC 5000</v>
+      </c>
+      <c r="N22" t="str">
         <f t="shared" si="6"/>
-        <v>003E 4598</v>
-      </c>
-      <c r="P6" t="str">
-        <f t="shared" si="7"/>
-        <v>023B 0000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="I7" t="str">
-        <f t="shared" si="0"/>
-        <v>3838 0111</v>
-      </c>
-      <c r="J7" t="str">
-        <f t="shared" si="1"/>
-        <v>0040 0010</v>
-      </c>
-      <c r="K7" t="str">
-        <f t="shared" si="2"/>
-        <v>0001 0101</v>
-      </c>
-      <c r="L7" t="str">
-        <f t="shared" si="3"/>
-        <v>0000 56E0</v>
-      </c>
-      <c r="M7" t="str">
-        <f t="shared" si="4"/>
-        <v>003D 8198</v>
-      </c>
-      <c r="N7" t="str">
-        <f t="shared" si="5"/>
-        <v>003F 10A8</v>
-      </c>
-      <c r="O7" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P7" t="str">
+        <v>C889 5100</v>
+      </c>
+      <c r="O22" t="str">
         <f t="shared" si="7"/>
         <v>0000 0000</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="P22" t="str">
+        <f t="shared" si="8"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="G8" s="2" t="s">
+      <c r="B23" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="1"/>
+        <v>1101 0E0E</v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="2"/>
+        <v>8001 4000</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="3"/>
+        <v>0301 0100</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="4"/>
+        <v>003D 0500</v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" si="5"/>
+        <v>C8F6 5000</v>
+      </c>
+      <c r="N23" t="str">
+        <f t="shared" si="6"/>
+        <v>C81C 5200</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="7"/>
+        <v>C84D 5200</v>
+      </c>
+      <c r="P23" t="str">
+        <f t="shared" si="8"/>
+        <v>0000 1102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H24" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="I8" t="str">
-        <f t="shared" si="0"/>
-        <v>3838 0312</v>
-      </c>
-      <c r="J8" t="str">
+      <c r="I24" t="str">
         <f t="shared" si="1"/>
-        <v>0040 0010</v>
-      </c>
-      <c r="K8" t="str">
+        <v>1101 0E0E</v>
+      </c>
+      <c r="J24" t="str">
         <f t="shared" si="2"/>
-        <v>0003 0901</v>
-      </c>
-      <c r="L8" t="str">
+        <v>4000 0001</v>
+      </c>
+      <c r="K24" t="str">
         <f t="shared" si="3"/>
-        <v>0000 5B20</v>
-      </c>
-      <c r="M8" t="str">
+        <v>0101 0100</v>
+      </c>
+      <c r="L24" t="str">
         <f t="shared" si="4"/>
-        <v>003E 4598</v>
-      </c>
-      <c r="N8" t="str">
+        <v>409D 0500</v>
+      </c>
+      <c r="M24" t="str">
         <f t="shared" si="5"/>
-        <v>0042 20A8</v>
-      </c>
-      <c r="O8" t="str">
+        <v>C81C 5200</v>
+      </c>
+      <c r="N24" t="str">
         <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P8" t="str">
+        <v>0886 5200</v>
+      </c>
+      <c r="O24" t="str">
         <f t="shared" si="7"/>
         <v>0000 0000</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="P24" t="str">
+        <f t="shared" si="8"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="H9" s="13" t="s">
+      <c r="H25" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="I9" t="str">
-        <f t="shared" si="0"/>
-        <v>1C38 0324</v>
-      </c>
-      <c r="J9" t="str">
+      <c r="I25" t="str">
         <f t="shared" si="1"/>
-        <v>0080 0080</v>
-      </c>
-      <c r="K9" t="str">
+        <v>1103 0E0E</v>
+      </c>
+      <c r="J25" t="str">
         <f t="shared" si="2"/>
-        <v>0006 0901</v>
-      </c>
-      <c r="L9" t="str">
+        <v>4000 0001</v>
+      </c>
+      <c r="K25" t="str">
         <f t="shared" si="3"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="M9" t="str">
+        <v>0109 0300</v>
+      </c>
+      <c r="L25" t="str">
         <f t="shared" si="4"/>
-        <v>003F 10A8</v>
-      </c>
-      <c r="N9" t="str">
+        <v>40DE 0500</v>
+      </c>
+      <c r="M25" t="str">
         <f t="shared" si="5"/>
-        <v>0045 30A8</v>
-      </c>
-      <c r="O9" t="str">
+        <v>C84D 5200</v>
+      </c>
+      <c r="N25" t="str">
         <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P9" t="str">
+        <v>084A 5300</v>
+      </c>
+      <c r="O25" t="str">
         <f t="shared" si="7"/>
         <v>0000 0000</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="I10" t="str">
-        <f t="shared" si="0"/>
-        <v>1C1C 0111</v>
-      </c>
-      <c r="J10" t="str">
+      <c r="P25" t="str">
+        <f t="shared" si="8"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="I26" t="str">
         <f t="shared" si="1"/>
-        <v>0020 0080</v>
-      </c>
-      <c r="K10" t="str">
+        <v>1101 0E0E</v>
+      </c>
+      <c r="J26" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0103</v>
-      </c>
-      <c r="L10" t="str">
+        <v>0002 4000</v>
+      </c>
+      <c r="K26" t="str">
         <f t="shared" si="3"/>
-        <v>0000 7F60</v>
-      </c>
-      <c r="M10" t="str">
+        <v>0301 0100</v>
+      </c>
+      <c r="L26" t="str">
         <f t="shared" si="4"/>
-        <v>0045 30A8</v>
-      </c>
-      <c r="N10" t="str">
+        <v>401F 0800</v>
+      </c>
+      <c r="M26" t="str">
         <f t="shared" si="5"/>
-        <v>0046 B8A8</v>
-      </c>
-      <c r="O10" t="str">
+        <v>084A 5300</v>
+      </c>
+      <c r="N26" t="str">
         <f t="shared" si="6"/>
-        <v>0047 1AA8</v>
-      </c>
-      <c r="P10" t="str">
+        <v>080E 5400</v>
+      </c>
+      <c r="O26" t="str">
         <f t="shared" si="7"/>
-        <v>021F 0000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="G11" s="2" t="s">
+        <v>083F 5400</v>
+      </c>
+      <c r="P26" t="str">
+        <f t="shared" si="8"/>
+        <v>0000 1102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H27" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="I11" t="str">
-        <f t="shared" si="0"/>
-        <v>1C1C 0111</v>
-      </c>
-      <c r="J11" t="str">
+      <c r="I27" t="str">
         <f t="shared" si="1"/>
-        <v>0080 0020</v>
-      </c>
-      <c r="K11" t="str">
+        <v>1101 0E0E</v>
+      </c>
+      <c r="J27" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0101</v>
-      </c>
-      <c r="L11" t="str">
+        <v>4000 0001</v>
+      </c>
+      <c r="K27" t="str">
         <f t="shared" si="3"/>
-        <v>0000 8F80</v>
-      </c>
-      <c r="M11" t="str">
+        <v>0101 0100</v>
+      </c>
+      <c r="L27" t="str">
         <f t="shared" si="4"/>
-        <v>0046 B8A8</v>
-      </c>
-      <c r="N11" t="str">
+        <v>809F 0800</v>
+      </c>
+      <c r="M27" t="str">
         <f t="shared" si="5"/>
-        <v>0047 83C8</v>
-      </c>
-      <c r="O11" t="str">
+        <v>080E 5400</v>
+      </c>
+      <c r="N27" t="str">
         <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P11" t="str">
+        <v>4877 5400</v>
+      </c>
+      <c r="O27" t="str">
         <f t="shared" si="7"/>
         <v>0000 0000</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="G12" s="2" t="s">
+      <c r="P27" t="str">
+        <f t="shared" si="8"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H28" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="I12" t="str">
-        <f t="shared" si="0"/>
-        <v>1C1C 0312</v>
-      </c>
-      <c r="J12" t="str">
+      <c r="I28" t="str">
         <f t="shared" si="1"/>
-        <v>0080 0020</v>
-      </c>
-      <c r="K12" t="str">
+        <v>1103 0E0E</v>
+      </c>
+      <c r="J28" t="str">
         <f t="shared" si="2"/>
-        <v>0003 0901</v>
-      </c>
-      <c r="L12" t="str">
+        <v>4000 0001</v>
+      </c>
+      <c r="K28" t="str">
         <f t="shared" si="3"/>
-        <v>0000 A000</v>
-      </c>
-      <c r="M12" t="str">
+        <v>0109 0300</v>
+      </c>
+      <c r="L28" t="str">
         <f t="shared" si="4"/>
-        <v>0047 1AA8</v>
-      </c>
-      <c r="N12" t="str">
+        <v>80E0 0800</v>
+      </c>
+      <c r="M28" t="str">
         <f t="shared" si="5"/>
-        <v>0049 0BC8</v>
-      </c>
-      <c r="O12" t="str">
+        <v>083F 5400</v>
+      </c>
+      <c r="N28" t="str">
         <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P12" t="str">
+        <v>483B 5500</v>
+      </c>
+      <c r="O28" t="str">
         <f t="shared" si="7"/>
         <v>0000 0000</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="I13" t="str">
-        <f t="shared" si="0"/>
-        <v>1C1C 0111</v>
-      </c>
-      <c r="J13" t="str">
+      <c r="P28" t="str">
+        <f t="shared" si="8"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I29" t="str">
         <f t="shared" si="1"/>
-        <v>0020 0100</v>
-      </c>
-      <c r="K13" t="str">
+        <v>1101 0E0E</v>
+      </c>
+      <c r="J29" t="str">
         <f t="shared" si="2"/>
-        <v>0001 0103</v>
-      </c>
-      <c r="L13" t="str">
+        <v>0002 E803</v>
+      </c>
+      <c r="K29" t="str">
         <f t="shared" si="3"/>
-        <v>0001 3080</v>
-      </c>
-      <c r="M13" t="str">
+        <v>0101 0100</v>
+      </c>
+      <c r="L29" t="str">
         <f t="shared" si="4"/>
-        <v>0047 83C8</v>
-      </c>
-      <c r="N13" t="str">
+        <v>8021 0B00</v>
+      </c>
+      <c r="M29" t="str">
         <f t="shared" si="5"/>
-        <v>004A 93C8</v>
-      </c>
-      <c r="O13" t="str">
+        <v>4877 5400</v>
+      </c>
+      <c r="N29" t="str">
         <f t="shared" si="6"/>
-        <v>004A F5C8</v>
-      </c>
-      <c r="P13" t="str">
-        <f t="shared" si="7"/>
-        <v>021F 0000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="I14" t="str">
-        <f t="shared" si="0"/>
-        <v>1C1C 0111</v>
-      </c>
-      <c r="J14" t="str">
-        <f t="shared" si="1"/>
-        <v>0080 0020</v>
-      </c>
-      <c r="K14" t="str">
-        <f t="shared" si="2"/>
-        <v>0001 0101</v>
-      </c>
-      <c r="L14" t="str">
-        <f t="shared" si="3"/>
-        <v>0001 50A0</v>
-      </c>
-      <c r="M14" t="str">
-        <f t="shared" si="4"/>
-        <v>004A 93C8</v>
-      </c>
-      <c r="N14" t="str">
-        <f t="shared" si="5"/>
-        <v>004B 5EE8</v>
-      </c>
-      <c r="O14" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P14" t="str">
+        <v>48FF 5500</v>
+      </c>
+      <c r="O29" t="str">
         <f t="shared" si="7"/>
         <v>0000 0000</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="G15" s="2" t="s">
+      <c r="P29" t="str">
+        <f t="shared" si="8"/>
+        <v>0000 0000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="E30" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H30" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="I15" t="str">
-        <f t="shared" si="0"/>
-        <v>1C1C 0312</v>
-      </c>
-      <c r="J15" t="str">
+      <c r="I30" t="str">
         <f t="shared" si="1"/>
-        <v>0080 0020</v>
-      </c>
-      <c r="K15" t="str">
+        <v>130E 0E01</v>
+      </c>
+      <c r="J30" t="str">
         <f t="shared" si="2"/>
-        <v>0003 0901</v>
-      </c>
-      <c r="L15" t="str">
+        <v>E803 E803</v>
+      </c>
+      <c r="K30" t="str">
         <f t="shared" si="3"/>
-        <v>0001 6120</v>
-      </c>
-      <c r="M15" t="str">
+        <v>01C4 0E00</v>
+      </c>
+      <c r="L30" t="str">
         <f t="shared" si="4"/>
-        <v>004A F5C8</v>
-      </c>
-      <c r="N15" t="str">
+        <v>0000 0000</v>
+      </c>
+      <c r="M30" t="str">
         <f t="shared" si="5"/>
-        <v>004C E6E8</v>
-      </c>
-      <c r="O15" t="str">
+        <v>48FF 5500</v>
+      </c>
+      <c r="N30" t="str">
         <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P15" t="str">
+        <v>E8FC 5800</v>
+      </c>
+      <c r="O30" t="str">
         <f t="shared" si="7"/>
         <v>0000 0000</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="I16" t="str">
-        <f t="shared" si="0"/>
-        <v>0E1C 0324</v>
-      </c>
-      <c r="J16" t="str">
-        <f t="shared" si="1"/>
-        <v>0100 0100</v>
-      </c>
-      <c r="K16" t="str">
-        <f t="shared" si="2"/>
-        <v>0006 0901</v>
-      </c>
-      <c r="L16" t="str">
-        <f t="shared" si="3"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="M16" t="str">
-        <f t="shared" si="4"/>
-        <v>004B 5EE8</v>
-      </c>
-      <c r="N16" t="str">
-        <f t="shared" si="5"/>
-        <v>004E 6EE8</v>
-      </c>
-      <c r="O16" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P16" t="str">
-        <f t="shared" si="7"/>
-        <v>0000 0000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="I17" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0111</v>
-      </c>
-      <c r="J17" t="str">
-        <f t="shared" si="1"/>
-        <v>0030 0100</v>
-      </c>
-      <c r="K17" t="str">
-        <f t="shared" si="2"/>
-        <v>0001 0103</v>
-      </c>
-      <c r="L17" t="str">
-        <f t="shared" si="3"/>
-        <v>0001 F1A0</v>
-      </c>
-      <c r="M17" t="str">
-        <f t="shared" si="4"/>
-        <v>004E 6EE8</v>
-      </c>
-      <c r="N17" t="str">
-        <f t="shared" si="5"/>
-        <v>004F 32E8</v>
-      </c>
-      <c r="O17" t="str">
-        <f t="shared" si="6"/>
-        <v>004F 57A8</v>
-      </c>
-      <c r="P17" t="str">
-        <f t="shared" si="7"/>
-        <v>0211 0000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="I18" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0111</v>
-      </c>
-      <c r="J18" t="str">
-        <f t="shared" si="1"/>
-        <v>00C0 0030</v>
-      </c>
-      <c r="K18" t="str">
-        <f t="shared" si="2"/>
-        <v>0001 0101</v>
-      </c>
-      <c r="L18" t="str">
-        <f t="shared" si="3"/>
-        <v>0002 21D0</v>
-      </c>
-      <c r="M18" t="str">
-        <f t="shared" si="4"/>
-        <v>004F 32E8</v>
-      </c>
-      <c r="N18" t="str">
-        <f t="shared" si="5"/>
-        <v>004F 81D8</v>
-      </c>
-      <c r="O18" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P18" t="str">
-        <f t="shared" si="7"/>
-        <v>0000 0000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="I19" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0312</v>
-      </c>
-      <c r="J19" t="str">
-        <f t="shared" si="1"/>
-        <v>00C0 0030</v>
-      </c>
-      <c r="K19" t="str">
-        <f t="shared" si="2"/>
-        <v>0003 0901</v>
-      </c>
-      <c r="L19" t="str">
-        <f t="shared" si="3"/>
-        <v>0002 4690</v>
-      </c>
-      <c r="M19" t="str">
-        <f t="shared" si="4"/>
-        <v>004F 57A8</v>
-      </c>
-      <c r="N19" t="str">
-        <f t="shared" si="5"/>
-        <v>0050 14D8</v>
-      </c>
-      <c r="O19" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P19" t="str">
-        <f t="shared" si="7"/>
-        <v>0000 0000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="I20" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0111</v>
-      </c>
-      <c r="J20" t="str">
-        <f t="shared" si="1"/>
-        <v>0030 0180</v>
-      </c>
-      <c r="K20" t="str">
-        <f t="shared" si="2"/>
-        <v>0001 0103</v>
-      </c>
-      <c r="L20" t="str">
-        <f t="shared" si="3"/>
-        <v>0003 8B50</v>
-      </c>
-      <c r="M20" t="str">
-        <f t="shared" si="4"/>
-        <v>004F 81D8</v>
-      </c>
-      <c r="N20" t="str">
-        <f t="shared" si="5"/>
-        <v>0050 A7D8</v>
-      </c>
-      <c r="O20" t="str">
-        <f t="shared" si="6"/>
-        <v>0050 CC98</v>
-      </c>
-      <c r="P20" t="str">
-        <f t="shared" si="7"/>
-        <v>0211 0000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="I21" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0111</v>
-      </c>
-      <c r="J21" t="str">
-        <f t="shared" si="1"/>
-        <v>00C0 0030</v>
-      </c>
-      <c r="K21" t="str">
-        <f t="shared" si="2"/>
-        <v>0001 0101</v>
-      </c>
-      <c r="L21" t="str">
-        <f t="shared" si="3"/>
-        <v>0003 D380</v>
-      </c>
-      <c r="M21" t="str">
-        <f t="shared" si="4"/>
-        <v>0050 A7D8</v>
-      </c>
-      <c r="N21" t="str">
-        <f t="shared" si="5"/>
-        <v>0050 F6C8</v>
-      </c>
-      <c r="O21" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P21" t="str">
-        <f t="shared" si="7"/>
-        <v>0000 0000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="I22" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0312</v>
-      </c>
-      <c r="J22" t="str">
-        <f t="shared" si="1"/>
-        <v>00C0 0030</v>
-      </c>
-      <c r="K22" t="str">
-        <f t="shared" si="2"/>
-        <v>0003 0901</v>
-      </c>
-      <c r="L22" t="str">
-        <f t="shared" si="3"/>
-        <v>0003 F840</v>
-      </c>
-      <c r="M22" t="str">
-        <f t="shared" si="4"/>
-        <v>0050 CC98</v>
-      </c>
-      <c r="N22" t="str">
-        <f t="shared" si="5"/>
-        <v>0051 89C8</v>
-      </c>
-      <c r="O22" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P22" t="str">
-        <f t="shared" si="7"/>
-        <v>0000 0000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="I23" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0111</v>
-      </c>
-      <c r="J23" t="str">
-        <f t="shared" si="1"/>
-        <v>0040 0180</v>
-      </c>
-      <c r="K23" t="str">
-        <f t="shared" si="2"/>
-        <v>0001 0103</v>
-      </c>
-      <c r="L23" t="str">
-        <f t="shared" si="3"/>
-        <v>0005 3D00</v>
-      </c>
-      <c r="M23" t="str">
-        <f t="shared" si="4"/>
-        <v>0050 F6C8</v>
-      </c>
-      <c r="N23" t="str">
-        <f t="shared" si="5"/>
-        <v>0052 1CC8</v>
-      </c>
-      <c r="O23" t="str">
-        <f t="shared" si="6"/>
-        <v>0052 4DC8</v>
-      </c>
-      <c r="P23" t="str">
-        <f t="shared" si="7"/>
-        <v>0211 0000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="I24" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0111</v>
-      </c>
-      <c r="J24" t="str">
-        <f t="shared" si="1"/>
-        <v>0100 0040</v>
-      </c>
-      <c r="K24" t="str">
-        <f t="shared" si="2"/>
-        <v>0001 0101</v>
-      </c>
-      <c r="L24" t="str">
-        <f t="shared" si="3"/>
-        <v>0005 9D40</v>
-      </c>
-      <c r="M24" t="str">
-        <f t="shared" si="4"/>
-        <v>0052 1CC8</v>
-      </c>
-      <c r="N24" t="str">
-        <f t="shared" si="5"/>
-        <v>0052 8608</v>
-      </c>
-      <c r="O24" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P24" t="str">
-        <f t="shared" si="7"/>
-        <v>0000 0000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="I25" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0312</v>
-      </c>
-      <c r="J25" t="str">
-        <f t="shared" si="1"/>
-        <v>0100 0040</v>
-      </c>
-      <c r="K25" t="str">
-        <f t="shared" si="2"/>
-        <v>0003 0901</v>
-      </c>
-      <c r="L25" t="str">
-        <f t="shared" si="3"/>
-        <v>0005 DE40</v>
-      </c>
-      <c r="M25" t="str">
-        <f t="shared" si="4"/>
-        <v>0052 4DC8</v>
-      </c>
-      <c r="N25" t="str">
-        <f t="shared" si="5"/>
-        <v>0053 4A08</v>
-      </c>
-      <c r="O25" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P25" t="str">
-        <f t="shared" si="7"/>
-        <v>0000 0000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="H26" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="I26" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0111</v>
-      </c>
-      <c r="J26" t="str">
-        <f t="shared" si="1"/>
-        <v>0040 0200</v>
-      </c>
-      <c r="K26" t="str">
-        <f t="shared" si="2"/>
-        <v>0001 0103</v>
-      </c>
-      <c r="L26" t="str">
-        <f t="shared" si="3"/>
-        <v>0008 1F40</v>
-      </c>
-      <c r="M26" t="str">
-        <f t="shared" si="4"/>
-        <v>0053 4A08</v>
-      </c>
-      <c r="N26" t="str">
-        <f t="shared" si="5"/>
-        <v>0054 0E08</v>
-      </c>
-      <c r="O26" t="str">
-        <f t="shared" si="6"/>
-        <v>0054 3F08</v>
-      </c>
-      <c r="P26" t="str">
-        <f t="shared" si="7"/>
-        <v>0211 0000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="I27" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0111</v>
-      </c>
-      <c r="J27" t="str">
-        <f t="shared" si="1"/>
-        <v>0100 0040</v>
-      </c>
-      <c r="K27" t="str">
-        <f t="shared" si="2"/>
-        <v>0001 0101</v>
-      </c>
-      <c r="L27" t="str">
-        <f t="shared" si="3"/>
-        <v>0008 9F80</v>
-      </c>
-      <c r="M27" t="str">
-        <f t="shared" si="4"/>
-        <v>0054 0E08</v>
-      </c>
-      <c r="N27" t="str">
-        <f t="shared" si="5"/>
-        <v>0054 7748</v>
-      </c>
-      <c r="O27" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P27" t="str">
-        <f t="shared" si="7"/>
-        <v>0000 0000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H28" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="I28" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0312</v>
-      </c>
-      <c r="J28" t="str">
-        <f t="shared" si="1"/>
-        <v>0100 0040</v>
-      </c>
-      <c r="K28" t="str">
-        <f t="shared" si="2"/>
-        <v>0003 0901</v>
-      </c>
-      <c r="L28" t="str">
-        <f t="shared" si="3"/>
-        <v>0008 E080</v>
-      </c>
-      <c r="M28" t="str">
-        <f t="shared" si="4"/>
-        <v>0054 3F08</v>
-      </c>
-      <c r="N28" t="str">
-        <f t="shared" si="5"/>
-        <v>0055 3B48</v>
-      </c>
-      <c r="O28" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P28" t="str">
-        <f t="shared" si="7"/>
-        <v>0000 0000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H29" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="I29" t="str">
-        <f t="shared" si="0"/>
-        <v>0E0E 0111</v>
-      </c>
-      <c r="J29" t="str">
-        <f t="shared" si="1"/>
-        <v>03E8 0200</v>
-      </c>
-      <c r="K29" t="str">
-        <f t="shared" si="2"/>
-        <v>0001 0101</v>
-      </c>
-      <c r="L29" t="str">
-        <f t="shared" si="3"/>
-        <v>000B 2180</v>
-      </c>
-      <c r="M29" t="str">
-        <f t="shared" si="4"/>
-        <v>0054 7748</v>
-      </c>
-      <c r="N29" t="str">
-        <f t="shared" si="5"/>
-        <v>0055 FF48</v>
-      </c>
-      <c r="O29" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="P29" t="str">
-        <f t="shared" si="7"/>
-        <v>0000 0000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="H30" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="I30" t="str">
-        <f t="shared" si="0"/>
-        <v>010E 0E15</v>
-      </c>
-      <c r="J30" t="str">
-        <f t="shared" si="1"/>
-        <v>03E8 03E8</v>
-      </c>
-      <c r="K30" t="str">
-        <f t="shared" si="2"/>
-        <v>000E C401</v>
-      </c>
-      <c r="L30" t="str">
-        <f t="shared" si="3"/>
-        <v>0000 0000</v>
-      </c>
-      <c r="M30" t="str">
-        <f t="shared" si="4"/>
-        <v>0055 FF48</v>
-      </c>
-      <c r="N30" t="str">
-        <f t="shared" si="5"/>
-        <v>0058 FCE8</v>
-      </c>
-      <c r="O30" t="str">
-        <f t="shared" si="6"/>
-        <v>0000 0000</v>
-      </c>
       <c r="P30" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0000 0000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update no-dma build, accum latency = 2
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0EDA27-467F-4C3D-9C18-EADD3A3580C4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7304E33B-957B-41BD-8DFB-9A36D65FBEB8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15870" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
   <sheets>
     <sheet name="SqueezeNet v2 MEC Parallel Ch" sheetId="2" r:id="rId1"/>
@@ -1313,8 +1313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80B23C6-EAEB-43B1-B045-456C36085CFA}">
   <dimension ref="A1:AL71"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7368,8 +7368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E501AE-4D2D-491C-85E4-0C34FDA03C89}">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:P30"/>
+    <sheetView zoomScale="76" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update reset signals and fifo readout logic, remove csb control to engine
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B26011-021C-4496-A9ED-AFF87AD9C078}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A914245-4CE6-4BBB-BF51-D82C7A8F57E5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
@@ -1061,8 +1061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80B23C6-EAEB-43B1-B045-456C36085CFA}">
   <dimension ref="A1:AD71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1315,8 +1315,8 @@
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2">
-        <f>G4*E4*D4</f>
-        <v>2043</v>
+        <f>G4*8*D4</f>
+        <v>5448</v>
       </c>
       <c r="O4" s="2">
         <f>D4^2*8*F4</f>

</xml_diff>

<commit_message>
Update fifo readout logic, remove csb control to engine
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B26011-021C-4496-A9ED-AFF87AD9C078}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A914245-4CE6-4BBB-BF51-D82C7A8F57E5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
@@ -1061,8 +1061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80B23C6-EAEB-43B1-B045-456C36085CFA}">
   <dimension ref="A1:AD71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1315,8 +1315,8 @@
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2">
-        <f>G4*E4*D4</f>
-        <v>2043</v>
+        <f>G4*8*D4</f>
+        <v>5448</v>
       </c>
       <c r="O4" s="2">
         <f>D4^2*8*F4</f>

</xml_diff>

<commit_message>
Add bram to optimize latency
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A914245-4CE6-4BBB-BF51-D82C7A8F57E5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9436D1-4C62-40FF-81A0-50DF0EB63C21}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="160">
   <si>
     <t>INPUT</t>
   </si>
@@ -512,6 +512,9 @@
   </si>
   <si>
     <t>stride2|ksize</t>
+  </si>
+  <si>
+    <t>w split</t>
   </si>
 </sst>
 </file>
@@ -1059,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80B23C6-EAEB-43B1-B045-456C36085CFA}">
-  <dimension ref="A1:AD71"/>
+  <dimension ref="A1:AE71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1078,23 +1081,25 @@
     <col min="11" max="12" width="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.44140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.88671875" style="18" customWidth="1"/>
-    <col min="28" max="28" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10" style="21" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8" customWidth="1"/>
+    <col min="17" max="18" width="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.88671875" style="18" customWidth="1"/>
+    <col min="29" max="29" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10" style="21" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" s="15"/>
       <c r="B1" s="16"/>
       <c r="C1" s="29" t="s">
@@ -1116,30 +1121,31 @@
         <v>157</v>
       </c>
       <c r="O1" s="31"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="32" t="s">
+      <c r="P1" s="14"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="S1" s="33"/>
-      <c r="T1" s="34"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="31" t="s">
+      <c r="T1" s="33"/>
+      <c r="U1" s="34"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="Y1" s="31"/>
       <c r="Z1" s="31"/>
-      <c r="AA1" s="30" t="s">
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="26"/>
-      <c r="AD1" s="14" t="s">
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="14" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
@@ -1183,52 +1189,55 @@
         <v>133</v>
       </c>
       <c r="P2" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q2" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="Q2" s="14" t="s">
+      <c r="R2" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="S2" s="14" t="s">
+      <c r="T2" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="T2" s="22" t="s">
+      <c r="U2" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="U2" s="14" t="s">
+      <c r="V2" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="V2" s="14" t="s">
+      <c r="W2" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="W2" s="14" t="s">
+      <c r="X2" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="X2" s="14" t="s">
+      <c r="Y2" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="Y2" s="14" t="s">
+      <c r="Z2" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="Z2" s="14" t="s">
+      <c r="AA2" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="AA2" s="9" t="s">
+      <c r="AB2" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="AB2" s="14" t="s">
+      <c r="AC2" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="AC2" s="22" t="s">
+      <c r="AD2" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="AD2" s="14" t="s">
+      <c r="AE2" s="14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1259,23 +1268,24 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="10"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
-      <c r="AA3" s="5"/>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="10"/>
-      <c r="AD3" s="14" t="s">
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="14" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -1323,65 +1333,69 @@
         <v>4608</v>
       </c>
       <c r="P4" s="2">
+        <f>D4^2*8*8</f>
+        <v>576</v>
+      </c>
+      <c r="Q4" s="2">
         <f>F4</f>
         <v>64</v>
       </c>
-      <c r="Q4" s="2">
-        <f>O4+P4</f>
+      <c r="R4" s="2">
+        <f>O4+Q4</f>
         <v>4672</v>
       </c>
-      <c r="R4" s="6" t="str">
+      <c r="S4" s="6" t="str">
         <f>DEC2HEX(J4,2)&amp;DEC2HEX(G4,2)&amp;"_"&amp;DEC2HEX(D4,2)&amp;DEC2HEX(H4,1)&amp;DEC2HEX(C4,1)</f>
         <v>71E3_0321</v>
       </c>
-      <c r="S4" s="2" t="str">
+      <c r="T4" s="2" t="str">
         <f>DEC2HEX(F4,4)&amp;"_"&amp;DEC2HEX(E4,4)</f>
         <v>0040_0003</v>
       </c>
-      <c r="T4" s="11" t="str">
+      <c r="U4" s="11" t="str">
         <f>DEC2HEX(D4*H4,4)&amp;"_"&amp;DEC2HEX(D4^2,2)&amp;"00"</f>
         <v>0006_0900</v>
       </c>
-      <c r="U4" s="2">
+      <c r="V4" s="2">
         <v>0.01</v>
       </c>
-      <c r="V4" s="2">
+      <c r="W4" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W4" s="2">
+      <c r="X4" s="2">
         <f>D4^2*E4</f>
         <v>27</v>
       </c>
-      <c r="X4" s="2">
-        <f>L4*W4</f>
+      <c r="Y4" s="2">
+        <f>L4*X4</f>
         <v>22064832</v>
       </c>
-      <c r="Y4" s="2">
-        <f>L4*W4*0.03</f>
+      <c r="Z4" s="2">
+        <f>L4*X4*0.03</f>
         <v>661944.96</v>
       </c>
-      <c r="Z4" s="2">
-        <f>L4*W4*U4*V4</f>
+      <c r="AA4" s="2">
+        <f>L4*X4*V4*W4</f>
         <v>13790.52</v>
       </c>
-      <c r="AA4" s="6">
+      <c r="AB4" s="6">
         <f>D4*J3*J4*F3</f>
         <v>230859</v>
       </c>
-      <c r="AB4" s="2">
-        <f>AA4*0.03</f>
+      <c r="AC4" s="2">
+        <f>AB4*0.03</f>
         <v>6925.7699999999995</v>
       </c>
-      <c r="AC4" s="11">
+      <c r="AD4" s="11">
         <f>D4*J3</f>
         <v>681</v>
       </c>
-      <c r="AD4" s="14">
-        <f>X4/AA4</f>
+      <c r="AE4" s="14">
+        <f>Y4/AB4</f>
         <v>95.57709251101322</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
@@ -1403,21 +1417,22 @@
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="12"/>
-      <c r="U5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="12"/>
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="3"/>
-      <c r="AC5" s="12"/>
-      <c r="AD5" s="14"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="12"/>
+      <c r="AE5" s="14"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
@@ -1463,58 +1478,59 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
-      <c r="R6" s="8" t="str">
+      <c r="R6" s="4"/>
+      <c r="S6" s="8" t="str">
         <f>DEC2HEX(J6,2)&amp;DEC2HEX(G6,2)&amp;"_"&amp;DEC2HEX(D6,2)&amp;DEC2HEX(H6,1)&amp;DEC2HEX(C6,1)</f>
         <v>3871_0322</v>
       </c>
-      <c r="S6" s="4" t="str">
+      <c r="T6" s="4" t="str">
         <f>DEC2HEX(F6,4)&amp;"_"&amp;DEC2HEX(F6,4)</f>
         <v>0040_0040</v>
       </c>
-      <c r="T6" s="13" t="str">
+      <c r="U6" s="13" t="str">
         <f>DEC2HEX(D6*H6,4)&amp;"_"&amp;DEC2HEX(D6^2,2)&amp;"00"</f>
         <v>0006_0900</v>
       </c>
-      <c r="U6" s="4">
+      <c r="V6" s="4">
         <v>0.01</v>
       </c>
-      <c r="V6" s="4">
+      <c r="W6" s="4">
         <v>6.25E-2</v>
       </c>
-      <c r="W6" s="4">
+      <c r="X6" s="4">
         <f>D6^2*E6</f>
         <v>9</v>
       </c>
-      <c r="X6" s="4">
-        <f>L6*W6</f>
+      <c r="Y6" s="4">
+        <f>L6*X6</f>
         <v>1806336</v>
       </c>
-      <c r="Y6" s="4">
-        <f>L6*W6*0.03</f>
+      <c r="Z6" s="4">
+        <f>L6*X6*0.03</f>
         <v>54190.079999999994</v>
       </c>
-      <c r="Z6" s="4">
-        <f>L6*W6*U6*V6</f>
+      <c r="AA6" s="4">
+        <f>L6*X6*V6*W6</f>
         <v>1128.96</v>
       </c>
-      <c r="AA6" s="8">
+      <c r="AB6" s="8">
         <f>D6*J4*J6*F4</f>
         <v>1214976</v>
       </c>
-      <c r="AB6" s="4">
-        <f>AA6*0.03</f>
+      <c r="AC6" s="4">
+        <f>AB6*0.03</f>
         <v>36449.279999999999</v>
       </c>
-      <c r="AC6" s="13">
+      <c r="AD6" s="13">
         <f>D6*J4</f>
         <v>339</v>
       </c>
-      <c r="AD6" s="14">
-        <f t="shared" ref="AD6:AD7" si="0">X6/AA6</f>
+      <c r="AE6" s="14">
+        <f t="shared" ref="AE6:AE7" si="0">Y6/AB6</f>
         <v>1.4867256637168142</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1565,65 +1581,69 @@
         <v>1024</v>
       </c>
       <c r="P7" s="2">
+        <f>D7^2*8*8</f>
+        <v>64</v>
+      </c>
+      <c r="Q7" s="2">
         <f>F7</f>
         <v>16</v>
       </c>
-      <c r="Q7" s="2">
-        <f>O7+P7</f>
+      <c r="R7" s="2">
+        <f>O7+Q7</f>
         <v>1040</v>
       </c>
-      <c r="R7" s="6" t="str">
+      <c r="S7" s="6" t="str">
         <f>DEC2HEX(J7,2)&amp;DEC2HEX(G7,2)&amp;"_"&amp;DEC2HEX(D7,2)&amp;DEC2HEX(H7,1)&amp;DEC2HEX(C7,1)</f>
         <v>3838_0111</v>
       </c>
-      <c r="S7" s="2" t="str">
+      <c r="T7" s="2" t="str">
         <f>DEC2HEX(F7,4)&amp;"_"&amp;DEC2HEX(E7,4)</f>
         <v>0010_0040</v>
       </c>
-      <c r="T7" s="11" t="str">
+      <c r="U7" s="11" t="str">
         <f>DEC2HEX(D7*H7,4)&amp;"_"&amp;DEC2HEX(D7^2,2)&amp;"00"</f>
         <v>0001_0100</v>
       </c>
-      <c r="U7" s="2">
+      <c r="V7" s="2">
         <v>0.01</v>
       </c>
-      <c r="V7" s="2">
+      <c r="W7" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W7" s="2">
+      <c r="X7" s="2">
         <f>D7^2*E7</f>
         <v>64</v>
       </c>
-      <c r="X7" s="2">
-        <f>L7*W7</f>
+      <c r="Y7" s="2">
+        <f>L7*X7</f>
         <v>3211264</v>
       </c>
-      <c r="Y7" s="2">
-        <f>L7*W7*0.03</f>
+      <c r="Z7" s="2">
+        <f>L7*X7*0.03</f>
         <v>96337.919999999998</v>
       </c>
-      <c r="Z7" s="2">
-        <f>L7*W7*U7*V7</f>
+      <c r="AA7" s="2">
+        <f>L7*X7*V7*W7</f>
         <v>2007.04</v>
       </c>
-      <c r="AA7" s="6">
+      <c r="AB7" s="6">
         <f>D7*J6*J7*F6</f>
         <v>200704</v>
       </c>
-      <c r="AB7" s="2">
-        <f>AA7*0.03</f>
+      <c r="AC7" s="2">
+        <f>AB7*0.03</f>
         <v>6021.12</v>
       </c>
-      <c r="AC7" s="11">
+      <c r="AD7" s="11">
         <f>D7*J6</f>
         <v>56</v>
       </c>
-      <c r="AD7" s="14">
+      <c r="AE7" s="14">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
@@ -1645,21 +1665,22 @@
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="12"/>
-      <c r="U8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="12"/>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
-      <c r="AA8" s="7"/>
-      <c r="AB8" s="3"/>
-      <c r="AC8" s="12"/>
-      <c r="AD8" s="14"/>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="12"/>
+      <c r="AE8" s="14"/>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -1707,65 +1728,69 @@
         <v>1024</v>
       </c>
       <c r="P9" s="2">
+        <f t="shared" ref="P9:P10" si="2">D9^2*8*8</f>
+        <v>64</v>
+      </c>
+      <c r="Q9" s="2">
         <f>F9</f>
         <v>64</v>
       </c>
-      <c r="Q9" s="2">
-        <f t="shared" ref="Q9:Q10" si="2">O9+P9</f>
+      <c r="R9" s="2">
+        <f t="shared" ref="R9:R10" si="3">O9+Q9</f>
         <v>1088</v>
       </c>
-      <c r="R9" s="6" t="str">
-        <f t="shared" ref="R9:R10" si="3">DEC2HEX(J9,2)&amp;DEC2HEX(G9,2)&amp;"_"&amp;DEC2HEX(D9,2)&amp;DEC2HEX(H9,1)&amp;DEC2HEX(C9,1)</f>
+      <c r="S9" s="6" t="str">
+        <f t="shared" ref="S9:S10" si="4">DEC2HEX(J9,2)&amp;DEC2HEX(G9,2)&amp;"_"&amp;DEC2HEX(D9,2)&amp;DEC2HEX(H9,1)&amp;DEC2HEX(C9,1)</f>
         <v>3838_0111</v>
       </c>
-      <c r="S9" s="2" t="str">
+      <c r="T9" s="2" t="str">
         <f>DEC2HEX(F9,4)&amp;"_"&amp;DEC2HEX(E9,4)</f>
         <v>0040_0010</v>
       </c>
-      <c r="T9" s="11" t="str">
+      <c r="U9" s="11" t="str">
         <f>DEC2HEX(D9*H9,4)&amp;"_"&amp;DEC2HEX(D9^2,2)&amp;"00"</f>
         <v>0001_0100</v>
       </c>
-      <c r="U9" s="2">
+      <c r="V9" s="2">
         <v>0.01</v>
       </c>
-      <c r="V9" s="2">
+      <c r="W9" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W9" s="2">
+      <c r="X9" s="2">
         <f>D9^2*E9</f>
         <v>16</v>
       </c>
-      <c r="X9" s="2">
-        <f>L9*W9</f>
+      <c r="Y9" s="2">
+        <f>L9*X9</f>
         <v>3211264</v>
       </c>
-      <c r="Y9" s="2">
-        <f>L9*W9*0.03</f>
+      <c r="Z9" s="2">
+        <f>L9*X9*0.03</f>
         <v>96337.919999999998</v>
       </c>
-      <c r="Z9" s="2">
-        <f>L9*W9*U9*V9</f>
+      <c r="AA9" s="2">
+        <f>L9*X9*V9*W9</f>
         <v>2007.04</v>
       </c>
-      <c r="AA9" s="6">
+      <c r="AB9" s="6">
         <f>D9*J7*J9*F7</f>
         <v>50176</v>
       </c>
-      <c r="AB9" s="2">
-        <f>AA9*0.03</f>
+      <c r="AC9" s="2">
+        <f>AB9*0.03</f>
         <v>1505.28</v>
       </c>
-      <c r="AC9" s="11">
+      <c r="AD9" s="11">
         <f>D9*J7</f>
         <v>56</v>
       </c>
-      <c r="AD9" s="14">
-        <f t="shared" ref="AD9:AD10" si="4">X9/AA9</f>
+      <c r="AE9" s="14">
+        <f t="shared" ref="AE9:AE10" si="5">Y9/AB9</f>
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -1813,65 +1838,69 @@
         <v>9216</v>
       </c>
       <c r="P10" s="2">
+        <f t="shared" si="2"/>
+        <v>576</v>
+      </c>
+      <c r="Q10" s="2">
         <f>F10</f>
         <v>64</v>
       </c>
-      <c r="Q10" s="2">
-        <f t="shared" si="2"/>
+      <c r="R10" s="2">
+        <f t="shared" si="3"/>
         <v>9280</v>
       </c>
-      <c r="R10" s="6" t="str">
-        <f t="shared" si="3"/>
+      <c r="S10" s="6" t="str">
+        <f t="shared" si="4"/>
         <v>3838_0311</v>
       </c>
-      <c r="S10" s="2" t="str">
+      <c r="T10" s="2" t="str">
         <f>DEC2HEX(F10,4)&amp;"_"&amp;DEC2HEX(E10,4)</f>
         <v>0040_0010</v>
       </c>
-      <c r="T10" s="11" t="str">
+      <c r="U10" s="11" t="str">
         <f>DEC2HEX(D10*H10,4)&amp;"_"&amp;DEC2HEX(D10^2,2)&amp;"00"</f>
         <v>0003_0900</v>
       </c>
-      <c r="U10" s="2">
+      <c r="V10" s="2">
         <v>0.01</v>
       </c>
-      <c r="V10" s="2">
+      <c r="W10" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W10" s="2">
+      <c r="X10" s="2">
         <f>D10^2*E10</f>
         <v>144</v>
       </c>
-      <c r="X10" s="2">
-        <f>L10*W10</f>
+      <c r="Y10" s="2">
+        <f>L10*X10</f>
         <v>28901376</v>
       </c>
-      <c r="Y10" s="2">
-        <f>L10*W10*0.03</f>
+      <c r="Z10" s="2">
+        <f>L10*X10*0.03</f>
         <v>867041.27999999991</v>
       </c>
-      <c r="Z10" s="2">
-        <f>L10*W10*U10*V10</f>
+      <c r="AA10" s="2">
+        <f>L10*X10*V10*W10</f>
         <v>18063.36</v>
       </c>
-      <c r="AA10" s="6">
+      <c r="AB10" s="6">
         <f>D10*J7*J10*F7</f>
         <v>150528</v>
       </c>
-      <c r="AB10" s="2">
-        <f>AA10*0.03</f>
+      <c r="AC10" s="2">
+        <f>AB10*0.03</f>
         <v>4515.84</v>
       </c>
-      <c r="AC10" s="11">
+      <c r="AD10" s="11">
         <f>D10*J7</f>
         <v>168</v>
       </c>
-      <c r="AD10" s="14">
-        <f t="shared" si="4"/>
+      <c r="AE10" s="14">
+        <f t="shared" si="5"/>
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
@@ -1893,21 +1922,22 @@
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="12"/>
-      <c r="U11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="12"/>
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
-      <c r="AA11" s="7"/>
-      <c r="AB11" s="3"/>
-      <c r="AC11" s="12"/>
-      <c r="AD11" s="14"/>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="12"/>
+      <c r="AE11" s="14"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>12</v>
       </c>
@@ -1929,21 +1959,22 @@
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="12"/>
-      <c r="U12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="12"/>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
-      <c r="AA12" s="7"/>
-      <c r="AB12" s="3"/>
-      <c r="AC12" s="12"/>
-      <c r="AD12" s="14"/>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="7"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="12"/>
+      <c r="AE12" s="14"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>19</v>
       </c>
@@ -1971,21 +2002,22 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="10"/>
-      <c r="U13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="10"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
-      <c r="AA13" s="5"/>
-      <c r="AB13" s="1"/>
-      <c r="AC13" s="10"/>
-      <c r="AD13" s="14"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="5"/>
+      <c r="AC13" s="1"/>
+      <c r="AD13" s="10"/>
+      <c r="AE13" s="14"/>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>13</v>
       </c>
@@ -2036,65 +2068,69 @@
         <v>2048</v>
       </c>
       <c r="P14" s="2">
+        <f>D14^2*8*8</f>
+        <v>64</v>
+      </c>
+      <c r="Q14" s="2">
         <f>F14</f>
         <v>16</v>
       </c>
-      <c r="Q14" s="2">
-        <f>O14+P14</f>
+      <c r="R14" s="2">
+        <f>O14+Q14</f>
         <v>2064</v>
       </c>
-      <c r="R14" s="6" t="str">
+      <c r="S14" s="6" t="str">
         <f>DEC2HEX(J14,2)&amp;DEC2HEX(G14,2)&amp;"_"&amp;DEC2HEX(D14,2)&amp;DEC2HEX(H14,1)&amp;DEC2HEX(C14,1)</f>
         <v>3838_0111</v>
       </c>
-      <c r="S14" s="2" t="str">
+      <c r="T14" s="2" t="str">
         <f>DEC2HEX(F14,4)&amp;"_"&amp;DEC2HEX(E14,4)</f>
         <v>0010_0080</v>
       </c>
-      <c r="T14" s="11" t="str">
+      <c r="U14" s="11" t="str">
         <f>DEC2HEX(D14*H14,4)&amp;"_"&amp;DEC2HEX(D14^2,2)&amp;"00"</f>
         <v>0001_0100</v>
       </c>
-      <c r="U14" s="2">
+      <c r="V14" s="2">
         <v>0.01</v>
       </c>
-      <c r="V14" s="2">
+      <c r="W14" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W14" s="2">
+      <c r="X14" s="2">
         <f>D14^2*E14</f>
         <v>128</v>
       </c>
-      <c r="X14" s="2">
-        <f>L14*W14</f>
+      <c r="Y14" s="2">
+        <f>L14*X14</f>
         <v>6422528</v>
       </c>
-      <c r="Y14" s="2">
-        <f>L14*W14*0.03</f>
+      <c r="Z14" s="2">
+        <f>L14*X14*0.03</f>
         <v>192675.84</v>
       </c>
-      <c r="Z14" s="2">
-        <f>L14*W14*U14*V14</f>
+      <c r="AA14" s="2">
+        <f>L14*X14*V14*W14</f>
         <v>4014.08</v>
       </c>
-      <c r="AA14" s="6">
+      <c r="AB14" s="6">
         <f>D14*J13*J14*F13</f>
         <v>401408</v>
       </c>
-      <c r="AB14" s="2">
-        <f>AA14*0.03</f>
+      <c r="AC14" s="2">
+        <f>AB14*0.03</f>
         <v>12042.24</v>
       </c>
-      <c r="AC14" s="11">
+      <c r="AD14" s="11">
         <f>D14*J13</f>
         <v>56</v>
       </c>
-      <c r="AD14" s="14">
-        <f>X14/AA14</f>
+      <c r="AE14" s="14">
+        <f>Y14/AB14</f>
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>14</v>
       </c>
@@ -2116,21 +2152,22 @@
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="3"/>
-      <c r="T15" s="12"/>
-      <c r="U15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="12"/>
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
-      <c r="AA15" s="7"/>
-      <c r="AB15" s="3"/>
-      <c r="AC15" s="12"/>
-      <c r="AD15" s="14"/>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA15" s="3"/>
+      <c r="AB15" s="7"/>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="12"/>
+      <c r="AE15" s="14"/>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
@@ -2170,7 +2207,7 @@
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2">
-        <f t="shared" ref="N16:N17" si="5">G16*E16*D16</f>
+        <f t="shared" ref="N16:N17" si="6">G16*E16*D16</f>
         <v>896</v>
       </c>
       <c r="O16" s="2">
@@ -2178,65 +2215,69 @@
         <v>1024</v>
       </c>
       <c r="P16" s="2">
+        <f t="shared" ref="P16:P17" si="7">D16^2*8*8</f>
+        <v>64</v>
+      </c>
+      <c r="Q16" s="2">
         <f>F16</f>
         <v>64</v>
       </c>
-      <c r="Q16" s="2">
-        <f t="shared" ref="Q16:Q17" si="6">O16+P16</f>
+      <c r="R16" s="2">
+        <f t="shared" ref="R16:R17" si="8">O16+Q16</f>
         <v>1088</v>
       </c>
-      <c r="R16" s="6" t="str">
-        <f t="shared" ref="R16:R17" si="7">DEC2HEX(J16,2)&amp;DEC2HEX(G16,2)&amp;"_"&amp;DEC2HEX(D16,2)&amp;DEC2HEX(H16,1)&amp;DEC2HEX(C16,1)</f>
+      <c r="S16" s="6" t="str">
+        <f t="shared" ref="S16:S17" si="9">DEC2HEX(J16,2)&amp;DEC2HEX(G16,2)&amp;"_"&amp;DEC2HEX(D16,2)&amp;DEC2HEX(H16,1)&amp;DEC2HEX(C16,1)</f>
         <v>3838_0111</v>
       </c>
-      <c r="S16" s="2" t="str">
+      <c r="T16" s="2" t="str">
         <f>DEC2HEX(F16,4)&amp;"_"&amp;DEC2HEX(E16,4)</f>
         <v>0040_0010</v>
       </c>
-      <c r="T16" s="11" t="str">
+      <c r="U16" s="11" t="str">
         <f>DEC2HEX(D16*H16,4)&amp;"_"&amp;DEC2HEX(D16^2,2)&amp;"00"</f>
         <v>0001_0100</v>
       </c>
-      <c r="U16" s="2">
+      <c r="V16" s="2">
         <v>0.01</v>
       </c>
-      <c r="V16" s="2">
+      <c r="W16" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W16" s="2">
+      <c r="X16" s="2">
         <f>D16^2*E16</f>
         <v>16</v>
       </c>
-      <c r="X16" s="2">
-        <f>L16*W16</f>
+      <c r="Y16" s="2">
+        <f>L16*X16</f>
         <v>3211264</v>
       </c>
-      <c r="Y16" s="2">
-        <f>L16*W16*0.03</f>
+      <c r="Z16" s="2">
+        <f>L16*X16*0.03</f>
         <v>96337.919999999998</v>
       </c>
-      <c r="Z16" s="2">
-        <f>L16*W16*U16*V16</f>
+      <c r="AA16" s="2">
+        <f>L16*X16*V16*W16</f>
         <v>2007.04</v>
       </c>
-      <c r="AA16" s="6">
+      <c r="AB16" s="6">
         <f>D16*J14*J16*F14</f>
         <v>50176</v>
       </c>
-      <c r="AB16" s="2">
-        <f>AA16*0.03</f>
+      <c r="AC16" s="2">
+        <f>AB16*0.03</f>
         <v>1505.28</v>
       </c>
-      <c r="AC16" s="11">
+      <c r="AD16" s="11">
         <f>D16*J14</f>
         <v>56</v>
       </c>
-      <c r="AD16" s="14">
-        <f t="shared" ref="AD16:AD17" si="8">X16/AA16</f>
+      <c r="AE16" s="14">
+        <f t="shared" ref="AE16:AE17" si="10">Y16/AB16</f>
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
@@ -2276,7 +2317,7 @@
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2688</v>
       </c>
       <c r="O17" s="2">
@@ -2284,65 +2325,69 @@
         <v>9216</v>
       </c>
       <c r="P17" s="2">
+        <f t="shared" si="7"/>
+        <v>576</v>
+      </c>
+      <c r="Q17" s="2">
         <f>F17</f>
         <v>64</v>
       </c>
-      <c r="Q17" s="2">
-        <f t="shared" si="6"/>
+      <c r="R17" s="2">
+        <f t="shared" si="8"/>
         <v>9280</v>
       </c>
-      <c r="R17" s="6" t="str">
-        <f t="shared" si="7"/>
+      <c r="S17" s="6" t="str">
+        <f t="shared" si="9"/>
         <v>3838_0311</v>
       </c>
-      <c r="S17" s="2" t="str">
+      <c r="T17" s="2" t="str">
         <f>DEC2HEX(F17,4)&amp;"_"&amp;DEC2HEX(E17,4)</f>
         <v>0040_0010</v>
       </c>
-      <c r="T17" s="11" t="str">
+      <c r="U17" s="11" t="str">
         <f>DEC2HEX(D17*H17,4)&amp;"_"&amp;DEC2HEX(D17^2,2)&amp;"00"</f>
         <v>0003_0900</v>
       </c>
-      <c r="U17" s="2">
+      <c r="V17" s="2">
         <v>0.01</v>
       </c>
-      <c r="V17" s="2">
+      <c r="W17" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W17" s="2">
+      <c r="X17" s="2">
         <f>D17^2*E17</f>
         <v>144</v>
       </c>
-      <c r="X17" s="2">
-        <f>L17*W17</f>
+      <c r="Y17" s="2">
+        <f>L17*X17</f>
         <v>28901376</v>
       </c>
-      <c r="Y17" s="2">
-        <f>L17*W17*0.03</f>
+      <c r="Z17" s="2">
+        <f>L17*X17*0.03</f>
         <v>867041.27999999991</v>
       </c>
-      <c r="Z17" s="2">
-        <f>L17*W17*U17*V17</f>
+      <c r="AA17" s="2">
+        <f>L17*X17*V17*W17</f>
         <v>18063.36</v>
       </c>
-      <c r="AA17" s="6">
+      <c r="AB17" s="6">
         <f>D17*J14*J17*F14</f>
         <v>150528</v>
       </c>
-      <c r="AB17" s="2">
-        <f>AA17*0.03</f>
+      <c r="AC17" s="2">
+        <f>AB17*0.03</f>
         <v>4515.84</v>
       </c>
-      <c r="AC17" s="11">
+      <c r="AD17" s="11">
         <f>D17*J14</f>
         <v>168</v>
       </c>
-      <c r="AD17" s="14">
-        <f t="shared" si="8"/>
+      <c r="AE17" s="14">
+        <f t="shared" si="10"/>
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>17</v>
       </c>
@@ -2364,21 +2409,22 @@
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
-      <c r="R18" s="7"/>
-      <c r="S18" s="3"/>
-      <c r="T18" s="12"/>
-      <c r="U18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="12"/>
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
-      <c r="AA18" s="7"/>
-      <c r="AB18" s="3"/>
-      <c r="AC18" s="12"/>
-      <c r="AD18" s="14"/>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA18" s="3"/>
+      <c r="AB18" s="7"/>
+      <c r="AC18" s="3"/>
+      <c r="AD18" s="12"/>
+      <c r="AE18" s="14"/>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>18</v>
       </c>
@@ -2400,21 +2446,22 @@
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
-      <c r="R19" s="7"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="12"/>
-      <c r="U19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="12"/>
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
-      <c r="AA19" s="7"/>
-      <c r="AB19" s="3"/>
-      <c r="AC19" s="12"/>
-      <c r="AD19" s="14"/>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA19" s="3"/>
+      <c r="AB19" s="7"/>
+      <c r="AC19" s="3"/>
+      <c r="AD19" s="12"/>
+      <c r="AE19" s="14"/>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>20</v>
       </c>
@@ -2442,21 +2489,22 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="10"/>
-      <c r="U20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="10"/>
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
-      <c r="AA20" s="5"/>
-      <c r="AB20" s="1"/>
-      <c r="AC20" s="10"/>
-      <c r="AD20" s="14"/>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="5"/>
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="10"/>
+      <c r="AE20" s="14"/>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>21</v>
       </c>
@@ -2502,58 +2550,59 @@
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
-      <c r="R21" s="8" t="str">
+      <c r="R21" s="4"/>
+      <c r="S21" s="8" t="str">
         <f>DEC2HEX(J21,2)&amp;DEC2HEX(G21,2)&amp;"_"&amp;DEC2HEX(D21,2)&amp;DEC2HEX(H21,1)&amp;DEC2HEX(C21,1)</f>
         <v>1C38_0322</v>
       </c>
-      <c r="S21" s="4" t="str">
+      <c r="T21" s="4" t="str">
         <f>DEC2HEX(F21,4)&amp;"_"&amp;DEC2HEX(F21,4)</f>
         <v>0080_0080</v>
       </c>
-      <c r="T21" s="13" t="str">
+      <c r="U21" s="13" t="str">
         <f>DEC2HEX(D21*H21,4)&amp;"_"&amp;DEC2HEX(D21^2,2)&amp;"00"</f>
         <v>0006_0900</v>
       </c>
-      <c r="U21" s="4">
+      <c r="V21" s="4">
         <v>0.01</v>
       </c>
-      <c r="V21" s="4">
+      <c r="W21" s="4">
         <v>6.25E-2</v>
       </c>
-      <c r="W21" s="4">
+      <c r="X21" s="4">
         <f>D21^2*E21</f>
         <v>9</v>
       </c>
-      <c r="X21" s="4">
-        <f>L21*W21</f>
+      <c r="Y21" s="4">
+        <f>L21*X21</f>
         <v>903168</v>
       </c>
-      <c r="Y21" s="4">
-        <f>L21*W21*0.03</f>
+      <c r="Z21" s="4">
+        <f>L21*X21*0.03</f>
         <v>27095.039999999997</v>
       </c>
-      <c r="Z21" s="4">
-        <f>L21*W21*U21*V21</f>
+      <c r="AA21" s="4">
+        <f>L21*X21*V21*W21</f>
         <v>564.48</v>
       </c>
-      <c r="AA21" s="8">
+      <c r="AB21" s="8">
         <f>D21*J20*J21*F20</f>
         <v>602112</v>
       </c>
-      <c r="AB21" s="4">
-        <f>AA21*0.03</f>
+      <c r="AC21" s="4">
+        <f>AB21*0.03</f>
         <v>18063.36</v>
       </c>
-      <c r="AC21" s="13">
+      <c r="AD21" s="13">
         <f>D21*J20</f>
         <v>168</v>
       </c>
-      <c r="AD21" s="14">
-        <f t="shared" ref="AD21:AD22" si="9">X21/AA21</f>
+      <c r="AE21" s="14">
+        <f t="shared" ref="AE21:AE22" si="11">Y21/AB21</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
@@ -2604,65 +2653,69 @@
         <v>4096</v>
       </c>
       <c r="P22" s="2">
+        <f>D22^2*8*8</f>
+        <v>64</v>
+      </c>
+      <c r="Q22" s="2">
         <f>F22</f>
         <v>32</v>
       </c>
-      <c r="Q22" s="2">
-        <f>O22+P22</f>
+      <c r="R22" s="2">
+        <f>O22+Q22</f>
         <v>4128</v>
       </c>
-      <c r="R22" s="6" t="str">
+      <c r="S22" s="6" t="str">
         <f>DEC2HEX(J22,2)&amp;DEC2HEX(G22,2)&amp;"_"&amp;DEC2HEX(D22,2)&amp;DEC2HEX(H22,1)&amp;DEC2HEX(C22,1)</f>
         <v>1C1C_0111</v>
       </c>
-      <c r="S22" s="2" t="str">
+      <c r="T22" s="2" t="str">
         <f>DEC2HEX(F22,4)&amp;"_"&amp;DEC2HEX(E22,4)</f>
         <v>0020_0080</v>
       </c>
-      <c r="T22" s="11" t="str">
+      <c r="U22" s="11" t="str">
         <f>DEC2HEX(D22*H22,4)&amp;"_"&amp;DEC2HEX(D22^2,2)&amp;"00"</f>
         <v>0001_0100</v>
       </c>
-      <c r="U22" s="2">
+      <c r="V22" s="2">
         <v>0.01</v>
       </c>
-      <c r="V22" s="2">
+      <c r="W22" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W22" s="2">
+      <c r="X22" s="2">
         <f>D22^2*E22</f>
         <v>128</v>
       </c>
-      <c r="X22" s="2">
-        <f>L22*W22</f>
+      <c r="Y22" s="2">
+        <f>L22*X22</f>
         <v>3211264</v>
       </c>
-      <c r="Y22" s="2">
-        <f>L22*W22*0.03</f>
+      <c r="Z22" s="2">
+        <f>L22*X22*0.03</f>
         <v>96337.919999999998</v>
       </c>
-      <c r="Z22" s="2">
-        <f>L22*W22*U22*V22</f>
+      <c r="AA22" s="2">
+        <f>L22*X22*V22*W22</f>
         <v>2007.04</v>
       </c>
-      <c r="AA22" s="6">
+      <c r="AB22" s="6">
         <f>D22*J21*J22*F21</f>
         <v>100352</v>
       </c>
-      <c r="AB22" s="2">
-        <f>AA22*0.03</f>
+      <c r="AC22" s="2">
+        <f>AB22*0.03</f>
         <v>3010.56</v>
       </c>
-      <c r="AC22" s="11">
+      <c r="AD22" s="11">
         <f>D22*J21</f>
         <v>28</v>
       </c>
-      <c r="AD22" s="14">
-        <f t="shared" si="9"/>
+      <c r="AE22" s="14">
+        <f t="shared" si="11"/>
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>23</v>
       </c>
@@ -2684,21 +2737,22 @@
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
-      <c r="R23" s="7"/>
-      <c r="S23" s="3"/>
-      <c r="T23" s="12"/>
-      <c r="U23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="12"/>
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
-      <c r="AA23" s="7"/>
-      <c r="AB23" s="3"/>
-      <c r="AC23" s="12"/>
-      <c r="AD23" s="14"/>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA23" s="3"/>
+      <c r="AB23" s="7"/>
+      <c r="AC23" s="3"/>
+      <c r="AD23" s="12"/>
+      <c r="AE23" s="14"/>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>24</v>
       </c>
@@ -2738,7 +2792,7 @@
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2">
-        <f t="shared" ref="N24:N25" si="10">G24*E24*D24</f>
+        <f t="shared" ref="N24:N25" si="12">G24*E24*D24</f>
         <v>896</v>
       </c>
       <c r="O24" s="2">
@@ -2746,65 +2800,69 @@
         <v>4096</v>
       </c>
       <c r="P24" s="2">
+        <f t="shared" ref="P24:P25" si="13">D24^2*8*8</f>
+        <v>64</v>
+      </c>
+      <c r="Q24" s="2">
         <f>F24</f>
         <v>128</v>
       </c>
-      <c r="Q24" s="2">
-        <f t="shared" ref="Q24:Q25" si="11">O24+P24</f>
+      <c r="R24" s="2">
+        <f t="shared" ref="R24:R25" si="14">O24+Q24</f>
         <v>4224</v>
       </c>
-      <c r="R24" s="6" t="str">
-        <f t="shared" ref="R24:R25" si="12">DEC2HEX(J24,2)&amp;DEC2HEX(G24,2)&amp;"_"&amp;DEC2HEX(D24,2)&amp;DEC2HEX(H24,1)&amp;DEC2HEX(C24,1)</f>
+      <c r="S24" s="6" t="str">
+        <f t="shared" ref="S24:S25" si="15">DEC2HEX(J24,2)&amp;DEC2HEX(G24,2)&amp;"_"&amp;DEC2HEX(D24,2)&amp;DEC2HEX(H24,1)&amp;DEC2HEX(C24,1)</f>
         <v>1C1C_0111</v>
       </c>
-      <c r="S24" s="2" t="str">
+      <c r="T24" s="2" t="str">
         <f>DEC2HEX(F24,4)&amp;"_"&amp;DEC2HEX(E24,4)</f>
         <v>0080_0020</v>
       </c>
-      <c r="T24" s="11" t="str">
+      <c r="U24" s="11" t="str">
         <f>DEC2HEX(D24*H24,4)&amp;"_"&amp;DEC2HEX(D24^2,2)&amp;"00"</f>
         <v>0001_0100</v>
       </c>
-      <c r="U24" s="2">
+      <c r="V24" s="2">
         <v>0.01</v>
       </c>
-      <c r="V24" s="2">
+      <c r="W24" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W24" s="2">
+      <c r="X24" s="2">
         <f>D24^2*E24</f>
         <v>32</v>
       </c>
-      <c r="X24" s="2">
-        <f>L24*W24</f>
+      <c r="Y24" s="2">
+        <f>L24*X24</f>
         <v>3211264</v>
       </c>
-      <c r="Y24" s="2">
-        <f>L24*W24*0.03</f>
+      <c r="Z24" s="2">
+        <f>L24*X24*0.03</f>
         <v>96337.919999999998</v>
       </c>
-      <c r="Z24" s="2">
-        <f>L24*W24*U24*V24</f>
+      <c r="AA24" s="2">
+        <f>L24*X24*V24*W24</f>
         <v>2007.04</v>
       </c>
-      <c r="AA24" s="6">
+      <c r="AB24" s="6">
         <f>D24*J22*J24*F22</f>
         <v>25088</v>
       </c>
-      <c r="AB24" s="2">
-        <f>AA24*0.03</f>
+      <c r="AC24" s="2">
+        <f>AB24*0.03</f>
         <v>752.64</v>
       </c>
-      <c r="AC24" s="11">
+      <c r="AD24" s="11">
         <f>D24*J22</f>
         <v>28</v>
       </c>
-      <c r="AD24" s="14">
-        <f t="shared" ref="AD24:AD25" si="13">X24/AA24</f>
+      <c r="AE24" s="14">
+        <f t="shared" ref="AE24:AE25" si="16">Y24/AB24</f>
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>25</v>
       </c>
@@ -2844,7 +2902,7 @@
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2688</v>
       </c>
       <c r="O25" s="2">
@@ -2852,65 +2910,69 @@
         <v>36864</v>
       </c>
       <c r="P25" s="2">
+        <f t="shared" si="13"/>
+        <v>576</v>
+      </c>
+      <c r="Q25" s="2">
         <f>F25</f>
         <v>128</v>
       </c>
-      <c r="Q25" s="2">
-        <f t="shared" si="11"/>
+      <c r="R25" s="2">
+        <f t="shared" si="14"/>
         <v>36992</v>
       </c>
-      <c r="R25" s="6" t="str">
-        <f t="shared" si="12"/>
+      <c r="S25" s="6" t="str">
+        <f t="shared" si="15"/>
         <v>1C1C_0311</v>
       </c>
-      <c r="S25" s="2" t="str">
+      <c r="T25" s="2" t="str">
         <f>DEC2HEX(F25,4)&amp;"_"&amp;DEC2HEX(E25,4)</f>
         <v>0080_0020</v>
       </c>
-      <c r="T25" s="11" t="str">
+      <c r="U25" s="11" t="str">
         <f>DEC2HEX(D25*H25,4)&amp;"_"&amp;DEC2HEX(D25^2,2)&amp;"00"</f>
         <v>0003_0900</v>
       </c>
-      <c r="U25" s="2">
+      <c r="V25" s="2">
         <v>0.01</v>
       </c>
-      <c r="V25" s="2">
+      <c r="W25" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W25" s="2">
+      <c r="X25" s="2">
         <f>D25^2*E25</f>
         <v>288</v>
       </c>
-      <c r="X25" s="2">
-        <f>L25*W25</f>
+      <c r="Y25" s="2">
+        <f>L25*X25</f>
         <v>28901376</v>
       </c>
-      <c r="Y25" s="2">
-        <f>L25*W25*0.03</f>
+      <c r="Z25" s="2">
+        <f>L25*X25*0.03</f>
         <v>867041.27999999991</v>
       </c>
-      <c r="Z25" s="2">
-        <f>L25*W25*U25*V25</f>
+      <c r="AA25" s="2">
+        <f>L25*X25*V25*W25</f>
         <v>18063.36</v>
       </c>
-      <c r="AA25" s="6">
+      <c r="AB25" s="6">
         <f>D25*J22*J25*F22</f>
         <v>75264</v>
       </c>
-      <c r="AB25" s="2">
-        <f>AA25*0.03</f>
+      <c r="AC25" s="2">
+        <f>AB25*0.03</f>
         <v>2257.92</v>
       </c>
-      <c r="AC25" s="11">
+      <c r="AD25" s="11">
         <f>D25*J22</f>
         <v>84</v>
       </c>
-      <c r="AD25" s="14">
-        <f t="shared" si="13"/>
+      <c r="AE25" s="14">
+        <f t="shared" si="16"/>
         <v>384</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>26</v>
       </c>
@@ -2932,21 +2994,22 @@
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
-      <c r="R26" s="7"/>
-      <c r="S26" s="3"/>
-      <c r="T26" s="12"/>
-      <c r="U26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="7"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="12"/>
       <c r="V26" s="3"/>
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
-      <c r="AA26" s="7"/>
-      <c r="AB26" s="3"/>
-      <c r="AC26" s="12"/>
-      <c r="AD26" s="14"/>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="7"/>
+      <c r="AC26" s="3"/>
+      <c r="AD26" s="12"/>
+      <c r="AE26" s="14"/>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>27</v>
       </c>
@@ -2968,21 +3031,22 @@
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
-      <c r="R27" s="7"/>
-      <c r="S27" s="3"/>
-      <c r="T27" s="12"/>
-      <c r="U27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="12"/>
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
       <c r="X27" s="3"/>
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
-      <c r="AA27" s="7"/>
-      <c r="AB27" s="3"/>
-      <c r="AC27" s="12"/>
-      <c r="AD27" s="14"/>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA27" s="3"/>
+      <c r="AB27" s="7"/>
+      <c r="AC27" s="3"/>
+      <c r="AD27" s="12"/>
+      <c r="AE27" s="14"/>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>28</v>
       </c>
@@ -3010,21 +3074,22 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
-      <c r="R28" s="5"/>
-      <c r="S28" s="1"/>
-      <c r="T28" s="10"/>
-      <c r="U28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="10"/>
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
-      <c r="AA28" s="5"/>
-      <c r="AB28" s="1"/>
-      <c r="AC28" s="10"/>
-      <c r="AD28" s="14"/>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA28" s="1"/>
+      <c r="AB28" s="5"/>
+      <c r="AC28" s="1"/>
+      <c r="AD28" s="10"/>
+      <c r="AE28" s="14"/>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>29</v>
       </c>
@@ -3075,65 +3140,69 @@
         <v>8192</v>
       </c>
       <c r="P29" s="2">
+        <f>D29^2*8*8</f>
+        <v>64</v>
+      </c>
+      <c r="Q29" s="2">
         <f>F29</f>
         <v>32</v>
       </c>
-      <c r="Q29" s="2">
-        <f>O29+P29</f>
+      <c r="R29" s="2">
+        <f>O29+Q29</f>
         <v>8224</v>
       </c>
-      <c r="R29" s="6" t="str">
+      <c r="S29" s="6" t="str">
         <f>DEC2HEX(J29,2)&amp;DEC2HEX(G29,2)&amp;"_"&amp;DEC2HEX(D29,2)&amp;DEC2HEX(H29,1)&amp;DEC2HEX(C29,1)</f>
         <v>1C1C_0111</v>
       </c>
-      <c r="S29" s="2" t="str">
+      <c r="T29" s="2" t="str">
         <f>DEC2HEX(F29,4)&amp;"_"&amp;DEC2HEX(E29,4)</f>
         <v>0020_0100</v>
       </c>
-      <c r="T29" s="11" t="str">
+      <c r="U29" s="11" t="str">
         <f>DEC2HEX(D29*H29,4)&amp;"_"&amp;DEC2HEX(D29^2,2)&amp;"00"</f>
         <v>0001_0100</v>
       </c>
-      <c r="U29" s="2">
+      <c r="V29" s="2">
         <v>0.01</v>
       </c>
-      <c r="V29" s="2">
+      <c r="W29" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W29" s="2">
+      <c r="X29" s="2">
         <f>D29^2*E29</f>
         <v>256</v>
       </c>
-      <c r="X29" s="2">
-        <f>L29*W29</f>
+      <c r="Y29" s="2">
+        <f>L29*X29</f>
         <v>6422528</v>
       </c>
-      <c r="Y29" s="2">
-        <f>L29*W29*0.03</f>
+      <c r="Z29" s="2">
+        <f>L29*X29*0.03</f>
         <v>192675.84</v>
       </c>
-      <c r="Z29" s="2">
-        <f>L29*W29*U29*V29</f>
+      <c r="AA29" s="2">
+        <f>L29*X29*V29*W29</f>
         <v>4014.08</v>
       </c>
-      <c r="AA29" s="6">
+      <c r="AB29" s="6">
         <f>D29*J28*J29*F28</f>
         <v>200704</v>
       </c>
-      <c r="AB29" s="2">
-        <f>AA29*0.03</f>
+      <c r="AC29" s="2">
+        <f>AB29*0.03</f>
         <v>6021.12</v>
       </c>
-      <c r="AC29" s="11">
+      <c r="AD29" s="11">
         <f>D29*J28</f>
         <v>28</v>
       </c>
-      <c r="AD29" s="14">
-        <f>X29/AA29</f>
+      <c r="AE29" s="14">
+        <f>Y29/AB29</f>
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>30</v>
       </c>
@@ -3155,21 +3224,22 @@
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
-      <c r="R30" s="7"/>
-      <c r="S30" s="3"/>
-      <c r="T30" s="12"/>
-      <c r="U30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="3"/>
+      <c r="U30" s="12"/>
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
       <c r="X30" s="3"/>
       <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
-      <c r="AA30" s="7"/>
-      <c r="AB30" s="3"/>
-      <c r="AC30" s="12"/>
-      <c r="AD30" s="14"/>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="7"/>
+      <c r="AC30" s="3"/>
+      <c r="AD30" s="12"/>
+      <c r="AE30" s="14"/>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>31</v>
       </c>
@@ -3209,7 +3279,7 @@
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2">
-        <f t="shared" ref="N31:N32" si="14">G31*E31*D31</f>
+        <f t="shared" ref="N31:N32" si="17">G31*E31*D31</f>
         <v>896</v>
       </c>
       <c r="O31" s="2">
@@ -3217,65 +3287,69 @@
         <v>4096</v>
       </c>
       <c r="P31" s="2">
+        <f t="shared" ref="P31:P32" si="18">D31^2*8*8</f>
+        <v>64</v>
+      </c>
+      <c r="Q31" s="2">
         <f>F31</f>
         <v>128</v>
       </c>
-      <c r="Q31" s="2">
-        <f t="shared" ref="Q31:Q32" si="15">O31+P31</f>
+      <c r="R31" s="2">
+        <f t="shared" ref="R31:R32" si="19">O31+Q31</f>
         <v>4224</v>
       </c>
-      <c r="R31" s="6" t="str">
-        <f t="shared" ref="R31:R32" si="16">DEC2HEX(J31,2)&amp;DEC2HEX(G31,2)&amp;"_"&amp;DEC2HEX(D31,2)&amp;DEC2HEX(H31,1)&amp;DEC2HEX(C31,1)</f>
+      <c r="S31" s="6" t="str">
+        <f t="shared" ref="S31:S32" si="20">DEC2HEX(J31,2)&amp;DEC2HEX(G31,2)&amp;"_"&amp;DEC2HEX(D31,2)&amp;DEC2HEX(H31,1)&amp;DEC2HEX(C31,1)</f>
         <v>1C1C_0111</v>
       </c>
-      <c r="S31" s="2" t="str">
+      <c r="T31" s="2" t="str">
         <f>DEC2HEX(F31,4)&amp;"_"&amp;DEC2HEX(E31,4)</f>
         <v>0080_0020</v>
       </c>
-      <c r="T31" s="11" t="str">
+      <c r="U31" s="11" t="str">
         <f>DEC2HEX(D31*H31,4)&amp;"_"&amp;DEC2HEX(D31^2,2)&amp;"00"</f>
         <v>0001_0100</v>
       </c>
-      <c r="U31" s="2">
+      <c r="V31" s="2">
         <v>0.01</v>
       </c>
-      <c r="V31" s="2">
+      <c r="W31" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W31" s="2">
+      <c r="X31" s="2">
         <f>D31^2*E31</f>
         <v>32</v>
       </c>
-      <c r="X31" s="2">
-        <f>L31*W31</f>
+      <c r="Y31" s="2">
+        <f>L31*X31</f>
         <v>3211264</v>
       </c>
-      <c r="Y31" s="2">
-        <f>L31*W31*0.03</f>
+      <c r="Z31" s="2">
+        <f>L31*X31*0.03</f>
         <v>96337.919999999998</v>
       </c>
-      <c r="Z31" s="2">
-        <f>L31*W31*U31*V31</f>
+      <c r="AA31" s="2">
+        <f>L31*X31*V31*W31</f>
         <v>2007.04</v>
       </c>
-      <c r="AA31" s="6">
+      <c r="AB31" s="6">
         <f>D31*J29*J31*F29</f>
         <v>25088</v>
       </c>
-      <c r="AB31" s="2">
-        <f>AA31*0.03</f>
+      <c r="AC31" s="2">
+        <f>AB31*0.03</f>
         <v>752.64</v>
       </c>
-      <c r="AC31" s="11">
+      <c r="AD31" s="11">
         <f>D31*J29</f>
         <v>28</v>
       </c>
-      <c r="AD31" s="14">
-        <f t="shared" ref="AD31:AD32" si="17">X31/AA31</f>
+      <c r="AE31" s="14">
+        <f t="shared" ref="AE31:AE32" si="21">Y31/AB31</f>
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>32</v>
       </c>
@@ -3315,7 +3389,7 @@
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>2688</v>
       </c>
       <c r="O32" s="2">
@@ -3323,65 +3397,69 @@
         <v>36864</v>
       </c>
       <c r="P32" s="2">
+        <f t="shared" si="18"/>
+        <v>576</v>
+      </c>
+      <c r="Q32" s="2">
         <f>F32</f>
         <v>128</v>
       </c>
-      <c r="Q32" s="2">
-        <f t="shared" si="15"/>
+      <c r="R32" s="2">
+        <f t="shared" si="19"/>
         <v>36992</v>
       </c>
-      <c r="R32" s="6" t="str">
-        <f t="shared" si="16"/>
+      <c r="S32" s="6" t="str">
+        <f t="shared" si="20"/>
         <v>1C1C_0311</v>
       </c>
-      <c r="S32" s="2" t="str">
+      <c r="T32" s="2" t="str">
         <f>DEC2HEX(F32,4)&amp;"_"&amp;DEC2HEX(E32,4)</f>
         <v>0080_0020</v>
       </c>
-      <c r="T32" s="11" t="str">
+      <c r="U32" s="11" t="str">
         <f>DEC2HEX(D32*H32,4)&amp;"_"&amp;DEC2HEX(D32^2,2)&amp;"00"</f>
         <v>0003_0900</v>
       </c>
-      <c r="U32" s="2">
+      <c r="V32" s="2">
         <v>0.01</v>
       </c>
-      <c r="V32" s="2">
+      <c r="W32" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W32" s="2">
+      <c r="X32" s="2">
         <f>D32^2*E32</f>
         <v>288</v>
       </c>
-      <c r="X32" s="2">
-        <f>L32*W32</f>
+      <c r="Y32" s="2">
+        <f>L32*X32</f>
         <v>28901376</v>
       </c>
-      <c r="Y32" s="2">
-        <f>L32*W32*0.03</f>
+      <c r="Z32" s="2">
+        <f>L32*X32*0.03</f>
         <v>867041.27999999991</v>
       </c>
-      <c r="Z32" s="2">
-        <f>L32*W32*U32*V32</f>
+      <c r="AA32" s="2">
+        <f>L32*X32*V32*W32</f>
         <v>18063.36</v>
       </c>
-      <c r="AA32" s="6">
+      <c r="AB32" s="6">
         <f>D32*J29*J32*F29</f>
         <v>75264</v>
       </c>
-      <c r="AB32" s="2">
-        <f>AA32*0.03</f>
+      <c r="AC32" s="2">
+        <f>AB32*0.03</f>
         <v>2257.92</v>
       </c>
-      <c r="AC32" s="11">
+      <c r="AD32" s="11">
         <f>D32*J29</f>
         <v>84</v>
       </c>
-      <c r="AD32" s="14">
-        <f t="shared" si="17"/>
+      <c r="AE32" s="14">
+        <f t="shared" si="21"/>
         <v>384</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>33</v>
       </c>
@@ -3403,21 +3481,22 @@
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
       <c r="Q33" s="3"/>
-      <c r="R33" s="7"/>
-      <c r="S33" s="3"/>
-      <c r="T33" s="12"/>
-      <c r="U33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="3"/>
+      <c r="U33" s="12"/>
       <c r="V33" s="3"/>
       <c r="W33" s="3"/>
       <c r="X33" s="3"/>
       <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
-      <c r="AA33" s="7"/>
-      <c r="AB33" s="3"/>
-      <c r="AC33" s="12"/>
-      <c r="AD33" s="14"/>
-    </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA33" s="3"/>
+      <c r="AB33" s="7"/>
+      <c r="AC33" s="3"/>
+      <c r="AD33" s="12"/>
+      <c r="AE33" s="14"/>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>34</v>
       </c>
@@ -3439,21 +3518,22 @@
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
       <c r="Q34" s="3"/>
-      <c r="R34" s="7"/>
-      <c r="S34" s="3"/>
-      <c r="T34" s="12"/>
-      <c r="U34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="3"/>
+      <c r="U34" s="12"/>
       <c r="V34" s="3"/>
       <c r="W34" s="3"/>
       <c r="X34" s="3"/>
       <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
-      <c r="AA34" s="7"/>
-      <c r="AB34" s="3"/>
-      <c r="AC34" s="12"/>
-      <c r="AD34" s="14"/>
-    </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA34" s="3"/>
+      <c r="AB34" s="7"/>
+      <c r="AC34" s="3"/>
+      <c r="AD34" s="12"/>
+      <c r="AE34" s="14"/>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>35</v>
       </c>
@@ -3481,21 +3561,22 @@
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
-      <c r="R35" s="5"/>
-      <c r="S35" s="1"/>
-      <c r="T35" s="10"/>
-      <c r="U35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="5"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="10"/>
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
       <c r="X35" s="1"/>
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
-      <c r="AA35" s="5"/>
-      <c r="AB35" s="1"/>
-      <c r="AC35" s="10"/>
-      <c r="AD35" s="14"/>
-    </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA35" s="1"/>
+      <c r="AB35" s="5"/>
+      <c r="AC35" s="1"/>
+      <c r="AD35" s="10"/>
+      <c r="AE35" s="14"/>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>36</v>
       </c>
@@ -3541,58 +3622,59 @@
       <c r="O36" s="4"/>
       <c r="P36" s="4"/>
       <c r="Q36" s="4"/>
-      <c r="R36" s="8" t="str">
+      <c r="R36" s="4"/>
+      <c r="S36" s="8" t="str">
         <f>DEC2HEX(J36,2)&amp;DEC2HEX(G36,2)&amp;"_"&amp;DEC2HEX(D36,2)&amp;DEC2HEX(H36,1)&amp;DEC2HEX(C36,1)</f>
         <v>0E1C_0322</v>
       </c>
-      <c r="S36" s="4" t="str">
+      <c r="T36" s="4" t="str">
         <f>DEC2HEX(F36,4)&amp;"_"&amp;DEC2HEX(F36,4)</f>
         <v>0100_0100</v>
       </c>
-      <c r="T36" s="13" t="str">
+      <c r="U36" s="13" t="str">
         <f>DEC2HEX(D36*H36,4)&amp;"_"&amp;DEC2HEX(D36^2,2)&amp;"00"</f>
         <v>0006_0900</v>
       </c>
-      <c r="U36" s="4">
+      <c r="V36" s="4">
         <v>0.01</v>
       </c>
-      <c r="V36" s="4">
+      <c r="W36" s="4">
         <v>6.25E-2</v>
       </c>
-      <c r="W36" s="4">
+      <c r="X36" s="4">
         <f>D36^2*E36</f>
         <v>9</v>
       </c>
-      <c r="X36" s="4">
-        <f>L36*W36</f>
+      <c r="Y36" s="4">
+        <f>L36*X36</f>
         <v>451584</v>
       </c>
-      <c r="Y36" s="4">
-        <f>L36*W36*0.03</f>
+      <c r="Z36" s="4">
+        <f>L36*X36*0.03</f>
         <v>13547.519999999999</v>
       </c>
-      <c r="Z36" s="4">
-        <f>L36*W36*U36*V36</f>
+      <c r="AA36" s="4">
+        <f>L36*X36*V36*W36</f>
         <v>282.24</v>
       </c>
-      <c r="AA36" s="8">
+      <c r="AB36" s="8">
         <f>D36*J35*J36*F35</f>
         <v>301056</v>
       </c>
-      <c r="AB36" s="4">
-        <f>AA36*0.03</f>
+      <c r="AC36" s="4">
+        <f>AB36*0.03</f>
         <v>9031.68</v>
       </c>
-      <c r="AC36" s="13">
+      <c r="AD36" s="13">
         <f>D36*J35</f>
         <v>84</v>
       </c>
-      <c r="AD36" s="14">
-        <f t="shared" ref="AD36:AD37" si="18">X36/AA36</f>
+      <c r="AE36" s="14">
+        <f t="shared" ref="AE36:AE37" si="22">Y36/AB36</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>37</v>
       </c>
@@ -3643,65 +3725,69 @@
         <v>12288</v>
       </c>
       <c r="P37" s="2">
+        <f>D37^2*8*8</f>
+        <v>64</v>
+      </c>
+      <c r="Q37" s="2">
         <f>F37</f>
         <v>48</v>
       </c>
-      <c r="Q37" s="2">
-        <f>O37+P37</f>
+      <c r="R37" s="2">
+        <f>O37+Q37</f>
         <v>12336</v>
       </c>
-      <c r="R37" s="6" t="str">
+      <c r="S37" s="6" t="str">
         <f>DEC2HEX(J37,2)&amp;DEC2HEX(G37,2)&amp;"_"&amp;DEC2HEX(D37,2)&amp;DEC2HEX(H37,1)&amp;DEC2HEX(C37,1)</f>
         <v>0E0E_0111</v>
       </c>
-      <c r="S37" s="2" t="str">
+      <c r="T37" s="2" t="str">
         <f>DEC2HEX(F37,4)&amp;"_"&amp;DEC2HEX(E37,4)</f>
         <v>0030_0100</v>
       </c>
-      <c r="T37" s="11" t="str">
+      <c r="U37" s="11" t="str">
         <f>DEC2HEX(D37*H37,4)&amp;"_"&amp;DEC2HEX(D37^2,2)&amp;"00"</f>
         <v>0001_0100</v>
       </c>
-      <c r="U37" s="2">
+      <c r="V37" s="2">
         <v>0.01</v>
       </c>
-      <c r="V37" s="2">
+      <c r="W37" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W37" s="2">
+      <c r="X37" s="2">
         <f>D37^2*E37</f>
         <v>256</v>
       </c>
-      <c r="X37" s="2">
-        <f>L37*W37</f>
+      <c r="Y37" s="2">
+        <f>L37*X37</f>
         <v>2408448</v>
       </c>
-      <c r="Y37" s="2">
-        <f>L37*W37*0.03</f>
+      <c r="Z37" s="2">
+        <f>L37*X37*0.03</f>
         <v>72253.440000000002</v>
       </c>
-      <c r="Z37" s="2">
-        <f>L37*W37*U37*V37</f>
+      <c r="AA37" s="2">
+        <f>L37*X37*V37*W37</f>
         <v>1505.28</v>
       </c>
-      <c r="AA37" s="6">
+      <c r="AB37" s="6">
         <f>D37*J36*J37*F36</f>
         <v>50176</v>
       </c>
-      <c r="AB37" s="2">
-        <f>AA37*0.03</f>
+      <c r="AC37" s="2">
+        <f>AB37*0.03</f>
         <v>1505.28</v>
       </c>
-      <c r="AC37" s="11">
+      <c r="AD37" s="11">
         <f>D37*J36</f>
         <v>14</v>
       </c>
-      <c r="AD37" s="14">
-        <f t="shared" si="18"/>
+      <c r="AE37" s="14">
+        <f t="shared" si="22"/>
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>38</v>
       </c>
@@ -3723,21 +3809,22 @@
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
       <c r="Q38" s="3"/>
-      <c r="R38" s="7"/>
-      <c r="S38" s="3"/>
-      <c r="T38" s="12"/>
-      <c r="U38" s="3"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="7"/>
+      <c r="T38" s="3"/>
+      <c r="U38" s="12"/>
       <c r="V38" s="3"/>
       <c r="W38" s="3"/>
       <c r="X38" s="3"/>
       <c r="Y38" s="3"/>
       <c r="Z38" s="3"/>
-      <c r="AA38" s="7"/>
-      <c r="AB38" s="3"/>
-      <c r="AC38" s="12"/>
-      <c r="AD38" s="14"/>
-    </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA38" s="3"/>
+      <c r="AB38" s="7"/>
+      <c r="AC38" s="3"/>
+      <c r="AD38" s="12"/>
+      <c r="AE38" s="14"/>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>39</v>
       </c>
@@ -3777,7 +3864,7 @@
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2">
-        <f t="shared" ref="N39:N40" si="19">G39*E39*D39</f>
+        <f t="shared" ref="N39:N40" si="23">G39*E39*D39</f>
         <v>672</v>
       </c>
       <c r="O39" s="2">
@@ -3785,65 +3872,69 @@
         <v>9216</v>
       </c>
       <c r="P39" s="2">
+        <f t="shared" ref="P39:P40" si="24">D39^2*8*8</f>
+        <v>64</v>
+      </c>
+      <c r="Q39" s="2">
         <f>F39</f>
         <v>192</v>
       </c>
-      <c r="Q39" s="2">
-        <f t="shared" ref="Q39:Q40" si="20">O39+P39</f>
+      <c r="R39" s="2">
+        <f t="shared" ref="R39:R40" si="25">O39+Q39</f>
         <v>9408</v>
       </c>
-      <c r="R39" s="6" t="str">
-        <f t="shared" ref="R39:R40" si="21">DEC2HEX(J39,2)&amp;DEC2HEX(G39,2)&amp;"_"&amp;DEC2HEX(D39,2)&amp;DEC2HEX(H39,1)&amp;DEC2HEX(C39,1)</f>
+      <c r="S39" s="6" t="str">
+        <f t="shared" ref="S39:S40" si="26">DEC2HEX(J39,2)&amp;DEC2HEX(G39,2)&amp;"_"&amp;DEC2HEX(D39,2)&amp;DEC2HEX(H39,1)&amp;DEC2HEX(C39,1)</f>
         <v>0E0E_0111</v>
       </c>
-      <c r="S39" s="2" t="str">
+      <c r="T39" s="2" t="str">
         <f>DEC2HEX(F39,4)&amp;"_"&amp;DEC2HEX(E39,4)</f>
         <v>00C0_0030</v>
       </c>
-      <c r="T39" s="11" t="str">
+      <c r="U39" s="11" t="str">
         <f>DEC2HEX(D39*H39,4)&amp;"_"&amp;DEC2HEX(D39^2,2)&amp;"00"</f>
         <v>0001_0100</v>
       </c>
-      <c r="U39" s="2">
+      <c r="V39" s="2">
         <v>0.01</v>
       </c>
-      <c r="V39" s="2">
+      <c r="W39" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W39" s="2">
+      <c r="X39" s="2">
         <f>D39^2*E39</f>
         <v>48</v>
       </c>
-      <c r="X39" s="2">
-        <f>L39*W39</f>
+      <c r="Y39" s="2">
+        <f>L39*X39</f>
         <v>1806336</v>
       </c>
-      <c r="Y39" s="2">
-        <f>L39*W39*0.03</f>
+      <c r="Z39" s="2">
+        <f>L39*X39*0.03</f>
         <v>54190.079999999994</v>
       </c>
-      <c r="Z39" s="2">
-        <f>L39*W39*U39*V39</f>
+      <c r="AA39" s="2">
+        <f>L39*X39*V39*W39</f>
         <v>1128.96</v>
       </c>
-      <c r="AA39" s="6">
+      <c r="AB39" s="6">
         <f>D39*J37*J39*F37</f>
         <v>9408</v>
       </c>
-      <c r="AB39" s="2">
-        <f>AA39*0.03</f>
+      <c r="AC39" s="2">
+        <f>AB39*0.03</f>
         <v>282.24</v>
       </c>
-      <c r="AC39" s="11">
+      <c r="AD39" s="11">
         <f>D39*J37</f>
         <v>14</v>
       </c>
-      <c r="AD39" s="14">
-        <f t="shared" ref="AD39:AD40" si="22">X39/AA39</f>
+      <c r="AE39" s="14">
+        <f t="shared" ref="AE39:AE40" si="27">Y39/AB39</f>
         <v>192</v>
       </c>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>40</v>
       </c>
@@ -3883,7 +3974,7 @@
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>2016</v>
       </c>
       <c r="O40" s="2">
@@ -3891,65 +3982,69 @@
         <v>82944</v>
       </c>
       <c r="P40" s="2">
+        <f t="shared" si="24"/>
+        <v>576</v>
+      </c>
+      <c r="Q40" s="2">
         <f>F40</f>
         <v>192</v>
       </c>
-      <c r="Q40" s="2">
-        <f t="shared" si="20"/>
+      <c r="R40" s="2">
+        <f t="shared" si="25"/>
         <v>83136</v>
       </c>
-      <c r="R40" s="6" t="str">
-        <f t="shared" si="21"/>
+      <c r="S40" s="6" t="str">
+        <f t="shared" si="26"/>
         <v>0E0E_0311</v>
       </c>
-      <c r="S40" s="2" t="str">
+      <c r="T40" s="2" t="str">
         <f>DEC2HEX(F40,4)&amp;"_"&amp;DEC2HEX(E40,4)</f>
         <v>00C0_0030</v>
       </c>
-      <c r="T40" s="11" t="str">
+      <c r="U40" s="11" t="str">
         <f>DEC2HEX(D40*H40,4)&amp;"_"&amp;DEC2HEX(D40^2,2)&amp;"00"</f>
         <v>0003_0900</v>
       </c>
-      <c r="U40" s="2">
+      <c r="V40" s="2">
         <v>0.01</v>
       </c>
-      <c r="V40" s="2">
+      <c r="W40" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W40" s="2">
+      <c r="X40" s="2">
         <f>D40^2*E40</f>
         <v>432</v>
       </c>
-      <c r="X40" s="2">
-        <f>L40*W40</f>
+      <c r="Y40" s="2">
+        <f>L40*X40</f>
         <v>16257024</v>
       </c>
-      <c r="Y40" s="2">
-        <f>L40*W40*0.03</f>
+      <c r="Z40" s="2">
+        <f>L40*X40*0.03</f>
         <v>487710.71999999997</v>
       </c>
-      <c r="Z40" s="2">
-        <f>L40*W40*U40*V40</f>
+      <c r="AA40" s="2">
+        <f>L40*X40*V40*W40</f>
         <v>10160.64</v>
       </c>
-      <c r="AA40" s="6">
+      <c r="AB40" s="6">
         <f>D40*J37*J40*F37</f>
         <v>28224</v>
       </c>
-      <c r="AB40" s="2">
-        <f>AA40*0.03</f>
+      <c r="AC40" s="2">
+        <f>AB40*0.03</f>
         <v>846.71999999999991</v>
       </c>
-      <c r="AC40" s="11">
+      <c r="AD40" s="11">
         <f>D40*J37</f>
         <v>42</v>
       </c>
-      <c r="AD40" s="14">
-        <f t="shared" si="22"/>
+      <c r="AE40" s="14">
+        <f t="shared" si="27"/>
         <v>576</v>
       </c>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>41</v>
       </c>
@@ -3971,21 +4066,22 @@
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
       <c r="Q41" s="3"/>
-      <c r="R41" s="7"/>
-      <c r="S41" s="3"/>
-      <c r="T41" s="12"/>
-      <c r="U41" s="3"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="7"/>
+      <c r="T41" s="3"/>
+      <c r="U41" s="12"/>
       <c r="V41" s="3"/>
       <c r="W41" s="3"/>
       <c r="X41" s="3"/>
       <c r="Y41" s="3"/>
       <c r="Z41" s="3"/>
-      <c r="AA41" s="7"/>
-      <c r="AB41" s="3"/>
-      <c r="AC41" s="12"/>
-      <c r="AD41" s="14"/>
-    </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA41" s="3"/>
+      <c r="AB41" s="7"/>
+      <c r="AC41" s="3"/>
+      <c r="AD41" s="12"/>
+      <c r="AE41" s="14"/>
+    </row>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>42</v>
       </c>
@@ -4007,21 +4103,22 @@
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
       <c r="Q42" s="3"/>
-      <c r="R42" s="7"/>
-      <c r="S42" s="3"/>
-      <c r="T42" s="12"/>
-      <c r="U42" s="3"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="7"/>
+      <c r="T42" s="3"/>
+      <c r="U42" s="12"/>
       <c r="V42" s="3"/>
       <c r="W42" s="3"/>
       <c r="X42" s="3"/>
       <c r="Y42" s="3"/>
       <c r="Z42" s="3"/>
-      <c r="AA42" s="7"/>
-      <c r="AB42" s="3"/>
-      <c r="AC42" s="12"/>
-      <c r="AD42" s="14"/>
-    </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA42" s="3"/>
+      <c r="AB42" s="7"/>
+      <c r="AC42" s="3"/>
+      <c r="AD42" s="12"/>
+      <c r="AE42" s="14"/>
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>43</v>
       </c>
@@ -4049,21 +4146,22 @@
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
-      <c r="R43" s="5"/>
-      <c r="S43" s="1"/>
-      <c r="T43" s="10"/>
-      <c r="U43" s="1"/>
+      <c r="R43" s="1"/>
+      <c r="S43" s="5"/>
+      <c r="T43" s="1"/>
+      <c r="U43" s="10"/>
       <c r="V43" s="1"/>
       <c r="W43" s="1"/>
       <c r="X43" s="1"/>
       <c r="Y43" s="1"/>
       <c r="Z43" s="1"/>
-      <c r="AA43" s="5"/>
-      <c r="AB43" s="1"/>
-      <c r="AC43" s="10"/>
-      <c r="AD43" s="14"/>
-    </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA43" s="1"/>
+      <c r="AB43" s="5"/>
+      <c r="AC43" s="1"/>
+      <c r="AD43" s="10"/>
+      <c r="AE43" s="14"/>
+    </row>
+    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>44</v>
       </c>
@@ -4114,65 +4212,69 @@
         <v>18432</v>
       </c>
       <c r="P44" s="2">
+        <f>D44^2*8*8</f>
+        <v>64</v>
+      </c>
+      <c r="Q44" s="2">
         <f>F44</f>
         <v>48</v>
       </c>
-      <c r="Q44" s="2">
-        <f>O44+P44</f>
+      <c r="R44" s="2">
+        <f>O44+Q44</f>
         <v>18480</v>
       </c>
-      <c r="R44" s="6" t="str">
+      <c r="S44" s="6" t="str">
         <f>DEC2HEX(J44,2)&amp;DEC2HEX(G44,2)&amp;"_"&amp;DEC2HEX(D44,2)&amp;DEC2HEX(H44,1)&amp;DEC2HEX(C44,1)</f>
         <v>0E0E_0111</v>
       </c>
-      <c r="S44" s="2" t="str">
+      <c r="T44" s="2" t="str">
         <f>DEC2HEX(F44,4)&amp;"_"&amp;DEC2HEX(E44,4)</f>
         <v>0030_0180</v>
       </c>
-      <c r="T44" s="11" t="str">
+      <c r="U44" s="11" t="str">
         <f>DEC2HEX(D44*H44,4)&amp;"_"&amp;DEC2HEX(D44^2,2)&amp;"00"</f>
         <v>0001_0100</v>
       </c>
-      <c r="U44" s="2">
+      <c r="V44" s="2">
         <v>0.01</v>
       </c>
-      <c r="V44" s="2">
+      <c r="W44" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W44" s="2">
+      <c r="X44" s="2">
         <f>D44^2*E44</f>
         <v>384</v>
       </c>
-      <c r="X44" s="2">
-        <f>L44*W44</f>
+      <c r="Y44" s="2">
+        <f>L44*X44</f>
         <v>3612672</v>
       </c>
-      <c r="Y44" s="2">
-        <f>L44*W44*0.03</f>
+      <c r="Z44" s="2">
+        <f>L44*X44*0.03</f>
         <v>108380.15999999999</v>
       </c>
-      <c r="Z44" s="2">
-        <f>L44*W44*U44*V44</f>
+      <c r="AA44" s="2">
+        <f>L44*X44*V44*W44</f>
         <v>2257.92</v>
       </c>
-      <c r="AA44" s="6">
+      <c r="AB44" s="6">
         <f>D44*J43*J44*F43</f>
         <v>75264</v>
       </c>
-      <c r="AB44" s="2">
-        <f>AA44*0.03</f>
+      <c r="AC44" s="2">
+        <f>AB44*0.03</f>
         <v>2257.92</v>
       </c>
-      <c r="AC44" s="11">
+      <c r="AD44" s="11">
         <f>D44*J43</f>
         <v>14</v>
       </c>
-      <c r="AD44" s="14">
-        <f>X44/AA44</f>
+      <c r="AE44" s="14">
+        <f>Y44/AB44</f>
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>45</v>
       </c>
@@ -4194,21 +4296,22 @@
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
       <c r="Q45" s="3"/>
-      <c r="R45" s="7"/>
-      <c r="S45" s="3"/>
-      <c r="T45" s="12"/>
-      <c r="U45" s="3"/>
+      <c r="R45" s="3"/>
+      <c r="S45" s="7"/>
+      <c r="T45" s="3"/>
+      <c r="U45" s="12"/>
       <c r="V45" s="3"/>
       <c r="W45" s="3"/>
       <c r="X45" s="3"/>
       <c r="Y45" s="3"/>
       <c r="Z45" s="3"/>
-      <c r="AA45" s="7"/>
-      <c r="AB45" s="3"/>
-      <c r="AC45" s="12"/>
-      <c r="AD45" s="14"/>
-    </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA45" s="3"/>
+      <c r="AB45" s="7"/>
+      <c r="AC45" s="3"/>
+      <c r="AD45" s="12"/>
+      <c r="AE45" s="14"/>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>46</v>
       </c>
@@ -4248,7 +4351,7 @@
       </c>
       <c r="M46" s="2"/>
       <c r="N46" s="2">
-        <f t="shared" ref="N46:N47" si="23">G46*E46*D46</f>
+        <f t="shared" ref="N46:N47" si="28">G46*E46*D46</f>
         <v>672</v>
       </c>
       <c r="O46" s="2">
@@ -4256,65 +4359,69 @@
         <v>9216</v>
       </c>
       <c r="P46" s="2">
+        <f t="shared" ref="P46:P47" si="29">D46^2*8*8</f>
+        <v>64</v>
+      </c>
+      <c r="Q46" s="2">
         <f>F46</f>
         <v>192</v>
       </c>
-      <c r="Q46" s="2">
-        <f t="shared" ref="Q46:Q47" si="24">O46+P46</f>
+      <c r="R46" s="2">
+        <f t="shared" ref="R46:R47" si="30">O46+Q46</f>
         <v>9408</v>
       </c>
-      <c r="R46" s="6" t="str">
-        <f t="shared" ref="R46:R47" si="25">DEC2HEX(J46,2)&amp;DEC2HEX(G46,2)&amp;"_"&amp;DEC2HEX(D46,2)&amp;DEC2HEX(H46,1)&amp;DEC2HEX(C46,1)</f>
+      <c r="S46" s="6" t="str">
+        <f t="shared" ref="S46:S47" si="31">DEC2HEX(J46,2)&amp;DEC2HEX(G46,2)&amp;"_"&amp;DEC2HEX(D46,2)&amp;DEC2HEX(H46,1)&amp;DEC2HEX(C46,1)</f>
         <v>0E0E_0111</v>
       </c>
-      <c r="S46" s="2" t="str">
+      <c r="T46" s="2" t="str">
         <f>DEC2HEX(F46,4)&amp;"_"&amp;DEC2HEX(E46,4)</f>
         <v>00C0_0030</v>
       </c>
-      <c r="T46" s="11" t="str">
+      <c r="U46" s="11" t="str">
         <f>DEC2HEX(D46*H46,4)&amp;"_"&amp;DEC2HEX(D46^2,2)&amp;"00"</f>
         <v>0001_0100</v>
       </c>
-      <c r="U46" s="2">
+      <c r="V46" s="2">
         <v>0.01</v>
       </c>
-      <c r="V46" s="2">
+      <c r="W46" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W46" s="2">
+      <c r="X46" s="2">
         <f>D46^2*E46</f>
         <v>48</v>
       </c>
-      <c r="X46" s="2">
-        <f>L46*W46</f>
+      <c r="Y46" s="2">
+        <f>L46*X46</f>
         <v>1806336</v>
       </c>
-      <c r="Y46" s="2">
-        <f>L46*W46*0.03</f>
+      <c r="Z46" s="2">
+        <f>L46*X46*0.03</f>
         <v>54190.079999999994</v>
       </c>
-      <c r="Z46" s="2">
-        <f>L46*W46*U46*V46</f>
+      <c r="AA46" s="2">
+        <f>L46*X46*V46*W46</f>
         <v>1128.96</v>
       </c>
-      <c r="AA46" s="6">
+      <c r="AB46" s="6">
         <f>D46*J44*J46*F44</f>
         <v>9408</v>
       </c>
-      <c r="AB46" s="2">
-        <f>AA46*0.03</f>
+      <c r="AC46" s="2">
+        <f>AB46*0.03</f>
         <v>282.24</v>
       </c>
-      <c r="AC46" s="11">
+      <c r="AD46" s="11">
         <f>D46*J44</f>
         <v>14</v>
       </c>
-      <c r="AD46" s="14">
-        <f t="shared" ref="AD46:AD47" si="26">X46/AA46</f>
+      <c r="AE46" s="14">
+        <f t="shared" ref="AE46:AE47" si="32">Y46/AB46</f>
         <v>192</v>
       </c>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>47</v>
       </c>
@@ -4354,7 +4461,7 @@
       </c>
       <c r="M47" s="2"/>
       <c r="N47" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>2016</v>
       </c>
       <c r="O47" s="2">
@@ -4362,65 +4469,69 @@
         <v>82944</v>
       </c>
       <c r="P47" s="2">
+        <f t="shared" si="29"/>
+        <v>576</v>
+      </c>
+      <c r="Q47" s="2">
         <f>F47</f>
         <v>192</v>
       </c>
-      <c r="Q47" s="2">
-        <f t="shared" si="24"/>
+      <c r="R47" s="2">
+        <f t="shared" si="30"/>
         <v>83136</v>
       </c>
-      <c r="R47" s="6" t="str">
-        <f t="shared" si="25"/>
+      <c r="S47" s="6" t="str">
+        <f t="shared" si="31"/>
         <v>0E0E_0311</v>
       </c>
-      <c r="S47" s="2" t="str">
+      <c r="T47" s="2" t="str">
         <f>DEC2HEX(F47,4)&amp;"_"&amp;DEC2HEX(E47,4)</f>
         <v>00C0_0030</v>
       </c>
-      <c r="T47" s="11" t="str">
+      <c r="U47" s="11" t="str">
         <f>DEC2HEX(D47*H47,4)&amp;"_"&amp;DEC2HEX(D47^2,2)&amp;"00"</f>
         <v>0003_0900</v>
       </c>
-      <c r="U47" s="2">
+      <c r="V47" s="2">
         <v>0.01</v>
       </c>
-      <c r="V47" s="2">
+      <c r="W47" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W47" s="2">
+      <c r="X47" s="2">
         <f>D47^2*E47</f>
         <v>432</v>
       </c>
-      <c r="X47" s="2">
-        <f>L47*W47</f>
+      <c r="Y47" s="2">
+        <f>L47*X47</f>
         <v>16257024</v>
       </c>
-      <c r="Y47" s="2">
-        <f>L47*W47*0.03</f>
+      <c r="Z47" s="2">
+        <f>L47*X47*0.03</f>
         <v>487710.71999999997</v>
       </c>
-      <c r="Z47" s="2">
-        <f>L47*W47*U47*V47</f>
+      <c r="AA47" s="2">
+        <f>L47*X47*V47*W47</f>
         <v>10160.64</v>
       </c>
-      <c r="AA47" s="6">
+      <c r="AB47" s="6">
         <f>D47*J44*J47*F44</f>
         <v>28224</v>
       </c>
-      <c r="AB47" s="2">
-        <f>AA47*0.03</f>
+      <c r="AC47" s="2">
+        <f>AB47*0.03</f>
         <v>846.71999999999991</v>
       </c>
-      <c r="AC47" s="11">
+      <c r="AD47" s="11">
         <f>D47*J44</f>
         <v>42</v>
       </c>
-      <c r="AD47" s="14">
-        <f t="shared" si="26"/>
+      <c r="AE47" s="14">
+        <f t="shared" si="32"/>
         <v>576</v>
       </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>48</v>
       </c>
@@ -4442,21 +4553,22 @@
       <c r="O48" s="3"/>
       <c r="P48" s="3"/>
       <c r="Q48" s="3"/>
-      <c r="R48" s="7"/>
-      <c r="S48" s="3"/>
-      <c r="T48" s="12"/>
-      <c r="U48" s="3"/>
+      <c r="R48" s="3"/>
+      <c r="S48" s="7"/>
+      <c r="T48" s="3"/>
+      <c r="U48" s="12"/>
       <c r="V48" s="3"/>
       <c r="W48" s="3"/>
       <c r="X48" s="3"/>
       <c r="Y48" s="3"/>
       <c r="Z48" s="3"/>
-      <c r="AA48" s="7"/>
-      <c r="AB48" s="3"/>
-      <c r="AC48" s="12"/>
-      <c r="AD48" s="14"/>
-    </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA48" s="3"/>
+      <c r="AB48" s="7"/>
+      <c r="AC48" s="3"/>
+      <c r="AD48" s="12"/>
+      <c r="AE48" s="14"/>
+    </row>
+    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>49</v>
       </c>
@@ -4478,21 +4590,22 @@
       <c r="O49" s="3"/>
       <c r="P49" s="3"/>
       <c r="Q49" s="3"/>
-      <c r="R49" s="7"/>
-      <c r="S49" s="3"/>
-      <c r="T49" s="12"/>
-      <c r="U49" s="3"/>
+      <c r="R49" s="3"/>
+      <c r="S49" s="7"/>
+      <c r="T49" s="3"/>
+      <c r="U49" s="12"/>
       <c r="V49" s="3"/>
       <c r="W49" s="3"/>
       <c r="X49" s="3"/>
       <c r="Y49" s="3"/>
       <c r="Z49" s="3"/>
-      <c r="AA49" s="7"/>
-      <c r="AB49" s="3"/>
-      <c r="AC49" s="12"/>
-      <c r="AD49" s="14"/>
-    </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA49" s="3"/>
+      <c r="AB49" s="7"/>
+      <c r="AC49" s="3"/>
+      <c r="AD49" s="12"/>
+      <c r="AE49" s="14"/>
+    </row>
+    <row r="50" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>50</v>
       </c>
@@ -4520,21 +4633,22 @@
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
-      <c r="R50" s="5"/>
-      <c r="S50" s="1"/>
-      <c r="T50" s="10"/>
-      <c r="U50" s="1"/>
+      <c r="R50" s="1"/>
+      <c r="S50" s="5"/>
+      <c r="T50" s="1"/>
+      <c r="U50" s="10"/>
       <c r="V50" s="1"/>
       <c r="W50" s="1"/>
       <c r="X50" s="1"/>
       <c r="Y50" s="1"/>
       <c r="Z50" s="1"/>
-      <c r="AA50" s="5"/>
-      <c r="AB50" s="1"/>
-      <c r="AC50" s="10"/>
-      <c r="AD50" s="14"/>
-    </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA50" s="1"/>
+      <c r="AB50" s="5"/>
+      <c r="AC50" s="1"/>
+      <c r="AD50" s="10"/>
+      <c r="AE50" s="14"/>
+    </row>
+    <row r="51" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
         <v>51</v>
       </c>
@@ -4585,65 +4699,69 @@
         <v>24576</v>
       </c>
       <c r="P51" s="2">
+        <f>D51^2*8*8</f>
+        <v>64</v>
+      </c>
+      <c r="Q51" s="2">
         <f>F51</f>
         <v>64</v>
       </c>
-      <c r="Q51" s="2">
-        <f>O51+P51</f>
+      <c r="R51" s="2">
+        <f>O51+Q51</f>
         <v>24640</v>
       </c>
-      <c r="R51" s="6" t="str">
+      <c r="S51" s="6" t="str">
         <f>DEC2HEX(J51,2)&amp;DEC2HEX(G51,2)&amp;"_"&amp;DEC2HEX(D51,2)&amp;DEC2HEX(H51,1)&amp;DEC2HEX(C51,1)</f>
         <v>0E0E_0111</v>
       </c>
-      <c r="S51" s="2" t="str">
+      <c r="T51" s="2" t="str">
         <f>DEC2HEX(F51,4)&amp;"_"&amp;DEC2HEX(E51,4)</f>
         <v>0040_0180</v>
       </c>
-      <c r="T51" s="11" t="str">
+      <c r="U51" s="11" t="str">
         <f>DEC2HEX(D51*H51,4)&amp;"_"&amp;DEC2HEX(D51^2,2)&amp;"00"</f>
         <v>0001_0100</v>
       </c>
-      <c r="U51" s="2">
+      <c r="V51" s="2">
         <v>0.01</v>
       </c>
-      <c r="V51" s="2">
+      <c r="W51" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W51" s="2">
+      <c r="X51" s="2">
         <f>D51^2*E51</f>
         <v>384</v>
       </c>
-      <c r="X51" s="2">
-        <f>L51*W51</f>
+      <c r="Y51" s="2">
+        <f>L51*X51</f>
         <v>4816896</v>
       </c>
-      <c r="Y51" s="2">
-        <f>L51*W51*0.03</f>
+      <c r="Z51" s="2">
+        <f>L51*X51*0.03</f>
         <v>144506.88</v>
       </c>
-      <c r="Z51" s="2">
-        <f>L51*W51*U51*V51</f>
+      <c r="AA51" s="2">
+        <f>L51*X51*V51*W51</f>
         <v>3010.56</v>
       </c>
-      <c r="AA51" s="6">
+      <c r="AB51" s="6">
         <f>D51*J50*J51*F50</f>
         <v>75264</v>
       </c>
-      <c r="AB51" s="2">
-        <f>AA51*0.03</f>
+      <c r="AC51" s="2">
+        <f>AB51*0.03</f>
         <v>2257.92</v>
       </c>
-      <c r="AC51" s="11">
+      <c r="AD51" s="11">
         <f>D51*J50</f>
         <v>14</v>
       </c>
-      <c r="AD51" s="14">
-        <f>X51/AA51</f>
+      <c r="AE51" s="14">
+        <f>Y51/AB51</f>
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>52</v>
       </c>
@@ -4665,21 +4783,22 @@
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
-      <c r="R52" s="7"/>
-      <c r="S52" s="3"/>
-      <c r="T52" s="12"/>
-      <c r="U52" s="3"/>
+      <c r="R52" s="3"/>
+      <c r="S52" s="7"/>
+      <c r="T52" s="3"/>
+      <c r="U52" s="12"/>
       <c r="V52" s="3"/>
       <c r="W52" s="3"/>
       <c r="X52" s="3"/>
       <c r="Y52" s="3"/>
       <c r="Z52" s="3"/>
-      <c r="AA52" s="7"/>
-      <c r="AB52" s="3"/>
-      <c r="AC52" s="12"/>
-      <c r="AD52" s="14"/>
-    </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA52" s="3"/>
+      <c r="AB52" s="7"/>
+      <c r="AC52" s="3"/>
+      <c r="AD52" s="12"/>
+      <c r="AE52" s="14"/>
+    </row>
+    <row r="53" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>53</v>
       </c>
@@ -4719,7 +4838,7 @@
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2">
-        <f t="shared" ref="N53:N54" si="27">G53*E53*D53</f>
+        <f t="shared" ref="N53:N54" si="33">G53*E53*D53</f>
         <v>896</v>
       </c>
       <c r="O53" s="2">
@@ -4727,65 +4846,69 @@
         <v>16384</v>
       </c>
       <c r="P53" s="2">
+        <f t="shared" ref="P53:P54" si="34">D53^2*8*8</f>
+        <v>64</v>
+      </c>
+      <c r="Q53" s="2">
         <f>F53</f>
         <v>256</v>
       </c>
-      <c r="Q53" s="2">
-        <f t="shared" ref="Q53:Q54" si="28">O53+P53</f>
+      <c r="R53" s="2">
+        <f t="shared" ref="R53:R54" si="35">O53+Q53</f>
         <v>16640</v>
       </c>
-      <c r="R53" s="6" t="str">
-        <f t="shared" ref="R53:R54" si="29">DEC2HEX(J53,2)&amp;DEC2HEX(G53,2)&amp;"_"&amp;DEC2HEX(D53,2)&amp;DEC2HEX(H53,1)&amp;DEC2HEX(C53,1)</f>
+      <c r="S53" s="6" t="str">
+        <f t="shared" ref="S53:S54" si="36">DEC2HEX(J53,2)&amp;DEC2HEX(G53,2)&amp;"_"&amp;DEC2HEX(D53,2)&amp;DEC2HEX(H53,1)&amp;DEC2HEX(C53,1)</f>
         <v>0E0E_0111</v>
       </c>
-      <c r="S53" s="2" t="str">
+      <c r="T53" s="2" t="str">
         <f>DEC2HEX(F53,4)&amp;"_"&amp;DEC2HEX(E53,4)</f>
         <v>0100_0040</v>
       </c>
-      <c r="T53" s="11" t="str">
+      <c r="U53" s="11" t="str">
         <f>DEC2HEX(D53*H53,4)&amp;"_"&amp;DEC2HEX(D53^2,2)&amp;"00"</f>
         <v>0001_0100</v>
       </c>
-      <c r="U53" s="2">
+      <c r="V53" s="2">
         <v>0.01</v>
       </c>
-      <c r="V53" s="2">
+      <c r="W53" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W53" s="2">
+      <c r="X53" s="2">
         <f>D53^2*E53</f>
         <v>64</v>
       </c>
-      <c r="X53" s="2">
-        <f>L53*W53</f>
+      <c r="Y53" s="2">
+        <f>L53*X53</f>
         <v>3211264</v>
       </c>
-      <c r="Y53" s="2">
-        <f>L53*W53*0.03</f>
+      <c r="Z53" s="2">
+        <f>L53*X53*0.03</f>
         <v>96337.919999999998</v>
       </c>
-      <c r="Z53" s="2">
-        <f>L53*W53*U53*V53</f>
+      <c r="AA53" s="2">
+        <f>L53*X53*V53*W53</f>
         <v>2007.04</v>
       </c>
-      <c r="AA53" s="6">
+      <c r="AB53" s="6">
         <f>D53*J51*J53*F51</f>
         <v>12544</v>
       </c>
-      <c r="AB53" s="2">
-        <f>AA53*0.03</f>
+      <c r="AC53" s="2">
+        <f>AB53*0.03</f>
         <v>376.32</v>
       </c>
-      <c r="AC53" s="11">
+      <c r="AD53" s="11">
         <f>D53*J51</f>
         <v>14</v>
       </c>
-      <c r="AD53" s="14">
-        <f t="shared" ref="AD53:AD54" si="30">X53/AA53</f>
+      <c r="AE53" s="14">
+        <f t="shared" ref="AE53:AE54" si="37">Y53/AB53</f>
         <v>256</v>
       </c>
     </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>54</v>
       </c>
@@ -4825,7 +4948,7 @@
       </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>2688</v>
       </c>
       <c r="O54" s="2">
@@ -4833,65 +4956,69 @@
         <v>147456</v>
       </c>
       <c r="P54" s="2">
+        <f t="shared" si="34"/>
+        <v>576</v>
+      </c>
+      <c r="Q54" s="2">
         <f>F54</f>
         <v>256</v>
       </c>
-      <c r="Q54" s="2">
-        <f t="shared" si="28"/>
+      <c r="R54" s="2">
+        <f t="shared" si="35"/>
         <v>147712</v>
       </c>
-      <c r="R54" s="6" t="str">
-        <f t="shared" si="29"/>
+      <c r="S54" s="6" t="str">
+        <f t="shared" si="36"/>
         <v>0E0E_0311</v>
       </c>
-      <c r="S54" s="2" t="str">
+      <c r="T54" s="2" t="str">
         <f>DEC2HEX(F54,4)&amp;"_"&amp;DEC2HEX(E54,4)</f>
         <v>0100_0040</v>
       </c>
-      <c r="T54" s="11" t="str">
+      <c r="U54" s="11" t="str">
         <f>DEC2HEX(D54*H54,4)&amp;"_"&amp;DEC2HEX(D54^2,2)&amp;"00"</f>
         <v>0003_0900</v>
       </c>
-      <c r="U54" s="2">
+      <c r="V54" s="2">
         <v>0.01</v>
       </c>
-      <c r="V54" s="2">
+      <c r="W54" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W54" s="2">
+      <c r="X54" s="2">
         <f>D54^2*E54</f>
         <v>576</v>
       </c>
-      <c r="X54" s="2">
-        <f>L54*W54</f>
+      <c r="Y54" s="2">
+        <f>L54*X54</f>
         <v>28901376</v>
       </c>
-      <c r="Y54" s="2">
-        <f>L54*W54*0.03</f>
+      <c r="Z54" s="2">
+        <f>L54*X54*0.03</f>
         <v>867041.27999999991</v>
       </c>
-      <c r="Z54" s="2">
-        <f>L54*W54*U54*V54</f>
+      <c r="AA54" s="2">
+        <f>L54*X54*V54*W54</f>
         <v>18063.36</v>
       </c>
-      <c r="AA54" s="6">
+      <c r="AB54" s="6">
         <f>D54*J51*J54*F51</f>
         <v>37632</v>
       </c>
-      <c r="AB54" s="2">
-        <f>AA54*0.03</f>
+      <c r="AC54" s="2">
+        <f>AB54*0.03</f>
         <v>1128.96</v>
       </c>
-      <c r="AC54" s="11">
+      <c r="AD54" s="11">
         <f>D54*J51</f>
         <v>42</v>
       </c>
-      <c r="AD54" s="14">
-        <f t="shared" si="30"/>
+      <c r="AE54" s="14">
+        <f t="shared" si="37"/>
         <v>768</v>
       </c>
     </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
         <v>55</v>
       </c>
@@ -4913,21 +5040,22 @@
       <c r="O55" s="3"/>
       <c r="P55" s="3"/>
       <c r="Q55" s="3"/>
-      <c r="R55" s="7"/>
-      <c r="S55" s="3"/>
-      <c r="T55" s="12"/>
-      <c r="U55" s="3"/>
+      <c r="R55" s="3"/>
+      <c r="S55" s="7"/>
+      <c r="T55" s="3"/>
+      <c r="U55" s="12"/>
       <c r="V55" s="3"/>
       <c r="W55" s="3"/>
       <c r="X55" s="3"/>
       <c r="Y55" s="3"/>
       <c r="Z55" s="3"/>
-      <c r="AA55" s="7"/>
-      <c r="AB55" s="3"/>
-      <c r="AC55" s="12"/>
-      <c r="AD55" s="14"/>
-    </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA55" s="3"/>
+      <c r="AB55" s="7"/>
+      <c r="AC55" s="3"/>
+      <c r="AD55" s="12"/>
+      <c r="AE55" s="14"/>
+    </row>
+    <row r="56" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
         <v>56</v>
       </c>
@@ -4949,21 +5077,22 @@
       <c r="O56" s="3"/>
       <c r="P56" s="3"/>
       <c r="Q56" s="3"/>
-      <c r="R56" s="7"/>
-      <c r="S56" s="3"/>
-      <c r="T56" s="12"/>
-      <c r="U56" s="3"/>
+      <c r="R56" s="3"/>
+      <c r="S56" s="7"/>
+      <c r="T56" s="3"/>
+      <c r="U56" s="12"/>
       <c r="V56" s="3"/>
       <c r="W56" s="3"/>
       <c r="X56" s="3"/>
       <c r="Y56" s="3"/>
       <c r="Z56" s="3"/>
-      <c r="AA56" s="7"/>
-      <c r="AB56" s="3"/>
-      <c r="AC56" s="12"/>
-      <c r="AD56" s="14"/>
-    </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA56" s="3"/>
+      <c r="AB56" s="7"/>
+      <c r="AC56" s="3"/>
+      <c r="AD56" s="12"/>
+      <c r="AE56" s="14"/>
+    </row>
+    <row r="57" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>57</v>
       </c>
@@ -4991,21 +5120,22 @@
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
-      <c r="R57" s="5"/>
-      <c r="S57" s="1"/>
-      <c r="T57" s="10"/>
-      <c r="U57" s="1"/>
+      <c r="R57" s="1"/>
+      <c r="S57" s="5"/>
+      <c r="T57" s="1"/>
+      <c r="U57" s="10"/>
       <c r="V57" s="1"/>
       <c r="W57" s="1"/>
       <c r="X57" s="1"/>
       <c r="Y57" s="1"/>
       <c r="Z57" s="1"/>
-      <c r="AA57" s="5"/>
-      <c r="AB57" s="1"/>
-      <c r="AC57" s="10"/>
-      <c r="AD57" s="14"/>
-    </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA57" s="1"/>
+      <c r="AB57" s="5"/>
+      <c r="AC57" s="1"/>
+      <c r="AD57" s="10"/>
+      <c r="AE57" s="14"/>
+    </row>
+    <row r="58" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>58</v>
       </c>
@@ -5056,65 +5186,69 @@
         <v>32768</v>
       </c>
       <c r="P58" s="2">
+        <f>D58^2*8*8</f>
+        <v>64</v>
+      </c>
+      <c r="Q58" s="2">
         <f>F58</f>
         <v>64</v>
       </c>
-      <c r="Q58" s="2">
-        <f>O58+P58</f>
+      <c r="R58" s="2">
+        <f>O58+Q58</f>
         <v>32832</v>
       </c>
-      <c r="R58" s="6" t="str">
+      <c r="S58" s="6" t="str">
         <f>DEC2HEX(J58,2)&amp;DEC2HEX(G58,2)&amp;"_"&amp;DEC2HEX(D58,2)&amp;DEC2HEX(H58,1)&amp;DEC2HEX(C58,1)</f>
         <v>0E0E_0111</v>
       </c>
-      <c r="S58" s="2" t="str">
+      <c r="T58" s="2" t="str">
         <f>DEC2HEX(F58,4)&amp;"_"&amp;DEC2HEX(E58,4)</f>
         <v>0040_0200</v>
       </c>
-      <c r="T58" s="11" t="str">
+      <c r="U58" s="11" t="str">
         <f>DEC2HEX(D58*H58,4)&amp;"_"&amp;DEC2HEX(D58^2,2)&amp;"00"</f>
         <v>0001_0100</v>
       </c>
-      <c r="U58" s="2">
+      <c r="V58" s="2">
         <v>0.01</v>
       </c>
-      <c r="V58" s="2">
+      <c r="W58" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W58" s="2">
+      <c r="X58" s="2">
         <f>D58^2*E58</f>
         <v>512</v>
       </c>
-      <c r="X58" s="2">
-        <f>L58*W58</f>
+      <c r="Y58" s="2">
+        <f>L58*X58</f>
         <v>6422528</v>
       </c>
-      <c r="Y58" s="2">
-        <f>L58*W58*0.03</f>
+      <c r="Z58" s="2">
+        <f>L58*X58*0.03</f>
         <v>192675.84</v>
       </c>
-      <c r="Z58" s="2">
-        <f>L58*W58*U58*V58</f>
+      <c r="AA58" s="2">
+        <f>L58*X58*V58*W58</f>
         <v>4014.08</v>
       </c>
-      <c r="AA58" s="6">
+      <c r="AB58" s="6">
         <f>D58*J57*J58*F57</f>
         <v>100352</v>
       </c>
-      <c r="AB58" s="2">
-        <f>AA58*0.03</f>
+      <c r="AC58" s="2">
+        <f>AB58*0.03</f>
         <v>3010.56</v>
       </c>
-      <c r="AC58" s="11">
+      <c r="AD58" s="11">
         <f>D58*J57</f>
         <v>14</v>
       </c>
-      <c r="AD58" s="14">
-        <f>X58/AA58</f>
+      <c r="AE58" s="14">
+        <f>Y58/AB58</f>
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
         <v>59</v>
       </c>
@@ -5136,21 +5270,22 @@
       <c r="O59" s="3"/>
       <c r="P59" s="3"/>
       <c r="Q59" s="3"/>
-      <c r="R59" s="7"/>
-      <c r="S59" s="3"/>
-      <c r="T59" s="12"/>
-      <c r="U59" s="3"/>
+      <c r="R59" s="3"/>
+      <c r="S59" s="7"/>
+      <c r="T59" s="3"/>
+      <c r="U59" s="12"/>
       <c r="V59" s="3"/>
       <c r="W59" s="3"/>
       <c r="X59" s="3"/>
       <c r="Y59" s="3"/>
       <c r="Z59" s="3"/>
-      <c r="AA59" s="7"/>
-      <c r="AB59" s="3"/>
-      <c r="AC59" s="12"/>
-      <c r="AD59" s="14"/>
-    </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA59" s="3"/>
+      <c r="AB59" s="7"/>
+      <c r="AC59" s="3"/>
+      <c r="AD59" s="12"/>
+      <c r="AE59" s="14"/>
+    </row>
+    <row r="60" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
         <v>60</v>
       </c>
@@ -5190,7 +5325,7 @@
       </c>
       <c r="M60" s="2"/>
       <c r="N60" s="2">
-        <f t="shared" ref="N60:N61" si="31">G60*E60*D60</f>
+        <f t="shared" ref="N60:N61" si="38">G60*E60*D60</f>
         <v>896</v>
       </c>
       <c r="O60" s="2">
@@ -5198,65 +5333,69 @@
         <v>16384</v>
       </c>
       <c r="P60" s="2">
+        <f t="shared" ref="P60:P61" si="39">D60^2*8*8</f>
+        <v>64</v>
+      </c>
+      <c r="Q60" s="2">
         <f>F60</f>
         <v>256</v>
       </c>
-      <c r="Q60" s="2">
-        <f t="shared" ref="Q60:Q61" si="32">O60+P60</f>
+      <c r="R60" s="2">
+        <f t="shared" ref="R60:R61" si="40">O60+Q60</f>
         <v>16640</v>
       </c>
-      <c r="R60" s="6" t="str">
-        <f t="shared" ref="R60:R61" si="33">DEC2HEX(J60,2)&amp;DEC2HEX(G60,2)&amp;"_"&amp;DEC2HEX(D60,2)&amp;DEC2HEX(H60,1)&amp;DEC2HEX(C60,1)</f>
+      <c r="S60" s="6" t="str">
+        <f t="shared" ref="S60:S61" si="41">DEC2HEX(J60,2)&amp;DEC2HEX(G60,2)&amp;"_"&amp;DEC2HEX(D60,2)&amp;DEC2HEX(H60,1)&amp;DEC2HEX(C60,1)</f>
         <v>0E0E_0111</v>
       </c>
-      <c r="S60" s="2" t="str">
+      <c r="T60" s="2" t="str">
         <f>DEC2HEX(F60,4)&amp;"_"&amp;DEC2HEX(E60,4)</f>
         <v>0100_0040</v>
       </c>
-      <c r="T60" s="11" t="str">
+      <c r="U60" s="11" t="str">
         <f>DEC2HEX(D60*H60,4)&amp;"_"&amp;DEC2HEX(D60^2,2)&amp;"00"</f>
         <v>0001_0100</v>
       </c>
-      <c r="U60" s="2">
+      <c r="V60" s="2">
         <v>0.01</v>
       </c>
-      <c r="V60" s="2">
+      <c r="W60" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W60" s="2">
+      <c r="X60" s="2">
         <f>D60^2*E60</f>
         <v>64</v>
       </c>
-      <c r="X60" s="2">
-        <f>L60*W60</f>
+      <c r="Y60" s="2">
+        <f>L60*X60</f>
         <v>3211264</v>
       </c>
-      <c r="Y60" s="2">
-        <f>L60*W60*0.03</f>
+      <c r="Z60" s="2">
+        <f>L60*X60*0.03</f>
         <v>96337.919999999998</v>
       </c>
-      <c r="Z60" s="2">
-        <f>L60*W60*U60*V60</f>
+      <c r="AA60" s="2">
+        <f>L60*X60*V60*W60</f>
         <v>2007.04</v>
       </c>
-      <c r="AA60" s="6">
+      <c r="AB60" s="6">
         <f>D60*J58*J60*F58</f>
         <v>12544</v>
       </c>
-      <c r="AB60" s="2">
-        <f>AA60*0.03</f>
+      <c r="AC60" s="2">
+        <f>AB60*0.03</f>
         <v>376.32</v>
       </c>
-      <c r="AC60" s="11">
+      <c r="AD60" s="11">
         <f>D60*J58</f>
         <v>14</v>
       </c>
-      <c r="AD60" s="14">
-        <f t="shared" ref="AD60:AD61" si="34">X60/AA60</f>
+      <c r="AE60" s="14">
+        <f t="shared" ref="AE60:AE61" si="42">Y60/AB60</f>
         <v>256</v>
       </c>
     </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
         <v>61</v>
       </c>
@@ -5296,7 +5435,7 @@
       </c>
       <c r="M61" s="2"/>
       <c r="N61" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>2688</v>
       </c>
       <c r="O61" s="2">
@@ -5304,65 +5443,69 @@
         <v>147456</v>
       </c>
       <c r="P61" s="2">
+        <f t="shared" si="39"/>
+        <v>576</v>
+      </c>
+      <c r="Q61" s="2">
         <f>F61</f>
         <v>256</v>
       </c>
-      <c r="Q61" s="2">
-        <f t="shared" si="32"/>
+      <c r="R61" s="2">
+        <f t="shared" si="40"/>
         <v>147712</v>
       </c>
-      <c r="R61" s="6" t="str">
-        <f t="shared" si="33"/>
+      <c r="S61" s="6" t="str">
+        <f t="shared" si="41"/>
         <v>0E0E_0311</v>
       </c>
-      <c r="S61" s="2" t="str">
+      <c r="T61" s="2" t="str">
         <f>DEC2HEX(F61,4)&amp;"_"&amp;DEC2HEX(E61,4)</f>
         <v>0100_0040</v>
       </c>
-      <c r="T61" s="11" t="str">
+      <c r="U61" s="11" t="str">
         <f>DEC2HEX(D61*H61,4)&amp;"_"&amp;DEC2HEX(D61^2,2)&amp;"00"</f>
         <v>0003_0900</v>
       </c>
-      <c r="U61" s="2">
+      <c r="V61" s="2">
         <v>0.01</v>
       </c>
-      <c r="V61" s="2">
+      <c r="W61" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W61" s="2">
+      <c r="X61" s="2">
         <f>D61^2*E61</f>
         <v>576</v>
       </c>
-      <c r="X61" s="2">
-        <f>L61*W61</f>
+      <c r="Y61" s="2">
+        <f>L61*X61</f>
         <v>28901376</v>
       </c>
-      <c r="Y61" s="2">
-        <f>L61*W61*0.03</f>
+      <c r="Z61" s="2">
+        <f>L61*X61*0.03</f>
         <v>867041.27999999991</v>
       </c>
-      <c r="Z61" s="2">
-        <f>L61*W61*U61*V61</f>
+      <c r="AA61" s="2">
+        <f>L61*X61*V61*W61</f>
         <v>18063.36</v>
       </c>
-      <c r="AA61" s="6">
+      <c r="AB61" s="6">
         <f>D61*J58*J61*F58</f>
         <v>37632</v>
       </c>
-      <c r="AB61" s="2">
-        <f>AA61*0.03</f>
+      <c r="AC61" s="2">
+        <f>AB61*0.03</f>
         <v>1128.96</v>
       </c>
-      <c r="AC61" s="11">
+      <c r="AD61" s="11">
         <f>D61*J58</f>
         <v>42</v>
       </c>
-      <c r="AD61" s="14">
-        <f t="shared" si="34"/>
+      <c r="AE61" s="14">
+        <f t="shared" si="42"/>
         <v>768</v>
       </c>
     </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
         <v>62</v>
       </c>
@@ -5384,21 +5527,22 @@
       <c r="O62" s="3"/>
       <c r="P62" s="3"/>
       <c r="Q62" s="3"/>
-      <c r="R62" s="7"/>
-      <c r="S62" s="3"/>
-      <c r="T62" s="12"/>
-      <c r="U62" s="3"/>
+      <c r="R62" s="3"/>
+      <c r="S62" s="7"/>
+      <c r="T62" s="3"/>
+      <c r="U62" s="12"/>
       <c r="V62" s="3"/>
       <c r="W62" s="3"/>
       <c r="X62" s="3"/>
       <c r="Y62" s="3"/>
       <c r="Z62" s="3"/>
-      <c r="AA62" s="7"/>
-      <c r="AB62" s="3"/>
-      <c r="AC62" s="12"/>
-      <c r="AD62" s="14"/>
-    </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA62" s="3"/>
+      <c r="AB62" s="7"/>
+      <c r="AC62" s="3"/>
+      <c r="AD62" s="12"/>
+      <c r="AE62" s="14"/>
+    </row>
+    <row r="63" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
         <v>63</v>
       </c>
@@ -5420,21 +5564,22 @@
       <c r="O63" s="3"/>
       <c r="P63" s="3"/>
       <c r="Q63" s="3"/>
-      <c r="R63" s="7"/>
-      <c r="S63" s="3"/>
-      <c r="T63" s="12"/>
-      <c r="U63" s="3"/>
+      <c r="R63" s="3"/>
+      <c r="S63" s="7"/>
+      <c r="T63" s="3"/>
+      <c r="U63" s="12"/>
       <c r="V63" s="3"/>
       <c r="W63" s="3"/>
       <c r="X63" s="3"/>
       <c r="Y63" s="3"/>
       <c r="Z63" s="3"/>
-      <c r="AA63" s="7"/>
-      <c r="AB63" s="3"/>
-      <c r="AC63" s="12"/>
-      <c r="AD63" s="14"/>
-    </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA63" s="3"/>
+      <c r="AB63" s="7"/>
+      <c r="AC63" s="3"/>
+      <c r="AD63" s="12"/>
+      <c r="AE63" s="14"/>
+    </row>
+    <row r="64" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>64</v>
       </c>
@@ -5462,21 +5607,22 @@
       <c r="O64" s="1"/>
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
-      <c r="R64" s="5"/>
-      <c r="S64" s="1"/>
-      <c r="T64" s="10"/>
-      <c r="U64" s="1"/>
+      <c r="R64" s="1"/>
+      <c r="S64" s="5"/>
+      <c r="T64" s="1"/>
+      <c r="U64" s="10"/>
       <c r="V64" s="1"/>
       <c r="W64" s="1"/>
       <c r="X64" s="1"/>
       <c r="Y64" s="1"/>
       <c r="Z64" s="1"/>
-      <c r="AA64" s="5"/>
-      <c r="AB64" s="1"/>
-      <c r="AC64" s="10"/>
-      <c r="AD64" s="14"/>
-    </row>
-    <row r="65" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA64" s="1"/>
+      <c r="AB64" s="5"/>
+      <c r="AC64" s="1"/>
+      <c r="AD64" s="10"/>
+      <c r="AE64" s="14"/>
+    </row>
+    <row r="65" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A65" s="19" t="s">
         <v>65</v>
       </c>
@@ -5498,21 +5644,22 @@
       <c r="O65" s="3"/>
       <c r="P65" s="3"/>
       <c r="Q65" s="3"/>
-      <c r="R65" s="7"/>
-      <c r="S65" s="3"/>
-      <c r="T65" s="12"/>
-      <c r="U65" s="3"/>
+      <c r="R65" s="3"/>
+      <c r="S65" s="7"/>
+      <c r="T65" s="3"/>
+      <c r="U65" s="12"/>
       <c r="V65" s="3"/>
       <c r="W65" s="3"/>
       <c r="X65" s="3"/>
       <c r="Y65" s="3"/>
       <c r="Z65" s="3"/>
-      <c r="AA65" s="7"/>
-      <c r="AB65" s="3"/>
-      <c r="AC65" s="12"/>
-      <c r="AD65" s="14"/>
-    </row>
-    <row r="66" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA65" s="3"/>
+      <c r="AB65" s="7"/>
+      <c r="AC65" s="3"/>
+      <c r="AD65" s="12"/>
+      <c r="AE65" s="14"/>
+    </row>
+    <row r="66" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
         <v>66</v>
       </c>
@@ -5560,65 +5707,69 @@
         <v>512000</v>
       </c>
       <c r="P66" s="2">
+        <f>D66^2*8*8</f>
+        <v>64</v>
+      </c>
+      <c r="Q66" s="2">
         <f>F66</f>
         <v>1000</v>
       </c>
-      <c r="Q66" s="2">
-        <f>O66+P66</f>
+      <c r="R66" s="2">
+        <f>O66+Q66</f>
         <v>513000</v>
       </c>
-      <c r="R66" s="6" t="str">
+      <c r="S66" s="6" t="str">
         <f>DEC2HEX(J66,2)&amp;DEC2HEX(G66,2)&amp;"_"&amp;DEC2HEX(D66,2)&amp;DEC2HEX(H66,1)&amp;DEC2HEX(C66,1)</f>
         <v>0E0E_0111</v>
       </c>
-      <c r="S66" s="2" t="str">
+      <c r="T66" s="2" t="str">
         <f>DEC2HEX(F66,4)&amp;"_"&amp;DEC2HEX(E66,4)</f>
         <v>03E8_0200</v>
       </c>
-      <c r="T66" s="11" t="str">
+      <c r="U66" s="11" t="str">
         <f>DEC2HEX(D66*H66,4)&amp;"_"&amp;DEC2HEX(D66^2,2)&amp;"00"</f>
         <v>0001_0100</v>
       </c>
-      <c r="U66" s="2">
+      <c r="V66" s="2">
         <v>0.01</v>
       </c>
-      <c r="V66" s="2">
+      <c r="W66" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="W66" s="2">
+      <c r="X66" s="2">
         <f>D66^2*E66</f>
         <v>512</v>
       </c>
-      <c r="X66" s="2">
-        <f>L66*W66</f>
+      <c r="Y66" s="2">
+        <f>L66*X66</f>
         <v>100352000</v>
       </c>
-      <c r="Y66" s="2">
-        <f>L66*W66*0.03</f>
+      <c r="Z66" s="2">
+        <f>L66*X66*0.03</f>
         <v>3010560</v>
       </c>
-      <c r="Z66" s="2">
-        <f>L66*W66*U66*V66</f>
+      <c r="AA66" s="2">
+        <f>L66*X66*V66*W66</f>
         <v>62720</v>
       </c>
-      <c r="AA66" s="6">
+      <c r="AB66" s="6">
         <f>D66*J64*J66*F64</f>
         <v>100352</v>
       </c>
-      <c r="AB66" s="2">
-        <f>AA66*0.03</f>
+      <c r="AC66" s="2">
+        <f>AB66*0.03</f>
         <v>3010.56</v>
       </c>
-      <c r="AC66" s="11">
+      <c r="AD66" s="11">
         <f>D66*J64</f>
         <v>14</v>
       </c>
-      <c r="AD66" s="14">
-        <f>X66/AA66</f>
+      <c r="AE66" s="14">
+        <f>Y66/AB66</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="67" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A67" s="7" t="s">
         <v>67</v>
       </c>
@@ -5640,21 +5791,22 @@
       <c r="O67" s="3"/>
       <c r="P67" s="3"/>
       <c r="Q67" s="3"/>
-      <c r="R67" s="7"/>
-      <c r="S67" s="3"/>
-      <c r="T67" s="12"/>
-      <c r="U67" s="3"/>
+      <c r="R67" s="3"/>
+      <c r="S67" s="7"/>
+      <c r="T67" s="3"/>
+      <c r="U67" s="12"/>
       <c r="V67" s="3"/>
       <c r="W67" s="3"/>
       <c r="X67" s="3"/>
       <c r="Y67" s="3"/>
       <c r="Z67" s="3"/>
-      <c r="AA67" s="7"/>
-      <c r="AB67" s="3"/>
-      <c r="AC67" s="12"/>
-      <c r="AD67" s="14"/>
-    </row>
-    <row r="68" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA67" s="3"/>
+      <c r="AB67" s="7"/>
+      <c r="AC67" s="3"/>
+      <c r="AD67" s="12"/>
+      <c r="AE67" s="14"/>
+    </row>
+    <row r="68" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A68" s="8" t="s">
         <v>68</v>
       </c>
@@ -5700,58 +5852,59 @@
       <c r="O68" s="4"/>
       <c r="P68" s="4"/>
       <c r="Q68" s="4"/>
-      <c r="R68" s="8" t="str">
+      <c r="R68" s="4"/>
+      <c r="S68" s="8" t="str">
         <f>DEC2HEX(J68,2)&amp;DEC2HEX(G68,2)&amp;"_"&amp;DEC2HEX(D68,2)&amp;DEC2HEX(H68,1)&amp;DEC2HEX(C68,1)</f>
         <v>010E_0E13</v>
       </c>
-      <c r="S68" s="4" t="str">
+      <c r="T68" s="4" t="str">
         <f>DEC2HEX(F68,4)&amp;"_"&amp;DEC2HEX(F68,4)</f>
         <v>03E8_03E8</v>
       </c>
-      <c r="T68" s="13" t="str">
+      <c r="U68" s="13" t="str">
         <f>DEC2HEX(D68*H68,4)&amp;"_"&amp;DEC2HEX(D68^2,2)&amp;"00"</f>
         <v>000E_C400</v>
       </c>
-      <c r="U68" s="4">
+      <c r="V68" s="4">
         <v>0.01</v>
       </c>
-      <c r="V68" s="4">
+      <c r="W68" s="4">
         <v>6.25E-2</v>
       </c>
-      <c r="W68" s="4">
+      <c r="X68" s="4">
         <f>D68^2*E68</f>
         <v>196</v>
       </c>
-      <c r="X68" s="4">
-        <f>L68*W68</f>
+      <c r="Y68" s="4">
+        <f>L68*X68</f>
         <v>196000</v>
       </c>
-      <c r="Y68" s="4">
-        <f>L68*W68*0.03</f>
+      <c r="Z68" s="4">
+        <f>L68*X68*0.03</f>
         <v>5880</v>
       </c>
-      <c r="Z68" s="4">
-        <f>L68*W68*U68*V68</f>
+      <c r="AA68" s="4">
+        <f>L68*X68*V68*W68</f>
         <v>122.5</v>
       </c>
-      <c r="AA68" s="8">
+      <c r="AB68" s="8">
         <f>D68*J66*J68*F66</f>
         <v>196000</v>
       </c>
-      <c r="AB68" s="4">
-        <f>AA68*0.03</f>
+      <c r="AC68" s="4">
+        <f>AB68*0.03</f>
         <v>5880</v>
       </c>
-      <c r="AC68" s="13">
+      <c r="AD68" s="13">
         <f>D68*J66</f>
         <v>196</v>
       </c>
-      <c r="AD68" s="14">
-        <f>X68/AA68</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE68" s="14">
+        <f>Y68/AB68</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>69</v>
       </c>
@@ -5773,20 +5926,21 @@
       <c r="O69" s="1"/>
       <c r="P69" s="1"/>
       <c r="Q69" s="1"/>
-      <c r="R69" s="5"/>
-      <c r="S69" s="1"/>
-      <c r="T69" s="10"/>
-      <c r="U69" s="1"/>
+      <c r="R69" s="1"/>
+      <c r="S69" s="5"/>
+      <c r="T69" s="1"/>
+      <c r="U69" s="10"/>
       <c r="V69" s="1"/>
       <c r="W69" s="1"/>
       <c r="X69" s="1"/>
       <c r="Y69" s="1"/>
       <c r="Z69" s="1"/>
-      <c r="AA69" s="5"/>
-      <c r="AB69" s="1"/>
-      <c r="AC69" s="10"/>
-    </row>
-    <row r="70" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA69" s="1"/>
+      <c r="AB69" s="5"/>
+      <c r="AC69" s="1"/>
+      <c r="AD69" s="10"/>
+    </row>
+    <row r="70" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A70" s="9"/>
       <c r="B70" s="14"/>
       <c r="C70" s="14"/>
@@ -5811,47 +5965,48 @@
         <f>SUM(O4:O69)</f>
         <v>1234432</v>
       </c>
-      <c r="P70" s="14">
-        <f>SUM(P4:P69)</f>
-        <v>3944</v>
-      </c>
+      <c r="P70" s="14"/>
       <c r="Q70" s="14">
         <f>SUM(Q4:Q69)</f>
+        <v>3944</v>
+      </c>
+      <c r="R70" s="14">
+        <f>SUM(R4:R69)</f>
         <v>1238376</v>
       </c>
-      <c r="R70" s="9"/>
-      <c r="S70" s="14"/>
-      <c r="T70" s="22"/>
-      <c r="U70" s="14"/>
+      <c r="S70" s="9"/>
+      <c r="T70" s="14"/>
+      <c r="U70" s="22"/>
       <c r="V70" s="14"/>
       <c r="W70" s="14"/>
-      <c r="X70" s="14">
-        <f t="shared" ref="X70" si="35">SUM(X4:X69)</f>
+      <c r="X70" s="14"/>
+      <c r="Y70" s="14">
+        <f t="shared" ref="Y70" si="43">SUM(Y4:Y69)</f>
         <v>391104608</v>
       </c>
-      <c r="Y70" s="14">
-        <f>SUM(Y3:Y69)</f>
+      <c r="Z70" s="14">
+        <f>SUM(Z3:Z69)</f>
         <v>11733138.239999998</v>
       </c>
-      <c r="Z70" s="24">
-        <f>SUM(Z3:Z69)</f>
+      <c r="AA70" s="24">
+        <f>SUM(AA3:AA69)</f>
         <v>244440.38</v>
       </c>
-      <c r="AA70" s="9">
-        <f>SUM(AA4:AA69)</f>
+      <c r="AB70" s="9">
+        <f>SUM(AB4:AB69)</f>
         <v>4627307</v>
       </c>
-      <c r="AB70" s="24">
-        <f>SUM(AB4:AB69)</f>
+      <c r="AC70" s="24">
+        <f>SUM(AC4:AC69)</f>
         <v>138819.21000000002</v>
       </c>
-      <c r="AC70" s="25"/>
-      <c r="AD70" s="14">
-        <f>Y70/AB70/16</f>
+      <c r="AD70" s="25"/>
+      <c r="AE70" s="14">
+        <f>Z70/AC70/16</f>
         <v>5.2825624061684247</v>
       </c>
     </row>
-    <row r="71" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A71" s="9"/>
       <c r="B71" s="14"/>
       <c r="C71" s="14"/>
@@ -5873,32 +6028,33 @@
         <f>O70*16/1024/8</f>
         <v>2411</v>
       </c>
-      <c r="P71" s="14">
-        <f>O70+P70</f>
+      <c r="P71" s="14"/>
+      <c r="Q71" s="14">
+        <f>O70+Q70</f>
         <v>1238376</v>
       </c>
-      <c r="Q71" s="14"/>
-      <c r="R71" s="9"/>
-      <c r="S71" s="14"/>
-      <c r="T71" s="22"/>
-      <c r="U71" s="14"/>
+      <c r="R71" s="14"/>
+      <c r="S71" s="9"/>
+      <c r="T71" s="14"/>
+      <c r="U71" s="22"/>
       <c r="V71" s="14"/>
       <c r="W71" s="14"/>
       <c r="X71" s="14"/>
       <c r="Y71" s="14"/>
       <c r="Z71" s="14"/>
-      <c r="AA71" s="9"/>
-      <c r="AB71" s="14"/>
-      <c r="AC71" s="22"/>
-      <c r="AD71" s="14"/>
+      <c r="AA71" s="14"/>
+      <c r="AB71" s="9"/>
+      <c r="AC71" s="14"/>
+      <c r="AD71" s="22"/>
+      <c r="AE71" s="14"/>
     </row>
   </sheetData>
   <autoFilter ref="B2:B71" xr:uid="{009522EF-F8DC-42BE-8F4B-D751FC8B03E1}"/>
   <mergeCells count="6">
     <mergeCell ref="C1:E1"/>
-    <mergeCell ref="AA1:AB1"/>
-    <mergeCell ref="X1:Z1"/>
-    <mergeCell ref="R1:T1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="S1:U1"/>
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="N1:O1"/>
   </mergeCells>

</xml_diff>

<commit_message>
BRAM SANITY PASS, speed up conv 36%
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9436D1-4C62-40FF-81A0-50DF0EB63C21}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78611BEB-7BEE-4115-A3D9-3CEBF737E519}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
+    <workbookView xWindow="-510" yWindow="1215" windowWidth="21600" windowHeight="11325" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
   <sheets>
     <sheet name="SqueezeNet v2 MEC Parallel Ch" sheetId="2" r:id="rId1"/>
@@ -1064,13 +1064,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80B23C6-EAEB-43B1-B045-456C36085CFA}">
   <dimension ref="A1:AE71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" style="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
@@ -1084,22 +1084,22 @@
     <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8" customWidth="1"/>
     <col min="17" max="18" width="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.42578125" style="18" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.88671875" style="18" customWidth="1"/>
-    <col min="29" max="29" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.85546875" style="18" customWidth="1"/>
+    <col min="29" max="29" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="10" style="21" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="15"/>
       <c r="B1" s="16"/>
       <c r="C1" s="29" t="s">
@@ -1121,7 +1121,7 @@
         <v>157</v>
       </c>
       <c r="O1" s="31"/>
-      <c r="P1" s="14"/>
+      <c r="P1" s="31"/>
       <c r="Q1" s="23"/>
       <c r="R1" s="28"/>
       <c r="S1" s="32" t="s">
@@ -1145,7 +1145,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>95.57709251101322</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
@@ -1432,7 +1432,7 @@
       <c r="AD5" s="12"/>
       <c r="AE5" s="14"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>1.4867256637168142</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
@@ -1680,7 +1680,7 @@
       <c r="AD8" s="12"/>
       <c r="AE8" s="14"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -1720,7 +1720,7 @@
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2">
-        <f t="shared" ref="N9:N10" si="1">G9*E9*D9</f>
+        <f>G9*E9*D9</f>
         <v>896</v>
       </c>
       <c r="O9" s="2">
@@ -1728,7 +1728,7 @@
         <v>1024</v>
       </c>
       <c r="P9" s="2">
-        <f t="shared" ref="P9:P10" si="2">D9^2*8*8</f>
+        <f>D9^2*8*8</f>
         <v>64</v>
       </c>
       <c r="Q9" s="2">
@@ -1736,11 +1736,11 @@
         <v>64</v>
       </c>
       <c r="R9" s="2">
-        <f t="shared" ref="R9:R10" si="3">O9+Q9</f>
+        <f t="shared" ref="R9:R10" si="1">O9+Q9</f>
         <v>1088</v>
       </c>
       <c r="S9" s="6" t="str">
-        <f t="shared" ref="S9:S10" si="4">DEC2HEX(J9,2)&amp;DEC2HEX(G9,2)&amp;"_"&amp;DEC2HEX(D9,2)&amp;DEC2HEX(H9,1)&amp;DEC2HEX(C9,1)</f>
+        <f>DEC2HEX(J9,2)&amp;DEC2HEX(G9,2)&amp;"_"&amp;DEC2HEX(D9,2)&amp;DEC2HEX(H9,1)&amp;DEC2HEX(C9,1)</f>
         <v>3838_0111</v>
       </c>
       <c r="T9" s="2" t="str">
@@ -1786,11 +1786,11 @@
         <v>56</v>
       </c>
       <c r="AE9" s="14">
-        <f t="shared" ref="AE9:AE10" si="5">Y9/AB9</f>
+        <f t="shared" ref="AE9:AE10" si="2">Y9/AB9</f>
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -1830,7 +1830,7 @@
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2">
-        <f t="shared" si="1"/>
+        <f>G10*E10*D10</f>
         <v>2688</v>
       </c>
       <c r="O10" s="2">
@@ -1838,7 +1838,7 @@
         <v>9216</v>
       </c>
       <c r="P10" s="2">
-        <f t="shared" si="2"/>
+        <f>D10^2*8*8</f>
         <v>576</v>
       </c>
       <c r="Q10" s="2">
@@ -1846,11 +1846,11 @@
         <v>64</v>
       </c>
       <c r="R10" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>9280</v>
       </c>
       <c r="S10" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f>DEC2HEX(J10,2)&amp;DEC2HEX(G10,2)&amp;"_"&amp;DEC2HEX(D10,2)&amp;DEC2HEX(H10,1)&amp;DEC2HEX(C10,1)</f>
         <v>3838_0311</v>
       </c>
       <c r="T10" s="2" t="str">
@@ -1896,11 +1896,11 @@
         <v>168</v>
       </c>
       <c r="AE10" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
@@ -1937,7 +1937,7 @@
       <c r="AD11" s="12"/>
       <c r="AE11" s="14"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>12</v>
       </c>
@@ -1974,7 +1974,7 @@
       <c r="AD12" s="12"/>
       <c r="AE12" s="14"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>19</v>
       </c>
@@ -2017,7 +2017,7 @@
       <c r="AD13" s="10"/>
       <c r="AE13" s="14"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>13</v>
       </c>
@@ -2130,7 +2130,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>14</v>
       </c>
@@ -2167,7 +2167,7 @@
       <c r="AD15" s="12"/>
       <c r="AE15" s="14"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
@@ -2207,7 +2207,7 @@
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2">
-        <f t="shared" ref="N16:N17" si="6">G16*E16*D16</f>
+        <f>G16*E16*D16</f>
         <v>896</v>
       </c>
       <c r="O16" s="2">
@@ -2215,7 +2215,7 @@
         <v>1024</v>
       </c>
       <c r="P16" s="2">
-        <f t="shared" ref="P16:P17" si="7">D16^2*8*8</f>
+        <f>D16^2*8*8</f>
         <v>64</v>
       </c>
       <c r="Q16" s="2">
@@ -2223,11 +2223,11 @@
         <v>64</v>
       </c>
       <c r="R16" s="2">
-        <f t="shared" ref="R16:R17" si="8">O16+Q16</f>
+        <f t="shared" ref="R16:R17" si="3">O16+Q16</f>
         <v>1088</v>
       </c>
       <c r="S16" s="6" t="str">
-        <f t="shared" ref="S16:S17" si="9">DEC2HEX(J16,2)&amp;DEC2HEX(G16,2)&amp;"_"&amp;DEC2HEX(D16,2)&amp;DEC2HEX(H16,1)&amp;DEC2HEX(C16,1)</f>
+        <f>DEC2HEX(J16,2)&amp;DEC2HEX(G16,2)&amp;"_"&amp;DEC2HEX(D16,2)&amp;DEC2HEX(H16,1)&amp;DEC2HEX(C16,1)</f>
         <v>3838_0111</v>
       </c>
       <c r="T16" s="2" t="str">
@@ -2273,11 +2273,11 @@
         <v>56</v>
       </c>
       <c r="AE16" s="14">
-        <f t="shared" ref="AE16:AE17" si="10">Y16/AB16</f>
+        <f t="shared" ref="AE16:AE17" si="4">Y16/AB16</f>
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2">
-        <f t="shared" si="6"/>
+        <f>G17*E17*D17</f>
         <v>2688</v>
       </c>
       <c r="O17" s="2">
@@ -2325,7 +2325,7 @@
         <v>9216</v>
       </c>
       <c r="P17" s="2">
-        <f t="shared" si="7"/>
+        <f>D17^2*8*8</f>
         <v>576</v>
       </c>
       <c r="Q17" s="2">
@@ -2333,11 +2333,11 @@
         <v>64</v>
       </c>
       <c r="R17" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>9280</v>
       </c>
       <c r="S17" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f>DEC2HEX(J17,2)&amp;DEC2HEX(G17,2)&amp;"_"&amp;DEC2HEX(D17,2)&amp;DEC2HEX(H17,1)&amp;DEC2HEX(C17,1)</f>
         <v>3838_0311</v>
       </c>
       <c r="T17" s="2" t="str">
@@ -2383,11 +2383,11 @@
         <v>168</v>
       </c>
       <c r="AE17" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>17</v>
       </c>
@@ -2424,7 +2424,7 @@
       <c r="AD18" s="12"/>
       <c r="AE18" s="14"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>18</v>
       </c>
@@ -2461,7 +2461,7 @@
       <c r="AD19" s="12"/>
       <c r="AE19" s="14"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>20</v>
       </c>
@@ -2504,7 +2504,7 @@
       <c r="AD20" s="10"/>
       <c r="AE20" s="14"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>21</v>
       </c>
@@ -2598,11 +2598,11 @@
         <v>168</v>
       </c>
       <c r="AE21" s="14">
-        <f t="shared" ref="AE21:AE22" si="11">Y21/AB21</f>
+        <f t="shared" ref="AE21:AE22" si="5">Y21/AB21</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
@@ -2711,11 +2711,11 @@
         <v>28</v>
       </c>
       <c r="AE22" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>23</v>
       </c>
@@ -2752,7 +2752,7 @@
       <c r="AD23" s="12"/>
       <c r="AE23" s="14"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>24</v>
       </c>
@@ -2792,7 +2792,7 @@
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2">
-        <f t="shared" ref="N24:N25" si="12">G24*E24*D24</f>
+        <f>G24*E24*D24</f>
         <v>896</v>
       </c>
       <c r="O24" s="2">
@@ -2800,7 +2800,7 @@
         <v>4096</v>
       </c>
       <c r="P24" s="2">
-        <f t="shared" ref="P24:P25" si="13">D24^2*8*8</f>
+        <f>D24^2*8*8</f>
         <v>64</v>
       </c>
       <c r="Q24" s="2">
@@ -2808,11 +2808,11 @@
         <v>128</v>
       </c>
       <c r="R24" s="2">
-        <f t="shared" ref="R24:R25" si="14">O24+Q24</f>
+        <f t="shared" ref="R24:R25" si="6">O24+Q24</f>
         <v>4224</v>
       </c>
       <c r="S24" s="6" t="str">
-        <f t="shared" ref="S24:S25" si="15">DEC2HEX(J24,2)&amp;DEC2HEX(G24,2)&amp;"_"&amp;DEC2HEX(D24,2)&amp;DEC2HEX(H24,1)&amp;DEC2HEX(C24,1)</f>
+        <f>DEC2HEX(J24,2)&amp;DEC2HEX(G24,2)&amp;"_"&amp;DEC2HEX(D24,2)&amp;DEC2HEX(H24,1)&amp;DEC2HEX(C24,1)</f>
         <v>1C1C_0111</v>
       </c>
       <c r="T24" s="2" t="str">
@@ -2858,11 +2858,11 @@
         <v>28</v>
       </c>
       <c r="AE24" s="14">
-        <f t="shared" ref="AE24:AE25" si="16">Y24/AB24</f>
+        <f t="shared" ref="AE24:AE25" si="7">Y24/AB24</f>
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>25</v>
       </c>
@@ -2902,7 +2902,7 @@
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2">
-        <f t="shared" si="12"/>
+        <f>G25*E25*D25</f>
         <v>2688</v>
       </c>
       <c r="O25" s="2">
@@ -2910,7 +2910,7 @@
         <v>36864</v>
       </c>
       <c r="P25" s="2">
-        <f t="shared" si="13"/>
+        <f>D25^2*8*8</f>
         <v>576</v>
       </c>
       <c r="Q25" s="2">
@@ -2918,11 +2918,11 @@
         <v>128</v>
       </c>
       <c r="R25" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="6"/>
         <v>36992</v>
       </c>
       <c r="S25" s="6" t="str">
-        <f t="shared" si="15"/>
+        <f>DEC2HEX(J25,2)&amp;DEC2HEX(G25,2)&amp;"_"&amp;DEC2HEX(D25,2)&amp;DEC2HEX(H25,1)&amp;DEC2HEX(C25,1)</f>
         <v>1C1C_0311</v>
       </c>
       <c r="T25" s="2" t="str">
@@ -2968,11 +2968,11 @@
         <v>84</v>
       </c>
       <c r="AE25" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>384</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>26</v>
       </c>
@@ -3009,7 +3009,7 @@
       <c r="AD26" s="12"/>
       <c r="AE26" s="14"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>27</v>
       </c>
@@ -3046,7 +3046,7 @@
       <c r="AD27" s="12"/>
       <c r="AE27" s="14"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>28</v>
       </c>
@@ -3089,7 +3089,7 @@
       <c r="AD28" s="10"/>
       <c r="AE28" s="14"/>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>29</v>
       </c>
@@ -3202,7 +3202,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>30</v>
       </c>
@@ -3239,7 +3239,7 @@
       <c r="AD30" s="12"/>
       <c r="AE30" s="14"/>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>31</v>
       </c>
@@ -3279,7 +3279,7 @@
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2">
-        <f t="shared" ref="N31:N32" si="17">G31*E31*D31</f>
+        <f>G31*E31*D31</f>
         <v>896</v>
       </c>
       <c r="O31" s="2">
@@ -3287,7 +3287,7 @@
         <v>4096</v>
       </c>
       <c r="P31" s="2">
-        <f t="shared" ref="P31:P32" si="18">D31^2*8*8</f>
+        <f>D31^2*8*8</f>
         <v>64</v>
       </c>
       <c r="Q31" s="2">
@@ -3295,11 +3295,11 @@
         <v>128</v>
       </c>
       <c r="R31" s="2">
-        <f t="shared" ref="R31:R32" si="19">O31+Q31</f>
+        <f t="shared" ref="R31:R32" si="8">O31+Q31</f>
         <v>4224</v>
       </c>
       <c r="S31" s="6" t="str">
-        <f t="shared" ref="S31:S32" si="20">DEC2HEX(J31,2)&amp;DEC2HEX(G31,2)&amp;"_"&amp;DEC2HEX(D31,2)&amp;DEC2HEX(H31,1)&amp;DEC2HEX(C31,1)</f>
+        <f>DEC2HEX(J31,2)&amp;DEC2HEX(G31,2)&amp;"_"&amp;DEC2HEX(D31,2)&amp;DEC2HEX(H31,1)&amp;DEC2HEX(C31,1)</f>
         <v>1C1C_0111</v>
       </c>
       <c r="T31" s="2" t="str">
@@ -3345,11 +3345,11 @@
         <v>28</v>
       </c>
       <c r="AE31" s="14">
-        <f t="shared" ref="AE31:AE32" si="21">Y31/AB31</f>
+        <f t="shared" ref="AE31:AE32" si="9">Y31/AB31</f>
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>32</v>
       </c>
@@ -3389,7 +3389,7 @@
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2">
-        <f t="shared" si="17"/>
+        <f>G32*E32*D32</f>
         <v>2688</v>
       </c>
       <c r="O32" s="2">
@@ -3397,7 +3397,7 @@
         <v>36864</v>
       </c>
       <c r="P32" s="2">
-        <f t="shared" si="18"/>
+        <f>D32^2*8*8</f>
         <v>576</v>
       </c>
       <c r="Q32" s="2">
@@ -3405,11 +3405,11 @@
         <v>128</v>
       </c>
       <c r="R32" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="8"/>
         <v>36992</v>
       </c>
       <c r="S32" s="6" t="str">
-        <f t="shared" si="20"/>
+        <f>DEC2HEX(J32,2)&amp;DEC2HEX(G32,2)&amp;"_"&amp;DEC2HEX(D32,2)&amp;DEC2HEX(H32,1)&amp;DEC2HEX(C32,1)</f>
         <v>1C1C_0311</v>
       </c>
       <c r="T32" s="2" t="str">
@@ -3455,11 +3455,11 @@
         <v>84</v>
       </c>
       <c r="AE32" s="14">
-        <f t="shared" si="21"/>
+        <f t="shared" si="9"/>
         <v>384</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>33</v>
       </c>
@@ -3496,7 +3496,7 @@
       <c r="AD33" s="12"/>
       <c r="AE33" s="14"/>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>34</v>
       </c>
@@ -3533,7 +3533,7 @@
       <c r="AD34" s="12"/>
       <c r="AE34" s="14"/>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>35</v>
       </c>
@@ -3576,7 +3576,7 @@
       <c r="AD35" s="10"/>
       <c r="AE35" s="14"/>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>36</v>
       </c>
@@ -3670,11 +3670,11 @@
         <v>84</v>
       </c>
       <c r="AE36" s="14">
-        <f t="shared" ref="AE36:AE37" si="22">Y36/AB36</f>
+        <f t="shared" ref="AE36:AE37" si="10">Y36/AB36</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>37</v>
       </c>
@@ -3783,11 +3783,11 @@
         <v>14</v>
       </c>
       <c r="AE37" s="14">
-        <f t="shared" si="22"/>
+        <f t="shared" si="10"/>
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>38</v>
       </c>
@@ -3824,7 +3824,7 @@
       <c r="AD38" s="12"/>
       <c r="AE38" s="14"/>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>39</v>
       </c>
@@ -3864,7 +3864,7 @@
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2">
-        <f t="shared" ref="N39:N40" si="23">G39*E39*D39</f>
+        <f>G39*E39*D39</f>
         <v>672</v>
       </c>
       <c r="O39" s="2">
@@ -3872,7 +3872,7 @@
         <v>9216</v>
       </c>
       <c r="P39" s="2">
-        <f t="shared" ref="P39:P40" si="24">D39^2*8*8</f>
+        <f>D39^2*8*8</f>
         <v>64</v>
       </c>
       <c r="Q39" s="2">
@@ -3880,11 +3880,11 @@
         <v>192</v>
       </c>
       <c r="R39" s="2">
-        <f t="shared" ref="R39:R40" si="25">O39+Q39</f>
+        <f t="shared" ref="R39:R40" si="11">O39+Q39</f>
         <v>9408</v>
       </c>
       <c r="S39" s="6" t="str">
-        <f t="shared" ref="S39:S40" si="26">DEC2HEX(J39,2)&amp;DEC2HEX(G39,2)&amp;"_"&amp;DEC2HEX(D39,2)&amp;DEC2HEX(H39,1)&amp;DEC2HEX(C39,1)</f>
+        <f>DEC2HEX(J39,2)&amp;DEC2HEX(G39,2)&amp;"_"&amp;DEC2HEX(D39,2)&amp;DEC2HEX(H39,1)&amp;DEC2HEX(C39,1)</f>
         <v>0E0E_0111</v>
       </c>
       <c r="T39" s="2" t="str">
@@ -3930,11 +3930,11 @@
         <v>14</v>
       </c>
       <c r="AE39" s="14">
-        <f t="shared" ref="AE39:AE40" si="27">Y39/AB39</f>
+        <f t="shared" ref="AE39:AE40" si="12">Y39/AB39</f>
         <v>192</v>
       </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>40</v>
       </c>
@@ -3974,7 +3974,7 @@
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2">
-        <f t="shared" si="23"/>
+        <f>G40*E40*D40</f>
         <v>2016</v>
       </c>
       <c r="O40" s="2">
@@ -3982,7 +3982,7 @@
         <v>82944</v>
       </c>
       <c r="P40" s="2">
-        <f t="shared" si="24"/>
+        <f>D40^2*8*8</f>
         <v>576</v>
       </c>
       <c r="Q40" s="2">
@@ -3990,11 +3990,11 @@
         <v>192</v>
       </c>
       <c r="R40" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="11"/>
         <v>83136</v>
       </c>
       <c r="S40" s="6" t="str">
-        <f t="shared" si="26"/>
+        <f>DEC2HEX(J40,2)&amp;DEC2HEX(G40,2)&amp;"_"&amp;DEC2HEX(D40,2)&amp;DEC2HEX(H40,1)&amp;DEC2HEX(C40,1)</f>
         <v>0E0E_0311</v>
       </c>
       <c r="T40" s="2" t="str">
@@ -4040,11 +4040,11 @@
         <v>42</v>
       </c>
       <c r="AE40" s="14">
-        <f t="shared" si="27"/>
+        <f t="shared" si="12"/>
         <v>576</v>
       </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>41</v>
       </c>
@@ -4081,7 +4081,7 @@
       <c r="AD41" s="12"/>
       <c r="AE41" s="14"/>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>42</v>
       </c>
@@ -4118,7 +4118,7 @@
       <c r="AD42" s="12"/>
       <c r="AE42" s="14"/>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>43</v>
       </c>
@@ -4161,7 +4161,7 @@
       <c r="AD43" s="10"/>
       <c r="AE43" s="14"/>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>44</v>
       </c>
@@ -4274,7 +4274,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>45</v>
       </c>
@@ -4311,7 +4311,7 @@
       <c r="AD45" s="12"/>
       <c r="AE45" s="14"/>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>46</v>
       </c>
@@ -4351,7 +4351,7 @@
       </c>
       <c r="M46" s="2"/>
       <c r="N46" s="2">
-        <f t="shared" ref="N46:N47" si="28">G46*E46*D46</f>
+        <f>G46*E46*D46</f>
         <v>672</v>
       </c>
       <c r="O46" s="2">
@@ -4359,7 +4359,7 @@
         <v>9216</v>
       </c>
       <c r="P46" s="2">
-        <f t="shared" ref="P46:P47" si="29">D46^2*8*8</f>
+        <f>D46^2*8*8</f>
         <v>64</v>
       </c>
       <c r="Q46" s="2">
@@ -4367,11 +4367,11 @@
         <v>192</v>
       </c>
       <c r="R46" s="2">
-        <f t="shared" ref="R46:R47" si="30">O46+Q46</f>
+        <f t="shared" ref="R46:R47" si="13">O46+Q46</f>
         <v>9408</v>
       </c>
       <c r="S46" s="6" t="str">
-        <f t="shared" ref="S46:S47" si="31">DEC2HEX(J46,2)&amp;DEC2HEX(G46,2)&amp;"_"&amp;DEC2HEX(D46,2)&amp;DEC2HEX(H46,1)&amp;DEC2HEX(C46,1)</f>
+        <f>DEC2HEX(J46,2)&amp;DEC2HEX(G46,2)&amp;"_"&amp;DEC2HEX(D46,2)&amp;DEC2HEX(H46,1)&amp;DEC2HEX(C46,1)</f>
         <v>0E0E_0111</v>
       </c>
       <c r="T46" s="2" t="str">
@@ -4417,11 +4417,11 @@
         <v>14</v>
       </c>
       <c r="AE46" s="14">
-        <f t="shared" ref="AE46:AE47" si="32">Y46/AB46</f>
+        <f t="shared" ref="AE46:AE47" si="14">Y46/AB46</f>
         <v>192</v>
       </c>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>47</v>
       </c>
@@ -4461,7 +4461,7 @@
       </c>
       <c r="M47" s="2"/>
       <c r="N47" s="2">
-        <f t="shared" si="28"/>
+        <f>G47*E47*D47</f>
         <v>2016</v>
       </c>
       <c r="O47" s="2">
@@ -4469,7 +4469,7 @@
         <v>82944</v>
       </c>
       <c r="P47" s="2">
-        <f t="shared" si="29"/>
+        <f>D47^2*8*8</f>
         <v>576</v>
       </c>
       <c r="Q47" s="2">
@@ -4477,11 +4477,11 @@
         <v>192</v>
       </c>
       <c r="R47" s="2">
-        <f t="shared" si="30"/>
+        <f t="shared" si="13"/>
         <v>83136</v>
       </c>
       <c r="S47" s="6" t="str">
-        <f t="shared" si="31"/>
+        <f>DEC2HEX(J47,2)&amp;DEC2HEX(G47,2)&amp;"_"&amp;DEC2HEX(D47,2)&amp;DEC2HEX(H47,1)&amp;DEC2HEX(C47,1)</f>
         <v>0E0E_0311</v>
       </c>
       <c r="T47" s="2" t="str">
@@ -4527,11 +4527,11 @@
         <v>42</v>
       </c>
       <c r="AE47" s="14">
-        <f t="shared" si="32"/>
+        <f t="shared" si="14"/>
         <v>576</v>
       </c>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>48</v>
       </c>
@@ -4568,7 +4568,7 @@
       <c r="AD48" s="12"/>
       <c r="AE48" s="14"/>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>49</v>
       </c>
@@ -4605,7 +4605,7 @@
       <c r="AD49" s="12"/>
       <c r="AE49" s="14"/>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>50</v>
       </c>
@@ -4648,7 +4648,7 @@
       <c r="AD50" s="10"/>
       <c r="AE50" s="14"/>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>51</v>
       </c>
@@ -4761,7 +4761,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>52</v>
       </c>
@@ -4798,7 +4798,7 @@
       <c r="AD52" s="12"/>
       <c r="AE52" s="14"/>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>53</v>
       </c>
@@ -4838,7 +4838,7 @@
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2">
-        <f t="shared" ref="N53:N54" si="33">G53*E53*D53</f>
+        <f>G53*E53*D53</f>
         <v>896</v>
       </c>
       <c r="O53" s="2">
@@ -4846,7 +4846,7 @@
         <v>16384</v>
       </c>
       <c r="P53" s="2">
-        <f t="shared" ref="P53:P54" si="34">D53^2*8*8</f>
+        <f>D53^2*8*8</f>
         <v>64</v>
       </c>
       <c r="Q53" s="2">
@@ -4854,11 +4854,11 @@
         <v>256</v>
       </c>
       <c r="R53" s="2">
-        <f t="shared" ref="R53:R54" si="35">O53+Q53</f>
+        <f t="shared" ref="R53:R54" si="15">O53+Q53</f>
         <v>16640</v>
       </c>
       <c r="S53" s="6" t="str">
-        <f t="shared" ref="S53:S54" si="36">DEC2HEX(J53,2)&amp;DEC2HEX(G53,2)&amp;"_"&amp;DEC2HEX(D53,2)&amp;DEC2HEX(H53,1)&amp;DEC2HEX(C53,1)</f>
+        <f>DEC2HEX(J53,2)&amp;DEC2HEX(G53,2)&amp;"_"&amp;DEC2HEX(D53,2)&amp;DEC2HEX(H53,1)&amp;DEC2HEX(C53,1)</f>
         <v>0E0E_0111</v>
       </c>
       <c r="T53" s="2" t="str">
@@ -4904,11 +4904,11 @@
         <v>14</v>
       </c>
       <c r="AE53" s="14">
-        <f t="shared" ref="AE53:AE54" si="37">Y53/AB53</f>
+        <f t="shared" ref="AE53:AE54" si="16">Y53/AB53</f>
         <v>256</v>
       </c>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>54</v>
       </c>
@@ -4948,7 +4948,7 @@
       </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2">
-        <f t="shared" si="33"/>
+        <f>G54*E54*D54</f>
         <v>2688</v>
       </c>
       <c r="O54" s="2">
@@ -4956,7 +4956,7 @@
         <v>147456</v>
       </c>
       <c r="P54" s="2">
-        <f t="shared" si="34"/>
+        <f>D54^2*8*8</f>
         <v>576</v>
       </c>
       <c r="Q54" s="2">
@@ -4964,11 +4964,11 @@
         <v>256</v>
       </c>
       <c r="R54" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="15"/>
         <v>147712</v>
       </c>
       <c r="S54" s="6" t="str">
-        <f t="shared" si="36"/>
+        <f>DEC2HEX(J54,2)&amp;DEC2HEX(G54,2)&amp;"_"&amp;DEC2HEX(D54,2)&amp;DEC2HEX(H54,1)&amp;DEC2HEX(C54,1)</f>
         <v>0E0E_0311</v>
       </c>
       <c r="T54" s="2" t="str">
@@ -5014,11 +5014,11 @@
         <v>42</v>
       </c>
       <c r="AE54" s="14">
-        <f t="shared" si="37"/>
+        <f t="shared" si="16"/>
         <v>768</v>
       </c>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>55</v>
       </c>
@@ -5055,7 +5055,7 @@
       <c r="AD55" s="12"/>
       <c r="AE55" s="14"/>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>56</v>
       </c>
@@ -5092,7 +5092,7 @@
       <c r="AD56" s="12"/>
       <c r="AE56" s="14"/>
     </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>57</v>
       </c>
@@ -5135,7 +5135,7 @@
       <c r="AD57" s="10"/>
       <c r="AE57" s="14"/>
     </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>58</v>
       </c>
@@ -5248,7 +5248,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>59</v>
       </c>
@@ -5285,7 +5285,7 @@
       <c r="AD59" s="12"/>
       <c r="AE59" s="14"/>
     </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>60</v>
       </c>
@@ -5325,7 +5325,7 @@
       </c>
       <c r="M60" s="2"/>
       <c r="N60" s="2">
-        <f t="shared" ref="N60:N61" si="38">G60*E60*D60</f>
+        <f>G60*E60*D60</f>
         <v>896</v>
       </c>
       <c r="O60" s="2">
@@ -5333,7 +5333,7 @@
         <v>16384</v>
       </c>
       <c r="P60" s="2">
-        <f t="shared" ref="P60:P61" si="39">D60^2*8*8</f>
+        <f>D60^2*8*8</f>
         <v>64</v>
       </c>
       <c r="Q60" s="2">
@@ -5341,11 +5341,11 @@
         <v>256</v>
       </c>
       <c r="R60" s="2">
-        <f t="shared" ref="R60:R61" si="40">O60+Q60</f>
+        <f t="shared" ref="R60:R61" si="17">O60+Q60</f>
         <v>16640</v>
       </c>
       <c r="S60" s="6" t="str">
-        <f t="shared" ref="S60:S61" si="41">DEC2HEX(J60,2)&amp;DEC2HEX(G60,2)&amp;"_"&amp;DEC2HEX(D60,2)&amp;DEC2HEX(H60,1)&amp;DEC2HEX(C60,1)</f>
+        <f>DEC2HEX(J60,2)&amp;DEC2HEX(G60,2)&amp;"_"&amp;DEC2HEX(D60,2)&amp;DEC2HEX(H60,1)&amp;DEC2HEX(C60,1)</f>
         <v>0E0E_0111</v>
       </c>
       <c r="T60" s="2" t="str">
@@ -5391,11 +5391,11 @@
         <v>14</v>
       </c>
       <c r="AE60" s="14">
-        <f t="shared" ref="AE60:AE61" si="42">Y60/AB60</f>
+        <f t="shared" ref="AE60:AE61" si="18">Y60/AB60</f>
         <v>256</v>
       </c>
     </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>61</v>
       </c>
@@ -5435,7 +5435,7 @@
       </c>
       <c r="M61" s="2"/>
       <c r="N61" s="2">
-        <f t="shared" si="38"/>
+        <f>G61*E61*D61</f>
         <v>2688</v>
       </c>
       <c r="O61" s="2">
@@ -5443,7 +5443,7 @@
         <v>147456</v>
       </c>
       <c r="P61" s="2">
-        <f t="shared" si="39"/>
+        <f>D61^2*8*8</f>
         <v>576</v>
       </c>
       <c r="Q61" s="2">
@@ -5451,11 +5451,11 @@
         <v>256</v>
       </c>
       <c r="R61" s="2">
-        <f t="shared" si="40"/>
+        <f t="shared" si="17"/>
         <v>147712</v>
       </c>
       <c r="S61" s="6" t="str">
-        <f t="shared" si="41"/>
+        <f>DEC2HEX(J61,2)&amp;DEC2HEX(G61,2)&amp;"_"&amp;DEC2HEX(D61,2)&amp;DEC2HEX(H61,1)&amp;DEC2HEX(C61,1)</f>
         <v>0E0E_0311</v>
       </c>
       <c r="T61" s="2" t="str">
@@ -5501,11 +5501,11 @@
         <v>42</v>
       </c>
       <c r="AE61" s="14">
-        <f t="shared" si="42"/>
+        <f t="shared" si="18"/>
         <v>768</v>
       </c>
     </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>62</v>
       </c>
@@ -5542,7 +5542,7 @@
       <c r="AD62" s="12"/>
       <c r="AE62" s="14"/>
     </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>63</v>
       </c>
@@ -5579,7 +5579,7 @@
       <c r="AD63" s="12"/>
       <c r="AE63" s="14"/>
     </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>64</v>
       </c>
@@ -5622,7 +5622,7 @@
       <c r="AD64" s="10"/>
       <c r="AE64" s="14"/>
     </row>
-    <row r="65" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A65" s="19" t="s">
         <v>65</v>
       </c>
@@ -5659,7 +5659,7 @@
       <c r="AD65" s="12"/>
       <c r="AE65" s="14"/>
     </row>
-    <row r="66" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>66</v>
       </c>
@@ -5769,7 +5769,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="67" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>67</v>
       </c>
@@ -5806,7 +5806,7 @@
       <c r="AD67" s="12"/>
       <c r="AE67" s="14"/>
     </row>
-    <row r="68" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>68</v>
       </c>
@@ -5904,7 +5904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>69</v>
       </c>
@@ -5940,7 +5940,7 @@
       <c r="AC69" s="1"/>
       <c r="AD69" s="10"/>
     </row>
-    <row r="70" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A70" s="9"/>
       <c r="B70" s="14"/>
       <c r="C70" s="14"/>
@@ -5981,7 +5981,7 @@
       <c r="W70" s="14"/>
       <c r="X70" s="14"/>
       <c r="Y70" s="14">
-        <f t="shared" ref="Y70" si="43">SUM(Y4:Y69)</f>
+        <f t="shared" ref="Y70" si="19">SUM(Y4:Y69)</f>
         <v>391104608</v>
       </c>
       <c r="Z70" s="14">
@@ -6006,7 +6006,7 @@
         <v>5.2825624061684247</v>
       </c>
     </row>
-    <row r="71" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A71" s="9"/>
       <c r="B71" s="14"/>
       <c r="C71" s="14"/>
@@ -6056,7 +6056,7 @@
     <mergeCell ref="Y1:AA1"/>
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="N1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6071,16 +6071,16 @@
       <selection activeCell="I1" sqref="I1:K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" customWidth="1"/>
-    <col min="9" max="13" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" customWidth="1"/>
+    <col min="9" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>148</v>
       </c>
@@ -6128,7 +6128,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>149</v>
       </c>
@@ -6176,7 +6176,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>140</v>
       </c>
@@ -6224,7 +6224,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>140</v>
       </c>
@@ -6272,7 +6272,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>150</v>
       </c>
@@ -6320,7 +6320,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>140</v>
       </c>
@@ -6368,7 +6368,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>140</v>
       </c>
@@ -6416,7 +6416,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>150</v>
       </c>
@@ -6464,7 +6464,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>151</v>
       </c>
@@ -6512,7 +6512,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>141</v>
       </c>
@@ -6560,7 +6560,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>141</v>
       </c>
@@ -6608,7 +6608,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>152</v>
       </c>
@@ -6656,7 +6656,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>141</v>
       </c>
@@ -6704,7 +6704,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>141</v>
       </c>
@@ -6752,7 +6752,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>152</v>
       </c>
@@ -6800,7 +6800,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>153</v>
       </c>
@@ -6848,7 +6848,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>142</v>
       </c>
@@ -6896,7 +6896,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>142</v>
       </c>
@@ -6944,7 +6944,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>154</v>
       </c>
@@ -6992,7 +6992,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>142</v>
       </c>
@@ -7040,7 +7040,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>142</v>
       </c>
@@ -7088,7 +7088,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>154</v>
       </c>
@@ -7136,7 +7136,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>142</v>
       </c>
@@ -7184,7 +7184,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>142</v>
       </c>
@@ -7232,7 +7232,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>154</v>
       </c>
@@ -7280,7 +7280,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>142</v>
       </c>
@@ -7328,7 +7328,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>142</v>
       </c>
@@ -7376,7 +7376,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>154</v>
       </c>
@@ -7424,7 +7424,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>142</v>
       </c>
@@ -7472,7 +7472,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
BRAM SANITY PASS, speed up conv 36%. Refine sacc with BRAM.
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9436D1-4C62-40FF-81A0-50DF0EB63C21}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78611BEB-7BEE-4115-A3D9-3CEBF737E519}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
+    <workbookView xWindow="-510" yWindow="1215" windowWidth="21600" windowHeight="11325" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
   <sheets>
     <sheet name="SqueezeNet v2 MEC Parallel Ch" sheetId="2" r:id="rId1"/>
@@ -1064,13 +1064,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80B23C6-EAEB-43B1-B045-456C36085CFA}">
   <dimension ref="A1:AE71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" style="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
@@ -1084,22 +1084,22 @@
     <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8" customWidth="1"/>
     <col min="17" max="18" width="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.42578125" style="18" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.88671875" style="18" customWidth="1"/>
-    <col min="29" max="29" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.85546875" style="18" customWidth="1"/>
+    <col min="29" max="29" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="10" style="21" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="15"/>
       <c r="B1" s="16"/>
       <c r="C1" s="29" t="s">
@@ -1121,7 +1121,7 @@
         <v>157</v>
       </c>
       <c r="O1" s="31"/>
-      <c r="P1" s="14"/>
+      <c r="P1" s="31"/>
       <c r="Q1" s="23"/>
       <c r="R1" s="28"/>
       <c r="S1" s="32" t="s">
@@ -1145,7 +1145,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>95.57709251101322</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
@@ -1432,7 +1432,7 @@
       <c r="AD5" s="12"/>
       <c r="AE5" s="14"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>1.4867256637168142</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
@@ -1680,7 +1680,7 @@
       <c r="AD8" s="12"/>
       <c r="AE8" s="14"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -1720,7 +1720,7 @@
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2">
-        <f t="shared" ref="N9:N10" si="1">G9*E9*D9</f>
+        <f>G9*E9*D9</f>
         <v>896</v>
       </c>
       <c r="O9" s="2">
@@ -1728,7 +1728,7 @@
         <v>1024</v>
       </c>
       <c r="P9" s="2">
-        <f t="shared" ref="P9:P10" si="2">D9^2*8*8</f>
+        <f>D9^2*8*8</f>
         <v>64</v>
       </c>
       <c r="Q9" s="2">
@@ -1736,11 +1736,11 @@
         <v>64</v>
       </c>
       <c r="R9" s="2">
-        <f t="shared" ref="R9:R10" si="3">O9+Q9</f>
+        <f t="shared" ref="R9:R10" si="1">O9+Q9</f>
         <v>1088</v>
       </c>
       <c r="S9" s="6" t="str">
-        <f t="shared" ref="S9:S10" si="4">DEC2HEX(J9,2)&amp;DEC2HEX(G9,2)&amp;"_"&amp;DEC2HEX(D9,2)&amp;DEC2HEX(H9,1)&amp;DEC2HEX(C9,1)</f>
+        <f>DEC2HEX(J9,2)&amp;DEC2HEX(G9,2)&amp;"_"&amp;DEC2HEX(D9,2)&amp;DEC2HEX(H9,1)&amp;DEC2HEX(C9,1)</f>
         <v>3838_0111</v>
       </c>
       <c r="T9" s="2" t="str">
@@ -1786,11 +1786,11 @@
         <v>56</v>
       </c>
       <c r="AE9" s="14">
-        <f t="shared" ref="AE9:AE10" si="5">Y9/AB9</f>
+        <f t="shared" ref="AE9:AE10" si="2">Y9/AB9</f>
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -1830,7 +1830,7 @@
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2">
-        <f t="shared" si="1"/>
+        <f>G10*E10*D10</f>
         <v>2688</v>
       </c>
       <c r="O10" s="2">
@@ -1838,7 +1838,7 @@
         <v>9216</v>
       </c>
       <c r="P10" s="2">
-        <f t="shared" si="2"/>
+        <f>D10^2*8*8</f>
         <v>576</v>
       </c>
       <c r="Q10" s="2">
@@ -1846,11 +1846,11 @@
         <v>64</v>
       </c>
       <c r="R10" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>9280</v>
       </c>
       <c r="S10" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f>DEC2HEX(J10,2)&amp;DEC2HEX(G10,2)&amp;"_"&amp;DEC2HEX(D10,2)&amp;DEC2HEX(H10,1)&amp;DEC2HEX(C10,1)</f>
         <v>3838_0311</v>
       </c>
       <c r="T10" s="2" t="str">
@@ -1896,11 +1896,11 @@
         <v>168</v>
       </c>
       <c r="AE10" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
@@ -1937,7 +1937,7 @@
       <c r="AD11" s="12"/>
       <c r="AE11" s="14"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>12</v>
       </c>
@@ -1974,7 +1974,7 @@
       <c r="AD12" s="12"/>
       <c r="AE12" s="14"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>19</v>
       </c>
@@ -2017,7 +2017,7 @@
       <c r="AD13" s="10"/>
       <c r="AE13" s="14"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>13</v>
       </c>
@@ -2130,7 +2130,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>14</v>
       </c>
@@ -2167,7 +2167,7 @@
       <c r="AD15" s="12"/>
       <c r="AE15" s="14"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
@@ -2207,7 +2207,7 @@
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2">
-        <f t="shared" ref="N16:N17" si="6">G16*E16*D16</f>
+        <f>G16*E16*D16</f>
         <v>896</v>
       </c>
       <c r="O16" s="2">
@@ -2215,7 +2215,7 @@
         <v>1024</v>
       </c>
       <c r="P16" s="2">
-        <f t="shared" ref="P16:P17" si="7">D16^2*8*8</f>
+        <f>D16^2*8*8</f>
         <v>64</v>
       </c>
       <c r="Q16" s="2">
@@ -2223,11 +2223,11 @@
         <v>64</v>
       </c>
       <c r="R16" s="2">
-        <f t="shared" ref="R16:R17" si="8">O16+Q16</f>
+        <f t="shared" ref="R16:R17" si="3">O16+Q16</f>
         <v>1088</v>
       </c>
       <c r="S16" s="6" t="str">
-        <f t="shared" ref="S16:S17" si="9">DEC2HEX(J16,2)&amp;DEC2HEX(G16,2)&amp;"_"&amp;DEC2HEX(D16,2)&amp;DEC2HEX(H16,1)&amp;DEC2HEX(C16,1)</f>
+        <f>DEC2HEX(J16,2)&amp;DEC2HEX(G16,2)&amp;"_"&amp;DEC2HEX(D16,2)&amp;DEC2HEX(H16,1)&amp;DEC2HEX(C16,1)</f>
         <v>3838_0111</v>
       </c>
       <c r="T16" s="2" t="str">
@@ -2273,11 +2273,11 @@
         <v>56</v>
       </c>
       <c r="AE16" s="14">
-        <f t="shared" ref="AE16:AE17" si="10">Y16/AB16</f>
+        <f t="shared" ref="AE16:AE17" si="4">Y16/AB16</f>
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2">
-        <f t="shared" si="6"/>
+        <f>G17*E17*D17</f>
         <v>2688</v>
       </c>
       <c r="O17" s="2">
@@ -2325,7 +2325,7 @@
         <v>9216</v>
       </c>
       <c r="P17" s="2">
-        <f t="shared" si="7"/>
+        <f>D17^2*8*8</f>
         <v>576</v>
       </c>
       <c r="Q17" s="2">
@@ -2333,11 +2333,11 @@
         <v>64</v>
       </c>
       <c r="R17" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>9280</v>
       </c>
       <c r="S17" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f>DEC2HEX(J17,2)&amp;DEC2HEX(G17,2)&amp;"_"&amp;DEC2HEX(D17,2)&amp;DEC2HEX(H17,1)&amp;DEC2HEX(C17,1)</f>
         <v>3838_0311</v>
       </c>
       <c r="T17" s="2" t="str">
@@ -2383,11 +2383,11 @@
         <v>168</v>
       </c>
       <c r="AE17" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>17</v>
       </c>
@@ -2424,7 +2424,7 @@
       <c r="AD18" s="12"/>
       <c r="AE18" s="14"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>18</v>
       </c>
@@ -2461,7 +2461,7 @@
       <c r="AD19" s="12"/>
       <c r="AE19" s="14"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>20</v>
       </c>
@@ -2504,7 +2504,7 @@
       <c r="AD20" s="10"/>
       <c r="AE20" s="14"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>21</v>
       </c>
@@ -2598,11 +2598,11 @@
         <v>168</v>
       </c>
       <c r="AE21" s="14">
-        <f t="shared" ref="AE21:AE22" si="11">Y21/AB21</f>
+        <f t="shared" ref="AE21:AE22" si="5">Y21/AB21</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
@@ -2711,11 +2711,11 @@
         <v>28</v>
       </c>
       <c r="AE22" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>23</v>
       </c>
@@ -2752,7 +2752,7 @@
       <c r="AD23" s="12"/>
       <c r="AE23" s="14"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>24</v>
       </c>
@@ -2792,7 +2792,7 @@
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2">
-        <f t="shared" ref="N24:N25" si="12">G24*E24*D24</f>
+        <f>G24*E24*D24</f>
         <v>896</v>
       </c>
       <c r="O24" s="2">
@@ -2800,7 +2800,7 @@
         <v>4096</v>
       </c>
       <c r="P24" s="2">
-        <f t="shared" ref="P24:P25" si="13">D24^2*8*8</f>
+        <f>D24^2*8*8</f>
         <v>64</v>
       </c>
       <c r="Q24" s="2">
@@ -2808,11 +2808,11 @@
         <v>128</v>
       </c>
       <c r="R24" s="2">
-        <f t="shared" ref="R24:R25" si="14">O24+Q24</f>
+        <f t="shared" ref="R24:R25" si="6">O24+Q24</f>
         <v>4224</v>
       </c>
       <c r="S24" s="6" t="str">
-        <f t="shared" ref="S24:S25" si="15">DEC2HEX(J24,2)&amp;DEC2HEX(G24,2)&amp;"_"&amp;DEC2HEX(D24,2)&amp;DEC2HEX(H24,1)&amp;DEC2HEX(C24,1)</f>
+        <f>DEC2HEX(J24,2)&amp;DEC2HEX(G24,2)&amp;"_"&amp;DEC2HEX(D24,2)&amp;DEC2HEX(H24,1)&amp;DEC2HEX(C24,1)</f>
         <v>1C1C_0111</v>
       </c>
       <c r="T24" s="2" t="str">
@@ -2858,11 +2858,11 @@
         <v>28</v>
       </c>
       <c r="AE24" s="14">
-        <f t="shared" ref="AE24:AE25" si="16">Y24/AB24</f>
+        <f t="shared" ref="AE24:AE25" si="7">Y24/AB24</f>
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>25</v>
       </c>
@@ -2902,7 +2902,7 @@
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2">
-        <f t="shared" si="12"/>
+        <f>G25*E25*D25</f>
         <v>2688</v>
       </c>
       <c r="O25" s="2">
@@ -2910,7 +2910,7 @@
         <v>36864</v>
       </c>
       <c r="P25" s="2">
-        <f t="shared" si="13"/>
+        <f>D25^2*8*8</f>
         <v>576</v>
       </c>
       <c r="Q25" s="2">
@@ -2918,11 +2918,11 @@
         <v>128</v>
       </c>
       <c r="R25" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="6"/>
         <v>36992</v>
       </c>
       <c r="S25" s="6" t="str">
-        <f t="shared" si="15"/>
+        <f>DEC2HEX(J25,2)&amp;DEC2HEX(G25,2)&amp;"_"&amp;DEC2HEX(D25,2)&amp;DEC2HEX(H25,1)&amp;DEC2HEX(C25,1)</f>
         <v>1C1C_0311</v>
       </c>
       <c r="T25" s="2" t="str">
@@ -2968,11 +2968,11 @@
         <v>84</v>
       </c>
       <c r="AE25" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>384</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>26</v>
       </c>
@@ -3009,7 +3009,7 @@
       <c r="AD26" s="12"/>
       <c r="AE26" s="14"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>27</v>
       </c>
@@ -3046,7 +3046,7 @@
       <c r="AD27" s="12"/>
       <c r="AE27" s="14"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>28</v>
       </c>
@@ -3089,7 +3089,7 @@
       <c r="AD28" s="10"/>
       <c r="AE28" s="14"/>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>29</v>
       </c>
@@ -3202,7 +3202,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>30</v>
       </c>
@@ -3239,7 +3239,7 @@
       <c r="AD30" s="12"/>
       <c r="AE30" s="14"/>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>31</v>
       </c>
@@ -3279,7 +3279,7 @@
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2">
-        <f t="shared" ref="N31:N32" si="17">G31*E31*D31</f>
+        <f>G31*E31*D31</f>
         <v>896</v>
       </c>
       <c r="O31" s="2">
@@ -3287,7 +3287,7 @@
         <v>4096</v>
       </c>
       <c r="P31" s="2">
-        <f t="shared" ref="P31:P32" si="18">D31^2*8*8</f>
+        <f>D31^2*8*8</f>
         <v>64</v>
       </c>
       <c r="Q31" s="2">
@@ -3295,11 +3295,11 @@
         <v>128</v>
       </c>
       <c r="R31" s="2">
-        <f t="shared" ref="R31:R32" si="19">O31+Q31</f>
+        <f t="shared" ref="R31:R32" si="8">O31+Q31</f>
         <v>4224</v>
       </c>
       <c r="S31" s="6" t="str">
-        <f t="shared" ref="S31:S32" si="20">DEC2HEX(J31,2)&amp;DEC2HEX(G31,2)&amp;"_"&amp;DEC2HEX(D31,2)&amp;DEC2HEX(H31,1)&amp;DEC2HEX(C31,1)</f>
+        <f>DEC2HEX(J31,2)&amp;DEC2HEX(G31,2)&amp;"_"&amp;DEC2HEX(D31,2)&amp;DEC2HEX(H31,1)&amp;DEC2HEX(C31,1)</f>
         <v>1C1C_0111</v>
       </c>
       <c r="T31" s="2" t="str">
@@ -3345,11 +3345,11 @@
         <v>28</v>
       </c>
       <c r="AE31" s="14">
-        <f t="shared" ref="AE31:AE32" si="21">Y31/AB31</f>
+        <f t="shared" ref="AE31:AE32" si="9">Y31/AB31</f>
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>32</v>
       </c>
@@ -3389,7 +3389,7 @@
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2">
-        <f t="shared" si="17"/>
+        <f>G32*E32*D32</f>
         <v>2688</v>
       </c>
       <c r="O32" s="2">
@@ -3397,7 +3397,7 @@
         <v>36864</v>
       </c>
       <c r="P32" s="2">
-        <f t="shared" si="18"/>
+        <f>D32^2*8*8</f>
         <v>576</v>
       </c>
       <c r="Q32" s="2">
@@ -3405,11 +3405,11 @@
         <v>128</v>
       </c>
       <c r="R32" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="8"/>
         <v>36992</v>
       </c>
       <c r="S32" s="6" t="str">
-        <f t="shared" si="20"/>
+        <f>DEC2HEX(J32,2)&amp;DEC2HEX(G32,2)&amp;"_"&amp;DEC2HEX(D32,2)&amp;DEC2HEX(H32,1)&amp;DEC2HEX(C32,1)</f>
         <v>1C1C_0311</v>
       </c>
       <c r="T32" s="2" t="str">
@@ -3455,11 +3455,11 @@
         <v>84</v>
       </c>
       <c r="AE32" s="14">
-        <f t="shared" si="21"/>
+        <f t="shared" si="9"/>
         <v>384</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>33</v>
       </c>
@@ -3496,7 +3496,7 @@
       <c r="AD33" s="12"/>
       <c r="AE33" s="14"/>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>34</v>
       </c>
@@ -3533,7 +3533,7 @@
       <c r="AD34" s="12"/>
       <c r="AE34" s="14"/>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>35</v>
       </c>
@@ -3576,7 +3576,7 @@
       <c r="AD35" s="10"/>
       <c r="AE35" s="14"/>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>36</v>
       </c>
@@ -3670,11 +3670,11 @@
         <v>84</v>
       </c>
       <c r="AE36" s="14">
-        <f t="shared" ref="AE36:AE37" si="22">Y36/AB36</f>
+        <f t="shared" ref="AE36:AE37" si="10">Y36/AB36</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>37</v>
       </c>
@@ -3783,11 +3783,11 @@
         <v>14</v>
       </c>
       <c r="AE37" s="14">
-        <f t="shared" si="22"/>
+        <f t="shared" si="10"/>
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>38</v>
       </c>
@@ -3824,7 +3824,7 @@
       <c r="AD38" s="12"/>
       <c r="AE38" s="14"/>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>39</v>
       </c>
@@ -3864,7 +3864,7 @@
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2">
-        <f t="shared" ref="N39:N40" si="23">G39*E39*D39</f>
+        <f>G39*E39*D39</f>
         <v>672</v>
       </c>
       <c r="O39" s="2">
@@ -3872,7 +3872,7 @@
         <v>9216</v>
       </c>
       <c r="P39" s="2">
-        <f t="shared" ref="P39:P40" si="24">D39^2*8*8</f>
+        <f>D39^2*8*8</f>
         <v>64</v>
       </c>
       <c r="Q39" s="2">
@@ -3880,11 +3880,11 @@
         <v>192</v>
       </c>
       <c r="R39" s="2">
-        <f t="shared" ref="R39:R40" si="25">O39+Q39</f>
+        <f t="shared" ref="R39:R40" si="11">O39+Q39</f>
         <v>9408</v>
       </c>
       <c r="S39" s="6" t="str">
-        <f t="shared" ref="S39:S40" si="26">DEC2HEX(J39,2)&amp;DEC2HEX(G39,2)&amp;"_"&amp;DEC2HEX(D39,2)&amp;DEC2HEX(H39,1)&amp;DEC2HEX(C39,1)</f>
+        <f>DEC2HEX(J39,2)&amp;DEC2HEX(G39,2)&amp;"_"&amp;DEC2HEX(D39,2)&amp;DEC2HEX(H39,1)&amp;DEC2HEX(C39,1)</f>
         <v>0E0E_0111</v>
       </c>
       <c r="T39" s="2" t="str">
@@ -3930,11 +3930,11 @@
         <v>14</v>
       </c>
       <c r="AE39" s="14">
-        <f t="shared" ref="AE39:AE40" si="27">Y39/AB39</f>
+        <f t="shared" ref="AE39:AE40" si="12">Y39/AB39</f>
         <v>192</v>
       </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>40</v>
       </c>
@@ -3974,7 +3974,7 @@
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2">
-        <f t="shared" si="23"/>
+        <f>G40*E40*D40</f>
         <v>2016</v>
       </c>
       <c r="O40" s="2">
@@ -3982,7 +3982,7 @@
         <v>82944</v>
       </c>
       <c r="P40" s="2">
-        <f t="shared" si="24"/>
+        <f>D40^2*8*8</f>
         <v>576</v>
       </c>
       <c r="Q40" s="2">
@@ -3990,11 +3990,11 @@
         <v>192</v>
       </c>
       <c r="R40" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="11"/>
         <v>83136</v>
       </c>
       <c r="S40" s="6" t="str">
-        <f t="shared" si="26"/>
+        <f>DEC2HEX(J40,2)&amp;DEC2HEX(G40,2)&amp;"_"&amp;DEC2HEX(D40,2)&amp;DEC2HEX(H40,1)&amp;DEC2HEX(C40,1)</f>
         <v>0E0E_0311</v>
       </c>
       <c r="T40" s="2" t="str">
@@ -4040,11 +4040,11 @@
         <v>42</v>
       </c>
       <c r="AE40" s="14">
-        <f t="shared" si="27"/>
+        <f t="shared" si="12"/>
         <v>576</v>
       </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>41</v>
       </c>
@@ -4081,7 +4081,7 @@
       <c r="AD41" s="12"/>
       <c r="AE41" s="14"/>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>42</v>
       </c>
@@ -4118,7 +4118,7 @@
       <c r="AD42" s="12"/>
       <c r="AE42" s="14"/>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>43</v>
       </c>
@@ -4161,7 +4161,7 @@
       <c r="AD43" s="10"/>
       <c r="AE43" s="14"/>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>44</v>
       </c>
@@ -4274,7 +4274,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>45</v>
       </c>
@@ -4311,7 +4311,7 @@
       <c r="AD45" s="12"/>
       <c r="AE45" s="14"/>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>46</v>
       </c>
@@ -4351,7 +4351,7 @@
       </c>
       <c r="M46" s="2"/>
       <c r="N46" s="2">
-        <f t="shared" ref="N46:N47" si="28">G46*E46*D46</f>
+        <f>G46*E46*D46</f>
         <v>672</v>
       </c>
       <c r="O46" s="2">
@@ -4359,7 +4359,7 @@
         <v>9216</v>
       </c>
       <c r="P46" s="2">
-        <f t="shared" ref="P46:P47" si="29">D46^2*8*8</f>
+        <f>D46^2*8*8</f>
         <v>64</v>
       </c>
       <c r="Q46" s="2">
@@ -4367,11 +4367,11 @@
         <v>192</v>
       </c>
       <c r="R46" s="2">
-        <f t="shared" ref="R46:R47" si="30">O46+Q46</f>
+        <f t="shared" ref="R46:R47" si="13">O46+Q46</f>
         <v>9408</v>
       </c>
       <c r="S46" s="6" t="str">
-        <f t="shared" ref="S46:S47" si="31">DEC2HEX(J46,2)&amp;DEC2HEX(G46,2)&amp;"_"&amp;DEC2HEX(D46,2)&amp;DEC2HEX(H46,1)&amp;DEC2HEX(C46,1)</f>
+        <f>DEC2HEX(J46,2)&amp;DEC2HEX(G46,2)&amp;"_"&amp;DEC2HEX(D46,2)&amp;DEC2HEX(H46,1)&amp;DEC2HEX(C46,1)</f>
         <v>0E0E_0111</v>
       </c>
       <c r="T46" s="2" t="str">
@@ -4417,11 +4417,11 @@
         <v>14</v>
       </c>
       <c r="AE46" s="14">
-        <f t="shared" ref="AE46:AE47" si="32">Y46/AB46</f>
+        <f t="shared" ref="AE46:AE47" si="14">Y46/AB46</f>
         <v>192</v>
       </c>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>47</v>
       </c>
@@ -4461,7 +4461,7 @@
       </c>
       <c r="M47" s="2"/>
       <c r="N47" s="2">
-        <f t="shared" si="28"/>
+        <f>G47*E47*D47</f>
         <v>2016</v>
       </c>
       <c r="O47" s="2">
@@ -4469,7 +4469,7 @@
         <v>82944</v>
       </c>
       <c r="P47" s="2">
-        <f t="shared" si="29"/>
+        <f>D47^2*8*8</f>
         <v>576</v>
       </c>
       <c r="Q47" s="2">
@@ -4477,11 +4477,11 @@
         <v>192</v>
       </c>
       <c r="R47" s="2">
-        <f t="shared" si="30"/>
+        <f t="shared" si="13"/>
         <v>83136</v>
       </c>
       <c r="S47" s="6" t="str">
-        <f t="shared" si="31"/>
+        <f>DEC2HEX(J47,2)&amp;DEC2HEX(G47,2)&amp;"_"&amp;DEC2HEX(D47,2)&amp;DEC2HEX(H47,1)&amp;DEC2HEX(C47,1)</f>
         <v>0E0E_0311</v>
       </c>
       <c r="T47" s="2" t="str">
@@ -4527,11 +4527,11 @@
         <v>42</v>
       </c>
       <c r="AE47" s="14">
-        <f t="shared" si="32"/>
+        <f t="shared" si="14"/>
         <v>576</v>
       </c>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>48</v>
       </c>
@@ -4568,7 +4568,7 @@
       <c r="AD48" s="12"/>
       <c r="AE48" s="14"/>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>49</v>
       </c>
@@ -4605,7 +4605,7 @@
       <c r="AD49" s="12"/>
       <c r="AE49" s="14"/>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>50</v>
       </c>
@@ -4648,7 +4648,7 @@
       <c r="AD50" s="10"/>
       <c r="AE50" s="14"/>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>51</v>
       </c>
@@ -4761,7 +4761,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>52</v>
       </c>
@@ -4798,7 +4798,7 @@
       <c r="AD52" s="12"/>
       <c r="AE52" s="14"/>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>53</v>
       </c>
@@ -4838,7 +4838,7 @@
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2">
-        <f t="shared" ref="N53:N54" si="33">G53*E53*D53</f>
+        <f>G53*E53*D53</f>
         <v>896</v>
       </c>
       <c r="O53" s="2">
@@ -4846,7 +4846,7 @@
         <v>16384</v>
       </c>
       <c r="P53" s="2">
-        <f t="shared" ref="P53:P54" si="34">D53^2*8*8</f>
+        <f>D53^2*8*8</f>
         <v>64</v>
       </c>
       <c r="Q53" s="2">
@@ -4854,11 +4854,11 @@
         <v>256</v>
       </c>
       <c r="R53" s="2">
-        <f t="shared" ref="R53:R54" si="35">O53+Q53</f>
+        <f t="shared" ref="R53:R54" si="15">O53+Q53</f>
         <v>16640</v>
       </c>
       <c r="S53" s="6" t="str">
-        <f t="shared" ref="S53:S54" si="36">DEC2HEX(J53,2)&amp;DEC2HEX(G53,2)&amp;"_"&amp;DEC2HEX(D53,2)&amp;DEC2HEX(H53,1)&amp;DEC2HEX(C53,1)</f>
+        <f>DEC2HEX(J53,2)&amp;DEC2HEX(G53,2)&amp;"_"&amp;DEC2HEX(D53,2)&amp;DEC2HEX(H53,1)&amp;DEC2HEX(C53,1)</f>
         <v>0E0E_0111</v>
       </c>
       <c r="T53" s="2" t="str">
@@ -4904,11 +4904,11 @@
         <v>14</v>
       </c>
       <c r="AE53" s="14">
-        <f t="shared" ref="AE53:AE54" si="37">Y53/AB53</f>
+        <f t="shared" ref="AE53:AE54" si="16">Y53/AB53</f>
         <v>256</v>
       </c>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>54</v>
       </c>
@@ -4948,7 +4948,7 @@
       </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2">
-        <f t="shared" si="33"/>
+        <f>G54*E54*D54</f>
         <v>2688</v>
       </c>
       <c r="O54" s="2">
@@ -4956,7 +4956,7 @@
         <v>147456</v>
       </c>
       <c r="P54" s="2">
-        <f t="shared" si="34"/>
+        <f>D54^2*8*8</f>
         <v>576</v>
       </c>
       <c r="Q54" s="2">
@@ -4964,11 +4964,11 @@
         <v>256</v>
       </c>
       <c r="R54" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="15"/>
         <v>147712</v>
       </c>
       <c r="S54" s="6" t="str">
-        <f t="shared" si="36"/>
+        <f>DEC2HEX(J54,2)&amp;DEC2HEX(G54,2)&amp;"_"&amp;DEC2HEX(D54,2)&amp;DEC2HEX(H54,1)&amp;DEC2HEX(C54,1)</f>
         <v>0E0E_0311</v>
       </c>
       <c r="T54" s="2" t="str">
@@ -5014,11 +5014,11 @@
         <v>42</v>
       </c>
       <c r="AE54" s="14">
-        <f t="shared" si="37"/>
+        <f t="shared" si="16"/>
         <v>768</v>
       </c>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>55</v>
       </c>
@@ -5055,7 +5055,7 @@
       <c r="AD55" s="12"/>
       <c r="AE55" s="14"/>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>56</v>
       </c>
@@ -5092,7 +5092,7 @@
       <c r="AD56" s="12"/>
       <c r="AE56" s="14"/>
     </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>57</v>
       </c>
@@ -5135,7 +5135,7 @@
       <c r="AD57" s="10"/>
       <c r="AE57" s="14"/>
     </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>58</v>
       </c>
@@ -5248,7 +5248,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>59</v>
       </c>
@@ -5285,7 +5285,7 @@
       <c r="AD59" s="12"/>
       <c r="AE59" s="14"/>
     </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>60</v>
       </c>
@@ -5325,7 +5325,7 @@
       </c>
       <c r="M60" s="2"/>
       <c r="N60" s="2">
-        <f t="shared" ref="N60:N61" si="38">G60*E60*D60</f>
+        <f>G60*E60*D60</f>
         <v>896</v>
       </c>
       <c r="O60" s="2">
@@ -5333,7 +5333,7 @@
         <v>16384</v>
       </c>
       <c r="P60" s="2">
-        <f t="shared" ref="P60:P61" si="39">D60^2*8*8</f>
+        <f>D60^2*8*8</f>
         <v>64</v>
       </c>
       <c r="Q60" s="2">
@@ -5341,11 +5341,11 @@
         <v>256</v>
       </c>
       <c r="R60" s="2">
-        <f t="shared" ref="R60:R61" si="40">O60+Q60</f>
+        <f t="shared" ref="R60:R61" si="17">O60+Q60</f>
         <v>16640</v>
       </c>
       <c r="S60" s="6" t="str">
-        <f t="shared" ref="S60:S61" si="41">DEC2HEX(J60,2)&amp;DEC2HEX(G60,2)&amp;"_"&amp;DEC2HEX(D60,2)&amp;DEC2HEX(H60,1)&amp;DEC2HEX(C60,1)</f>
+        <f>DEC2HEX(J60,2)&amp;DEC2HEX(G60,2)&amp;"_"&amp;DEC2HEX(D60,2)&amp;DEC2HEX(H60,1)&amp;DEC2HEX(C60,1)</f>
         <v>0E0E_0111</v>
       </c>
       <c r="T60" s="2" t="str">
@@ -5391,11 +5391,11 @@
         <v>14</v>
       </c>
       <c r="AE60" s="14">
-        <f t="shared" ref="AE60:AE61" si="42">Y60/AB60</f>
+        <f t="shared" ref="AE60:AE61" si="18">Y60/AB60</f>
         <v>256</v>
       </c>
     </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>61</v>
       </c>
@@ -5435,7 +5435,7 @@
       </c>
       <c r="M61" s="2"/>
       <c r="N61" s="2">
-        <f t="shared" si="38"/>
+        <f>G61*E61*D61</f>
         <v>2688</v>
       </c>
       <c r="O61" s="2">
@@ -5443,7 +5443,7 @@
         <v>147456</v>
       </c>
       <c r="P61" s="2">
-        <f t="shared" si="39"/>
+        <f>D61^2*8*8</f>
         <v>576</v>
       </c>
       <c r="Q61" s="2">
@@ -5451,11 +5451,11 @@
         <v>256</v>
       </c>
       <c r="R61" s="2">
-        <f t="shared" si="40"/>
+        <f t="shared" si="17"/>
         <v>147712</v>
       </c>
       <c r="S61" s="6" t="str">
-        <f t="shared" si="41"/>
+        <f>DEC2HEX(J61,2)&amp;DEC2HEX(G61,2)&amp;"_"&amp;DEC2HEX(D61,2)&amp;DEC2HEX(H61,1)&amp;DEC2HEX(C61,1)</f>
         <v>0E0E_0311</v>
       </c>
       <c r="T61" s="2" t="str">
@@ -5501,11 +5501,11 @@
         <v>42</v>
       </c>
       <c r="AE61" s="14">
-        <f t="shared" si="42"/>
+        <f t="shared" si="18"/>
         <v>768</v>
       </c>
     </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>62</v>
       </c>
@@ -5542,7 +5542,7 @@
       <c r="AD62" s="12"/>
       <c r="AE62" s="14"/>
     </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>63</v>
       </c>
@@ -5579,7 +5579,7 @@
       <c r="AD63" s="12"/>
       <c r="AE63" s="14"/>
     </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>64</v>
       </c>
@@ -5622,7 +5622,7 @@
       <c r="AD64" s="10"/>
       <c r="AE64" s="14"/>
     </row>
-    <row r="65" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A65" s="19" t="s">
         <v>65</v>
       </c>
@@ -5659,7 +5659,7 @@
       <c r="AD65" s="12"/>
       <c r="AE65" s="14"/>
     </row>
-    <row r="66" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>66</v>
       </c>
@@ -5769,7 +5769,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="67" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>67</v>
       </c>
@@ -5806,7 +5806,7 @@
       <c r="AD67" s="12"/>
       <c r="AE67" s="14"/>
     </row>
-    <row r="68" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>68</v>
       </c>
@@ -5904,7 +5904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>69</v>
       </c>
@@ -5940,7 +5940,7 @@
       <c r="AC69" s="1"/>
       <c r="AD69" s="10"/>
     </row>
-    <row r="70" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A70" s="9"/>
       <c r="B70" s="14"/>
       <c r="C70" s="14"/>
@@ -5981,7 +5981,7 @@
       <c r="W70" s="14"/>
       <c r="X70" s="14"/>
       <c r="Y70" s="14">
-        <f t="shared" ref="Y70" si="43">SUM(Y4:Y69)</f>
+        <f t="shared" ref="Y70" si="19">SUM(Y4:Y69)</f>
         <v>391104608</v>
       </c>
       <c r="Z70" s="14">
@@ -6006,7 +6006,7 @@
         <v>5.2825624061684247</v>
       </c>
     </row>
-    <row r="71" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A71" s="9"/>
       <c r="B71" s="14"/>
       <c r="C71" s="14"/>
@@ -6056,7 +6056,7 @@
     <mergeCell ref="Y1:AA1"/>
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="N1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6071,16 +6071,16 @@
       <selection activeCell="I1" sqref="I1:K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" customWidth="1"/>
-    <col min="9" max="13" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" customWidth="1"/>
+    <col min="9" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>148</v>
       </c>
@@ -6128,7 +6128,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>149</v>
       </c>
@@ -6176,7 +6176,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>140</v>
       </c>
@@ -6224,7 +6224,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>140</v>
       </c>
@@ -6272,7 +6272,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>150</v>
       </c>
@@ -6320,7 +6320,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>140</v>
       </c>
@@ -6368,7 +6368,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>140</v>
       </c>
@@ -6416,7 +6416,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>150</v>
       </c>
@@ -6464,7 +6464,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>151</v>
       </c>
@@ -6512,7 +6512,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>141</v>
       </c>
@@ -6560,7 +6560,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>141</v>
       </c>
@@ -6608,7 +6608,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>152</v>
       </c>
@@ -6656,7 +6656,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>141</v>
       </c>
@@ -6704,7 +6704,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>141</v>
       </c>
@@ -6752,7 +6752,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>152</v>
       </c>
@@ -6800,7 +6800,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>153</v>
       </c>
@@ -6848,7 +6848,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>142</v>
       </c>
@@ -6896,7 +6896,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>142</v>
       </c>
@@ -6944,7 +6944,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>154</v>
       </c>
@@ -6992,7 +6992,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>142</v>
       </c>
@@ -7040,7 +7040,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>142</v>
       </c>
@@ -7088,7 +7088,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>154</v>
       </c>
@@ -7136,7 +7136,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>142</v>
       </c>
@@ -7184,7 +7184,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>142</v>
       </c>
@@ -7232,7 +7232,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>154</v>
       </c>
@@ -7280,7 +7280,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>142</v>
       </c>
@@ -7328,7 +7328,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>142</v>
       </c>
@@ -7376,7 +7376,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>154</v>
       </c>
@@ -7424,7 +7424,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>142</v>
       </c>
@@ -7472,7 +7472,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
Add padding in command
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC51559-283E-4DE5-8A7D-4D18F58ED3C2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD708D2-79D6-4954-B6CE-4249B37661E0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
   <sheets>
     <sheet name="SqueezeNet v2 MEC Parallel Ch" sheetId="2" r:id="rId1"/>
@@ -721,13 +721,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1061,13 +1061,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80B23C6-EAEB-43B1-B045-456C36085CFA}">
   <dimension ref="A1:AG71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" style="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
@@ -1083,29 +1083,29 @@
     <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="4" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="26.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="26.44140625" style="18" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="10" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="10" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.85546875" style="18" customWidth="1"/>
-    <col min="31" max="31" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.88671875" style="18" customWidth="1"/>
+    <col min="31" max="31" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="10" style="21" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" s="15"/>
       <c r="B1" s="16"/>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
       <c r="F1" s="17"/>
       <c r="G1" s="17"/>
       <c r="H1" s="16"/>
@@ -1114,11 +1114,11 @@
       <c r="K1" s="23"/>
       <c r="L1" s="23"/>
       <c r="M1" s="23"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
       <c r="S1" s="23"/>
       <c r="T1" s="28"/>
       <c r="U1" s="32" t="s">
@@ -1128,21 +1128,21 @@
       <c r="W1" s="34"/>
       <c r="Y1" s="23"/>
       <c r="Z1" s="27"/>
-      <c r="AA1" s="31" t="s">
+      <c r="AA1" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="30" t="s">
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="AE1" s="29"/>
+      <c r="AE1" s="30"/>
       <c r="AF1" s="26"/>
       <c r="AG1" s="14" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
@@ -1173,10 +1173,10 @@
       <c r="J2" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="L2" s="31"/>
+      <c r="L2" s="29"/>
       <c r="M2" s="14" t="s">
         <v>154</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>0040_0003</v>
       </c>
       <c r="W4" s="11" t="str">
-        <f>DEC2HEX(D4*H4,4)&amp;"_"&amp;DEC2HEX(D4^2,2)&amp;"00"</f>
+        <f>DEC2HEX(D4*H4,4)&amp;"_"&amp;DEC2HEX(D4^2,2)&amp;DEC2HEX(I4,2)</f>
         <v>0006_0900</v>
       </c>
       <c r="X4" s="2">
@@ -1412,7 +1412,7 @@
         <v>95.57709251101322</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
@@ -1451,7 +1451,7 @@
       <c r="AF5" s="12"/>
       <c r="AG5" s="14"/>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>0040_0040</v>
       </c>
       <c r="W6" s="13" t="str">
-        <f>DEC2HEX(D6*H6,4)&amp;"_"&amp;DEC2HEX(D6^2,2)&amp;"00"</f>
+        <f>DEC2HEX(D6*H6,4)&amp;"_"&amp;DEC2HEX(D6^2,2)&amp;DEC2HEX(I6,2)</f>
         <v>0006_0900</v>
       </c>
       <c r="X6" s="4">
@@ -1557,7 +1557,7 @@
         <v>1.4867256637168142</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>0010_0040</v>
       </c>
       <c r="W7" s="11" t="str">
-        <f>DEC2HEX(D7*H7,4)&amp;"_"&amp;DEC2HEX(D7^2,2)&amp;"00"</f>
+        <f>DEC2HEX(D7*H7,4)&amp;"_"&amp;DEC2HEX(D7^2,2)&amp;DEC2HEX(I7,2)</f>
         <v>0001_0100</v>
       </c>
       <c r="X7" s="2">
@@ -1678,7 +1678,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
@@ -1717,7 +1717,7 @@
       <c r="AF8" s="12"/>
       <c r="AG8" s="14"/>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>0040_0010</v>
       </c>
       <c r="W9" s="11" t="str">
-        <f>DEC2HEX(D9*H9,4)&amp;"_"&amp;DEC2HEX(D9^2,2)&amp;"00"</f>
+        <f t="shared" ref="W9:W10" si="4">DEC2HEX(D9*H9,4)&amp;"_"&amp;DEC2HEX(D9^2,2)&amp;DEC2HEX(I9,2)</f>
         <v>0001_0100</v>
       </c>
       <c r="X9" s="2">
@@ -1834,11 +1834,11 @@
         <v>56</v>
       </c>
       <c r="AG9" s="14">
-        <f t="shared" ref="AG9:AG10" si="4">AA9/AD9</f>
+        <f t="shared" ref="AG9:AG10" si="5">AA9/AD9</f>
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -1917,8 +1917,8 @@
         <v>0040_0010</v>
       </c>
       <c r="W10" s="11" t="str">
-        <f>DEC2HEX(D10*H10,4)&amp;"_"&amp;DEC2HEX(D10^2,2)&amp;"00"</f>
-        <v>0003_0900</v>
+        <f t="shared" si="4"/>
+        <v>0003_0901</v>
       </c>
       <c r="X10" s="2">
         <v>0.01</v>
@@ -1955,11 +1955,11 @@
         <v>168</v>
       </c>
       <c r="AG10" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
@@ -1998,7 +1998,7 @@
       <c r="AF11" s="12"/>
       <c r="AG11" s="14"/>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>12</v>
       </c>
@@ -2037,7 +2037,7 @@
       <c r="AF12" s="12"/>
       <c r="AG12" s="14"/>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>19</v>
       </c>
@@ -2082,7 +2082,7 @@
       <c r="AF13" s="10"/>
       <c r="AG13" s="14"/>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>13</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>0010_0080</v>
       </c>
       <c r="W14" s="11" t="str">
-        <f>DEC2HEX(D14*H14,4)&amp;"_"&amp;DEC2HEX(D14^2,2)&amp;"00"</f>
+        <f>DEC2HEX(D14*H14,4)&amp;"_"&amp;DEC2HEX(D14^2,2)&amp;DEC2HEX(I14,2)</f>
         <v>0001_0100</v>
       </c>
       <c r="X14" s="2">
@@ -2203,7 +2203,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>14</v>
       </c>
@@ -2242,7 +2242,7 @@
       <c r="AF15" s="12"/>
       <c r="AG15" s="14"/>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
@@ -2281,15 +2281,15 @@
         <v>200704</v>
       </c>
       <c r="M16" s="2">
-        <f t="shared" ref="M16:M17" si="5">G16^2*E16*D16</f>
+        <f t="shared" ref="M16:M17" si="6">G16^2*E16*D16</f>
         <v>50176</v>
       </c>
       <c r="N16" s="2">
-        <f t="shared" ref="N16:N17" si="6">M16/G16</f>
+        <f t="shared" ref="N16:N17" si="7">M16/G16</f>
         <v>896</v>
       </c>
       <c r="O16" s="2">
-        <f t="shared" ref="O16:O17" si="7">N16/8</f>
+        <f t="shared" ref="O16:O17" si="8">N16/8</f>
         <v>112</v>
       </c>
       <c r="P16" s="2">
@@ -2321,7 +2321,7 @@
         <v>0040_0010</v>
       </c>
       <c r="W16" s="11" t="str">
-        <f>DEC2HEX(D16*H16,4)&amp;"_"&amp;DEC2HEX(D16^2,2)&amp;"00"</f>
+        <f t="shared" ref="W16:W17" si="9">DEC2HEX(D16*H16,4)&amp;"_"&amp;DEC2HEX(D16^2,2)&amp;DEC2HEX(I16,2)</f>
         <v>0001_0100</v>
       </c>
       <c r="X16" s="2">
@@ -2359,11 +2359,11 @@
         <v>56</v>
       </c>
       <c r="AG16" s="14">
-        <f t="shared" ref="AG16:AG17" si="8">AA16/AD16</f>
+        <f t="shared" ref="AG16:AG17" si="10">AA16/AD16</f>
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
@@ -2402,15 +2402,15 @@
         <v>200704</v>
       </c>
       <c r="M17" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>150528</v>
       </c>
       <c r="N17" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2688</v>
       </c>
       <c r="O17" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>336</v>
       </c>
       <c r="P17" s="2">
@@ -2442,8 +2442,8 @@
         <v>0040_0010</v>
       </c>
       <c r="W17" s="11" t="str">
-        <f>DEC2HEX(D17*H17,4)&amp;"_"&amp;DEC2HEX(D17^2,2)&amp;"00"</f>
-        <v>0003_0900</v>
+        <f t="shared" si="9"/>
+        <v>0003_0901</v>
       </c>
       <c r="X17" s="2">
         <v>0.01</v>
@@ -2480,11 +2480,11 @@
         <v>168</v>
       </c>
       <c r="AG17" s="14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>17</v>
       </c>
@@ -2523,7 +2523,7 @@
       <c r="AF18" s="12"/>
       <c r="AG18" s="14"/>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>18</v>
       </c>
@@ -2562,7 +2562,7 @@
       <c r="AF19" s="12"/>
       <c r="AG19" s="14"/>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>20</v>
       </c>
@@ -2607,7 +2607,7 @@
       <c r="AF20" s="10"/>
       <c r="AG20" s="14"/>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>21</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>0080_0080</v>
       </c>
       <c r="W21" s="13" t="str">
-        <f>DEC2HEX(D21*H21,4)&amp;"_"&amp;DEC2HEX(D21^2,2)&amp;"00"</f>
+        <f>DEC2HEX(D21*H21,4)&amp;"_"&amp;DEC2HEX(D21^2,2)&amp;DEC2HEX(I21,2)</f>
         <v>0006_0900</v>
       </c>
       <c r="X21" s="4">
@@ -2709,11 +2709,11 @@
         <v>168</v>
       </c>
       <c r="AG21" s="14">
-        <f t="shared" ref="AG21:AG22" si="9">AA21/AD21</f>
+        <f t="shared" ref="AG21:AG22" si="11">AA21/AD21</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>0020_0080</v>
       </c>
       <c r="W22" s="11" t="str">
-        <f>DEC2HEX(D22*H22,4)&amp;"_"&amp;DEC2HEX(D22^2,2)&amp;"00"</f>
+        <f>DEC2HEX(D22*H22,4)&amp;"_"&amp;DEC2HEX(D22^2,2)&amp;DEC2HEX(I22,2)</f>
         <v>0001_0100</v>
       </c>
       <c r="X22" s="2">
@@ -2830,11 +2830,11 @@
         <v>28</v>
       </c>
       <c r="AG22" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>23</v>
       </c>
@@ -2873,7 +2873,7 @@
       <c r="AF23" s="12"/>
       <c r="AG23" s="14"/>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>24</v>
       </c>
@@ -2912,15 +2912,15 @@
         <v>100352</v>
       </c>
       <c r="M24" s="2">
-        <f t="shared" ref="M24:M25" si="10">G24^2*E24*D24</f>
+        <f t="shared" ref="M24:M25" si="12">G24^2*E24*D24</f>
         <v>25088</v>
       </c>
       <c r="N24" s="2">
-        <f t="shared" ref="N24:N25" si="11">M24/G24</f>
+        <f t="shared" ref="N24:N25" si="13">M24/G24</f>
         <v>896</v>
       </c>
       <c r="O24" s="2">
-        <f t="shared" ref="O24:O25" si="12">N24/8</f>
+        <f t="shared" ref="O24:O25" si="14">N24/8</f>
         <v>112</v>
       </c>
       <c r="P24" s="2">
@@ -2952,7 +2952,7 @@
         <v>0080_0020</v>
       </c>
       <c r="W24" s="11" t="str">
-        <f>DEC2HEX(D24*H24,4)&amp;"_"&amp;DEC2HEX(D24^2,2)&amp;"00"</f>
+        <f t="shared" ref="W24:W25" si="15">DEC2HEX(D24*H24,4)&amp;"_"&amp;DEC2HEX(D24^2,2)&amp;DEC2HEX(I24,2)</f>
         <v>0001_0100</v>
       </c>
       <c r="X24" s="2">
@@ -2990,11 +2990,11 @@
         <v>28</v>
       </c>
       <c r="AG24" s="14">
-        <f t="shared" ref="AG24:AG25" si="13">AA24/AD24</f>
+        <f t="shared" ref="AG24:AG25" si="16">AA24/AD24</f>
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>25</v>
       </c>
@@ -3033,15 +3033,15 @@
         <v>100352</v>
       </c>
       <c r="M25" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>75264</v>
       </c>
       <c r="N25" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>2688</v>
       </c>
       <c r="O25" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>336</v>
       </c>
       <c r="P25" s="2">
@@ -3073,8 +3073,8 @@
         <v>0080_0020</v>
       </c>
       <c r="W25" s="11" t="str">
-        <f>DEC2HEX(D25*H25,4)&amp;"_"&amp;DEC2HEX(D25^2,2)&amp;"00"</f>
-        <v>0003_0900</v>
+        <f t="shared" si="15"/>
+        <v>0003_0901</v>
       </c>
       <c r="X25" s="2">
         <v>0.01</v>
@@ -3111,11 +3111,11 @@
         <v>84</v>
       </c>
       <c r="AG25" s="14">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>384</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>26</v>
       </c>
@@ -3154,7 +3154,7 @@
       <c r="AF26" s="12"/>
       <c r="AG26" s="14"/>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>27</v>
       </c>
@@ -3193,7 +3193,7 @@
       <c r="AF27" s="12"/>
       <c r="AG27" s="14"/>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>28</v>
       </c>
@@ -3238,7 +3238,7 @@
       <c r="AF28" s="10"/>
       <c r="AG28" s="14"/>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>29</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>0020_0100</v>
       </c>
       <c r="W29" s="11" t="str">
-        <f>DEC2HEX(D29*H29,4)&amp;"_"&amp;DEC2HEX(D29^2,2)&amp;"00"</f>
+        <f>DEC2HEX(D29*H29,4)&amp;"_"&amp;DEC2HEX(D29^2,2)&amp;DEC2HEX(I29,2)</f>
         <v>0001_0100</v>
       </c>
       <c r="X29" s="2">
@@ -3359,7 +3359,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>30</v>
       </c>
@@ -3398,7 +3398,7 @@
       <c r="AF30" s="12"/>
       <c r="AG30" s="14"/>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>31</v>
       </c>
@@ -3437,15 +3437,15 @@
         <v>100352</v>
       </c>
       <c r="M31" s="2">
-        <f t="shared" ref="M31:M32" si="14">G31^2*E31*D31</f>
+        <f t="shared" ref="M31:M32" si="17">G31^2*E31*D31</f>
         <v>25088</v>
       </c>
       <c r="N31" s="2">
-        <f t="shared" ref="N31:N32" si="15">M31/G31</f>
+        <f t="shared" ref="N31:N32" si="18">M31/G31</f>
         <v>896</v>
       </c>
       <c r="O31" s="2">
-        <f t="shared" ref="O31:O32" si="16">N31/8</f>
+        <f t="shared" ref="O31:O32" si="19">N31/8</f>
         <v>112</v>
       </c>
       <c r="P31" s="2">
@@ -3477,7 +3477,7 @@
         <v>0080_0020</v>
       </c>
       <c r="W31" s="11" t="str">
-        <f>DEC2HEX(D31*H31,4)&amp;"_"&amp;DEC2HEX(D31^2,2)&amp;"00"</f>
+        <f t="shared" ref="W31:W32" si="20">DEC2HEX(D31*H31,4)&amp;"_"&amp;DEC2HEX(D31^2,2)&amp;DEC2HEX(I31,2)</f>
         <v>0001_0100</v>
       </c>
       <c r="X31" s="2">
@@ -3515,11 +3515,11 @@
         <v>28</v>
       </c>
       <c r="AG31" s="14">
-        <f t="shared" ref="AG31:AG32" si="17">AA31/AD31</f>
+        <f t="shared" ref="AG31:AG32" si="21">AA31/AD31</f>
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>32</v>
       </c>
@@ -3558,15 +3558,15 @@
         <v>100352</v>
       </c>
       <c r="M32" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>75264</v>
       </c>
       <c r="N32" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>2688</v>
       </c>
       <c r="O32" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>336</v>
       </c>
       <c r="P32" s="2">
@@ -3598,8 +3598,8 @@
         <v>0080_0020</v>
       </c>
       <c r="W32" s="11" t="str">
-        <f>DEC2HEX(D32*H32,4)&amp;"_"&amp;DEC2HEX(D32^2,2)&amp;"00"</f>
-        <v>0003_0900</v>
+        <f t="shared" si="20"/>
+        <v>0003_0901</v>
       </c>
       <c r="X32" s="2">
         <v>0.01</v>
@@ -3636,11 +3636,11 @@
         <v>84</v>
       </c>
       <c r="AG32" s="14">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>384</v>
       </c>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>33</v>
       </c>
@@ -3679,7 +3679,7 @@
       <c r="AF33" s="12"/>
       <c r="AG33" s="14"/>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>34</v>
       </c>
@@ -3718,7 +3718,7 @@
       <c r="AF34" s="12"/>
       <c r="AG34" s="14"/>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>35</v>
       </c>
@@ -3763,7 +3763,7 @@
       <c r="AF35" s="10"/>
       <c r="AG35" s="14"/>
     </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>36</v>
       </c>
@@ -3827,7 +3827,7 @@
         <v>0100_0100</v>
       </c>
       <c r="W36" s="13" t="str">
-        <f>DEC2HEX(D36*H36,4)&amp;"_"&amp;DEC2HEX(D36^2,2)&amp;"00"</f>
+        <f>DEC2HEX(D36*H36,4)&amp;"_"&amp;DEC2HEX(D36^2,2)&amp;DEC2HEX(I36,2)</f>
         <v>0006_0900</v>
       </c>
       <c r="X36" s="4">
@@ -3865,11 +3865,11 @@
         <v>84</v>
       </c>
       <c r="AG36" s="14">
-        <f t="shared" ref="AG36:AG37" si="18">AA36/AD36</f>
+        <f t="shared" ref="AG36:AG37" si="22">AA36/AD36</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>37</v>
       </c>
@@ -3948,7 +3948,7 @@
         <v>0030_0100</v>
       </c>
       <c r="W37" s="11" t="str">
-        <f>DEC2HEX(D37*H37,4)&amp;"_"&amp;DEC2HEX(D37^2,2)&amp;"00"</f>
+        <f>DEC2HEX(D37*H37,4)&amp;"_"&amp;DEC2HEX(D37^2,2)&amp;DEC2HEX(I37,2)</f>
         <v>0001_0100</v>
       </c>
       <c r="X37" s="2">
@@ -3986,11 +3986,11 @@
         <v>14</v>
       </c>
       <c r="AG37" s="14">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>38</v>
       </c>
@@ -4029,7 +4029,7 @@
       <c r="AF38" s="12"/>
       <c r="AG38" s="14"/>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>39</v>
       </c>
@@ -4068,15 +4068,15 @@
         <v>37632</v>
       </c>
       <c r="M39" s="2">
-        <f t="shared" ref="M39:M40" si="19">G39^2*E39*D39</f>
+        <f t="shared" ref="M39:M40" si="23">G39^2*E39*D39</f>
         <v>9408</v>
       </c>
       <c r="N39" s="2">
-        <f t="shared" ref="N39:N40" si="20">M39/G39</f>
+        <f t="shared" ref="N39:N40" si="24">M39/G39</f>
         <v>672</v>
       </c>
       <c r="O39" s="2">
-        <f t="shared" ref="O39:O40" si="21">N39/8</f>
+        <f t="shared" ref="O39:O40" si="25">N39/8</f>
         <v>84</v>
       </c>
       <c r="P39" s="2">
@@ -4108,7 +4108,7 @@
         <v>00C0_0030</v>
       </c>
       <c r="W39" s="11" t="str">
-        <f>DEC2HEX(D39*H39,4)&amp;"_"&amp;DEC2HEX(D39^2,2)&amp;"00"</f>
+        <f t="shared" ref="W39:W40" si="26">DEC2HEX(D39*H39,4)&amp;"_"&amp;DEC2HEX(D39^2,2)&amp;DEC2HEX(I39,2)</f>
         <v>0001_0100</v>
       </c>
       <c r="X39" s="2">
@@ -4146,11 +4146,11 @@
         <v>14</v>
       </c>
       <c r="AG39" s="14">
-        <f t="shared" ref="AG39:AG40" si="22">AA39/AD39</f>
+        <f t="shared" ref="AG39:AG40" si="27">AA39/AD39</f>
         <v>192</v>
       </c>
     </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>40</v>
       </c>
@@ -4189,15 +4189,15 @@
         <v>37632</v>
       </c>
       <c r="M40" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>28224</v>
       </c>
       <c r="N40" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>2016</v>
       </c>
       <c r="O40" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>252</v>
       </c>
       <c r="P40" s="2">
@@ -4229,8 +4229,8 @@
         <v>00C0_0030</v>
       </c>
       <c r="W40" s="11" t="str">
-        <f>DEC2HEX(D40*H40,4)&amp;"_"&amp;DEC2HEX(D40^2,2)&amp;"00"</f>
-        <v>0003_0900</v>
+        <f t="shared" si="26"/>
+        <v>0003_0901</v>
       </c>
       <c r="X40" s="2">
         <v>0.01</v>
@@ -4267,11 +4267,11 @@
         <v>42</v>
       </c>
       <c r="AG40" s="14">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>576</v>
       </c>
     </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>41</v>
       </c>
@@ -4310,7 +4310,7 @@
       <c r="AF41" s="12"/>
       <c r="AG41" s="14"/>
     </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>42</v>
       </c>
@@ -4349,7 +4349,7 @@
       <c r="AF42" s="12"/>
       <c r="AG42" s="14"/>
     </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>43</v>
       </c>
@@ -4394,7 +4394,7 @@
       <c r="AF43" s="10"/>
       <c r="AG43" s="14"/>
     </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>44</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>0030_0180</v>
       </c>
       <c r="W44" s="11" t="str">
-        <f>DEC2HEX(D44*H44,4)&amp;"_"&amp;DEC2HEX(D44^2,2)&amp;"00"</f>
+        <f>DEC2HEX(D44*H44,4)&amp;"_"&amp;DEC2HEX(D44^2,2)&amp;DEC2HEX(I44,2)</f>
         <v>0001_0100</v>
       </c>
       <c r="X44" s="2">
@@ -4515,7 +4515,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>45</v>
       </c>
@@ -4554,7 +4554,7 @@
       <c r="AF45" s="12"/>
       <c r="AG45" s="14"/>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>46</v>
       </c>
@@ -4593,15 +4593,15 @@
         <v>37632</v>
       </c>
       <c r="M46" s="2">
-        <f t="shared" ref="M46:M47" si="23">G46^2*E46*D46</f>
+        <f t="shared" ref="M46:M47" si="28">G46^2*E46*D46</f>
         <v>9408</v>
       </c>
       <c r="N46" s="2">
-        <f t="shared" ref="N46:N47" si="24">M46/G46</f>
+        <f t="shared" ref="N46:N47" si="29">M46/G46</f>
         <v>672</v>
       </c>
       <c r="O46" s="2">
-        <f t="shared" ref="O46:O47" si="25">N46/8</f>
+        <f t="shared" ref="O46:O47" si="30">N46/8</f>
         <v>84</v>
       </c>
       <c r="P46" s="2">
@@ -4633,7 +4633,7 @@
         <v>00C0_0030</v>
       </c>
       <c r="W46" s="11" t="str">
-        <f>DEC2HEX(D46*H46,4)&amp;"_"&amp;DEC2HEX(D46^2,2)&amp;"00"</f>
+        <f t="shared" ref="W46:W47" si="31">DEC2HEX(D46*H46,4)&amp;"_"&amp;DEC2HEX(D46^2,2)&amp;DEC2HEX(I46,2)</f>
         <v>0001_0100</v>
       </c>
       <c r="X46" s="2">
@@ -4671,11 +4671,11 @@
         <v>14</v>
       </c>
       <c r="AG46" s="14">
-        <f t="shared" ref="AG46:AG47" si="26">AA46/AD46</f>
+        <f t="shared" ref="AG46:AG47" si="32">AA46/AD46</f>
         <v>192</v>
       </c>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>47</v>
       </c>
@@ -4714,15 +4714,15 @@
         <v>37632</v>
       </c>
       <c r="M47" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>28224</v>
       </c>
       <c r="N47" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>2016</v>
       </c>
       <c r="O47" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>252</v>
       </c>
       <c r="P47" s="2">
@@ -4754,8 +4754,8 @@
         <v>00C0_0030</v>
       </c>
       <c r="W47" s="11" t="str">
-        <f>DEC2HEX(D47*H47,4)&amp;"_"&amp;DEC2HEX(D47^2,2)&amp;"00"</f>
-        <v>0003_0900</v>
+        <f t="shared" si="31"/>
+        <v>0003_0901</v>
       </c>
       <c r="X47" s="2">
         <v>0.01</v>
@@ -4792,11 +4792,11 @@
         <v>42</v>
       </c>
       <c r="AG47" s="14">
-        <f t="shared" si="26"/>
+        <f t="shared" si="32"/>
         <v>576</v>
       </c>
     </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>48</v>
       </c>
@@ -4835,7 +4835,7 @@
       <c r="AF48" s="12"/>
       <c r="AG48" s="14"/>
     </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>49</v>
       </c>
@@ -4874,7 +4874,7 @@
       <c r="AF49" s="12"/>
       <c r="AG49" s="14"/>
     </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>50</v>
       </c>
@@ -4919,7 +4919,7 @@
       <c r="AF50" s="10"/>
       <c r="AG50" s="14"/>
     </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
         <v>51</v>
       </c>
@@ -4998,7 +4998,7 @@
         <v>0040_0180</v>
       </c>
       <c r="W51" s="11" t="str">
-        <f>DEC2HEX(D51*H51,4)&amp;"_"&amp;DEC2HEX(D51^2,2)&amp;"00"</f>
+        <f>DEC2HEX(D51*H51,4)&amp;"_"&amp;DEC2HEX(D51^2,2)&amp;DEC2HEX(I51,2)</f>
         <v>0001_0100</v>
       </c>
       <c r="X51" s="2">
@@ -5040,7 +5040,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>52</v>
       </c>
@@ -5079,7 +5079,7 @@
       <c r="AF52" s="12"/>
       <c r="AG52" s="14"/>
     </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>53</v>
       </c>
@@ -5118,15 +5118,15 @@
         <v>50176</v>
       </c>
       <c r="M53" s="2">
-        <f t="shared" ref="M53:M54" si="27">G53^2*E53*D53</f>
+        <f t="shared" ref="M53:M54" si="33">G53^2*E53*D53</f>
         <v>12544</v>
       </c>
       <c r="N53" s="2">
-        <f t="shared" ref="N53:N54" si="28">M53/G53</f>
+        <f t="shared" ref="N53:N54" si="34">M53/G53</f>
         <v>896</v>
       </c>
       <c r="O53" s="2">
-        <f t="shared" ref="O53:O54" si="29">N53/8</f>
+        <f t="shared" ref="O53:O54" si="35">N53/8</f>
         <v>112</v>
       </c>
       <c r="P53" s="2">
@@ -5158,7 +5158,7 @@
         <v>0100_0040</v>
       </c>
       <c r="W53" s="11" t="str">
-        <f>DEC2HEX(D53*H53,4)&amp;"_"&amp;DEC2HEX(D53^2,2)&amp;"00"</f>
+        <f t="shared" ref="W53:W54" si="36">DEC2HEX(D53*H53,4)&amp;"_"&amp;DEC2HEX(D53^2,2)&amp;DEC2HEX(I53,2)</f>
         <v>0001_0100</v>
       </c>
       <c r="X53" s="2">
@@ -5196,11 +5196,11 @@
         <v>14</v>
       </c>
       <c r="AG53" s="14">
-        <f t="shared" ref="AG53:AG54" si="30">AA53/AD53</f>
+        <f t="shared" ref="AG53:AG54" si="37">AA53/AD53</f>
         <v>256</v>
       </c>
     </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>54</v>
       </c>
@@ -5239,15 +5239,15 @@
         <v>50176</v>
       </c>
       <c r="M54" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>37632</v>
       </c>
       <c r="N54" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>2688</v>
       </c>
       <c r="O54" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>336</v>
       </c>
       <c r="P54" s="2">
@@ -5279,8 +5279,8 @@
         <v>0100_0040</v>
       </c>
       <c r="W54" s="11" t="str">
-        <f>DEC2HEX(D54*H54,4)&amp;"_"&amp;DEC2HEX(D54^2,2)&amp;"00"</f>
-        <v>0003_0900</v>
+        <f t="shared" si="36"/>
+        <v>0003_0901</v>
       </c>
       <c r="X54" s="2">
         <v>0.01</v>
@@ -5317,11 +5317,11 @@
         <v>42</v>
       </c>
       <c r="AG54" s="14">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>768</v>
       </c>
     </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
         <v>55</v>
       </c>
@@ -5360,7 +5360,7 @@
       <c r="AF55" s="12"/>
       <c r="AG55" s="14"/>
     </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
         <v>56</v>
       </c>
@@ -5399,7 +5399,7 @@
       <c r="AF56" s="12"/>
       <c r="AG56" s="14"/>
     </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>57</v>
       </c>
@@ -5444,7 +5444,7 @@
       <c r="AF57" s="10"/>
       <c r="AG57" s="14"/>
     </row>
-    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>58</v>
       </c>
@@ -5523,7 +5523,7 @@
         <v>0040_0200</v>
       </c>
       <c r="W58" s="11" t="str">
-        <f>DEC2HEX(D58*H58,4)&amp;"_"&amp;DEC2HEX(D58^2,2)&amp;"00"</f>
+        <f>DEC2HEX(D58*H58,4)&amp;"_"&amp;DEC2HEX(D58^2,2)&amp;DEC2HEX(I58,2)</f>
         <v>0001_0100</v>
       </c>
       <c r="X58" s="2">
@@ -5565,7 +5565,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
         <v>59</v>
       </c>
@@ -5604,7 +5604,7 @@
       <c r="AF59" s="12"/>
       <c r="AG59" s="14"/>
     </row>
-    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
         <v>60</v>
       </c>
@@ -5643,15 +5643,15 @@
         <v>50176</v>
       </c>
       <c r="M60" s="2">
-        <f t="shared" ref="M60:M61" si="31">G60^2*E60*D60</f>
+        <f t="shared" ref="M60:M61" si="38">G60^2*E60*D60</f>
         <v>12544</v>
       </c>
       <c r="N60" s="2">
-        <f t="shared" ref="N60:N61" si="32">M60/G60</f>
+        <f t="shared" ref="N60:N61" si="39">M60/G60</f>
         <v>896</v>
       </c>
       <c r="O60" s="2">
-        <f t="shared" ref="O60:O61" si="33">N60/8</f>
+        <f t="shared" ref="O60:O61" si="40">N60/8</f>
         <v>112</v>
       </c>
       <c r="P60" s="2">
@@ -5683,7 +5683,7 @@
         <v>0100_0040</v>
       </c>
       <c r="W60" s="11" t="str">
-        <f>DEC2HEX(D60*H60,4)&amp;"_"&amp;DEC2HEX(D60^2,2)&amp;"00"</f>
+        <f t="shared" ref="W60:W61" si="41">DEC2HEX(D60*H60,4)&amp;"_"&amp;DEC2HEX(D60^2,2)&amp;DEC2HEX(I60,2)</f>
         <v>0001_0100</v>
       </c>
       <c r="X60" s="2">
@@ -5721,11 +5721,11 @@
         <v>14</v>
       </c>
       <c r="AG60" s="14">
-        <f t="shared" ref="AG60:AG61" si="34">AA60/AD60</f>
+        <f t="shared" ref="AG60:AG61" si="42">AA60/AD60</f>
         <v>256</v>
       </c>
     </row>
-    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
         <v>61</v>
       </c>
@@ -5764,15 +5764,15 @@
         <v>50176</v>
       </c>
       <c r="M61" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>37632</v>
       </c>
       <c r="N61" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="39"/>
         <v>2688</v>
       </c>
       <c r="O61" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="40"/>
         <v>336</v>
       </c>
       <c r="P61" s="2">
@@ -5804,8 +5804,8 @@
         <v>0100_0040</v>
       </c>
       <c r="W61" s="11" t="str">
-        <f>DEC2HEX(D61*H61,4)&amp;"_"&amp;DEC2HEX(D61^2,2)&amp;"00"</f>
-        <v>0003_0900</v>
+        <f t="shared" si="41"/>
+        <v>0003_0901</v>
       </c>
       <c r="X61" s="2">
         <v>0.01</v>
@@ -5842,11 +5842,11 @@
         <v>42</v>
       </c>
       <c r="AG61" s="14">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>768</v>
       </c>
     </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
         <v>62</v>
       </c>
@@ -5885,7 +5885,7 @@
       <c r="AF62" s="12"/>
       <c r="AG62" s="14"/>
     </row>
-    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
         <v>63</v>
       </c>
@@ -5924,7 +5924,7 @@
       <c r="AF63" s="12"/>
       <c r="AG63" s="14"/>
     </row>
-    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>64</v>
       </c>
@@ -5969,7 +5969,7 @@
       <c r="AF64" s="10"/>
       <c r="AG64" s="14"/>
     </row>
-    <row r="65" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A65" s="19" t="s">
         <v>65</v>
       </c>
@@ -6008,7 +6008,7 @@
       <c r="AF65" s="12"/>
       <c r="AG65" s="14"/>
     </row>
-    <row r="66" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
         <v>66</v>
       </c>
@@ -6087,7 +6087,7 @@
         <v>03E8_0200</v>
       </c>
       <c r="W66" s="11" t="str">
-        <f>DEC2HEX(D66*H66,4)&amp;"_"&amp;DEC2HEX(D66^2,2)&amp;"00"</f>
+        <f>DEC2HEX(D66*H66,4)&amp;"_"&amp;DEC2HEX(D66^2,2)&amp;DEC2HEX(I66,2)</f>
         <v>0001_0100</v>
       </c>
       <c r="X66" s="2">
@@ -6129,7 +6129,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="67" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A67" s="7" t="s">
         <v>67</v>
       </c>
@@ -6168,7 +6168,7 @@
       <c r="AF67" s="12"/>
       <c r="AG67" s="14"/>
     </row>
-    <row r="68" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A68" s="8" t="s">
         <v>68</v>
       </c>
@@ -6232,7 +6232,7 @@
         <v>03E8_03E8</v>
       </c>
       <c r="W68" s="13" t="str">
-        <f>DEC2HEX(D68*H68,4)&amp;"_"&amp;DEC2HEX(D68^2,2)&amp;"00"</f>
+        <f>DEC2HEX(D68*H68,4)&amp;"_"&amp;DEC2HEX(D68^2,2)&amp;DEC2HEX(I68,2)</f>
         <v>000E_C400</v>
       </c>
       <c r="X68" s="4">
@@ -6274,7 +6274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>69</v>
       </c>
@@ -6312,7 +6312,7 @@
       <c r="AE69" s="1"/>
       <c r="AF69" s="10"/>
     </row>
-    <row r="70" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A70" s="9"/>
       <c r="B70" s="14"/>
       <c r="C70" s="14"/>
@@ -6355,7 +6355,7 @@
       <c r="Y70" s="14"/>
       <c r="Z70" s="14"/>
       <c r="AA70" s="14">
-        <f t="shared" ref="AA70" si="35">SUM(AA4:AA69)</f>
+        <f t="shared" ref="AA70" si="43">SUM(AA4:AA69)</f>
         <v>391104608</v>
       </c>
       <c r="AB70" s="14">
@@ -6380,7 +6380,7 @@
         <v>5.2825624061684247</v>
       </c>
     </row>
-    <row r="71" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A71" s="9"/>
       <c r="B71" s="14"/>
       <c r="C71" s="14"/>
@@ -6447,16 +6447,16 @@
       <selection activeCell="I1" sqref="I1:K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" customWidth="1"/>
-    <col min="9" max="13" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="9" max="13" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>146</v>
       </c>
@@ -6504,7 +6504,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>147</v>
       </c>
@@ -6552,7 +6552,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>138</v>
       </c>
@@ -6600,7 +6600,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>138</v>
       </c>
@@ -6648,7 +6648,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>148</v>
       </c>
@@ -6696,7 +6696,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>138</v>
       </c>
@@ -6744,7 +6744,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>138</v>
       </c>
@@ -6792,7 +6792,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>148</v>
       </c>
@@ -6840,7 +6840,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>149</v>
       </c>
@@ -6888,7 +6888,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>139</v>
       </c>
@@ -6936,7 +6936,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>139</v>
       </c>
@@ -6984,7 +6984,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>150</v>
       </c>
@@ -7032,7 +7032,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>139</v>
       </c>
@@ -7080,7 +7080,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>139</v>
       </c>
@@ -7128,7 +7128,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>150</v>
       </c>
@@ -7176,7 +7176,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>151</v>
       </c>
@@ -7224,7 +7224,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>140</v>
       </c>
@@ -7272,7 +7272,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>140</v>
       </c>
@@ -7320,7 +7320,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>152</v>
       </c>
@@ -7368,7 +7368,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>140</v>
       </c>
@@ -7416,7 +7416,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>140</v>
       </c>
@@ -7464,7 +7464,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>152</v>
       </c>
@@ -7512,7 +7512,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>140</v>
       </c>
@@ -7560,7 +7560,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>140</v>
       </c>
@@ -7608,7 +7608,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>152</v>
       </c>
@@ -7656,7 +7656,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>140</v>
       </c>
@@ -7704,7 +7704,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>140</v>
       </c>
@@ -7752,7 +7752,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>152</v>
       </c>
@@ -7800,7 +7800,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>140</v>
       </c>
@@ -7848,7 +7848,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>153</v>
       </c>

</xml_diff>

<commit_message>
CONV 1x1 is correct now
Reset fsum in design
Split data cube in host client
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD708D2-79D6-4954-B6CE-4249B37661E0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7809BB2-3F7A-4427-9575-2A304E3985B2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="158">
   <si>
     <t>INPUT</t>
   </si>
@@ -460,21 +460,9 @@
     <t>0E0E_0111</t>
   </si>
   <si>
-    <t>0006_0901</t>
-  </si>
-  <si>
-    <t>0001_0103</t>
-  </si>
-  <si>
-    <t>0001_0101</t>
-  </si>
-  <si>
     <t>0003_0901</t>
   </si>
   <si>
-    <t>000E_C401</t>
-  </si>
-  <si>
     <t>71E3_0321</t>
   </si>
   <si>
@@ -512,6 +500,15 @@
   </si>
   <si>
     <t>num</t>
+  </si>
+  <si>
+    <t>0006_0900</t>
+  </si>
+  <si>
+    <t>0001_0100</t>
+  </si>
+  <si>
+    <t>000E_C400</t>
   </si>
 </sst>
 </file>
@@ -1061,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80B23C6-EAEB-43B1-B045-456C36085CFA}">
   <dimension ref="A1:AG71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1178,22 +1175,22 @@
       </c>
       <c r="L2" s="29"/>
       <c r="M2" s="14" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="O2" s="24" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="P2" s="14" t="s">
         <v>133</v>
       </c>
       <c r="Q2" s="24" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="R2" s="14" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="S2" s="14" t="s">
         <v>131</v>
@@ -1208,7 +1205,7 @@
         <v>117</v>
       </c>
       <c r="W2" s="22" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="X2" s="14" t="s">
         <v>93</v>
@@ -6458,13 +6455,13 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>141</v>
+      <c r="C1" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -6481,7 +6478,7 @@
       </c>
       <c r="K1" t="str">
         <f t="shared" si="0"/>
-        <v>0109 0600</v>
+        <v>0009 0600</v>
       </c>
       <c r="L1" t="str">
         <f t="shared" si="0"/>
@@ -6506,13 +6503,13 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>141</v>
+      <c r="C2" s="13" t="s">
+        <v>155</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -6529,7 +6526,7 @@
       </c>
       <c r="K2" t="str">
         <f t="shared" si="0"/>
-        <v>0109 0600</v>
+        <v>0009 0600</v>
       </c>
       <c r="L2" t="str">
         <f t="shared" si="0"/>
@@ -6559,8 +6556,8 @@
       <c r="B3" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>142</v>
+      <c r="C3" s="11" t="s">
+        <v>156</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -6577,7 +6574,7 @@
       </c>
       <c r="K3" t="str">
         <f t="shared" si="0"/>
-        <v>0301 0100</v>
+        <v>0001 0100</v>
       </c>
       <c r="L3" t="str">
         <f t="shared" si="0"/>
@@ -6607,8 +6604,8 @@
       <c r="B4" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>143</v>
+      <c r="C4" s="11" t="s">
+        <v>156</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -6625,7 +6622,7 @@
       </c>
       <c r="K4" t="str">
         <f t="shared" si="0"/>
-        <v>0101 0100</v>
+        <v>0001 0100</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" si="0"/>
@@ -6650,13 +6647,13 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>144</v>
+      <c r="C5" s="11" t="s">
+        <v>141</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -6703,8 +6700,8 @@
       <c r="B6" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>142</v>
+      <c r="C6" s="11" t="s">
+        <v>156</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -6721,7 +6718,7 @@
       </c>
       <c r="K6" t="str">
         <f t="shared" si="0"/>
-        <v>0301 0100</v>
+        <v>0001 0100</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="0"/>
@@ -6751,8 +6748,8 @@
       <c r="B7" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>143</v>
+      <c r="C7" s="11" t="s">
+        <v>156</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -6769,7 +6766,7 @@
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
-        <v>0101 0100</v>
+        <v>0001 0100</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="0"/>
@@ -6794,13 +6791,13 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>144</v>
+      <c r="C8" s="11" t="s">
+        <v>141</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -6842,13 +6839,13 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>141</v>
+      <c r="C9" s="13" t="s">
+        <v>155</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -6865,7 +6862,7 @@
       </c>
       <c r="K9" t="str">
         <f t="shared" si="0"/>
-        <v>0109 0600</v>
+        <v>0009 0600</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="0"/>
@@ -6895,8 +6892,8 @@
       <c r="B10" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>142</v>
+      <c r="C10" s="11" t="s">
+        <v>156</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -6913,7 +6910,7 @@
       </c>
       <c r="K10" t="str">
         <f t="shared" si="0"/>
-        <v>0301 0100</v>
+        <v>0001 0100</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="0"/>
@@ -6943,8 +6940,8 @@
       <c r="B11" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>143</v>
+      <c r="C11" s="11" t="s">
+        <v>156</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -6961,7 +6958,7 @@
       </c>
       <c r="K11" t="str">
         <f t="shared" si="0"/>
-        <v>0101 0100</v>
+        <v>0001 0100</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="0"/>
@@ -6986,13 +6983,13 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>144</v>
+      <c r="C12" s="11" t="s">
+        <v>141</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -7039,8 +7036,8 @@
       <c r="B13" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>142</v>
+      <c r="C13" s="11" t="s">
+        <v>156</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -7057,7 +7054,7 @@
       </c>
       <c r="K13" t="str">
         <f t="shared" si="0"/>
-        <v>0301 0100</v>
+        <v>0001 0100</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="0"/>
@@ -7087,8 +7084,8 @@
       <c r="B14" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>143</v>
+      <c r="C14" s="11" t="s">
+        <v>156</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -7105,7 +7102,7 @@
       </c>
       <c r="K14" t="str">
         <f t="shared" si="0"/>
-        <v>0101 0100</v>
+        <v>0001 0100</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="0"/>
@@ -7130,13 +7127,13 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>144</v>
+      <c r="C15" s="11" t="s">
+        <v>141</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -7178,13 +7175,13 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>141</v>
+      <c r="C16" s="13" t="s">
+        <v>155</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -7201,7 +7198,7 @@
       </c>
       <c r="K16" t="str">
         <f t="shared" si="0"/>
-        <v>0109 0600</v>
+        <v>0009 0600</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="0"/>
@@ -7231,8 +7228,8 @@
       <c r="B17" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>142</v>
+      <c r="C17" s="11" t="s">
+        <v>156</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -7249,7 +7246,7 @@
       </c>
       <c r="K17" t="str">
         <f t="shared" ref="K17:K30" si="3">RIGHT(SUBSTITUTE(C17,"_",),2)&amp;MID(SUBSTITUTE(C17,"_",),5,2)&amp;" "&amp;MID(SUBSTITUTE(C17,"_",),3,2)&amp;LEFT(SUBSTITUTE(C17,"_",),2)</f>
-        <v>0301 0100</v>
+        <v>0001 0100</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" ref="L17:L30" si="4">RIGHT(SUBSTITUTE(D17,"_",),2)&amp;MID(SUBSTITUTE(D17,"_",),5,2)&amp;" "&amp;MID(SUBSTITUTE(D17,"_",),3,2)&amp;LEFT(SUBSTITUTE(D17,"_",),2)</f>
@@ -7279,8 +7276,8 @@
       <c r="B18" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>143</v>
+      <c r="C18" s="11" t="s">
+        <v>156</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -7297,7 +7294,7 @@
       </c>
       <c r="K18" t="str">
         <f t="shared" si="3"/>
-        <v>0101 0100</v>
+        <v>0001 0100</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="4"/>
@@ -7322,13 +7319,13 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>144</v>
+      <c r="C19" s="11" t="s">
+        <v>141</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -7375,8 +7372,8 @@
       <c r="B20" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>142</v>
+      <c r="C20" s="11" t="s">
+        <v>156</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -7393,7 +7390,7 @@
       </c>
       <c r="K20" t="str">
         <f t="shared" si="3"/>
-        <v>0301 0100</v>
+        <v>0001 0100</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="4"/>
@@ -7423,8 +7420,8 @@
       <c r="B21" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>143</v>
+      <c r="C21" s="11" t="s">
+        <v>156</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -7441,7 +7438,7 @@
       </c>
       <c r="K21" t="str">
         <f t="shared" si="3"/>
-        <v>0101 0100</v>
+        <v>0001 0100</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" si="4"/>
@@ -7466,13 +7463,13 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>144</v>
+      <c r="C22" s="11" t="s">
+        <v>141</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -7519,8 +7516,8 @@
       <c r="B23" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>142</v>
+      <c r="C23" s="11" t="s">
+        <v>156</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -7537,7 +7534,7 @@
       </c>
       <c r="K23" t="str">
         <f t="shared" si="3"/>
-        <v>0301 0100</v>
+        <v>0001 0100</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" si="4"/>
@@ -7567,8 +7564,8 @@
       <c r="B24" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>143</v>
+      <c r="C24" s="11" t="s">
+        <v>156</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -7585,7 +7582,7 @@
       </c>
       <c r="K24" t="str">
         <f t="shared" si="3"/>
-        <v>0101 0100</v>
+        <v>0001 0100</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" si="4"/>
@@ -7610,13 +7607,13 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>144</v>
+      <c r="C25" s="11" t="s">
+        <v>141</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -7663,8 +7660,8 @@
       <c r="B26" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>142</v>
+      <c r="C26" s="11" t="s">
+        <v>156</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -7681,7 +7678,7 @@
       </c>
       <c r="K26" t="str">
         <f t="shared" si="3"/>
-        <v>0301 0100</v>
+        <v>0001 0100</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" si="4"/>
@@ -7711,8 +7708,8 @@
       <c r="B27" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>143</v>
+      <c r="C27" s="11" t="s">
+        <v>156</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -7729,7 +7726,7 @@
       </c>
       <c r="K27" t="str">
         <f t="shared" si="3"/>
-        <v>0101 0100</v>
+        <v>0001 0100</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" si="4"/>
@@ -7754,13 +7751,13 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>144</v>
+      <c r="C28" s="11" t="s">
+        <v>141</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -7807,8 +7804,8 @@
       <c r="B29" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>143</v>
+      <c r="C29" s="11" t="s">
+        <v>156</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -7825,7 +7822,7 @@
       </c>
       <c r="K29" t="str">
         <f t="shared" si="3"/>
-        <v>0101 0100</v>
+        <v>0001 0100</v>
       </c>
       <c r="L29" t="str">
         <f t="shared" si="4"/>
@@ -7850,13 +7847,13 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>145</v>
+      <c r="C30" s="13" t="s">
+        <v>157</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -7873,7 +7870,7 @@
       </c>
       <c r="K30" t="str">
         <f t="shared" si="3"/>
-        <v>01C4 0E00</v>
+        <v>00C4 0E00</v>
       </c>
       <c r="L30" t="str">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
optimiza for thesis writing
</commit_message>
<xml_diff>
--- a/docs/Squeezenet.xlsx
+++ b/docs/Squeezenet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9661AE8-9121-4FAC-8F8F-D361E5DB4074}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2275CA-602D-415D-9866-ACC840416100}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="960" windowWidth="21600" windowHeight="11205" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9317FBE-E145-410C-9025-73E70D2DEE99}"/>
   </bookViews>
   <sheets>
     <sheet name="SqueezeNet v2 MEC Parallel Ch" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SqueezeNet v2 MEC Parallel Ch'!$B$2:$B$71</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'SqueezeNet v2 MEC Parallel Ch'!$A$1:$Z$69</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -524,11 +525,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -554,6 +555,13 @@
       <color theme="1"/>
       <name val="Ubuntu Mono"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1067,13 +1075,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80B23C6-EAEB-43B1-B045-456C36085CFA}">
   <dimension ref="A1:AJ71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:Z69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.4140625" style="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
@@ -1091,22 +1099,22 @@
     <col min="20" max="20" width="6" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="4" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="8" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="26.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="26.4140625" style="18" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="10" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="22.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.9140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.9140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.9140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.9140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.9140625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="10" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="7.88671875" style="18" customWidth="1"/>
-    <col min="34" max="34" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.9140625" style="18" customWidth="1"/>
+    <col min="34" max="34" width="13.9140625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="10" style="21" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.9140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36">
       <c r="A1" s="15"/>
       <c r="B1" s="16"/>
       <c r="C1" s="30" t="s">
@@ -1155,7 +1163,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36">
       <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
@@ -1263,7 +1271,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1316,7 +1324,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -1447,7 +1455,7 @@
         <v>95.57709251101322</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
@@ -1489,7 +1497,7 @@
       <c r="AI5" s="12"/>
       <c r="AJ5" s="14"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36">
       <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
@@ -1605,7 +1613,7 @@
         <v>1.4867256637168142</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1736,7 +1744,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36">
       <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
@@ -1778,7 +1786,7 @@
       <c r="AI8" s="12"/>
       <c r="AJ8" s="14"/>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -1909,7 +1917,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -2040,7 +2048,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36">
       <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
@@ -2082,7 +2090,7 @@
       <c r="AI11" s="12"/>
       <c r="AJ11" s="14"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36">
       <c r="A12" s="7" t="s">
         <v>12</v>
       </c>
@@ -2124,7 +2132,7 @@
       <c r="AI12" s="12"/>
       <c r="AJ12" s="14"/>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36">
       <c r="A13" s="5" t="s">
         <v>19</v>
       </c>
@@ -2172,7 +2180,7 @@
       <c r="AI13" s="10"/>
       <c r="AJ13" s="14"/>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36">
       <c r="A14" s="6" t="s">
         <v>13</v>
       </c>
@@ -2303,7 +2311,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36">
       <c r="A15" s="7" t="s">
         <v>14</v>
       </c>
@@ -2345,7 +2353,7 @@
       <c r="AI15" s="12"/>
       <c r="AJ15" s="14"/>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36">
       <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
@@ -2476,7 +2484,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:36">
       <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
@@ -2607,7 +2615,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:36">
       <c r="A18" s="7" t="s">
         <v>17</v>
       </c>
@@ -2649,7 +2657,7 @@
       <c r="AI18" s="12"/>
       <c r="AJ18" s="14"/>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:36">
       <c r="A19" s="7" t="s">
         <v>18</v>
       </c>
@@ -2691,7 +2699,7 @@
       <c r="AI19" s="12"/>
       <c r="AJ19" s="14"/>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:36">
       <c r="A20" s="5" t="s">
         <v>20</v>
       </c>
@@ -2739,7 +2747,7 @@
       <c r="AI20" s="10"/>
       <c r="AJ20" s="14"/>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:36">
       <c r="A21" s="8" t="s">
         <v>21</v>
       </c>
@@ -2855,7 +2863,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:36">
       <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
@@ -2986,7 +2994,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:36">
       <c r="A23" s="7" t="s">
         <v>23</v>
       </c>
@@ -3028,7 +3036,7 @@
       <c r="AI23" s="12"/>
       <c r="AJ23" s="14"/>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:36">
       <c r="A24" s="6" t="s">
         <v>24</v>
       </c>
@@ -3159,7 +3167,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:36">
       <c r="A25" s="6" t="s">
         <v>25</v>
       </c>
@@ -3290,7 +3298,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:36">
       <c r="A26" s="7" t="s">
         <v>26</v>
       </c>
@@ -3332,7 +3340,7 @@
       <c r="AI26" s="12"/>
       <c r="AJ26" s="14"/>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:36">
       <c r="A27" s="7" t="s">
         <v>27</v>
       </c>
@@ -3374,7 +3382,7 @@
       <c r="AI27" s="12"/>
       <c r="AJ27" s="14"/>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:36">
       <c r="A28" s="5" t="s">
         <v>28</v>
       </c>
@@ -3422,7 +3430,7 @@
       <c r="AI28" s="10"/>
       <c r="AJ28" s="14"/>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:36">
       <c r="A29" s="6" t="s">
         <v>29</v>
       </c>
@@ -3553,7 +3561,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:36">
       <c r="A30" s="7" t="s">
         <v>30</v>
       </c>
@@ -3595,7 +3603,7 @@
       <c r="AI30" s="12"/>
       <c r="AJ30" s="14"/>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:36">
       <c r="A31" s="6" t="s">
         <v>31</v>
       </c>
@@ -3726,7 +3734,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:36">
       <c r="A32" s="6" t="s">
         <v>32</v>
       </c>
@@ -3857,7 +3865,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:36">
       <c r="A33" s="7" t="s">
         <v>33</v>
       </c>
@@ -3899,7 +3907,7 @@
       <c r="AI33" s="12"/>
       <c r="AJ33" s="14"/>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:36">
       <c r="A34" s="7" t="s">
         <v>34</v>
       </c>
@@ -3941,7 +3949,7 @@
       <c r="AI34" s="12"/>
       <c r="AJ34" s="14"/>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:36">
       <c r="A35" s="5" t="s">
         <v>35</v>
       </c>
@@ -3989,7 +3997,7 @@
       <c r="AI35" s="10"/>
       <c r="AJ35" s="14"/>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:36">
       <c r="A36" s="8" t="s">
         <v>36</v>
       </c>
@@ -4105,7 +4113,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:36">
       <c r="A37" s="6" t="s">
         <v>37</v>
       </c>
@@ -4236,7 +4244,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:36">
       <c r="A38" s="7" t="s">
         <v>38</v>
       </c>
@@ -4278,7 +4286,7 @@
       <c r="AI38" s="12"/>
       <c r="AJ38" s="14"/>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:36">
       <c r="A39" s="6" t="s">
         <v>39</v>
       </c>
@@ -4409,7 +4417,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:36">
       <c r="A40" s="6" t="s">
         <v>40</v>
       </c>
@@ -4540,7 +4548,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:36">
       <c r="A41" s="7" t="s">
         <v>41</v>
       </c>
@@ -4582,7 +4590,7 @@
       <c r="AI41" s="12"/>
       <c r="AJ41" s="14"/>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:36">
       <c r="A42" s="7" t="s">
         <v>42</v>
       </c>
@@ -4624,7 +4632,7 @@
       <c r="AI42" s="12"/>
       <c r="AJ42" s="14"/>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:36">
       <c r="A43" s="5" t="s">
         <v>43</v>
       </c>
@@ -4672,7 +4680,7 @@
       <c r="AI43" s="10"/>
       <c r="AJ43" s="14"/>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:36">
       <c r="A44" s="6" t="s">
         <v>44</v>
       </c>
@@ -4803,7 +4811,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:36">
       <c r="A45" s="7" t="s">
         <v>45</v>
       </c>
@@ -4845,7 +4853,7 @@
       <c r="AI45" s="12"/>
       <c r="AJ45" s="14"/>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:36">
       <c r="A46" s="6" t="s">
         <v>46</v>
       </c>
@@ -4976,7 +4984,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:36">
       <c r="A47" s="6" t="s">
         <v>47</v>
       </c>
@@ -5107,7 +5115,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:36">
       <c r="A48" s="7" t="s">
         <v>48</v>
       </c>
@@ -5149,7 +5157,7 @@
       <c r="AI48" s="12"/>
       <c r="AJ48" s="14"/>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:36">
       <c r="A49" s="7" t="s">
         <v>49</v>
       </c>
@@ -5191,7 +5199,7 @@
       <c r="AI49" s="12"/>
       <c r="AJ49" s="14"/>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:36">
       <c r="A50" s="5" t="s">
         <v>50</v>
       </c>
@@ -5239,7 +5247,7 @@
       <c r="AI50" s="10"/>
       <c r="AJ50" s="14"/>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:36">
       <c r="A51" s="6" t="s">
         <v>51</v>
       </c>
@@ -5370,7 +5378,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:36">
       <c r="A52" s="7" t="s">
         <v>52</v>
       </c>
@@ -5412,7 +5420,7 @@
       <c r="AI52" s="12"/>
       <c r="AJ52" s="14"/>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:36">
       <c r="A53" s="6" t="s">
         <v>53</v>
       </c>
@@ -5543,7 +5551,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:36">
       <c r="A54" s="6" t="s">
         <v>54</v>
       </c>
@@ -5674,7 +5682,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:36">
       <c r="A55" s="7" t="s">
         <v>55</v>
       </c>
@@ -5716,7 +5724,7 @@
       <c r="AI55" s="12"/>
       <c r="AJ55" s="14"/>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:36">
       <c r="A56" s="7" t="s">
         <v>56</v>
       </c>
@@ -5758,7 +5766,7 @@
       <c r="AI56" s="12"/>
       <c r="AJ56" s="14"/>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:36">
       <c r="A57" s="5" t="s">
         <v>57</v>
       </c>
@@ -5806,7 +5814,7 @@
       <c r="AI57" s="10"/>
       <c r="AJ57" s="14"/>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:36">
       <c r="A58" s="6" t="s">
         <v>58</v>
       </c>
@@ -5937,7 +5945,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:36">
       <c r="A59" s="7" t="s">
         <v>59</v>
       </c>
@@ -5979,7 +5987,7 @@
       <c r="AI59" s="12"/>
       <c r="AJ59" s="14"/>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:36">
       <c r="A60" s="6" t="s">
         <v>60</v>
       </c>
@@ -6110,7 +6118,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:36">
       <c r="A61" s="6" t="s">
         <v>61</v>
       </c>
@@ -6241,7 +6249,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:36">
       <c r="A62" s="7" t="s">
         <v>62</v>
       </c>
@@ -6283,7 +6291,7 @@
       <c r="AI62" s="12"/>
       <c r="AJ62" s="14"/>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:36">
       <c r="A63" s="7" t="s">
         <v>63</v>
       </c>
@@ -6325,7 +6333,7 @@
       <c r="AI63" s="12"/>
       <c r="AJ63" s="14"/>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:36">
       <c r="A64" s="5" t="s">
         <v>64</v>
       </c>
@@ -6373,7 +6381,7 @@
       <c r="AI64" s="10"/>
       <c r="AJ64" s="14"/>
     </row>
-    <row r="65" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:36">
       <c r="A65" s="19" t="s">
         <v>65</v>
       </c>
@@ -6415,7 +6423,7 @@
       <c r="AI65" s="12"/>
       <c r="AJ65" s="14"/>
     </row>
-    <row r="66" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:36">
       <c r="A66" s="6" t="s">
         <v>66</v>
       </c>
@@ -6546,7 +6554,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="67" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:36">
       <c r="A67" s="7" t="s">
         <v>67</v>
       </c>
@@ -6588,7 +6596,7 @@
       <c r="AI67" s="12"/>
       <c r="AJ67" s="14"/>
     </row>
-    <row r="68" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:36">
       <c r="A68" s="8" t="s">
         <v>68</v>
       </c>
@@ -6704,7 +6712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:36">
       <c r="A69" s="5" t="s">
         <v>69</v>
       </c>
@@ -6745,7 +6753,7 @@
       <c r="AH69" s="1"/>
       <c r="AI69" s="10"/>
     </row>
-    <row r="70" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:36">
       <c r="A70" s="9"/>
       <c r="B70" s="14"/>
       <c r="C70" s="14"/>
@@ -6816,7 +6824,7 @@
         <v>5.2825624061684247</v>
       </c>
     </row>
-    <row r="71" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:36">
       <c r="A71" s="9"/>
       <c r="B71" s="14"/>
       <c r="C71" s="14"/>
@@ -6874,6 +6882,7 @@
     <mergeCell ref="Q1:U1"/>
     <mergeCell ref="J1:L1"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -6887,16 +6896,16 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" customWidth="1"/>
-    <col min="9" max="13" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="9.9140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.9140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.9140625" customWidth="1"/>
+    <col min="9" max="13" width="10.08203125" bestFit="1" customWidth="1"/>
     <col min="14" max="16" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16">
       <c r="A1" s="6" t="s">
         <v>141</v>
       </c>
@@ -6944,7 +6953,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16">
       <c r="A2" s="8" t="s">
         <v>142</v>
       </c>
@@ -6992,7 +7001,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16">
       <c r="A3" s="6" t="s">
         <v>138</v>
       </c>
@@ -7040,7 +7049,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16">
       <c r="A4" s="6" t="s">
         <v>138</v>
       </c>
@@ -7088,7 +7097,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16">
       <c r="A5" s="6" t="s">
         <v>143</v>
       </c>
@@ -7136,7 +7145,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16">
       <c r="A6" s="6" t="s">
         <v>138</v>
       </c>
@@ -7184,7 +7193,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16">
       <c r="A7" s="6" t="s">
         <v>138</v>
       </c>
@@ -7232,7 +7241,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16">
       <c r="A8" s="6" t="s">
         <v>143</v>
       </c>
@@ -7280,7 +7289,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16">
       <c r="A9" s="8" t="s">
         <v>144</v>
       </c>
@@ -7328,7 +7337,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16">
       <c r="A10" s="6" t="s">
         <v>139</v>
       </c>
@@ -7376,7 +7385,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16">
       <c r="A11" s="6" t="s">
         <v>139</v>
       </c>
@@ -7424,7 +7433,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16">
       <c r="A12" s="6" t="s">
         <v>145</v>
       </c>
@@ -7472,7 +7481,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16">
       <c r="A13" s="6" t="s">
         <v>139</v>
       </c>
@@ -7520,7 +7529,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16">
       <c r="A14" s="6" t="s">
         <v>139</v>
       </c>
@@ -7568,7 +7577,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16">
       <c r="A15" s="6" t="s">
         <v>145</v>
       </c>
@@ -7616,7 +7625,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16">
       <c r="A16" s="8" t="s">
         <v>146</v>
       </c>
@@ -7664,7 +7673,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16">
       <c r="A17" s="6" t="s">
         <v>140</v>
       </c>
@@ -7712,7 +7721,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16">
       <c r="A18" s="6" t="s">
         <v>140</v>
       </c>
@@ -7760,7 +7769,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16">
       <c r="A19" s="6" t="s">
         <v>147</v>
       </c>
@@ -7808,7 +7817,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16">
       <c r="A20" s="6" t="s">
         <v>140</v>
       </c>
@@ -7856,7 +7865,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16">
       <c r="A21" s="6" t="s">
         <v>140</v>
       </c>
@@ -7904,7 +7913,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16">
       <c r="A22" s="6" t="s">
         <v>147</v>
       </c>
@@ -7952,7 +7961,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16">
       <c r="A23" s="6" t="s">
         <v>140</v>
       </c>
@@ -8000,7 +8009,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16">
       <c r="A24" s="6" t="s">
         <v>140</v>
       </c>
@@ -8048,7 +8057,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16">
       <c r="A25" s="6" t="s">
         <v>147</v>
       </c>
@@ -8096,7 +8105,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16">
       <c r="A26" s="6" t="s">
         <v>140</v>
       </c>
@@ -8144,7 +8153,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16">
       <c r="A27" s="6" t="s">
         <v>140</v>
       </c>
@@ -8192,7 +8201,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16">
       <c r="A28" s="6" t="s">
         <v>147</v>
       </c>
@@ -8240,7 +8249,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16">
       <c r="A29" s="6" t="s">
         <v>140</v>
       </c>
@@ -8288,7 +8297,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16">
       <c r="A30" s="8" t="s">
         <v>148</v>
       </c>
@@ -8337,6 +8346,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>